<commit_message>
Added profile_template.xlsx file in default_templates
</commit_message>
<xml_diff>
--- a/webroot/export/customexcel/default_templates/profile_template.xlsx
+++ b/webroot/export/customexcel/default_templates/profile_template.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10209"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/umairah/Documents/KORDIT-SQL/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{213FC426-E9D0-EB4D-B111-9088946EB965}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8000" yWindow="760" windowWidth="25600" windowHeight="15620" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7995" yWindow="765" windowWidth="20730" windowHeight="11760" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -327,7 +321,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -612,6 +606,27 @@
     <xf numFmtId="49" fontId="8" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="49" fontId="8" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -627,27 +642,6 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -986,29 +980,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R1019"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28:XFD28"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28:C28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.83203125" customWidth="1"/>
+    <col min="1" max="1" width="16.875" customWidth="1"/>
     <col min="2" max="2" width="14.5" customWidth="1"/>
-    <col min="3" max="3" width="25.1640625" customWidth="1"/>
+    <col min="3" max="3" width="25.125" customWidth="1"/>
     <col min="4" max="4" width="6.5" style="14" customWidth="1"/>
     <col min="5" max="5" width="24.5" customWidth="1"/>
     <col min="6" max="6" width="16.5" customWidth="1"/>
     <col min="7" max="7" width="18" customWidth="1"/>
-    <col min="8" max="8" width="10.6640625" customWidth="1"/>
+    <col min="8" max="8" width="10.625" customWidth="1"/>
     <col min="9" max="18" width="10.5" customWidth="1"/>
-    <col min="19" max="27" width="11.1640625" customWidth="1"/>
+    <col min="19" max="27" width="11.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="44" t="s">
+    <row r="1" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="38" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3"/>
@@ -1028,15 +1022,15 @@
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
     </row>
-    <row r="2" spans="1:18" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="45"/>
+    <row r="2" spans="1:18" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="39"/>
       <c r="B2" s="15"/>
-      <c r="C2" s="46" t="s">
+      <c r="C2" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
       <c r="G2" s="6"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
@@ -1049,15 +1043,15 @@
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
     </row>
-    <row r="3" spans="1:18" s="14" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="45"/>
+    <row r="3" spans="1:18" s="14" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="39"/>
       <c r="B3" s="16"/>
-      <c r="C3" s="47" t="s">
+      <c r="C3" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="47"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="41"/>
       <c r="G3" s="6"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
@@ -1070,8 +1064,8 @@
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
     </row>
-    <row r="4" spans="1:18" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="45"/>
+    <row r="4" spans="1:18" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="39"/>
       <c r="B4" s="3"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -1089,7 +1083,7 @@
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
     </row>
-    <row r="5" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -1109,7 +1103,7 @@
       <c r="Q5" s="1"/>
       <c r="R5" s="1"/>
     </row>
-    <row r="6" spans="1:18" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>2</v>
       </c>
@@ -1137,7 +1131,7 @@
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
     </row>
-    <row r="7" spans="1:18" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>5</v>
       </c>
@@ -1165,7 +1159,7 @@
       <c r="Q7" s="1"/>
       <c r="R7" s="1"/>
     </row>
-    <row r="8" spans="1:18" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:18" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>6</v>
       </c>
@@ -1193,7 +1187,7 @@
       <c r="Q8" s="1"/>
       <c r="R8" s="1"/>
     </row>
-    <row r="9" spans="1:18" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:18" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>7</v>
       </c>
@@ -1221,7 +1215,7 @@
       <c r="Q9" s="1"/>
       <c r="R9" s="1"/>
     </row>
-    <row r="10" spans="1:18" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>8</v>
       </c>
@@ -1249,7 +1243,7 @@
       <c r="Q10" s="1"/>
       <c r="R10" s="1"/>
     </row>
-    <row r="11" spans="1:18" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:18" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>9</v>
       </c>
@@ -1277,7 +1271,7 @@
       <c r="Q11" s="1"/>
       <c r="R11" s="1"/>
     </row>
-    <row r="12" spans="1:18" s="14" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:18" s="14" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="9"/>
       <c r="B12" s="9"/>
       <c r="C12" s="9"/>
@@ -1297,18 +1291,18 @@
       <c r="Q12" s="1"/>
       <c r="R12" s="1"/>
     </row>
-    <row r="13" spans="1:18" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="41" t="s">
+    <row r="13" spans="1:18" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="42" t="s">
         <v>39</v>
       </c>
-      <c r="B13" s="42"/>
-      <c r="C13" s="43"/>
+      <c r="B13" s="43"/>
+      <c r="C13" s="44"/>
       <c r="D13" s="2"/>
-      <c r="E13" s="39" t="s">
+      <c r="E13" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="F13" s="40"/>
-      <c r="G13" s="40"/>
+      <c r="F13" s="49"/>
+      <c r="G13" s="49"/>
       <c r="H13" s="10"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
@@ -1321,7 +1315,7 @@
       <c r="Q13" s="1"/>
       <c r="R13" s="1"/>
     </row>
-    <row r="14" spans="1:18" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:18" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="22" t="s">
         <v>28</v>
       </c>
@@ -1353,7 +1347,7 @@
       <c r="Q14" s="1"/>
       <c r="R14" s="1"/>
     </row>
-    <row r="15" spans="1:18" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:18" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="27" t="s">
         <v>31</v>
       </c>
@@ -1383,7 +1377,7 @@
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
     </row>
-    <row r="16" spans="1:18" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:18" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="23" t="s">
         <v>43</v>
       </c>
@@ -1417,7 +1411,7 @@
       <c r="Q16" s="1"/>
       <c r="R16" s="1"/>
     </row>
-    <row r="17" spans="1:18" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:18" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="21"/>
       <c r="B17" s="24"/>
       <c r="C17" s="24"/>
@@ -1437,18 +1431,18 @@
       <c r="Q17" s="1"/>
       <c r="R17" s="1"/>
     </row>
-    <row r="18" spans="1:18" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="41" t="s">
+    <row r="18" spans="1:18" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="42" t="s">
         <v>40</v>
       </c>
-      <c r="B18" s="42"/>
-      <c r="C18" s="43"/>
+      <c r="B18" s="43"/>
+      <c r="C18" s="44"/>
       <c r="D18" s="2"/>
-      <c r="E18" s="41" t="s">
+      <c r="E18" s="42" t="s">
         <v>47</v>
       </c>
-      <c r="F18" s="42"/>
-      <c r="G18" s="43"/>
+      <c r="F18" s="43"/>
+      <c r="G18" s="44"/>
       <c r="H18" s="11"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
@@ -1461,7 +1455,7 @@
       <c r="Q18" s="1"/>
       <c r="R18" s="1"/>
     </row>
-    <row r="19" spans="1:18" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:18" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="22" t="s">
         <v>41</v>
       </c>
@@ -1493,7 +1487,7 @@
       <c r="Q19" s="1"/>
       <c r="R19" s="1"/>
     </row>
-    <row r="20" spans="1:18" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:18" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="26" t="s">
         <v>44</v>
       </c>
@@ -1525,7 +1519,7 @@
       <c r="Q20" s="1"/>
       <c r="R20" s="1"/>
     </row>
-    <row r="21" spans="1:18" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:18" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="23" t="s">
         <v>43</v>
       </c>
@@ -1559,7 +1553,7 @@
       <c r="Q21" s="1"/>
       <c r="R21" s="1"/>
     </row>
-    <row r="22" spans="1:18" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:18" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="21"/>
       <c r="B22" s="24"/>
       <c r="C22" s="24"/>
@@ -1579,18 +1573,18 @@
       <c r="Q22" s="1"/>
       <c r="R22" s="1"/>
     </row>
-    <row r="23" spans="1:18" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="37" t="s">
+    <row r="23" spans="1:18" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="46" t="s">
         <v>56</v>
       </c>
-      <c r="B23" s="38"/>
-      <c r="C23" s="38"/>
+      <c r="B23" s="47"/>
+      <c r="C23" s="47"/>
       <c r="D23" s="1"/>
-      <c r="E23" s="37" t="s">
+      <c r="E23" s="46" t="s">
         <v>57</v>
       </c>
-      <c r="F23" s="38"/>
-      <c r="G23" s="38"/>
+      <c r="F23" s="47"/>
+      <c r="G23" s="47"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
@@ -1603,7 +1597,7 @@
       <c r="Q23" s="1"/>
       <c r="R23" s="1"/>
     </row>
-    <row r="24" spans="1:18" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:18" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="22" t="s">
         <v>52</v>
       </c>
@@ -1635,7 +1629,7 @@
       <c r="Q24" s="1"/>
       <c r="R24" s="1"/>
     </row>
-    <row r="25" spans="1:18" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:18" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="26" t="s">
         <v>81</v>
       </c>
@@ -1667,7 +1661,7 @@
       <c r="Q25" s="1"/>
       <c r="R25" s="1"/>
     </row>
-    <row r="26" spans="1:18" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:18" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="23" t="s">
         <v>43</v>
       </c>
@@ -1701,7 +1695,7 @@
       <c r="Q26" s="1"/>
       <c r="R26" s="1"/>
     </row>
-    <row r="27" spans="1:18" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:18" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="21"/>
       <c r="B27" s="24"/>
       <c r="C27" s="24"/>
@@ -1721,18 +1715,18 @@
       <c r="Q27" s="1"/>
       <c r="R27" s="1"/>
     </row>
-    <row r="28" spans="1:18" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="37" t="s">
+    <row r="28" spans="1:18" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="46" t="s">
         <v>58</v>
       </c>
-      <c r="B28" s="38"/>
-      <c r="C28" s="38"/>
+      <c r="B28" s="47"/>
+      <c r="C28" s="47"/>
       <c r="D28" s="24"/>
-      <c r="E28" s="37" t="s">
+      <c r="E28" s="46" t="s">
         <v>59</v>
       </c>
-      <c r="F28" s="38"/>
-      <c r="G28" s="38"/>
+      <c r="F28" s="47"/>
+      <c r="G28" s="47"/>
       <c r="H28" s="11"/>
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
@@ -1745,7 +1739,7 @@
       <c r="Q28" s="1"/>
       <c r="R28" s="1"/>
     </row>
-    <row r="29" spans="1:18" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:18" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="22" t="s">
         <v>52</v>
       </c>
@@ -1777,7 +1771,7 @@
       <c r="Q29" s="1"/>
       <c r="R29" s="1"/>
     </row>
-    <row r="30" spans="1:18" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:18" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="26" t="s">
         <v>81</v>
       </c>
@@ -1809,7 +1803,7 @@
       <c r="Q30" s="1"/>
       <c r="R30" s="1"/>
     </row>
-    <row r="31" spans="1:18" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:18" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="23" t="s">
         <v>43</v>
       </c>
@@ -1843,7 +1837,7 @@
       <c r="Q31" s="1"/>
       <c r="R31" s="1"/>
     </row>
-    <row r="32" spans="1:18" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:18" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="21"/>
       <c r="B32" s="24"/>
       <c r="C32" s="24"/>
@@ -1863,7 +1857,7 @@
       <c r="Q32" s="1"/>
       <c r="R32" s="1"/>
     </row>
-    <row r="33" spans="1:18" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:18" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="12" t="s">
         <v>60</v>
       </c>
@@ -1891,7 +1885,7 @@
       <c r="Q33" s="1"/>
       <c r="R33" s="1"/>
     </row>
-    <row r="34" spans="1:18" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:18" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="21"/>
       <c r="B34" s="24"/>
       <c r="C34" s="24"/>
@@ -1911,11 +1905,11 @@
       <c r="Q34" s="1"/>
       <c r="R34" s="1"/>
     </row>
-    <row r="35" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="36" t="s">
+    <row r="35" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="45" t="s">
         <v>91</v>
       </c>
-      <c r="B35" s="36"/>
+      <c r="B35" s="45"/>
       <c r="C35" s="9"/>
       <c r="D35" s="9"/>
       <c r="E35" s="35" t="s">
@@ -1937,11 +1931,11 @@
       <c r="Q35" s="1"/>
       <c r="R35" s="1"/>
     </row>
-    <row r="36" spans="1:18" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="48" t="s">
+    <row r="36" spans="1:18" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="36" t="s">
         <v>93</v>
       </c>
-      <c r="B36" s="49" t="s">
+      <c r="B36" s="37" t="s">
         <v>94</v>
       </c>
       <c r="C36" s="9"/>
@@ -1965,7 +1959,7 @@
       <c r="Q36" s="1"/>
       <c r="R36" s="1"/>
     </row>
-    <row r="37" spans="1:18" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:18" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="26" t="s">
         <v>92</v>
       </c>
@@ -1993,7 +1987,7 @@
       <c r="Q37" s="1"/>
       <c r="R37" s="1"/>
     </row>
-    <row r="38" spans="1:18" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:18" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
       <c r="E38" s="35" t="s">
@@ -2016,7 +2010,7 @@
       <c r="Q38" s="1"/>
       <c r="R38" s="1"/>
     </row>
-    <row r="39" spans="1:18" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:18" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
       <c r="E39" s="34" t="s">
@@ -2032,7 +2026,7 @@
       <c r="K39" s="1"/>
       <c r="L39" s="1"/>
     </row>
-    <row r="40" spans="1:18" s="14" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:18" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
       <c r="E40" s="34" t="s">
@@ -2048,7 +2042,7 @@
       <c r="K40" s="1"/>
       <c r="L40" s="1"/>
     </row>
-    <row r="41" spans="1:18" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:18" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
       <c r="E41" s="35" t="s">
@@ -2064,7 +2058,7 @@
       <c r="K41" s="1"/>
       <c r="L41" s="1"/>
     </row>
-    <row r="42" spans="1:18" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:18" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
       <c r="E42" s="1"/>
@@ -2076,7 +2070,7 @@
       <c r="K42" s="1"/>
       <c r="L42" s="1"/>
     </row>
-    <row r="43" spans="1:18" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:18" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="I43" s="1"/>
@@ -2090,7 +2084,7 @@
       <c r="Q43" s="1"/>
       <c r="R43" s="1"/>
     </row>
-    <row r="44" spans="1:18" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:18" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C44"/>
       <c r="D44"/>
       <c r="E44"/>
@@ -2105,7 +2099,7 @@
       <c r="N44" s="1"/>
       <c r="O44" s="1"/>
     </row>
-    <row r="45" spans="1:18" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:18" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F45" s="1"/>
       <c r="G45" s="1"/>
       <c r="H45" s="1"/>
@@ -2117,7 +2111,7 @@
       <c r="N45" s="1"/>
       <c r="O45" s="1"/>
     </row>
-    <row r="46" spans="1:18" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:18" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C46"/>
       <c r="D46"/>
       <c r="E46"/>
@@ -2132,7 +2126,7 @@
       <c r="N46" s="1"/>
       <c r="O46" s="1"/>
     </row>
-    <row r="47" spans="1:18" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:18" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C47"/>
       <c r="E47"/>
       <c r="F47"/>
@@ -2149,7 +2143,7 @@
       <c r="Q47" s="1"/>
       <c r="R47" s="1"/>
     </row>
-    <row r="48" spans="1:18" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:18" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I48" s="1"/>
       <c r="J48" s="1"/>
       <c r="K48" s="1"/>
@@ -2161,977 +2155,977 @@
       <c r="Q48" s="1"/>
       <c r="R48" s="1"/>
     </row>
-    <row r="49" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="50" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="51" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="52" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="53" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="54" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="55" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="56" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="57" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="58" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="59" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="60" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="61" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="62" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="63" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="64" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="65" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="66" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="67" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="68" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="69" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="70" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="71" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="72" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="73" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="74" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="75" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="76" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="77" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="78" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="79" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="80" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="81" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="82" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="83" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="84" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="85" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="86" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="87" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="88" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="89" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="90" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="91" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="92" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="93" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="94" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="95" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="96" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="97" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="98" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="99" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="100" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="101" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="102" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="103" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="104" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="105" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="106" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="107" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="108" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="109" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="110" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="111" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="112" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="113" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="114" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="115" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="116" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="117" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="118" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="119" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="120" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="121" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="122" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="123" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="124" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="125" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="126" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="127" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="128" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="129" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="130" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="131" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="132" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="133" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="134" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="135" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="136" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="137" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="138" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="139" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="140" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="141" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="142" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="143" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="144" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="145" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="146" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="147" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="148" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="149" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="150" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="151" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="152" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="153" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="154" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="155" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="156" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="157" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="158" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="159" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="160" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="161" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="162" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="163" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="164" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="165" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="166" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="167" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="168" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="169" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="170" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="171" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="172" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="173" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="174" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="175" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="176" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="177" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="178" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="179" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="180" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="181" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="182" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="183" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="184" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="185" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="186" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="187" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="188" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="189" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="190" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="192" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="193" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="194" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="195" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="196" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="197" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="198" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="199" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="200" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="201" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="202" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="203" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="204" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="205" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="206" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="207" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="208" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="209" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="210" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="211" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="212" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="213" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="214" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="215" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="216" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="217" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="218" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="219" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="220" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="221" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="222" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="223" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="224" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="225" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="226" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="227" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="228" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="229" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="230" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="231" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="232" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="233" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="234" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="235" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="236" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="237" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="238" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="239" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="240" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="241" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="242" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="243" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="244" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="245" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="246" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="247" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="248" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="249" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="250" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="251" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="252" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="253" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="254" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="255" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="256" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="257" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="258" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="259" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="260" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="261" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="262" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="263" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="264" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="265" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="266" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="267" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="268" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="269" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="270" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="271" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="272" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="273" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="274" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="275" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="276" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="277" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="278" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="279" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="280" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="281" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="282" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="283" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="284" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="285" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="286" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="287" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="288" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="289" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="290" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="291" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="292" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="293" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="294" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="295" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="296" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="297" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="298" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="299" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="300" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="301" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="302" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="303" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="304" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="305" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="306" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="307" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="308" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="309" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="310" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="311" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="312" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="313" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="314" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="315" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="316" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="317" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="318" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="319" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="320" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="321" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="322" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="323" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="324" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="325" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="326" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="327" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="328" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="329" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="330" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="331" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="332" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="333" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="334" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="335" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="336" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="337" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="338" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="339" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="340" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="341" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="342" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="343" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="344" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="345" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="346" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="347" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="348" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="349" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="350" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="351" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="352" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="353" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="354" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="355" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="356" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="357" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="358" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="359" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="360" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="361" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="362" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="363" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="364" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="365" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="366" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="367" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="368" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="369" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="370" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="371" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="372" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="373" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="374" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="375" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="376" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="377" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="378" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="379" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="380" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="381" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="382" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="383" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="384" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="385" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="386" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="387" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="388" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="389" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="390" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="391" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="392" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="393" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="394" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="395" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="396" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="397" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="398" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="399" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="400" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="401" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="402" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="403" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="404" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="405" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="406" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="407" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="408" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="409" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="410" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="411" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="412" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="413" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="414" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="415" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="416" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="417" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="418" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="419" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="420" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="421" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="422" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="423" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="424" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="425" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="426" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="427" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="428" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="429" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="430" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="431" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="432" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="433" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="434" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="435" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="436" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="437" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="438" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="439" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="440" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="441" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="442" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="443" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="444" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="445" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="446" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="447" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="448" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="449" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="450" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="451" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="452" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="453" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="454" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="455" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="456" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="457" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="458" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="459" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="460" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="461" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="462" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="463" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="464" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="465" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="466" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="467" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="468" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="469" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="470" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="471" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="472" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="473" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="474" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="475" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="476" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="477" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="478" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="479" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="480" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="481" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="482" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="483" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="484" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="485" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="486" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="487" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="488" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="489" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="490" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="491" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="492" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="493" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="494" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="495" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="496" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="497" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="498" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="499" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="500" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="501" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="502" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="503" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="504" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="505" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="506" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="507" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="508" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="509" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="510" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="511" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="512" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="513" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="514" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="515" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="516" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="517" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="518" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="519" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="520" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="521" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="522" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="523" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="524" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="525" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="526" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="527" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="528" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="529" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="530" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="531" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="532" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="533" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="534" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="535" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="536" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="537" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="538" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="539" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="540" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="541" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="542" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="543" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="544" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="545" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="546" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="547" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="548" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="549" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="550" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="551" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="552" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="553" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="554" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="555" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="556" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="557" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="558" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="559" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="560" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="561" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="562" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="563" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="564" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="565" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="566" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="567" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="568" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="569" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="570" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="571" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="572" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="573" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="574" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="575" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="576" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="577" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="578" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="579" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="580" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="581" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="582" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="583" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="584" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="585" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="586" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="587" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="588" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="589" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="590" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="591" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="592" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="593" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="594" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="595" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="596" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="597" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="598" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="599" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="600" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="601" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="602" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="603" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="604" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="605" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="606" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="607" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="608" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="609" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="610" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="611" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="612" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="613" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="614" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="615" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="616" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="617" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="618" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="619" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="620" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="621" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="622" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="623" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="624" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="625" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="626" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="627" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="628" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="629" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="630" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="631" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="632" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="633" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="634" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="635" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="636" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="637" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="638" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="639" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="640" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="641" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="642" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="643" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="644" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="645" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="646" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="647" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="648" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="649" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="650" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="651" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="652" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="653" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="654" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="655" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="656" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="657" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="658" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="659" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="660" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="661" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="662" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="663" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="664" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="665" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="666" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="667" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="668" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="669" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="670" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="671" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="672" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="673" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="674" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="675" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="676" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="677" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="678" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="679" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="680" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="681" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="682" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="683" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="684" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="685" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="686" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="687" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="688" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="689" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="690" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="691" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="692" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="693" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="694" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="695" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="696" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="697" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="698" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="699" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="700" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="701" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="702" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="703" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="704" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="705" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="706" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="707" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="708" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="709" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="710" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="711" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="712" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="713" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="714" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="715" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="716" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="717" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="718" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="719" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="720" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="721" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="722" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="723" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="724" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="725" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="726" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="727" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="728" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="729" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="730" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="731" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="732" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="733" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="734" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="735" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="736" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="737" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="738" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="739" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="740" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="741" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="742" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="743" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="744" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="745" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="746" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="747" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="748" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="749" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="750" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="751" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="752" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="753" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="754" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="755" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="756" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="757" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="758" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="759" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="760" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="761" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="762" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="763" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="764" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="765" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="766" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="767" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="768" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="769" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="770" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="771" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="772" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="773" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="774" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="775" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="776" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="777" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="778" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="779" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="780" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="781" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="782" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="783" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="784" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="785" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="786" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="787" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="788" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="789" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="790" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="791" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="792" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="793" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="794" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="795" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="796" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="797" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="798" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="799" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="800" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="801" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="802" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="803" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="804" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="805" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="806" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="807" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="808" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="809" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="810" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="811" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="812" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="813" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="814" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="815" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="816" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="817" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="818" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="819" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="820" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="821" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="822" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="823" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="824" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="825" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="826" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="827" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="828" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="829" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="830" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="831" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="832" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="833" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="834" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="835" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="836" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="837" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="838" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="839" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="840" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="841" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="842" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="843" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="844" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="845" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="846" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="847" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="848" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="849" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="850" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="851" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="852" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="853" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="854" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="855" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="856" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="857" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="858" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="859" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="860" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="861" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="862" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="863" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="864" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="865" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="866" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="867" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="868" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="869" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="870" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="871" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="872" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="873" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="874" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="875" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="876" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="877" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="878" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="879" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="880" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="881" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="882" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="883" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="884" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="885" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="886" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="887" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="888" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="889" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="890" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="891" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="892" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="893" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="894" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="895" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="896" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="897" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="898" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="899" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="900" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="901" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="902" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="903" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="904" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="905" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="906" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="907" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="908" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="909" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="910" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="911" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="912" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="913" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="914" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="915" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="916" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="917" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="918" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="919" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="920" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="921" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="922" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="923" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="924" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="925" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="926" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="927" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="928" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="929" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="930" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="931" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="932" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="933" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="934" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="935" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="936" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="937" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="938" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="939" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="940" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="941" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="942" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="943" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="944" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="945" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="946" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="947" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="948" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="949" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="950" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="951" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="952" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="953" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="954" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="955" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="956" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="957" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="958" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="959" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="960" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="961" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="962" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="963" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="964" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="965" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="966" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="967" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="968" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="969" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="970" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="971" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="972" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="973" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="974" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="975" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="976" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="977" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="978" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="979" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="980" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="981" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="982" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="983" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="984" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="985" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="986" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="987" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="988" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="989" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="990" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="991" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="992" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="993" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="994" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="995" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="996" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="997" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1001" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1002" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1003" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1004" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1005" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1006" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1007" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1008" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1009" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1010" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1011" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1012" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1013" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1014" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1015" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1016" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1017" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1018" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1019" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="49" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="50" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="51" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="52" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="53" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="54" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="55" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="56" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="57" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="58" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="59" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="60" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="61" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="62" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="63" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="64" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="65" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="66" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="67" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="68" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="69" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="70" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="71" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="72" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="73" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="74" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="75" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="76" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="77" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="79" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="80" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="81" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="82" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="83" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="84" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="85" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="86" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="87" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="88" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="89" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="90" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="91" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="92" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="93" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="94" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="95" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="96" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="97" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="98" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="99" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="100" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="101" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="102" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="103" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="104" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="105" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="106" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="107" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="108" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="109" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="110" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="111" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="112" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="113" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="114" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="115" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="116" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="117" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="118" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="119" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="120" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="121" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="122" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="123" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="124" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="125" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="126" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="127" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="128" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="129" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="130" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="131" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="132" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="133" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="134" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="135" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="136" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="137" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="138" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="139" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="140" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="141" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="142" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="143" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="144" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="145" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="146" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="147" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="148" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="149" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="150" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="151" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="152" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="153" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="154" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="155" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="156" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="157" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="158" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="159" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="160" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="161" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="162" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="163" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="164" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="165" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="166" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="167" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="168" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="169" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="170" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="171" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="172" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="173" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="174" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="175" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="176" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="177" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="178" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="179" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="180" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="181" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="182" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="183" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="184" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="185" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="186" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="187" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="188" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="189" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="190" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="192" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="193" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="194" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="195" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="196" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="197" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="198" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="199" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="200" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="201" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="202" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="203" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="204" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="205" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="206" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="207" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="208" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="209" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="210" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="211" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="212" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="213" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="214" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="215" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="216" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="217" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="218" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="219" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="220" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="221" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="222" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="223" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="224" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="225" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="226" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="227" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="228" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="229" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="230" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="231" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="232" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="233" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="234" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="235" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="236" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="237" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="238" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="239" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="240" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="241" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="242" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="243" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="244" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="245" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="246" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="247" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="248" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="249" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="250" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="251" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="252" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="253" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="254" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="255" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="256" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="257" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="258" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="259" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="260" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="261" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="262" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="263" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="264" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="265" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="266" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="267" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="268" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="269" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="270" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="271" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="272" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="273" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="274" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="275" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="276" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="277" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="278" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="279" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="280" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="281" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="282" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="283" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="284" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="285" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="286" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="287" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="288" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="289" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="290" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="291" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="292" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="293" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="294" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="295" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="296" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="297" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="298" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="299" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="300" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="301" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="302" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="303" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="304" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="305" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="306" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="307" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="308" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="309" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="310" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="311" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="312" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="313" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="314" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="315" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="316" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="317" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="318" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="319" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="320" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="321" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="322" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="323" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="324" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="325" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="326" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="327" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="328" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="329" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="330" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="331" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="332" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="333" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="334" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="335" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="336" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="337" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="338" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="339" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="340" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="341" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="342" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="343" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="344" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="345" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="346" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="347" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="348" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="349" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="350" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="351" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="352" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="353" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="354" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="355" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="356" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="357" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="358" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="359" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="360" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="361" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="362" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="363" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="364" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="365" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="366" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="367" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="368" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="369" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="370" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="371" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="372" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="373" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="374" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="375" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="376" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="377" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="378" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="379" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="380" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="381" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="382" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="383" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="384" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="385" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="386" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="387" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="388" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="389" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="390" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="391" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="392" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="393" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="394" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="395" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="396" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="397" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="398" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="399" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="400" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="401" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="402" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="403" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="404" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="405" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="406" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="407" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="408" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="409" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="410" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="411" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="412" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="413" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="414" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="415" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="416" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="417" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="418" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="419" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="420" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="421" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="422" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="423" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="424" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="425" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="426" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="427" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="428" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="429" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="430" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="431" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="432" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="433" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="434" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="435" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="436" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="437" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="438" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="439" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="440" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="441" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="442" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="443" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="444" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="445" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="446" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="447" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="448" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="449" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="450" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="451" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="452" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="453" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="454" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="455" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="456" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="457" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="458" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="459" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="460" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="461" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="462" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="463" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="464" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="465" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="466" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="467" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="468" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="469" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="470" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="471" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="472" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="473" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="474" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="475" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="476" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="477" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="478" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="479" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="480" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="481" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="482" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="483" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="484" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="485" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="486" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="487" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="488" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="489" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="490" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="491" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="492" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="493" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="494" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="495" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="496" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="497" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="498" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="499" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="500" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="501" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="502" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="503" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="504" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="505" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="506" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="507" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="508" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="509" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="510" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="511" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="512" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="513" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="514" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="515" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="516" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="517" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="518" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="519" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="520" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="521" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="522" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="523" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="524" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="525" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="526" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="527" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="528" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="529" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="530" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="531" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="532" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="533" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="534" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="535" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="536" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="537" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="538" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="539" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="540" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="541" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="542" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="543" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="544" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="545" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="546" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="547" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="548" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="549" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="550" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="551" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="552" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="553" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="554" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="555" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="556" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="557" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="558" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="559" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="560" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="561" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="562" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="563" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="564" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="565" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="566" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="567" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="568" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="569" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="570" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="571" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="572" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="573" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="574" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="575" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="576" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="577" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="578" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="579" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="580" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="581" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="582" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="583" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="584" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="585" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="586" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="587" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="588" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="589" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="590" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="591" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="592" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="593" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="594" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="595" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="596" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="597" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="598" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="599" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="600" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="601" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="602" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="603" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="604" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="605" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="606" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="607" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="608" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="609" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="610" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="611" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="612" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="613" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="614" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="615" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="616" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="617" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="618" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="619" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="620" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="621" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="622" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="623" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="624" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="625" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="626" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="627" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="628" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="629" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="630" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="631" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="632" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="633" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="634" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="635" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="636" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="637" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="638" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="639" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="640" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="641" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="642" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="643" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="644" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="645" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="646" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="647" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="648" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="649" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="650" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="651" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="652" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="653" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="654" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="655" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="656" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="657" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="658" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="659" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="660" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="661" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="662" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="663" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="664" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="665" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="666" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="667" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="668" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="669" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="670" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="671" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="672" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="673" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="674" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="675" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="676" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="677" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="678" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="679" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="680" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="681" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="682" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="683" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="684" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="685" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="686" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="687" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="688" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="689" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="690" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="691" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="692" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="693" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="694" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="695" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="696" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="697" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="698" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="699" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="700" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="701" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="702" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="703" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="704" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="705" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="706" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="707" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="708" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="709" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="710" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="711" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="712" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="713" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="714" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="715" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="716" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="717" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="718" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="719" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="720" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="721" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="722" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="723" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="724" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="725" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="726" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="727" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="728" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="729" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="730" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="731" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="732" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="733" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="734" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="735" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="736" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="737" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="738" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="739" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="740" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="741" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="742" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="743" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="744" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="745" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="746" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="747" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="748" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="749" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="750" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="751" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="752" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="753" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="754" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="755" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="756" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="757" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="758" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="759" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="760" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="761" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="762" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="763" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="764" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="765" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="766" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="767" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="768" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="769" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="770" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="771" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="772" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="773" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="774" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="775" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="776" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="777" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="778" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="779" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="780" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="781" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="782" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="783" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="784" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="785" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="786" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="787" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="788" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="789" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="790" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="791" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="792" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="793" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="794" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="795" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="796" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="797" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="798" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="799" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="800" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="801" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="802" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="803" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="804" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="805" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="806" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="807" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="808" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="809" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="810" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="811" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="812" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="813" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="814" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="815" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="816" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="817" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="818" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="819" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="820" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="821" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="822" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="823" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="824" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="825" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="826" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="827" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="828" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="829" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="830" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="831" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="832" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="833" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="834" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="835" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="836" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="837" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="838" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="839" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="840" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="841" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="842" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="843" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="844" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="845" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="846" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="847" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="848" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="849" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="850" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="851" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="852" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="853" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="854" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="855" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="856" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="857" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="858" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="859" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="860" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="861" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="862" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="863" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="864" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="865" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="866" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="867" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="868" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="869" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="870" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="871" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="872" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="873" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="874" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="875" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="876" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="877" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="878" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="879" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="880" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="881" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="882" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="883" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="884" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="885" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="886" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="887" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="888" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="889" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="890" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="891" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="892" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="893" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="894" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="895" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="896" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="897" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="898" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="899" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="900" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="901" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="902" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="903" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="904" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="905" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="906" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="907" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="908" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="909" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="910" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="911" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="912" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="913" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="914" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="915" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="916" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="917" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="918" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="919" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="920" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="921" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="922" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="923" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="924" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="925" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="926" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="927" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="928" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="929" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="930" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="931" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="932" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="933" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="934" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="935" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="936" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="937" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="938" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="939" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="940" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="941" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="942" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="943" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="944" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="945" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="946" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="947" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="948" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="949" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="950" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="951" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="952" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="953" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="954" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="955" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="956" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="957" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="958" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="959" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="960" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="961" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="962" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="963" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="964" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="965" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="966" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="967" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="968" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="969" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="970" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="971" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="972" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="973" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="974" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="975" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="976" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="977" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="978" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="979" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="980" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="981" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="982" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="983" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="984" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="985" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="986" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="987" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="988" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="989" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="990" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="991" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="992" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="993" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="994" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="995" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="996" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="997" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1001" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1002" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1003" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1004" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1005" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1006" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1007" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1008" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1009" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1010" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1011" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1012" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1013" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1014" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1015" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1016" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1017" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1018" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1019" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="12">
     <mergeCell ref="A1:A4"/>

</xml_diff>

<commit_message>
Add fields in excel template
</commit_message>
<xml_diff>
--- a/webroot/export/customexcel/default_templates/profile_template.xlsx
+++ b/webroot/export/customexcel/default_templates/profile_template.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="101">
   <si>
     <t xml:space="preserve">${"image":{"displayValue":"Institutions.logo_content","imageWidth":"100","imageMarginLeft":"20","imageMarginTop":"5"}}</t>
   </si>
@@ -158,6 +158,18 @@
   </si>
   <si>
     <t xml:space="preserve">${TotalStudents}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total number of absent students</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${StudentTotalAbsences}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total number of absent staff</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${StaffTotalAbsences}</t>
   </si>
   <si>
     <t xml:space="preserve">School Area</t>
@@ -327,7 +339,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -381,6 +393,13 @@
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="9"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="0"/>
     </font>
   </fonts>
   <fills count="3">
@@ -473,7 +492,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -555,6 +574,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -687,7 +710,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:IV1030"/>
+  <dimension ref="A1:IV1034"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -7926,10 +7949,10 @@
       <c r="IV35" s="1"/>
     </row>
     <row r="36" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="10" t="s">
+      <c r="A36" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="B36" s="21" t="s">
+      <c r="B36" s="11" t="s">
         <v>45</v>
       </c>
       <c r="C36" s="17"/>
@@ -8188,10 +8211,10 @@
       <c r="IV36" s="1"/>
     </row>
     <row r="37" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="10" t="s">
+      <c r="A37" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="B37" s="21" t="s">
+      <c r="B37" s="11" t="s">
         <v>47</v>
       </c>
       <c r="C37" s="17"/>
@@ -8450,12 +8473,8 @@
       <c r="IV37" s="1"/>
     </row>
     <row r="38" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="B38" s="21" t="s">
-        <v>49</v>
-      </c>
+      <c r="A38" s="16"/>
+      <c r="B38" s="17"/>
       <c r="C38" s="17"/>
       <c r="D38" s="17"/>
       <c r="E38" s="13"/>
@@ -8712,12 +8731,8 @@
       <c r="IV38" s="1"/>
     </row>
     <row r="39" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="B39" s="21" t="s">
-        <v>51</v>
-      </c>
+      <c r="A39" s="16"/>
+      <c r="B39" s="17"/>
       <c r="C39" s="17"/>
       <c r="D39" s="17"/>
       <c r="E39" s="13"/>
@@ -8975,10 +8990,10 @@
     </row>
     <row r="40" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="10" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
-      <c r="B40" s="21" t="s">
-        <v>53</v>
+      <c r="B40" s="22" t="s">
+        <v>49</v>
       </c>
       <c r="C40" s="17"/>
       <c r="D40" s="17"/>
@@ -9237,10 +9252,10 @@
     </row>
     <row r="41" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="10" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
-      <c r="B41" s="21" t="s">
-        <v>55</v>
+      <c r="B41" s="22" t="s">
+        <v>51</v>
       </c>
       <c r="C41" s="17"/>
       <c r="D41" s="17"/>
@@ -9499,10 +9514,10 @@
     </row>
     <row r="42" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="10" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
-      <c r="B42" s="21" t="s">
-        <v>57</v>
+      <c r="B42" s="22" t="s">
+        <v>53</v>
       </c>
       <c r="C42" s="17"/>
       <c r="D42" s="17"/>
@@ -9760,8 +9775,12 @@
       <c r="IV42" s="1"/>
     </row>
     <row r="43" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A43" s="16"/>
-      <c r="B43" s="17"/>
+      <c r="A43" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B43" s="22" t="s">
+        <v>55</v>
+      </c>
       <c r="C43" s="17"/>
       <c r="D43" s="17"/>
       <c r="E43" s="13"/>
@@ -10018,8 +10037,12 @@
       <c r="IV43" s="1"/>
     </row>
     <row r="44" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A44" s="16"/>
-      <c r="B44" s="17"/>
+      <c r="A44" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="B44" s="22" t="s">
+        <v>57</v>
+      </c>
       <c r="C44" s="17"/>
       <c r="D44" s="17"/>
       <c r="E44" s="13"/>
@@ -10275,17 +10298,19 @@
       <c r="IU44" s="1"/>
       <c r="IV44" s="1"/>
     </row>
-    <row r="45" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A45" s="22" t="s">
+    <row r="45" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A45" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="B45" s="22"/>
-      <c r="C45" s="15"/>
-      <c r="D45" s="15"/>
-      <c r="E45" s="6"/>
-      <c r="F45" s="6"/>
-      <c r="G45" s="15"/>
-      <c r="H45" s="15"/>
+      <c r="B45" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="C45" s="17"/>
+      <c r="D45" s="17"/>
+      <c r="E45" s="13"/>
+      <c r="F45" s="13"/>
+      <c r="G45" s="13"/>
+      <c r="H45" s="13"/>
       <c r="I45" s="6"/>
       <c r="J45" s="6"/>
       <c r="K45" s="6"/>
@@ -10296,20 +10321,258 @@
       <c r="P45" s="6"/>
       <c r="Q45" s="6"/>
       <c r="R45" s="6"/>
+      <c r="S45" s="1"/>
+      <c r="T45" s="1"/>
+      <c r="U45" s="1"/>
+      <c r="V45" s="1"/>
+      <c r="W45" s="1"/>
+      <c r="X45" s="1"/>
+      <c r="Y45" s="1"/>
+      <c r="Z45" s="1"/>
+      <c r="AA45" s="1"/>
+      <c r="AB45" s="1"/>
+      <c r="AC45" s="1"/>
+      <c r="AD45" s="1"/>
+      <c r="AE45" s="1"/>
+      <c r="AF45" s="1"/>
+      <c r="AG45" s="1"/>
+      <c r="AH45" s="1"/>
+      <c r="AI45" s="1"/>
+      <c r="AJ45" s="1"/>
+      <c r="AK45" s="1"/>
+      <c r="AL45" s="1"/>
+      <c r="AM45" s="1"/>
+      <c r="AN45" s="1"/>
+      <c r="AO45" s="1"/>
+      <c r="AP45" s="1"/>
+      <c r="AQ45" s="1"/>
+      <c r="AR45" s="1"/>
+      <c r="AS45" s="1"/>
+      <c r="AT45" s="1"/>
+      <c r="AU45" s="1"/>
+      <c r="AV45" s="1"/>
+      <c r="AW45" s="1"/>
+      <c r="AX45" s="1"/>
+      <c r="AY45" s="1"/>
+      <c r="AZ45" s="1"/>
+      <c r="BA45" s="1"/>
+      <c r="BB45" s="1"/>
+      <c r="BC45" s="1"/>
+      <c r="BD45" s="1"/>
+      <c r="BE45" s="1"/>
+      <c r="BF45" s="1"/>
+      <c r="BG45" s="1"/>
+      <c r="BH45" s="1"/>
+      <c r="BI45" s="1"/>
+      <c r="BJ45" s="1"/>
+      <c r="BK45" s="1"/>
+      <c r="BL45" s="1"/>
+      <c r="BM45" s="1"/>
+      <c r="BN45" s="1"/>
+      <c r="BO45" s="1"/>
+      <c r="BP45" s="1"/>
+      <c r="BQ45" s="1"/>
+      <c r="BR45" s="1"/>
+      <c r="BS45" s="1"/>
+      <c r="BT45" s="1"/>
+      <c r="BU45" s="1"/>
+      <c r="BV45" s="1"/>
+      <c r="BW45" s="1"/>
+      <c r="BX45" s="1"/>
+      <c r="BY45" s="1"/>
+      <c r="BZ45" s="1"/>
+      <c r="CA45" s="1"/>
+      <c r="CB45" s="1"/>
+      <c r="CC45" s="1"/>
+      <c r="CD45" s="1"/>
+      <c r="CE45" s="1"/>
+      <c r="CF45" s="1"/>
+      <c r="CG45" s="1"/>
+      <c r="CH45" s="1"/>
+      <c r="CI45" s="1"/>
+      <c r="CJ45" s="1"/>
+      <c r="CK45" s="1"/>
+      <c r="CL45" s="1"/>
+      <c r="CM45" s="1"/>
+      <c r="CN45" s="1"/>
+      <c r="CO45" s="1"/>
+      <c r="CP45" s="1"/>
+      <c r="CQ45" s="1"/>
+      <c r="CR45" s="1"/>
+      <c r="CS45" s="1"/>
+      <c r="CT45" s="1"/>
+      <c r="CU45" s="1"/>
+      <c r="CV45" s="1"/>
+      <c r="CW45" s="1"/>
+      <c r="CX45" s="1"/>
+      <c r="CY45" s="1"/>
+      <c r="CZ45" s="1"/>
+      <c r="DA45" s="1"/>
+      <c r="DB45" s="1"/>
+      <c r="DC45" s="1"/>
+      <c r="DD45" s="1"/>
+      <c r="DE45" s="1"/>
+      <c r="DF45" s="1"/>
+      <c r="DG45" s="1"/>
+      <c r="DH45" s="1"/>
+      <c r="DI45" s="1"/>
+      <c r="DJ45" s="1"/>
+      <c r="DK45" s="1"/>
+      <c r="DL45" s="1"/>
+      <c r="DM45" s="1"/>
+      <c r="DN45" s="1"/>
+      <c r="DO45" s="1"/>
+      <c r="DP45" s="1"/>
+      <c r="DQ45" s="1"/>
+      <c r="DR45" s="1"/>
+      <c r="DS45" s="1"/>
+      <c r="DT45" s="1"/>
+      <c r="DU45" s="1"/>
+      <c r="DV45" s="1"/>
+      <c r="DW45" s="1"/>
+      <c r="DX45" s="1"/>
+      <c r="DY45" s="1"/>
+      <c r="DZ45" s="1"/>
+      <c r="EA45" s="1"/>
+      <c r="EB45" s="1"/>
+      <c r="EC45" s="1"/>
+      <c r="ED45" s="1"/>
+      <c r="EE45" s="1"/>
+      <c r="EF45" s="1"/>
+      <c r="EG45" s="1"/>
+      <c r="EH45" s="1"/>
+      <c r="EI45" s="1"/>
+      <c r="EJ45" s="1"/>
+      <c r="EK45" s="1"/>
+      <c r="EL45" s="1"/>
+      <c r="EM45" s="1"/>
+      <c r="EN45" s="1"/>
+      <c r="EO45" s="1"/>
+      <c r="EP45" s="1"/>
+      <c r="EQ45" s="1"/>
+      <c r="ER45" s="1"/>
+      <c r="ES45" s="1"/>
+      <c r="ET45" s="1"/>
+      <c r="EU45" s="1"/>
+      <c r="EV45" s="1"/>
+      <c r="EW45" s="1"/>
+      <c r="EX45" s="1"/>
+      <c r="EY45" s="1"/>
+      <c r="EZ45" s="1"/>
+      <c r="FA45" s="1"/>
+      <c r="FB45" s="1"/>
+      <c r="FC45" s="1"/>
+      <c r="FD45" s="1"/>
+      <c r="FE45" s="1"/>
+      <c r="FF45" s="1"/>
+      <c r="FG45" s="1"/>
+      <c r="FH45" s="1"/>
+      <c r="FI45" s="1"/>
+      <c r="FJ45" s="1"/>
+      <c r="FK45" s="1"/>
+      <c r="FL45" s="1"/>
+      <c r="FM45" s="1"/>
+      <c r="FN45" s="1"/>
+      <c r="FO45" s="1"/>
+      <c r="FP45" s="1"/>
+      <c r="FQ45" s="1"/>
+      <c r="FR45" s="1"/>
+      <c r="FS45" s="1"/>
+      <c r="FT45" s="1"/>
+      <c r="FU45" s="1"/>
+      <c r="FV45" s="1"/>
+      <c r="FW45" s="1"/>
+      <c r="FX45" s="1"/>
+      <c r="FY45" s="1"/>
+      <c r="FZ45" s="1"/>
+      <c r="GA45" s="1"/>
+      <c r="GB45" s="1"/>
+      <c r="GC45" s="1"/>
+      <c r="GD45" s="1"/>
+      <c r="GE45" s="1"/>
+      <c r="GF45" s="1"/>
+      <c r="GG45" s="1"/>
+      <c r="GH45" s="1"/>
+      <c r="GI45" s="1"/>
+      <c r="GJ45" s="1"/>
+      <c r="GK45" s="1"/>
+      <c r="GL45" s="1"/>
+      <c r="GM45" s="1"/>
+      <c r="GN45" s="1"/>
+      <c r="GO45" s="1"/>
+      <c r="GP45" s="1"/>
+      <c r="GQ45" s="1"/>
+      <c r="GR45" s="1"/>
+      <c r="GS45" s="1"/>
+      <c r="GT45" s="1"/>
+      <c r="GU45" s="1"/>
+      <c r="GV45" s="1"/>
+      <c r="GW45" s="1"/>
+      <c r="GX45" s="1"/>
+      <c r="GY45" s="1"/>
+      <c r="GZ45" s="1"/>
+      <c r="HA45" s="1"/>
+      <c r="HB45" s="1"/>
+      <c r="HC45" s="1"/>
+      <c r="HD45" s="1"/>
+      <c r="HE45" s="1"/>
+      <c r="HF45" s="1"/>
+      <c r="HG45" s="1"/>
+      <c r="HH45" s="1"/>
+      <c r="HI45" s="1"/>
+      <c r="HJ45" s="1"/>
+      <c r="HK45" s="1"/>
+      <c r="HL45" s="1"/>
+      <c r="HM45" s="1"/>
+      <c r="HN45" s="1"/>
+      <c r="HO45" s="1"/>
+      <c r="HP45" s="1"/>
+      <c r="HQ45" s="1"/>
+      <c r="HR45" s="1"/>
+      <c r="HS45" s="1"/>
+      <c r="HT45" s="1"/>
+      <c r="HU45" s="1"/>
+      <c r="HV45" s="1"/>
+      <c r="HW45" s="1"/>
+      <c r="HX45" s="1"/>
+      <c r="HY45" s="1"/>
+      <c r="HZ45" s="1"/>
+      <c r="IA45" s="1"/>
+      <c r="IB45" s="1"/>
+      <c r="IC45" s="1"/>
+      <c r="ID45" s="1"/>
+      <c r="IE45" s="1"/>
+      <c r="IF45" s="1"/>
+      <c r="IG45" s="1"/>
+      <c r="IH45" s="1"/>
+      <c r="II45" s="1"/>
+      <c r="IJ45" s="1"/>
+      <c r="IK45" s="1"/>
+      <c r="IL45" s="1"/>
+      <c r="IM45" s="1"/>
+      <c r="IN45" s="1"/>
+      <c r="IO45" s="1"/>
+      <c r="IP45" s="1"/>
+      <c r="IQ45" s="1"/>
+      <c r="IR45" s="1"/>
+      <c r="IS45" s="1"/>
+      <c r="IT45" s="1"/>
+      <c r="IU45" s="1"/>
+      <c r="IV45" s="1"/>
     </row>
     <row r="46" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A46" s="23" t="s">
-        <v>59</v>
-      </c>
-      <c r="B46" s="24" t="s">
+      <c r="A46" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="C46" s="15"/>
-      <c r="D46" s="15"/>
-      <c r="E46" s="6"/>
-      <c r="F46" s="6"/>
-      <c r="G46" s="15"/>
-      <c r="H46" s="15"/>
+      <c r="B46" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="C46" s="17"/>
+      <c r="D46" s="17"/>
+      <c r="E46" s="13"/>
+      <c r="F46" s="13"/>
+      <c r="G46" s="13"/>
+      <c r="H46" s="13"/>
       <c r="I46" s="6"/>
       <c r="J46" s="6"/>
       <c r="K46" s="6"/>
@@ -10559,19 +10822,15 @@
       <c r="IU46" s="1"/>
       <c r="IV46" s="1"/>
     </row>
-    <row r="47" customFormat="false" ht="15.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A47" s="25" t="s">
-        <v>61</v>
-      </c>
-      <c r="B47" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="C47" s="6"/>
-      <c r="D47" s="6"/>
-      <c r="E47" s="6"/>
-      <c r="F47" s="6"/>
-      <c r="G47" s="6"/>
-      <c r="H47" s="6"/>
+    <row r="47" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A47" s="16"/>
+      <c r="B47" s="17"/>
+      <c r="C47" s="17"/>
+      <c r="D47" s="17"/>
+      <c r="E47" s="13"/>
+      <c r="F47" s="13"/>
+      <c r="G47" s="13"/>
+      <c r="H47" s="13"/>
       <c r="I47" s="6"/>
       <c r="J47" s="6"/>
       <c r="K47" s="6"/>
@@ -10821,15 +11080,15 @@
       <c r="IU47" s="1"/>
       <c r="IV47" s="1"/>
     </row>
-    <row r="48" customFormat="false" ht="15.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A48" s="1"/>
-      <c r="B48" s="1"/>
-      <c r="C48" s="6"/>
-      <c r="D48" s="6"/>
-      <c r="E48" s="6"/>
-      <c r="F48" s="6"/>
-      <c r="G48" s="6"/>
-      <c r="H48" s="6"/>
+    <row r="48" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A48" s="16"/>
+      <c r="B48" s="17"/>
+      <c r="C48" s="17"/>
+      <c r="D48" s="17"/>
+      <c r="E48" s="13"/>
+      <c r="F48" s="13"/>
+      <c r="G48" s="13"/>
+      <c r="H48" s="13"/>
       <c r="I48" s="6"/>
       <c r="J48" s="6"/>
       <c r="K48" s="6"/>
@@ -11079,283 +11338,51 @@
       <c r="IU48" s="1"/>
       <c r="IV48" s="1"/>
     </row>
-    <row r="49" customFormat="false" ht="15.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A49" s="1"/>
-      <c r="B49" s="1"/>
-      <c r="C49" s="6"/>
-      <c r="D49" s="6"/>
+    <row r="49" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A49" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="B49" s="23"/>
+      <c r="C49" s="15"/>
+      <c r="D49" s="15"/>
       <c r="E49" s="6"/>
       <c r="F49" s="6"/>
-      <c r="G49" s="6"/>
-      <c r="H49" s="6"/>
+      <c r="G49" s="15"/>
+      <c r="H49" s="15"/>
       <c r="I49" s="6"/>
       <c r="J49" s="6"/>
       <c r="K49" s="6"/>
       <c r="L49" s="6"/>
-      <c r="M49" s="1"/>
-      <c r="N49" s="1"/>
-      <c r="O49" s="1"/>
-      <c r="P49" s="1"/>
-      <c r="Q49" s="1"/>
-      <c r="R49" s="1"/>
-      <c r="S49" s="1"/>
-      <c r="T49" s="1"/>
-      <c r="U49" s="1"/>
-      <c r="V49" s="1"/>
-      <c r="W49" s="1"/>
-      <c r="X49" s="1"/>
-      <c r="Y49" s="1"/>
-      <c r="Z49" s="1"/>
-      <c r="AA49" s="1"/>
-      <c r="AB49" s="1"/>
-      <c r="AC49" s="1"/>
-      <c r="AD49" s="1"/>
-      <c r="AE49" s="1"/>
-      <c r="AF49" s="1"/>
-      <c r="AG49" s="1"/>
-      <c r="AH49" s="1"/>
-      <c r="AI49" s="1"/>
-      <c r="AJ49" s="1"/>
-      <c r="AK49" s="1"/>
-      <c r="AL49" s="1"/>
-      <c r="AM49" s="1"/>
-      <c r="AN49" s="1"/>
-      <c r="AO49" s="1"/>
-      <c r="AP49" s="1"/>
-      <c r="AQ49" s="1"/>
-      <c r="AR49" s="1"/>
-      <c r="AS49" s="1"/>
-      <c r="AT49" s="1"/>
-      <c r="AU49" s="1"/>
-      <c r="AV49" s="1"/>
-      <c r="AW49" s="1"/>
-      <c r="AX49" s="1"/>
-      <c r="AY49" s="1"/>
-      <c r="AZ49" s="1"/>
-      <c r="BA49" s="1"/>
-      <c r="BB49" s="1"/>
-      <c r="BC49" s="1"/>
-      <c r="BD49" s="1"/>
-      <c r="BE49" s="1"/>
-      <c r="BF49" s="1"/>
-      <c r="BG49" s="1"/>
-      <c r="BH49" s="1"/>
-      <c r="BI49" s="1"/>
-      <c r="BJ49" s="1"/>
-      <c r="BK49" s="1"/>
-      <c r="BL49" s="1"/>
-      <c r="BM49" s="1"/>
-      <c r="BN49" s="1"/>
-      <c r="BO49" s="1"/>
-      <c r="BP49" s="1"/>
-      <c r="BQ49" s="1"/>
-      <c r="BR49" s="1"/>
-      <c r="BS49" s="1"/>
-      <c r="BT49" s="1"/>
-      <c r="BU49" s="1"/>
-      <c r="BV49" s="1"/>
-      <c r="BW49" s="1"/>
-      <c r="BX49" s="1"/>
-      <c r="BY49" s="1"/>
-      <c r="BZ49" s="1"/>
-      <c r="CA49" s="1"/>
-      <c r="CB49" s="1"/>
-      <c r="CC49" s="1"/>
-      <c r="CD49" s="1"/>
-      <c r="CE49" s="1"/>
-      <c r="CF49" s="1"/>
-      <c r="CG49" s="1"/>
-      <c r="CH49" s="1"/>
-      <c r="CI49" s="1"/>
-      <c r="CJ49" s="1"/>
-      <c r="CK49" s="1"/>
-      <c r="CL49" s="1"/>
-      <c r="CM49" s="1"/>
-      <c r="CN49" s="1"/>
-      <c r="CO49" s="1"/>
-      <c r="CP49" s="1"/>
-      <c r="CQ49" s="1"/>
-      <c r="CR49" s="1"/>
-      <c r="CS49" s="1"/>
-      <c r="CT49" s="1"/>
-      <c r="CU49" s="1"/>
-      <c r="CV49" s="1"/>
-      <c r="CW49" s="1"/>
-      <c r="CX49" s="1"/>
-      <c r="CY49" s="1"/>
-      <c r="CZ49" s="1"/>
-      <c r="DA49" s="1"/>
-      <c r="DB49" s="1"/>
-      <c r="DC49" s="1"/>
-      <c r="DD49" s="1"/>
-      <c r="DE49" s="1"/>
-      <c r="DF49" s="1"/>
-      <c r="DG49" s="1"/>
-      <c r="DH49" s="1"/>
-      <c r="DI49" s="1"/>
-      <c r="DJ49" s="1"/>
-      <c r="DK49" s="1"/>
-      <c r="DL49" s="1"/>
-      <c r="DM49" s="1"/>
-      <c r="DN49" s="1"/>
-      <c r="DO49" s="1"/>
-      <c r="DP49" s="1"/>
-      <c r="DQ49" s="1"/>
-      <c r="DR49" s="1"/>
-      <c r="DS49" s="1"/>
-      <c r="DT49" s="1"/>
-      <c r="DU49" s="1"/>
-      <c r="DV49" s="1"/>
-      <c r="DW49" s="1"/>
-      <c r="DX49" s="1"/>
-      <c r="DY49" s="1"/>
-      <c r="DZ49" s="1"/>
-      <c r="EA49" s="1"/>
-      <c r="EB49" s="1"/>
-      <c r="EC49" s="1"/>
-      <c r="ED49" s="1"/>
-      <c r="EE49" s="1"/>
-      <c r="EF49" s="1"/>
-      <c r="EG49" s="1"/>
-      <c r="EH49" s="1"/>
-      <c r="EI49" s="1"/>
-      <c r="EJ49" s="1"/>
-      <c r="EK49" s="1"/>
-      <c r="EL49" s="1"/>
-      <c r="EM49" s="1"/>
-      <c r="EN49" s="1"/>
-      <c r="EO49" s="1"/>
-      <c r="EP49" s="1"/>
-      <c r="EQ49" s="1"/>
-      <c r="ER49" s="1"/>
-      <c r="ES49" s="1"/>
-      <c r="ET49" s="1"/>
-      <c r="EU49" s="1"/>
-      <c r="EV49" s="1"/>
-      <c r="EW49" s="1"/>
-      <c r="EX49" s="1"/>
-      <c r="EY49" s="1"/>
-      <c r="EZ49" s="1"/>
-      <c r="FA49" s="1"/>
-      <c r="FB49" s="1"/>
-      <c r="FC49" s="1"/>
-      <c r="FD49" s="1"/>
-      <c r="FE49" s="1"/>
-      <c r="FF49" s="1"/>
-      <c r="FG49" s="1"/>
-      <c r="FH49" s="1"/>
-      <c r="FI49" s="1"/>
-      <c r="FJ49" s="1"/>
-      <c r="FK49" s="1"/>
-      <c r="FL49" s="1"/>
-      <c r="FM49" s="1"/>
-      <c r="FN49" s="1"/>
-      <c r="FO49" s="1"/>
-      <c r="FP49" s="1"/>
-      <c r="FQ49" s="1"/>
-      <c r="FR49" s="1"/>
-      <c r="FS49" s="1"/>
-      <c r="FT49" s="1"/>
-      <c r="FU49" s="1"/>
-      <c r="FV49" s="1"/>
-      <c r="FW49" s="1"/>
-      <c r="FX49" s="1"/>
-      <c r="FY49" s="1"/>
-      <c r="FZ49" s="1"/>
-      <c r="GA49" s="1"/>
-      <c r="GB49" s="1"/>
-      <c r="GC49" s="1"/>
-      <c r="GD49" s="1"/>
-      <c r="GE49" s="1"/>
-      <c r="GF49" s="1"/>
-      <c r="GG49" s="1"/>
-      <c r="GH49" s="1"/>
-      <c r="GI49" s="1"/>
-      <c r="GJ49" s="1"/>
-      <c r="GK49" s="1"/>
-      <c r="GL49" s="1"/>
-      <c r="GM49" s="1"/>
-      <c r="GN49" s="1"/>
-      <c r="GO49" s="1"/>
-      <c r="GP49" s="1"/>
-      <c r="GQ49" s="1"/>
-      <c r="GR49" s="1"/>
-      <c r="GS49" s="1"/>
-      <c r="GT49" s="1"/>
-      <c r="GU49" s="1"/>
-      <c r="GV49" s="1"/>
-      <c r="GW49" s="1"/>
-      <c r="GX49" s="1"/>
-      <c r="GY49" s="1"/>
-      <c r="GZ49" s="1"/>
-      <c r="HA49" s="1"/>
-      <c r="HB49" s="1"/>
-      <c r="HC49" s="1"/>
-      <c r="HD49" s="1"/>
-      <c r="HE49" s="1"/>
-      <c r="HF49" s="1"/>
-      <c r="HG49" s="1"/>
-      <c r="HH49" s="1"/>
-      <c r="HI49" s="1"/>
-      <c r="HJ49" s="1"/>
-      <c r="HK49" s="1"/>
-      <c r="HL49" s="1"/>
-      <c r="HM49" s="1"/>
-      <c r="HN49" s="1"/>
-      <c r="HO49" s="1"/>
-      <c r="HP49" s="1"/>
-      <c r="HQ49" s="1"/>
-      <c r="HR49" s="1"/>
-      <c r="HS49" s="1"/>
-      <c r="HT49" s="1"/>
-      <c r="HU49" s="1"/>
-      <c r="HV49" s="1"/>
-      <c r="HW49" s="1"/>
-      <c r="HX49" s="1"/>
-      <c r="HY49" s="1"/>
-      <c r="HZ49" s="1"/>
-      <c r="IA49" s="1"/>
-      <c r="IB49" s="1"/>
-      <c r="IC49" s="1"/>
-      <c r="ID49" s="1"/>
-      <c r="IE49" s="1"/>
-      <c r="IF49" s="1"/>
-      <c r="IG49" s="1"/>
-      <c r="IH49" s="1"/>
-      <c r="II49" s="1"/>
-      <c r="IJ49" s="1"/>
-      <c r="IK49" s="1"/>
-      <c r="IL49" s="1"/>
-      <c r="IM49" s="1"/>
-      <c r="IN49" s="1"/>
-      <c r="IO49" s="1"/>
-      <c r="IP49" s="1"/>
-      <c r="IQ49" s="1"/>
-      <c r="IR49" s="1"/>
-      <c r="IS49" s="1"/>
-      <c r="IT49" s="1"/>
-      <c r="IU49" s="1"/>
-      <c r="IV49" s="1"/>
+      <c r="M49" s="6"/>
+      <c r="N49" s="6"/>
+      <c r="O49" s="6"/>
+      <c r="P49" s="6"/>
+      <c r="Q49" s="6"/>
+      <c r="R49" s="6"/>
     </row>
-    <row r="50" customFormat="false" ht="15.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A50" s="1"/>
-      <c r="B50" s="1"/>
-      <c r="C50" s="6"/>
-      <c r="D50" s="6"/>
+    <row r="50" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A50" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="B50" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="C50" s="15"/>
+      <c r="D50" s="15"/>
       <c r="E50" s="6"/>
       <c r="F50" s="6"/>
-      <c r="G50" s="6"/>
-      <c r="H50" s="6"/>
+      <c r="G50" s="15"/>
+      <c r="H50" s="15"/>
       <c r="I50" s="6"/>
       <c r="J50" s="6"/>
       <c r="K50" s="6"/>
       <c r="L50" s="6"/>
-      <c r="M50" s="1"/>
-      <c r="N50" s="1"/>
-      <c r="O50" s="1"/>
-      <c r="P50" s="1"/>
-      <c r="Q50" s="1"/>
-      <c r="R50" s="1"/>
+      <c r="M50" s="6"/>
+      <c r="N50" s="6"/>
+      <c r="O50" s="6"/>
+      <c r="P50" s="6"/>
+      <c r="Q50" s="6"/>
+      <c r="R50" s="6"/>
       <c r="S50" s="1"/>
       <c r="T50" s="1"/>
       <c r="U50" s="1"/>
@@ -11595,9 +11622,13 @@
       <c r="IU50" s="1"/>
       <c r="IV50" s="1"/>
     </row>
-    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="1"/>
-      <c r="B51" s="1"/>
+    <row r="51" customFormat="false" ht="15.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A51" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="B51" s="22" t="s">
+        <v>66</v>
+      </c>
       <c r="C51" s="6"/>
       <c r="D51" s="6"/>
       <c r="E51" s="6"/>
@@ -11608,12 +11639,12 @@
       <c r="J51" s="6"/>
       <c r="K51" s="6"/>
       <c r="L51" s="6"/>
-      <c r="M51" s="1"/>
-      <c r="N51" s="1"/>
-      <c r="O51" s="1"/>
-      <c r="P51" s="1"/>
-      <c r="Q51" s="1"/>
-      <c r="R51" s="1"/>
+      <c r="M51" s="6"/>
+      <c r="N51" s="6"/>
+      <c r="O51" s="6"/>
+      <c r="P51" s="6"/>
+      <c r="Q51" s="6"/>
+      <c r="R51" s="6"/>
       <c r="S51" s="1"/>
       <c r="T51" s="1"/>
       <c r="U51" s="1"/>
@@ -11853,7 +11884,7 @@
       <c r="IU51" s="1"/>
       <c r="IV51" s="1"/>
     </row>
-    <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="15.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="6"/>
@@ -11866,12 +11897,12 @@
       <c r="J52" s="6"/>
       <c r="K52" s="6"/>
       <c r="L52" s="6"/>
-      <c r="M52" s="1"/>
-      <c r="N52" s="1"/>
-      <c r="O52" s="1"/>
-      <c r="P52" s="1"/>
-      <c r="Q52" s="1"/>
-      <c r="R52" s="1"/>
+      <c r="M52" s="6"/>
+      <c r="N52" s="6"/>
+      <c r="O52" s="6"/>
+      <c r="P52" s="6"/>
+      <c r="Q52" s="6"/>
+      <c r="R52" s="6"/>
       <c r="S52" s="1"/>
       <c r="T52" s="1"/>
       <c r="U52" s="1"/>
@@ -12111,7 +12142,7 @@
       <c r="IU52" s="1"/>
       <c r="IV52" s="1"/>
     </row>
-    <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="15.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="6"/>
@@ -12369,24 +12400,25 @@
       <c r="IU53" s="1"/>
       <c r="IV53" s="1"/>
     </row>
-    <row r="54" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="15.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
-      <c r="C54" s="1"/>
-      <c r="E54" s="1"/>
-      <c r="F54" s="1"/>
-      <c r="G54" s="1"/>
-      <c r="H54" s="1"/>
+      <c r="C54" s="6"/>
+      <c r="D54" s="6"/>
+      <c r="E54" s="6"/>
+      <c r="F54" s="6"/>
+      <c r="G54" s="6"/>
+      <c r="H54" s="6"/>
       <c r="I54" s="6"/>
       <c r="J54" s="6"/>
       <c r="K54" s="6"/>
       <c r="L54" s="6"/>
-      <c r="M54" s="6"/>
-      <c r="N54" s="6"/>
-      <c r="O54" s="6"/>
-      <c r="P54" s="6"/>
-      <c r="Q54" s="6"/>
-      <c r="R54" s="6"/>
+      <c r="M54" s="1"/>
+      <c r="N54" s="1"/>
+      <c r="O54" s="1"/>
+      <c r="P54" s="1"/>
+      <c r="Q54" s="1"/>
+      <c r="R54" s="1"/>
       <c r="S54" s="1"/>
       <c r="T54" s="1"/>
       <c r="U54" s="1"/>
@@ -12626,11 +12658,12 @@
       <c r="IU54" s="1"/>
       <c r="IV54" s="1"/>
     </row>
-    <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
-      <c r="C55" s="1"/>
-      <c r="E55" s="1"/>
+      <c r="C55" s="6"/>
+      <c r="D55" s="6"/>
+      <c r="E55" s="6"/>
       <c r="F55" s="6"/>
       <c r="G55" s="6"/>
       <c r="H55" s="6"/>
@@ -12638,9 +12671,9 @@
       <c r="J55" s="6"/>
       <c r="K55" s="6"/>
       <c r="L55" s="6"/>
-      <c r="M55" s="6"/>
-      <c r="N55" s="6"/>
-      <c r="O55" s="6"/>
+      <c r="M55" s="1"/>
+      <c r="N55" s="1"/>
+      <c r="O55" s="1"/>
       <c r="P55" s="1"/>
       <c r="Q55" s="1"/>
       <c r="R55" s="1"/>
@@ -12886,8 +12919,9 @@
     <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
-      <c r="C56" s="1"/>
-      <c r="E56" s="1"/>
+      <c r="C56" s="6"/>
+      <c r="D56" s="6"/>
+      <c r="E56" s="6"/>
       <c r="F56" s="6"/>
       <c r="G56" s="6"/>
       <c r="H56" s="6"/>
@@ -12895,9 +12929,9 @@
       <c r="J56" s="6"/>
       <c r="K56" s="6"/>
       <c r="L56" s="6"/>
-      <c r="M56" s="6"/>
-      <c r="N56" s="6"/>
-      <c r="O56" s="6"/>
+      <c r="M56" s="1"/>
+      <c r="N56" s="1"/>
+      <c r="O56" s="1"/>
       <c r="P56" s="1"/>
       <c r="Q56" s="1"/>
       <c r="R56" s="1"/>
@@ -13143,8 +13177,9 @@
     <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
-      <c r="C57" s="1"/>
-      <c r="E57" s="1"/>
+      <c r="C57" s="6"/>
+      <c r="D57" s="6"/>
+      <c r="E57" s="6"/>
       <c r="F57" s="6"/>
       <c r="G57" s="6"/>
       <c r="H57" s="6"/>
@@ -13152,9 +13187,9 @@
       <c r="J57" s="6"/>
       <c r="K57" s="6"/>
       <c r="L57" s="6"/>
-      <c r="M57" s="6"/>
-      <c r="N57" s="6"/>
-      <c r="O57" s="6"/>
+      <c r="M57" s="1"/>
+      <c r="N57" s="1"/>
+      <c r="O57" s="1"/>
       <c r="P57" s="1"/>
       <c r="Q57" s="1"/>
       <c r="R57" s="1"/>
@@ -13397,7 +13432,7 @@
       <c r="IU57" s="1"/>
       <c r="IV57" s="1"/>
     </row>
-    <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -13654,7 +13689,14 @@
       <c r="IU58" s="1"/>
       <c r="IV58" s="1"/>
     </row>
-    <row r="59" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A59" s="1"/>
+      <c r="B59" s="1"/>
+      <c r="C59" s="1"/>
+      <c r="E59" s="1"/>
+      <c r="F59" s="6"/>
+      <c r="G59" s="6"/>
+      <c r="H59" s="6"/>
       <c r="I59" s="6"/>
       <c r="J59" s="6"/>
       <c r="K59" s="6"/>
@@ -13662,14 +13704,1031 @@
       <c r="M59" s="6"/>
       <c r="N59" s="6"/>
       <c r="O59" s="6"/>
-      <c r="P59" s="6"/>
-      <c r="Q59" s="6"/>
-      <c r="R59" s="6"/>
+      <c r="P59" s="1"/>
+      <c r="Q59" s="1"/>
+      <c r="R59" s="1"/>
+      <c r="S59" s="1"/>
+      <c r="T59" s="1"/>
+      <c r="U59" s="1"/>
+      <c r="V59" s="1"/>
+      <c r="W59" s="1"/>
+      <c r="X59" s="1"/>
+      <c r="Y59" s="1"/>
+      <c r="Z59" s="1"/>
+      <c r="AA59" s="1"/>
+      <c r="AB59" s="1"/>
+      <c r="AC59" s="1"/>
+      <c r="AD59" s="1"/>
+      <c r="AE59" s="1"/>
+      <c r="AF59" s="1"/>
+      <c r="AG59" s="1"/>
+      <c r="AH59" s="1"/>
+      <c r="AI59" s="1"/>
+      <c r="AJ59" s="1"/>
+      <c r="AK59" s="1"/>
+      <c r="AL59" s="1"/>
+      <c r="AM59" s="1"/>
+      <c r="AN59" s="1"/>
+      <c r="AO59" s="1"/>
+      <c r="AP59" s="1"/>
+      <c r="AQ59" s="1"/>
+      <c r="AR59" s="1"/>
+      <c r="AS59" s="1"/>
+      <c r="AT59" s="1"/>
+      <c r="AU59" s="1"/>
+      <c r="AV59" s="1"/>
+      <c r="AW59" s="1"/>
+      <c r="AX59" s="1"/>
+      <c r="AY59" s="1"/>
+      <c r="AZ59" s="1"/>
+      <c r="BA59" s="1"/>
+      <c r="BB59" s="1"/>
+      <c r="BC59" s="1"/>
+      <c r="BD59" s="1"/>
+      <c r="BE59" s="1"/>
+      <c r="BF59" s="1"/>
+      <c r="BG59" s="1"/>
+      <c r="BH59" s="1"/>
+      <c r="BI59" s="1"/>
+      <c r="BJ59" s="1"/>
+      <c r="BK59" s="1"/>
+      <c r="BL59" s="1"/>
+      <c r="BM59" s="1"/>
+      <c r="BN59" s="1"/>
+      <c r="BO59" s="1"/>
+      <c r="BP59" s="1"/>
+      <c r="BQ59" s="1"/>
+      <c r="BR59" s="1"/>
+      <c r="BS59" s="1"/>
+      <c r="BT59" s="1"/>
+      <c r="BU59" s="1"/>
+      <c r="BV59" s="1"/>
+      <c r="BW59" s="1"/>
+      <c r="BX59" s="1"/>
+      <c r="BY59" s="1"/>
+      <c r="BZ59" s="1"/>
+      <c r="CA59" s="1"/>
+      <c r="CB59" s="1"/>
+      <c r="CC59" s="1"/>
+      <c r="CD59" s="1"/>
+      <c r="CE59" s="1"/>
+      <c r="CF59" s="1"/>
+      <c r="CG59" s="1"/>
+      <c r="CH59" s="1"/>
+      <c r="CI59" s="1"/>
+      <c r="CJ59" s="1"/>
+      <c r="CK59" s="1"/>
+      <c r="CL59" s="1"/>
+      <c r="CM59" s="1"/>
+      <c r="CN59" s="1"/>
+      <c r="CO59" s="1"/>
+      <c r="CP59" s="1"/>
+      <c r="CQ59" s="1"/>
+      <c r="CR59" s="1"/>
+      <c r="CS59" s="1"/>
+      <c r="CT59" s="1"/>
+      <c r="CU59" s="1"/>
+      <c r="CV59" s="1"/>
+      <c r="CW59" s="1"/>
+      <c r="CX59" s="1"/>
+      <c r="CY59" s="1"/>
+      <c r="CZ59" s="1"/>
+      <c r="DA59" s="1"/>
+      <c r="DB59" s="1"/>
+      <c r="DC59" s="1"/>
+      <c r="DD59" s="1"/>
+      <c r="DE59" s="1"/>
+      <c r="DF59" s="1"/>
+      <c r="DG59" s="1"/>
+      <c r="DH59" s="1"/>
+      <c r="DI59" s="1"/>
+      <c r="DJ59" s="1"/>
+      <c r="DK59" s="1"/>
+      <c r="DL59" s="1"/>
+      <c r="DM59" s="1"/>
+      <c r="DN59" s="1"/>
+      <c r="DO59" s="1"/>
+      <c r="DP59" s="1"/>
+      <c r="DQ59" s="1"/>
+      <c r="DR59" s="1"/>
+      <c r="DS59" s="1"/>
+      <c r="DT59" s="1"/>
+      <c r="DU59" s="1"/>
+      <c r="DV59" s="1"/>
+      <c r="DW59" s="1"/>
+      <c r="DX59" s="1"/>
+      <c r="DY59" s="1"/>
+      <c r="DZ59" s="1"/>
+      <c r="EA59" s="1"/>
+      <c r="EB59" s="1"/>
+      <c r="EC59" s="1"/>
+      <c r="ED59" s="1"/>
+      <c r="EE59" s="1"/>
+      <c r="EF59" s="1"/>
+      <c r="EG59" s="1"/>
+      <c r="EH59" s="1"/>
+      <c r="EI59" s="1"/>
+      <c r="EJ59" s="1"/>
+      <c r="EK59" s="1"/>
+      <c r="EL59" s="1"/>
+      <c r="EM59" s="1"/>
+      <c r="EN59" s="1"/>
+      <c r="EO59" s="1"/>
+      <c r="EP59" s="1"/>
+      <c r="EQ59" s="1"/>
+      <c r="ER59" s="1"/>
+      <c r="ES59" s="1"/>
+      <c r="ET59" s="1"/>
+      <c r="EU59" s="1"/>
+      <c r="EV59" s="1"/>
+      <c r="EW59" s="1"/>
+      <c r="EX59" s="1"/>
+      <c r="EY59" s="1"/>
+      <c r="EZ59" s="1"/>
+      <c r="FA59" s="1"/>
+      <c r="FB59" s="1"/>
+      <c r="FC59" s="1"/>
+      <c r="FD59" s="1"/>
+      <c r="FE59" s="1"/>
+      <c r="FF59" s="1"/>
+      <c r="FG59" s="1"/>
+      <c r="FH59" s="1"/>
+      <c r="FI59" s="1"/>
+      <c r="FJ59" s="1"/>
+      <c r="FK59" s="1"/>
+      <c r="FL59" s="1"/>
+      <c r="FM59" s="1"/>
+      <c r="FN59" s="1"/>
+      <c r="FO59" s="1"/>
+      <c r="FP59" s="1"/>
+      <c r="FQ59" s="1"/>
+      <c r="FR59" s="1"/>
+      <c r="FS59" s="1"/>
+      <c r="FT59" s="1"/>
+      <c r="FU59" s="1"/>
+      <c r="FV59" s="1"/>
+      <c r="FW59" s="1"/>
+      <c r="FX59" s="1"/>
+      <c r="FY59" s="1"/>
+      <c r="FZ59" s="1"/>
+      <c r="GA59" s="1"/>
+      <c r="GB59" s="1"/>
+      <c r="GC59" s="1"/>
+      <c r="GD59" s="1"/>
+      <c r="GE59" s="1"/>
+      <c r="GF59" s="1"/>
+      <c r="GG59" s="1"/>
+      <c r="GH59" s="1"/>
+      <c r="GI59" s="1"/>
+      <c r="GJ59" s="1"/>
+      <c r="GK59" s="1"/>
+      <c r="GL59" s="1"/>
+      <c r="GM59" s="1"/>
+      <c r="GN59" s="1"/>
+      <c r="GO59" s="1"/>
+      <c r="GP59" s="1"/>
+      <c r="GQ59" s="1"/>
+      <c r="GR59" s="1"/>
+      <c r="GS59" s="1"/>
+      <c r="GT59" s="1"/>
+      <c r="GU59" s="1"/>
+      <c r="GV59" s="1"/>
+      <c r="GW59" s="1"/>
+      <c r="GX59" s="1"/>
+      <c r="GY59" s="1"/>
+      <c r="GZ59" s="1"/>
+      <c r="HA59" s="1"/>
+      <c r="HB59" s="1"/>
+      <c r="HC59" s="1"/>
+      <c r="HD59" s="1"/>
+      <c r="HE59" s="1"/>
+      <c r="HF59" s="1"/>
+      <c r="HG59" s="1"/>
+      <c r="HH59" s="1"/>
+      <c r="HI59" s="1"/>
+      <c r="HJ59" s="1"/>
+      <c r="HK59" s="1"/>
+      <c r="HL59" s="1"/>
+      <c r="HM59" s="1"/>
+      <c r="HN59" s="1"/>
+      <c r="HO59" s="1"/>
+      <c r="HP59" s="1"/>
+      <c r="HQ59" s="1"/>
+      <c r="HR59" s="1"/>
+      <c r="HS59" s="1"/>
+      <c r="HT59" s="1"/>
+      <c r="HU59" s="1"/>
+      <c r="HV59" s="1"/>
+      <c r="HW59" s="1"/>
+      <c r="HX59" s="1"/>
+      <c r="HY59" s="1"/>
+      <c r="HZ59" s="1"/>
+      <c r="IA59" s="1"/>
+      <c r="IB59" s="1"/>
+      <c r="IC59" s="1"/>
+      <c r="ID59" s="1"/>
+      <c r="IE59" s="1"/>
+      <c r="IF59" s="1"/>
+      <c r="IG59" s="1"/>
+      <c r="IH59" s="1"/>
+      <c r="II59" s="1"/>
+      <c r="IJ59" s="1"/>
+      <c r="IK59" s="1"/>
+      <c r="IL59" s="1"/>
+      <c r="IM59" s="1"/>
+      <c r="IN59" s="1"/>
+      <c r="IO59" s="1"/>
+      <c r="IP59" s="1"/>
+      <c r="IQ59" s="1"/>
+      <c r="IR59" s="1"/>
+      <c r="IS59" s="1"/>
+      <c r="IT59" s="1"/>
+      <c r="IU59" s="1"/>
+      <c r="IV59" s="1"/>
     </row>
-    <row r="60" customFormat="false" ht="15.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="61" customFormat="false" ht="15.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="62" customFormat="false" ht="15.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="63" customFormat="false" ht="15.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A60" s="1"/>
+      <c r="B60" s="1"/>
+      <c r="C60" s="1"/>
+      <c r="E60" s="1"/>
+      <c r="F60" s="6"/>
+      <c r="G60" s="6"/>
+      <c r="H60" s="6"/>
+      <c r="I60" s="6"/>
+      <c r="J60" s="6"/>
+      <c r="K60" s="6"/>
+      <c r="L60" s="6"/>
+      <c r="M60" s="6"/>
+      <c r="N60" s="6"/>
+      <c r="O60" s="6"/>
+      <c r="P60" s="1"/>
+      <c r="Q60" s="1"/>
+      <c r="R60" s="1"/>
+      <c r="S60" s="1"/>
+      <c r="T60" s="1"/>
+      <c r="U60" s="1"/>
+      <c r="V60" s="1"/>
+      <c r="W60" s="1"/>
+      <c r="X60" s="1"/>
+      <c r="Y60" s="1"/>
+      <c r="Z60" s="1"/>
+      <c r="AA60" s="1"/>
+      <c r="AB60" s="1"/>
+      <c r="AC60" s="1"/>
+      <c r="AD60" s="1"/>
+      <c r="AE60" s="1"/>
+      <c r="AF60" s="1"/>
+      <c r="AG60" s="1"/>
+      <c r="AH60" s="1"/>
+      <c r="AI60" s="1"/>
+      <c r="AJ60" s="1"/>
+      <c r="AK60" s="1"/>
+      <c r="AL60" s="1"/>
+      <c r="AM60" s="1"/>
+      <c r="AN60" s="1"/>
+      <c r="AO60" s="1"/>
+      <c r="AP60" s="1"/>
+      <c r="AQ60" s="1"/>
+      <c r="AR60" s="1"/>
+      <c r="AS60" s="1"/>
+      <c r="AT60" s="1"/>
+      <c r="AU60" s="1"/>
+      <c r="AV60" s="1"/>
+      <c r="AW60" s="1"/>
+      <c r="AX60" s="1"/>
+      <c r="AY60" s="1"/>
+      <c r="AZ60" s="1"/>
+      <c r="BA60" s="1"/>
+      <c r="BB60" s="1"/>
+      <c r="BC60" s="1"/>
+      <c r="BD60" s="1"/>
+      <c r="BE60" s="1"/>
+      <c r="BF60" s="1"/>
+      <c r="BG60" s="1"/>
+      <c r="BH60" s="1"/>
+      <c r="BI60" s="1"/>
+      <c r="BJ60" s="1"/>
+      <c r="BK60" s="1"/>
+      <c r="BL60" s="1"/>
+      <c r="BM60" s="1"/>
+      <c r="BN60" s="1"/>
+      <c r="BO60" s="1"/>
+      <c r="BP60" s="1"/>
+      <c r="BQ60" s="1"/>
+      <c r="BR60" s="1"/>
+      <c r="BS60" s="1"/>
+      <c r="BT60" s="1"/>
+      <c r="BU60" s="1"/>
+      <c r="BV60" s="1"/>
+      <c r="BW60" s="1"/>
+      <c r="BX60" s="1"/>
+      <c r="BY60" s="1"/>
+      <c r="BZ60" s="1"/>
+      <c r="CA60" s="1"/>
+      <c r="CB60" s="1"/>
+      <c r="CC60" s="1"/>
+      <c r="CD60" s="1"/>
+      <c r="CE60" s="1"/>
+      <c r="CF60" s="1"/>
+      <c r="CG60" s="1"/>
+      <c r="CH60" s="1"/>
+      <c r="CI60" s="1"/>
+      <c r="CJ60" s="1"/>
+      <c r="CK60" s="1"/>
+      <c r="CL60" s="1"/>
+      <c r="CM60" s="1"/>
+      <c r="CN60" s="1"/>
+      <c r="CO60" s="1"/>
+      <c r="CP60" s="1"/>
+      <c r="CQ60" s="1"/>
+      <c r="CR60" s="1"/>
+      <c r="CS60" s="1"/>
+      <c r="CT60" s="1"/>
+      <c r="CU60" s="1"/>
+      <c r="CV60" s="1"/>
+      <c r="CW60" s="1"/>
+      <c r="CX60" s="1"/>
+      <c r="CY60" s="1"/>
+      <c r="CZ60" s="1"/>
+      <c r="DA60" s="1"/>
+      <c r="DB60" s="1"/>
+      <c r="DC60" s="1"/>
+      <c r="DD60" s="1"/>
+      <c r="DE60" s="1"/>
+      <c r="DF60" s="1"/>
+      <c r="DG60" s="1"/>
+      <c r="DH60" s="1"/>
+      <c r="DI60" s="1"/>
+      <c r="DJ60" s="1"/>
+      <c r="DK60" s="1"/>
+      <c r="DL60" s="1"/>
+      <c r="DM60" s="1"/>
+      <c r="DN60" s="1"/>
+      <c r="DO60" s="1"/>
+      <c r="DP60" s="1"/>
+      <c r="DQ60" s="1"/>
+      <c r="DR60" s="1"/>
+      <c r="DS60" s="1"/>
+      <c r="DT60" s="1"/>
+      <c r="DU60" s="1"/>
+      <c r="DV60" s="1"/>
+      <c r="DW60" s="1"/>
+      <c r="DX60" s="1"/>
+      <c r="DY60" s="1"/>
+      <c r="DZ60" s="1"/>
+      <c r="EA60" s="1"/>
+      <c r="EB60" s="1"/>
+      <c r="EC60" s="1"/>
+      <c r="ED60" s="1"/>
+      <c r="EE60" s="1"/>
+      <c r="EF60" s="1"/>
+      <c r="EG60" s="1"/>
+      <c r="EH60" s="1"/>
+      <c r="EI60" s="1"/>
+      <c r="EJ60" s="1"/>
+      <c r="EK60" s="1"/>
+      <c r="EL60" s="1"/>
+      <c r="EM60" s="1"/>
+      <c r="EN60" s="1"/>
+      <c r="EO60" s="1"/>
+      <c r="EP60" s="1"/>
+      <c r="EQ60" s="1"/>
+      <c r="ER60" s="1"/>
+      <c r="ES60" s="1"/>
+      <c r="ET60" s="1"/>
+      <c r="EU60" s="1"/>
+      <c r="EV60" s="1"/>
+      <c r="EW60" s="1"/>
+      <c r="EX60" s="1"/>
+      <c r="EY60" s="1"/>
+      <c r="EZ60" s="1"/>
+      <c r="FA60" s="1"/>
+      <c r="FB60" s="1"/>
+      <c r="FC60" s="1"/>
+      <c r="FD60" s="1"/>
+      <c r="FE60" s="1"/>
+      <c r="FF60" s="1"/>
+      <c r="FG60" s="1"/>
+      <c r="FH60" s="1"/>
+      <c r="FI60" s="1"/>
+      <c r="FJ60" s="1"/>
+      <c r="FK60" s="1"/>
+      <c r="FL60" s="1"/>
+      <c r="FM60" s="1"/>
+      <c r="FN60" s="1"/>
+      <c r="FO60" s="1"/>
+      <c r="FP60" s="1"/>
+      <c r="FQ60" s="1"/>
+      <c r="FR60" s="1"/>
+      <c r="FS60" s="1"/>
+      <c r="FT60" s="1"/>
+      <c r="FU60" s="1"/>
+      <c r="FV60" s="1"/>
+      <c r="FW60" s="1"/>
+      <c r="FX60" s="1"/>
+      <c r="FY60" s="1"/>
+      <c r="FZ60" s="1"/>
+      <c r="GA60" s="1"/>
+      <c r="GB60" s="1"/>
+      <c r="GC60" s="1"/>
+      <c r="GD60" s="1"/>
+      <c r="GE60" s="1"/>
+      <c r="GF60" s="1"/>
+      <c r="GG60" s="1"/>
+      <c r="GH60" s="1"/>
+      <c r="GI60" s="1"/>
+      <c r="GJ60" s="1"/>
+      <c r="GK60" s="1"/>
+      <c r="GL60" s="1"/>
+      <c r="GM60" s="1"/>
+      <c r="GN60" s="1"/>
+      <c r="GO60" s="1"/>
+      <c r="GP60" s="1"/>
+      <c r="GQ60" s="1"/>
+      <c r="GR60" s="1"/>
+      <c r="GS60" s="1"/>
+      <c r="GT60" s="1"/>
+      <c r="GU60" s="1"/>
+      <c r="GV60" s="1"/>
+      <c r="GW60" s="1"/>
+      <c r="GX60" s="1"/>
+      <c r="GY60" s="1"/>
+      <c r="GZ60" s="1"/>
+      <c r="HA60" s="1"/>
+      <c r="HB60" s="1"/>
+      <c r="HC60" s="1"/>
+      <c r="HD60" s="1"/>
+      <c r="HE60" s="1"/>
+      <c r="HF60" s="1"/>
+      <c r="HG60" s="1"/>
+      <c r="HH60" s="1"/>
+      <c r="HI60" s="1"/>
+      <c r="HJ60" s="1"/>
+      <c r="HK60" s="1"/>
+      <c r="HL60" s="1"/>
+      <c r="HM60" s="1"/>
+      <c r="HN60" s="1"/>
+      <c r="HO60" s="1"/>
+      <c r="HP60" s="1"/>
+      <c r="HQ60" s="1"/>
+      <c r="HR60" s="1"/>
+      <c r="HS60" s="1"/>
+      <c r="HT60" s="1"/>
+      <c r="HU60" s="1"/>
+      <c r="HV60" s="1"/>
+      <c r="HW60" s="1"/>
+      <c r="HX60" s="1"/>
+      <c r="HY60" s="1"/>
+      <c r="HZ60" s="1"/>
+      <c r="IA60" s="1"/>
+      <c r="IB60" s="1"/>
+      <c r="IC60" s="1"/>
+      <c r="ID60" s="1"/>
+      <c r="IE60" s="1"/>
+      <c r="IF60" s="1"/>
+      <c r="IG60" s="1"/>
+      <c r="IH60" s="1"/>
+      <c r="II60" s="1"/>
+      <c r="IJ60" s="1"/>
+      <c r="IK60" s="1"/>
+      <c r="IL60" s="1"/>
+      <c r="IM60" s="1"/>
+      <c r="IN60" s="1"/>
+      <c r="IO60" s="1"/>
+      <c r="IP60" s="1"/>
+      <c r="IQ60" s="1"/>
+      <c r="IR60" s="1"/>
+      <c r="IS60" s="1"/>
+      <c r="IT60" s="1"/>
+      <c r="IU60" s="1"/>
+      <c r="IV60" s="1"/>
+    </row>
+    <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A61" s="1"/>
+      <c r="B61" s="1"/>
+      <c r="C61" s="1"/>
+      <c r="E61" s="1"/>
+      <c r="F61" s="6"/>
+      <c r="G61" s="6"/>
+      <c r="H61" s="6"/>
+      <c r="I61" s="6"/>
+      <c r="J61" s="6"/>
+      <c r="K61" s="6"/>
+      <c r="L61" s="6"/>
+      <c r="M61" s="6"/>
+      <c r="N61" s="6"/>
+      <c r="O61" s="6"/>
+      <c r="P61" s="1"/>
+      <c r="Q61" s="1"/>
+      <c r="R61" s="1"/>
+      <c r="S61" s="1"/>
+      <c r="T61" s="1"/>
+      <c r="U61" s="1"/>
+      <c r="V61" s="1"/>
+      <c r="W61" s="1"/>
+      <c r="X61" s="1"/>
+      <c r="Y61" s="1"/>
+      <c r="Z61" s="1"/>
+      <c r="AA61" s="1"/>
+      <c r="AB61" s="1"/>
+      <c r="AC61" s="1"/>
+      <c r="AD61" s="1"/>
+      <c r="AE61" s="1"/>
+      <c r="AF61" s="1"/>
+      <c r="AG61" s="1"/>
+      <c r="AH61" s="1"/>
+      <c r="AI61" s="1"/>
+      <c r="AJ61" s="1"/>
+      <c r="AK61" s="1"/>
+      <c r="AL61" s="1"/>
+      <c r="AM61" s="1"/>
+      <c r="AN61" s="1"/>
+      <c r="AO61" s="1"/>
+      <c r="AP61" s="1"/>
+      <c r="AQ61" s="1"/>
+      <c r="AR61" s="1"/>
+      <c r="AS61" s="1"/>
+      <c r="AT61" s="1"/>
+      <c r="AU61" s="1"/>
+      <c r="AV61" s="1"/>
+      <c r="AW61" s="1"/>
+      <c r="AX61" s="1"/>
+      <c r="AY61" s="1"/>
+      <c r="AZ61" s="1"/>
+      <c r="BA61" s="1"/>
+      <c r="BB61" s="1"/>
+      <c r="BC61" s="1"/>
+      <c r="BD61" s="1"/>
+      <c r="BE61" s="1"/>
+      <c r="BF61" s="1"/>
+      <c r="BG61" s="1"/>
+      <c r="BH61" s="1"/>
+      <c r="BI61" s="1"/>
+      <c r="BJ61" s="1"/>
+      <c r="BK61" s="1"/>
+      <c r="BL61" s="1"/>
+      <c r="BM61" s="1"/>
+      <c r="BN61" s="1"/>
+      <c r="BO61" s="1"/>
+      <c r="BP61" s="1"/>
+      <c r="BQ61" s="1"/>
+      <c r="BR61" s="1"/>
+      <c r="BS61" s="1"/>
+      <c r="BT61" s="1"/>
+      <c r="BU61" s="1"/>
+      <c r="BV61" s="1"/>
+      <c r="BW61" s="1"/>
+      <c r="BX61" s="1"/>
+      <c r="BY61" s="1"/>
+      <c r="BZ61" s="1"/>
+      <c r="CA61" s="1"/>
+      <c r="CB61" s="1"/>
+      <c r="CC61" s="1"/>
+      <c r="CD61" s="1"/>
+      <c r="CE61" s="1"/>
+      <c r="CF61" s="1"/>
+      <c r="CG61" s="1"/>
+      <c r="CH61" s="1"/>
+      <c r="CI61" s="1"/>
+      <c r="CJ61" s="1"/>
+      <c r="CK61" s="1"/>
+      <c r="CL61" s="1"/>
+      <c r="CM61" s="1"/>
+      <c r="CN61" s="1"/>
+      <c r="CO61" s="1"/>
+      <c r="CP61" s="1"/>
+      <c r="CQ61" s="1"/>
+      <c r="CR61" s="1"/>
+      <c r="CS61" s="1"/>
+      <c r="CT61" s="1"/>
+      <c r="CU61" s="1"/>
+      <c r="CV61" s="1"/>
+      <c r="CW61" s="1"/>
+      <c r="CX61" s="1"/>
+      <c r="CY61" s="1"/>
+      <c r="CZ61" s="1"/>
+      <c r="DA61" s="1"/>
+      <c r="DB61" s="1"/>
+      <c r="DC61" s="1"/>
+      <c r="DD61" s="1"/>
+      <c r="DE61" s="1"/>
+      <c r="DF61" s="1"/>
+      <c r="DG61" s="1"/>
+      <c r="DH61" s="1"/>
+      <c r="DI61" s="1"/>
+      <c r="DJ61" s="1"/>
+      <c r="DK61" s="1"/>
+      <c r="DL61" s="1"/>
+      <c r="DM61" s="1"/>
+      <c r="DN61" s="1"/>
+      <c r="DO61" s="1"/>
+      <c r="DP61" s="1"/>
+      <c r="DQ61" s="1"/>
+      <c r="DR61" s="1"/>
+      <c r="DS61" s="1"/>
+      <c r="DT61" s="1"/>
+      <c r="DU61" s="1"/>
+      <c r="DV61" s="1"/>
+      <c r="DW61" s="1"/>
+      <c r="DX61" s="1"/>
+      <c r="DY61" s="1"/>
+      <c r="DZ61" s="1"/>
+      <c r="EA61" s="1"/>
+      <c r="EB61" s="1"/>
+      <c r="EC61" s="1"/>
+      <c r="ED61" s="1"/>
+      <c r="EE61" s="1"/>
+      <c r="EF61" s="1"/>
+      <c r="EG61" s="1"/>
+      <c r="EH61" s="1"/>
+      <c r="EI61" s="1"/>
+      <c r="EJ61" s="1"/>
+      <c r="EK61" s="1"/>
+      <c r="EL61" s="1"/>
+      <c r="EM61" s="1"/>
+      <c r="EN61" s="1"/>
+      <c r="EO61" s="1"/>
+      <c r="EP61" s="1"/>
+      <c r="EQ61" s="1"/>
+      <c r="ER61" s="1"/>
+      <c r="ES61" s="1"/>
+      <c r="ET61" s="1"/>
+      <c r="EU61" s="1"/>
+      <c r="EV61" s="1"/>
+      <c r="EW61" s="1"/>
+      <c r="EX61" s="1"/>
+      <c r="EY61" s="1"/>
+      <c r="EZ61" s="1"/>
+      <c r="FA61" s="1"/>
+      <c r="FB61" s="1"/>
+      <c r="FC61" s="1"/>
+      <c r="FD61" s="1"/>
+      <c r="FE61" s="1"/>
+      <c r="FF61" s="1"/>
+      <c r="FG61" s="1"/>
+      <c r="FH61" s="1"/>
+      <c r="FI61" s="1"/>
+      <c r="FJ61" s="1"/>
+      <c r="FK61" s="1"/>
+      <c r="FL61" s="1"/>
+      <c r="FM61" s="1"/>
+      <c r="FN61" s="1"/>
+      <c r="FO61" s="1"/>
+      <c r="FP61" s="1"/>
+      <c r="FQ61" s="1"/>
+      <c r="FR61" s="1"/>
+      <c r="FS61" s="1"/>
+      <c r="FT61" s="1"/>
+      <c r="FU61" s="1"/>
+      <c r="FV61" s="1"/>
+      <c r="FW61" s="1"/>
+      <c r="FX61" s="1"/>
+      <c r="FY61" s="1"/>
+      <c r="FZ61" s="1"/>
+      <c r="GA61" s="1"/>
+      <c r="GB61" s="1"/>
+      <c r="GC61" s="1"/>
+      <c r="GD61" s="1"/>
+      <c r="GE61" s="1"/>
+      <c r="GF61" s="1"/>
+      <c r="GG61" s="1"/>
+      <c r="GH61" s="1"/>
+      <c r="GI61" s="1"/>
+      <c r="GJ61" s="1"/>
+      <c r="GK61" s="1"/>
+      <c r="GL61" s="1"/>
+      <c r="GM61" s="1"/>
+      <c r="GN61" s="1"/>
+      <c r="GO61" s="1"/>
+      <c r="GP61" s="1"/>
+      <c r="GQ61" s="1"/>
+      <c r="GR61" s="1"/>
+      <c r="GS61" s="1"/>
+      <c r="GT61" s="1"/>
+      <c r="GU61" s="1"/>
+      <c r="GV61" s="1"/>
+      <c r="GW61" s="1"/>
+      <c r="GX61" s="1"/>
+      <c r="GY61" s="1"/>
+      <c r="GZ61" s="1"/>
+      <c r="HA61" s="1"/>
+      <c r="HB61" s="1"/>
+      <c r="HC61" s="1"/>
+      <c r="HD61" s="1"/>
+      <c r="HE61" s="1"/>
+      <c r="HF61" s="1"/>
+      <c r="HG61" s="1"/>
+      <c r="HH61" s="1"/>
+      <c r="HI61" s="1"/>
+      <c r="HJ61" s="1"/>
+      <c r="HK61" s="1"/>
+      <c r="HL61" s="1"/>
+      <c r="HM61" s="1"/>
+      <c r="HN61" s="1"/>
+      <c r="HO61" s="1"/>
+      <c r="HP61" s="1"/>
+      <c r="HQ61" s="1"/>
+      <c r="HR61" s="1"/>
+      <c r="HS61" s="1"/>
+      <c r="HT61" s="1"/>
+      <c r="HU61" s="1"/>
+      <c r="HV61" s="1"/>
+      <c r="HW61" s="1"/>
+      <c r="HX61" s="1"/>
+      <c r="HY61" s="1"/>
+      <c r="HZ61" s="1"/>
+      <c r="IA61" s="1"/>
+      <c r="IB61" s="1"/>
+      <c r="IC61" s="1"/>
+      <c r="ID61" s="1"/>
+      <c r="IE61" s="1"/>
+      <c r="IF61" s="1"/>
+      <c r="IG61" s="1"/>
+      <c r="IH61" s="1"/>
+      <c r="II61" s="1"/>
+      <c r="IJ61" s="1"/>
+      <c r="IK61" s="1"/>
+      <c r="IL61" s="1"/>
+      <c r="IM61" s="1"/>
+      <c r="IN61" s="1"/>
+      <c r="IO61" s="1"/>
+      <c r="IP61" s="1"/>
+      <c r="IQ61" s="1"/>
+      <c r="IR61" s="1"/>
+      <c r="IS61" s="1"/>
+      <c r="IT61" s="1"/>
+      <c r="IU61" s="1"/>
+      <c r="IV61" s="1"/>
+    </row>
+    <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A62" s="1"/>
+      <c r="B62" s="1"/>
+      <c r="C62" s="1"/>
+      <c r="E62" s="1"/>
+      <c r="F62" s="1"/>
+      <c r="G62" s="1"/>
+      <c r="H62" s="1"/>
+      <c r="I62" s="6"/>
+      <c r="J62" s="6"/>
+      <c r="K62" s="6"/>
+      <c r="L62" s="6"/>
+      <c r="M62" s="6"/>
+      <c r="N62" s="6"/>
+      <c r="O62" s="6"/>
+      <c r="P62" s="6"/>
+      <c r="Q62" s="6"/>
+      <c r="R62" s="6"/>
+      <c r="S62" s="1"/>
+      <c r="T62" s="1"/>
+      <c r="U62" s="1"/>
+      <c r="V62" s="1"/>
+      <c r="W62" s="1"/>
+      <c r="X62" s="1"/>
+      <c r="Y62" s="1"/>
+      <c r="Z62" s="1"/>
+      <c r="AA62" s="1"/>
+      <c r="AB62" s="1"/>
+      <c r="AC62" s="1"/>
+      <c r="AD62" s="1"/>
+      <c r="AE62" s="1"/>
+      <c r="AF62" s="1"/>
+      <c r="AG62" s="1"/>
+      <c r="AH62" s="1"/>
+      <c r="AI62" s="1"/>
+      <c r="AJ62" s="1"/>
+      <c r="AK62" s="1"/>
+      <c r="AL62" s="1"/>
+      <c r="AM62" s="1"/>
+      <c r="AN62" s="1"/>
+      <c r="AO62" s="1"/>
+      <c r="AP62" s="1"/>
+      <c r="AQ62" s="1"/>
+      <c r="AR62" s="1"/>
+      <c r="AS62" s="1"/>
+      <c r="AT62" s="1"/>
+      <c r="AU62" s="1"/>
+      <c r="AV62" s="1"/>
+      <c r="AW62" s="1"/>
+      <c r="AX62" s="1"/>
+      <c r="AY62" s="1"/>
+      <c r="AZ62" s="1"/>
+      <c r="BA62" s="1"/>
+      <c r="BB62" s="1"/>
+      <c r="BC62" s="1"/>
+      <c r="BD62" s="1"/>
+      <c r="BE62" s="1"/>
+      <c r="BF62" s="1"/>
+      <c r="BG62" s="1"/>
+      <c r="BH62" s="1"/>
+      <c r="BI62" s="1"/>
+      <c r="BJ62" s="1"/>
+      <c r="BK62" s="1"/>
+      <c r="BL62" s="1"/>
+      <c r="BM62" s="1"/>
+      <c r="BN62" s="1"/>
+      <c r="BO62" s="1"/>
+      <c r="BP62" s="1"/>
+      <c r="BQ62" s="1"/>
+      <c r="BR62" s="1"/>
+      <c r="BS62" s="1"/>
+      <c r="BT62" s="1"/>
+      <c r="BU62" s="1"/>
+      <c r="BV62" s="1"/>
+      <c r="BW62" s="1"/>
+      <c r="BX62" s="1"/>
+      <c r="BY62" s="1"/>
+      <c r="BZ62" s="1"/>
+      <c r="CA62" s="1"/>
+      <c r="CB62" s="1"/>
+      <c r="CC62" s="1"/>
+      <c r="CD62" s="1"/>
+      <c r="CE62" s="1"/>
+      <c r="CF62" s="1"/>
+      <c r="CG62" s="1"/>
+      <c r="CH62" s="1"/>
+      <c r="CI62" s="1"/>
+      <c r="CJ62" s="1"/>
+      <c r="CK62" s="1"/>
+      <c r="CL62" s="1"/>
+      <c r="CM62" s="1"/>
+      <c r="CN62" s="1"/>
+      <c r="CO62" s="1"/>
+      <c r="CP62" s="1"/>
+      <c r="CQ62" s="1"/>
+      <c r="CR62" s="1"/>
+      <c r="CS62" s="1"/>
+      <c r="CT62" s="1"/>
+      <c r="CU62" s="1"/>
+      <c r="CV62" s="1"/>
+      <c r="CW62" s="1"/>
+      <c r="CX62" s="1"/>
+      <c r="CY62" s="1"/>
+      <c r="CZ62" s="1"/>
+      <c r="DA62" s="1"/>
+      <c r="DB62" s="1"/>
+      <c r="DC62" s="1"/>
+      <c r="DD62" s="1"/>
+      <c r="DE62" s="1"/>
+      <c r="DF62" s="1"/>
+      <c r="DG62" s="1"/>
+      <c r="DH62" s="1"/>
+      <c r="DI62" s="1"/>
+      <c r="DJ62" s="1"/>
+      <c r="DK62" s="1"/>
+      <c r="DL62" s="1"/>
+      <c r="DM62" s="1"/>
+      <c r="DN62" s="1"/>
+      <c r="DO62" s="1"/>
+      <c r="DP62" s="1"/>
+      <c r="DQ62" s="1"/>
+      <c r="DR62" s="1"/>
+      <c r="DS62" s="1"/>
+      <c r="DT62" s="1"/>
+      <c r="DU62" s="1"/>
+      <c r="DV62" s="1"/>
+      <c r="DW62" s="1"/>
+      <c r="DX62" s="1"/>
+      <c r="DY62" s="1"/>
+      <c r="DZ62" s="1"/>
+      <c r="EA62" s="1"/>
+      <c r="EB62" s="1"/>
+      <c r="EC62" s="1"/>
+      <c r="ED62" s="1"/>
+      <c r="EE62" s="1"/>
+      <c r="EF62" s="1"/>
+      <c r="EG62" s="1"/>
+      <c r="EH62" s="1"/>
+      <c r="EI62" s="1"/>
+      <c r="EJ62" s="1"/>
+      <c r="EK62" s="1"/>
+      <c r="EL62" s="1"/>
+      <c r="EM62" s="1"/>
+      <c r="EN62" s="1"/>
+      <c r="EO62" s="1"/>
+      <c r="EP62" s="1"/>
+      <c r="EQ62" s="1"/>
+      <c r="ER62" s="1"/>
+      <c r="ES62" s="1"/>
+      <c r="ET62" s="1"/>
+      <c r="EU62" s="1"/>
+      <c r="EV62" s="1"/>
+      <c r="EW62" s="1"/>
+      <c r="EX62" s="1"/>
+      <c r="EY62" s="1"/>
+      <c r="EZ62" s="1"/>
+      <c r="FA62" s="1"/>
+      <c r="FB62" s="1"/>
+      <c r="FC62" s="1"/>
+      <c r="FD62" s="1"/>
+      <c r="FE62" s="1"/>
+      <c r="FF62" s="1"/>
+      <c r="FG62" s="1"/>
+      <c r="FH62" s="1"/>
+      <c r="FI62" s="1"/>
+      <c r="FJ62" s="1"/>
+      <c r="FK62" s="1"/>
+      <c r="FL62" s="1"/>
+      <c r="FM62" s="1"/>
+      <c r="FN62" s="1"/>
+      <c r="FO62" s="1"/>
+      <c r="FP62" s="1"/>
+      <c r="FQ62" s="1"/>
+      <c r="FR62" s="1"/>
+      <c r="FS62" s="1"/>
+      <c r="FT62" s="1"/>
+      <c r="FU62" s="1"/>
+      <c r="FV62" s="1"/>
+      <c r="FW62" s="1"/>
+      <c r="FX62" s="1"/>
+      <c r="FY62" s="1"/>
+      <c r="FZ62" s="1"/>
+      <c r="GA62" s="1"/>
+      <c r="GB62" s="1"/>
+      <c r="GC62" s="1"/>
+      <c r="GD62" s="1"/>
+      <c r="GE62" s="1"/>
+      <c r="GF62" s="1"/>
+      <c r="GG62" s="1"/>
+      <c r="GH62" s="1"/>
+      <c r="GI62" s="1"/>
+      <c r="GJ62" s="1"/>
+      <c r="GK62" s="1"/>
+      <c r="GL62" s="1"/>
+      <c r="GM62" s="1"/>
+      <c r="GN62" s="1"/>
+      <c r="GO62" s="1"/>
+      <c r="GP62" s="1"/>
+      <c r="GQ62" s="1"/>
+      <c r="GR62" s="1"/>
+      <c r="GS62" s="1"/>
+      <c r="GT62" s="1"/>
+      <c r="GU62" s="1"/>
+      <c r="GV62" s="1"/>
+      <c r="GW62" s="1"/>
+      <c r="GX62" s="1"/>
+      <c r="GY62" s="1"/>
+      <c r="GZ62" s="1"/>
+      <c r="HA62" s="1"/>
+      <c r="HB62" s="1"/>
+      <c r="HC62" s="1"/>
+      <c r="HD62" s="1"/>
+      <c r="HE62" s="1"/>
+      <c r="HF62" s="1"/>
+      <c r="HG62" s="1"/>
+      <c r="HH62" s="1"/>
+      <c r="HI62" s="1"/>
+      <c r="HJ62" s="1"/>
+      <c r="HK62" s="1"/>
+      <c r="HL62" s="1"/>
+      <c r="HM62" s="1"/>
+      <c r="HN62" s="1"/>
+      <c r="HO62" s="1"/>
+      <c r="HP62" s="1"/>
+      <c r="HQ62" s="1"/>
+      <c r="HR62" s="1"/>
+      <c r="HS62" s="1"/>
+      <c r="HT62" s="1"/>
+      <c r="HU62" s="1"/>
+      <c r="HV62" s="1"/>
+      <c r="HW62" s="1"/>
+      <c r="HX62" s="1"/>
+      <c r="HY62" s="1"/>
+      <c r="HZ62" s="1"/>
+      <c r="IA62" s="1"/>
+      <c r="IB62" s="1"/>
+      <c r="IC62" s="1"/>
+      <c r="ID62" s="1"/>
+      <c r="IE62" s="1"/>
+      <c r="IF62" s="1"/>
+      <c r="IG62" s="1"/>
+      <c r="IH62" s="1"/>
+      <c r="II62" s="1"/>
+      <c r="IJ62" s="1"/>
+      <c r="IK62" s="1"/>
+      <c r="IL62" s="1"/>
+      <c r="IM62" s="1"/>
+      <c r="IN62" s="1"/>
+      <c r="IO62" s="1"/>
+      <c r="IP62" s="1"/>
+      <c r="IQ62" s="1"/>
+      <c r="IR62" s="1"/>
+      <c r="IS62" s="1"/>
+      <c r="IT62" s="1"/>
+      <c r="IU62" s="1"/>
+      <c r="IV62" s="1"/>
+    </row>
+    <row r="63" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="I63" s="6"/>
+      <c r="J63" s="6"/>
+      <c r="K63" s="6"/>
+      <c r="L63" s="6"/>
+      <c r="M63" s="6"/>
+      <c r="N63" s="6"/>
+      <c r="O63" s="6"/>
+      <c r="P63" s="6"/>
+      <c r="Q63" s="6"/>
+      <c r="R63" s="6"/>
+    </row>
     <row r="64" customFormat="false" ht="15.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="65" customFormat="false" ht="15.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="66" customFormat="false" ht="15.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -14637,13 +15696,17 @@
     <row r="1028" customFormat="false" ht="15.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1029" customFormat="false" ht="15.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1030" customFormat="false" ht="15.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1031" customFormat="false" ht="15.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1032" customFormat="false" ht="15.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1033" customFormat="false" ht="15.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1034" customFormat="false" ht="15.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="A1:A4"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="A24:C24"/>
-    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="A49:B49"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
@@ -14674,31 +15737,31 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="18" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="B1" s="18"/>
       <c r="C1" s="18"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="26" t="s">
-        <v>64</v>
+      <c r="A2" s="27" t="s">
+        <v>68</v>
       </c>
-      <c r="B2" s="26" t="s">
-        <v>65</v>
+      <c r="B2" s="27" t="s">
+        <v>69</v>
       </c>
-      <c r="C2" s="26" t="s">
-        <v>66</v>
+      <c r="C2" s="27" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="27" t="s">
-        <v>67</v>
+      <c r="A3" s="28" t="s">
+        <v>71</v>
       </c>
-      <c r="B3" s="27" t="s">
-        <v>68</v>
+      <c r="B3" s="28" t="s">
+        <v>72</v>
       </c>
-      <c r="C3" s="27" t="s">
-        <v>69</v>
+      <c r="C3" s="28" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -14733,38 +15796,38 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="28" t="s">
-        <v>70</v>
+      <c r="A1" s="29" t="s">
+        <v>74</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="26" t="s">
-        <v>71</v>
+      <c r="A2" s="27" t="s">
+        <v>75</v>
       </c>
-      <c r="B2" s="26" t="s">
-        <v>72</v>
+      <c r="B2" s="27" t="s">
+        <v>76</v>
       </c>
-      <c r="C2" s="26" t="s">
-        <v>65</v>
+      <c r="C2" s="27" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="27" t="s">
-        <v>73</v>
+      <c r="A3" s="28" t="s">
+        <v>77</v>
       </c>
-      <c r="B3" s="27" t="s">
-        <v>74</v>
+      <c r="B3" s="28" t="s">
+        <v>78</v>
       </c>
-      <c r="C3" s="27" t="s">
-        <v>75</v>
+      <c r="C3" s="28" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="29"/>
-      <c r="B4" s="30"/>
-      <c r="C4" s="30"/>
+      <c r="A4" s="30"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -14798,38 +15861,38 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="31" t="s">
-        <v>76</v>
+      <c r="A1" s="32" t="s">
+        <v>80</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="26" t="s">
-        <v>77</v>
+      <c r="A2" s="27" t="s">
+        <v>81</v>
       </c>
-      <c r="B2" s="26" t="s">
-        <v>71</v>
+      <c r="B2" s="27" t="s">
+        <v>75</v>
       </c>
-      <c r="C2" s="26" t="s">
-        <v>78</v>
+      <c r="C2" s="27" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="11" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
-      <c r="C3" s="21" t="s">
-        <v>81</v>
+      <c r="C3" s="22" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="11"/>
-      <c r="B4" s="32"/>
-      <c r="C4" s="32"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -14863,38 +15926,38 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="31" t="s">
-        <v>82</v>
+      <c r="A1" s="32" t="s">
+        <v>86</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="26" t="s">
-        <v>77</v>
+      <c r="A2" s="27" t="s">
+        <v>81</v>
       </c>
-      <c r="B2" s="26" t="s">
-        <v>83</v>
+      <c r="B2" s="27" t="s">
+        <v>87</v>
       </c>
-      <c r="C2" s="26" t="s">
-        <v>78</v>
+      <c r="C2" s="27" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="11" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
-      <c r="C3" s="21" t="s">
-        <v>86</v>
+      <c r="C3" s="22" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="29"/>
-      <c r="B4" s="32"/>
-      <c r="C4" s="32"/>
+      <c r="A4" s="30"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -14928,36 +15991,36 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="31" t="s">
-        <v>87</v>
+      <c r="A1" s="32" t="s">
+        <v>91</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="8" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="11" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
-      <c r="C3" s="21" t="s">
-        <v>91</v>
+      <c r="C3" s="22" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="33"/>
+      <c r="A4" s="34"/>
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
     </row>
@@ -14993,36 +16056,36 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="31" t="s">
-        <v>92</v>
+      <c r="A1" s="32" t="s">
+        <v>96</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="8" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="11" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
-      <c r="C3" s="21" t="s">
-        <v>96</v>
+      <c r="C3" s="22" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="33"/>
+      <c r="A4" s="34"/>
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
     </row>

</xml_diff>

<commit_message>
code enhance for profile template
</commit_message>
<xml_diff>
--- a/webroot/export/customexcel/default_templates/profile_template.xlsx
+++ b/webroot/export/customexcel/default_templates/profile_template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190"/>
+    <workbookView xWindow="0" yWindow="495" windowWidth="20730" windowHeight="11760" tabRatio="933" firstSheet="1" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="196">
   <si>
     <t>${"image":{"displayValue":"Institutions.logo_content","imageWidth":"100","imageMarginLeft":"20","imageMarginTop":"5"}}</t>
   </si>
@@ -537,12 +537,90 @@
   <si>
     <t xml:space="preserve">${Institutions.date_opened} </t>
   </si>
+  <si>
+    <t>Grade 1</t>
+  </si>
+  <si>
+    <t>Grade 2</t>
+  </si>
+  <si>
+    <t>Grade 3</t>
+  </si>
+  <si>
+    <t>Grade 4</t>
+  </si>
+  <si>
+    <t>Education Grade/Area Administrative</t>
+  </si>
+  <si>
+    <t>Count of students</t>
+  </si>
+  <si>
+    <t>Count of Staff</t>
+  </si>
+  <si>
+    <t>Endor(sum of all staff in this country)</t>
+  </si>
+  <si>
+    <t>District 1(sum of all staff in this district)</t>
+  </si>
+  <si>
+    <t>District 1(sum of all student in this district)</t>
+  </si>
+  <si>
+    <t>North(sum of all student in this region)</t>
+  </si>
+  <si>
+    <t>Endor(sum of all student in this country)</t>
+  </si>
+  <si>
+    <t>${institution_staff_count.area_administrative}</t>
+  </si>
+  <si>
+    <t>${institution_student_count.area_administrative}</t>
+  </si>
+  <si>
+    <t>${institution_student_count.education_grade}</t>
+  </si>
+  <si>
+    <t>${institution_staff_count.education_grade}</t>
+  </si>
+  <si>
+    <t>&lt;--------------------</t>
+  </si>
+  <si>
+    <t>&lt;------------------</t>
+  </si>
+  <si>
+    <t>North(sum of all staff in this region)</t>
+  </si>
+  <si>
+    <t>District</t>
+  </si>
+  <si>
+    <t>${"match": {"displayValue": "InstitutionEducationGrade.name","rows": {"matchFrom": "InstitutionEducationGrade.id","matchTo": "InstitutionEducationGrade.id"}}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${"match": {"displayValue": "InstitutionStudentCount.district","type":"number","rows": {"matchFrom": "InstitutionEducationGrade.id","matchTo": "InstitutionEducationGrade.id"}}} </t>
+  </si>
+  <si>
+    <t>Region</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${"match": {"displayValue": "InstitutionStudentCount.region","type":"number","rows": {"matchFrom": "InstitutionEducationGrade.id","matchTo": "InstitutionEducationGrade.id"}}} </t>
+  </si>
+  <si>
+    <t xml:space="preserve">${"match": {"displayValue": "InstitutionStudentCount.country","type":"number","rows": {"matchFrom": "InstitutionEducationGrade.id","matchTo": "InstitutionEducationGrade.id"}}} </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -605,6 +683,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -620,7 +704,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -702,11 +786,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -794,6 +891,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -812,9 +919,6 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -889,6 +993,14 @@
       <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1179,11 +1291,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:IV1048"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView topLeftCell="A34" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="B57" sqref="B57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="63.140625" customWidth="1"/>
     <col min="2" max="2" width="54.28515625" customWidth="1"/>
@@ -1201,7 +1313,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:256" ht="15" customHeight="1">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="45" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4"/>
@@ -1222,13 +1334,13 @@
       <c r="Q1" s="7"/>
     </row>
     <row r="2" spans="1:256" ht="25.5" customHeight="1">
-      <c r="A2" s="39"/>
-      <c r="B2" s="40" t="s">
+      <c r="A2" s="45"/>
+      <c r="B2" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
       <c r="F2" s="8"/>
       <c r="G2" s="9"/>
       <c r="H2" s="7"/>
@@ -1482,13 +1594,13 @@
       <c r="IV2" s="3"/>
     </row>
     <row r="3" spans="1:256" ht="25.5" customHeight="1">
-      <c r="A3" s="39"/>
-      <c r="B3" s="41" t="s">
+      <c r="A3" s="45"/>
+      <c r="B3" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="41"/>
-      <c r="D3" s="41"/>
-      <c r="E3" s="41"/>
+      <c r="C3" s="47"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="47"/>
       <c r="F3" s="9"/>
       <c r="G3" s="9"/>
       <c r="H3" s="7"/>
@@ -1742,7 +1854,7 @@
       <c r="IV3" s="3"/>
     </row>
     <row r="4" spans="1:256" ht="22.5" customHeight="1">
-      <c r="A4" s="39"/>
+      <c r="A4" s="45"/>
       <c r="B4" s="4"/>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
@@ -4782,7 +4894,7 @@
       <c r="A22" s="11" t="s">
         <v>164</v>
       </c>
-      <c r="B22" s="46" t="s">
+      <c r="B22" s="40" t="s">
         <v>165</v>
       </c>
       <c r="C22" s="13"/>
@@ -5044,7 +5156,7 @@
       <c r="A23" s="11" t="s">
         <v>166</v>
       </c>
-      <c r="B23" s="46" t="s">
+      <c r="B23" s="40" t="s">
         <v>167</v>
       </c>
       <c r="C23" s="13"/>
@@ -5306,7 +5418,7 @@
       <c r="A24" s="11" t="s">
         <v>168</v>
       </c>
-      <c r="B24" s="46" t="s">
+      <c r="B24" s="40" t="s">
         <v>169</v>
       </c>
       <c r="C24" s="13"/>
@@ -5565,9 +5677,9 @@
       <c r="IV24" s="3"/>
     </row>
     <row r="25" spans="1:256" ht="12" customHeight="1">
-      <c r="A25" s="47"/>
-      <c r="B25" s="47"/>
-      <c r="C25" s="45"/>
+      <c r="A25" s="41"/>
+      <c r="B25" s="41"/>
+      <c r="C25" s="39"/>
       <c r="D25" s="18"/>
       <c r="E25" s="14"/>
       <c r="F25" s="14"/>
@@ -5823,9 +5935,9 @@
       <c r="IV25" s="3"/>
     </row>
     <row r="26" spans="1:256" ht="12" customHeight="1">
-      <c r="A26" s="47"/>
-      <c r="B26" s="47"/>
-      <c r="C26" s="45"/>
+      <c r="A26" s="41"/>
+      <c r="B26" s="41"/>
+      <c r="C26" s="39"/>
       <c r="D26" s="18"/>
       <c r="E26" s="14"/>
       <c r="F26" s="14"/>
@@ -19850,11 +19962,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView zoomScale="98" zoomScaleNormal="98" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="256" width="26.42578125" customWidth="1"/>
     <col min="257" max="1023" width="16.140625" customWidth="1"/>
@@ -19862,12 +19974,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="48" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="26" t="s">
@@ -19915,10 +20027,10 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="256" width="24.42578125" customWidth="1"/>
     <col min="257" max="1023" width="16.140625" customWidth="1"/>
@@ -19926,11 +20038,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="49" t="s">
         <v>79</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="26" t="s">
@@ -19980,7 +20092,7 @@
       <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="256" width="22.42578125" customWidth="1"/>
     <col min="257" max="1023" width="16.140625" customWidth="1"/>
@@ -19988,11 +20100,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="50" t="s">
         <v>85</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="26" t="s">
@@ -20038,11 +20150,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScalePageLayoutView="60" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScalePageLayoutView="60" workbookViewId="0">
       <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="256" width="22.42578125" customWidth="1"/>
     <col min="257" max="1023" width="16.140625" customWidth="1"/>
@@ -20050,11 +20162,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="50" t="s">
         <v>91</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="26" t="s">
@@ -20104,7 +20216,7 @@
       <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="256" width="22.42578125" customWidth="1"/>
     <col min="257" max="1023" width="16.140625" customWidth="1"/>
@@ -20112,11 +20224,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="50" t="s">
         <v>96</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="9" t="s">
@@ -20166,7 +20278,7 @@
       <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="256" width="22.42578125" customWidth="1"/>
     <col min="257" max="1023" width="16.140625" customWidth="1"/>
@@ -20174,11 +20286,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="50" t="s">
         <v>101</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="9" t="s">
@@ -20222,31 +20334,32 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T3"/>
+  <dimension ref="A1:T41"/>
   <sheetViews>
-    <sheetView zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1023" width="12.5703125" customWidth="1"/>
+    <col min="1" max="1" width="18.85546875" customWidth="1"/>
+    <col min="2" max="1023" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="50" t="s">
         <v>106</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="44"/>
-      <c r="J1" s="44"/>
-      <c r="K1" s="44"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="50"/>
+      <c r="I1" s="50"/>
+      <c r="J1" s="50"/>
+      <c r="K1" s="50"/>
       <c r="L1" s="30"/>
       <c r="M1" s="30"/>
       <c r="N1" s="30"/>
@@ -20381,6 +20494,239 @@
         <v>141</v>
       </c>
     </row>
+    <row r="15" spans="1:20">
+      <c r="A15" s="42" t="s">
+        <v>175</v>
+      </c>
+      <c r="B15" s="42"/>
+      <c r="C15" s="42"/>
+      <c r="D15" s="42"/>
+      <c r="E15" t="s">
+        <v>186</v>
+      </c>
+      <c r="F15" s="42" t="s">
+        <v>175</v>
+      </c>
+      <c r="G15" s="42"/>
+      <c r="H15" s="42"/>
+      <c r="I15" s="42"/>
+    </row>
+    <row r="16" spans="1:20">
+      <c r="A16" s="44" t="s">
+        <v>73</v>
+      </c>
+      <c r="B16" s="44" t="s">
+        <v>189</v>
+      </c>
+      <c r="C16" s="44" t="s">
+        <v>192</v>
+      </c>
+      <c r="D16" s="44" t="s">
+        <v>193</v>
+      </c>
+      <c r="F16" s="43" t="s">
+        <v>174</v>
+      </c>
+      <c r="G16" s="43" t="s">
+        <v>179</v>
+      </c>
+      <c r="H16" s="43" t="s">
+        <v>180</v>
+      </c>
+      <c r="I16" s="43" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" s="43" t="s">
+        <v>190</v>
+      </c>
+      <c r="B17" t="s">
+        <v>191</v>
+      </c>
+      <c r="C17" t="s">
+        <v>194</v>
+      </c>
+      <c r="D17" t="s">
+        <v>195</v>
+      </c>
+      <c r="F17" s="43" t="s">
+        <v>170</v>
+      </c>
+      <c r="G17" s="43">
+        <v>150</v>
+      </c>
+      <c r="H17" s="43">
+        <v>1500</v>
+      </c>
+      <c r="I17" s="43">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="F18" s="43" t="s">
+        <v>171</v>
+      </c>
+      <c r="G18" s="43">
+        <v>200</v>
+      </c>
+      <c r="H18" s="43">
+        <v>2000</v>
+      </c>
+      <c r="I18" s="43">
+        <v>45000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="F19" s="43" t="s">
+        <v>172</v>
+      </c>
+      <c r="G19" s="43">
+        <v>250</v>
+      </c>
+      <c r="H19" s="43">
+        <v>2500</v>
+      </c>
+      <c r="I19" s="43">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="F20" s="43" t="s">
+        <v>173</v>
+      </c>
+      <c r="G20" s="43">
+        <v>300</v>
+      </c>
+      <c r="H20" s="43">
+        <v>3000</v>
+      </c>
+      <c r="I20" s="43">
+        <v>60000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="F21" s="43"/>
+      <c r="G21" s="43"/>
+      <c r="H21" s="43"/>
+      <c r="I21" s="43"/>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="F23" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
+      <c r="F24" s="43" t="s">
+        <v>184</v>
+      </c>
+      <c r="G24" s="43"/>
+    </row>
+    <row r="30" spans="1:9">
+      <c r="E30" t="s">
+        <v>187</v>
+      </c>
+      <c r="F30" s="42" t="s">
+        <v>176</v>
+      </c>
+      <c r="G30" s="42"/>
+      <c r="H30" s="42"/>
+      <c r="I30" s="42"/>
+    </row>
+    <row r="31" spans="1:9">
+      <c r="F31" s="43" t="s">
+        <v>174</v>
+      </c>
+      <c r="G31" s="43" t="s">
+        <v>178</v>
+      </c>
+      <c r="H31" s="43" t="s">
+        <v>188</v>
+      </c>
+      <c r="I31" s="43" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9">
+      <c r="F32" s="43" t="s">
+        <v>170</v>
+      </c>
+      <c r="G32" s="43">
+        <v>30</v>
+      </c>
+      <c r="H32" s="43">
+        <v>300</v>
+      </c>
+      <c r="I32" s="43">
+        <v>3500</v>
+      </c>
+    </row>
+    <row r="33" spans="6:9">
+      <c r="F33" s="43" t="s">
+        <v>171</v>
+      </c>
+      <c r="G33" s="43">
+        <v>40</v>
+      </c>
+      <c r="H33" s="43">
+        <v>400</v>
+      </c>
+      <c r="I33" s="43">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="34" spans="6:9">
+      <c r="F34" s="43" t="s">
+        <v>172</v>
+      </c>
+      <c r="G34" s="43">
+        <v>50</v>
+      </c>
+      <c r="H34" s="43">
+        <v>500</v>
+      </c>
+      <c r="I34" s="43">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="35" spans="6:9">
+      <c r="F35" s="43" t="s">
+        <v>173</v>
+      </c>
+      <c r="G35" s="43">
+        <v>60</v>
+      </c>
+      <c r="H35" s="43">
+        <v>600</v>
+      </c>
+      <c r="I35" s="43">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="36" spans="6:9">
+      <c r="F36" s="43"/>
+      <c r="G36" s="43"/>
+      <c r="H36" s="43"/>
+      <c r="I36" s="43"/>
+    </row>
+    <row r="39" spans="6:9">
+      <c r="F39" s="42" t="s">
+        <v>176</v>
+      </c>
+      <c r="G39" s="42"/>
+    </row>
+    <row r="40" spans="6:9">
+      <c r="F40" s="43"/>
+      <c r="G40" s="43" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="41" spans="6:9">
+      <c r="F41" s="43" t="s">
+        <v>185</v>
+      </c>
+      <c r="G41" s="43"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:K1"/>

</xml_diff>

<commit_message>
code enhance for column name
</commit_message>
<xml_diff>
--- a/webroot/export/customexcel/default_templates/profile_template.xlsx
+++ b/webroot/export/customexcel/default_templates/profile_template.xlsx
@@ -595,13 +595,16 @@
     <t>North(sum of all staff in this region)</t>
   </si>
   <si>
-    <t>District</t>
-  </si>
-  <si>
     <t>${"match": {"displayValue": "InstitutionEducationGrade.name","rows": {"matchFrom": "InstitutionEducationGrade.id","matchTo": "InstitutionEducationGrade.id"}}}</t>
   </si>
   <si>
     <t xml:space="preserve">${"match": {"displayValue": "InstitutionStudentCount.district","type":"number","rows": {"matchFrom": "InstitutionEducationGrade.id","matchTo": "InstitutionEducationGrade.id"}}} </t>
+  </si>
+  <si>
+    <t xml:space="preserve">${"match": {"displayValue": "InstitutionStudentCount.region","type":"number","rows": {"matchFrom": "InstitutionEducationGrade.id","matchTo": "InstitutionEducationGrade.id"}}} </t>
+  </si>
+  <si>
+    <t xml:space="preserve">${"match": {"displayValue": "InstitutionStudentCount.country","type":"number","rows": {"matchFrom": "InstitutionEducationGrade.id","matchTo": "InstitutionEducationGrade.id"}}} </t>
   </si>
   <si>
     <t>Region</t>
@@ -610,10 +613,7 @@
     <t>Country</t>
   </si>
   <si>
-    <t xml:space="preserve">${"match": {"displayValue": "InstitutionStudentCount.region","type":"number","rows": {"matchFrom": "InstitutionEducationGrade.id","matchTo": "InstitutionEducationGrade.id"}}} </t>
-  </si>
-  <si>
-    <t xml:space="preserve">${"match": {"displayValue": "InstitutionStudentCount.country","type":"number","rows": {"matchFrom": "InstitutionEducationGrade.id","matchTo": "InstitutionEducationGrade.id"}}} </t>
+    <t xml:space="preserve">${"match": {"displayValue": "InstitutionStudentCount.district_name","columns": {"matchFrom": "InstitutionEducationGrade.id","matchTo": "InstitutionEducationGrade.id"}}} </t>
   </si>
 </sst>
 </file>
@@ -20336,8 +20336,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:T41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
@@ -20516,13 +20516,13 @@
         <v>73</v>
       </c>
       <c r="B16" s="44" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
       <c r="C16" s="44" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="D16" s="44" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="F16" s="43" t="s">
         <v>174</v>
@@ -20539,16 +20539,16 @@
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="43" t="s">
+        <v>189</v>
+      </c>
+      <c r="B17" t="s">
         <v>190</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>191</v>
       </c>
-      <c r="C17" t="s">
-        <v>194</v>
-      </c>
       <c r="D17" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="F17" s="43" t="s">
         <v>170</v>

</xml_diff>

<commit_message>
code enahnce for student and staff count
</commit_message>
<xml_diff>
--- a/webroot/export/customexcel/default_templates/profile_template.xlsx
+++ b/webroot/export/customexcel/default_templates/profile_template.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="187">
   <si>
     <t>${"image":{"displayValue":"Institutions.logo_content","imageWidth":"100","imageMarginLeft":"20","imageMarginTop":"5"}}</t>
   </si>
@@ -538,82 +538,55 @@
     <t xml:space="preserve">${Institutions.date_opened} </t>
   </si>
   <si>
-    <t>Grade 1</t>
-  </si>
-  <si>
-    <t>Grade 2</t>
-  </si>
-  <si>
-    <t>Grade 3</t>
-  </si>
-  <si>
-    <t>Grade 4</t>
-  </si>
-  <si>
-    <t>Education Grade/Area Administrative</t>
-  </si>
-  <si>
-    <t>Count of students</t>
-  </si>
-  <si>
     <t>Count of Staff</t>
-  </si>
-  <si>
-    <t>Endor(sum of all staff in this country)</t>
-  </si>
-  <si>
-    <t>District 1(sum of all staff in this district)</t>
-  </si>
-  <si>
-    <t>District 1(sum of all student in this district)</t>
-  </si>
-  <si>
-    <t>North(sum of all student in this region)</t>
-  </si>
-  <si>
-    <t>Endor(sum of all student in this country)</t>
-  </si>
-  <si>
-    <t>${institution_staff_count.area_administrative}</t>
-  </si>
-  <si>
-    <t>${institution_student_count.area_administrative}</t>
-  </si>
-  <si>
-    <t>${institution_student_count.education_grade}</t>
-  </si>
-  <si>
-    <t>${institution_staff_count.education_grade}</t>
-  </si>
-  <si>
-    <t>&lt;--------------------</t>
-  </si>
-  <si>
-    <t>&lt;------------------</t>
-  </si>
-  <si>
-    <t>North(sum of all staff in this region)</t>
   </si>
   <si>
     <t>${"match": {"displayValue": "InstitutionEducationGrade.name","rows": {"matchFrom": "InstitutionEducationGrade.id","matchTo": "InstitutionEducationGrade.id"}}}</t>
   </si>
   <si>
-    <t xml:space="preserve">${"match": {"displayValue": "InstitutionStudentCount.district","type":"number","rows": {"matchFrom": "InstitutionEducationGrade.id","matchTo": "InstitutionEducationGrade.id"}}} </t>
+    <t xml:space="preserve">${"match": {"displayValue": "InstitutionStudentEnrolled.area_level:1","rows": {"matchFrom": "InstitutionEducationGrade.id","matchTo": "InstitutionEducationGrade.id"}}} </t>
   </si>
   <si>
-    <t xml:space="preserve">${"match": {"displayValue": "InstitutionStudentCount.region","type":"number","rows": {"matchFrom": "InstitutionEducationGrade.id","matchTo": "InstitutionEducationGrade.id"}}} </t>
+    <t xml:space="preserve">${"match": {"displayValue": "InstitutionStudentEnrolled.area_level:2","rows": {"matchFrom": "InstitutionEducationGrade.id","matchTo": "InstitutionEducationGrade.id"}}} </t>
   </si>
   <si>
-    <t xml:space="preserve">${"match": {"displayValue": "InstitutionStudentCount.country","type":"number","rows": {"matchFrom": "InstitutionEducationGrade.id","matchTo": "InstitutionEducationGrade.id"}}} </t>
+    <t xml:space="preserve">${"match": {"displayValue": "InstitutionStudentEnrolled.area_level:3","rows": {"matchFrom": "InstitutionEducationGrade.id","matchTo": "InstitutionEducationGrade.id"}}} </t>
   </si>
   <si>
-    <t>Region</t>
+    <t>Count of  Withdrawn students</t>
   </si>
   <si>
-    <t>Country</t>
+    <t>Count of  Enrolled students</t>
   </si>
   <si>
-    <t xml:space="preserve">${"match": {"displayValue": "InstitutionStudentCount.district_name","columns": {"matchFrom": "InstitutionEducationGrade.id","matchTo": "InstitutionEducationGrade.id"}}} </t>
+    <t xml:space="preserve">${"match": {"displayValue": "InstitutionStudentWithdrawn.area_level:1","rows": {"matchFrom": "InstitutionEducationGrade.id","matchTo": "InstitutionEducationGrade.id"}}} </t>
+  </si>
+  <si>
+    <t xml:space="preserve">${"match": {"displayValue": "InstitutionStudentWithdrawn.area_level:2","rows": {"matchFrom": "InstitutionEducationGrade.id","matchTo": "InstitutionEducationGrade.id"}}} </t>
+  </si>
+  <si>
+    <t xml:space="preserve">${"match": {"displayValue": "InstitutionStudentWithdrawn.area_level:3","rows": {"matchFrom": "InstitutionEducationGrade.id","matchTo": "InstitutionEducationGrade.id"}}} </t>
+  </si>
+  <si>
+    <t>Count of Transferred students</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${"match": {"displayValue": "InstitutionStudentTransferred.area_level:1","rows": {"matchFrom": "InstitutionEducationGrade.id","matchTo": "InstitutionEducationGrade.id"}}} </t>
+  </si>
+  <si>
+    <t xml:space="preserve">${"match": {"displayValue": "InstitutionStudentTransferred.area_level:2","rows": {"matchFrom": "InstitutionEducationGrade.id","matchTo": "InstitutionEducationGrade.id"}}} </t>
+  </si>
+  <si>
+    <t xml:space="preserve">${"match": {"displayValue": "InstitutionStudentTransferred.area_level:3","rows": {"matchFrom": "InstitutionEducationGrade.id","matchTo": "InstitutionEducationGrade.id"}}} </t>
+  </si>
+  <si>
+    <t xml:space="preserve">${"match": {"displayValue": "InstitutionStaffCount.area_level:1","rows": {"matchFrom": "InstitutionEducationGrade.id","matchTo": "InstitutionEducationGrade.id"}}} </t>
+  </si>
+  <si>
+    <t xml:space="preserve">${"match": {"displayValue": "InstitutionStaffCount.area_level:2","rows": {"matchFrom": "InstitutionEducationGrade.id","matchTo": "InstitutionEducationGrade.id"}}} </t>
+  </si>
+  <si>
+    <t xml:space="preserve">${"match": {"displayValue": "InstitutionStaffCount.area_level:3","rows": {"matchFrom": "InstitutionEducationGrade.id","matchTo": "InstitutionEducationGrade.id"}}} </t>
   </si>
 </sst>
 </file>
@@ -20334,10 +20307,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T41"/>
+  <dimension ref="A1:T59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
@@ -20496,236 +20469,91 @@
     </row>
     <row r="15" spans="1:20">
       <c r="A15" s="42" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B15" s="42"/>
       <c r="C15" s="42"/>
       <c r="D15" s="42"/>
-      <c r="E15" t="s">
-        <v>186</v>
+    </row>
+    <row r="16" spans="1:20">
+      <c r="A16" s="43" t="s">
+        <v>171</v>
       </c>
-      <c r="F15" s="42" t="s">
+      <c r="B16" s="44" t="s">
+        <v>172</v>
+      </c>
+      <c r="C16" s="44" t="s">
+        <v>173</v>
+      </c>
+      <c r="D16" s="44" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="42" t="s">
         <v>175</v>
       </c>
-      <c r="G15" s="42"/>
-      <c r="H15" s="42"/>
-      <c r="I15" s="42"/>
+      <c r="B28" s="42"/>
+      <c r="C28" s="42"/>
+      <c r="D28" s="42"/>
     </row>
-    <row r="16" spans="1:20">
-      <c r="A16" s="44" t="s">
-        <v>73</v>
+    <row r="29" spans="1:4">
+      <c r="A29" s="43" t="s">
+        <v>171</v>
       </c>
-      <c r="B16" s="44" t="s">
-        <v>195</v>
+      <c r="B29" s="44" t="s">
+        <v>177</v>
       </c>
-      <c r="C16" s="44" t="s">
-        <v>193</v>
+      <c r="C29" s="44" t="s">
+        <v>178</v>
       </c>
-      <c r="D16" s="44" t="s">
-        <v>194</v>
-      </c>
-      <c r="F16" s="43" t="s">
-        <v>174</v>
-      </c>
-      <c r="G16" s="43" t="s">
+      <c r="D29" s="44" t="s">
         <v>179</v>
       </c>
-      <c r="H16" s="43" t="s">
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" s="42" t="s">
         <v>180</v>
       </c>
-      <c r="I16" s="43" t="s">
+      <c r="B44" s="42"/>
+      <c r="C44" s="42"/>
+      <c r="D44" s="42"/>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" s="43" t="s">
+        <v>171</v>
+      </c>
+      <c r="B45" s="44" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="17" spans="1:9">
-      <c r="A17" s="43" t="s">
-        <v>189</v>
+      <c r="C45" s="44" t="s">
+        <v>182</v>
       </c>
-      <c r="B17" t="s">
-        <v>190</v>
-      </c>
-      <c r="C17" t="s">
-        <v>191</v>
-      </c>
-      <c r="D17" t="s">
-        <v>192</v>
-      </c>
-      <c r="F17" s="43" t="s">
-        <v>170</v>
-      </c>
-      <c r="G17" s="43">
-        <v>150</v>
-      </c>
-      <c r="H17" s="43">
-        <v>1500</v>
-      </c>
-      <c r="I17" s="43">
-        <v>40000</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9">
-      <c r="F18" s="43" t="s">
-        <v>171</v>
-      </c>
-      <c r="G18" s="43">
-        <v>200</v>
-      </c>
-      <c r="H18" s="43">
-        <v>2000</v>
-      </c>
-      <c r="I18" s="43">
-        <v>45000</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9">
-      <c r="F19" s="43" t="s">
-        <v>172</v>
-      </c>
-      <c r="G19" s="43">
-        <v>250</v>
-      </c>
-      <c r="H19" s="43">
-        <v>2500</v>
-      </c>
-      <c r="I19" s="43">
-        <v>50000</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9">
-      <c r="F20" s="43" t="s">
-        <v>173</v>
-      </c>
-      <c r="G20" s="43">
-        <v>300</v>
-      </c>
-      <c r="H20" s="43">
-        <v>3000</v>
-      </c>
-      <c r="I20" s="43">
-        <v>60000</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9">
-      <c r="F21" s="43"/>
-      <c r="G21" s="43"/>
-      <c r="H21" s="43"/>
-      <c r="I21" s="43"/>
-    </row>
-    <row r="23" spans="1:9">
-      <c r="F23" t="s">
+      <c r="D45" s="44" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
-      <c r="F24" s="43" t="s">
+    <row r="58" spans="1:4">
+      <c r="A58" s="42" t="s">
+        <v>170</v>
+      </c>
+      <c r="B58" s="42"/>
+      <c r="C58" s="42"/>
+      <c r="D58" s="42"/>
+    </row>
+    <row r="59" spans="1:4">
+      <c r="A59" s="43" t="s">
+        <v>171</v>
+      </c>
+      <c r="B59" s="44" t="s">
         <v>184</v>
       </c>
-      <c r="G24" s="43"/>
-    </row>
-    <row r="30" spans="1:9">
-      <c r="E30" t="s">
-        <v>187</v>
-      </c>
-      <c r="F30" s="42" t="s">
-        <v>176</v>
-      </c>
-      <c r="G30" s="42"/>
-      <c r="H30" s="42"/>
-      <c r="I30" s="42"/>
-    </row>
-    <row r="31" spans="1:9">
-      <c r="F31" s="43" t="s">
-        <v>174</v>
-      </c>
-      <c r="G31" s="43" t="s">
-        <v>178</v>
-      </c>
-      <c r="H31" s="43" t="s">
-        <v>188</v>
-      </c>
-      <c r="I31" s="43" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9">
-      <c r="F32" s="43" t="s">
-        <v>170</v>
-      </c>
-      <c r="G32" s="43">
-        <v>30</v>
-      </c>
-      <c r="H32" s="43">
-        <v>300</v>
-      </c>
-      <c r="I32" s="43">
-        <v>3500</v>
-      </c>
-    </row>
-    <row r="33" spans="6:9">
-      <c r="F33" s="43" t="s">
-        <v>171</v>
-      </c>
-      <c r="G33" s="43">
-        <v>40</v>
-      </c>
-      <c r="H33" s="43">
-        <v>400</v>
-      </c>
-      <c r="I33" s="43">
-        <v>4000</v>
-      </c>
-    </row>
-    <row r="34" spans="6:9">
-      <c r="F34" s="43" t="s">
-        <v>172</v>
-      </c>
-      <c r="G34" s="43">
-        <v>50</v>
-      </c>
-      <c r="H34" s="43">
-        <v>500</v>
-      </c>
-      <c r="I34" s="43">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="35" spans="6:9">
-      <c r="F35" s="43" t="s">
-        <v>173</v>
-      </c>
-      <c r="G35" s="43">
-        <v>60</v>
-      </c>
-      <c r="H35" s="43">
-        <v>600</v>
-      </c>
-      <c r="I35" s="43">
-        <v>6000</v>
-      </c>
-    </row>
-    <row r="36" spans="6:9">
-      <c r="F36" s="43"/>
-      <c r="G36" s="43"/>
-      <c r="H36" s="43"/>
-      <c r="I36" s="43"/>
-    </row>
-    <row r="39" spans="6:9">
-      <c r="F39" s="42" t="s">
-        <v>176</v>
-      </c>
-      <c r="G39" s="42"/>
-    </row>
-    <row r="40" spans="6:9">
-      <c r="F40" s="43"/>
-      <c r="G40" s="43" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="41" spans="6:9">
-      <c r="F41" s="43" t="s">
+      <c r="C59" s="44" t="s">
         <v>185</v>
       </c>
-      <c r="G41" s="43"/>
+      <c r="D59" s="44" t="s">
+        <v>186</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
code enahnce for infrastructure rooms
</commit_message>
<xml_diff>
--- a/webroot/export/customexcel/default_templates/profile_template.xlsx
+++ b/webroot/export/customexcel/default_templates/profile_template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="495" windowWidth="20730" windowHeight="11760" tabRatio="933" firstSheet="1" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="495" windowWidth="20730" windowHeight="11760" tabRatio="933" firstSheet="4" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,15 @@
   </sheets>
   <calcPr calcId="124519"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
     </ext>
@@ -26,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="192">
   <si>
     <t>${"image":{"displayValue":"Institutions.logo_content","imageWidth":"100","imageMarginLeft":"20","imageMarginTop":"5"}}</t>
   </si>
@@ -588,6 +597,21 @@
   <si>
     <t xml:space="preserve">${"match": {"displayValue": "InstitutionStaffCount.area_level:3","rows": {"matchFrom": "InstitutionEducationGrade.id","matchTo": "InstitutionEducationGrade.id"}}} </t>
   </si>
+  <si>
+    <t>Count of Infrastructure Room Types</t>
+  </si>
+  <si>
+    <t>${"match": {"displayValue": "InstitutionRoomTypes.name","rows": {"matchFrom": "InstitutionRoomTypes.id","matchTo": "InstitutionRoomTypes.id"}}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${"match": {"displayValue": "InstitutionRoomTypesCount.area_level:1","rows": {"matchFrom": "InstitutionRoomTypes.id","matchTo": "InstitutionRoomTypes.id"}}} </t>
+  </si>
+  <si>
+    <t xml:space="preserve">${"match": {"displayValue": "InstitutionRoomTypesCount.area_level:2","rows": {"matchFrom": "InstitutionRoomTypes.id","matchTo": "InstitutionRoomTypes.id"}}} </t>
+  </si>
+  <si>
+    <t xml:space="preserve">${"match": {"displayValue": "InstitutionRoomTypesCount.area_level:3","rows": {"matchFrom": "InstitutionRoomTypes.id","matchTo": "InstitutionRoomTypes.id"}}} </t>
+  </si>
 </sst>
 </file>
 
@@ -637,6 +661,7 @@
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -661,6 +686,7 @@
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -776,7 +802,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -872,6 +898,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1286,7 +1315,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:256" ht="15" customHeight="1">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="46" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4"/>
@@ -1307,13 +1336,13 @@
       <c r="Q1" s="7"/>
     </row>
     <row r="2" spans="1:256" ht="25.5" customHeight="1">
-      <c r="A2" s="45"/>
-      <c r="B2" s="46" t="s">
+      <c r="A2" s="46"/>
+      <c r="B2" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
       <c r="F2" s="8"/>
       <c r="G2" s="9"/>
       <c r="H2" s="7"/>
@@ -1567,13 +1596,13 @@
       <c r="IV2" s="3"/>
     </row>
     <row r="3" spans="1:256" ht="25.5" customHeight="1">
-      <c r="A3" s="45"/>
-      <c r="B3" s="47" t="s">
+      <c r="A3" s="46"/>
+      <c r="B3" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="47"/>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47"/>
+      <c r="C3" s="48"/>
+      <c r="D3" s="48"/>
+      <c r="E3" s="48"/>
       <c r="F3" s="9"/>
       <c r="G3" s="9"/>
       <c r="H3" s="7"/>
@@ -1827,7 +1856,7 @@
       <c r="IV3" s="3"/>
     </row>
     <row r="4" spans="1:256" ht="22.5" customHeight="1">
-      <c r="A4" s="45"/>
+      <c r="A4" s="46"/>
       <c r="B4" s="4"/>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
@@ -19947,12 +19976,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="49" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="26" t="s">
@@ -20011,11 +20040,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="50" t="s">
         <v>79</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="26" t="s">
@@ -20073,11 +20102,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="51" t="s">
         <v>85</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="26" t="s">
@@ -20135,11 +20164,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="51" t="s">
         <v>91</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="26" t="s">
@@ -20197,11 +20226,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="51" t="s">
         <v>96</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="9" t="s">
@@ -20259,11 +20288,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="51" t="s">
         <v>101</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="9" t="s">
@@ -20307,10 +20336,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T59"/>
+  <dimension ref="A1:T81"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" topLeftCell="A57" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="D81" sqref="D81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
@@ -20320,19 +20349,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="51" t="s">
         <v>106</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
-      <c r="J1" s="50"/>
-      <c r="K1" s="50"/>
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
+      <c r="G1" s="51"/>
+      <c r="H1" s="51"/>
+      <c r="I1" s="51"/>
+      <c r="J1" s="51"/>
+      <c r="K1" s="51"/>
       <c r="L1" s="30"/>
       <c r="M1" s="30"/>
       <c r="N1" s="30"/>
@@ -20555,6 +20584,28 @@
         <v>186</v>
       </c>
     </row>
+    <row r="80" spans="1:4">
+      <c r="A80" s="42" t="s">
+        <v>187</v>
+      </c>
+      <c r="B80" s="42"/>
+      <c r="C80" s="42"/>
+      <c r="D80" s="42"/>
+    </row>
+    <row r="81" spans="1:4">
+      <c r="A81" s="43" t="s">
+        <v>188</v>
+      </c>
+      <c r="B81" s="45" t="s">
+        <v>189</v>
+      </c>
+      <c r="C81" s="45" t="s">
+        <v>190</v>
+      </c>
+      <c r="D81" s="45" t="s">
+        <v>191</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:K1"/>

</xml_diff>

<commit_message>
code enhance for non teaching
</commit_message>
<xml_diff>
--- a/webroot/export/customexcel/default_templates/profile_template.xlsx
+++ b/webroot/export/customexcel/default_templates/profile_template.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="197">
   <si>
     <t>${"image":{"displayValue":"Institutions.logo_content","imageWidth":"100","imageMarginLeft":"20","imageMarginTop":"5"}}</t>
   </si>
@@ -612,6 +612,21 @@
   <si>
     <t xml:space="preserve">${"match": {"displayValue": "InstitutionRoomTypesCount.area_level:3","rows": {"matchFrom": "InstitutionRoomTypes.id","matchTo": "InstitutionRoomTypes.id"}}} </t>
   </si>
+  <si>
+    <t>Number of Non-teaching Staff by Area</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${"match": {"displayValue": "NonTeachingStaffCount.area_level:1","rows": {"matchFrom": "staff_position_titles.type","matchTo": "staff_position_titles.type"}}} </t>
+  </si>
+  <si>
+    <t xml:space="preserve">${"match": {"displayValue": "NonTeachingStaffCount.area_level:2","rows": {"matchFrom": "staff_position_titles.type","matchTo": "staff_position_titles.type"}}} </t>
+  </si>
+  <si>
+    <t xml:space="preserve">${"match": {"displayValue": "NonTeachingStaffCount.area_level:3","rows": {"matchFrom": "staff_position_titles.type","matchTo": "staff_position_titles.type"}}} </t>
+  </si>
+  <si>
+    <t>${"match": {"displayValue": "InstitutionAreaName.name","rows": {"matchFrom": "InstitutionAreaName.id","matchTo": "InstitutionAreaName.id"}}}</t>
+  </si>
 </sst>
 </file>
 
@@ -703,7 +718,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -798,11 +813,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -903,6 +938,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -920,6 +958,15 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1315,7 +1362,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:256" ht="15" customHeight="1">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4"/>
@@ -1336,13 +1383,13 @@
       <c r="Q1" s="7"/>
     </row>
     <row r="2" spans="1:256" ht="25.5" customHeight="1">
-      <c r="A2" s="46"/>
-      <c r="B2" s="47" t="s">
+      <c r="A2" s="47"/>
+      <c r="B2" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
       <c r="F2" s="8"/>
       <c r="G2" s="9"/>
       <c r="H2" s="7"/>
@@ -1596,13 +1643,13 @@
       <c r="IV2" s="3"/>
     </row>
     <row r="3" spans="1:256" ht="25.5" customHeight="1">
-      <c r="A3" s="46"/>
-      <c r="B3" s="48" t="s">
+      <c r="A3" s="47"/>
+      <c r="B3" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="48"/>
-      <c r="D3" s="48"/>
-      <c r="E3" s="48"/>
+      <c r="C3" s="49"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
       <c r="F3" s="9"/>
       <c r="G3" s="9"/>
       <c r="H3" s="7"/>
@@ -1856,7 +1903,7 @@
       <c r="IV3" s="3"/>
     </row>
     <row r="4" spans="1:256" ht="22.5" customHeight="1">
-      <c r="A4" s="46"/>
+      <c r="A4" s="47"/>
       <c r="B4" s="4"/>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
@@ -19976,12 +20023,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="50" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="26" t="s">
@@ -20040,11 +20087,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="51" t="s">
         <v>79</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="26" t="s">
@@ -20102,11 +20149,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="52" t="s">
         <v>85</v>
       </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="51"/>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="26" t="s">
@@ -20164,11 +20211,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="52" t="s">
         <v>91</v>
       </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="51"/>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="26" t="s">
@@ -20226,11 +20273,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="52" t="s">
         <v>96</v>
       </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="51"/>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="9" t="s">
@@ -20288,11 +20335,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="52" t="s">
         <v>101</v>
       </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="51"/>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="9" t="s">
@@ -20336,10 +20383,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T81"/>
+  <dimension ref="A1:T95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="D81" sqref="D81"/>
+    <sheetView tabSelected="1" topLeftCell="A79" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="A95" sqref="A95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
@@ -20349,19 +20396,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="52" t="s">
         <v>106</v>
       </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
-      <c r="G1" s="51"/>
-      <c r="H1" s="51"/>
-      <c r="I1" s="51"/>
-      <c r="J1" s="51"/>
-      <c r="K1" s="51"/>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="52"/>
+      <c r="H1" s="52"/>
+      <c r="I1" s="52"/>
+      <c r="J1" s="52"/>
+      <c r="K1" s="52"/>
       <c r="L1" s="30"/>
       <c r="M1" s="30"/>
       <c r="N1" s="30"/>
@@ -20606,9 +20653,32 @@
         <v>191</v>
       </c>
     </row>
+    <row r="94" spans="1:4">
+      <c r="A94" s="53" t="s">
+        <v>192</v>
+      </c>
+      <c r="B94" s="54"/>
+      <c r="C94" s="54"/>
+      <c r="D94" s="55"/>
+    </row>
+    <row r="95" spans="1:4">
+      <c r="A95" s="43" t="s">
+        <v>196</v>
+      </c>
+      <c r="B95" s="46" t="s">
+        <v>193</v>
+      </c>
+      <c r="C95" s="46" t="s">
+        <v>194</v>
+      </c>
+      <c r="D95" s="46" t="s">
+        <v>195</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A94:D94"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
code enhane for non teaching staff
</commit_message>
<xml_diff>
--- a/webroot/export/customexcel/default_templates/profile_template.xlsx
+++ b/webroot/export/customexcel/default_templates/profile_template.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="195">
   <si>
     <t>${"image":{"displayValue":"Institutions.logo_content","imageWidth":"100","imageMarginLeft":"20","imageMarginTop":"5"}}</t>
   </si>
@@ -616,16 +616,10 @@
     <t>Number of Non-teaching Staff by Area</t>
   </si>
   <si>
-    <t xml:space="preserve">${"match": {"displayValue": "NonTeachingStaffCount.area_level:1","rows": {"matchFrom": "staff_position_titles.type","matchTo": "staff_position_titles.type"}}} </t>
+    <t>${"match": {"displayValue": "InstitutionAreaName.name","rows": {"matchFrom": "InstitutionAreaName.id","matchTo": "InstitutionAreaName.id"}}}</t>
   </si>
   <si>
-    <t xml:space="preserve">${"match": {"displayValue": "NonTeachingStaffCount.area_level:2","rows": {"matchFrom": "staff_position_titles.type","matchTo": "staff_position_titles.type"}}} </t>
-  </si>
-  <si>
-    <t xml:space="preserve">${"match": {"displayValue": "NonTeachingStaffCount.area_level:3","rows": {"matchFrom": "staff_position_titles.type","matchTo": "staff_position_titles.type"}}} </t>
-  </si>
-  <si>
-    <t>${"match": {"displayValue": "InstitutionAreaName.name","rows": {"matchFrom": "InstitutionAreaName.id","matchTo": "InstitutionAreaName.id"}}}</t>
+    <t xml:space="preserve">${"match": {"displayValue": "NonTeachingStaffCount.area_level","rows": {"matchFrom": "InstitutionAreaName.id","matchTo": "InstitutionAreaName.id"}}} </t>
   </si>
 </sst>
 </file>
@@ -718,7 +712,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -822,22 +816,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -938,9 +921,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -959,14 +939,14 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1362,7 +1342,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:256" ht="15" customHeight="1">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="46" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4"/>
@@ -1383,13 +1363,13 @@
       <c r="Q1" s="7"/>
     </row>
     <row r="2" spans="1:256" ht="25.5" customHeight="1">
-      <c r="A2" s="47"/>
-      <c r="B2" s="48" t="s">
+      <c r="A2" s="46"/>
+      <c r="B2" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="48"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
       <c r="F2" s="8"/>
       <c r="G2" s="9"/>
       <c r="H2" s="7"/>
@@ -1643,13 +1623,13 @@
       <c r="IV2" s="3"/>
     </row>
     <row r="3" spans="1:256" ht="25.5" customHeight="1">
-      <c r="A3" s="47"/>
-      <c r="B3" s="49" t="s">
+      <c r="A3" s="46"/>
+      <c r="B3" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="49"/>
-      <c r="D3" s="49"/>
-      <c r="E3" s="49"/>
+      <c r="C3" s="48"/>
+      <c r="D3" s="48"/>
+      <c r="E3" s="48"/>
       <c r="F3" s="9"/>
       <c r="G3" s="9"/>
       <c r="H3" s="7"/>
@@ -1903,7 +1883,7 @@
       <c r="IV3" s="3"/>
     </row>
     <row r="4" spans="1:256" ht="22.5" customHeight="1">
-      <c r="A4" s="47"/>
+      <c r="A4" s="46"/>
       <c r="B4" s="4"/>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
@@ -20023,12 +20003,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="49" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="26" t="s">
@@ -20087,11 +20067,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="50" t="s">
         <v>79</v>
       </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="51"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="26" t="s">
@@ -20149,11 +20129,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="51" t="s">
         <v>85</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="26" t="s">
@@ -20211,11 +20191,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="51" t="s">
         <v>91</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="26" t="s">
@@ -20273,11 +20253,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="51" t="s">
         <v>96</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="9" t="s">
@@ -20335,11 +20315,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="51" t="s">
         <v>101</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="9" t="s">
@@ -20383,32 +20363,33 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T95"/>
+  <dimension ref="A1:T94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="A95" sqref="A95"/>
+    <sheetView tabSelected="1" topLeftCell="A67" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="C93" sqref="C93:D93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="18.85546875" customWidth="1"/>
-    <col min="2" max="1023" width="12.42578125" customWidth="1"/>
+    <col min="2" max="2" width="31.5703125" customWidth="1"/>
+    <col min="3" max="1023" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="51" t="s">
         <v>106</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
-      <c r="I1" s="52"/>
-      <c r="J1" s="52"/>
-      <c r="K1" s="52"/>
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
+      <c r="G1" s="51"/>
+      <c r="H1" s="51"/>
+      <c r="I1" s="51"/>
+      <c r="J1" s="51"/>
+      <c r="K1" s="51"/>
       <c r="L1" s="30"/>
       <c r="M1" s="30"/>
       <c r="N1" s="30"/>
@@ -20653,35 +20634,29 @@
         <v>191</v>
       </c>
     </row>
-    <row r="94" spans="1:4">
-      <c r="A94" s="53" t="s">
+    <row r="93" spans="1:4">
+      <c r="A93" s="53" t="s">
         <v>192</v>
       </c>
-      <c r="B94" s="54"/>
-      <c r="C94" s="54"/>
-      <c r="D94" s="55"/>
+      <c r="B93" s="54"/>
+      <c r="C93" s="42"/>
+      <c r="D93" s="42"/>
     </row>
-    <row r="95" spans="1:4">
-      <c r="A95" s="43" t="s">
-        <v>196</v>
-      </c>
-      <c r="B95" s="46" t="s">
+    <row r="94" spans="1:4" ht="60">
+      <c r="A94" s="43" t="s">
         <v>193</v>
       </c>
-      <c r="C95" s="46" t="s">
+      <c r="B94" s="52" t="s">
         <v>194</v>
-      </c>
-      <c r="D95" s="46" t="s">
-        <v>195</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A94:D94"/>
+    <mergeCell ref="A93:B93"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>

</xml_diff>

<commit_message>
POCOR-6519 : code enhance for institution custom fields | status: in progress
</commit_message>
<xml_diff>
--- a/webroot/export/customexcel/default_templates/profile_template.xlsx
+++ b/webroot/export/customexcel/default_templates/profile_template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="495" windowWidth="20730" windowHeight="11760" tabRatio="933" firstSheet="4" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="495" windowWidth="20730" windowHeight="11760" tabRatio="933"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="203">
   <si>
     <t>${"image":{"displayValue":"Institutions.logo_content","imageWidth":"100","imageMarginLeft":"20","imageMarginTop":"5"}}</t>
   </si>
@@ -621,6 +621,30 @@
   <si>
     <t xml:space="preserve">${"match": {"displayValue": "NonTeachingStaffCount.area_level","rows": {"matchFrom": "InstitutionAreaName.id","matchTo": "InstitutionAreaName.id"}}} </t>
   </si>
+  <si>
+    <t>Institution Custom Fields</t>
+  </si>
+  <si>
+    <t>Fields</t>
+  </si>
+  <si>
+    <t>Values</t>
+  </si>
+  <si>
+    <t>${"match": {"displayValue": "InstitutionCustomFields.name","rows": {"matchFrom": "InstitutionCustomFields.id","matchTo": "InstitutionCustomFields.id"}}}</t>
+  </si>
+  <si>
+    <t>${"match": {"displayValue": "InstitutionCustomFieldValues.data","rows": {"matchFrom": "InstitutionCustomFieldValues.id","matchTo": "InstitutionCustomFieldValues.id"}}}</t>
+  </si>
+  <si>
+    <t>Infrastructure Room Custom Fields</t>
+  </si>
+  <si>
+    <t>Question</t>
+  </si>
+  <si>
+    <t>Answer</t>
+  </si>
 </sst>
 </file>
 
@@ -921,6 +945,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -938,9 +965,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1320,8 +1344,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:IV1048"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="B57" sqref="B57"/>
+    <sheetView tabSelected="1" topLeftCell="A77" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="B86" sqref="B86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75"/>
@@ -1342,7 +1366,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:256" ht="15" customHeight="1">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4"/>
@@ -1363,13 +1387,13 @@
       <c r="Q1" s="7"/>
     </row>
     <row r="2" spans="1:256" ht="25.5" customHeight="1">
-      <c r="A2" s="46"/>
-      <c r="B2" s="47" t="s">
+      <c r="A2" s="47"/>
+      <c r="B2" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
       <c r="F2" s="8"/>
       <c r="G2" s="9"/>
       <c r="H2" s="7"/>
@@ -1623,13 +1647,13 @@
       <c r="IV2" s="3"/>
     </row>
     <row r="3" spans="1:256" ht="25.5" customHeight="1">
-      <c r="A3" s="46"/>
-      <c r="B3" s="48" t="s">
+      <c r="A3" s="47"/>
+      <c r="B3" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="48"/>
-      <c r="D3" s="48"/>
-      <c r="E3" s="48"/>
+      <c r="C3" s="49"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
       <c r="F3" s="9"/>
       <c r="G3" s="9"/>
       <c r="H3" s="7"/>
@@ -1883,7 +1907,7 @@
       <c r="IV3" s="3"/>
     </row>
     <row r="4" spans="1:256" ht="22.5" customHeight="1">
-      <c r="A4" s="46"/>
+      <c r="A4" s="47"/>
       <c r="B4" s="4"/>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
@@ -19003,39 +19027,72 @@
     </row>
     <row r="78" spans="1:256" ht="15.95" customHeight="1"/>
     <row r="79" spans="1:256" ht="15.95" customHeight="1"/>
-    <row r="80" spans="1:256" ht="15.95" customHeight="1"/>
-    <row r="81" ht="15.95" customHeight="1"/>
-    <row r="82" ht="15.95" customHeight="1"/>
-    <row r="83" ht="15.95" customHeight="1"/>
-    <row r="84" ht="15.95" customHeight="1"/>
-    <row r="85" ht="15.95" customHeight="1"/>
-    <row r="86" ht="15.95" customHeight="1"/>
-    <row r="87" ht="15.95" customHeight="1"/>
-    <row r="88" ht="15.95" customHeight="1"/>
-    <row r="89" ht="15.95" customHeight="1"/>
-    <row r="90" ht="15.95" customHeight="1"/>
-    <row r="91" ht="15.95" customHeight="1"/>
-    <row r="92" ht="15.95" customHeight="1"/>
-    <row r="93" ht="15.95" customHeight="1"/>
-    <row r="94" ht="15.95" customHeight="1"/>
-    <row r="95" ht="15.95" customHeight="1"/>
-    <row r="96" ht="15.95" customHeight="1"/>
-    <row r="97" ht="15.95" customHeight="1"/>
-    <row r="98" ht="15.95" customHeight="1"/>
-    <row r="99" ht="15.95" customHeight="1"/>
-    <row r="100" ht="15.95" customHeight="1"/>
-    <row r="101" ht="15.95" customHeight="1"/>
-    <row r="102" ht="15.95" customHeight="1"/>
-    <row r="103" ht="15.95" customHeight="1"/>
-    <row r="104" ht="15.95" customHeight="1"/>
-    <row r="105" ht="15.95" customHeight="1"/>
-    <row r="106" ht="15.95" customHeight="1"/>
-    <row r="107" ht="15.95" customHeight="1"/>
-    <row r="108" ht="15.95" customHeight="1"/>
-    <row r="109" ht="15.95" customHeight="1"/>
-    <row r="110" ht="15.95" customHeight="1"/>
-    <row r="111" ht="15.95" customHeight="1"/>
-    <row r="112" ht="15.95" customHeight="1"/>
+    <row r="80" spans="1:256" ht="15.95" customHeight="1">
+      <c r="A80" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B80" s="1"/>
+    </row>
+    <row r="81" spans="1:2" ht="15.95" customHeight="1">
+      <c r="A81" s="23" t="s">
+        <v>196</v>
+      </c>
+      <c r="B81" s="24" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" ht="15.95" customHeight="1">
+      <c r="A82" s="25" t="s">
+        <v>198</v>
+      </c>
+      <c r="B82" s="25" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" ht="15.95" customHeight="1"/>
+    <row r="84" spans="1:2" ht="15.95" customHeight="1"/>
+    <row r="85" spans="1:2" ht="15.95" customHeight="1"/>
+    <row r="86" spans="1:2" ht="15.95" customHeight="1"/>
+    <row r="87" spans="1:2" ht="15.95" customHeight="1"/>
+    <row r="88" spans="1:2" ht="15.95" customHeight="1"/>
+    <row r="89" spans="1:2" ht="15.95" customHeight="1"/>
+    <row r="90" spans="1:2" ht="15.95" customHeight="1"/>
+    <row r="91" spans="1:2" ht="15.95" customHeight="1"/>
+    <row r="92" spans="1:2" ht="15.95" customHeight="1"/>
+    <row r="93" spans="1:2" ht="15.95" customHeight="1"/>
+    <row r="94" spans="1:2" ht="15.95" customHeight="1"/>
+    <row r="95" spans="1:2" ht="15.95" customHeight="1"/>
+    <row r="96" spans="1:2" ht="15.95" customHeight="1"/>
+    <row r="97" spans="1:2" ht="15.95" customHeight="1"/>
+    <row r="98" spans="1:2" ht="15.95" customHeight="1"/>
+    <row r="99" spans="1:2" ht="15.95" customHeight="1"/>
+    <row r="100" spans="1:2" ht="15.95" customHeight="1"/>
+    <row r="101" spans="1:2" ht="15.95" customHeight="1"/>
+    <row r="102" spans="1:2" ht="15.95" customHeight="1">
+      <c r="A102" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="B102" s="1"/>
+    </row>
+    <row r="103" spans="1:2" ht="15.95" customHeight="1">
+      <c r="A103" s="23" t="s">
+        <v>201</v>
+      </c>
+      <c r="B103" s="24" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" ht="15.95" customHeight="1">
+      <c r="B104" s="22"/>
+    </row>
+    <row r="105" spans="1:2" ht="15.95" customHeight="1"/>
+    <row r="106" spans="1:2" ht="15.95" customHeight="1"/>
+    <row r="107" spans="1:2" ht="15.95" customHeight="1"/>
+    <row r="108" spans="1:2" ht="15.95" customHeight="1"/>
+    <row r="109" spans="1:2" ht="15.95" customHeight="1"/>
+    <row r="110" spans="1:2" ht="15.95" customHeight="1"/>
+    <row r="111" spans="1:2" ht="15.95" customHeight="1"/>
+    <row r="112" spans="1:2" ht="15.95" customHeight="1"/>
     <row r="113" ht="15.95" customHeight="1"/>
     <row r="114" ht="15.95" customHeight="1"/>
     <row r="115" ht="15.95" customHeight="1"/>
@@ -20003,12 +20060,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="50" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="26" t="s">
@@ -20067,11 +20124,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="51" t="s">
         <v>79</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="26" t="s">
@@ -20129,11 +20186,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="52" t="s">
         <v>85</v>
       </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="51"/>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="26" t="s">
@@ -20191,11 +20248,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="52" t="s">
         <v>91</v>
       </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="51"/>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="26" t="s">
@@ -20253,11 +20310,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="52" t="s">
         <v>96</v>
       </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="51"/>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="9" t="s">
@@ -20315,11 +20372,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="52" t="s">
         <v>101</v>
       </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="51"/>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="9" t="s">
@@ -20365,7 +20422,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:T94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" zoomScalePageLayoutView="60" workbookViewId="0">
+    <sheetView topLeftCell="A85" zoomScalePageLayoutView="60" workbookViewId="0">
       <selection activeCell="C93" sqref="C93:D93"/>
     </sheetView>
   </sheetViews>
@@ -20377,19 +20434,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="52" t="s">
         <v>106</v>
       </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
-      <c r="G1" s="51"/>
-      <c r="H1" s="51"/>
-      <c r="I1" s="51"/>
-      <c r="J1" s="51"/>
-      <c r="K1" s="51"/>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="52"/>
+      <c r="H1" s="52"/>
+      <c r="I1" s="52"/>
+      <c r="J1" s="52"/>
+      <c r="K1" s="52"/>
       <c r="L1" s="30"/>
       <c r="M1" s="30"/>
       <c r="N1" s="30"/>
@@ -20646,7 +20703,7 @@
       <c r="A94" s="43" t="s">
         <v>193</v>
       </c>
-      <c r="B94" s="52" t="s">
+      <c r="B94" s="46" t="s">
         <v>194</v>
       </c>
     </row>

</xml_diff>

<commit_message>
POCOR-6519: Update changes by adding new placeholders in excel | status: Done
</commit_message>
<xml_diff>
--- a/webroot/export/customexcel/default_templates/profile_template.xlsx
+++ b/webroot/export/customexcel/default_templates/profile_template.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="246">
   <si>
     <t>${"image":{"displayValue":"Institutions.logo_content","imageWidth":"100","imageMarginLeft":"20","imageMarginTop":"5"}}</t>
   </si>
@@ -640,10 +640,139 @@
     <t>Infrastructure Room Custom Fields</t>
   </si>
   <si>
-    <t>Question</t>
-  </si>
-  <si>
-    <t>Answer</t>
+    <t>Report Student Assessment Summary</t>
+  </si>
+  <si>
+    <t>Academic Period</t>
+  </si>
+  <si>
+    <t>Area Code</t>
+  </si>
+  <si>
+    <t>Area Name</t>
+  </si>
+  <si>
+    <t>Institution Code</t>
+  </si>
+  <si>
+    <t>Institution  Name</t>
+  </si>
+  <si>
+    <t>Grade Code</t>
+  </si>
+  <si>
+    <t>Grade Name</t>
+  </si>
+  <si>
+    <t>Subject Code</t>
+  </si>
+  <si>
+    <t>Subject Name</t>
+  </si>
+  <si>
+    <t>Subject Weight</t>
+  </si>
+  <si>
+    <t>Assessment Code</t>
+  </si>
+  <si>
+    <t>Assessment Name</t>
+  </si>
+  <si>
+    <t>Period Code</t>
+  </si>
+  <si>
+    <t>Period Name</t>
+  </si>
+  <si>
+    <t>Period Weight</t>
+  </si>
+  <si>
+    <t>Average Marks</t>
+  </si>
+  <si>
+    <t>${"match": {"displayValue": "ReportStudentAssessmentSummary.academic_period_name","rows": {"matchFrom": "ReportStudentAssessmentSummary.id","matchTo": "ReportStudentAssessmentSummary.id"}}}</t>
+  </si>
+  <si>
+    <t>${"match": {"displayValue": "ReportStudentAssessmentSummary.area_code","rows": {"matchFrom": "ReportStudentAssessmentSummary.id","matchTo": "ReportStudentAssessmentSummary.id"}}}</t>
+  </si>
+  <si>
+    <t>${"match": {"displayValue": "ReportStudentAssessmentSummary.area_name","rows": {"matchFrom": "ReportStudentAssessmentSummary.id","matchTo": "ReportStudentAssessmentSummary.id"}}}</t>
+  </si>
+  <si>
+    <t>${"match": {"displayValue": "ReportStudentAssessmentSummary.institution_code","rows": {"matchFrom": "ReportStudentAssessmentSummary.id","matchTo": "ReportStudentAssessmentSummary.id"}}}</t>
+  </si>
+  <si>
+    <t>${"match": {"displayValue": "ReportStudentAssessmentSummary.institution_name","rows": {"matchFrom": "ReportStudentAssessmentSummary.id","matchTo": "ReportStudentAssessmentSummary.id"}}}</t>
+  </si>
+  <si>
+    <t>${"match": {"displayValue": "ReportStudentAssessmentSummary.grade_code","rows": {"matchFrom": "ReportStudentAssessmentSummary.id","matchTo": "ReportStudentAssessmentSummary.id"}}}</t>
+  </si>
+  <si>
+    <t>${"match": {"displayValue": "ReportStudentAssessmentSummary.grade_name","rows": {"matchFrom": "ReportStudentAssessmentSummary.id","matchTo": "ReportStudentAssessmentSummary.id"}}}</t>
+  </si>
+  <si>
+    <t>${"match": {"displayValue": "ReportStudentAssessmentSummary.subject_code","rows": {"matchFrom": "ReportStudentAssessmentSummary.id","matchTo": "ReportStudentAssessmentSummary.id"}}}</t>
+  </si>
+  <si>
+    <t>${"match": {"displayValue": "ReportStudentAssessmentSummary.subject_name","rows": {"matchFrom": "ReportStudentAssessmentSummary.id","matchTo": "ReportStudentAssessmentSummary.id"}}}</t>
+  </si>
+  <si>
+    <t>${"match": {"displayValue": "ReportStudentAssessmentSummary.subject_weight","rows": {"matchFrom": "ReportStudentAssessmentSummary.id","matchTo": "ReportStudentAssessmentSummary.id"}}}</t>
+  </si>
+  <si>
+    <t>${"match": {"displayValue": "ReportStudentAssessmentSummary.assessment_code","rows": {"matchFrom": "ReportStudentAssessmentSummary.id","matchTo": "ReportStudentAssessmentSummary.id"}}}</t>
+  </si>
+  <si>
+    <t>${"match": {"displayValue": "ReportStudentAssessmentSummary.assessment_name","rows": {"matchFrom": "ReportStudentAssessmentSummary.id","matchTo": "ReportStudentAssessmentSummary.id"}}}</t>
+  </si>
+  <si>
+    <t>${"match": {"displayValue": "ReportStudentAssessmentSummary.period_code","rows": {"matchFrom": "ReportStudentAssessmentSummary.id","matchTo": "ReportStudentAssessmentSummary.id"}}}</t>
+  </si>
+  <si>
+    <t>${"match": {"displayValue": "ReportStudentAssessmentSummary.period_name","rows": {"matchFrom": "ReportStudentAssessmentSummary.id","matchTo": "ReportStudentAssessmentSummary.id"}}}</t>
+  </si>
+  <si>
+    <t>${"match": {"displayValue": "ReportStudentAssessmentSummary.period_weight","rows": {"matchFrom": "ReportStudentAssessmentSummary.id","matchTo": "ReportStudentAssessmentSummary.id"}}}</t>
+  </si>
+  <si>
+    <t>${"match": {"displayValue": "ReportStudentAssessmentSummary.average_marks","rows": {"matchFrom": "ReportStudentAssessmentSummary.id","matchTo": "ReportStudentAssessmentSummary.id"}}}</t>
+  </si>
+  <si>
+    <t>Institution Room Code</t>
+  </si>
+  <si>
+    <t>Institution Room Name</t>
+  </si>
+  <si>
+    <t>Room Area</t>
+  </si>
+  <si>
+    <t>Room Type</t>
+  </si>
+  <si>
+    <t>Custom Field Name</t>
+  </si>
+  <si>
+    <t>Custom Field Value</t>
+  </si>
+  <si>
+    <t>${"match": {"displayValue": "InfrastructureRoomCustomFields.code","rows": {"matchFrom": "InfrastructureRoomCustomFields.id","matchTo": "InfrastructureRoomCustomFields.id"}}}</t>
+  </si>
+  <si>
+    <t>${"match": {"displayValue": "InfrastructureRoomCustomFields.name","rows": {"matchFrom": "InfrastructureRoomCustomFields.id","matchTo": "InfrastructureRoomCustomFields.id"}}}</t>
+  </si>
+  <si>
+    <t>${"match": {"displayValue": "InfrastructureRoomCustomFields.area","rows": {"matchFrom": "InfrastructureRoomCustomFields.id","matchTo": "InfrastructureRoomCustomFields.id"}}}</t>
+  </si>
+  <si>
+    <t>${"match": {"displayValue": "InfrastructureRoomCustomFields.room_type","rows": {"matchFrom": "InfrastructureRoomCustomFields.id","matchTo": "InfrastructureRoomCustomFields.id"}}}</t>
+  </si>
+  <si>
+    <t>${"match": {"displayValue": "InfrastructureRoomCustomFields.custom_field_name","rows": {"matchFrom": "InfrastructureRoomCustomFields.id","matchTo": "InfrastructureRoomCustomFields.id"}}}</t>
+  </si>
+  <si>
+    <t>${"match": {"displayValue": "InfrastructureRoomCustomFields.custom_field_value","rows": {"matchFrom": "InfrastructureRoomCustomFields.id","matchTo": "InfrastructureRoomCustomFields.id"}}}</t>
   </si>
 </sst>
 </file>
@@ -1342,10 +1471,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:IV1048"/>
+  <dimension ref="A1:IV1041"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A77" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="B86" sqref="B86"/>
+    <sheetView tabSelected="1" topLeftCell="A155" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="A168" sqref="A168"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75"/>
@@ -17732,8 +17861,10 @@
       <c r="IV71" s="3"/>
     </row>
     <row r="72" spans="1:256" ht="12" customHeight="1">
-      <c r="A72" s="3"/>
-      <c r="B72" s="3"/>
+      <c r="A72" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B72" s="1"/>
       <c r="C72" s="3"/>
       <c r="E72" s="3"/>
       <c r="F72" s="3"/>
@@ -17989,8 +18120,12 @@
       <c r="IV72" s="3"/>
     </row>
     <row r="73" spans="1:256" ht="15.75" customHeight="1">
-      <c r="A73" s="3"/>
-      <c r="B73" s="3"/>
+      <c r="A73" s="23" t="s">
+        <v>196</v>
+      </c>
+      <c r="B73" s="24" t="s">
+        <v>197</v>
+      </c>
       <c r="C73" s="3"/>
       <c r="E73" s="3"/>
       <c r="F73" s="7"/>
@@ -18246,8 +18381,12 @@
       <c r="IV73" s="3"/>
     </row>
     <row r="74" spans="1:256" ht="15.75" customHeight="1">
-      <c r="A74" s="3"/>
-      <c r="B74" s="3"/>
+      <c r="A74" s="25" t="s">
+        <v>198</v>
+      </c>
+      <c r="B74" s="25" t="s">
+        <v>199</v>
+      </c>
       <c r="C74" s="3"/>
       <c r="E74" s="3"/>
       <c r="F74" s="7"/>
@@ -19027,72 +19166,156 @@
     </row>
     <row r="78" spans="1:256" ht="15.95" customHeight="1"/>
     <row r="79" spans="1:256" ht="15.95" customHeight="1"/>
-    <row r="80" spans="1:256" ht="15.95" customHeight="1">
-      <c r="A80" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="B80" s="1"/>
+    <row r="80" spans="1:256" ht="15.95" customHeight="1"/>
+    <row r="81" ht="15.95" customHeight="1"/>
+    <row r="82" ht="15.95" customHeight="1"/>
+    <row r="83" ht="15.95" customHeight="1"/>
+    <row r="84" ht="15.95" customHeight="1"/>
+    <row r="85" ht="15.95" customHeight="1"/>
+    <row r="86" ht="15.95" customHeight="1"/>
+    <row r="87" ht="15.95" customHeight="1"/>
+    <row r="88" ht="15.95" customHeight="1"/>
+    <row r="89" ht="15.95" customHeight="1"/>
+    <row r="90" ht="15.95" customHeight="1"/>
+    <row r="91" ht="15.95" customHeight="1"/>
+    <row r="92" ht="15.95" customHeight="1"/>
+    <row r="93" ht="15.95" customHeight="1"/>
+    <row r="94" ht="15.95" customHeight="1"/>
+    <row r="95" ht="15.95" customHeight="1"/>
+    <row r="96" ht="15.95" customHeight="1"/>
+    <row r="97" spans="1:16" ht="15.95" customHeight="1"/>
+    <row r="98" spans="1:16" ht="15.95" customHeight="1">
+      <c r="A98" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B98" s="1"/>
+      <c r="C98" s="1"/>
+      <c r="D98" s="1"/>
+      <c r="E98" s="1"/>
+      <c r="F98" s="1"/>
+      <c r="G98" s="1"/>
+      <c r="H98" s="1"/>
+      <c r="I98" s="1"/>
+      <c r="J98" s="1"/>
+      <c r="K98" s="1"/>
+      <c r="L98" s="1"/>
+      <c r="M98" s="1"/>
+      <c r="N98" s="1"/>
+      <c r="O98" s="1"/>
+      <c r="P98" s="1"/>
     </row>
-    <row r="81" spans="1:2" ht="15.95" customHeight="1">
-      <c r="A81" s="23" t="s">
-        <v>196</v>
-      </c>
-      <c r="B81" s="24" t="s">
-        <v>197</v>
+    <row r="99" spans="1:16" ht="15.95" customHeight="1">
+      <c r="A99" s="23" t="s">
+        <v>202</v>
+      </c>
+      <c r="B99" s="23" t="s">
+        <v>203</v>
+      </c>
+      <c r="C99" s="23" t="s">
+        <v>204</v>
+      </c>
+      <c r="D99" s="23" t="s">
+        <v>205</v>
+      </c>
+      <c r="E99" s="23" t="s">
+        <v>206</v>
+      </c>
+      <c r="F99" s="23" t="s">
+        <v>207</v>
+      </c>
+      <c r="G99" s="23" t="s">
+        <v>208</v>
+      </c>
+      <c r="H99" s="23" t="s">
+        <v>209</v>
+      </c>
+      <c r="I99" s="23" t="s">
+        <v>210</v>
+      </c>
+      <c r="J99" s="23" t="s">
+        <v>211</v>
+      </c>
+      <c r="K99" s="23" t="s">
+        <v>212</v>
+      </c>
+      <c r="L99" s="23" t="s">
+        <v>213</v>
+      </c>
+      <c r="M99" s="23" t="s">
+        <v>214</v>
+      </c>
+      <c r="N99" s="23" t="s">
+        <v>215</v>
+      </c>
+      <c r="O99" s="23" t="s">
+        <v>216</v>
+      </c>
+      <c r="P99" s="23" t="s">
+        <v>217</v>
       </c>
     </row>
-    <row r="82" spans="1:2" ht="15.95" customHeight="1">
-      <c r="A82" s="25" t="s">
-        <v>198</v>
-      </c>
-      <c r="B82" s="25" t="s">
-        <v>199</v>
+    <row r="100" spans="1:16" ht="15.95" customHeight="1">
+      <c r="A100" s="25" t="s">
+        <v>218</v>
+      </c>
+      <c r="B100" s="25" t="s">
+        <v>219</v>
+      </c>
+      <c r="C100" s="25" t="s">
+        <v>220</v>
+      </c>
+      <c r="D100" s="25" t="s">
+        <v>221</v>
+      </c>
+      <c r="E100" s="25" t="s">
+        <v>222</v>
+      </c>
+      <c r="F100" s="25" t="s">
+        <v>223</v>
+      </c>
+      <c r="G100" s="25" t="s">
+        <v>224</v>
+      </c>
+      <c r="H100" s="25" t="s">
+        <v>225</v>
+      </c>
+      <c r="I100" s="25" t="s">
+        <v>226</v>
+      </c>
+      <c r="J100" s="25" t="s">
+        <v>227</v>
+      </c>
+      <c r="K100" s="25" t="s">
+        <v>228</v>
+      </c>
+      <c r="L100" s="25" t="s">
+        <v>229</v>
+      </c>
+      <c r="M100" s="25" t="s">
+        <v>230</v>
+      </c>
+      <c r="N100" s="25" t="s">
+        <v>231</v>
+      </c>
+      <c r="O100" s="25" t="s">
+        <v>232</v>
+      </c>
+      <c r="P100" s="25" t="s">
+        <v>233</v>
       </c>
     </row>
-    <row r="83" spans="1:2" ht="15.95" customHeight="1"/>
-    <row r="84" spans="1:2" ht="15.95" customHeight="1"/>
-    <row r="85" spans="1:2" ht="15.95" customHeight="1"/>
-    <row r="86" spans="1:2" ht="15.95" customHeight="1"/>
-    <row r="87" spans="1:2" ht="15.95" customHeight="1"/>
-    <row r="88" spans="1:2" ht="15.95" customHeight="1"/>
-    <row r="89" spans="1:2" ht="15.95" customHeight="1"/>
-    <row r="90" spans="1:2" ht="15.95" customHeight="1"/>
-    <row r="91" spans="1:2" ht="15.95" customHeight="1"/>
-    <row r="92" spans="1:2" ht="15.95" customHeight="1"/>
-    <row r="93" spans="1:2" ht="15.95" customHeight="1"/>
-    <row r="94" spans="1:2" ht="15.95" customHeight="1"/>
-    <row r="95" spans="1:2" ht="15.95" customHeight="1"/>
-    <row r="96" spans="1:2" ht="15.95" customHeight="1"/>
-    <row r="97" spans="1:2" ht="15.95" customHeight="1"/>
-    <row r="98" spans="1:2" ht="15.95" customHeight="1"/>
-    <row r="99" spans="1:2" ht="15.95" customHeight="1"/>
-    <row r="100" spans="1:2" ht="15.95" customHeight="1"/>
-    <row r="101" spans="1:2" ht="15.95" customHeight="1"/>
-    <row r="102" spans="1:2" ht="15.95" customHeight="1">
-      <c r="A102" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="B102" s="1"/>
-    </row>
-    <row r="103" spans="1:2" ht="15.95" customHeight="1">
-      <c r="A103" s="23" t="s">
-        <v>201</v>
-      </c>
-      <c r="B103" s="24" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2" ht="15.95" customHeight="1">
-      <c r="B104" s="22"/>
-    </row>
-    <row r="105" spans="1:2" ht="15.95" customHeight="1"/>
-    <row r="106" spans="1:2" ht="15.95" customHeight="1"/>
-    <row r="107" spans="1:2" ht="15.95" customHeight="1"/>
-    <row r="108" spans="1:2" ht="15.95" customHeight="1"/>
-    <row r="109" spans="1:2" ht="15.95" customHeight="1"/>
-    <row r="110" spans="1:2" ht="15.95" customHeight="1"/>
-    <row r="111" spans="1:2" ht="15.95" customHeight="1"/>
-    <row r="112" spans="1:2" ht="15.95" customHeight="1"/>
+    <row r="101" spans="1:16" ht="15.95" customHeight="1"/>
+    <row r="102" spans="1:16" ht="15.95" customHeight="1"/>
+    <row r="103" spans="1:16" ht="15.95" customHeight="1"/>
+    <row r="104" spans="1:16" ht="15.95" customHeight="1"/>
+    <row r="105" spans="1:16" ht="15.95" customHeight="1"/>
+    <row r="106" spans="1:16" ht="15.95" customHeight="1"/>
+    <row r="107" spans="1:16" ht="15.95" customHeight="1"/>
+    <row r="108" spans="1:16" ht="15.95" customHeight="1"/>
+    <row r="109" spans="1:16" ht="15.95" customHeight="1"/>
+    <row r="110" spans="1:16" ht="15.95" customHeight="1"/>
+    <row r="111" spans="1:16" ht="15.95" customHeight="1"/>
+    <row r="112" spans="1:16" ht="15.95" customHeight="1"/>
     <row r="113" ht="15.95" customHeight="1"/>
     <row r="114" ht="15.95" customHeight="1"/>
     <row r="115" ht="15.95" customHeight="1"/>
@@ -19141,22 +19364,69 @@
     <row r="158" ht="15.95" customHeight="1"/>
     <row r="159" ht="15.95" customHeight="1"/>
     <row r="160" ht="15.95" customHeight="1"/>
-    <row r="161" ht="15.95" customHeight="1"/>
-    <row r="162" ht="15.95" customHeight="1"/>
-    <row r="163" ht="15.95" customHeight="1"/>
-    <row r="164" ht="15.95" customHeight="1"/>
-    <row r="165" ht="15.95" customHeight="1"/>
-    <row r="166" ht="15.95" customHeight="1"/>
-    <row r="167" ht="15.95" customHeight="1"/>
-    <row r="168" ht="15.95" customHeight="1"/>
-    <row r="169" ht="15.95" customHeight="1"/>
-    <row r="170" ht="15.95" customHeight="1"/>
-    <row r="171" ht="15.95" customHeight="1"/>
-    <row r="172" ht="15.95" customHeight="1"/>
-    <row r="173" ht="15.95" customHeight="1"/>
-    <row r="174" ht="15.95" customHeight="1"/>
-    <row r="175" ht="15.95" customHeight="1"/>
-    <row r="176" ht="15.95" customHeight="1"/>
+    <row r="161" spans="1:6" ht="15.95" customHeight="1"/>
+    <row r="162" spans="1:6" ht="15.95" customHeight="1"/>
+    <row r="163" spans="1:6" ht="15.95" customHeight="1"/>
+    <row r="164" spans="1:6" ht="15.95" customHeight="1"/>
+    <row r="165" spans="1:6" ht="15.95" customHeight="1"/>
+    <row r="166" spans="1:6" ht="15.95" customHeight="1"/>
+    <row r="167" spans="1:6" ht="15.95" customHeight="1"/>
+    <row r="168" spans="1:6" ht="15.95" customHeight="1"/>
+    <row r="169" spans="1:6" ht="15.95" customHeight="1"/>
+    <row r="170" spans="1:6" ht="15.95" customHeight="1"/>
+    <row r="171" spans="1:6" ht="15.95" customHeight="1">
+      <c r="A171" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="B171" s="1"/>
+      <c r="C171" s="1"/>
+      <c r="D171" s="1"/>
+      <c r="E171" s="1"/>
+      <c r="F171" s="1"/>
+    </row>
+    <row r="172" spans="1:6" ht="15.95" customHeight="1">
+      <c r="A172" s="23" t="s">
+        <v>234</v>
+      </c>
+      <c r="B172" s="23" t="s">
+        <v>235</v>
+      </c>
+      <c r="C172" s="23" t="s">
+        <v>236</v>
+      </c>
+      <c r="D172" s="23" t="s">
+        <v>237</v>
+      </c>
+      <c r="E172" s="23" t="s">
+        <v>238</v>
+      </c>
+      <c r="F172" s="23" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="173" spans="1:6" ht="15.95" customHeight="1">
+      <c r="A173" s="25" t="s">
+        <v>240</v>
+      </c>
+      <c r="B173" s="25" t="s">
+        <v>241</v>
+      </c>
+      <c r="C173" s="25" t="s">
+        <v>242</v>
+      </c>
+      <c r="D173" s="25" t="s">
+        <v>243</v>
+      </c>
+      <c r="E173" s="25" t="s">
+        <v>244</v>
+      </c>
+      <c r="F173" s="25" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="174" spans="1:6" ht="15.95" customHeight="1"/>
+    <row r="175" spans="1:6" ht="15.95" customHeight="1"/>
+    <row r="176" spans="1:6" ht="15.95" customHeight="1"/>
     <row r="177" ht="15.95" customHeight="1"/>
     <row r="178" ht="15.95" customHeight="1"/>
     <row r="179" ht="15.95" customHeight="1"/>
@@ -20022,13 +20292,6 @@
     <row r="1039" ht="15.95" customHeight="1"/>
     <row r="1040" ht="15.95" customHeight="1"/>
     <row r="1041" ht="15.95" customHeight="1"/>
-    <row r="1042" ht="15.95" customHeight="1"/>
-    <row r="1043" ht="15.95" customHeight="1"/>
-    <row r="1044" ht="15.95" customHeight="1"/>
-    <row r="1045" ht="15.95" customHeight="1"/>
-    <row r="1046" ht="15.95" customHeight="1"/>
-    <row r="1047" ht="15.95" customHeight="1"/>
-    <row r="1048" ht="15.95" customHeight="1"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:A4"/>
@@ -20422,7 +20685,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:T94"/>
   <sheetViews>
-    <sheetView topLeftCell="A85" zoomScalePageLayoutView="60" workbookViewId="0">
+    <sheetView zoomScalePageLayoutView="60" workbookViewId="0">
       <selection activeCell="C93" sqref="C93:D93"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
POCOR-6646|added sheet into profile template and update Reportcard file|status:in-progress
</commit_message>
<xml_diff>
--- a/webroot/export/customexcel/default_templates/profile_template.xlsx
+++ b/webroot/export/customexcel/default_templates/profile_template.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\pocor-openemis-core\webroot\export\customexcel\default_templates\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11260991-4D1F-4CAF-B37D-E9EFE172E349}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="495" windowWidth="20730" windowHeight="11760" tabRatio="933" firstSheet="4" activeTab="7"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="1000" firstSheet="3" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -15,18 +21,10 @@
     <sheet name="Staff by Positions and Qualific" sheetId="6" r:id="rId6"/>
     <sheet name="Staff by Staff Type and Qualifi" sheetId="7" r:id="rId7"/>
     <sheet name="Extra details" sheetId="8" r:id="rId8"/>
+    <sheet name="POCOR6646" sheetId="10" r:id="rId9"/>
   </sheets>
   <calcPr calcId="124519"/>
   <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
     </ext>
@@ -34,8 +32,84 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Microsoft Office User</author>
+  </authors>
+  <commentList>
+    <comment ref="F2" authorId="0" shapeId="0" xr:uid="{EB7E133D-ED08-4475-ABE3-E99C03AB3FA6}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Microsoft Office User:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>First Name + Middle Name + Third Name + Last Name</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H2" authorId="0" shapeId="0" xr:uid="{4F4FA01F-3BB2-4E2D-BE7D-0F574B55055E}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Microsoft Office User:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Please account for case when subjects can have different weights. Simple average may not always work</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="207">
   <si>
     <t>${"image":{"displayValue":"Institutions.logo_content","imageWidth":"100","imageMarginLeft":"20","imageMarginTop":"5"}}</t>
   </si>
@@ -621,12 +695,48 @@
   <si>
     <t xml:space="preserve">${"match": {"displayValue": "NonTeachingStaffCount.area_level","rows": {"matchFrom": "InstitutionAreaName.id","matchTo": "InstitutionAreaName.id"}}} </t>
   </si>
+  <si>
+    <t>Education Grade</t>
+  </si>
+  <si>
+    <t>Homeroom Teacher</t>
+  </si>
+  <si>
+    <t>OpenEMIS ID</t>
+  </si>
+  <si>
+    <t>Default Identity Number</t>
+  </si>
+  <si>
+    <t>Student Name</t>
+  </si>
+  <si>
+    <t>Education Subjects Name</t>
+  </si>
+  <si>
+    <t>Average Result</t>
+  </si>
+  <si>
+    <t>Individual Results</t>
+  </si>
+  <si>
+    <t>Number of Days Absence</t>
+  </si>
+  <si>
+    <t>Class Name</t>
+  </si>
+  <si>
+    <t>Student Abesence Records</t>
+  </si>
+  <si>
+    <t>${"match": {"displayValue": "EducationGrade.name","rows": {"matchFrom": "EducationGrade.id","matchTo": "EducationGrade.id"}}}</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="11">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -695,6 +805,34 @@
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF172B4D"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -820,7 +958,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -921,6 +1059,15 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -939,15 +1086,14 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1076,7 +1222,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1108,9 +1254,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1142,6 +1306,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1317,32 +1499,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:IV1048"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="B57" sqref="B57"/>
+    <sheetView topLeftCell="B55" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="B60" sqref="B60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="63.140625" customWidth="1"/>
-    <col min="2" max="2" width="54.28515625" customWidth="1"/>
+    <col min="1" max="1" width="63.1796875" customWidth="1"/>
+    <col min="2" max="2" width="54.26953125" customWidth="1"/>
     <col min="3" max="3" width="53" customWidth="1"/>
-    <col min="4" max="4" width="24.28515625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="61.28515625" customWidth="1"/>
-    <col min="6" max="6" width="51.85546875" customWidth="1"/>
+    <col min="4" max="4" width="24.26953125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="61.26953125" customWidth="1"/>
+    <col min="6" max="6" width="51.81640625" customWidth="1"/>
     <col min="7" max="7" width="58" customWidth="1"/>
     <col min="8" max="8" width="40" customWidth="1"/>
-    <col min="9" max="18" width="39.42578125" customWidth="1"/>
-    <col min="19" max="27" width="41.85546875" customWidth="1"/>
-    <col min="28" max="256" width="39.7109375" customWidth="1"/>
-    <col min="257" max="1023" width="16.140625" customWidth="1"/>
-    <col min="1024" max="1025" width="11.7109375" customWidth="1"/>
+    <col min="9" max="18" width="39.453125" customWidth="1"/>
+    <col min="19" max="27" width="41.81640625" customWidth="1"/>
+    <col min="28" max="256" width="39.7265625" customWidth="1"/>
+    <col min="257" max="1023" width="16.1796875" customWidth="1"/>
+    <col min="1024" max="1025" width="11.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:256" ht="15" customHeight="1">
-      <c r="A1" s="46" t="s">
+    <row r="1" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="49" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4"/>
@@ -1362,14 +1544,14 @@
       <c r="P1" s="7"/>
       <c r="Q1" s="7"/>
     </row>
-    <row r="2" spans="1:256" ht="25.5" customHeight="1">
-      <c r="A2" s="46"/>
-      <c r="B2" s="47" t="s">
+    <row r="2" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="49"/>
+      <c r="B2" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
       <c r="F2" s="8"/>
       <c r="G2" s="9"/>
       <c r="H2" s="7"/>
@@ -1622,14 +1804,14 @@
       <c r="IU2" s="3"/>
       <c r="IV2" s="3"/>
     </row>
-    <row r="3" spans="1:256" ht="25.5" customHeight="1">
-      <c r="A3" s="46"/>
-      <c r="B3" s="48" t="s">
+    <row r="3" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="49"/>
+      <c r="B3" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="48"/>
-      <c r="D3" s="48"/>
-      <c r="E3" s="48"/>
+      <c r="C3" s="51"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
       <c r="F3" s="9"/>
       <c r="G3" s="9"/>
       <c r="H3" s="7"/>
@@ -1882,8 +2064,8 @@
       <c r="IU3" s="3"/>
       <c r="IV3" s="3"/>
     </row>
-    <row r="4" spans="1:256" ht="22.5" customHeight="1">
-      <c r="A4" s="46"/>
+    <row r="4" spans="1:256" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="49"/>
       <c r="B4" s="4"/>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
@@ -1901,7 +2083,7 @@
       <c r="P4" s="7"/>
       <c r="Q4" s="7"/>
     </row>
-    <row r="5" spans="1:256" ht="15.75" customHeight="1">
+    <row r="5" spans="1:256" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="10"/>
       <c r="B5" s="10"/>
       <c r="C5" s="10"/>
@@ -1921,7 +2103,7 @@
       <c r="Q5" s="7"/>
       <c r="R5" s="7"/>
     </row>
-    <row r="6" spans="1:256" ht="12" customHeight="1">
+    <row r="6" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="11" t="s">
         <v>3</v>
       </c>
@@ -1945,7 +2127,7 @@
       <c r="Q6" s="7"/>
       <c r="R6" s="7"/>
     </row>
-    <row r="7" spans="1:256" ht="12" customHeight="1">
+    <row r="7" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="11" t="s">
         <v>5</v>
       </c>
@@ -1969,7 +2151,7 @@
       <c r="Q7" s="7"/>
       <c r="R7" s="7"/>
     </row>
-    <row r="8" spans="1:256" ht="12" customHeight="1">
+    <row r="8" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="11" t="s">
         <v>7</v>
       </c>
@@ -1993,7 +2175,7 @@
       <c r="Q8" s="7"/>
       <c r="R8" s="7"/>
     </row>
-    <row r="9" spans="1:256" ht="12" customHeight="1">
+    <row r="9" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="11" t="s">
         <v>9</v>
       </c>
@@ -2017,7 +2199,7 @@
       <c r="Q9" s="7"/>
       <c r="R9" s="7"/>
     </row>
-    <row r="10" spans="1:256" ht="12" customHeight="1">
+    <row r="10" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="11" t="s">
         <v>11</v>
       </c>
@@ -2041,7 +2223,7 @@
       <c r="Q10" s="7"/>
       <c r="R10" s="7"/>
     </row>
-    <row r="11" spans="1:256" ht="12" customHeight="1">
+    <row r="11" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="11" t="s">
         <v>13</v>
       </c>
@@ -2303,7 +2485,7 @@
       <c r="IU11" s="3"/>
       <c r="IV11" s="3"/>
     </row>
-    <row r="12" spans="1:256" ht="16.5" customHeight="1">
+    <row r="12" spans="1:256" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="16"/>
       <c r="B12" s="16"/>
       <c r="C12" s="16"/>
@@ -2561,7 +2743,7 @@
       <c r="IU12" s="3"/>
       <c r="IV12" s="3"/>
     </row>
-    <row r="13" spans="1:256" ht="16.5" customHeight="1">
+    <row r="13" spans="1:256" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="11" t="s">
         <v>15</v>
       </c>
@@ -2823,7 +3005,7 @@
       <c r="IU13" s="3"/>
       <c r="IV13" s="3"/>
     </row>
-    <row r="14" spans="1:256" ht="16.5" customHeight="1">
+    <row r="14" spans="1:256" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="11" t="s">
         <v>17</v>
       </c>
@@ -3085,7 +3267,7 @@
       <c r="IU14" s="3"/>
       <c r="IV14" s="3"/>
     </row>
-    <row r="15" spans="1:256" ht="12" customHeight="1">
+    <row r="15" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="11" t="s">
         <v>19</v>
       </c>
@@ -3347,7 +3529,7 @@
       <c r="IU15" s="3"/>
       <c r="IV15" s="3"/>
     </row>
-    <row r="16" spans="1:256" ht="12" customHeight="1">
+    <row r="16" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="11" t="s">
         <v>21</v>
       </c>
@@ -3609,7 +3791,7 @@
       <c r="IU16" s="3"/>
       <c r="IV16" s="3"/>
     </row>
-    <row r="17" spans="1:256" ht="12" customHeight="1">
+    <row r="17" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="11" t="s">
         <v>23</v>
       </c>
@@ -3871,7 +4053,7 @@
       <c r="IU17" s="3"/>
       <c r="IV17" s="3"/>
     </row>
-    <row r="18" spans="1:256" ht="12" customHeight="1">
+    <row r="18" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="11" t="s">
         <v>25</v>
       </c>
@@ -4133,7 +4315,7 @@
       <c r="IU18" s="3"/>
       <c r="IV18" s="3"/>
     </row>
-    <row r="19" spans="1:256" ht="12" customHeight="1">
+    <row r="19" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="11" t="s">
         <v>27</v>
       </c>
@@ -4395,7 +4577,7 @@
       <c r="IU19" s="3"/>
       <c r="IV19" s="3"/>
     </row>
-    <row r="20" spans="1:256" ht="12" customHeight="1">
+    <row r="20" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="11" t="s">
         <v>15</v>
       </c>
@@ -4657,7 +4839,7 @@
       <c r="IU20" s="3"/>
       <c r="IV20" s="3"/>
     </row>
-    <row r="21" spans="1:256" ht="12" customHeight="1">
+    <row r="21" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="11" t="s">
         <v>29</v>
       </c>
@@ -4919,7 +5101,7 @@
       <c r="IU21" s="3"/>
       <c r="IV21" s="3"/>
     </row>
-    <row r="22" spans="1:256" ht="12" customHeight="1">
+    <row r="22" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="11" t="s">
         <v>164</v>
       </c>
@@ -5181,7 +5363,7 @@
       <c r="IU22" s="3"/>
       <c r="IV22" s="3"/>
     </row>
-    <row r="23" spans="1:256" ht="12" customHeight="1">
+    <row r="23" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="11" t="s">
         <v>166</v>
       </c>
@@ -5443,7 +5625,7 @@
       <c r="IU23" s="3"/>
       <c r="IV23" s="3"/>
     </row>
-    <row r="24" spans="1:256" ht="12" customHeight="1">
+    <row r="24" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="11" t="s">
         <v>168</v>
       </c>
@@ -5705,7 +5887,7 @@
       <c r="IU24" s="3"/>
       <c r="IV24" s="3"/>
     </row>
-    <row r="25" spans="1:256" ht="12" customHeight="1">
+    <row r="25" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="41"/>
       <c r="B25" s="41"/>
       <c r="C25" s="39"/>
@@ -5963,7 +6145,7 @@
       <c r="IU25" s="3"/>
       <c r="IV25" s="3"/>
     </row>
-    <row r="26" spans="1:256" ht="12" customHeight="1">
+    <row r="26" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="41"/>
       <c r="B26" s="41"/>
       <c r="C26" s="39"/>
@@ -6221,7 +6403,7 @@
       <c r="IU26" s="3"/>
       <c r="IV26" s="3"/>
     </row>
-    <row r="27" spans="1:256" ht="12" customHeight="1">
+    <row r="27" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
         <v>31</v>
       </c>
@@ -6481,7 +6663,7 @@
       <c r="IU27" s="3"/>
       <c r="IV27" s="3"/>
     </row>
-    <row r="28" spans="1:256" ht="12" customHeight="1">
+    <row r="28" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="9" t="s">
         <v>32</v>
       </c>
@@ -6745,7 +6927,7 @@
       <c r="IU28" s="3"/>
       <c r="IV28" s="3"/>
     </row>
-    <row r="29" spans="1:256" ht="12" customHeight="1">
+    <row r="29" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="12" t="s">
         <v>35</v>
       </c>
@@ -7009,7 +7191,7 @@
       <c r="IU29" s="3"/>
       <c r="IV29" s="3"/>
     </row>
-    <row r="30" spans="1:256" ht="12" customHeight="1">
+    <row r="30" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="7"/>
       <c r="B30" s="7"/>
       <c r="C30" s="7"/>
@@ -7267,7 +7449,7 @@
       <c r="IU30" s="3"/>
       <c r="IV30" s="3"/>
     </row>
-    <row r="31" spans="1:256" ht="12" customHeight="1">
+    <row r="31" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="7"/>
       <c r="B31" s="7"/>
       <c r="C31" s="7"/>
@@ -7525,7 +7707,7 @@
       <c r="IU31" s="3"/>
       <c r="IV31" s="3"/>
     </row>
-    <row r="32" spans="1:256" ht="12" customHeight="1">
+    <row r="32" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="20" t="s">
         <v>38</v>
       </c>
@@ -7787,7 +7969,7 @@
       <c r="IU32" s="3"/>
       <c r="IV32" s="3"/>
     </row>
-    <row r="33" spans="1:256" ht="12" customHeight="1">
+    <row r="33" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="20" t="s">
         <v>40</v>
       </c>
@@ -8049,7 +8231,7 @@
       <c r="IU33" s="3"/>
       <c r="IV33" s="3"/>
     </row>
-    <row r="34" spans="1:256" ht="12" customHeight="1">
+    <row r="34" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="17"/>
       <c r="B34" s="18"/>
       <c r="C34" s="18"/>
@@ -8307,7 +8489,7 @@
       <c r="IU34" s="3"/>
       <c r="IV34" s="3"/>
     </row>
-    <row r="35" spans="1:256" ht="12" customHeight="1">
+    <row r="35" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="17"/>
       <c r="B35" s="18"/>
       <c r="C35" s="18"/>
@@ -8565,7 +8747,7 @@
       <c r="IU35" s="3"/>
       <c r="IV35" s="3"/>
     </row>
-    <row r="36" spans="1:256" ht="12" customHeight="1">
+    <row r="36" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="20" t="s">
         <v>42</v>
       </c>
@@ -8827,7 +9009,7 @@
       <c r="IU36" s="3"/>
       <c r="IV36" s="3"/>
     </row>
-    <row r="37" spans="1:256" ht="12" customHeight="1">
+    <row r="37" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="20" t="s">
         <v>44</v>
       </c>
@@ -9089,7 +9271,7 @@
       <c r="IU37" s="3"/>
       <c r="IV37" s="3"/>
     </row>
-    <row r="38" spans="1:256" ht="12" customHeight="1">
+    <row r="38" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="17"/>
       <c r="B38" s="18"/>
       <c r="C38" s="18"/>
@@ -9347,7 +9529,7 @@
       <c r="IU38" s="3"/>
       <c r="IV38" s="3"/>
     </row>
-    <row r="39" spans="1:256" ht="12" customHeight="1">
+    <row r="39" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="17"/>
       <c r="B39" s="18"/>
       <c r="C39" s="18"/>
@@ -9605,7 +9787,7 @@
       <c r="IU39" s="3"/>
       <c r="IV39" s="3"/>
     </row>
-    <row r="40" spans="1:256" ht="12" customHeight="1">
+    <row r="40" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="21" t="s">
         <v>46</v>
       </c>
@@ -9867,7 +10049,7 @@
       <c r="IU40" s="3"/>
       <c r="IV40" s="3"/>
     </row>
-    <row r="41" spans="1:256" ht="12" customHeight="1">
+    <row r="41" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="21" t="s">
         <v>48</v>
       </c>
@@ -10129,7 +10311,7 @@
       <c r="IU41" s="3"/>
       <c r="IV41" s="3"/>
     </row>
-    <row r="42" spans="1:256" ht="12" customHeight="1">
+    <row r="42" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="17"/>
       <c r="B42" s="18"/>
       <c r="C42" s="18"/>
@@ -10387,7 +10569,7 @@
       <c r="IU42" s="3"/>
       <c r="IV42" s="3"/>
     </row>
-    <row r="43" spans="1:256" ht="12" customHeight="1">
+    <row r="43" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="17"/>
       <c r="B43" s="18"/>
       <c r="C43" s="18"/>
@@ -10645,7 +10827,7 @@
       <c r="IU43" s="3"/>
       <c r="IV43" s="3"/>
     </row>
-    <row r="44" spans="1:256" ht="12" customHeight="1">
+    <row r="44" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="11" t="s">
         <v>50</v>
       </c>
@@ -10907,7 +11089,7 @@
       <c r="IU44" s="3"/>
       <c r="IV44" s="3"/>
     </row>
-    <row r="45" spans="1:256" ht="12" customHeight="1">
+    <row r="45" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="11" t="s">
         <v>52</v>
       </c>
@@ -11169,7 +11351,7 @@
       <c r="IU45" s="3"/>
       <c r="IV45" s="3"/>
     </row>
-    <row r="46" spans="1:256" ht="12" customHeight="1">
+    <row r="46" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="11" t="s">
         <v>54</v>
       </c>
@@ -11431,7 +11613,7 @@
       <c r="IU46" s="3"/>
       <c r="IV46" s="3"/>
     </row>
-    <row r="47" spans="1:256" ht="12" customHeight="1">
+    <row r="47" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="11" t="s">
         <v>56</v>
       </c>
@@ -11693,7 +11875,7 @@
       <c r="IU47" s="3"/>
       <c r="IV47" s="3"/>
     </row>
-    <row r="48" spans="1:256" ht="12" customHeight="1">
+    <row r="48" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="11" t="s">
         <v>58</v>
       </c>
@@ -11955,7 +12137,7 @@
       <c r="IU48" s="3"/>
       <c r="IV48" s="3"/>
     </row>
-    <row r="49" spans="1:256" ht="12" customHeight="1">
+    <row r="49" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="11" t="s">
         <v>60</v>
       </c>
@@ -12217,7 +12399,7 @@
       <c r="IU49" s="3"/>
       <c r="IV49" s="3"/>
     </row>
-    <row r="50" spans="1:256" ht="12" customHeight="1">
+    <row r="50" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="11" t="s">
         <v>62</v>
       </c>
@@ -12479,7 +12661,7 @@
       <c r="IU50" s="3"/>
       <c r="IV50" s="3"/>
     </row>
-    <row r="51" spans="1:256" ht="12" customHeight="1">
+    <row r="51" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" s="11" t="s">
         <v>64</v>
       </c>
@@ -12739,7 +12921,7 @@
       <c r="IU51" s="3"/>
       <c r="IV51" s="3"/>
     </row>
-    <row r="52" spans="1:256" ht="12" customHeight="1">
+    <row r="52" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" s="11" t="s">
         <v>65</v>
       </c>
@@ -13001,7 +13183,7 @@
       <c r="IU52" s="3"/>
       <c r="IV52" s="3"/>
     </row>
-    <row r="53" spans="1:256" ht="12" customHeight="1">
+    <row r="53" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" s="17"/>
       <c r="B53" s="18"/>
       <c r="C53" s="18"/>
@@ -13259,7 +13441,7 @@
       <c r="IU53" s="3"/>
       <c r="IV53" s="3"/>
     </row>
-    <row r="54" spans="1:256" ht="12" customHeight="1">
+    <row r="54" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A54" s="17"/>
       <c r="B54" s="18"/>
       <c r="C54" s="18"/>
@@ -13517,7 +13699,7 @@
       <c r="IU54" s="3"/>
       <c r="IV54" s="3"/>
     </row>
-    <row r="55" spans="1:256" ht="12" customHeight="1">
+    <row r="55" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" s="2" t="s">
         <v>142</v>
       </c>
@@ -13777,7 +13959,7 @@
       <c r="IU55" s="3"/>
       <c r="IV55" s="3"/>
     </row>
-    <row r="56" spans="1:256" ht="12" customHeight="1">
+    <row r="56" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A56" s="35" t="s">
         <v>143</v>
       </c>
@@ -14041,7 +14223,7 @@
       <c r="IU56" s="3"/>
       <c r="IV56" s="3"/>
     </row>
-    <row r="57" spans="1:256" ht="12" customHeight="1">
+    <row r="57" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A57" s="36" t="s">
         <v>146</v>
       </c>
@@ -14305,7 +14487,7 @@
       <c r="IU57" s="3"/>
       <c r="IV57" s="3"/>
     </row>
-    <row r="58" spans="1:256" ht="12" customHeight="1">
+    <row r="58" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A58" s="36" t="s">
         <v>149</v>
       </c>
@@ -14569,7 +14751,7 @@
       <c r="IU58" s="3"/>
       <c r="IV58" s="3"/>
     </row>
-    <row r="59" spans="1:256" ht="12" customHeight="1">
+    <row r="59" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A59" s="36" t="s">
         <v>152</v>
       </c>
@@ -14833,7 +15015,7 @@
       <c r="IU59" s="3"/>
       <c r="IV59" s="3"/>
     </row>
-    <row r="60" spans="1:256" ht="12" customHeight="1">
+    <row r="60" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A60" s="36" t="s">
         <v>155</v>
       </c>
@@ -15097,7 +15279,7 @@
       <c r="IU60" s="3"/>
       <c r="IV60" s="3"/>
     </row>
-    <row r="61" spans="1:256" ht="12" customHeight="1">
+    <row r="61" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A61" s="17"/>
       <c r="B61" s="18"/>
       <c r="C61" s="18"/>
@@ -15355,7 +15537,7 @@
       <c r="IU61" s="3"/>
       <c r="IV61" s="3"/>
     </row>
-    <row r="62" spans="1:256" ht="12" customHeight="1">
+    <row r="62" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
         <v>67</v>
       </c>
@@ -15615,7 +15797,7 @@
       <c r="IU62" s="3"/>
       <c r="IV62" s="3"/>
     </row>
-    <row r="63" spans="1:256" ht="16.5" customHeight="1">
+    <row r="63" spans="1:256" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="23" t="s">
         <v>68</v>
       </c>
@@ -15639,7 +15821,7 @@
       <c r="Q63" s="7"/>
       <c r="R63" s="7"/>
     </row>
-    <row r="64" spans="1:256" ht="12" customHeight="1">
+    <row r="64" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A64" s="25" t="s">
         <v>70</v>
       </c>
@@ -15901,7 +16083,7 @@
       <c r="IU64" s="3"/>
       <c r="IV64" s="3"/>
     </row>
-    <row r="65" spans="1:256" ht="15.95" customHeight="1">
+    <row r="65" spans="1:256" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A65" s="3"/>
       <c r="B65" s="3"/>
       <c r="C65" s="7"/>
@@ -16159,7 +16341,7 @@
       <c r="IU65" s="3"/>
       <c r="IV65" s="3"/>
     </row>
-    <row r="66" spans="1:256" ht="15.95" customHeight="1">
+    <row r="66" spans="1:256" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A66" s="3"/>
       <c r="B66" s="3"/>
       <c r="C66" s="7"/>
@@ -16417,7 +16599,7 @@
       <c r="IU66" s="3"/>
       <c r="IV66" s="3"/>
     </row>
-    <row r="67" spans="1:256" ht="15.95" customHeight="1">
+    <row r="67" spans="1:256" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A67" s="3"/>
       <c r="B67" s="3"/>
       <c r="C67" s="7"/>
@@ -16675,7 +16857,7 @@
       <c r="IU67" s="3"/>
       <c r="IV67" s="3"/>
     </row>
-    <row r="68" spans="1:256" ht="15.95" customHeight="1">
+    <row r="68" spans="1:256" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A68" s="3"/>
       <c r="B68" s="3"/>
       <c r="C68" s="7"/>
@@ -16933,7 +17115,7 @@
       <c r="IU68" s="3"/>
       <c r="IV68" s="3"/>
     </row>
-    <row r="69" spans="1:256">
+    <row r="69" spans="1:256" x14ac:dyDescent="0.35">
       <c r="A69" s="3"/>
       <c r="B69" s="3"/>
       <c r="C69" s="7"/>
@@ -17191,7 +17373,7 @@
       <c r="IU69" s="3"/>
       <c r="IV69" s="3"/>
     </row>
-    <row r="70" spans="1:256" ht="15.75" customHeight="1">
+    <row r="70" spans="1:256" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A70" s="3"/>
       <c r="B70" s="3"/>
       <c r="C70" s="7"/>
@@ -17449,7 +17631,7 @@
       <c r="IU70" s="3"/>
       <c r="IV70" s="3"/>
     </row>
-    <row r="71" spans="1:256" ht="15.75" customHeight="1">
+    <row r="71" spans="1:256" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A71" s="3"/>
       <c r="B71" s="3"/>
       <c r="C71" s="3"/>
@@ -17707,7 +17889,7 @@
       <c r="IU71" s="3"/>
       <c r="IV71" s="3"/>
     </row>
-    <row r="72" spans="1:256" ht="12" customHeight="1">
+    <row r="72" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A72" s="3"/>
       <c r="B72" s="3"/>
       <c r="C72" s="3"/>
@@ -17964,7 +18146,7 @@
       <c r="IU72" s="3"/>
       <c r="IV72" s="3"/>
     </row>
-    <row r="73" spans="1:256" ht="15.75" customHeight="1">
+    <row r="73" spans="1:256" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A73" s="3"/>
       <c r="B73" s="3"/>
       <c r="C73" s="3"/>
@@ -18221,7 +18403,7 @@
       <c r="IU73" s="3"/>
       <c r="IV73" s="3"/>
     </row>
-    <row r="74" spans="1:256" ht="15.75" customHeight="1">
+    <row r="74" spans="1:256" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A74" s="3"/>
       <c r="B74" s="3"/>
       <c r="C74" s="3"/>
@@ -18478,7 +18660,7 @@
       <c r="IU74" s="3"/>
       <c r="IV74" s="3"/>
     </row>
-    <row r="75" spans="1:256" ht="15.75" customHeight="1">
+    <row r="75" spans="1:256" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A75" s="3"/>
       <c r="B75" s="3"/>
       <c r="C75" s="3"/>
@@ -18735,7 +18917,7 @@
       <c r="IU75" s="3"/>
       <c r="IV75" s="3"/>
     </row>
-    <row r="76" spans="1:256" ht="15.75" customHeight="1">
+    <row r="76" spans="1:256" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E76" s="3"/>
       <c r="F76" s="3"/>
       <c r="G76" s="3"/>
@@ -18989,7 +19171,7 @@
       <c r="IU76" s="3"/>
       <c r="IV76" s="3"/>
     </row>
-    <row r="77" spans="1:256" ht="12" customHeight="1">
+    <row r="77" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="I77" s="7"/>
       <c r="J77" s="7"/>
       <c r="K77" s="7"/>
@@ -19001,977 +19183,977 @@
       <c r="Q77" s="7"/>
       <c r="R77" s="7"/>
     </row>
-    <row r="78" spans="1:256" ht="15.95" customHeight="1"/>
-    <row r="79" spans="1:256" ht="15.95" customHeight="1"/>
-    <row r="80" spans="1:256" ht="15.95" customHeight="1"/>
-    <row r="81" ht="15.95" customHeight="1"/>
-    <row r="82" ht="15.95" customHeight="1"/>
-    <row r="83" ht="15.95" customHeight="1"/>
-    <row r="84" ht="15.95" customHeight="1"/>
-    <row r="85" ht="15.95" customHeight="1"/>
-    <row r="86" ht="15.95" customHeight="1"/>
-    <row r="87" ht="15.95" customHeight="1"/>
-    <row r="88" ht="15.95" customHeight="1"/>
-    <row r="89" ht="15.95" customHeight="1"/>
-    <row r="90" ht="15.95" customHeight="1"/>
-    <row r="91" ht="15.95" customHeight="1"/>
-    <row r="92" ht="15.95" customHeight="1"/>
-    <row r="93" ht="15.95" customHeight="1"/>
-    <row r="94" ht="15.95" customHeight="1"/>
-    <row r="95" ht="15.95" customHeight="1"/>
-    <row r="96" ht="15.95" customHeight="1"/>
-    <row r="97" ht="15.95" customHeight="1"/>
-    <row r="98" ht="15.95" customHeight="1"/>
-    <row r="99" ht="15.95" customHeight="1"/>
-    <row r="100" ht="15.95" customHeight="1"/>
-    <row r="101" ht="15.95" customHeight="1"/>
-    <row r="102" ht="15.95" customHeight="1"/>
-    <row r="103" ht="15.95" customHeight="1"/>
-    <row r="104" ht="15.95" customHeight="1"/>
-    <row r="105" ht="15.95" customHeight="1"/>
-    <row r="106" ht="15.95" customHeight="1"/>
-    <row r="107" ht="15.95" customHeight="1"/>
-    <row r="108" ht="15.95" customHeight="1"/>
-    <row r="109" ht="15.95" customHeight="1"/>
-    <row r="110" ht="15.95" customHeight="1"/>
-    <row r="111" ht="15.95" customHeight="1"/>
-    <row r="112" ht="15.95" customHeight="1"/>
-    <row r="113" ht="15.95" customHeight="1"/>
-    <row r="114" ht="15.95" customHeight="1"/>
-    <row r="115" ht="15.95" customHeight="1"/>
-    <row r="116" ht="15.95" customHeight="1"/>
-    <row r="117" ht="15.95" customHeight="1"/>
-    <row r="118" ht="15.95" customHeight="1"/>
-    <row r="119" ht="15.95" customHeight="1"/>
-    <row r="120" ht="15.95" customHeight="1"/>
-    <row r="121" ht="15.95" customHeight="1"/>
-    <row r="122" ht="15.95" customHeight="1"/>
-    <row r="123" ht="15.95" customHeight="1"/>
-    <row r="124" ht="15.95" customHeight="1"/>
-    <row r="125" ht="15.95" customHeight="1"/>
-    <row r="126" ht="15.95" customHeight="1"/>
-    <row r="127" ht="15.95" customHeight="1"/>
-    <row r="128" ht="15.95" customHeight="1"/>
-    <row r="129" ht="15.95" customHeight="1"/>
-    <row r="130" ht="15.95" customHeight="1"/>
-    <row r="131" ht="15.95" customHeight="1"/>
-    <row r="132" ht="15.95" customHeight="1"/>
-    <row r="133" ht="15.95" customHeight="1"/>
-    <row r="134" ht="15.95" customHeight="1"/>
-    <row r="135" ht="15.95" customHeight="1"/>
-    <row r="136" ht="15.95" customHeight="1"/>
-    <row r="137" ht="15.95" customHeight="1"/>
-    <row r="138" ht="15.95" customHeight="1"/>
-    <row r="139" ht="15.95" customHeight="1"/>
-    <row r="140" ht="15.95" customHeight="1"/>
-    <row r="141" ht="15.95" customHeight="1"/>
-    <row r="142" ht="15.95" customHeight="1"/>
-    <row r="143" ht="15.95" customHeight="1"/>
-    <row r="144" ht="15.95" customHeight="1"/>
-    <row r="145" ht="15.95" customHeight="1"/>
-    <row r="146" ht="15.95" customHeight="1"/>
-    <row r="147" ht="15.95" customHeight="1"/>
-    <row r="148" ht="15.95" customHeight="1"/>
-    <row r="149" ht="15.95" customHeight="1"/>
-    <row r="150" ht="15.95" customHeight="1"/>
-    <row r="151" ht="15.95" customHeight="1"/>
-    <row r="152" ht="15.95" customHeight="1"/>
-    <row r="153" ht="15.95" customHeight="1"/>
-    <row r="154" ht="15.95" customHeight="1"/>
-    <row r="155" ht="15.95" customHeight="1"/>
-    <row r="156" ht="15.95" customHeight="1"/>
-    <row r="157" ht="15.95" customHeight="1"/>
-    <row r="158" ht="15.95" customHeight="1"/>
-    <row r="159" ht="15.95" customHeight="1"/>
-    <row r="160" ht="15.95" customHeight="1"/>
-    <row r="161" ht="15.95" customHeight="1"/>
-    <row r="162" ht="15.95" customHeight="1"/>
-    <row r="163" ht="15.95" customHeight="1"/>
-    <row r="164" ht="15.95" customHeight="1"/>
-    <row r="165" ht="15.95" customHeight="1"/>
-    <row r="166" ht="15.95" customHeight="1"/>
-    <row r="167" ht="15.95" customHeight="1"/>
-    <row r="168" ht="15.95" customHeight="1"/>
-    <row r="169" ht="15.95" customHeight="1"/>
-    <row r="170" ht="15.95" customHeight="1"/>
-    <row r="171" ht="15.95" customHeight="1"/>
-    <row r="172" ht="15.95" customHeight="1"/>
-    <row r="173" ht="15.95" customHeight="1"/>
-    <row r="174" ht="15.95" customHeight="1"/>
-    <row r="175" ht="15.95" customHeight="1"/>
-    <row r="176" ht="15.95" customHeight="1"/>
-    <row r="177" ht="15.95" customHeight="1"/>
-    <row r="178" ht="15.95" customHeight="1"/>
-    <row r="179" ht="15.95" customHeight="1"/>
-    <row r="180" ht="15.95" customHeight="1"/>
-    <row r="181" ht="15.95" customHeight="1"/>
-    <row r="182" ht="15.95" customHeight="1"/>
-    <row r="183" ht="15.95" customHeight="1"/>
-    <row r="184" ht="15.95" customHeight="1"/>
-    <row r="185" ht="15.95" customHeight="1"/>
-    <row r="186" ht="15.95" customHeight="1"/>
-    <row r="187" ht="15.95" customHeight="1"/>
-    <row r="188" ht="15.95" customHeight="1"/>
-    <row r="189" ht="15.95" customHeight="1"/>
-    <row r="190" ht="15.95" customHeight="1"/>
-    <row r="191" ht="15.95" customHeight="1"/>
-    <row r="192" ht="15.95" customHeight="1"/>
-    <row r="193" ht="15.95" customHeight="1"/>
-    <row r="194" ht="15.95" customHeight="1"/>
-    <row r="195" ht="15.95" customHeight="1"/>
-    <row r="196" ht="15.95" customHeight="1"/>
-    <row r="197" ht="15.95" customHeight="1"/>
-    <row r="198" ht="15.95" customHeight="1"/>
-    <row r="199" ht="15.95" customHeight="1"/>
-    <row r="200" ht="15.95" customHeight="1"/>
-    <row r="201" ht="15.95" customHeight="1"/>
-    <row r="202" ht="15.95" customHeight="1"/>
-    <row r="203" ht="15.95" customHeight="1"/>
-    <row r="204" ht="15.95" customHeight="1"/>
-    <row r="205" ht="15.95" customHeight="1"/>
-    <row r="206" ht="15.95" customHeight="1"/>
-    <row r="207" ht="15.95" customHeight="1"/>
-    <row r="208" ht="15.95" customHeight="1"/>
-    <row r="209" ht="15.95" customHeight="1"/>
-    <row r="210" ht="15.95" customHeight="1"/>
-    <row r="211" ht="15.95" customHeight="1"/>
-    <row r="212" ht="15.95" customHeight="1"/>
-    <row r="213" ht="15.95" customHeight="1"/>
-    <row r="214" ht="15.95" customHeight="1"/>
-    <row r="215" ht="15.95" customHeight="1"/>
-    <row r="216" ht="15.95" customHeight="1"/>
-    <row r="217" ht="15.95" customHeight="1"/>
-    <row r="218" ht="15.95" customHeight="1"/>
-    <row r="219" ht="15.95" customHeight="1"/>
-    <row r="220" ht="15.95" customHeight="1"/>
-    <row r="221" ht="15.95" customHeight="1"/>
-    <row r="222" ht="15.95" customHeight="1"/>
-    <row r="223" ht="15.95" customHeight="1"/>
-    <row r="224" ht="15.95" customHeight="1"/>
-    <row r="225" ht="15.95" customHeight="1"/>
-    <row r="226" ht="15.95" customHeight="1"/>
-    <row r="227" ht="15.95" customHeight="1"/>
-    <row r="228" ht="15.95" customHeight="1"/>
-    <row r="229" ht="15.95" customHeight="1"/>
-    <row r="230" ht="15.95" customHeight="1"/>
-    <row r="231" ht="15.95" customHeight="1"/>
-    <row r="232" ht="15.95" customHeight="1"/>
-    <row r="233" ht="15.95" customHeight="1"/>
-    <row r="234" ht="15.95" customHeight="1"/>
-    <row r="235" ht="15.95" customHeight="1"/>
-    <row r="236" ht="15.95" customHeight="1"/>
-    <row r="237" ht="15.95" customHeight="1"/>
-    <row r="238" ht="15.95" customHeight="1"/>
-    <row r="239" ht="15.95" customHeight="1"/>
-    <row r="240" ht="15.95" customHeight="1"/>
-    <row r="241" ht="15.95" customHeight="1"/>
-    <row r="242" ht="15.95" customHeight="1"/>
-    <row r="243" ht="15.95" customHeight="1"/>
-    <row r="244" ht="15.95" customHeight="1"/>
-    <row r="245" ht="15.95" customHeight="1"/>
-    <row r="246" ht="15.95" customHeight="1"/>
-    <row r="247" ht="15.95" customHeight="1"/>
-    <row r="248" ht="15.95" customHeight="1"/>
-    <row r="249" ht="15.95" customHeight="1"/>
-    <row r="250" ht="15.95" customHeight="1"/>
-    <row r="251" ht="15.95" customHeight="1"/>
-    <row r="252" ht="15.95" customHeight="1"/>
-    <row r="253" ht="15.95" customHeight="1"/>
-    <row r="254" ht="15.95" customHeight="1"/>
-    <row r="255" ht="15.95" customHeight="1"/>
-    <row r="256" ht="15.95" customHeight="1"/>
-    <row r="257" ht="15.95" customHeight="1"/>
-    <row r="258" ht="15.95" customHeight="1"/>
-    <row r="259" ht="15.95" customHeight="1"/>
-    <row r="260" ht="15.95" customHeight="1"/>
-    <row r="261" ht="15.95" customHeight="1"/>
-    <row r="262" ht="15.95" customHeight="1"/>
-    <row r="263" ht="15.95" customHeight="1"/>
-    <row r="264" ht="15.95" customHeight="1"/>
-    <row r="265" ht="15.95" customHeight="1"/>
-    <row r="266" ht="15.95" customHeight="1"/>
-    <row r="267" ht="15.95" customHeight="1"/>
-    <row r="268" ht="15.95" customHeight="1"/>
-    <row r="269" ht="15.95" customHeight="1"/>
-    <row r="270" ht="15.95" customHeight="1"/>
-    <row r="271" ht="15.95" customHeight="1"/>
-    <row r="272" ht="15.95" customHeight="1"/>
-    <row r="273" ht="15.95" customHeight="1"/>
-    <row r="274" ht="15.95" customHeight="1"/>
-    <row r="275" ht="15.95" customHeight="1"/>
-    <row r="276" ht="15.95" customHeight="1"/>
-    <row r="277" ht="15.95" customHeight="1"/>
-    <row r="278" ht="15.95" customHeight="1"/>
-    <row r="279" ht="15.95" customHeight="1"/>
-    <row r="280" ht="15.95" customHeight="1"/>
-    <row r="281" ht="15.95" customHeight="1"/>
-    <row r="282" ht="15.95" customHeight="1"/>
-    <row r="283" ht="15.95" customHeight="1"/>
-    <row r="284" ht="15.95" customHeight="1"/>
-    <row r="285" ht="15.95" customHeight="1"/>
-    <row r="286" ht="15.95" customHeight="1"/>
-    <row r="287" ht="15.95" customHeight="1"/>
-    <row r="288" ht="15.95" customHeight="1"/>
-    <row r="289" ht="15.95" customHeight="1"/>
-    <row r="290" ht="15.95" customHeight="1"/>
-    <row r="291" ht="15.95" customHeight="1"/>
-    <row r="292" ht="15.95" customHeight="1"/>
-    <row r="293" ht="15.95" customHeight="1"/>
-    <row r="294" ht="15.95" customHeight="1"/>
-    <row r="295" ht="15.95" customHeight="1"/>
-    <row r="296" ht="15.95" customHeight="1"/>
-    <row r="297" ht="15.95" customHeight="1"/>
-    <row r="298" ht="15.95" customHeight="1"/>
-    <row r="299" ht="15.95" customHeight="1"/>
-    <row r="300" ht="15.95" customHeight="1"/>
-    <row r="301" ht="15.95" customHeight="1"/>
-    <row r="302" ht="15.95" customHeight="1"/>
-    <row r="303" ht="15.95" customHeight="1"/>
-    <row r="304" ht="15.95" customHeight="1"/>
-    <row r="305" ht="15.95" customHeight="1"/>
-    <row r="306" ht="15.95" customHeight="1"/>
-    <row r="307" ht="15.95" customHeight="1"/>
-    <row r="308" ht="15.95" customHeight="1"/>
-    <row r="309" ht="15.95" customHeight="1"/>
-    <row r="310" ht="15.95" customHeight="1"/>
-    <row r="311" ht="15.95" customHeight="1"/>
-    <row r="312" ht="15.95" customHeight="1"/>
-    <row r="313" ht="15.95" customHeight="1"/>
-    <row r="314" ht="15.95" customHeight="1"/>
-    <row r="315" ht="15.95" customHeight="1"/>
-    <row r="316" ht="15.95" customHeight="1"/>
-    <row r="317" ht="15.95" customHeight="1"/>
-    <row r="318" ht="15.95" customHeight="1"/>
-    <row r="319" ht="15.95" customHeight="1"/>
-    <row r="320" ht="15.95" customHeight="1"/>
-    <row r="321" ht="15.95" customHeight="1"/>
-    <row r="322" ht="15.95" customHeight="1"/>
-    <row r="323" ht="15.95" customHeight="1"/>
-    <row r="324" ht="15.95" customHeight="1"/>
-    <row r="325" ht="15.95" customHeight="1"/>
-    <row r="326" ht="15.95" customHeight="1"/>
-    <row r="327" ht="15.95" customHeight="1"/>
-    <row r="328" ht="15.95" customHeight="1"/>
-    <row r="329" ht="15.95" customHeight="1"/>
-    <row r="330" ht="15.95" customHeight="1"/>
-    <row r="331" ht="15.95" customHeight="1"/>
-    <row r="332" ht="15.95" customHeight="1"/>
-    <row r="333" ht="15.95" customHeight="1"/>
-    <row r="334" ht="15.95" customHeight="1"/>
-    <row r="335" ht="15.95" customHeight="1"/>
-    <row r="336" ht="15.95" customHeight="1"/>
-    <row r="337" ht="15.95" customHeight="1"/>
-    <row r="338" ht="15.95" customHeight="1"/>
-    <row r="339" ht="15.95" customHeight="1"/>
-    <row r="340" ht="15.95" customHeight="1"/>
-    <row r="341" ht="15.95" customHeight="1"/>
-    <row r="342" ht="15.95" customHeight="1"/>
-    <row r="343" ht="15.95" customHeight="1"/>
-    <row r="344" ht="15.95" customHeight="1"/>
-    <row r="345" ht="15.95" customHeight="1"/>
-    <row r="346" ht="15.95" customHeight="1"/>
-    <row r="347" ht="15.95" customHeight="1"/>
-    <row r="348" ht="15.95" customHeight="1"/>
-    <row r="349" ht="15.95" customHeight="1"/>
-    <row r="350" ht="15.95" customHeight="1"/>
-    <row r="351" ht="15.95" customHeight="1"/>
-    <row r="352" ht="15.95" customHeight="1"/>
-    <row r="353" ht="15.95" customHeight="1"/>
-    <row r="354" ht="15.95" customHeight="1"/>
-    <row r="355" ht="15.95" customHeight="1"/>
-    <row r="356" ht="15.95" customHeight="1"/>
-    <row r="357" ht="15.95" customHeight="1"/>
-    <row r="358" ht="15.95" customHeight="1"/>
-    <row r="359" ht="15.95" customHeight="1"/>
-    <row r="360" ht="15.95" customHeight="1"/>
-    <row r="361" ht="15.95" customHeight="1"/>
-    <row r="362" ht="15.95" customHeight="1"/>
-    <row r="363" ht="15.95" customHeight="1"/>
-    <row r="364" ht="15.95" customHeight="1"/>
-    <row r="365" ht="15.95" customHeight="1"/>
-    <row r="366" ht="15.95" customHeight="1"/>
-    <row r="367" ht="15.95" customHeight="1"/>
-    <row r="368" ht="15.95" customHeight="1"/>
-    <row r="369" ht="15.95" customHeight="1"/>
-    <row r="370" ht="15.95" customHeight="1"/>
-    <row r="371" ht="15.95" customHeight="1"/>
-    <row r="372" ht="15.95" customHeight="1"/>
-    <row r="373" ht="15.95" customHeight="1"/>
-    <row r="374" ht="15.95" customHeight="1"/>
-    <row r="375" ht="15.95" customHeight="1"/>
-    <row r="376" ht="15.95" customHeight="1"/>
-    <row r="377" ht="15.95" customHeight="1"/>
-    <row r="378" ht="15.95" customHeight="1"/>
-    <row r="379" ht="15.95" customHeight="1"/>
-    <row r="380" ht="15.95" customHeight="1"/>
-    <row r="381" ht="15.95" customHeight="1"/>
-    <row r="382" ht="15.95" customHeight="1"/>
-    <row r="383" ht="15.95" customHeight="1"/>
-    <row r="384" ht="15.95" customHeight="1"/>
-    <row r="385" ht="15.95" customHeight="1"/>
-    <row r="386" ht="15.95" customHeight="1"/>
-    <row r="387" ht="15.95" customHeight="1"/>
-    <row r="388" ht="15.95" customHeight="1"/>
-    <row r="389" ht="15.95" customHeight="1"/>
-    <row r="390" ht="15.95" customHeight="1"/>
-    <row r="391" ht="15.95" customHeight="1"/>
-    <row r="392" ht="15.95" customHeight="1"/>
-    <row r="393" ht="15.95" customHeight="1"/>
-    <row r="394" ht="15.95" customHeight="1"/>
-    <row r="395" ht="15.95" customHeight="1"/>
-    <row r="396" ht="15.95" customHeight="1"/>
-    <row r="397" ht="15.95" customHeight="1"/>
-    <row r="398" ht="15.95" customHeight="1"/>
-    <row r="399" ht="15.95" customHeight="1"/>
-    <row r="400" ht="15.95" customHeight="1"/>
-    <row r="401" ht="15.95" customHeight="1"/>
-    <row r="402" ht="15.95" customHeight="1"/>
-    <row r="403" ht="15.95" customHeight="1"/>
-    <row r="404" ht="15.95" customHeight="1"/>
-    <row r="405" ht="15.95" customHeight="1"/>
-    <row r="406" ht="15.95" customHeight="1"/>
-    <row r="407" ht="15.95" customHeight="1"/>
-    <row r="408" ht="15.95" customHeight="1"/>
-    <row r="409" ht="15.95" customHeight="1"/>
-    <row r="410" ht="15.95" customHeight="1"/>
-    <row r="411" ht="15.95" customHeight="1"/>
-    <row r="412" ht="15.95" customHeight="1"/>
-    <row r="413" ht="15.95" customHeight="1"/>
-    <row r="414" ht="15.95" customHeight="1"/>
-    <row r="415" ht="15.95" customHeight="1"/>
-    <row r="416" ht="15.95" customHeight="1"/>
-    <row r="417" ht="15.95" customHeight="1"/>
-    <row r="418" ht="15.95" customHeight="1"/>
-    <row r="419" ht="15.95" customHeight="1"/>
-    <row r="420" ht="15.95" customHeight="1"/>
-    <row r="421" ht="15.95" customHeight="1"/>
-    <row r="422" ht="15.95" customHeight="1"/>
-    <row r="423" ht="15.95" customHeight="1"/>
-    <row r="424" ht="15.95" customHeight="1"/>
-    <row r="425" ht="15.95" customHeight="1"/>
-    <row r="426" ht="15.95" customHeight="1"/>
-    <row r="427" ht="15.95" customHeight="1"/>
-    <row r="428" ht="15.95" customHeight="1"/>
-    <row r="429" ht="15.95" customHeight="1"/>
-    <row r="430" ht="15.95" customHeight="1"/>
-    <row r="431" ht="15.95" customHeight="1"/>
-    <row r="432" ht="15.95" customHeight="1"/>
-    <row r="433" ht="15.95" customHeight="1"/>
-    <row r="434" ht="15.95" customHeight="1"/>
-    <row r="435" ht="15.95" customHeight="1"/>
-    <row r="436" ht="15.95" customHeight="1"/>
-    <row r="437" ht="15.95" customHeight="1"/>
-    <row r="438" ht="15.95" customHeight="1"/>
-    <row r="439" ht="15.95" customHeight="1"/>
-    <row r="440" ht="15.95" customHeight="1"/>
-    <row r="441" ht="15.95" customHeight="1"/>
-    <row r="442" ht="15.95" customHeight="1"/>
-    <row r="443" ht="15.95" customHeight="1"/>
-    <row r="444" ht="15.95" customHeight="1"/>
-    <row r="445" ht="15.95" customHeight="1"/>
-    <row r="446" ht="15.95" customHeight="1"/>
-    <row r="447" ht="15.95" customHeight="1"/>
-    <row r="448" ht="15.95" customHeight="1"/>
-    <row r="449" ht="15.95" customHeight="1"/>
-    <row r="450" ht="15.95" customHeight="1"/>
-    <row r="451" ht="15.95" customHeight="1"/>
-    <row r="452" ht="15.95" customHeight="1"/>
-    <row r="453" ht="15.95" customHeight="1"/>
-    <row r="454" ht="15.95" customHeight="1"/>
-    <row r="455" ht="15.95" customHeight="1"/>
-    <row r="456" ht="15.95" customHeight="1"/>
-    <row r="457" ht="15.95" customHeight="1"/>
-    <row r="458" ht="15.95" customHeight="1"/>
-    <row r="459" ht="15.95" customHeight="1"/>
-    <row r="460" ht="15.95" customHeight="1"/>
-    <row r="461" ht="15.95" customHeight="1"/>
-    <row r="462" ht="15.95" customHeight="1"/>
-    <row r="463" ht="15.95" customHeight="1"/>
-    <row r="464" ht="15.95" customHeight="1"/>
-    <row r="465" ht="15.95" customHeight="1"/>
-    <row r="466" ht="15.95" customHeight="1"/>
-    <row r="467" ht="15.95" customHeight="1"/>
-    <row r="468" ht="15.95" customHeight="1"/>
-    <row r="469" ht="15.95" customHeight="1"/>
-    <row r="470" ht="15.95" customHeight="1"/>
-    <row r="471" ht="15.95" customHeight="1"/>
-    <row r="472" ht="15.95" customHeight="1"/>
-    <row r="473" ht="15.95" customHeight="1"/>
-    <row r="474" ht="15.95" customHeight="1"/>
-    <row r="475" ht="15.95" customHeight="1"/>
-    <row r="476" ht="15.95" customHeight="1"/>
-    <row r="477" ht="15.95" customHeight="1"/>
-    <row r="478" ht="15.95" customHeight="1"/>
-    <row r="479" ht="15.95" customHeight="1"/>
-    <row r="480" ht="15.95" customHeight="1"/>
-    <row r="481" ht="15.95" customHeight="1"/>
-    <row r="482" ht="15.95" customHeight="1"/>
-    <row r="483" ht="15.95" customHeight="1"/>
-    <row r="484" ht="15.95" customHeight="1"/>
-    <row r="485" ht="15.95" customHeight="1"/>
-    <row r="486" ht="15.95" customHeight="1"/>
-    <row r="487" ht="15.95" customHeight="1"/>
-    <row r="488" ht="15.95" customHeight="1"/>
-    <row r="489" ht="15.95" customHeight="1"/>
-    <row r="490" ht="15.95" customHeight="1"/>
-    <row r="491" ht="15.95" customHeight="1"/>
-    <row r="492" ht="15.95" customHeight="1"/>
-    <row r="493" ht="15.95" customHeight="1"/>
-    <row r="494" ht="15.95" customHeight="1"/>
-    <row r="495" ht="15.95" customHeight="1"/>
-    <row r="496" ht="15.95" customHeight="1"/>
-    <row r="497" ht="15.95" customHeight="1"/>
-    <row r="498" ht="15.95" customHeight="1"/>
-    <row r="499" ht="15.95" customHeight="1"/>
-    <row r="500" ht="15.95" customHeight="1"/>
-    <row r="501" ht="15.95" customHeight="1"/>
-    <row r="502" ht="15.95" customHeight="1"/>
-    <row r="503" ht="15.95" customHeight="1"/>
-    <row r="504" ht="15.95" customHeight="1"/>
-    <row r="505" ht="15.95" customHeight="1"/>
-    <row r="506" ht="15.95" customHeight="1"/>
-    <row r="507" ht="15.95" customHeight="1"/>
-    <row r="508" ht="15.95" customHeight="1"/>
-    <row r="509" ht="15.95" customHeight="1"/>
-    <row r="510" ht="15.95" customHeight="1"/>
-    <row r="511" ht="15.95" customHeight="1"/>
-    <row r="512" ht="15.95" customHeight="1"/>
-    <row r="513" ht="15.95" customHeight="1"/>
-    <row r="514" ht="15.95" customHeight="1"/>
-    <row r="515" ht="15.95" customHeight="1"/>
-    <row r="516" ht="15.95" customHeight="1"/>
-    <row r="517" ht="15.95" customHeight="1"/>
-    <row r="518" ht="15.95" customHeight="1"/>
-    <row r="519" ht="15.95" customHeight="1"/>
-    <row r="520" ht="15.95" customHeight="1"/>
-    <row r="521" ht="15.95" customHeight="1"/>
-    <row r="522" ht="15.95" customHeight="1"/>
-    <row r="523" ht="15.95" customHeight="1"/>
-    <row r="524" ht="15.95" customHeight="1"/>
-    <row r="525" ht="15.95" customHeight="1"/>
-    <row r="526" ht="15.95" customHeight="1"/>
-    <row r="527" ht="15.95" customHeight="1"/>
-    <row r="528" ht="15.95" customHeight="1"/>
-    <row r="529" ht="15.95" customHeight="1"/>
-    <row r="530" ht="15.95" customHeight="1"/>
-    <row r="531" ht="15.95" customHeight="1"/>
-    <row r="532" ht="15.95" customHeight="1"/>
-    <row r="533" ht="15.95" customHeight="1"/>
-    <row r="534" ht="15.95" customHeight="1"/>
-    <row r="535" ht="15.95" customHeight="1"/>
-    <row r="536" ht="15.95" customHeight="1"/>
-    <row r="537" ht="15.95" customHeight="1"/>
-    <row r="538" ht="15.95" customHeight="1"/>
-    <row r="539" ht="15.95" customHeight="1"/>
-    <row r="540" ht="15.95" customHeight="1"/>
-    <row r="541" ht="15.95" customHeight="1"/>
-    <row r="542" ht="15.95" customHeight="1"/>
-    <row r="543" ht="15.95" customHeight="1"/>
-    <row r="544" ht="15.95" customHeight="1"/>
-    <row r="545" ht="15.95" customHeight="1"/>
-    <row r="546" ht="15.95" customHeight="1"/>
-    <row r="547" ht="15.95" customHeight="1"/>
-    <row r="548" ht="15.95" customHeight="1"/>
-    <row r="549" ht="15.95" customHeight="1"/>
-    <row r="550" ht="15.95" customHeight="1"/>
-    <row r="551" ht="15.95" customHeight="1"/>
-    <row r="552" ht="15.95" customHeight="1"/>
-    <row r="553" ht="15.95" customHeight="1"/>
-    <row r="554" ht="15.95" customHeight="1"/>
-    <row r="555" ht="15.95" customHeight="1"/>
-    <row r="556" ht="15.95" customHeight="1"/>
-    <row r="557" ht="15.95" customHeight="1"/>
-    <row r="558" ht="15.95" customHeight="1"/>
-    <row r="559" ht="15.95" customHeight="1"/>
-    <row r="560" ht="15.95" customHeight="1"/>
-    <row r="561" ht="15.95" customHeight="1"/>
-    <row r="562" ht="15.95" customHeight="1"/>
-    <row r="563" ht="15.95" customHeight="1"/>
-    <row r="564" ht="15.95" customHeight="1"/>
-    <row r="565" ht="15.95" customHeight="1"/>
-    <row r="566" ht="15.95" customHeight="1"/>
-    <row r="567" ht="15.95" customHeight="1"/>
-    <row r="568" ht="15.95" customHeight="1"/>
-    <row r="569" ht="15.95" customHeight="1"/>
-    <row r="570" ht="15.95" customHeight="1"/>
-    <row r="571" ht="15.95" customHeight="1"/>
-    <row r="572" ht="15.95" customHeight="1"/>
-    <row r="573" ht="15.95" customHeight="1"/>
-    <row r="574" ht="15.95" customHeight="1"/>
-    <row r="575" ht="15.95" customHeight="1"/>
-    <row r="576" ht="15.95" customHeight="1"/>
-    <row r="577" ht="15.95" customHeight="1"/>
-    <row r="578" ht="15.95" customHeight="1"/>
-    <row r="579" ht="15.95" customHeight="1"/>
-    <row r="580" ht="15.95" customHeight="1"/>
-    <row r="581" ht="15.95" customHeight="1"/>
-    <row r="582" ht="15.95" customHeight="1"/>
-    <row r="583" ht="15.95" customHeight="1"/>
-    <row r="584" ht="15.95" customHeight="1"/>
-    <row r="585" ht="15.95" customHeight="1"/>
-    <row r="586" ht="15.95" customHeight="1"/>
-    <row r="587" ht="15.95" customHeight="1"/>
-    <row r="588" ht="15.95" customHeight="1"/>
-    <row r="589" ht="15.95" customHeight="1"/>
-    <row r="590" ht="15.95" customHeight="1"/>
-    <row r="591" ht="15.95" customHeight="1"/>
-    <row r="592" ht="15.95" customHeight="1"/>
-    <row r="593" ht="15.95" customHeight="1"/>
-    <row r="594" ht="15.95" customHeight="1"/>
-    <row r="595" ht="15.95" customHeight="1"/>
-    <row r="596" ht="15.95" customHeight="1"/>
-    <row r="597" ht="15.95" customHeight="1"/>
-    <row r="598" ht="15.95" customHeight="1"/>
-    <row r="599" ht="15.95" customHeight="1"/>
-    <row r="600" ht="15.95" customHeight="1"/>
-    <row r="601" ht="15.95" customHeight="1"/>
-    <row r="602" ht="15.95" customHeight="1"/>
-    <row r="603" ht="15.95" customHeight="1"/>
-    <row r="604" ht="15.95" customHeight="1"/>
-    <row r="605" ht="15.95" customHeight="1"/>
-    <row r="606" ht="15.95" customHeight="1"/>
-    <row r="607" ht="15.95" customHeight="1"/>
-    <row r="608" ht="15.95" customHeight="1"/>
-    <row r="609" ht="15.95" customHeight="1"/>
-    <row r="610" ht="15.95" customHeight="1"/>
-    <row r="611" ht="15.95" customHeight="1"/>
-    <row r="612" ht="15.95" customHeight="1"/>
-    <row r="613" ht="15.95" customHeight="1"/>
-    <row r="614" ht="15.95" customHeight="1"/>
-    <row r="615" ht="15.95" customHeight="1"/>
-    <row r="616" ht="15.95" customHeight="1"/>
-    <row r="617" ht="15.95" customHeight="1"/>
-    <row r="618" ht="15.95" customHeight="1"/>
-    <row r="619" ht="15.95" customHeight="1"/>
-    <row r="620" ht="15.95" customHeight="1"/>
-    <row r="621" ht="15.95" customHeight="1"/>
-    <row r="622" ht="15.95" customHeight="1"/>
-    <row r="623" ht="15.95" customHeight="1"/>
-    <row r="624" ht="15.95" customHeight="1"/>
-    <row r="625" ht="15.95" customHeight="1"/>
-    <row r="626" ht="15.95" customHeight="1"/>
-    <row r="627" ht="15.95" customHeight="1"/>
-    <row r="628" ht="15.95" customHeight="1"/>
-    <row r="629" ht="15.95" customHeight="1"/>
-    <row r="630" ht="15.95" customHeight="1"/>
-    <row r="631" ht="15.95" customHeight="1"/>
-    <row r="632" ht="15.95" customHeight="1"/>
-    <row r="633" ht="15.95" customHeight="1"/>
-    <row r="634" ht="15.95" customHeight="1"/>
-    <row r="635" ht="15.95" customHeight="1"/>
-    <row r="636" ht="15.95" customHeight="1"/>
-    <row r="637" ht="15.95" customHeight="1"/>
-    <row r="638" ht="15.95" customHeight="1"/>
-    <row r="639" ht="15.95" customHeight="1"/>
-    <row r="640" ht="15.95" customHeight="1"/>
-    <row r="641" ht="15.95" customHeight="1"/>
-    <row r="642" ht="15.95" customHeight="1"/>
-    <row r="643" ht="15.95" customHeight="1"/>
-    <row r="644" ht="15.95" customHeight="1"/>
-    <row r="645" ht="15.95" customHeight="1"/>
-    <row r="646" ht="15.95" customHeight="1"/>
-    <row r="647" ht="15.95" customHeight="1"/>
-    <row r="648" ht="15.95" customHeight="1"/>
-    <row r="649" ht="15.95" customHeight="1"/>
-    <row r="650" ht="15.95" customHeight="1"/>
-    <row r="651" ht="15.95" customHeight="1"/>
-    <row r="652" ht="15.95" customHeight="1"/>
-    <row r="653" ht="15.95" customHeight="1"/>
-    <row r="654" ht="15.95" customHeight="1"/>
-    <row r="655" ht="15.95" customHeight="1"/>
-    <row r="656" ht="15.95" customHeight="1"/>
-    <row r="657" ht="15.95" customHeight="1"/>
-    <row r="658" ht="15.95" customHeight="1"/>
-    <row r="659" ht="15.95" customHeight="1"/>
-    <row r="660" ht="15.95" customHeight="1"/>
-    <row r="661" ht="15.95" customHeight="1"/>
-    <row r="662" ht="15.95" customHeight="1"/>
-    <row r="663" ht="15.95" customHeight="1"/>
-    <row r="664" ht="15.95" customHeight="1"/>
-    <row r="665" ht="15.95" customHeight="1"/>
-    <row r="666" ht="15.95" customHeight="1"/>
-    <row r="667" ht="15.95" customHeight="1"/>
-    <row r="668" ht="15.95" customHeight="1"/>
-    <row r="669" ht="15.95" customHeight="1"/>
-    <row r="670" ht="15.95" customHeight="1"/>
-    <row r="671" ht="15.95" customHeight="1"/>
-    <row r="672" ht="15.95" customHeight="1"/>
-    <row r="673" ht="15.95" customHeight="1"/>
-    <row r="674" ht="15.95" customHeight="1"/>
-    <row r="675" ht="15.95" customHeight="1"/>
-    <row r="676" ht="15.95" customHeight="1"/>
-    <row r="677" ht="15.95" customHeight="1"/>
-    <row r="678" ht="15.95" customHeight="1"/>
-    <row r="679" ht="15.95" customHeight="1"/>
-    <row r="680" ht="15.95" customHeight="1"/>
-    <row r="681" ht="15.95" customHeight="1"/>
-    <row r="682" ht="15.95" customHeight="1"/>
-    <row r="683" ht="15.95" customHeight="1"/>
-    <row r="684" ht="15.95" customHeight="1"/>
-    <row r="685" ht="15.95" customHeight="1"/>
-    <row r="686" ht="15.95" customHeight="1"/>
-    <row r="687" ht="15.95" customHeight="1"/>
-    <row r="688" ht="15.95" customHeight="1"/>
-    <row r="689" ht="15.95" customHeight="1"/>
-    <row r="690" ht="15.95" customHeight="1"/>
-    <row r="691" ht="15.95" customHeight="1"/>
-    <row r="692" ht="15.95" customHeight="1"/>
-    <row r="693" ht="15.95" customHeight="1"/>
-    <row r="694" ht="15.95" customHeight="1"/>
-    <row r="695" ht="15.95" customHeight="1"/>
-    <row r="696" ht="15.95" customHeight="1"/>
-    <row r="697" ht="15.95" customHeight="1"/>
-    <row r="698" ht="15.95" customHeight="1"/>
-    <row r="699" ht="15.95" customHeight="1"/>
-    <row r="700" ht="15.95" customHeight="1"/>
-    <row r="701" ht="15.95" customHeight="1"/>
-    <row r="702" ht="15.95" customHeight="1"/>
-    <row r="703" ht="15.95" customHeight="1"/>
-    <row r="704" ht="15.95" customHeight="1"/>
-    <row r="705" ht="15.95" customHeight="1"/>
-    <row r="706" ht="15.95" customHeight="1"/>
-    <row r="707" ht="15.95" customHeight="1"/>
-    <row r="708" ht="15.95" customHeight="1"/>
-    <row r="709" ht="15.95" customHeight="1"/>
-    <row r="710" ht="15.95" customHeight="1"/>
-    <row r="711" ht="15.95" customHeight="1"/>
-    <row r="712" ht="15.95" customHeight="1"/>
-    <row r="713" ht="15.95" customHeight="1"/>
-    <row r="714" ht="15.95" customHeight="1"/>
-    <row r="715" ht="15.95" customHeight="1"/>
-    <row r="716" ht="15.95" customHeight="1"/>
-    <row r="717" ht="15.95" customHeight="1"/>
-    <row r="718" ht="15.95" customHeight="1"/>
-    <row r="719" ht="15.95" customHeight="1"/>
-    <row r="720" ht="15.95" customHeight="1"/>
-    <row r="721" ht="15.95" customHeight="1"/>
-    <row r="722" ht="15.95" customHeight="1"/>
-    <row r="723" ht="15.95" customHeight="1"/>
-    <row r="724" ht="15.95" customHeight="1"/>
-    <row r="725" ht="15.95" customHeight="1"/>
-    <row r="726" ht="15.95" customHeight="1"/>
-    <row r="727" ht="15.95" customHeight="1"/>
-    <row r="728" ht="15.95" customHeight="1"/>
-    <row r="729" ht="15.95" customHeight="1"/>
-    <row r="730" ht="15.95" customHeight="1"/>
-    <row r="731" ht="15.95" customHeight="1"/>
-    <row r="732" ht="15.95" customHeight="1"/>
-    <row r="733" ht="15.95" customHeight="1"/>
-    <row r="734" ht="15.95" customHeight="1"/>
-    <row r="735" ht="15.95" customHeight="1"/>
-    <row r="736" ht="15.95" customHeight="1"/>
-    <row r="737" ht="15.95" customHeight="1"/>
-    <row r="738" ht="15.95" customHeight="1"/>
-    <row r="739" ht="15.95" customHeight="1"/>
-    <row r="740" ht="15.95" customHeight="1"/>
-    <row r="741" ht="15.95" customHeight="1"/>
-    <row r="742" ht="15.95" customHeight="1"/>
-    <row r="743" ht="15.95" customHeight="1"/>
-    <row r="744" ht="15.95" customHeight="1"/>
-    <row r="745" ht="15.95" customHeight="1"/>
-    <row r="746" ht="15.95" customHeight="1"/>
-    <row r="747" ht="15.95" customHeight="1"/>
-    <row r="748" ht="15.95" customHeight="1"/>
-    <row r="749" ht="15.95" customHeight="1"/>
-    <row r="750" ht="15.95" customHeight="1"/>
-    <row r="751" ht="15.95" customHeight="1"/>
-    <row r="752" ht="15.95" customHeight="1"/>
-    <row r="753" ht="15.95" customHeight="1"/>
-    <row r="754" ht="15.95" customHeight="1"/>
-    <row r="755" ht="15.95" customHeight="1"/>
-    <row r="756" ht="15.95" customHeight="1"/>
-    <row r="757" ht="15.95" customHeight="1"/>
-    <row r="758" ht="15.95" customHeight="1"/>
-    <row r="759" ht="15.95" customHeight="1"/>
-    <row r="760" ht="15.95" customHeight="1"/>
-    <row r="761" ht="15.95" customHeight="1"/>
-    <row r="762" ht="15.95" customHeight="1"/>
-    <row r="763" ht="15.95" customHeight="1"/>
-    <row r="764" ht="15.95" customHeight="1"/>
-    <row r="765" ht="15.95" customHeight="1"/>
-    <row r="766" ht="15.95" customHeight="1"/>
-    <row r="767" ht="15.95" customHeight="1"/>
-    <row r="768" ht="15.95" customHeight="1"/>
-    <row r="769" ht="15.95" customHeight="1"/>
-    <row r="770" ht="15.95" customHeight="1"/>
-    <row r="771" ht="15.95" customHeight="1"/>
-    <row r="772" ht="15.95" customHeight="1"/>
-    <row r="773" ht="15.95" customHeight="1"/>
-    <row r="774" ht="15.95" customHeight="1"/>
-    <row r="775" ht="15.95" customHeight="1"/>
-    <row r="776" ht="15.95" customHeight="1"/>
-    <row r="777" ht="15.95" customHeight="1"/>
-    <row r="778" ht="15.95" customHeight="1"/>
-    <row r="779" ht="15.95" customHeight="1"/>
-    <row r="780" ht="15.95" customHeight="1"/>
-    <row r="781" ht="15.95" customHeight="1"/>
-    <row r="782" ht="15.95" customHeight="1"/>
-    <row r="783" ht="15.95" customHeight="1"/>
-    <row r="784" ht="15.95" customHeight="1"/>
-    <row r="785" ht="15.95" customHeight="1"/>
-    <row r="786" ht="15.95" customHeight="1"/>
-    <row r="787" ht="15.95" customHeight="1"/>
-    <row r="788" ht="15.95" customHeight="1"/>
-    <row r="789" ht="15.95" customHeight="1"/>
-    <row r="790" ht="15.95" customHeight="1"/>
-    <row r="791" ht="15.95" customHeight="1"/>
-    <row r="792" ht="15.95" customHeight="1"/>
-    <row r="793" ht="15.95" customHeight="1"/>
-    <row r="794" ht="15.95" customHeight="1"/>
-    <row r="795" ht="15.95" customHeight="1"/>
-    <row r="796" ht="15.95" customHeight="1"/>
-    <row r="797" ht="15.95" customHeight="1"/>
-    <row r="798" ht="15.95" customHeight="1"/>
-    <row r="799" ht="15.95" customHeight="1"/>
-    <row r="800" ht="15.95" customHeight="1"/>
-    <row r="801" ht="15.95" customHeight="1"/>
-    <row r="802" ht="15.95" customHeight="1"/>
-    <row r="803" ht="15.95" customHeight="1"/>
-    <row r="804" ht="15.95" customHeight="1"/>
-    <row r="805" ht="15.95" customHeight="1"/>
-    <row r="806" ht="15.95" customHeight="1"/>
-    <row r="807" ht="15.95" customHeight="1"/>
-    <row r="808" ht="15.95" customHeight="1"/>
-    <row r="809" ht="15.95" customHeight="1"/>
-    <row r="810" ht="15.95" customHeight="1"/>
-    <row r="811" ht="15.95" customHeight="1"/>
-    <row r="812" ht="15.95" customHeight="1"/>
-    <row r="813" ht="15.95" customHeight="1"/>
-    <row r="814" ht="15.95" customHeight="1"/>
-    <row r="815" ht="15.95" customHeight="1"/>
-    <row r="816" ht="15.95" customHeight="1"/>
-    <row r="817" ht="15.95" customHeight="1"/>
-    <row r="818" ht="15.95" customHeight="1"/>
-    <row r="819" ht="15.95" customHeight="1"/>
-    <row r="820" ht="15.95" customHeight="1"/>
-    <row r="821" ht="15.95" customHeight="1"/>
-    <row r="822" ht="15.95" customHeight="1"/>
-    <row r="823" ht="15.95" customHeight="1"/>
-    <row r="824" ht="15.95" customHeight="1"/>
-    <row r="825" ht="15.95" customHeight="1"/>
-    <row r="826" ht="15.95" customHeight="1"/>
-    <row r="827" ht="15.95" customHeight="1"/>
-    <row r="828" ht="15.95" customHeight="1"/>
-    <row r="829" ht="15.95" customHeight="1"/>
-    <row r="830" ht="15.95" customHeight="1"/>
-    <row r="831" ht="15.95" customHeight="1"/>
-    <row r="832" ht="15.95" customHeight="1"/>
-    <row r="833" ht="15.95" customHeight="1"/>
-    <row r="834" ht="15.95" customHeight="1"/>
-    <row r="835" ht="15.95" customHeight="1"/>
-    <row r="836" ht="15.95" customHeight="1"/>
-    <row r="837" ht="15.95" customHeight="1"/>
-    <row r="838" ht="15.95" customHeight="1"/>
-    <row r="839" ht="15.95" customHeight="1"/>
-    <row r="840" ht="15.95" customHeight="1"/>
-    <row r="841" ht="15.95" customHeight="1"/>
-    <row r="842" ht="15.95" customHeight="1"/>
-    <row r="843" ht="15.95" customHeight="1"/>
-    <row r="844" ht="15.95" customHeight="1"/>
-    <row r="845" ht="15.95" customHeight="1"/>
-    <row r="846" ht="15.95" customHeight="1"/>
-    <row r="847" ht="15.95" customHeight="1"/>
-    <row r="848" ht="15.95" customHeight="1"/>
-    <row r="849" ht="15.95" customHeight="1"/>
-    <row r="850" ht="15.95" customHeight="1"/>
-    <row r="851" ht="15.95" customHeight="1"/>
-    <row r="852" ht="15.95" customHeight="1"/>
-    <row r="853" ht="15.95" customHeight="1"/>
-    <row r="854" ht="15.95" customHeight="1"/>
-    <row r="855" ht="15.95" customHeight="1"/>
-    <row r="856" ht="15.95" customHeight="1"/>
-    <row r="857" ht="15.95" customHeight="1"/>
-    <row r="858" ht="15.95" customHeight="1"/>
-    <row r="859" ht="15.95" customHeight="1"/>
-    <row r="860" ht="15.95" customHeight="1"/>
-    <row r="861" ht="15.95" customHeight="1"/>
-    <row r="862" ht="15.95" customHeight="1"/>
-    <row r="863" ht="15.95" customHeight="1"/>
-    <row r="864" ht="15.95" customHeight="1"/>
-    <row r="865" ht="15.95" customHeight="1"/>
-    <row r="866" ht="15.95" customHeight="1"/>
-    <row r="867" ht="15.95" customHeight="1"/>
-    <row r="868" ht="15.95" customHeight="1"/>
-    <row r="869" ht="15.95" customHeight="1"/>
-    <row r="870" ht="15.95" customHeight="1"/>
-    <row r="871" ht="15.95" customHeight="1"/>
-    <row r="872" ht="15.95" customHeight="1"/>
-    <row r="873" ht="15.95" customHeight="1"/>
-    <row r="874" ht="15.95" customHeight="1"/>
-    <row r="875" ht="15.95" customHeight="1"/>
-    <row r="876" ht="15.95" customHeight="1"/>
-    <row r="877" ht="15.95" customHeight="1"/>
-    <row r="878" ht="15.95" customHeight="1"/>
-    <row r="879" ht="15.95" customHeight="1"/>
-    <row r="880" ht="15.95" customHeight="1"/>
-    <row r="881" ht="15.95" customHeight="1"/>
-    <row r="882" ht="15.95" customHeight="1"/>
-    <row r="883" ht="15.95" customHeight="1"/>
-    <row r="884" ht="15.95" customHeight="1"/>
-    <row r="885" ht="15.95" customHeight="1"/>
-    <row r="886" ht="15.95" customHeight="1"/>
-    <row r="887" ht="15.95" customHeight="1"/>
-    <row r="888" ht="15.95" customHeight="1"/>
-    <row r="889" ht="15.95" customHeight="1"/>
-    <row r="890" ht="15.95" customHeight="1"/>
-    <row r="891" ht="15.95" customHeight="1"/>
-    <row r="892" ht="15.95" customHeight="1"/>
-    <row r="893" ht="15.95" customHeight="1"/>
-    <row r="894" ht="15.95" customHeight="1"/>
-    <row r="895" ht="15.95" customHeight="1"/>
-    <row r="896" ht="15.95" customHeight="1"/>
-    <row r="897" ht="15.95" customHeight="1"/>
-    <row r="898" ht="15.95" customHeight="1"/>
-    <row r="899" ht="15.95" customHeight="1"/>
-    <row r="900" ht="15.95" customHeight="1"/>
-    <row r="901" ht="15.95" customHeight="1"/>
-    <row r="902" ht="15.95" customHeight="1"/>
-    <row r="903" ht="15.95" customHeight="1"/>
-    <row r="904" ht="15.95" customHeight="1"/>
-    <row r="905" ht="15.95" customHeight="1"/>
-    <row r="906" ht="15.95" customHeight="1"/>
-    <row r="907" ht="15.95" customHeight="1"/>
-    <row r="908" ht="15.95" customHeight="1"/>
-    <row r="909" ht="15.95" customHeight="1"/>
-    <row r="910" ht="15.95" customHeight="1"/>
-    <row r="911" ht="15.95" customHeight="1"/>
-    <row r="912" ht="15.95" customHeight="1"/>
-    <row r="913" ht="15.95" customHeight="1"/>
-    <row r="914" ht="15.95" customHeight="1"/>
-    <row r="915" ht="15.95" customHeight="1"/>
-    <row r="916" ht="15.95" customHeight="1"/>
-    <row r="917" ht="15.95" customHeight="1"/>
-    <row r="918" ht="15.95" customHeight="1"/>
-    <row r="919" ht="15.95" customHeight="1"/>
-    <row r="920" ht="15.95" customHeight="1"/>
-    <row r="921" ht="15.95" customHeight="1"/>
-    <row r="922" ht="15.95" customHeight="1"/>
-    <row r="923" ht="15.95" customHeight="1"/>
-    <row r="924" ht="15.95" customHeight="1"/>
-    <row r="925" ht="15.95" customHeight="1"/>
-    <row r="926" ht="15.95" customHeight="1"/>
-    <row r="927" ht="15.95" customHeight="1"/>
-    <row r="928" ht="15.95" customHeight="1"/>
-    <row r="929" ht="15.95" customHeight="1"/>
-    <row r="930" ht="15.95" customHeight="1"/>
-    <row r="931" ht="15.95" customHeight="1"/>
-    <row r="932" ht="15.95" customHeight="1"/>
-    <row r="933" ht="15.95" customHeight="1"/>
-    <row r="934" ht="15.95" customHeight="1"/>
-    <row r="935" ht="15.95" customHeight="1"/>
-    <row r="936" ht="15.95" customHeight="1"/>
-    <row r="937" ht="15.95" customHeight="1"/>
-    <row r="938" ht="15.95" customHeight="1"/>
-    <row r="939" ht="15.95" customHeight="1"/>
-    <row r="940" ht="15.95" customHeight="1"/>
-    <row r="941" ht="15.95" customHeight="1"/>
-    <row r="942" ht="15.95" customHeight="1"/>
-    <row r="943" ht="15.95" customHeight="1"/>
-    <row r="944" ht="15.95" customHeight="1"/>
-    <row r="945" ht="15.95" customHeight="1"/>
-    <row r="946" ht="15.95" customHeight="1"/>
-    <row r="947" ht="15.95" customHeight="1"/>
-    <row r="948" ht="15.95" customHeight="1"/>
-    <row r="949" ht="15.95" customHeight="1"/>
-    <row r="950" ht="15.95" customHeight="1"/>
-    <row r="951" ht="15.95" customHeight="1"/>
-    <row r="952" ht="15.95" customHeight="1"/>
-    <row r="953" ht="15.95" customHeight="1"/>
-    <row r="954" ht="15.95" customHeight="1"/>
-    <row r="955" ht="15.95" customHeight="1"/>
-    <row r="956" ht="15.95" customHeight="1"/>
-    <row r="957" ht="15.95" customHeight="1"/>
-    <row r="958" ht="15.95" customHeight="1"/>
-    <row r="959" ht="15.95" customHeight="1"/>
-    <row r="960" ht="15.95" customHeight="1"/>
-    <row r="961" ht="15.95" customHeight="1"/>
-    <row r="962" ht="15.95" customHeight="1"/>
-    <row r="963" ht="15.95" customHeight="1"/>
-    <row r="964" ht="15.95" customHeight="1"/>
-    <row r="965" ht="15.95" customHeight="1"/>
-    <row r="966" ht="15.95" customHeight="1"/>
-    <row r="967" ht="15.95" customHeight="1"/>
-    <row r="968" ht="15.95" customHeight="1"/>
-    <row r="969" ht="15.95" customHeight="1"/>
-    <row r="970" ht="15.95" customHeight="1"/>
-    <row r="971" ht="15.95" customHeight="1"/>
-    <row r="972" ht="15.95" customHeight="1"/>
-    <row r="973" ht="15.95" customHeight="1"/>
-    <row r="974" ht="15.95" customHeight="1"/>
-    <row r="975" ht="15.95" customHeight="1"/>
-    <row r="976" ht="15.95" customHeight="1"/>
-    <row r="977" ht="15.95" customHeight="1"/>
-    <row r="978" ht="15.95" customHeight="1"/>
-    <row r="979" ht="15.95" customHeight="1"/>
-    <row r="980" ht="15.95" customHeight="1"/>
-    <row r="981" ht="15.95" customHeight="1"/>
-    <row r="982" ht="15.95" customHeight="1"/>
-    <row r="983" ht="15.95" customHeight="1"/>
-    <row r="984" ht="15.95" customHeight="1"/>
-    <row r="985" ht="15.95" customHeight="1"/>
-    <row r="986" ht="15.95" customHeight="1"/>
-    <row r="987" ht="15.95" customHeight="1"/>
-    <row r="988" ht="15.95" customHeight="1"/>
-    <row r="989" ht="15.95" customHeight="1"/>
-    <row r="990" ht="15.95" customHeight="1"/>
-    <row r="991" ht="15.95" customHeight="1"/>
-    <row r="992" ht="15.95" customHeight="1"/>
-    <row r="993" ht="15.95" customHeight="1"/>
-    <row r="994" ht="15.95" customHeight="1"/>
-    <row r="995" ht="15.95" customHeight="1"/>
-    <row r="996" ht="15.95" customHeight="1"/>
-    <row r="997" ht="15.95" customHeight="1"/>
-    <row r="998" ht="15.95" customHeight="1"/>
-    <row r="999" ht="15.95" customHeight="1"/>
-    <row r="1000" ht="15.95" customHeight="1"/>
-    <row r="1001" ht="15.95" customHeight="1"/>
-    <row r="1002" ht="15.95" customHeight="1"/>
-    <row r="1003" ht="15.95" customHeight="1"/>
-    <row r="1004" ht="15.95" customHeight="1"/>
-    <row r="1005" ht="15.95" customHeight="1"/>
-    <row r="1006" ht="15.95" customHeight="1"/>
-    <row r="1007" ht="15.95" customHeight="1"/>
-    <row r="1008" ht="15.95" customHeight="1"/>
-    <row r="1009" ht="15.95" customHeight="1"/>
-    <row r="1010" ht="15.95" customHeight="1"/>
-    <row r="1011" ht="15.95" customHeight="1"/>
-    <row r="1012" ht="15.95" customHeight="1"/>
-    <row r="1013" ht="15.95" customHeight="1"/>
-    <row r="1014" ht="15.95" customHeight="1"/>
-    <row r="1015" ht="15.95" customHeight="1"/>
-    <row r="1016" ht="15.95" customHeight="1"/>
-    <row r="1017" ht="15.95" customHeight="1"/>
-    <row r="1018" ht="15.95" customHeight="1"/>
-    <row r="1019" ht="15.95" customHeight="1"/>
-    <row r="1020" ht="15.95" customHeight="1"/>
-    <row r="1021" ht="15.95" customHeight="1"/>
-    <row r="1022" ht="15.95" customHeight="1"/>
-    <row r="1023" ht="15.95" customHeight="1"/>
-    <row r="1024" ht="15.95" customHeight="1"/>
-    <row r="1025" ht="15.95" customHeight="1"/>
-    <row r="1026" ht="15.95" customHeight="1"/>
-    <row r="1027" ht="15.95" customHeight="1"/>
-    <row r="1028" ht="15.95" customHeight="1"/>
-    <row r="1029" ht="15.95" customHeight="1"/>
-    <row r="1030" ht="15.95" customHeight="1"/>
-    <row r="1031" ht="15.95" customHeight="1"/>
-    <row r="1032" ht="15.95" customHeight="1"/>
-    <row r="1033" ht="15.95" customHeight="1"/>
-    <row r="1034" ht="15.95" customHeight="1"/>
-    <row r="1035" ht="15.95" customHeight="1"/>
-    <row r="1036" ht="15.95" customHeight="1"/>
-    <row r="1037" ht="15.95" customHeight="1"/>
-    <row r="1038" ht="15.95" customHeight="1"/>
-    <row r="1039" ht="15.95" customHeight="1"/>
-    <row r="1040" ht="15.95" customHeight="1"/>
-    <row r="1041" ht="15.95" customHeight="1"/>
-    <row r="1042" ht="15.95" customHeight="1"/>
-    <row r="1043" ht="15.95" customHeight="1"/>
-    <row r="1044" ht="15.95" customHeight="1"/>
-    <row r="1045" ht="15.95" customHeight="1"/>
-    <row r="1046" ht="15.95" customHeight="1"/>
-    <row r="1047" ht="15.95" customHeight="1"/>
-    <row r="1048" ht="15.95" customHeight="1"/>
+    <row r="78" spans="1:256" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="79" spans="1:256" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="80" spans="1:256" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="81" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="82" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="83" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="84" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="85" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="86" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="87" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="88" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="89" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="90" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="91" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="92" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="93" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="94" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="95" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="96" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="97" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="98" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="99" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="100" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="101" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="102" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="103" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="104" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="105" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="106" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="107" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="108" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="109" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="110" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="111" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="112" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="113" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="114" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="115" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="116" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="117" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="118" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="119" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="120" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="121" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="122" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="123" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="124" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="125" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="126" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="127" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="128" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="129" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="130" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="131" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="132" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="133" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="134" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="135" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="136" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="137" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="138" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="139" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="140" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="141" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="142" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="143" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="144" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="145" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="146" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="147" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="148" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="149" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="150" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="151" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="152" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="153" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="154" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="155" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="156" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="157" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="158" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="159" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="160" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="161" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="162" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="163" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="164" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="165" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="166" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="167" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="168" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="169" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="170" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="171" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="172" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="173" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="174" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="175" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="176" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="177" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="178" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="179" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="180" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="181" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="182" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="183" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="184" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="185" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="186" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="187" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="188" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="189" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="190" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="191" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="192" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="193" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="194" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="195" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="196" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="197" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="198" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="199" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="200" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="201" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="202" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="203" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="204" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="205" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="206" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="207" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="208" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="209" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="210" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="211" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="212" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="213" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="214" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="215" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="216" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="217" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="218" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="219" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="220" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="221" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="222" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="223" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="224" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="225" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="226" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="227" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="228" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="229" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="230" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="231" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="232" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="233" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="234" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="235" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="236" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="237" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="238" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="239" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="240" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="241" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="242" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="243" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="244" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="245" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="246" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="247" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="248" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="249" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="250" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="251" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="252" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="253" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="254" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="255" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="256" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="257" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="258" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="259" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="260" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="261" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="262" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="263" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="264" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="265" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="266" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="267" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="268" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="269" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="270" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="271" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="272" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="273" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="274" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="275" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="276" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="277" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="278" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="279" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="280" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="281" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="282" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="283" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="284" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="285" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="286" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="287" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="288" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="289" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="290" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="291" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="292" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="293" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="294" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="295" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="296" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="297" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="298" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="299" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="300" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="301" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="302" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="303" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="304" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="305" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="306" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="307" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="308" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="309" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="310" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="311" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="312" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="313" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="314" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="315" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="316" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="317" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="318" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="319" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="320" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="321" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="322" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="323" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="324" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="325" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="326" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="327" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="328" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="329" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="330" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="331" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="332" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="333" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="334" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="335" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="336" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="337" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="338" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="339" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="340" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="341" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="342" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="343" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="344" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="345" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="346" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="347" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="348" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="349" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="350" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="351" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="352" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="353" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="354" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="355" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="356" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="357" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="358" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="359" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="360" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="361" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="362" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="363" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="364" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="365" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="366" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="367" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="368" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="369" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="370" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="371" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="372" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="373" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="374" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="375" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="376" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="377" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="378" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="379" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="380" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="381" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="382" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="383" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="384" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="385" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="386" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="387" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="388" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="389" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="390" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="391" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="392" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="393" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="394" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="395" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="396" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="397" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="398" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="399" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="400" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="401" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="402" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="403" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="404" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="405" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="406" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="407" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="408" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="409" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="410" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="411" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="412" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="413" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="414" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="415" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="416" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="417" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="418" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="419" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="420" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="421" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="422" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="423" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="424" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="425" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="426" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="427" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="428" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="429" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="430" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="431" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="432" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="433" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="434" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="435" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="436" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="437" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="438" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="439" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="440" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="441" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="442" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="443" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="444" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="445" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="446" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="447" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="448" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="449" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="450" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="451" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="452" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="453" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="454" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="455" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="456" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="457" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="458" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="459" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="460" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="461" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="462" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="463" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="464" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="465" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="466" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="467" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="468" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="469" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="470" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="471" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="472" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="473" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="474" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="475" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="476" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="477" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="478" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="479" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="480" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="481" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="482" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="483" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="484" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="485" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="486" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="487" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="488" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="489" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="490" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="491" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="492" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="493" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="494" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="495" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="496" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="497" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="498" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="499" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="500" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="501" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="502" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="503" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="504" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="505" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="506" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="507" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="508" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="509" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="510" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="511" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="512" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="513" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="514" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="515" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="516" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="517" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="518" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="519" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="520" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="521" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="522" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="523" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="524" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="525" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="526" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="527" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="528" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="529" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="530" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="531" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="532" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="533" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="534" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="535" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="536" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="537" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="538" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="539" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="540" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="541" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="542" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="543" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="544" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="545" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="546" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="547" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="548" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="549" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="550" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="551" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="552" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="553" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="554" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="555" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="556" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="557" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="558" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="559" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="560" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="561" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="562" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="563" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="564" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="565" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="566" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="567" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="568" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="569" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="570" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="571" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="572" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="573" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="574" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="575" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="576" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="577" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="578" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="579" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="580" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="581" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="582" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="583" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="584" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="585" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="586" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="587" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="588" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="589" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="590" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="591" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="592" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="593" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="594" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="595" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="596" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="597" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="598" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="599" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="600" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="601" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="602" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="603" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="604" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="605" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="606" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="607" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="608" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="609" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="610" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="611" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="612" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="613" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="614" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="615" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="616" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="617" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="618" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="619" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="620" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="621" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="622" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="623" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="624" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="625" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="626" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="627" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="628" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="629" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="630" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="631" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="632" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="633" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="634" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="635" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="636" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="637" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="638" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="639" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="640" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="641" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="642" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="643" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="644" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="645" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="646" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="647" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="648" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="649" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="650" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="651" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="652" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="653" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="654" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="655" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="656" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="657" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="658" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="659" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="660" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="661" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="662" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="663" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="664" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="665" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="666" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="667" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="668" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="669" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="670" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="671" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="672" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="673" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="674" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="675" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="676" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="677" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="678" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="679" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="680" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="681" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="682" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="683" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="684" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="685" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="686" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="687" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="688" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="689" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="690" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="691" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="692" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="693" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="694" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="695" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="696" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="697" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="698" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="699" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="700" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="701" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="702" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="703" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="704" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="705" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="706" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="707" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="708" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="709" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="710" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="711" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="712" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="713" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="714" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="715" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="716" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="717" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="718" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="719" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="720" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="721" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="722" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="723" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="724" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="725" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="726" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="727" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="728" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="729" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="730" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="731" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="732" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="733" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="734" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="735" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="736" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="737" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="738" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="739" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="740" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="741" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="742" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="743" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="744" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="745" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="746" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="747" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="748" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="749" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="750" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="751" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="752" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="753" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="754" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="755" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="756" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="757" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="758" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="759" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="760" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="761" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="762" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="763" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="764" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="765" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="766" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="767" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="768" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="769" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="770" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="771" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="772" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="773" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="774" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="775" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="776" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="777" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="778" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="779" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="780" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="781" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="782" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="783" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="784" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="785" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="786" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="787" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="788" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="789" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="790" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="791" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="792" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="793" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="794" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="795" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="796" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="797" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="798" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="799" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="800" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="801" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="802" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="803" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="804" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="805" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="806" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="807" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="808" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="809" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="810" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="811" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="812" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="813" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="814" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="815" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="816" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="817" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="818" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="819" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="820" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="821" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="822" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="823" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="824" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="825" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="826" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="827" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="828" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="829" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="830" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="831" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="832" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="833" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="834" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="835" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="836" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="837" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="838" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="839" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="840" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="841" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="842" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="843" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="844" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="845" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="846" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="847" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="848" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="849" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="850" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="851" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="852" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="853" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="854" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="855" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="856" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="857" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="858" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="859" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="860" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="861" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="862" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="863" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="864" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="865" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="866" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="867" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="868" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="869" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="870" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="871" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="872" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="873" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="874" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="875" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="876" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="877" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="878" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="879" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="880" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="881" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="882" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="883" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="884" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="885" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="886" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="887" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="888" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="889" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="890" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="891" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="892" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="893" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="894" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="895" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="896" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="897" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="898" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="899" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="900" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="901" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="902" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="903" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="904" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="905" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="906" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="907" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="908" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="909" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="910" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="911" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="912" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="913" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="914" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="915" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="916" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="917" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="918" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="919" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="920" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="921" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="922" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="923" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="924" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="925" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="926" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="927" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="928" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="929" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="930" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="931" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="932" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="933" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="934" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="935" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="936" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="937" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="938" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="939" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="940" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="941" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="942" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="943" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="944" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="945" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="946" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="947" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="948" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="949" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="950" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="951" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="952" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="953" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="954" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="955" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="956" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="957" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="958" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="959" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="960" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="961" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="962" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="963" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="964" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="965" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="966" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="967" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="968" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="969" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="970" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="971" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="972" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="973" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="974" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="975" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="976" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="977" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="978" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="979" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="980" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="981" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="982" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="983" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="984" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="985" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="986" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="987" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="988" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="989" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="990" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="991" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="992" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="993" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="994" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="995" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="996" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="997" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="998" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="999" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="1000" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="1001" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="1002" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="1003" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="1004" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="1005" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="1006" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="1007" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="1008" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="1009" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="1010" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="1011" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="1012" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="1013" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="1014" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="1015" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="1016" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="1017" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="1018" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="1019" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="1020" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="1021" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="1022" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="1023" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="1024" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="1025" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="1026" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="1027" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="1028" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="1029" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="1030" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="1031" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="1032" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="1033" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="1034" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="1035" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="1036" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="1037" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="1038" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="1039" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="1040" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="1041" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="1042" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="1043" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="1044" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="1045" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="1046" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="1047" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="1048" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:A4"/>
@@ -19988,29 +20170,29 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView zoomScale="98" zoomScaleNormal="98" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="256" width="26.42578125" customWidth="1"/>
-    <col min="257" max="1023" width="16.140625" customWidth="1"/>
-    <col min="1024" max="1025" width="11.7109375" customWidth="1"/>
+    <col min="1" max="256" width="26.453125" customWidth="1"/>
+    <col min="257" max="1023" width="16.1796875" customWidth="1"/>
+    <col min="1024" max="1025" width="11.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="49" t="s">
+    <row r="1" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A1" s="52" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="26" t="s">
         <v>162</v>
       </c>
@@ -20024,7 +20206,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" ht="13" x14ac:dyDescent="0.3">
       <c r="A3" s="27" t="s">
         <v>163</v>
       </c>
@@ -20052,28 +20234,28 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="256" width="24.42578125" customWidth="1"/>
-    <col min="257" max="1023" width="16.140625" customWidth="1"/>
-    <col min="1024" max="1025" width="11.7109375" customWidth="1"/>
+    <col min="1" max="256" width="24.453125" customWidth="1"/>
+    <col min="257" max="1023" width="16.1796875" customWidth="1"/>
+    <col min="1024" max="1025" width="11.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="50" t="s">
+    <row r="1" spans="1:3" ht="13" x14ac:dyDescent="0.3">
+      <c r="A1" s="53" t="s">
         <v>79</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="26" t="s">
         <v>80</v>
       </c>
@@ -20084,7 +20266,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" ht="13" x14ac:dyDescent="0.3">
       <c r="A3" s="27" t="s">
         <v>82</v>
       </c>
@@ -20095,7 +20277,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="28"/>
       <c r="B4" s="29"/>
       <c r="C4" s="29"/>
@@ -20114,28 +20296,28 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="256" width="22.42578125" customWidth="1"/>
-    <col min="257" max="1023" width="16.140625" customWidth="1"/>
-    <col min="1024" max="1025" width="11.7109375" customWidth="1"/>
+    <col min="1" max="256" width="22.453125" customWidth="1"/>
+    <col min="257" max="1023" width="16.1796875" customWidth="1"/>
+    <col min="1024" max="1025" width="11.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="51" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="54" t="s">
         <v>85</v>
       </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="51"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="26" t="s">
         <v>86</v>
       </c>
@@ -20146,7 +20328,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" ht="13" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
         <v>88</v>
       </c>
@@ -20157,7 +20339,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" ht="13" x14ac:dyDescent="0.3">
       <c r="A4" s="12"/>
       <c r="B4" s="31"/>
       <c r="C4" s="31"/>
@@ -20176,28 +20358,28 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScalePageLayoutView="60" workbookViewId="0">
+    <sheetView zoomScalePageLayoutView="60" workbookViewId="0">
       <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="256" width="22.42578125" customWidth="1"/>
-    <col min="257" max="1023" width="16.140625" customWidth="1"/>
-    <col min="1024" max="1025" width="11.7109375" customWidth="1"/>
+    <col min="1" max="256" width="22.453125" customWidth="1"/>
+    <col min="257" max="1023" width="16.1796875" customWidth="1"/>
+    <col min="1024" max="1025" width="11.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="51" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="54" t="s">
         <v>91</v>
       </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="51"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="26" t="s">
         <v>86</v>
       </c>
@@ -20208,7 +20390,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" ht="13" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
         <v>93</v>
       </c>
@@ -20219,7 +20401,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="28"/>
       <c r="B4" s="31"/>
       <c r="C4" s="31"/>
@@ -20238,28 +20420,28 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView zoomScalePageLayoutView="60" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="60" workbookViewId="0">
       <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="256" width="22.42578125" customWidth="1"/>
-    <col min="257" max="1023" width="16.140625" customWidth="1"/>
-    <col min="1024" max="1025" width="11.7109375" customWidth="1"/>
+    <col min="1" max="256" width="22.453125" customWidth="1"/>
+    <col min="257" max="1023" width="16.1796875" customWidth="1"/>
+    <col min="1024" max="1025" width="11.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="51" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="54" t="s">
         <v>96</v>
       </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="51"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>86</v>
       </c>
@@ -20270,7 +20452,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" ht="13" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
         <v>98</v>
       </c>
@@ -20281,7 +20463,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="32"/>
       <c r="B4" s="9"/>
       <c r="C4" s="9"/>
@@ -20300,28 +20482,28 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection sqref="A1:C1"/>
+    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="256" width="22.42578125" customWidth="1"/>
-    <col min="257" max="1023" width="16.140625" customWidth="1"/>
-    <col min="1024" max="1025" width="11.7109375" customWidth="1"/>
+    <col min="1" max="256" width="22.453125" customWidth="1"/>
+    <col min="257" max="1023" width="16.1796875" customWidth="1"/>
+    <col min="1024" max="1025" width="11.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="51" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="54" t="s">
         <v>101</v>
       </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="51"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>86</v>
       </c>
@@ -20332,7 +20514,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" ht="13" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
         <v>103</v>
       </c>
@@ -20343,7 +20525,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="32"/>
       <c r="B4" s="9"/>
       <c r="C4" s="9"/>
@@ -20362,34 +20544,34 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:T94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="C93" sqref="C93:D93"/>
+    <sheetView zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" customWidth="1"/>
-    <col min="2" max="2" width="31.5703125" customWidth="1"/>
-    <col min="3" max="1023" width="12.42578125" customWidth="1"/>
+    <col min="1" max="1" width="18.81640625" customWidth="1"/>
+    <col min="2" max="2" width="31.54296875" customWidth="1"/>
+    <col min="3" max="1023" width="12.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20">
-      <c r="A1" s="51" t="s">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1" s="54" t="s">
         <v>106</v>
       </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
-      <c r="G1" s="51"/>
-      <c r="H1" s="51"/>
-      <c r="I1" s="51"/>
-      <c r="J1" s="51"/>
-      <c r="K1" s="51"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
       <c r="L1" s="30"/>
       <c r="M1" s="30"/>
       <c r="N1" s="30"/>
@@ -20400,7 +20582,7 @@
       <c r="S1" s="30"/>
       <c r="T1" s="30"/>
     </row>
-    <row r="2" spans="1:20">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">
         <v>81</v>
       </c>
@@ -20462,7 +20644,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="3" spans="1:20">
+    <row r="3" spans="1:20" ht="13" x14ac:dyDescent="0.3">
       <c r="A3" s="33" t="s">
         <v>124</v>
       </c>
@@ -20524,7 +20706,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="15" spans="1:20">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="42" t="s">
         <v>176</v>
       </c>
@@ -20532,7 +20714,7 @@
       <c r="C15" s="42"/>
       <c r="D15" s="42"/>
     </row>
-    <row r="16" spans="1:20">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="43" t="s">
         <v>171</v>
       </c>
@@ -20546,7 +20728,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="42" t="s">
         <v>175</v>
       </c>
@@ -20554,7 +20736,7 @@
       <c r="C28" s="42"/>
       <c r="D28" s="42"/>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="43" t="s">
         <v>171</v>
       </c>
@@ -20568,7 +20750,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="42" t="s">
         <v>180</v>
       </c>
@@ -20576,7 +20758,7 @@
       <c r="C44" s="42"/>
       <c r="D44" s="42"/>
     </row>
-    <row r="45" spans="1:4">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="43" t="s">
         <v>171</v>
       </c>
@@ -20590,7 +20772,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="58" spans="1:4">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="42" t="s">
         <v>170</v>
       </c>
@@ -20598,7 +20780,7 @@
       <c r="C58" s="42"/>
       <c r="D58" s="42"/>
     </row>
-    <row r="59" spans="1:4">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="43" t="s">
         <v>171</v>
       </c>
@@ -20612,7 +20794,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="80" spans="1:4">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="42" t="s">
         <v>187</v>
       </c>
@@ -20620,7 +20802,7 @@
       <c r="C80" s="42"/>
       <c r="D80" s="42"/>
     </row>
-    <row r="81" spans="1:4">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="43" t="s">
         <v>188</v>
       </c>
@@ -20634,19 +20816,19 @@
         <v>191</v>
       </c>
     </row>
-    <row r="93" spans="1:4">
-      <c r="A93" s="53" t="s">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" s="55" t="s">
         <v>192</v>
       </c>
-      <c r="B93" s="54"/>
+      <c r="B93" s="56"/>
       <c r="C93" s="42"/>
       <c r="D93" s="42"/>
     </row>
-    <row r="94" spans="1:4" ht="60">
+    <row r="94" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A94" s="43" t="s">
         <v>193</v>
       </c>
-      <c r="B94" s="52" t="s">
+      <c r="B94" s="46" t="s">
         <v>194</v>
       </c>
     </row>
@@ -20662,4 +20844,96 @@
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03DDC5C3-BD6D-444D-BAD4-1FA02546E2E3}">
+  <dimension ref="A1:L4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.453125" customWidth="1"/>
+    <col min="2" max="2" width="11.90625" customWidth="1"/>
+    <col min="3" max="3" width="17.81640625" customWidth="1"/>
+    <col min="4" max="4" width="13.08984375" customWidth="1"/>
+    <col min="5" max="5" width="19" customWidth="1"/>
+    <col min="6" max="6" width="15.1796875" customWidth="1"/>
+    <col min="7" max="7" width="21.7265625" customWidth="1"/>
+    <col min="8" max="8" width="14.6328125" customWidth="1"/>
+    <col min="9" max="9" width="14.36328125" customWidth="1"/>
+    <col min="10" max="10" width="20" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="54" t="s">
+        <v>205</v>
+      </c>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+    </row>
+    <row r="2" spans="1:12" ht="13" x14ac:dyDescent="0.3">
+      <c r="A2" s="47" t="s">
+        <v>195</v>
+      </c>
+      <c r="B2" s="47" t="s">
+        <v>204</v>
+      </c>
+      <c r="C2" s="47" t="s">
+        <v>196</v>
+      </c>
+      <c r="D2" s="47" t="s">
+        <v>197</v>
+      </c>
+      <c r="E2" s="47" t="s">
+        <v>198</v>
+      </c>
+      <c r="F2" s="47" t="s">
+        <v>199</v>
+      </c>
+      <c r="G2" s="47" t="s">
+        <v>200</v>
+      </c>
+      <c r="H2" s="47" t="s">
+        <v>201</v>
+      </c>
+      <c r="I2" s="47" t="s">
+        <v>202</v>
+      </c>
+      <c r="J2" s="47" t="s">
+        <v>203</v>
+      </c>
+      <c r="K2" s="47"/>
+      <c r="L2" s="47"/>
+    </row>
+    <row r="3" spans="1:12" ht="13" x14ac:dyDescent="0.3">
+      <c r="A3" s="58" t="s">
+        <v>206</v>
+      </c>
+      <c r="B3" s="12"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="57"/>
+      <c r="E3" s="57"/>
+      <c r="F3" s="57"/>
+      <c r="G3" s="57"/>
+      <c r="H3" s="57"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="48"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
POCOR-6646|added extra sheet for Student performance summary and modified institution card table to get sheet data|status:ReadyToDeploy
</commit_message>
<xml_diff>
--- a/webroot/export/customexcel/default_templates/profile_template.xlsx
+++ b/webroot/export/customexcel/default_templates/profile_template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\pocor-openemis-core\webroot\export\customexcel\default_templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\poona\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11260991-4D1F-4CAF-B37D-E9EFE172E349}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{613322A7-21FD-4253-83DB-1B04836A2A3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="1000" firstSheet="3" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="6" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <sheet name="Staff by Positions and Qualific" sheetId="6" r:id="rId6"/>
     <sheet name="Staff by Staff Type and Qualifi" sheetId="7" r:id="rId7"/>
     <sheet name="Extra details" sheetId="8" r:id="rId8"/>
-    <sheet name="POCOR6646" sheetId="10" r:id="rId9"/>
+    <sheet name="Student Performance Summary" sheetId="10" r:id="rId9"/>
   </sheets>
   <calcPr calcId="124519"/>
   <extLst>
@@ -109,7 +109,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="216">
   <si>
     <t>${"image":{"displayValue":"Institutions.logo_content","imageWidth":"100","imageMarginLeft":"20","imageMarginTop":"5"}}</t>
   </si>
@@ -726,17 +726,45 @@
     <t>Class Name</t>
   </si>
   <si>
-    <t>Student Abesence Records</t>
-  </si>
-  <si>
-    <t>${"match": {"displayValue": "EducationGrade.name","rows": {"matchFrom": "EducationGrade.id","matchTo": "EducationGrade.id"}}}</t>
+    <t>${"match": {"displayValue": "StudentDetails.openemis_no","rows": {"matchFrom": "StudentDetails.id","matchTo": "StudentDetails.id"}}}</t>
+  </si>
+  <si>
+    <t>${"match": {"displayValue": "StudentDetails.identity_number","rows": {"matchFrom": "StudentDetails.id","matchTo": "StudentDetails.id"}}}</t>
+  </si>
+  <si>
+    <t>${"match": {"displayValue": "StudentDetails.student_name","rows": {"matchFrom": "StudentDetails.id","matchTo": "StudentDetails.id"}}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${"match": {"displayValue": "StudentDetails.class_name","rows": {"matchFrom": "StudentDetails.id","matchTo": "StudentDetails.id"}}}
+</t>
+  </si>
+  <si>
+    <t>${"match": {"displayValue": "StudentDetails.grade_name","rows": {"matchFrom": "StudentDetails.id","matchTo": "StudentDetails.id"}}}</t>
+  </si>
+  <si>
+    <t>${"match": {"displayValue": "StudentDetails.homeroom_teacher","rows": {"matchFrom": "StudentDetails.id","matchTo": "StudentDetails.id"}}}</t>
+  </si>
+  <si>
+    <t>${"match": {"displayValue": "StudentDetails.subject_name","rows": {"matchFrom": "StudentDetails.id","matchTo": "StudentDetails.id"}}}</t>
+  </si>
+  <si>
+    <t>${"match": {"displayValue": "StudentDetails.absence_day","rows": {"matchFrom": "StudentDetails.id","matchTo": "StudentDetails.id"}}}</t>
+  </si>
+  <si>
+    <t>${"match": {"displayValue": "StudentDetails.average_marks","rows": {"matchFrom": "StudentDetails.id","matchTo": "StudentDetails.id"}}}</t>
+  </si>
+  <si>
+    <t>${"match": {"displayValue": "StudentDetails.individual_result","rows": {"matchFrom": "StudentDetails.id","matchTo": "StudentDetails.id"}}}</t>
+  </si>
+  <si>
+    <t>Student Performance Summary</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -816,13 +844,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color rgb="FF172B4D"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -834,6 +855,19 @@
       <color rgb="FF000000"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FF172B4D"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF172B4D"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -958,7 +992,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1065,7 +1099,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1092,8 +1126,24 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -20238,7 +20288,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -20424,7 +20474,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -20486,7 +20536,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -20548,7 +20598,7 @@
   <dimension ref="A1:T94"/>
   <sheetViews>
     <sheetView zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection sqref="A1:K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -20851,7 +20901,7 @@
   <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -20869,16 +20919,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="54" t="s">
-        <v>205</v>
-      </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
-      <c r="F1" s="57"/>
-      <c r="G1" s="57"/>
-      <c r="H1" s="57"/>
+      <c r="A1" s="58" t="s">
+        <v>215</v>
+      </c>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="59"/>
+      <c r="H1" s="59"/>
+      <c r="I1" s="59"/>
+      <c r="J1" s="59"/>
     </row>
     <row r="2" spans="1:12" ht="13" x14ac:dyDescent="0.3">
       <c r="A2" s="47" t="s">
@@ -20914,26 +20966,48 @@
       <c r="K2" s="47"/>
       <c r="L2" s="47"/>
     </row>
-    <row r="3" spans="1:12" ht="13" x14ac:dyDescent="0.3">
-      <c r="A3" s="58" t="s">
+    <row r="3" spans="1:12" ht="15.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="57" t="s">
+        <v>209</v>
+      </c>
+      <c r="B3" s="60" t="s">
+        <v>208</v>
+      </c>
+      <c r="C3" s="61" t="s">
+        <v>210</v>
+      </c>
+      <c r="D3" s="57" t="s">
+        <v>205</v>
+      </c>
+      <c r="E3" s="60" t="s">
         <v>206</v>
       </c>
-      <c r="B3" s="12"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="57"/>
-      <c r="E3" s="57"/>
-      <c r="F3" s="57"/>
-      <c r="G3" s="57"/>
-      <c r="H3" s="57"/>
+      <c r="F3" s="60" t="s">
+        <v>207</v>
+      </c>
+      <c r="G3" s="60" t="s">
+        <v>211</v>
+      </c>
+      <c r="H3" s="62" t="s">
+        <v>213</v>
+      </c>
+      <c r="I3" s="62" t="s">
+        <v>214</v>
+      </c>
+      <c r="J3" s="60" t="s">
+        <v>212</v>
+      </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="48"/>
+      <c r="D4" s="48"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A1:J1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
POCOR-6691|Added two new placeholder into Institution>Profile>Report and also write migration cript to create new table|status:ReadyToTest
</commit_message>
<xml_diff>
--- a/webroot/export/customexcel/default_templates/profile_template.xlsx
+++ b/webroot/export/customexcel/default_templates/profile_template.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\pocor-openemis-core\webroot\export\customexcel\default_templates\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A86A1D4-1E9A-46CE-81D4-E4BC01AC619F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="495" windowWidth="20730" windowHeight="11760" tabRatio="933"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="933" firstSheet="3" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -18,15 +24,6 @@
   </sheets>
   <calcPr calcId="124519"/>
   <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
     </ext>
@@ -35,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="255">
   <si>
     <t>${"image":{"displayValue":"Institutions.logo_content","imageWidth":"100","imageMarginLeft":"20","imageMarginTop":"5"}}</t>
   </si>
@@ -773,13 +770,40 @@
   </si>
   <si>
     <t>${"match": {"displayValue": "InfrastructureRoomCustomFields.custom_field_value","rows": {"matchFrom": "InfrastructureRoomCustomFields.id","matchTo": "InfrastructureRoomCustomFields.id"}}}</t>
+  </si>
+  <si>
+    <t>Count of Infrastructure Room Areas</t>
+  </si>
+  <si>
+    <t>${"match": {"displayValue": "InstitutionRooms.area","rows": {"matchFrom": "InstitutionRooms.id","matchTo": "InstitutionRooms.id"}}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${"match": {"displayValue": "InstitutionRoomsArea.area_level:1","rows": {"matchFrom": "InstitutionRooms.id","matchTo": "InstitutionRooms.id"}}} </t>
+  </si>
+  <si>
+    <t xml:space="preserve">${"match": {"displayValue": "InstitutionRoomsArea.area_level:2","rows": {"matchFrom": "InstitutionRooms.id","matchTo": "InstitutionRooms.id"}}} </t>
+  </si>
+  <si>
+    <t>Count of Repeater Students</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${"match": {"displayValue": "InstitutionStudentRepeater.area_level:1","rows": {"matchFrom": "InstitutionEducationGrade.id","matchTo": "InstitutionEducationGrade.id"}}} </t>
+  </si>
+  <si>
+    <t xml:space="preserve">${"match": {"displayValue": "InstitutionStudentRepeater.area_level:2","rows": {"matchFrom": "InstitutionEducationGrade.id","matchTo": "InstitutionEducationGrade.id"}}} </t>
+  </si>
+  <si>
+    <t xml:space="preserve">${"match": {"displayValue": "InstitutionStudentRepeater.area_level:3","rows": {"matchFrom": "InstitutionEducationGrade.id","matchTo": "InstitutionEducationGrade.id"}}} </t>
+  </si>
+  <si>
+    <t xml:space="preserve">${"match": {"displayValue": "InstitutionRoomsArea.area_level:3","rows": {"matchFrom": "InstitutionRooms.id","matchTo": "InstitutionRooms.id"}}} </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="11">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -848,6 +872,17 @@
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -973,7 +1008,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1077,6 +1112,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1229,7 +1270,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1261,9 +1302,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1295,6 +1354,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1470,32 +1547,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:IV1041"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A155" zoomScalePageLayoutView="60" workbookViewId="0">
+    <sheetView topLeftCell="A155" zoomScalePageLayoutView="60" workbookViewId="0">
       <selection activeCell="A168" sqref="A168"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="63.140625" customWidth="1"/>
-    <col min="2" max="2" width="54.28515625" customWidth="1"/>
+    <col min="1" max="1" width="63.1796875" customWidth="1"/>
+    <col min="2" max="2" width="54.26953125" customWidth="1"/>
     <col min="3" max="3" width="53" customWidth="1"/>
-    <col min="4" max="4" width="24.28515625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="61.28515625" customWidth="1"/>
-    <col min="6" max="6" width="51.85546875" customWidth="1"/>
+    <col min="4" max="4" width="24.26953125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="61.26953125" customWidth="1"/>
+    <col min="6" max="6" width="51.81640625" customWidth="1"/>
     <col min="7" max="7" width="58" customWidth="1"/>
     <col min="8" max="8" width="40" customWidth="1"/>
-    <col min="9" max="18" width="39.42578125" customWidth="1"/>
-    <col min="19" max="27" width="41.85546875" customWidth="1"/>
-    <col min="28" max="256" width="39.7109375" customWidth="1"/>
-    <col min="257" max="1023" width="16.140625" customWidth="1"/>
-    <col min="1024" max="1025" width="11.7109375" customWidth="1"/>
+    <col min="9" max="18" width="39.453125" customWidth="1"/>
+    <col min="19" max="27" width="41.81640625" customWidth="1"/>
+    <col min="28" max="256" width="39.7265625" customWidth="1"/>
+    <col min="257" max="1023" width="16.1796875" customWidth="1"/>
+    <col min="1024" max="1025" width="11.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:256" ht="15" customHeight="1">
-      <c r="A1" s="47" t="s">
+    <row r="1" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="51" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4"/>
@@ -1515,14 +1592,14 @@
       <c r="P1" s="7"/>
       <c r="Q1" s="7"/>
     </row>
-    <row r="2" spans="1:256" ht="25.5" customHeight="1">
-      <c r="A2" s="47"/>
-      <c r="B2" s="48" t="s">
+    <row r="2" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="51"/>
+      <c r="B2" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="48"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
       <c r="F2" s="8"/>
       <c r="G2" s="9"/>
       <c r="H2" s="7"/>
@@ -1775,14 +1852,14 @@
       <c r="IU2" s="3"/>
       <c r="IV2" s="3"/>
     </row>
-    <row r="3" spans="1:256" ht="25.5" customHeight="1">
-      <c r="A3" s="47"/>
-      <c r="B3" s="49" t="s">
+    <row r="3" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="51"/>
+      <c r="B3" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="49"/>
-      <c r="D3" s="49"/>
-      <c r="E3" s="49"/>
+      <c r="C3" s="53"/>
+      <c r="D3" s="53"/>
+      <c r="E3" s="53"/>
       <c r="F3" s="9"/>
       <c r="G3" s="9"/>
       <c r="H3" s="7"/>
@@ -2035,8 +2112,8 @@
       <c r="IU3" s="3"/>
       <c r="IV3" s="3"/>
     </row>
-    <row r="4" spans="1:256" ht="22.5" customHeight="1">
-      <c r="A4" s="47"/>
+    <row r="4" spans="1:256" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="51"/>
       <c r="B4" s="4"/>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
@@ -2054,7 +2131,7 @@
       <c r="P4" s="7"/>
       <c r="Q4" s="7"/>
     </row>
-    <row r="5" spans="1:256" ht="15.75" customHeight="1">
+    <row r="5" spans="1:256" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="10"/>
       <c r="B5" s="10"/>
       <c r="C5" s="10"/>
@@ -2074,7 +2151,7 @@
       <c r="Q5" s="7"/>
       <c r="R5" s="7"/>
     </row>
-    <row r="6" spans="1:256" ht="12" customHeight="1">
+    <row r="6" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="11" t="s">
         <v>3</v>
       </c>
@@ -2098,7 +2175,7 @@
       <c r="Q6" s="7"/>
       <c r="R6" s="7"/>
     </row>
-    <row r="7" spans="1:256" ht="12" customHeight="1">
+    <row r="7" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="11" t="s">
         <v>5</v>
       </c>
@@ -2122,7 +2199,7 @@
       <c r="Q7" s="7"/>
       <c r="R7" s="7"/>
     </row>
-    <row r="8" spans="1:256" ht="12" customHeight="1">
+    <row r="8" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="11" t="s">
         <v>7</v>
       </c>
@@ -2146,7 +2223,7 @@
       <c r="Q8" s="7"/>
       <c r="R8" s="7"/>
     </row>
-    <row r="9" spans="1:256" ht="12" customHeight="1">
+    <row r="9" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="11" t="s">
         <v>9</v>
       </c>
@@ -2170,7 +2247,7 @@
       <c r="Q9" s="7"/>
       <c r="R9" s="7"/>
     </row>
-    <row r="10" spans="1:256" ht="12" customHeight="1">
+    <row r="10" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="11" t="s">
         <v>11</v>
       </c>
@@ -2194,7 +2271,7 @@
       <c r="Q10" s="7"/>
       <c r="R10" s="7"/>
     </row>
-    <row r="11" spans="1:256" ht="12" customHeight="1">
+    <row r="11" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="11" t="s">
         <v>13</v>
       </c>
@@ -2456,7 +2533,7 @@
       <c r="IU11" s="3"/>
       <c r="IV11" s="3"/>
     </row>
-    <row r="12" spans="1:256" ht="16.5" customHeight="1">
+    <row r="12" spans="1:256" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="16"/>
       <c r="B12" s="16"/>
       <c r="C12" s="16"/>
@@ -2714,7 +2791,7 @@
       <c r="IU12" s="3"/>
       <c r="IV12" s="3"/>
     </row>
-    <row r="13" spans="1:256" ht="16.5" customHeight="1">
+    <row r="13" spans="1:256" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="11" t="s">
         <v>15</v>
       </c>
@@ -2976,7 +3053,7 @@
       <c r="IU13" s="3"/>
       <c r="IV13" s="3"/>
     </row>
-    <row r="14" spans="1:256" ht="16.5" customHeight="1">
+    <row r="14" spans="1:256" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="11" t="s">
         <v>17</v>
       </c>
@@ -3238,7 +3315,7 @@
       <c r="IU14" s="3"/>
       <c r="IV14" s="3"/>
     </row>
-    <row r="15" spans="1:256" ht="12" customHeight="1">
+    <row r="15" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="11" t="s">
         <v>19</v>
       </c>
@@ -3500,7 +3577,7 @@
       <c r="IU15" s="3"/>
       <c r="IV15" s="3"/>
     </row>
-    <row r="16" spans="1:256" ht="12" customHeight="1">
+    <row r="16" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="11" t="s">
         <v>21</v>
       </c>
@@ -3762,7 +3839,7 @@
       <c r="IU16" s="3"/>
       <c r="IV16" s="3"/>
     </row>
-    <row r="17" spans="1:256" ht="12" customHeight="1">
+    <row r="17" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="11" t="s">
         <v>23</v>
       </c>
@@ -4024,7 +4101,7 @@
       <c r="IU17" s="3"/>
       <c r="IV17" s="3"/>
     </row>
-    <row r="18" spans="1:256" ht="12" customHeight="1">
+    <row r="18" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="11" t="s">
         <v>25</v>
       </c>
@@ -4286,7 +4363,7 @@
       <c r="IU18" s="3"/>
       <c r="IV18" s="3"/>
     </row>
-    <row r="19" spans="1:256" ht="12" customHeight="1">
+    <row r="19" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="11" t="s">
         <v>27</v>
       </c>
@@ -4548,7 +4625,7 @@
       <c r="IU19" s="3"/>
       <c r="IV19" s="3"/>
     </row>
-    <row r="20" spans="1:256" ht="12" customHeight="1">
+    <row r="20" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="11" t="s">
         <v>15</v>
       </c>
@@ -4810,7 +4887,7 @@
       <c r="IU20" s="3"/>
       <c r="IV20" s="3"/>
     </row>
-    <row r="21" spans="1:256" ht="12" customHeight="1">
+    <row r="21" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="11" t="s">
         <v>29</v>
       </c>
@@ -5072,7 +5149,7 @@
       <c r="IU21" s="3"/>
       <c r="IV21" s="3"/>
     </row>
-    <row r="22" spans="1:256" ht="12" customHeight="1">
+    <row r="22" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="11" t="s">
         <v>164</v>
       </c>
@@ -5334,7 +5411,7 @@
       <c r="IU22" s="3"/>
       <c r="IV22" s="3"/>
     </row>
-    <row r="23" spans="1:256" ht="12" customHeight="1">
+    <row r="23" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="11" t="s">
         <v>166</v>
       </c>
@@ -5596,7 +5673,7 @@
       <c r="IU23" s="3"/>
       <c r="IV23" s="3"/>
     </row>
-    <row r="24" spans="1:256" ht="12" customHeight="1">
+    <row r="24" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="11" t="s">
         <v>168</v>
       </c>
@@ -5858,7 +5935,7 @@
       <c r="IU24" s="3"/>
       <c r="IV24" s="3"/>
     </row>
-    <row r="25" spans="1:256" ht="12" customHeight="1">
+    <row r="25" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="41"/>
       <c r="B25" s="41"/>
       <c r="C25" s="39"/>
@@ -6116,7 +6193,7 @@
       <c r="IU25" s="3"/>
       <c r="IV25" s="3"/>
     </row>
-    <row r="26" spans="1:256" ht="12" customHeight="1">
+    <row r="26" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="41"/>
       <c r="B26" s="41"/>
       <c r="C26" s="39"/>
@@ -6374,7 +6451,7 @@
       <c r="IU26" s="3"/>
       <c r="IV26" s="3"/>
     </row>
-    <row r="27" spans="1:256" ht="12" customHeight="1">
+    <row r="27" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
         <v>31</v>
       </c>
@@ -6634,7 +6711,7 @@
       <c r="IU27" s="3"/>
       <c r="IV27" s="3"/>
     </row>
-    <row r="28" spans="1:256" ht="12" customHeight="1">
+    <row r="28" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="9" t="s">
         <v>32</v>
       </c>
@@ -6898,7 +6975,7 @@
       <c r="IU28" s="3"/>
       <c r="IV28" s="3"/>
     </row>
-    <row r="29" spans="1:256" ht="12" customHeight="1">
+    <row r="29" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="12" t="s">
         <v>35</v>
       </c>
@@ -7162,7 +7239,7 @@
       <c r="IU29" s="3"/>
       <c r="IV29" s="3"/>
     </row>
-    <row r="30" spans="1:256" ht="12" customHeight="1">
+    <row r="30" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="7"/>
       <c r="B30" s="7"/>
       <c r="C30" s="7"/>
@@ -7420,7 +7497,7 @@
       <c r="IU30" s="3"/>
       <c r="IV30" s="3"/>
     </row>
-    <row r="31" spans="1:256" ht="12" customHeight="1">
+    <row r="31" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="7"/>
       <c r="B31" s="7"/>
       <c r="C31" s="7"/>
@@ -7678,7 +7755,7 @@
       <c r="IU31" s="3"/>
       <c r="IV31" s="3"/>
     </row>
-    <row r="32" spans="1:256" ht="12" customHeight="1">
+    <row r="32" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="20" t="s">
         <v>38</v>
       </c>
@@ -7940,7 +8017,7 @@
       <c r="IU32" s="3"/>
       <c r="IV32" s="3"/>
     </row>
-    <row r="33" spans="1:256" ht="12" customHeight="1">
+    <row r="33" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="20" t="s">
         <v>40</v>
       </c>
@@ -8202,7 +8279,7 @@
       <c r="IU33" s="3"/>
       <c r="IV33" s="3"/>
     </row>
-    <row r="34" spans="1:256" ht="12" customHeight="1">
+    <row r="34" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="17"/>
       <c r="B34" s="18"/>
       <c r="C34" s="18"/>
@@ -8460,7 +8537,7 @@
       <c r="IU34" s="3"/>
       <c r="IV34" s="3"/>
     </row>
-    <row r="35" spans="1:256" ht="12" customHeight="1">
+    <row r="35" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="17"/>
       <c r="B35" s="18"/>
       <c r="C35" s="18"/>
@@ -8718,7 +8795,7 @@
       <c r="IU35" s="3"/>
       <c r="IV35" s="3"/>
     </row>
-    <row r="36" spans="1:256" ht="12" customHeight="1">
+    <row r="36" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="20" t="s">
         <v>42</v>
       </c>
@@ -8980,7 +9057,7 @@
       <c r="IU36" s="3"/>
       <c r="IV36" s="3"/>
     </row>
-    <row r="37" spans="1:256" ht="12" customHeight="1">
+    <row r="37" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="20" t="s">
         <v>44</v>
       </c>
@@ -9242,7 +9319,7 @@
       <c r="IU37" s="3"/>
       <c r="IV37" s="3"/>
     </row>
-    <row r="38" spans="1:256" ht="12" customHeight="1">
+    <row r="38" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="17"/>
       <c r="B38" s="18"/>
       <c r="C38" s="18"/>
@@ -9500,7 +9577,7 @@
       <c r="IU38" s="3"/>
       <c r="IV38" s="3"/>
     </row>
-    <row r="39" spans="1:256" ht="12" customHeight="1">
+    <row r="39" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="17"/>
       <c r="B39" s="18"/>
       <c r="C39" s="18"/>
@@ -9758,7 +9835,7 @@
       <c r="IU39" s="3"/>
       <c r="IV39" s="3"/>
     </row>
-    <row r="40" spans="1:256" ht="12" customHeight="1">
+    <row r="40" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="21" t="s">
         <v>46</v>
       </c>
@@ -10020,7 +10097,7 @@
       <c r="IU40" s="3"/>
       <c r="IV40" s="3"/>
     </row>
-    <row r="41" spans="1:256" ht="12" customHeight="1">
+    <row r="41" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="21" t="s">
         <v>48</v>
       </c>
@@ -10282,7 +10359,7 @@
       <c r="IU41" s="3"/>
       <c r="IV41" s="3"/>
     </row>
-    <row r="42" spans="1:256" ht="12" customHeight="1">
+    <row r="42" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="17"/>
       <c r="B42" s="18"/>
       <c r="C42" s="18"/>
@@ -10540,7 +10617,7 @@
       <c r="IU42" s="3"/>
       <c r="IV42" s="3"/>
     </row>
-    <row r="43" spans="1:256" ht="12" customHeight="1">
+    <row r="43" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="17"/>
       <c r="B43" s="18"/>
       <c r="C43" s="18"/>
@@ -10798,7 +10875,7 @@
       <c r="IU43" s="3"/>
       <c r="IV43" s="3"/>
     </row>
-    <row r="44" spans="1:256" ht="12" customHeight="1">
+    <row r="44" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="11" t="s">
         <v>50</v>
       </c>
@@ -11060,7 +11137,7 @@
       <c r="IU44" s="3"/>
       <c r="IV44" s="3"/>
     </row>
-    <row r="45" spans="1:256" ht="12" customHeight="1">
+    <row r="45" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="11" t="s">
         <v>52</v>
       </c>
@@ -11322,7 +11399,7 @@
       <c r="IU45" s="3"/>
       <c r="IV45" s="3"/>
     </row>
-    <row r="46" spans="1:256" ht="12" customHeight="1">
+    <row r="46" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="11" t="s">
         <v>54</v>
       </c>
@@ -11584,7 +11661,7 @@
       <c r="IU46" s="3"/>
       <c r="IV46" s="3"/>
     </row>
-    <row r="47" spans="1:256" ht="12" customHeight="1">
+    <row r="47" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="11" t="s">
         <v>56</v>
       </c>
@@ -11846,7 +11923,7 @@
       <c r="IU47" s="3"/>
       <c r="IV47" s="3"/>
     </row>
-    <row r="48" spans="1:256" ht="12" customHeight="1">
+    <row r="48" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="11" t="s">
         <v>58</v>
       </c>
@@ -12108,7 +12185,7 @@
       <c r="IU48" s="3"/>
       <c r="IV48" s="3"/>
     </row>
-    <row r="49" spans="1:256" ht="12" customHeight="1">
+    <row r="49" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="11" t="s">
         <v>60</v>
       </c>
@@ -12370,7 +12447,7 @@
       <c r="IU49" s="3"/>
       <c r="IV49" s="3"/>
     </row>
-    <row r="50" spans="1:256" ht="12" customHeight="1">
+    <row r="50" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="11" t="s">
         <v>62</v>
       </c>
@@ -12632,7 +12709,7 @@
       <c r="IU50" s="3"/>
       <c r="IV50" s="3"/>
     </row>
-    <row r="51" spans="1:256" ht="12" customHeight="1">
+    <row r="51" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" s="11" t="s">
         <v>64</v>
       </c>
@@ -12892,7 +12969,7 @@
       <c r="IU51" s="3"/>
       <c r="IV51" s="3"/>
     </row>
-    <row r="52" spans="1:256" ht="12" customHeight="1">
+    <row r="52" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" s="11" t="s">
         <v>65</v>
       </c>
@@ -13154,7 +13231,7 @@
       <c r="IU52" s="3"/>
       <c r="IV52" s="3"/>
     </row>
-    <row r="53" spans="1:256" ht="12" customHeight="1">
+    <row r="53" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" s="17"/>
       <c r="B53" s="18"/>
       <c r="C53" s="18"/>
@@ -13412,7 +13489,7 @@
       <c r="IU53" s="3"/>
       <c r="IV53" s="3"/>
     </row>
-    <row r="54" spans="1:256" ht="12" customHeight="1">
+    <row r="54" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A54" s="17"/>
       <c r="B54" s="18"/>
       <c r="C54" s="18"/>
@@ -13670,7 +13747,7 @@
       <c r="IU54" s="3"/>
       <c r="IV54" s="3"/>
     </row>
-    <row r="55" spans="1:256" ht="12" customHeight="1">
+    <row r="55" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" s="2" t="s">
         <v>142</v>
       </c>
@@ -13930,7 +14007,7 @@
       <c r="IU55" s="3"/>
       <c r="IV55" s="3"/>
     </row>
-    <row r="56" spans="1:256" ht="12" customHeight="1">
+    <row r="56" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A56" s="35" t="s">
         <v>143</v>
       </c>
@@ -14194,7 +14271,7 @@
       <c r="IU56" s="3"/>
       <c r="IV56" s="3"/>
     </row>
-    <row r="57" spans="1:256" ht="12" customHeight="1">
+    <row r="57" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A57" s="36" t="s">
         <v>146</v>
       </c>
@@ -14458,7 +14535,7 @@
       <c r="IU57" s="3"/>
       <c r="IV57" s="3"/>
     </row>
-    <row r="58" spans="1:256" ht="12" customHeight="1">
+    <row r="58" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A58" s="36" t="s">
         <v>149</v>
       </c>
@@ -14722,7 +14799,7 @@
       <c r="IU58" s="3"/>
       <c r="IV58" s="3"/>
     </row>
-    <row r="59" spans="1:256" ht="12" customHeight="1">
+    <row r="59" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A59" s="36" t="s">
         <v>152</v>
       </c>
@@ -14986,7 +15063,7 @@
       <c r="IU59" s="3"/>
       <c r="IV59" s="3"/>
     </row>
-    <row r="60" spans="1:256" ht="12" customHeight="1">
+    <row r="60" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A60" s="36" t="s">
         <v>155</v>
       </c>
@@ -15250,7 +15327,7 @@
       <c r="IU60" s="3"/>
       <c r="IV60" s="3"/>
     </row>
-    <row r="61" spans="1:256" ht="12" customHeight="1">
+    <row r="61" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A61" s="17"/>
       <c r="B61" s="18"/>
       <c r="C61" s="18"/>
@@ -15508,7 +15585,7 @@
       <c r="IU61" s="3"/>
       <c r="IV61" s="3"/>
     </row>
-    <row r="62" spans="1:256" ht="12" customHeight="1">
+    <row r="62" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
         <v>67</v>
       </c>
@@ -15768,7 +15845,7 @@
       <c r="IU62" s="3"/>
       <c r="IV62" s="3"/>
     </row>
-    <row r="63" spans="1:256" ht="16.5" customHeight="1">
+    <row r="63" spans="1:256" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="23" t="s">
         <v>68</v>
       </c>
@@ -15792,7 +15869,7 @@
       <c r="Q63" s="7"/>
       <c r="R63" s="7"/>
     </row>
-    <row r="64" spans="1:256" ht="12" customHeight="1">
+    <row r="64" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A64" s="25" t="s">
         <v>70</v>
       </c>
@@ -16054,7 +16131,7 @@
       <c r="IU64" s="3"/>
       <c r="IV64" s="3"/>
     </row>
-    <row r="65" spans="1:256" ht="15.95" customHeight="1">
+    <row r="65" spans="1:256" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A65" s="3"/>
       <c r="B65" s="3"/>
       <c r="C65" s="7"/>
@@ -16312,7 +16389,7 @@
       <c r="IU65" s="3"/>
       <c r="IV65" s="3"/>
     </row>
-    <row r="66" spans="1:256" ht="15.95" customHeight="1">
+    <row r="66" spans="1:256" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A66" s="3"/>
       <c r="B66" s="3"/>
       <c r="C66" s="7"/>
@@ -16570,7 +16647,7 @@
       <c r="IU66" s="3"/>
       <c r="IV66" s="3"/>
     </row>
-    <row r="67" spans="1:256" ht="15.95" customHeight="1">
+    <row r="67" spans="1:256" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A67" s="3"/>
       <c r="B67" s="3"/>
       <c r="C67" s="7"/>
@@ -16828,7 +16905,7 @@
       <c r="IU67" s="3"/>
       <c r="IV67" s="3"/>
     </row>
-    <row r="68" spans="1:256" ht="15.95" customHeight="1">
+    <row r="68" spans="1:256" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A68" s="3"/>
       <c r="B68" s="3"/>
       <c r="C68" s="7"/>
@@ -17086,7 +17163,7 @@
       <c r="IU68" s="3"/>
       <c r="IV68" s="3"/>
     </row>
-    <row r="69" spans="1:256">
+    <row r="69" spans="1:256" x14ac:dyDescent="0.35">
       <c r="A69" s="3"/>
       <c r="B69" s="3"/>
       <c r="C69" s="7"/>
@@ -17344,7 +17421,7 @@
       <c r="IU69" s="3"/>
       <c r="IV69" s="3"/>
     </row>
-    <row r="70" spans="1:256" ht="15.75" customHeight="1">
+    <row r="70" spans="1:256" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A70" s="3"/>
       <c r="B70" s="3"/>
       <c r="C70" s="7"/>
@@ -17602,7 +17679,7 @@
       <c r="IU70" s="3"/>
       <c r="IV70" s="3"/>
     </row>
-    <row r="71" spans="1:256" ht="15.75" customHeight="1">
+    <row r="71" spans="1:256" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A71" s="3"/>
       <c r="B71" s="3"/>
       <c r="C71" s="3"/>
@@ -17860,7 +17937,7 @@
       <c r="IU71" s="3"/>
       <c r="IV71" s="3"/>
     </row>
-    <row r="72" spans="1:256" ht="12" customHeight="1">
+    <row r="72" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A72" s="1" t="s">
         <v>195</v>
       </c>
@@ -18119,7 +18196,7 @@
       <c r="IU72" s="3"/>
       <c r="IV72" s="3"/>
     </row>
-    <row r="73" spans="1:256" ht="15.75" customHeight="1">
+    <row r="73" spans="1:256" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A73" s="23" t="s">
         <v>196</v>
       </c>
@@ -18380,7 +18457,7 @@
       <c r="IU73" s="3"/>
       <c r="IV73" s="3"/>
     </row>
-    <row r="74" spans="1:256" ht="15.75" customHeight="1">
+    <row r="74" spans="1:256" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A74" s="25" t="s">
         <v>198</v>
       </c>
@@ -18641,7 +18718,7 @@
       <c r="IU74" s="3"/>
       <c r="IV74" s="3"/>
     </row>
-    <row r="75" spans="1:256" ht="15.75" customHeight="1">
+    <row r="75" spans="1:256" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A75" s="3"/>
       <c r="B75" s="3"/>
       <c r="C75" s="3"/>
@@ -18898,7 +18975,7 @@
       <c r="IU75" s="3"/>
       <c r="IV75" s="3"/>
     </row>
-    <row r="76" spans="1:256" ht="15.75" customHeight="1">
+    <row r="76" spans="1:256" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E76" s="3"/>
       <c r="F76" s="3"/>
       <c r="G76" s="3"/>
@@ -19152,7 +19229,7 @@
       <c r="IU76" s="3"/>
       <c r="IV76" s="3"/>
     </row>
-    <row r="77" spans="1:256" ht="12" customHeight="1">
+    <row r="77" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="I77" s="7"/>
       <c r="J77" s="7"/>
       <c r="K77" s="7"/>
@@ -19164,27 +19241,27 @@
       <c r="Q77" s="7"/>
       <c r="R77" s="7"/>
     </row>
-    <row r="78" spans="1:256" ht="15.95" customHeight="1"/>
-    <row r="79" spans="1:256" ht="15.95" customHeight="1"/>
-    <row r="80" spans="1:256" ht="15.95" customHeight="1"/>
-    <row r="81" ht="15.95" customHeight="1"/>
-    <row r="82" ht="15.95" customHeight="1"/>
-    <row r="83" ht="15.95" customHeight="1"/>
-    <row r="84" ht="15.95" customHeight="1"/>
-    <row r="85" ht="15.95" customHeight="1"/>
-    <row r="86" ht="15.95" customHeight="1"/>
-    <row r="87" ht="15.95" customHeight="1"/>
-    <row r="88" ht="15.95" customHeight="1"/>
-    <row r="89" ht="15.95" customHeight="1"/>
-    <row r="90" ht="15.95" customHeight="1"/>
-    <row r="91" ht="15.95" customHeight="1"/>
-    <row r="92" ht="15.95" customHeight="1"/>
-    <row r="93" ht="15.95" customHeight="1"/>
-    <row r="94" ht="15.95" customHeight="1"/>
-    <row r="95" ht="15.95" customHeight="1"/>
-    <row r="96" ht="15.95" customHeight="1"/>
-    <row r="97" spans="1:16" ht="15.95" customHeight="1"/>
-    <row r="98" spans="1:16" ht="15.95" customHeight="1">
+    <row r="78" spans="1:256" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="79" spans="1:256" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="80" spans="1:256" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="81" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="82" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="83" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="84" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="85" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="86" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="87" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="88" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="89" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="90" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="91" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="92" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="93" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="94" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="95" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="96" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="97" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="98" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
         <v>201</v>
       </c>
@@ -19204,7 +19281,7 @@
       <c r="O98" s="1"/>
       <c r="P98" s="1"/>
     </row>
-    <row r="99" spans="1:16" ht="15.95" customHeight="1">
+    <row r="99" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A99" s="23" t="s">
         <v>202</v>
       </c>
@@ -19254,7 +19331,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="100" spans="1:16" ht="15.95" customHeight="1">
+    <row r="100" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A100" s="25" t="s">
         <v>218</v>
       </c>
@@ -19304,77 +19381,77 @@
         <v>233</v>
       </c>
     </row>
-    <row r="101" spans="1:16" ht="15.95" customHeight="1"/>
-    <row r="102" spans="1:16" ht="15.95" customHeight="1"/>
-    <row r="103" spans="1:16" ht="15.95" customHeight="1"/>
-    <row r="104" spans="1:16" ht="15.95" customHeight="1"/>
-    <row r="105" spans="1:16" ht="15.95" customHeight="1"/>
-    <row r="106" spans="1:16" ht="15.95" customHeight="1"/>
-    <row r="107" spans="1:16" ht="15.95" customHeight="1"/>
-    <row r="108" spans="1:16" ht="15.95" customHeight="1"/>
-    <row r="109" spans="1:16" ht="15.95" customHeight="1"/>
-    <row r="110" spans="1:16" ht="15.95" customHeight="1"/>
-    <row r="111" spans="1:16" ht="15.95" customHeight="1"/>
-    <row r="112" spans="1:16" ht="15.95" customHeight="1"/>
-    <row r="113" ht="15.95" customHeight="1"/>
-    <row r="114" ht="15.95" customHeight="1"/>
-    <row r="115" ht="15.95" customHeight="1"/>
-    <row r="116" ht="15.95" customHeight="1"/>
-    <row r="117" ht="15.95" customHeight="1"/>
-    <row r="118" ht="15.95" customHeight="1"/>
-    <row r="119" ht="15.95" customHeight="1"/>
-    <row r="120" ht="15.95" customHeight="1"/>
-    <row r="121" ht="15.95" customHeight="1"/>
-    <row r="122" ht="15.95" customHeight="1"/>
-    <row r="123" ht="15.95" customHeight="1"/>
-    <row r="124" ht="15.95" customHeight="1"/>
-    <row r="125" ht="15.95" customHeight="1"/>
-    <row r="126" ht="15.95" customHeight="1"/>
-    <row r="127" ht="15.95" customHeight="1"/>
-    <row r="128" ht="15.95" customHeight="1"/>
-    <row r="129" ht="15.95" customHeight="1"/>
-    <row r="130" ht="15.95" customHeight="1"/>
-    <row r="131" ht="15.95" customHeight="1"/>
-    <row r="132" ht="15.95" customHeight="1"/>
-    <row r="133" ht="15.95" customHeight="1"/>
-    <row r="134" ht="15.95" customHeight="1"/>
-    <row r="135" ht="15.95" customHeight="1"/>
-    <row r="136" ht="15.95" customHeight="1"/>
-    <row r="137" ht="15.95" customHeight="1"/>
-    <row r="138" ht="15.95" customHeight="1"/>
-    <row r="139" ht="15.95" customHeight="1"/>
-    <row r="140" ht="15.95" customHeight="1"/>
-    <row r="141" ht="15.95" customHeight="1"/>
-    <row r="142" ht="15.95" customHeight="1"/>
-    <row r="143" ht="15.95" customHeight="1"/>
-    <row r="144" ht="15.95" customHeight="1"/>
-    <row r="145" ht="15.95" customHeight="1"/>
-    <row r="146" ht="15.95" customHeight="1"/>
-    <row r="147" ht="15.95" customHeight="1"/>
-    <row r="148" ht="15.95" customHeight="1"/>
-    <row r="149" ht="15.95" customHeight="1"/>
-    <row r="150" ht="15.95" customHeight="1"/>
-    <row r="151" ht="15.95" customHeight="1"/>
-    <row r="152" ht="15.95" customHeight="1"/>
-    <row r="153" ht="15.95" customHeight="1"/>
-    <row r="154" ht="15.95" customHeight="1"/>
-    <row r="155" ht="15.95" customHeight="1"/>
-    <row r="156" ht="15.95" customHeight="1"/>
-    <row r="157" ht="15.95" customHeight="1"/>
-    <row r="158" ht="15.95" customHeight="1"/>
-    <row r="159" ht="15.95" customHeight="1"/>
-    <row r="160" ht="15.95" customHeight="1"/>
-    <row r="161" spans="1:6" ht="15.95" customHeight="1"/>
-    <row r="162" spans="1:6" ht="15.95" customHeight="1"/>
-    <row r="163" spans="1:6" ht="15.95" customHeight="1"/>
-    <row r="164" spans="1:6" ht="15.95" customHeight="1"/>
-    <row r="165" spans="1:6" ht="15.95" customHeight="1"/>
-    <row r="166" spans="1:6" ht="15.95" customHeight="1"/>
-    <row r="167" spans="1:6" ht="15.95" customHeight="1"/>
-    <row r="168" spans="1:6" ht="15.95" customHeight="1"/>
-    <row r="169" spans="1:6" ht="15.95" customHeight="1"/>
-    <row r="170" spans="1:6" ht="15.95" customHeight="1"/>
-    <row r="171" spans="1:6" ht="15.95" customHeight="1">
+    <row r="101" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="102" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="103" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="104" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="105" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="106" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="107" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="108" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="109" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="110" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="111" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="112" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="113" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="114" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="115" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="116" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="117" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="118" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="119" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="120" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="121" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="122" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="123" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="124" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="125" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="126" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="127" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="128" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="129" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="130" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="131" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="132" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="133" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="134" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="135" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="136" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="137" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="138" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="139" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="140" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="141" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="142" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="143" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="144" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="145" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="146" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="147" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="148" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="149" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="150" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="151" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="152" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="153" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="154" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="155" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="156" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="157" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="158" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="159" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="160" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="161" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="162" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="163" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="164" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="165" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="166" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="167" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="168" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="169" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="170" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="171" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A171" s="1" t="s">
         <v>200</v>
       </c>
@@ -19384,7 +19461,7 @@
       <c r="E171" s="1"/>
       <c r="F171" s="1"/>
     </row>
-    <row r="172" spans="1:6" ht="15.95" customHeight="1">
+    <row r="172" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A172" s="23" t="s">
         <v>234</v>
       </c>
@@ -19404,7 +19481,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="173" spans="1:6" ht="15.95" customHeight="1">
+    <row r="173" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A173" s="25" t="s">
         <v>240</v>
       </c>
@@ -19424,874 +19501,874 @@
         <v>245</v>
       </c>
     </row>
-    <row r="174" spans="1:6" ht="15.95" customHeight="1"/>
-    <row r="175" spans="1:6" ht="15.95" customHeight="1"/>
-    <row r="176" spans="1:6" ht="15.95" customHeight="1"/>
-    <row r="177" ht="15.95" customHeight="1"/>
-    <row r="178" ht="15.95" customHeight="1"/>
-    <row r="179" ht="15.95" customHeight="1"/>
-    <row r="180" ht="15.95" customHeight="1"/>
-    <row r="181" ht="15.95" customHeight="1"/>
-    <row r="182" ht="15.95" customHeight="1"/>
-    <row r="183" ht="15.95" customHeight="1"/>
-    <row r="184" ht="15.95" customHeight="1"/>
-    <row r="185" ht="15.95" customHeight="1"/>
-    <row r="186" ht="15.95" customHeight="1"/>
-    <row r="187" ht="15.95" customHeight="1"/>
-    <row r="188" ht="15.95" customHeight="1"/>
-    <row r="189" ht="15.95" customHeight="1"/>
-    <row r="190" ht="15.95" customHeight="1"/>
-    <row r="191" ht="15.95" customHeight="1"/>
-    <row r="192" ht="15.95" customHeight="1"/>
-    <row r="193" ht="15.95" customHeight="1"/>
-    <row r="194" ht="15.95" customHeight="1"/>
-    <row r="195" ht="15.95" customHeight="1"/>
-    <row r="196" ht="15.95" customHeight="1"/>
-    <row r="197" ht="15.95" customHeight="1"/>
-    <row r="198" ht="15.95" customHeight="1"/>
-    <row r="199" ht="15.95" customHeight="1"/>
-    <row r="200" ht="15.95" customHeight="1"/>
-    <row r="201" ht="15.95" customHeight="1"/>
-    <row r="202" ht="15.95" customHeight="1"/>
-    <row r="203" ht="15.95" customHeight="1"/>
-    <row r="204" ht="15.95" customHeight="1"/>
-    <row r="205" ht="15.95" customHeight="1"/>
-    <row r="206" ht="15.95" customHeight="1"/>
-    <row r="207" ht="15.95" customHeight="1"/>
-    <row r="208" ht="15.95" customHeight="1"/>
-    <row r="209" ht="15.95" customHeight="1"/>
-    <row r="210" ht="15.95" customHeight="1"/>
-    <row r="211" ht="15.95" customHeight="1"/>
-    <row r="212" ht="15.95" customHeight="1"/>
-    <row r="213" ht="15.95" customHeight="1"/>
-    <row r="214" ht="15.95" customHeight="1"/>
-    <row r="215" ht="15.95" customHeight="1"/>
-    <row r="216" ht="15.95" customHeight="1"/>
-    <row r="217" ht="15.95" customHeight="1"/>
-    <row r="218" ht="15.95" customHeight="1"/>
-    <row r="219" ht="15.95" customHeight="1"/>
-    <row r="220" ht="15.95" customHeight="1"/>
-    <row r="221" ht="15.95" customHeight="1"/>
-    <row r="222" ht="15.95" customHeight="1"/>
-    <row r="223" ht="15.95" customHeight="1"/>
-    <row r="224" ht="15.95" customHeight="1"/>
-    <row r="225" ht="15.95" customHeight="1"/>
-    <row r="226" ht="15.95" customHeight="1"/>
-    <row r="227" ht="15.95" customHeight="1"/>
-    <row r="228" ht="15.95" customHeight="1"/>
-    <row r="229" ht="15.95" customHeight="1"/>
-    <row r="230" ht="15.95" customHeight="1"/>
-    <row r="231" ht="15.95" customHeight="1"/>
-    <row r="232" ht="15.95" customHeight="1"/>
-    <row r="233" ht="15.95" customHeight="1"/>
-    <row r="234" ht="15.95" customHeight="1"/>
-    <row r="235" ht="15.95" customHeight="1"/>
-    <row r="236" ht="15.95" customHeight="1"/>
-    <row r="237" ht="15.95" customHeight="1"/>
-    <row r="238" ht="15.95" customHeight="1"/>
-    <row r="239" ht="15.95" customHeight="1"/>
-    <row r="240" ht="15.95" customHeight="1"/>
-    <row r="241" ht="15.95" customHeight="1"/>
-    <row r="242" ht="15.95" customHeight="1"/>
-    <row r="243" ht="15.95" customHeight="1"/>
-    <row r="244" ht="15.95" customHeight="1"/>
-    <row r="245" ht="15.95" customHeight="1"/>
-    <row r="246" ht="15.95" customHeight="1"/>
-    <row r="247" ht="15.95" customHeight="1"/>
-    <row r="248" ht="15.95" customHeight="1"/>
-    <row r="249" ht="15.95" customHeight="1"/>
-    <row r="250" ht="15.95" customHeight="1"/>
-    <row r="251" ht="15.95" customHeight="1"/>
-    <row r="252" ht="15.95" customHeight="1"/>
-    <row r="253" ht="15.95" customHeight="1"/>
-    <row r="254" ht="15.95" customHeight="1"/>
-    <row r="255" ht="15.95" customHeight="1"/>
-    <row r="256" ht="15.95" customHeight="1"/>
-    <row r="257" ht="15.95" customHeight="1"/>
-    <row r="258" ht="15.95" customHeight="1"/>
-    <row r="259" ht="15.95" customHeight="1"/>
-    <row r="260" ht="15.95" customHeight="1"/>
-    <row r="261" ht="15.95" customHeight="1"/>
-    <row r="262" ht="15.95" customHeight="1"/>
-    <row r="263" ht="15.95" customHeight="1"/>
-    <row r="264" ht="15.95" customHeight="1"/>
-    <row r="265" ht="15.95" customHeight="1"/>
-    <row r="266" ht="15.95" customHeight="1"/>
-    <row r="267" ht="15.95" customHeight="1"/>
-    <row r="268" ht="15.95" customHeight="1"/>
-    <row r="269" ht="15.95" customHeight="1"/>
-    <row r="270" ht="15.95" customHeight="1"/>
-    <row r="271" ht="15.95" customHeight="1"/>
-    <row r="272" ht="15.95" customHeight="1"/>
-    <row r="273" ht="15.95" customHeight="1"/>
-    <row r="274" ht="15.95" customHeight="1"/>
-    <row r="275" ht="15.95" customHeight="1"/>
-    <row r="276" ht="15.95" customHeight="1"/>
-    <row r="277" ht="15.95" customHeight="1"/>
-    <row r="278" ht="15.95" customHeight="1"/>
-    <row r="279" ht="15.95" customHeight="1"/>
-    <row r="280" ht="15.95" customHeight="1"/>
-    <row r="281" ht="15.95" customHeight="1"/>
-    <row r="282" ht="15.95" customHeight="1"/>
-    <row r="283" ht="15.95" customHeight="1"/>
-    <row r="284" ht="15.95" customHeight="1"/>
-    <row r="285" ht="15.95" customHeight="1"/>
-    <row r="286" ht="15.95" customHeight="1"/>
-    <row r="287" ht="15.95" customHeight="1"/>
-    <row r="288" ht="15.95" customHeight="1"/>
-    <row r="289" ht="15.95" customHeight="1"/>
-    <row r="290" ht="15.95" customHeight="1"/>
-    <row r="291" ht="15.95" customHeight="1"/>
-    <row r="292" ht="15.95" customHeight="1"/>
-    <row r="293" ht="15.95" customHeight="1"/>
-    <row r="294" ht="15.95" customHeight="1"/>
-    <row r="295" ht="15.95" customHeight="1"/>
-    <row r="296" ht="15.95" customHeight="1"/>
-    <row r="297" ht="15.95" customHeight="1"/>
-    <row r="298" ht="15.95" customHeight="1"/>
-    <row r="299" ht="15.95" customHeight="1"/>
-    <row r="300" ht="15.95" customHeight="1"/>
-    <row r="301" ht="15.95" customHeight="1"/>
-    <row r="302" ht="15.95" customHeight="1"/>
-    <row r="303" ht="15.95" customHeight="1"/>
-    <row r="304" ht="15.95" customHeight="1"/>
-    <row r="305" ht="15.95" customHeight="1"/>
-    <row r="306" ht="15.95" customHeight="1"/>
-    <row r="307" ht="15.95" customHeight="1"/>
-    <row r="308" ht="15.95" customHeight="1"/>
-    <row r="309" ht="15.95" customHeight="1"/>
-    <row r="310" ht="15.95" customHeight="1"/>
-    <row r="311" ht="15.95" customHeight="1"/>
-    <row r="312" ht="15.95" customHeight="1"/>
-    <row r="313" ht="15.95" customHeight="1"/>
-    <row r="314" ht="15.95" customHeight="1"/>
-    <row r="315" ht="15.95" customHeight="1"/>
-    <row r="316" ht="15.95" customHeight="1"/>
-    <row r="317" ht="15.95" customHeight="1"/>
-    <row r="318" ht="15.95" customHeight="1"/>
-    <row r="319" ht="15.95" customHeight="1"/>
-    <row r="320" ht="15.95" customHeight="1"/>
-    <row r="321" ht="15.95" customHeight="1"/>
-    <row r="322" ht="15.95" customHeight="1"/>
-    <row r="323" ht="15.95" customHeight="1"/>
-    <row r="324" ht="15.95" customHeight="1"/>
-    <row r="325" ht="15.95" customHeight="1"/>
-    <row r="326" ht="15.95" customHeight="1"/>
-    <row r="327" ht="15.95" customHeight="1"/>
-    <row r="328" ht="15.95" customHeight="1"/>
-    <row r="329" ht="15.95" customHeight="1"/>
-    <row r="330" ht="15.95" customHeight="1"/>
-    <row r="331" ht="15.95" customHeight="1"/>
-    <row r="332" ht="15.95" customHeight="1"/>
-    <row r="333" ht="15.95" customHeight="1"/>
-    <row r="334" ht="15.95" customHeight="1"/>
-    <row r="335" ht="15.95" customHeight="1"/>
-    <row r="336" ht="15.95" customHeight="1"/>
-    <row r="337" ht="15.95" customHeight="1"/>
-    <row r="338" ht="15.95" customHeight="1"/>
-    <row r="339" ht="15.95" customHeight="1"/>
-    <row r="340" ht="15.95" customHeight="1"/>
-    <row r="341" ht="15.95" customHeight="1"/>
-    <row r="342" ht="15.95" customHeight="1"/>
-    <row r="343" ht="15.95" customHeight="1"/>
-    <row r="344" ht="15.95" customHeight="1"/>
-    <row r="345" ht="15.95" customHeight="1"/>
-    <row r="346" ht="15.95" customHeight="1"/>
-    <row r="347" ht="15.95" customHeight="1"/>
-    <row r="348" ht="15.95" customHeight="1"/>
-    <row r="349" ht="15.95" customHeight="1"/>
-    <row r="350" ht="15.95" customHeight="1"/>
-    <row r="351" ht="15.95" customHeight="1"/>
-    <row r="352" ht="15.95" customHeight="1"/>
-    <row r="353" ht="15.95" customHeight="1"/>
-    <row r="354" ht="15.95" customHeight="1"/>
-    <row r="355" ht="15.95" customHeight="1"/>
-    <row r="356" ht="15.95" customHeight="1"/>
-    <row r="357" ht="15.95" customHeight="1"/>
-    <row r="358" ht="15.95" customHeight="1"/>
-    <row r="359" ht="15.95" customHeight="1"/>
-    <row r="360" ht="15.95" customHeight="1"/>
-    <row r="361" ht="15.95" customHeight="1"/>
-    <row r="362" ht="15.95" customHeight="1"/>
-    <row r="363" ht="15.95" customHeight="1"/>
-    <row r="364" ht="15.95" customHeight="1"/>
-    <row r="365" ht="15.95" customHeight="1"/>
-    <row r="366" ht="15.95" customHeight="1"/>
-    <row r="367" ht="15.95" customHeight="1"/>
-    <row r="368" ht="15.95" customHeight="1"/>
-    <row r="369" ht="15.95" customHeight="1"/>
-    <row r="370" ht="15.95" customHeight="1"/>
-    <row r="371" ht="15.95" customHeight="1"/>
-    <row r="372" ht="15.95" customHeight="1"/>
-    <row r="373" ht="15.95" customHeight="1"/>
-    <row r="374" ht="15.95" customHeight="1"/>
-    <row r="375" ht="15.95" customHeight="1"/>
-    <row r="376" ht="15.95" customHeight="1"/>
-    <row r="377" ht="15.95" customHeight="1"/>
-    <row r="378" ht="15.95" customHeight="1"/>
-    <row r="379" ht="15.95" customHeight="1"/>
-    <row r="380" ht="15.95" customHeight="1"/>
-    <row r="381" ht="15.95" customHeight="1"/>
-    <row r="382" ht="15.95" customHeight="1"/>
-    <row r="383" ht="15.95" customHeight="1"/>
-    <row r="384" ht="15.95" customHeight="1"/>
-    <row r="385" ht="15.95" customHeight="1"/>
-    <row r="386" ht="15.95" customHeight="1"/>
-    <row r="387" ht="15.95" customHeight="1"/>
-    <row r="388" ht="15.95" customHeight="1"/>
-    <row r="389" ht="15.95" customHeight="1"/>
-    <row r="390" ht="15.95" customHeight="1"/>
-    <row r="391" ht="15.95" customHeight="1"/>
-    <row r="392" ht="15.95" customHeight="1"/>
-    <row r="393" ht="15.95" customHeight="1"/>
-    <row r="394" ht="15.95" customHeight="1"/>
-    <row r="395" ht="15.95" customHeight="1"/>
-    <row r="396" ht="15.95" customHeight="1"/>
-    <row r="397" ht="15.95" customHeight="1"/>
-    <row r="398" ht="15.95" customHeight="1"/>
-    <row r="399" ht="15.95" customHeight="1"/>
-    <row r="400" ht="15.95" customHeight="1"/>
-    <row r="401" ht="15.95" customHeight="1"/>
-    <row r="402" ht="15.95" customHeight="1"/>
-    <row r="403" ht="15.95" customHeight="1"/>
-    <row r="404" ht="15.95" customHeight="1"/>
-    <row r="405" ht="15.95" customHeight="1"/>
-    <row r="406" ht="15.95" customHeight="1"/>
-    <row r="407" ht="15.95" customHeight="1"/>
-    <row r="408" ht="15.95" customHeight="1"/>
-    <row r="409" ht="15.95" customHeight="1"/>
-    <row r="410" ht="15.95" customHeight="1"/>
-    <row r="411" ht="15.95" customHeight="1"/>
-    <row r="412" ht="15.95" customHeight="1"/>
-    <row r="413" ht="15.95" customHeight="1"/>
-    <row r="414" ht="15.95" customHeight="1"/>
-    <row r="415" ht="15.95" customHeight="1"/>
-    <row r="416" ht="15.95" customHeight="1"/>
-    <row r="417" ht="15.95" customHeight="1"/>
-    <row r="418" ht="15.95" customHeight="1"/>
-    <row r="419" ht="15.95" customHeight="1"/>
-    <row r="420" ht="15.95" customHeight="1"/>
-    <row r="421" ht="15.95" customHeight="1"/>
-    <row r="422" ht="15.95" customHeight="1"/>
-    <row r="423" ht="15.95" customHeight="1"/>
-    <row r="424" ht="15.95" customHeight="1"/>
-    <row r="425" ht="15.95" customHeight="1"/>
-    <row r="426" ht="15.95" customHeight="1"/>
-    <row r="427" ht="15.95" customHeight="1"/>
-    <row r="428" ht="15.95" customHeight="1"/>
-    <row r="429" ht="15.95" customHeight="1"/>
-    <row r="430" ht="15.95" customHeight="1"/>
-    <row r="431" ht="15.95" customHeight="1"/>
-    <row r="432" ht="15.95" customHeight="1"/>
-    <row r="433" ht="15.95" customHeight="1"/>
-    <row r="434" ht="15.95" customHeight="1"/>
-    <row r="435" ht="15.95" customHeight="1"/>
-    <row r="436" ht="15.95" customHeight="1"/>
-    <row r="437" ht="15.95" customHeight="1"/>
-    <row r="438" ht="15.95" customHeight="1"/>
-    <row r="439" ht="15.95" customHeight="1"/>
-    <row r="440" ht="15.95" customHeight="1"/>
-    <row r="441" ht="15.95" customHeight="1"/>
-    <row r="442" ht="15.95" customHeight="1"/>
-    <row r="443" ht="15.95" customHeight="1"/>
-    <row r="444" ht="15.95" customHeight="1"/>
-    <row r="445" ht="15.95" customHeight="1"/>
-    <row r="446" ht="15.95" customHeight="1"/>
-    <row r="447" ht="15.95" customHeight="1"/>
-    <row r="448" ht="15.95" customHeight="1"/>
-    <row r="449" ht="15.95" customHeight="1"/>
-    <row r="450" ht="15.95" customHeight="1"/>
-    <row r="451" ht="15.95" customHeight="1"/>
-    <row r="452" ht="15.95" customHeight="1"/>
-    <row r="453" ht="15.95" customHeight="1"/>
-    <row r="454" ht="15.95" customHeight="1"/>
-    <row r="455" ht="15.95" customHeight="1"/>
-    <row r="456" ht="15.95" customHeight="1"/>
-    <row r="457" ht="15.95" customHeight="1"/>
-    <row r="458" ht="15.95" customHeight="1"/>
-    <row r="459" ht="15.95" customHeight="1"/>
-    <row r="460" ht="15.95" customHeight="1"/>
-    <row r="461" ht="15.95" customHeight="1"/>
-    <row r="462" ht="15.95" customHeight="1"/>
-    <row r="463" ht="15.95" customHeight="1"/>
-    <row r="464" ht="15.95" customHeight="1"/>
-    <row r="465" ht="15.95" customHeight="1"/>
-    <row r="466" ht="15.95" customHeight="1"/>
-    <row r="467" ht="15.95" customHeight="1"/>
-    <row r="468" ht="15.95" customHeight="1"/>
-    <row r="469" ht="15.95" customHeight="1"/>
-    <row r="470" ht="15.95" customHeight="1"/>
-    <row r="471" ht="15.95" customHeight="1"/>
-    <row r="472" ht="15.95" customHeight="1"/>
-    <row r="473" ht="15.95" customHeight="1"/>
-    <row r="474" ht="15.95" customHeight="1"/>
-    <row r="475" ht="15.95" customHeight="1"/>
-    <row r="476" ht="15.95" customHeight="1"/>
-    <row r="477" ht="15.95" customHeight="1"/>
-    <row r="478" ht="15.95" customHeight="1"/>
-    <row r="479" ht="15.95" customHeight="1"/>
-    <row r="480" ht="15.95" customHeight="1"/>
-    <row r="481" ht="15.95" customHeight="1"/>
-    <row r="482" ht="15.95" customHeight="1"/>
-    <row r="483" ht="15.95" customHeight="1"/>
-    <row r="484" ht="15.95" customHeight="1"/>
-    <row r="485" ht="15.95" customHeight="1"/>
-    <row r="486" ht="15.95" customHeight="1"/>
-    <row r="487" ht="15.95" customHeight="1"/>
-    <row r="488" ht="15.95" customHeight="1"/>
-    <row r="489" ht="15.95" customHeight="1"/>
-    <row r="490" ht="15.95" customHeight="1"/>
-    <row r="491" ht="15.95" customHeight="1"/>
-    <row r="492" ht="15.95" customHeight="1"/>
-    <row r="493" ht="15.95" customHeight="1"/>
-    <row r="494" ht="15.95" customHeight="1"/>
-    <row r="495" ht="15.95" customHeight="1"/>
-    <row r="496" ht="15.95" customHeight="1"/>
-    <row r="497" ht="15.95" customHeight="1"/>
-    <row r="498" ht="15.95" customHeight="1"/>
-    <row r="499" ht="15.95" customHeight="1"/>
-    <row r="500" ht="15.95" customHeight="1"/>
-    <row r="501" ht="15.95" customHeight="1"/>
-    <row r="502" ht="15.95" customHeight="1"/>
-    <row r="503" ht="15.95" customHeight="1"/>
-    <row r="504" ht="15.95" customHeight="1"/>
-    <row r="505" ht="15.95" customHeight="1"/>
-    <row r="506" ht="15.95" customHeight="1"/>
-    <row r="507" ht="15.95" customHeight="1"/>
-    <row r="508" ht="15.95" customHeight="1"/>
-    <row r="509" ht="15.95" customHeight="1"/>
-    <row r="510" ht="15.95" customHeight="1"/>
-    <row r="511" ht="15.95" customHeight="1"/>
-    <row r="512" ht="15.95" customHeight="1"/>
-    <row r="513" ht="15.95" customHeight="1"/>
-    <row r="514" ht="15.95" customHeight="1"/>
-    <row r="515" ht="15.95" customHeight="1"/>
-    <row r="516" ht="15.95" customHeight="1"/>
-    <row r="517" ht="15.95" customHeight="1"/>
-    <row r="518" ht="15.95" customHeight="1"/>
-    <row r="519" ht="15.95" customHeight="1"/>
-    <row r="520" ht="15.95" customHeight="1"/>
-    <row r="521" ht="15.95" customHeight="1"/>
-    <row r="522" ht="15.95" customHeight="1"/>
-    <row r="523" ht="15.95" customHeight="1"/>
-    <row r="524" ht="15.95" customHeight="1"/>
-    <row r="525" ht="15.95" customHeight="1"/>
-    <row r="526" ht="15.95" customHeight="1"/>
-    <row r="527" ht="15.95" customHeight="1"/>
-    <row r="528" ht="15.95" customHeight="1"/>
-    <row r="529" ht="15.95" customHeight="1"/>
-    <row r="530" ht="15.95" customHeight="1"/>
-    <row r="531" ht="15.95" customHeight="1"/>
-    <row r="532" ht="15.95" customHeight="1"/>
-    <row r="533" ht="15.95" customHeight="1"/>
-    <row r="534" ht="15.95" customHeight="1"/>
-    <row r="535" ht="15.95" customHeight="1"/>
-    <row r="536" ht="15.95" customHeight="1"/>
-    <row r="537" ht="15.95" customHeight="1"/>
-    <row r="538" ht="15.95" customHeight="1"/>
-    <row r="539" ht="15.95" customHeight="1"/>
-    <row r="540" ht="15.95" customHeight="1"/>
-    <row r="541" ht="15.95" customHeight="1"/>
-    <row r="542" ht="15.95" customHeight="1"/>
-    <row r="543" ht="15.95" customHeight="1"/>
-    <row r="544" ht="15.95" customHeight="1"/>
-    <row r="545" ht="15.95" customHeight="1"/>
-    <row r="546" ht="15.95" customHeight="1"/>
-    <row r="547" ht="15.95" customHeight="1"/>
-    <row r="548" ht="15.95" customHeight="1"/>
-    <row r="549" ht="15.95" customHeight="1"/>
-    <row r="550" ht="15.95" customHeight="1"/>
-    <row r="551" ht="15.95" customHeight="1"/>
-    <row r="552" ht="15.95" customHeight="1"/>
-    <row r="553" ht="15.95" customHeight="1"/>
-    <row r="554" ht="15.95" customHeight="1"/>
-    <row r="555" ht="15.95" customHeight="1"/>
-    <row r="556" ht="15.95" customHeight="1"/>
-    <row r="557" ht="15.95" customHeight="1"/>
-    <row r="558" ht="15.95" customHeight="1"/>
-    <row r="559" ht="15.95" customHeight="1"/>
-    <row r="560" ht="15.95" customHeight="1"/>
-    <row r="561" ht="15.95" customHeight="1"/>
-    <row r="562" ht="15.95" customHeight="1"/>
-    <row r="563" ht="15.95" customHeight="1"/>
-    <row r="564" ht="15.95" customHeight="1"/>
-    <row r="565" ht="15.95" customHeight="1"/>
-    <row r="566" ht="15.95" customHeight="1"/>
-    <row r="567" ht="15.95" customHeight="1"/>
-    <row r="568" ht="15.95" customHeight="1"/>
-    <row r="569" ht="15.95" customHeight="1"/>
-    <row r="570" ht="15.95" customHeight="1"/>
-    <row r="571" ht="15.95" customHeight="1"/>
-    <row r="572" ht="15.95" customHeight="1"/>
-    <row r="573" ht="15.95" customHeight="1"/>
-    <row r="574" ht="15.95" customHeight="1"/>
-    <row r="575" ht="15.95" customHeight="1"/>
-    <row r="576" ht="15.95" customHeight="1"/>
-    <row r="577" ht="15.95" customHeight="1"/>
-    <row r="578" ht="15.95" customHeight="1"/>
-    <row r="579" ht="15.95" customHeight="1"/>
-    <row r="580" ht="15.95" customHeight="1"/>
-    <row r="581" ht="15.95" customHeight="1"/>
-    <row r="582" ht="15.95" customHeight="1"/>
-    <row r="583" ht="15.95" customHeight="1"/>
-    <row r="584" ht="15.95" customHeight="1"/>
-    <row r="585" ht="15.95" customHeight="1"/>
-    <row r="586" ht="15.95" customHeight="1"/>
-    <row r="587" ht="15.95" customHeight="1"/>
-    <row r="588" ht="15.95" customHeight="1"/>
-    <row r="589" ht="15.95" customHeight="1"/>
-    <row r="590" ht="15.95" customHeight="1"/>
-    <row r="591" ht="15.95" customHeight="1"/>
-    <row r="592" ht="15.95" customHeight="1"/>
-    <row r="593" ht="15.95" customHeight="1"/>
-    <row r="594" ht="15.95" customHeight="1"/>
-    <row r="595" ht="15.95" customHeight="1"/>
-    <row r="596" ht="15.95" customHeight="1"/>
-    <row r="597" ht="15.95" customHeight="1"/>
-    <row r="598" ht="15.95" customHeight="1"/>
-    <row r="599" ht="15.95" customHeight="1"/>
-    <row r="600" ht="15.95" customHeight="1"/>
-    <row r="601" ht="15.95" customHeight="1"/>
-    <row r="602" ht="15.95" customHeight="1"/>
-    <row r="603" ht="15.95" customHeight="1"/>
-    <row r="604" ht="15.95" customHeight="1"/>
-    <row r="605" ht="15.95" customHeight="1"/>
-    <row r="606" ht="15.95" customHeight="1"/>
-    <row r="607" ht="15.95" customHeight="1"/>
-    <row r="608" ht="15.95" customHeight="1"/>
-    <row r="609" ht="15.95" customHeight="1"/>
-    <row r="610" ht="15.95" customHeight="1"/>
-    <row r="611" ht="15.95" customHeight="1"/>
-    <row r="612" ht="15.95" customHeight="1"/>
-    <row r="613" ht="15.95" customHeight="1"/>
-    <row r="614" ht="15.95" customHeight="1"/>
-    <row r="615" ht="15.95" customHeight="1"/>
-    <row r="616" ht="15.95" customHeight="1"/>
-    <row r="617" ht="15.95" customHeight="1"/>
-    <row r="618" ht="15.95" customHeight="1"/>
-    <row r="619" ht="15.95" customHeight="1"/>
-    <row r="620" ht="15.95" customHeight="1"/>
-    <row r="621" ht="15.95" customHeight="1"/>
-    <row r="622" ht="15.95" customHeight="1"/>
-    <row r="623" ht="15.95" customHeight="1"/>
-    <row r="624" ht="15.95" customHeight="1"/>
-    <row r="625" ht="15.95" customHeight="1"/>
-    <row r="626" ht="15.95" customHeight="1"/>
-    <row r="627" ht="15.95" customHeight="1"/>
-    <row r="628" ht="15.95" customHeight="1"/>
-    <row r="629" ht="15.95" customHeight="1"/>
-    <row r="630" ht="15.95" customHeight="1"/>
-    <row r="631" ht="15.95" customHeight="1"/>
-    <row r="632" ht="15.95" customHeight="1"/>
-    <row r="633" ht="15.95" customHeight="1"/>
-    <row r="634" ht="15.95" customHeight="1"/>
-    <row r="635" ht="15.95" customHeight="1"/>
-    <row r="636" ht="15.95" customHeight="1"/>
-    <row r="637" ht="15.95" customHeight="1"/>
-    <row r="638" ht="15.95" customHeight="1"/>
-    <row r="639" ht="15.95" customHeight="1"/>
-    <row r="640" ht="15.95" customHeight="1"/>
-    <row r="641" ht="15.95" customHeight="1"/>
-    <row r="642" ht="15.95" customHeight="1"/>
-    <row r="643" ht="15.95" customHeight="1"/>
-    <row r="644" ht="15.95" customHeight="1"/>
-    <row r="645" ht="15.95" customHeight="1"/>
-    <row r="646" ht="15.95" customHeight="1"/>
-    <row r="647" ht="15.95" customHeight="1"/>
-    <row r="648" ht="15.95" customHeight="1"/>
-    <row r="649" ht="15.95" customHeight="1"/>
-    <row r="650" ht="15.95" customHeight="1"/>
-    <row r="651" ht="15.95" customHeight="1"/>
-    <row r="652" ht="15.95" customHeight="1"/>
-    <row r="653" ht="15.95" customHeight="1"/>
-    <row r="654" ht="15.95" customHeight="1"/>
-    <row r="655" ht="15.95" customHeight="1"/>
-    <row r="656" ht="15.95" customHeight="1"/>
-    <row r="657" ht="15.95" customHeight="1"/>
-    <row r="658" ht="15.95" customHeight="1"/>
-    <row r="659" ht="15.95" customHeight="1"/>
-    <row r="660" ht="15.95" customHeight="1"/>
-    <row r="661" ht="15.95" customHeight="1"/>
-    <row r="662" ht="15.95" customHeight="1"/>
-    <row r="663" ht="15.95" customHeight="1"/>
-    <row r="664" ht="15.95" customHeight="1"/>
-    <row r="665" ht="15.95" customHeight="1"/>
-    <row r="666" ht="15.95" customHeight="1"/>
-    <row r="667" ht="15.95" customHeight="1"/>
-    <row r="668" ht="15.95" customHeight="1"/>
-    <row r="669" ht="15.95" customHeight="1"/>
-    <row r="670" ht="15.95" customHeight="1"/>
-    <row r="671" ht="15.95" customHeight="1"/>
-    <row r="672" ht="15.95" customHeight="1"/>
-    <row r="673" ht="15.95" customHeight="1"/>
-    <row r="674" ht="15.95" customHeight="1"/>
-    <row r="675" ht="15.95" customHeight="1"/>
-    <row r="676" ht="15.95" customHeight="1"/>
-    <row r="677" ht="15.95" customHeight="1"/>
-    <row r="678" ht="15.95" customHeight="1"/>
-    <row r="679" ht="15.95" customHeight="1"/>
-    <row r="680" ht="15.95" customHeight="1"/>
-    <row r="681" ht="15.95" customHeight="1"/>
-    <row r="682" ht="15.95" customHeight="1"/>
-    <row r="683" ht="15.95" customHeight="1"/>
-    <row r="684" ht="15.95" customHeight="1"/>
-    <row r="685" ht="15.95" customHeight="1"/>
-    <row r="686" ht="15.95" customHeight="1"/>
-    <row r="687" ht="15.95" customHeight="1"/>
-    <row r="688" ht="15.95" customHeight="1"/>
-    <row r="689" ht="15.95" customHeight="1"/>
-    <row r="690" ht="15.95" customHeight="1"/>
-    <row r="691" ht="15.95" customHeight="1"/>
-    <row r="692" ht="15.95" customHeight="1"/>
-    <row r="693" ht="15.95" customHeight="1"/>
-    <row r="694" ht="15.95" customHeight="1"/>
-    <row r="695" ht="15.95" customHeight="1"/>
-    <row r="696" ht="15.95" customHeight="1"/>
-    <row r="697" ht="15.95" customHeight="1"/>
-    <row r="698" ht="15.95" customHeight="1"/>
-    <row r="699" ht="15.95" customHeight="1"/>
-    <row r="700" ht="15.95" customHeight="1"/>
-    <row r="701" ht="15.95" customHeight="1"/>
-    <row r="702" ht="15.95" customHeight="1"/>
-    <row r="703" ht="15.95" customHeight="1"/>
-    <row r="704" ht="15.95" customHeight="1"/>
-    <row r="705" ht="15.95" customHeight="1"/>
-    <row r="706" ht="15.95" customHeight="1"/>
-    <row r="707" ht="15.95" customHeight="1"/>
-    <row r="708" ht="15.95" customHeight="1"/>
-    <row r="709" ht="15.95" customHeight="1"/>
-    <row r="710" ht="15.95" customHeight="1"/>
-    <row r="711" ht="15.95" customHeight="1"/>
-    <row r="712" ht="15.95" customHeight="1"/>
-    <row r="713" ht="15.95" customHeight="1"/>
-    <row r="714" ht="15.95" customHeight="1"/>
-    <row r="715" ht="15.95" customHeight="1"/>
-    <row r="716" ht="15.95" customHeight="1"/>
-    <row r="717" ht="15.95" customHeight="1"/>
-    <row r="718" ht="15.95" customHeight="1"/>
-    <row r="719" ht="15.95" customHeight="1"/>
-    <row r="720" ht="15.95" customHeight="1"/>
-    <row r="721" ht="15.95" customHeight="1"/>
-    <row r="722" ht="15.95" customHeight="1"/>
-    <row r="723" ht="15.95" customHeight="1"/>
-    <row r="724" ht="15.95" customHeight="1"/>
-    <row r="725" ht="15.95" customHeight="1"/>
-    <row r="726" ht="15.95" customHeight="1"/>
-    <row r="727" ht="15.95" customHeight="1"/>
-    <row r="728" ht="15.95" customHeight="1"/>
-    <row r="729" ht="15.95" customHeight="1"/>
-    <row r="730" ht="15.95" customHeight="1"/>
-    <row r="731" ht="15.95" customHeight="1"/>
-    <row r="732" ht="15.95" customHeight="1"/>
-    <row r="733" ht="15.95" customHeight="1"/>
-    <row r="734" ht="15.95" customHeight="1"/>
-    <row r="735" ht="15.95" customHeight="1"/>
-    <row r="736" ht="15.95" customHeight="1"/>
-    <row r="737" ht="15.95" customHeight="1"/>
-    <row r="738" ht="15.95" customHeight="1"/>
-    <row r="739" ht="15.95" customHeight="1"/>
-    <row r="740" ht="15.95" customHeight="1"/>
-    <row r="741" ht="15.95" customHeight="1"/>
-    <row r="742" ht="15.95" customHeight="1"/>
-    <row r="743" ht="15.95" customHeight="1"/>
-    <row r="744" ht="15.95" customHeight="1"/>
-    <row r="745" ht="15.95" customHeight="1"/>
-    <row r="746" ht="15.95" customHeight="1"/>
-    <row r="747" ht="15.95" customHeight="1"/>
-    <row r="748" ht="15.95" customHeight="1"/>
-    <row r="749" ht="15.95" customHeight="1"/>
-    <row r="750" ht="15.95" customHeight="1"/>
-    <row r="751" ht="15.95" customHeight="1"/>
-    <row r="752" ht="15.95" customHeight="1"/>
-    <row r="753" ht="15.95" customHeight="1"/>
-    <row r="754" ht="15.95" customHeight="1"/>
-    <row r="755" ht="15.95" customHeight="1"/>
-    <row r="756" ht="15.95" customHeight="1"/>
-    <row r="757" ht="15.95" customHeight="1"/>
-    <row r="758" ht="15.95" customHeight="1"/>
-    <row r="759" ht="15.95" customHeight="1"/>
-    <row r="760" ht="15.95" customHeight="1"/>
-    <row r="761" ht="15.95" customHeight="1"/>
-    <row r="762" ht="15.95" customHeight="1"/>
-    <row r="763" ht="15.95" customHeight="1"/>
-    <row r="764" ht="15.95" customHeight="1"/>
-    <row r="765" ht="15.95" customHeight="1"/>
-    <row r="766" ht="15.95" customHeight="1"/>
-    <row r="767" ht="15.95" customHeight="1"/>
-    <row r="768" ht="15.95" customHeight="1"/>
-    <row r="769" ht="15.95" customHeight="1"/>
-    <row r="770" ht="15.95" customHeight="1"/>
-    <row r="771" ht="15.95" customHeight="1"/>
-    <row r="772" ht="15.95" customHeight="1"/>
-    <row r="773" ht="15.95" customHeight="1"/>
-    <row r="774" ht="15.95" customHeight="1"/>
-    <row r="775" ht="15.95" customHeight="1"/>
-    <row r="776" ht="15.95" customHeight="1"/>
-    <row r="777" ht="15.95" customHeight="1"/>
-    <row r="778" ht="15.95" customHeight="1"/>
-    <row r="779" ht="15.95" customHeight="1"/>
-    <row r="780" ht="15.95" customHeight="1"/>
-    <row r="781" ht="15.95" customHeight="1"/>
-    <row r="782" ht="15.95" customHeight="1"/>
-    <row r="783" ht="15.95" customHeight="1"/>
-    <row r="784" ht="15.95" customHeight="1"/>
-    <row r="785" ht="15.95" customHeight="1"/>
-    <row r="786" ht="15.95" customHeight="1"/>
-    <row r="787" ht="15.95" customHeight="1"/>
-    <row r="788" ht="15.95" customHeight="1"/>
-    <row r="789" ht="15.95" customHeight="1"/>
-    <row r="790" ht="15.95" customHeight="1"/>
-    <row r="791" ht="15.95" customHeight="1"/>
-    <row r="792" ht="15.95" customHeight="1"/>
-    <row r="793" ht="15.95" customHeight="1"/>
-    <row r="794" ht="15.95" customHeight="1"/>
-    <row r="795" ht="15.95" customHeight="1"/>
-    <row r="796" ht="15.95" customHeight="1"/>
-    <row r="797" ht="15.95" customHeight="1"/>
-    <row r="798" ht="15.95" customHeight="1"/>
-    <row r="799" ht="15.95" customHeight="1"/>
-    <row r="800" ht="15.95" customHeight="1"/>
-    <row r="801" ht="15.95" customHeight="1"/>
-    <row r="802" ht="15.95" customHeight="1"/>
-    <row r="803" ht="15.95" customHeight="1"/>
-    <row r="804" ht="15.95" customHeight="1"/>
-    <row r="805" ht="15.95" customHeight="1"/>
-    <row r="806" ht="15.95" customHeight="1"/>
-    <row r="807" ht="15.95" customHeight="1"/>
-    <row r="808" ht="15.95" customHeight="1"/>
-    <row r="809" ht="15.95" customHeight="1"/>
-    <row r="810" ht="15.95" customHeight="1"/>
-    <row r="811" ht="15.95" customHeight="1"/>
-    <row r="812" ht="15.95" customHeight="1"/>
-    <row r="813" ht="15.95" customHeight="1"/>
-    <row r="814" ht="15.95" customHeight="1"/>
-    <row r="815" ht="15.95" customHeight="1"/>
-    <row r="816" ht="15.95" customHeight="1"/>
-    <row r="817" ht="15.95" customHeight="1"/>
-    <row r="818" ht="15.95" customHeight="1"/>
-    <row r="819" ht="15.95" customHeight="1"/>
-    <row r="820" ht="15.95" customHeight="1"/>
-    <row r="821" ht="15.95" customHeight="1"/>
-    <row r="822" ht="15.95" customHeight="1"/>
-    <row r="823" ht="15.95" customHeight="1"/>
-    <row r="824" ht="15.95" customHeight="1"/>
-    <row r="825" ht="15.95" customHeight="1"/>
-    <row r="826" ht="15.95" customHeight="1"/>
-    <row r="827" ht="15.95" customHeight="1"/>
-    <row r="828" ht="15.95" customHeight="1"/>
-    <row r="829" ht="15.95" customHeight="1"/>
-    <row r="830" ht="15.95" customHeight="1"/>
-    <row r="831" ht="15.95" customHeight="1"/>
-    <row r="832" ht="15.95" customHeight="1"/>
-    <row r="833" ht="15.95" customHeight="1"/>
-    <row r="834" ht="15.95" customHeight="1"/>
-    <row r="835" ht="15.95" customHeight="1"/>
-    <row r="836" ht="15.95" customHeight="1"/>
-    <row r="837" ht="15.95" customHeight="1"/>
-    <row r="838" ht="15.95" customHeight="1"/>
-    <row r="839" ht="15.95" customHeight="1"/>
-    <row r="840" ht="15.95" customHeight="1"/>
-    <row r="841" ht="15.95" customHeight="1"/>
-    <row r="842" ht="15.95" customHeight="1"/>
-    <row r="843" ht="15.95" customHeight="1"/>
-    <row r="844" ht="15.95" customHeight="1"/>
-    <row r="845" ht="15.95" customHeight="1"/>
-    <row r="846" ht="15.95" customHeight="1"/>
-    <row r="847" ht="15.95" customHeight="1"/>
-    <row r="848" ht="15.95" customHeight="1"/>
-    <row r="849" ht="15.95" customHeight="1"/>
-    <row r="850" ht="15.95" customHeight="1"/>
-    <row r="851" ht="15.95" customHeight="1"/>
-    <row r="852" ht="15.95" customHeight="1"/>
-    <row r="853" ht="15.95" customHeight="1"/>
-    <row r="854" ht="15.95" customHeight="1"/>
-    <row r="855" ht="15.95" customHeight="1"/>
-    <row r="856" ht="15.95" customHeight="1"/>
-    <row r="857" ht="15.95" customHeight="1"/>
-    <row r="858" ht="15.95" customHeight="1"/>
-    <row r="859" ht="15.95" customHeight="1"/>
-    <row r="860" ht="15.95" customHeight="1"/>
-    <row r="861" ht="15.95" customHeight="1"/>
-    <row r="862" ht="15.95" customHeight="1"/>
-    <row r="863" ht="15.95" customHeight="1"/>
-    <row r="864" ht="15.95" customHeight="1"/>
-    <row r="865" ht="15.95" customHeight="1"/>
-    <row r="866" ht="15.95" customHeight="1"/>
-    <row r="867" ht="15.95" customHeight="1"/>
-    <row r="868" ht="15.95" customHeight="1"/>
-    <row r="869" ht="15.95" customHeight="1"/>
-    <row r="870" ht="15.95" customHeight="1"/>
-    <row r="871" ht="15.95" customHeight="1"/>
-    <row r="872" ht="15.95" customHeight="1"/>
-    <row r="873" ht="15.95" customHeight="1"/>
-    <row r="874" ht="15.95" customHeight="1"/>
-    <row r="875" ht="15.95" customHeight="1"/>
-    <row r="876" ht="15.95" customHeight="1"/>
-    <row r="877" ht="15.95" customHeight="1"/>
-    <row r="878" ht="15.95" customHeight="1"/>
-    <row r="879" ht="15.95" customHeight="1"/>
-    <row r="880" ht="15.95" customHeight="1"/>
-    <row r="881" ht="15.95" customHeight="1"/>
-    <row r="882" ht="15.95" customHeight="1"/>
-    <row r="883" ht="15.95" customHeight="1"/>
-    <row r="884" ht="15.95" customHeight="1"/>
-    <row r="885" ht="15.95" customHeight="1"/>
-    <row r="886" ht="15.95" customHeight="1"/>
-    <row r="887" ht="15.95" customHeight="1"/>
-    <row r="888" ht="15.95" customHeight="1"/>
-    <row r="889" ht="15.95" customHeight="1"/>
-    <row r="890" ht="15.95" customHeight="1"/>
-    <row r="891" ht="15.95" customHeight="1"/>
-    <row r="892" ht="15.95" customHeight="1"/>
-    <row r="893" ht="15.95" customHeight="1"/>
-    <row r="894" ht="15.95" customHeight="1"/>
-    <row r="895" ht="15.95" customHeight="1"/>
-    <row r="896" ht="15.95" customHeight="1"/>
-    <row r="897" ht="15.95" customHeight="1"/>
-    <row r="898" ht="15.95" customHeight="1"/>
-    <row r="899" ht="15.95" customHeight="1"/>
-    <row r="900" ht="15.95" customHeight="1"/>
-    <row r="901" ht="15.95" customHeight="1"/>
-    <row r="902" ht="15.95" customHeight="1"/>
-    <row r="903" ht="15.95" customHeight="1"/>
-    <row r="904" ht="15.95" customHeight="1"/>
-    <row r="905" ht="15.95" customHeight="1"/>
-    <row r="906" ht="15.95" customHeight="1"/>
-    <row r="907" ht="15.95" customHeight="1"/>
-    <row r="908" ht="15.95" customHeight="1"/>
-    <row r="909" ht="15.95" customHeight="1"/>
-    <row r="910" ht="15.95" customHeight="1"/>
-    <row r="911" ht="15.95" customHeight="1"/>
-    <row r="912" ht="15.95" customHeight="1"/>
-    <row r="913" ht="15.95" customHeight="1"/>
-    <row r="914" ht="15.95" customHeight="1"/>
-    <row r="915" ht="15.95" customHeight="1"/>
-    <row r="916" ht="15.95" customHeight="1"/>
-    <row r="917" ht="15.95" customHeight="1"/>
-    <row r="918" ht="15.95" customHeight="1"/>
-    <row r="919" ht="15.95" customHeight="1"/>
-    <row r="920" ht="15.95" customHeight="1"/>
-    <row r="921" ht="15.95" customHeight="1"/>
-    <row r="922" ht="15.95" customHeight="1"/>
-    <row r="923" ht="15.95" customHeight="1"/>
-    <row r="924" ht="15.95" customHeight="1"/>
-    <row r="925" ht="15.95" customHeight="1"/>
-    <row r="926" ht="15.95" customHeight="1"/>
-    <row r="927" ht="15.95" customHeight="1"/>
-    <row r="928" ht="15.95" customHeight="1"/>
-    <row r="929" ht="15.95" customHeight="1"/>
-    <row r="930" ht="15.95" customHeight="1"/>
-    <row r="931" ht="15.95" customHeight="1"/>
-    <row r="932" ht="15.95" customHeight="1"/>
-    <row r="933" ht="15.95" customHeight="1"/>
-    <row r="934" ht="15.95" customHeight="1"/>
-    <row r="935" ht="15.95" customHeight="1"/>
-    <row r="936" ht="15.95" customHeight="1"/>
-    <row r="937" ht="15.95" customHeight="1"/>
-    <row r="938" ht="15.95" customHeight="1"/>
-    <row r="939" ht="15.95" customHeight="1"/>
-    <row r="940" ht="15.95" customHeight="1"/>
-    <row r="941" ht="15.95" customHeight="1"/>
-    <row r="942" ht="15.95" customHeight="1"/>
-    <row r="943" ht="15.95" customHeight="1"/>
-    <row r="944" ht="15.95" customHeight="1"/>
-    <row r="945" ht="15.95" customHeight="1"/>
-    <row r="946" ht="15.95" customHeight="1"/>
-    <row r="947" ht="15.95" customHeight="1"/>
-    <row r="948" ht="15.95" customHeight="1"/>
-    <row r="949" ht="15.95" customHeight="1"/>
-    <row r="950" ht="15.95" customHeight="1"/>
-    <row r="951" ht="15.95" customHeight="1"/>
-    <row r="952" ht="15.95" customHeight="1"/>
-    <row r="953" ht="15.95" customHeight="1"/>
-    <row r="954" ht="15.95" customHeight="1"/>
-    <row r="955" ht="15.95" customHeight="1"/>
-    <row r="956" ht="15.95" customHeight="1"/>
-    <row r="957" ht="15.95" customHeight="1"/>
-    <row r="958" ht="15.95" customHeight="1"/>
-    <row r="959" ht="15.95" customHeight="1"/>
-    <row r="960" ht="15.95" customHeight="1"/>
-    <row r="961" ht="15.95" customHeight="1"/>
-    <row r="962" ht="15.95" customHeight="1"/>
-    <row r="963" ht="15.95" customHeight="1"/>
-    <row r="964" ht="15.95" customHeight="1"/>
-    <row r="965" ht="15.95" customHeight="1"/>
-    <row r="966" ht="15.95" customHeight="1"/>
-    <row r="967" ht="15.95" customHeight="1"/>
-    <row r="968" ht="15.95" customHeight="1"/>
-    <row r="969" ht="15.95" customHeight="1"/>
-    <row r="970" ht="15.95" customHeight="1"/>
-    <row r="971" ht="15.95" customHeight="1"/>
-    <row r="972" ht="15.95" customHeight="1"/>
-    <row r="973" ht="15.95" customHeight="1"/>
-    <row r="974" ht="15.95" customHeight="1"/>
-    <row r="975" ht="15.95" customHeight="1"/>
-    <row r="976" ht="15.95" customHeight="1"/>
-    <row r="977" ht="15.95" customHeight="1"/>
-    <row r="978" ht="15.95" customHeight="1"/>
-    <row r="979" ht="15.95" customHeight="1"/>
-    <row r="980" ht="15.95" customHeight="1"/>
-    <row r="981" ht="15.95" customHeight="1"/>
-    <row r="982" ht="15.95" customHeight="1"/>
-    <row r="983" ht="15.95" customHeight="1"/>
-    <row r="984" ht="15.95" customHeight="1"/>
-    <row r="985" ht="15.95" customHeight="1"/>
-    <row r="986" ht="15.95" customHeight="1"/>
-    <row r="987" ht="15.95" customHeight="1"/>
-    <row r="988" ht="15.95" customHeight="1"/>
-    <row r="989" ht="15.95" customHeight="1"/>
-    <row r="990" ht="15.95" customHeight="1"/>
-    <row r="991" ht="15.95" customHeight="1"/>
-    <row r="992" ht="15.95" customHeight="1"/>
-    <row r="993" ht="15.95" customHeight="1"/>
-    <row r="994" ht="15.95" customHeight="1"/>
-    <row r="995" ht="15.95" customHeight="1"/>
-    <row r="996" ht="15.95" customHeight="1"/>
-    <row r="997" ht="15.95" customHeight="1"/>
-    <row r="998" ht="15.95" customHeight="1"/>
-    <row r="999" ht="15.95" customHeight="1"/>
-    <row r="1000" ht="15.95" customHeight="1"/>
-    <row r="1001" ht="15.95" customHeight="1"/>
-    <row r="1002" ht="15.95" customHeight="1"/>
-    <row r="1003" ht="15.95" customHeight="1"/>
-    <row r="1004" ht="15.95" customHeight="1"/>
-    <row r="1005" ht="15.95" customHeight="1"/>
-    <row r="1006" ht="15.95" customHeight="1"/>
-    <row r="1007" ht="15.95" customHeight="1"/>
-    <row r="1008" ht="15.95" customHeight="1"/>
-    <row r="1009" ht="15.95" customHeight="1"/>
-    <row r="1010" ht="15.95" customHeight="1"/>
-    <row r="1011" ht="15.95" customHeight="1"/>
-    <row r="1012" ht="15.95" customHeight="1"/>
-    <row r="1013" ht="15.95" customHeight="1"/>
-    <row r="1014" ht="15.95" customHeight="1"/>
-    <row r="1015" ht="15.95" customHeight="1"/>
-    <row r="1016" ht="15.95" customHeight="1"/>
-    <row r="1017" ht="15.95" customHeight="1"/>
-    <row r="1018" ht="15.95" customHeight="1"/>
-    <row r="1019" ht="15.95" customHeight="1"/>
-    <row r="1020" ht="15.95" customHeight="1"/>
-    <row r="1021" ht="15.95" customHeight="1"/>
-    <row r="1022" ht="15.95" customHeight="1"/>
-    <row r="1023" ht="15.95" customHeight="1"/>
-    <row r="1024" ht="15.95" customHeight="1"/>
-    <row r="1025" ht="15.95" customHeight="1"/>
-    <row r="1026" ht="15.95" customHeight="1"/>
-    <row r="1027" ht="15.95" customHeight="1"/>
-    <row r="1028" ht="15.95" customHeight="1"/>
-    <row r="1029" ht="15.95" customHeight="1"/>
-    <row r="1030" ht="15.95" customHeight="1"/>
-    <row r="1031" ht="15.95" customHeight="1"/>
-    <row r="1032" ht="15.95" customHeight="1"/>
-    <row r="1033" ht="15.95" customHeight="1"/>
-    <row r="1034" ht="15.95" customHeight="1"/>
-    <row r="1035" ht="15.95" customHeight="1"/>
-    <row r="1036" ht="15.95" customHeight="1"/>
-    <row r="1037" ht="15.95" customHeight="1"/>
-    <row r="1038" ht="15.95" customHeight="1"/>
-    <row r="1039" ht="15.95" customHeight="1"/>
-    <row r="1040" ht="15.95" customHeight="1"/>
-    <row r="1041" ht="15.95" customHeight="1"/>
+    <row r="174" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="175" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="176" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="177" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="178" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="179" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="180" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="181" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="182" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="183" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="184" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="185" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="186" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="187" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="188" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="189" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="190" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="191" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="192" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="193" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="194" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="195" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="196" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="197" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="198" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="199" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="200" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="201" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="202" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="203" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="204" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="205" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="206" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="207" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="208" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="209" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="210" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="211" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="212" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="213" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="214" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="215" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="216" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="217" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="218" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="219" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="220" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="221" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="222" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="223" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="224" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="225" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="226" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="227" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="228" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="229" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="230" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="231" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="232" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="233" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="234" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="235" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="236" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="237" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="238" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="239" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="240" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="241" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="242" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="243" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="244" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="245" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="246" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="247" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="248" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="249" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="250" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="251" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="252" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="253" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="254" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="255" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="256" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="257" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="258" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="259" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="260" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="261" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="262" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="263" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="264" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="265" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="266" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="267" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="268" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="269" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="270" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="271" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="272" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="273" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="274" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="275" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="276" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="277" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="278" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="279" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="280" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="281" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="282" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="283" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="284" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="285" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="286" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="287" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="288" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="289" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="290" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="291" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="292" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="293" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="294" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="295" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="296" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="297" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="298" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="299" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="300" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="301" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="302" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="303" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="304" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="305" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="306" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="307" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="308" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="309" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="310" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="311" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="312" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="313" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="314" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="315" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="316" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="317" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="318" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="319" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="320" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="321" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="322" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="323" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="324" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="325" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="326" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="327" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="328" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="329" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="330" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="331" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="332" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="333" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="334" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="335" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="336" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="337" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="338" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="339" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="340" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="341" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="342" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="343" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="344" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="345" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="346" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="347" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="348" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="349" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="350" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="351" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="352" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="353" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="354" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="355" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="356" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="357" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="358" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="359" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="360" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="361" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="362" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="363" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="364" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="365" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="366" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="367" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="368" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="369" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="370" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="371" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="372" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="373" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="374" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="375" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="376" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="377" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="378" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="379" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="380" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="381" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="382" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="383" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="384" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="385" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="386" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="387" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="388" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="389" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="390" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="391" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="392" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="393" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="394" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="395" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="396" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="397" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="398" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="399" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="400" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="401" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="402" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="403" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="404" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="405" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="406" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="407" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="408" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="409" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="410" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="411" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="412" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="413" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="414" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="415" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="416" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="417" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="418" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="419" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="420" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="421" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="422" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="423" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="424" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="425" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="426" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="427" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="428" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="429" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="430" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="431" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="432" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="433" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="434" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="435" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="436" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="437" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="438" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="439" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="440" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="441" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="442" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="443" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="444" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="445" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="446" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="447" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="448" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="449" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="450" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="451" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="452" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="453" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="454" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="455" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="456" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="457" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="458" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="459" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="460" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="461" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="462" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="463" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="464" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="465" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="466" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="467" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="468" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="469" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="470" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="471" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="472" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="473" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="474" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="475" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="476" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="477" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="478" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="479" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="480" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="481" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="482" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="483" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="484" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="485" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="486" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="487" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="488" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="489" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="490" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="491" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="492" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="493" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="494" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="495" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="496" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="497" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="498" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="499" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="500" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="501" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="502" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="503" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="504" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="505" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="506" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="507" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="508" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="509" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="510" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="511" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="512" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="513" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="514" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="515" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="516" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="517" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="518" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="519" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="520" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="521" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="522" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="523" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="524" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="525" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="526" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="527" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="528" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="529" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="530" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="531" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="532" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="533" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="534" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="535" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="536" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="537" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="538" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="539" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="540" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="541" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="542" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="543" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="544" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="545" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="546" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="547" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="548" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="549" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="550" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="551" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="552" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="553" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="554" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="555" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="556" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="557" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="558" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="559" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="560" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="561" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="562" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="563" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="564" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="565" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="566" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="567" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="568" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="569" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="570" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="571" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="572" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="573" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="574" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="575" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="576" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="577" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="578" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="579" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="580" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="581" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="582" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="583" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="584" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="585" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="586" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="587" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="588" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="589" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="590" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="591" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="592" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="593" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="594" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="595" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="596" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="597" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="598" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="599" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="600" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="601" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="602" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="603" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="604" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="605" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="606" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="607" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="608" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="609" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="610" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="611" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="612" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="613" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="614" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="615" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="616" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="617" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="618" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="619" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="620" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="621" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="622" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="623" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="624" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="625" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="626" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="627" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="628" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="629" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="630" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="631" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="632" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="633" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="634" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="635" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="636" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="637" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="638" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="639" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="640" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="641" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="642" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="643" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="644" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="645" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="646" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="647" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="648" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="649" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="650" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="651" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="652" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="653" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="654" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="655" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="656" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="657" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="658" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="659" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="660" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="661" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="662" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="663" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="664" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="665" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="666" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="667" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="668" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="669" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="670" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="671" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="672" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="673" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="674" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="675" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="676" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="677" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="678" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="679" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="680" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="681" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="682" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="683" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="684" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="685" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="686" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="687" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="688" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="689" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="690" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="691" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="692" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="693" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="694" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="695" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="696" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="697" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="698" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="699" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="700" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="701" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="702" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="703" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="704" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="705" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="706" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="707" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="708" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="709" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="710" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="711" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="712" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="713" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="714" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="715" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="716" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="717" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="718" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="719" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="720" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="721" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="722" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="723" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="724" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="725" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="726" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="727" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="728" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="729" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="730" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="731" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="732" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="733" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="734" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="735" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="736" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="737" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="738" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="739" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="740" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="741" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="742" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="743" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="744" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="745" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="746" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="747" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="748" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="749" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="750" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="751" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="752" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="753" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="754" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="755" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="756" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="757" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="758" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="759" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="760" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="761" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="762" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="763" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="764" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="765" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="766" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="767" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="768" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="769" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="770" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="771" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="772" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="773" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="774" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="775" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="776" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="777" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="778" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="779" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="780" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="781" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="782" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="783" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="784" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="785" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="786" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="787" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="788" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="789" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="790" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="791" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="792" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="793" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="794" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="795" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="796" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="797" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="798" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="799" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="800" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="801" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="802" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="803" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="804" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="805" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="806" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="807" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="808" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="809" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="810" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="811" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="812" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="813" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="814" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="815" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="816" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="817" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="818" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="819" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="820" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="821" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="822" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="823" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="824" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="825" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="826" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="827" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="828" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="829" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="830" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="831" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="832" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="833" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="834" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="835" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="836" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="837" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="838" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="839" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="840" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="841" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="842" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="843" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="844" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="845" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="846" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="847" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="848" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="849" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="850" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="851" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="852" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="853" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="854" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="855" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="856" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="857" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="858" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="859" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="860" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="861" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="862" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="863" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="864" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="865" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="866" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="867" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="868" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="869" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="870" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="871" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="872" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="873" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="874" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="875" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="876" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="877" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="878" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="879" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="880" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="881" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="882" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="883" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="884" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="885" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="886" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="887" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="888" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="889" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="890" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="891" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="892" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="893" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="894" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="895" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="896" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="897" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="898" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="899" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="900" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="901" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="902" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="903" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="904" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="905" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="906" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="907" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="908" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="909" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="910" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="911" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="912" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="913" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="914" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="915" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="916" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="917" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="918" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="919" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="920" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="921" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="922" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="923" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="924" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="925" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="926" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="927" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="928" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="929" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="930" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="931" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="932" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="933" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="934" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="935" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="936" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="937" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="938" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="939" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="940" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="941" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="942" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="943" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="944" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="945" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="946" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="947" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="948" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="949" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="950" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="951" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="952" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="953" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="954" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="955" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="956" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="957" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="958" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="959" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="960" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="961" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="962" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="963" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="964" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="965" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="966" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="967" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="968" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="969" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="970" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="971" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="972" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="973" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="974" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="975" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="976" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="977" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="978" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="979" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="980" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="981" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="982" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="983" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="984" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="985" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="986" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="987" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="988" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="989" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="990" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="991" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="992" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="993" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="994" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="995" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="996" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="997" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="998" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="999" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="1000" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="1001" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="1002" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="1003" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="1004" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="1005" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="1006" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="1007" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="1008" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="1009" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="1010" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="1011" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="1012" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="1013" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="1014" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="1015" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="1016" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="1017" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="1018" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="1019" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="1020" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="1021" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="1022" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="1023" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="1024" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="1025" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="1026" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="1027" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="1028" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="1029" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="1030" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="1031" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="1032" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="1033" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="1034" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="1035" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="1036" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="1037" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="1038" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="1039" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="1040" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="1041" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:A4"/>
@@ -20308,29 +20385,29 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView zoomScale="98" zoomScaleNormal="98" zoomScalePageLayoutView="60" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="256" width="26.42578125" customWidth="1"/>
-    <col min="257" max="1023" width="16.140625" customWidth="1"/>
-    <col min="1024" max="1025" width="11.7109375" customWidth="1"/>
+    <col min="1" max="256" width="26.453125" customWidth="1"/>
+    <col min="257" max="1023" width="16.1796875" customWidth="1"/>
+    <col min="1024" max="1025" width="11.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="50" t="s">
+    <row r="1" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A1" s="54" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="26" t="s">
         <v>162</v>
       </c>
@@ -20344,7 +20421,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" ht="13" x14ac:dyDescent="0.3">
       <c r="A3" s="27" t="s">
         <v>163</v>
       </c>
@@ -20372,28 +20449,28 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView zoomScalePageLayoutView="60" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="256" width="24.42578125" customWidth="1"/>
-    <col min="257" max="1023" width="16.140625" customWidth="1"/>
-    <col min="1024" max="1025" width="11.7109375" customWidth="1"/>
+    <col min="1" max="256" width="24.453125" customWidth="1"/>
+    <col min="257" max="1023" width="16.1796875" customWidth="1"/>
+    <col min="1024" max="1025" width="11.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="51" t="s">
+    <row r="1" spans="1:3" ht="13" x14ac:dyDescent="0.3">
+      <c r="A1" s="55" t="s">
         <v>79</v>
       </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="51"/>
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="26" t="s">
         <v>80</v>
       </c>
@@ -20404,7 +20481,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" ht="13" x14ac:dyDescent="0.3">
       <c r="A3" s="27" t="s">
         <v>82</v>
       </c>
@@ -20415,7 +20492,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="28"/>
       <c r="B4" s="29"/>
       <c r="C4" s="29"/>
@@ -20434,28 +20511,28 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView zoomScalePageLayoutView="60" workbookViewId="0">
       <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="256" width="22.42578125" customWidth="1"/>
-    <col min="257" max="1023" width="16.140625" customWidth="1"/>
-    <col min="1024" max="1025" width="11.7109375" customWidth="1"/>
+    <col min="1" max="256" width="22.453125" customWidth="1"/>
+    <col min="257" max="1023" width="16.1796875" customWidth="1"/>
+    <col min="1024" max="1025" width="11.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="52" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="56" t="s">
         <v>85</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="26" t="s">
         <v>86</v>
       </c>
@@ -20466,7 +20543,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" ht="13" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
         <v>88</v>
       </c>
@@ -20477,7 +20554,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" ht="13" x14ac:dyDescent="0.3">
       <c r="A4" s="12"/>
       <c r="B4" s="31"/>
       <c r="C4" s="31"/>
@@ -20496,28 +20573,28 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView topLeftCell="A13" zoomScalePageLayoutView="60" workbookViewId="0">
       <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="256" width="22.42578125" customWidth="1"/>
-    <col min="257" max="1023" width="16.140625" customWidth="1"/>
-    <col min="1024" max="1025" width="11.7109375" customWidth="1"/>
+    <col min="1" max="256" width="22.453125" customWidth="1"/>
+    <col min="257" max="1023" width="16.1796875" customWidth="1"/>
+    <col min="1024" max="1025" width="11.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="52" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="56" t="s">
         <v>91</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="26" t="s">
         <v>86</v>
       </c>
@@ -20528,7 +20605,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" ht="13" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
         <v>93</v>
       </c>
@@ -20539,7 +20616,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="28"/>
       <c r="B4" s="31"/>
       <c r="C4" s="31"/>
@@ -20558,28 +20635,28 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView zoomScalePageLayoutView="60" workbookViewId="0">
       <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="256" width="22.42578125" customWidth="1"/>
-    <col min="257" max="1023" width="16.140625" customWidth="1"/>
-    <col min="1024" max="1025" width="11.7109375" customWidth="1"/>
+    <col min="1" max="256" width="22.453125" customWidth="1"/>
+    <col min="257" max="1023" width="16.1796875" customWidth="1"/>
+    <col min="1024" max="1025" width="11.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="52" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="56" t="s">
         <v>96</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>86</v>
       </c>
@@ -20590,7 +20667,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" ht="13" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
         <v>98</v>
       </c>
@@ -20601,7 +20678,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="32"/>
       <c r="B4" s="9"/>
       <c r="C4" s="9"/>
@@ -20620,28 +20697,28 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView zoomScalePageLayoutView="60" workbookViewId="0">
       <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="256" width="22.42578125" customWidth="1"/>
-    <col min="257" max="1023" width="16.140625" customWidth="1"/>
-    <col min="1024" max="1025" width="11.7109375" customWidth="1"/>
+    <col min="1" max="256" width="22.453125" customWidth="1"/>
+    <col min="257" max="1023" width="16.1796875" customWidth="1"/>
+    <col min="1024" max="1025" width="11.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="52" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="56" t="s">
         <v>101</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>86</v>
       </c>
@@ -20652,7 +20729,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" ht="13" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
         <v>103</v>
       </c>
@@ -20663,7 +20740,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="32"/>
       <c r="B4" s="9"/>
       <c r="C4" s="9"/>
@@ -20682,34 +20759,34 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T94"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <dimension ref="A1:T125"/>
   <sheetViews>
-    <sheetView zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="C93" sqref="C93:D93"/>
+    <sheetView tabSelected="1" topLeftCell="A90" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="C110" sqref="C110"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" customWidth="1"/>
-    <col min="2" max="2" width="31.5703125" customWidth="1"/>
-    <col min="3" max="1023" width="12.42578125" customWidth="1"/>
+    <col min="1" max="1" width="18.81640625" customWidth="1"/>
+    <col min="2" max="2" width="31.54296875" customWidth="1"/>
+    <col min="3" max="1023" width="12.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20">
-      <c r="A1" s="52" t="s">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1" s="56" t="s">
         <v>106</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
-      <c r="I1" s="52"/>
-      <c r="J1" s="52"/>
-      <c r="K1" s="52"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
+      <c r="J1" s="56"/>
+      <c r="K1" s="56"/>
       <c r="L1" s="30"/>
       <c r="M1" s="30"/>
       <c r="N1" s="30"/>
@@ -20720,7 +20797,7 @@
       <c r="S1" s="30"/>
       <c r="T1" s="30"/>
     </row>
-    <row r="2" spans="1:20">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">
         <v>81</v>
       </c>
@@ -20782,7 +20859,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="3" spans="1:20">
+    <row r="3" spans="1:20" ht="13" x14ac:dyDescent="0.3">
       <c r="A3" s="33" t="s">
         <v>124</v>
       </c>
@@ -20844,7 +20921,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="15" spans="1:20">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="42" t="s">
         <v>176</v>
       </c>
@@ -20852,7 +20929,7 @@
       <c r="C15" s="42"/>
       <c r="D15" s="42"/>
     </row>
-    <row r="16" spans="1:20">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="43" t="s">
         <v>171</v>
       </c>
@@ -20866,7 +20943,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="42" t="s">
         <v>175</v>
       </c>
@@ -20874,7 +20951,7 @@
       <c r="C28" s="42"/>
       <c r="D28" s="42"/>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="43" t="s">
         <v>171</v>
       </c>
@@ -20888,7 +20965,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="42" t="s">
         <v>180</v>
       </c>
@@ -20896,11 +20973,11 @@
       <c r="C44" s="42"/>
       <c r="D44" s="42"/>
     </row>
-    <row r="45" spans="1:4">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="43" t="s">
         <v>171</v>
       </c>
-      <c r="B45" s="44" t="s">
+      <c r="B45" s="45" t="s">
         <v>181</v>
       </c>
       <c r="C45" s="44" t="s">
@@ -20910,70 +20987,122 @@
         <v>183</v>
       </c>
     </row>
-    <row r="58" spans="1:4">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="42" t="s">
-        <v>170</v>
+        <v>250</v>
       </c>
       <c r="B58" s="42"/>
       <c r="C58" s="42"/>
       <c r="D58" s="42"/>
     </row>
-    <row r="59" spans="1:4">
-      <c r="A59" s="43" t="s">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A59" s="48" t="s">
         <v>171</v>
       </c>
-      <c r="B59" s="44" t="s">
+      <c r="B59" s="49" t="s">
+        <v>251</v>
+      </c>
+      <c r="C59" s="49" t="s">
+        <v>252</v>
+      </c>
+      <c r="D59" s="49" t="s">
+        <v>253</v>
+      </c>
+      <c r="E59" s="50"/>
+      <c r="F59" s="50"/>
+      <c r="G59" s="50"/>
+      <c r="H59" s="50"/>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="42" t="s">
+        <v>170</v>
+      </c>
+      <c r="B71" s="42"/>
+      <c r="C71" s="42"/>
+      <c r="D71" s="42"/>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="43" t="s">
+        <v>171</v>
+      </c>
+      <c r="B72" s="44" t="s">
         <v>184</v>
       </c>
-      <c r="C59" s="44" t="s">
+      <c r="C72" s="44" t="s">
         <v>185</v>
       </c>
-      <c r="D59" s="44" t="s">
+      <c r="D72" s="44" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="80" spans="1:4">
-      <c r="A80" s="42" t="s">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" s="42" t="s">
         <v>187</v>
       </c>
-      <c r="B80" s="42"/>
-      <c r="C80" s="42"/>
-      <c r="D80" s="42"/>
-    </row>
-    <row r="81" spans="1:4">
-      <c r="A81" s="43" t="s">
-        <v>188</v>
-      </c>
-      <c r="B81" s="45" t="s">
-        <v>189</v>
-      </c>
-      <c r="C81" s="45" t="s">
-        <v>190</v>
-      </c>
-      <c r="D81" s="45" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4">
-      <c r="A93" s="53" t="s">
-        <v>192</v>
-      </c>
-      <c r="B93" s="54"/>
+      <c r="B93" s="42"/>
       <c r="C93" s="42"/>
       <c r="D93" s="42"/>
     </row>
-    <row r="94" spans="1:4" ht="60">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="43" t="s">
+        <v>188</v>
+      </c>
+      <c r="B94" s="45" t="s">
+        <v>189</v>
+      </c>
+      <c r="C94" s="45" t="s">
+        <v>190</v>
+      </c>
+      <c r="D94" s="45" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A109" s="42" t="s">
+        <v>246</v>
+      </c>
+      <c r="B109" s="42"/>
+      <c r="C109" s="42"/>
+      <c r="D109" s="42"/>
+    </row>
+    <row r="110" spans="1:8" s="47" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A110" s="48" t="s">
+        <v>247</v>
+      </c>
+      <c r="B110" s="49" t="s">
+        <v>248</v>
+      </c>
+      <c r="C110" s="49" t="s">
+        <v>249</v>
+      </c>
+      <c r="D110" s="49" t="s">
+        <v>254</v>
+      </c>
+      <c r="E110" s="50"/>
+      <c r="F110" s="50"/>
+      <c r="G110" s="50"/>
+      <c r="H110" s="50"/>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A124" s="57" t="s">
+        <v>192</v>
+      </c>
+      <c r="B124" s="58"/>
+      <c r="C124" s="42"/>
+      <c r="D124" s="42"/>
+    </row>
+    <row r="125" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A125" s="43" t="s">
         <v>193</v>
       </c>
-      <c r="B94" s="46" t="s">
+      <c r="B125" s="46" t="s">
         <v>194</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A93:B93"/>
+    <mergeCell ref="A124:B124"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
POCOR-6646|modified condition to get record into report|status:ReadyToDeploy
</commit_message>
<xml_diff>
--- a/webroot/export/customexcel/default_templates/profile_template.xlsx
+++ b/webroot/export/customexcel/default_templates/profile_template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\pocor-openemis-core\webroot\export\customexcel\default_templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\poona\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AC4A4D9-B7DC-4E96-8F26-7D4F172C589B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{613322A7-21FD-4253-83DB-1B04836A2A3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="933" firstSheet="4" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="6" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <sheet name="Staff by Positions and Qualific" sheetId="6" r:id="rId6"/>
     <sheet name="Staff by Staff Type and Qualifi" sheetId="7" r:id="rId7"/>
     <sheet name="Extra details" sheetId="8" r:id="rId8"/>
-    <sheet name="Student Performance Summary" sheetId="9" r:id="rId9"/>
+    <sheet name="Student Performance Summary" sheetId="10" r:id="rId9"/>
   </sheets>
   <calcPr calcId="124519"/>
   <extLst>
@@ -38,7 +38,7 @@
     <author>Microsoft Office User</author>
   </authors>
   <commentList>
-    <comment ref="F2" authorId="0" shapeId="0" xr:uid="{67D43D7F-F299-4988-BFF1-DCE1E588C4D9}">
+    <comment ref="F2" authorId="0" shapeId="0" xr:uid="{EB7E133D-ED08-4475-ABE3-E99C03AB3FA6}">
       <text>
         <r>
           <rPr>
@@ -71,7 +71,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H2" authorId="0" shapeId="0" xr:uid="{5C71ACE4-B0A0-4BFB-AC8D-FDA9000C54C4}">
+    <comment ref="H2" authorId="0" shapeId="0" xr:uid="{4F4FA01F-3BB2-4E2D-BE7D-0F574B55055E}">
       <text>
         <r>
           <rPr>
@@ -109,7 +109,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="216">
   <si>
     <t>${"image":{"displayValue":"Institutions.logo_content","imageWidth":"100","imageMarginLeft":"20","imageMarginTop":"5"}}</t>
   </si>
@@ -696,228 +696,75 @@
     <t xml:space="preserve">${"match": {"displayValue": "NonTeachingStaffCount.area_level","rows": {"matchFrom": "InstitutionAreaName.id","matchTo": "InstitutionAreaName.id"}}} </t>
   </si>
   <si>
-    <t>Institution Custom Fields</t>
-  </si>
-  <si>
-    <t>Fields</t>
-  </si>
-  <si>
-    <t>Values</t>
-  </si>
-  <si>
-    <t>${"match": {"displayValue": "InstitutionCustomFields.name","rows": {"matchFrom": "InstitutionCustomFields.id","matchTo": "InstitutionCustomFields.id"}}}</t>
-  </si>
-  <si>
-    <t>${"match": {"displayValue": "InstitutionCustomFieldValues.data","rows": {"matchFrom": "InstitutionCustomFieldValues.id","matchTo": "InstitutionCustomFieldValues.id"}}}</t>
-  </si>
-  <si>
-    <t>Infrastructure Room Custom Fields</t>
-  </si>
-  <si>
-    <t>Report Student Assessment Summary</t>
-  </si>
-  <si>
-    <t>Academic Period</t>
-  </si>
-  <si>
-    <t>Area Code</t>
-  </si>
-  <si>
-    <t>Area Name</t>
-  </si>
-  <si>
-    <t>Institution Code</t>
-  </si>
-  <si>
-    <t>Institution  Name</t>
-  </si>
-  <si>
-    <t>Grade Code</t>
-  </si>
-  <si>
-    <t>Grade Name</t>
-  </si>
-  <si>
-    <t>Subject Code</t>
-  </si>
-  <si>
-    <t>Subject Name</t>
-  </si>
-  <si>
-    <t>Subject Weight</t>
-  </si>
-  <si>
-    <t>Assessment Code</t>
-  </si>
-  <si>
-    <t>Assessment Name</t>
-  </si>
-  <si>
-    <t>Period Code</t>
-  </si>
-  <si>
-    <t>Period Name</t>
-  </si>
-  <si>
-    <t>Period Weight</t>
-  </si>
-  <si>
-    <t>Average Marks</t>
-  </si>
-  <si>
-    <t>${"match": {"displayValue": "ReportStudentAssessmentSummary.academic_period_name","rows": {"matchFrom": "ReportStudentAssessmentSummary.id","matchTo": "ReportStudentAssessmentSummary.id"}}}</t>
-  </si>
-  <si>
-    <t>${"match": {"displayValue": "ReportStudentAssessmentSummary.area_code","rows": {"matchFrom": "ReportStudentAssessmentSummary.id","matchTo": "ReportStudentAssessmentSummary.id"}}}</t>
-  </si>
-  <si>
-    <t>${"match": {"displayValue": "ReportStudentAssessmentSummary.area_name","rows": {"matchFrom": "ReportStudentAssessmentSummary.id","matchTo": "ReportStudentAssessmentSummary.id"}}}</t>
-  </si>
-  <si>
-    <t>${"match": {"displayValue": "ReportStudentAssessmentSummary.institution_code","rows": {"matchFrom": "ReportStudentAssessmentSummary.id","matchTo": "ReportStudentAssessmentSummary.id"}}}</t>
-  </si>
-  <si>
-    <t>${"match": {"displayValue": "ReportStudentAssessmentSummary.institution_name","rows": {"matchFrom": "ReportStudentAssessmentSummary.id","matchTo": "ReportStudentAssessmentSummary.id"}}}</t>
-  </si>
-  <si>
-    <t>${"match": {"displayValue": "ReportStudentAssessmentSummary.grade_code","rows": {"matchFrom": "ReportStudentAssessmentSummary.id","matchTo": "ReportStudentAssessmentSummary.id"}}}</t>
-  </si>
-  <si>
-    <t>${"match": {"displayValue": "ReportStudentAssessmentSummary.grade_name","rows": {"matchFrom": "ReportStudentAssessmentSummary.id","matchTo": "ReportStudentAssessmentSummary.id"}}}</t>
-  </si>
-  <si>
-    <t>${"match": {"displayValue": "ReportStudentAssessmentSummary.subject_code","rows": {"matchFrom": "ReportStudentAssessmentSummary.id","matchTo": "ReportStudentAssessmentSummary.id"}}}</t>
-  </si>
-  <si>
-    <t>${"match": {"displayValue": "ReportStudentAssessmentSummary.subject_name","rows": {"matchFrom": "ReportStudentAssessmentSummary.id","matchTo": "ReportStudentAssessmentSummary.id"}}}</t>
-  </si>
-  <si>
-    <t>${"match": {"displayValue": "ReportStudentAssessmentSummary.subject_weight","rows": {"matchFrom": "ReportStudentAssessmentSummary.id","matchTo": "ReportStudentAssessmentSummary.id"}}}</t>
-  </si>
-  <si>
-    <t>${"match": {"displayValue": "ReportStudentAssessmentSummary.assessment_code","rows": {"matchFrom": "ReportStudentAssessmentSummary.id","matchTo": "ReportStudentAssessmentSummary.id"}}}</t>
-  </si>
-  <si>
-    <t>${"match": {"displayValue": "ReportStudentAssessmentSummary.assessment_name","rows": {"matchFrom": "ReportStudentAssessmentSummary.id","matchTo": "ReportStudentAssessmentSummary.id"}}}</t>
-  </si>
-  <si>
-    <t>${"match": {"displayValue": "ReportStudentAssessmentSummary.period_code","rows": {"matchFrom": "ReportStudentAssessmentSummary.id","matchTo": "ReportStudentAssessmentSummary.id"}}}</t>
-  </si>
-  <si>
-    <t>${"match": {"displayValue": "ReportStudentAssessmentSummary.period_name","rows": {"matchFrom": "ReportStudentAssessmentSummary.id","matchTo": "ReportStudentAssessmentSummary.id"}}}</t>
-  </si>
-  <si>
-    <t>${"match": {"displayValue": "ReportStudentAssessmentSummary.period_weight","rows": {"matchFrom": "ReportStudentAssessmentSummary.id","matchTo": "ReportStudentAssessmentSummary.id"}}}</t>
-  </si>
-  <si>
-    <t>${"match": {"displayValue": "ReportStudentAssessmentSummary.average_marks","rows": {"matchFrom": "ReportStudentAssessmentSummary.id","matchTo": "ReportStudentAssessmentSummary.id"}}}</t>
-  </si>
-  <si>
-    <t>Institution Room Code</t>
-  </si>
-  <si>
-    <t>Institution Room Name</t>
-  </si>
-  <si>
-    <t>Room Area</t>
-  </si>
-  <si>
-    <t>Room Type</t>
-  </si>
-  <si>
-    <t>Custom Field Name</t>
-  </si>
-  <si>
-    <t>Custom Field Value</t>
-  </si>
-  <si>
-    <t>${"match": {"displayValue": "InfrastructureRoomCustomFields.code","rows": {"matchFrom": "InfrastructureRoomCustomFields.id","matchTo": "InfrastructureRoomCustomFields.id"}}}</t>
-  </si>
-  <si>
-    <t>${"match": {"displayValue": "InfrastructureRoomCustomFields.name","rows": {"matchFrom": "InfrastructureRoomCustomFields.id","matchTo": "InfrastructureRoomCustomFields.id"}}}</t>
-  </si>
-  <si>
-    <t>${"match": {"displayValue": "InfrastructureRoomCustomFields.area","rows": {"matchFrom": "InfrastructureRoomCustomFields.id","matchTo": "InfrastructureRoomCustomFields.id"}}}</t>
-  </si>
-  <si>
-    <t>${"match": {"displayValue": "InfrastructureRoomCustomFields.room_type","rows": {"matchFrom": "InfrastructureRoomCustomFields.id","matchTo": "InfrastructureRoomCustomFields.id"}}}</t>
-  </si>
-  <si>
-    <t>${"match": {"displayValue": "InfrastructureRoomCustomFields.custom_field_name","rows": {"matchFrom": "InfrastructureRoomCustomFields.id","matchTo": "InfrastructureRoomCustomFields.id"}}}</t>
-  </si>
-  <si>
-    <t>${"match": {"displayValue": "InfrastructureRoomCustomFields.custom_field_value","rows": {"matchFrom": "InfrastructureRoomCustomFields.id","matchTo": "InfrastructureRoomCustomFields.id"}}}</t>
-  </si>
-  <si>
-    <t>Student Performance Summary</t>
-  </si>
-  <si>
     <t>Education Grade</t>
   </si>
   <si>
+    <t>Homeroom Teacher</t>
+  </si>
+  <si>
+    <t>OpenEMIS ID</t>
+  </si>
+  <si>
+    <t>Default Identity Number</t>
+  </si>
+  <si>
+    <t>Student Name</t>
+  </si>
+  <si>
+    <t>Education Subjects Name</t>
+  </si>
+  <si>
+    <t>Average Result</t>
+  </si>
+  <si>
+    <t>Individual Results</t>
+  </si>
+  <si>
+    <t>Number of Days Absence</t>
+  </si>
+  <si>
     <t>Class Name</t>
   </si>
   <si>
-    <t>Homeroom Teacher</t>
-  </si>
-  <si>
-    <t>OpenEMIS ID</t>
-  </si>
-  <si>
-    <t>Default Identity Number</t>
-  </si>
-  <si>
-    <t>Student Name</t>
-  </si>
-  <si>
-    <t>Education Subjects Name</t>
-  </si>
-  <si>
-    <t>Average Result</t>
-  </si>
-  <si>
-    <t>Individual Results</t>
-  </si>
-  <si>
-    <t>Number of Days Absence</t>
-  </si>
-  <si>
-    <t>${"match": {"displayValue": "StudentDetails.grade_name","rows": {"matchFrom": "StudentDetails.id","matchTo": "StudentDetails.id"}}}</t>
+    <t>${"match": {"displayValue": "StudentDetails.openemis_no","rows": {"matchFrom": "StudentDetails.id","matchTo": "StudentDetails.id"}}}</t>
+  </si>
+  <si>
+    <t>${"match": {"displayValue": "StudentDetails.identity_number","rows": {"matchFrom": "StudentDetails.id","matchTo": "StudentDetails.id"}}}</t>
+  </si>
+  <si>
+    <t>${"match": {"displayValue": "StudentDetails.student_name","rows": {"matchFrom": "StudentDetails.id","matchTo": "StudentDetails.id"}}}</t>
   </si>
   <si>
     <t xml:space="preserve">${"match": {"displayValue": "StudentDetails.class_name","rows": {"matchFrom": "StudentDetails.id","matchTo": "StudentDetails.id"}}}
 </t>
   </si>
   <si>
+    <t>${"match": {"displayValue": "StudentDetails.grade_name","rows": {"matchFrom": "StudentDetails.id","matchTo": "StudentDetails.id"}}}</t>
+  </si>
+  <si>
     <t>${"match": {"displayValue": "StudentDetails.homeroom_teacher","rows": {"matchFrom": "StudentDetails.id","matchTo": "StudentDetails.id"}}}</t>
   </si>
   <si>
-    <t>${"match": {"displayValue": "StudentDetails.openemis_no","rows": {"matchFrom": "StudentDetails.id","matchTo": "StudentDetails.id"}}}</t>
-  </si>
-  <si>
-    <t>${"match": {"displayValue": "StudentDetails.identity_number","rows": {"matchFrom": "StudentDetails.id","matchTo": "StudentDetails.id"}}}</t>
-  </si>
-  <si>
-    <t>${"match": {"displayValue": "StudentDetails.student_name","rows": {"matchFrom": "StudentDetails.id","matchTo": "StudentDetails.id"}}}</t>
-  </si>
-  <si>
     <t>${"match": {"displayValue": "StudentDetails.subject_name","rows": {"matchFrom": "StudentDetails.id","matchTo": "StudentDetails.id"}}}</t>
   </si>
   <si>
+    <t>${"match": {"displayValue": "StudentDetails.absence_day","rows": {"matchFrom": "StudentDetails.id","matchTo": "StudentDetails.id"}}}</t>
+  </si>
+  <si>
     <t>${"match": {"displayValue": "StudentDetails.average_marks","rows": {"matchFrom": "StudentDetails.id","matchTo": "StudentDetails.id"}}}</t>
   </si>
   <si>
     <t>${"match": {"displayValue": "StudentDetails.individual_result","rows": {"matchFrom": "StudentDetails.id","matchTo": "StudentDetails.id"}}}</t>
   </si>
   <si>
-    <t>${"match": {"displayValue": "StudentDetails.absence_day","rows": {"matchFrom": "StudentDetails.id","matchTo": "StudentDetails.id"}}}</t>
+    <t>Student Performance Summary</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -997,13 +844,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color rgb="FF172B4D"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1015,6 +855,19 @@
       <color rgb="FF000000"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FF172B4D"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF172B4D"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1139,7 +992,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1243,6 +1096,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1267,22 +1126,22 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -1691,10 +1550,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:IV1041"/>
+  <dimension ref="A1:IV1048"/>
   <sheetViews>
-    <sheetView topLeftCell="A155" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="A168" sqref="A168"/>
+    <sheetView topLeftCell="B55" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="B60" sqref="B60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1715,7 +1574,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="49" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4"/>
@@ -1736,13 +1595,13 @@
       <c r="Q1" s="7"/>
     </row>
     <row r="2" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="47"/>
-      <c r="B2" s="48" t="s">
+      <c r="A2" s="49"/>
+      <c r="B2" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="48"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
       <c r="F2" s="8"/>
       <c r="G2" s="9"/>
       <c r="H2" s="7"/>
@@ -1996,13 +1855,13 @@
       <c r="IV2" s="3"/>
     </row>
     <row r="3" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="47"/>
-      <c r="B3" s="49" t="s">
+      <c r="A3" s="49"/>
+      <c r="B3" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="49"/>
-      <c r="D3" s="49"/>
-      <c r="E3" s="49"/>
+      <c r="C3" s="51"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
       <c r="F3" s="9"/>
       <c r="G3" s="9"/>
       <c r="H3" s="7"/>
@@ -2256,7 +2115,7 @@
       <c r="IV3" s="3"/>
     </row>
     <row r="4" spans="1:256" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="47"/>
+      <c r="A4" s="49"/>
       <c r="B4" s="4"/>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
@@ -18081,10 +17940,8 @@
       <c r="IV71" s="3"/>
     </row>
     <row r="72" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A72" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="B72" s="1"/>
+      <c r="A72" s="3"/>
+      <c r="B72" s="3"/>
       <c r="C72" s="3"/>
       <c r="E72" s="3"/>
       <c r="F72" s="3"/>
@@ -18340,12 +18197,8 @@
       <c r="IV72" s="3"/>
     </row>
     <row r="73" spans="1:256" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A73" s="23" t="s">
-        <v>196</v>
-      </c>
-      <c r="B73" s="24" t="s">
-        <v>197</v>
-      </c>
+      <c r="A73" s="3"/>
+      <c r="B73" s="3"/>
       <c r="C73" s="3"/>
       <c r="E73" s="3"/>
       <c r="F73" s="7"/>
@@ -18601,12 +18454,8 @@
       <c r="IV73" s="3"/>
     </row>
     <row r="74" spans="1:256" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A74" s="25" t="s">
-        <v>198</v>
-      </c>
-      <c r="B74" s="25" t="s">
-        <v>199</v>
-      </c>
+      <c r="A74" s="3"/>
+      <c r="B74" s="3"/>
       <c r="C74" s="3"/>
       <c r="E74" s="3"/>
       <c r="F74" s="7"/>
@@ -19403,139 +19252,22 @@
     <row r="94" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="95" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="96" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="97" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="98" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A98" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="B98" s="1"/>
-      <c r="C98" s="1"/>
-      <c r="D98" s="1"/>
-      <c r="E98" s="1"/>
-      <c r="F98" s="1"/>
-      <c r="G98" s="1"/>
-      <c r="H98" s="1"/>
-      <c r="I98" s="1"/>
-      <c r="J98" s="1"/>
-      <c r="K98" s="1"/>
-      <c r="L98" s="1"/>
-      <c r="M98" s="1"/>
-      <c r="N98" s="1"/>
-      <c r="O98" s="1"/>
-      <c r="P98" s="1"/>
-    </row>
-    <row r="99" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A99" s="23" t="s">
-        <v>202</v>
-      </c>
-      <c r="B99" s="23" t="s">
-        <v>203</v>
-      </c>
-      <c r="C99" s="23" t="s">
-        <v>204</v>
-      </c>
-      <c r="D99" s="23" t="s">
-        <v>205</v>
-      </c>
-      <c r="E99" s="23" t="s">
-        <v>206</v>
-      </c>
-      <c r="F99" s="23" t="s">
-        <v>207</v>
-      </c>
-      <c r="G99" s="23" t="s">
-        <v>208</v>
-      </c>
-      <c r="H99" s="23" t="s">
-        <v>209</v>
-      </c>
-      <c r="I99" s="23" t="s">
-        <v>210</v>
-      </c>
-      <c r="J99" s="23" t="s">
-        <v>211</v>
-      </c>
-      <c r="K99" s="23" t="s">
-        <v>212</v>
-      </c>
-      <c r="L99" s="23" t="s">
-        <v>213</v>
-      </c>
-      <c r="M99" s="23" t="s">
-        <v>214</v>
-      </c>
-      <c r="N99" s="23" t="s">
-        <v>215</v>
-      </c>
-      <c r="O99" s="23" t="s">
-        <v>216</v>
-      </c>
-      <c r="P99" s="23" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="100" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A100" s="25" t="s">
-        <v>218</v>
-      </c>
-      <c r="B100" s="25" t="s">
-        <v>219</v>
-      </c>
-      <c r="C100" s="25" t="s">
-        <v>220</v>
-      </c>
-      <c r="D100" s="25" t="s">
-        <v>221</v>
-      </c>
-      <c r="E100" s="25" t="s">
-        <v>222</v>
-      </c>
-      <c r="F100" s="25" t="s">
-        <v>223</v>
-      </c>
-      <c r="G100" s="25" t="s">
-        <v>224</v>
-      </c>
-      <c r="H100" s="25" t="s">
-        <v>225</v>
-      </c>
-      <c r="I100" s="25" t="s">
-        <v>226</v>
-      </c>
-      <c r="J100" s="25" t="s">
-        <v>227</v>
-      </c>
-      <c r="K100" s="25" t="s">
-        <v>228</v>
-      </c>
-      <c r="L100" s="25" t="s">
-        <v>229</v>
-      </c>
-      <c r="M100" s="25" t="s">
-        <v>230</v>
-      </c>
-      <c r="N100" s="25" t="s">
-        <v>231</v>
-      </c>
-      <c r="O100" s="25" t="s">
-        <v>232</v>
-      </c>
-      <c r="P100" s="25" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="101" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="102" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="103" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="104" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="105" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="106" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="107" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="108" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="109" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="110" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="111" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="112" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="97" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="98" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="99" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="100" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="101" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="102" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="103" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="104" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="105" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="106" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="107" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="108" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="109" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="110" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="111" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="112" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="113" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="114" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="115" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -19584,69 +19316,22 @@
     <row r="158" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="159" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="160" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="161" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="162" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="163" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="164" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="165" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="166" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="167" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="168" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="169" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="170" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="171" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A171" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="B171" s="1"/>
-      <c r="C171" s="1"/>
-      <c r="D171" s="1"/>
-      <c r="E171" s="1"/>
-      <c r="F171" s="1"/>
-    </row>
-    <row r="172" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A172" s="23" t="s">
-        <v>234</v>
-      </c>
-      <c r="B172" s="23" t="s">
-        <v>235</v>
-      </c>
-      <c r="C172" s="23" t="s">
-        <v>236</v>
-      </c>
-      <c r="D172" s="23" t="s">
-        <v>237</v>
-      </c>
-      <c r="E172" s="23" t="s">
-        <v>238</v>
-      </c>
-      <c r="F172" s="23" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="173" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A173" s="25" t="s">
-        <v>240</v>
-      </c>
-      <c r="B173" s="25" t="s">
-        <v>241</v>
-      </c>
-      <c r="C173" s="25" t="s">
-        <v>242</v>
-      </c>
-      <c r="D173" s="25" t="s">
-        <v>243</v>
-      </c>
-      <c r="E173" s="25" t="s">
-        <v>244</v>
-      </c>
-      <c r="F173" s="25" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="174" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="175" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="176" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="161" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="162" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="163" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="164" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="165" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="166" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="167" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="168" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="169" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="170" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="171" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="172" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="173" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="174" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="175" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="176" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="177" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="178" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="179" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -20512,6 +20197,13 @@
     <row r="1039" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="1040" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="1041" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="1042" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="1043" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="1044" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="1045" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="1046" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="1047" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="1048" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:A4"/>
@@ -20532,7 +20224,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView zoomScale="98" zoomScaleNormal="98" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -20543,12 +20235,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="13" x14ac:dyDescent="0.3">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="52" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="26" t="s">
@@ -20596,7 +20288,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -20607,11 +20299,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="13" x14ac:dyDescent="0.3">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="53" t="s">
         <v>79</v>
       </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="51"/>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="26" t="s">
@@ -20658,7 +20350,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -20669,11 +20361,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="54" t="s">
         <v>85</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="26" t="s">
@@ -20719,7 +20411,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScalePageLayoutView="60" workbookViewId="0">
+    <sheetView zoomScalePageLayoutView="60" workbookViewId="0">
       <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
@@ -20731,11 +20423,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="54" t="s">
         <v>91</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="26" t="s">
@@ -20781,8 +20473,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection sqref="A1:C1"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -20793,11 +20485,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="54" t="s">
         <v>96</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
@@ -20843,8 +20535,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection sqref="A1:C1"/>
+    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -20855,11 +20547,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="54" t="s">
         <v>101</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
@@ -20906,7 +20598,7 @@
   <dimension ref="A1:T94"/>
   <sheetViews>
     <sheetView zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection sqref="A1:K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -20917,19 +20609,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="54" t="s">
         <v>106</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
-      <c r="I1" s="52"/>
-      <c r="J1" s="52"/>
-      <c r="K1" s="52"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
       <c r="L1" s="30"/>
       <c r="M1" s="30"/>
       <c r="N1" s="30"/>
@@ -21175,10 +20867,10 @@
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" s="53" t="s">
+      <c r="A93" s="55" t="s">
         <v>192</v>
       </c>
-      <c r="B93" s="54"/>
+      <c r="B93" s="56"/>
       <c r="C93" s="42"/>
       <c r="D93" s="42"/>
     </row>
@@ -21205,110 +20897,117 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4374B4A3-7A12-40D7-B707-A882C2CD9BFF}">
-  <dimension ref="A1:J3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03DDC5C3-BD6D-444D-BAD4-1FA02546E2E3}">
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.08984375" customWidth="1"/>
-    <col min="2" max="2" width="12.26953125" customWidth="1"/>
-    <col min="3" max="3" width="16.36328125" customWidth="1"/>
-    <col min="4" max="4" width="13.81640625" customWidth="1"/>
-    <col min="5" max="5" width="18.26953125" customWidth="1"/>
-    <col min="6" max="6" width="15.26953125" customWidth="1"/>
-    <col min="7" max="7" width="22.26953125" customWidth="1"/>
-    <col min="8" max="8" width="15.6328125" customWidth="1"/>
-    <col min="9" max="9" width="14.81640625" customWidth="1"/>
-    <col min="10" max="10" width="21" customWidth="1"/>
+    <col min="1" max="1" width="14.453125" customWidth="1"/>
+    <col min="2" max="2" width="11.90625" customWidth="1"/>
+    <col min="3" max="3" width="17.81640625" customWidth="1"/>
+    <col min="4" max="4" width="13.08984375" customWidth="1"/>
+    <col min="5" max="5" width="19" customWidth="1"/>
+    <col min="6" max="6" width="15.1796875" customWidth="1"/>
+    <col min="7" max="7" width="21.7265625" customWidth="1"/>
+    <col min="8" max="8" width="14.6328125" customWidth="1"/>
+    <col min="9" max="9" width="14.36328125" customWidth="1"/>
+    <col min="10" max="10" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="55" t="s">
-        <v>246</v>
-      </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="56"/>
-      <c r="J1" s="56"/>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="58" t="s">
+        <v>215</v>
+      </c>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="59"/>
+      <c r="H1" s="59"/>
+      <c r="I1" s="59"/>
+      <c r="J1" s="59"/>
     </row>
-    <row r="2" spans="1:10" ht="13" x14ac:dyDescent="0.3">
-      <c r="A2" s="57" t="s">
-        <v>247</v>
-      </c>
-      <c r="B2" s="57" t="s">
-        <v>248</v>
-      </c>
-      <c r="C2" s="57" t="s">
-        <v>249</v>
-      </c>
-      <c r="D2" s="57" t="s">
-        <v>250</v>
-      </c>
-      <c r="E2" s="57" t="s">
-        <v>251</v>
-      </c>
-      <c r="F2" s="57" t="s">
-        <v>252</v>
-      </c>
-      <c r="G2" s="57" t="s">
-        <v>253</v>
-      </c>
-      <c r="H2" s="57" t="s">
-        <v>254</v>
-      </c>
-      <c r="I2" s="57" t="s">
-        <v>255</v>
-      </c>
-      <c r="J2" s="57" t="s">
-        <v>256</v>
-      </c>
+    <row r="2" spans="1:12" ht="13" x14ac:dyDescent="0.3">
+      <c r="A2" s="47" t="s">
+        <v>195</v>
+      </c>
+      <c r="B2" s="47" t="s">
+        <v>204</v>
+      </c>
+      <c r="C2" s="47" t="s">
+        <v>196</v>
+      </c>
+      <c r="D2" s="47" t="s">
+        <v>197</v>
+      </c>
+      <c r="E2" s="47" t="s">
+        <v>198</v>
+      </c>
+      <c r="F2" s="47" t="s">
+        <v>199</v>
+      </c>
+      <c r="G2" s="47" t="s">
+        <v>200</v>
+      </c>
+      <c r="H2" s="47" t="s">
+        <v>201</v>
+      </c>
+      <c r="I2" s="47" t="s">
+        <v>202</v>
+      </c>
+      <c r="J2" s="47" t="s">
+        <v>203</v>
+      </c>
+      <c r="K2" s="47"/>
+      <c r="L2" s="47"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="58" t="s">
-        <v>257</v>
-      </c>
-      <c r="B3" s="59" t="s">
-        <v>258</v>
-      </c>
-      <c r="C3" s="60" t="s">
-        <v>259</v>
-      </c>
-      <c r="D3" s="58" t="s">
-        <v>260</v>
-      </c>
-      <c r="E3" s="59" t="s">
-        <v>261</v>
-      </c>
-      <c r="F3" s="59" t="s">
-        <v>262</v>
-      </c>
-      <c r="G3" s="59" t="s">
-        <v>263</v>
-      </c>
-      <c r="H3" s="59" t="s">
-        <v>264</v>
-      </c>
-      <c r="I3" s="59" t="s">
-        <v>265</v>
-      </c>
-      <c r="J3" s="59" t="s">
-        <v>266</v>
-      </c>
+    <row r="3" spans="1:12" ht="15.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="57" t="s">
+        <v>209</v>
+      </c>
+      <c r="B3" s="60" t="s">
+        <v>208</v>
+      </c>
+      <c r="C3" s="61" t="s">
+        <v>210</v>
+      </c>
+      <c r="D3" s="57" t="s">
+        <v>205</v>
+      </c>
+      <c r="E3" s="60" t="s">
+        <v>206</v>
+      </c>
+      <c r="F3" s="60" t="s">
+        <v>207</v>
+      </c>
+      <c r="G3" s="60" t="s">
+        <v>211</v>
+      </c>
+      <c r="H3" s="62" t="s">
+        <v>213</v>
+      </c>
+      <c r="I3" s="62" t="s">
+        <v>214</v>
+      </c>
+      <c r="J3" s="60" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="48"/>
+      <c r="D4" s="48"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:J1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
POCOR-6646|modified query to get correct sum of absent days of student|Status:ReadyToDeloy
</commit_message>
<xml_diff>
--- a/webroot/export/customexcel/default_templates/profile_template.xlsx
+++ b/webroot/export/customexcel/default_templates/profile_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\poona\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\pocor-openemis-core\webroot\export\customexcel\default_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{613322A7-21FD-4253-83DB-1B04836A2A3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C140BC6F-C971-4E16-9493-08C056585DA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="6" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="933" firstSheet="4" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <sheet name="Staff by Positions and Qualific" sheetId="6" r:id="rId6"/>
     <sheet name="Staff by Staff Type and Qualifi" sheetId="7" r:id="rId7"/>
     <sheet name="Extra details" sheetId="8" r:id="rId8"/>
-    <sheet name="Student Performance Summary" sheetId="10" r:id="rId9"/>
+    <sheet name="Student Performance Summary" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="124519"/>
   <extLst>
@@ -38,7 +38,7 @@
     <author>Microsoft Office User</author>
   </authors>
   <commentList>
-    <comment ref="F2" authorId="0" shapeId="0" xr:uid="{EB7E133D-ED08-4475-ABE3-E99C03AB3FA6}">
+    <comment ref="F2" authorId="0" shapeId="0" xr:uid="{F01695D2-B671-4E84-9F87-A62CD3489B50}">
       <text>
         <r>
           <rPr>
@@ -71,7 +71,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H2" authorId="0" shapeId="0" xr:uid="{4F4FA01F-3BB2-4E2D-BE7D-0F574B55055E}">
+    <comment ref="H2" authorId="0" shapeId="0" xr:uid="{1D9C0F74-2025-4507-A482-610EFCC338CD}">
       <text>
         <r>
           <rPr>
@@ -109,7 +109,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="267">
   <si>
     <t>${"image":{"displayValue":"Institutions.logo_content","imageWidth":"100","imageMarginLeft":"20","imageMarginTop":"5"}}</t>
   </si>
@@ -696,9 +696,168 @@
     <t xml:space="preserve">${"match": {"displayValue": "NonTeachingStaffCount.area_level","rows": {"matchFrom": "InstitutionAreaName.id","matchTo": "InstitutionAreaName.id"}}} </t>
   </si>
   <si>
+    <t>Institution Custom Fields</t>
+  </si>
+  <si>
+    <t>Fields</t>
+  </si>
+  <si>
+    <t>Values</t>
+  </si>
+  <si>
+    <t>${"match": {"displayValue": "InstitutionCustomFields.name","rows": {"matchFrom": "InstitutionCustomFields.id","matchTo": "InstitutionCustomFields.id"}}}</t>
+  </si>
+  <si>
+    <t>${"match": {"displayValue": "InstitutionCustomFieldValues.data","rows": {"matchFrom": "InstitutionCustomFieldValues.id","matchTo": "InstitutionCustomFieldValues.id"}}}</t>
+  </si>
+  <si>
+    <t>Infrastructure Room Custom Fields</t>
+  </si>
+  <si>
+    <t>Report Student Assessment Summary</t>
+  </si>
+  <si>
+    <t>Academic Period</t>
+  </si>
+  <si>
+    <t>Area Code</t>
+  </si>
+  <si>
+    <t>Area Name</t>
+  </si>
+  <si>
+    <t>Institution Code</t>
+  </si>
+  <si>
+    <t>Institution  Name</t>
+  </si>
+  <si>
+    <t>Grade Code</t>
+  </si>
+  <si>
+    <t>Grade Name</t>
+  </si>
+  <si>
+    <t>Subject Code</t>
+  </si>
+  <si>
+    <t>Subject Name</t>
+  </si>
+  <si>
+    <t>Subject Weight</t>
+  </si>
+  <si>
+    <t>Assessment Code</t>
+  </si>
+  <si>
+    <t>Assessment Name</t>
+  </si>
+  <si>
+    <t>Period Code</t>
+  </si>
+  <si>
+    <t>Period Name</t>
+  </si>
+  <si>
+    <t>Period Weight</t>
+  </si>
+  <si>
+    <t>Average Marks</t>
+  </si>
+  <si>
+    <t>${"match": {"displayValue": "ReportStudentAssessmentSummary.academic_period_name","rows": {"matchFrom": "ReportStudentAssessmentSummary.id","matchTo": "ReportStudentAssessmentSummary.id"}}}</t>
+  </si>
+  <si>
+    <t>${"match": {"displayValue": "ReportStudentAssessmentSummary.area_code","rows": {"matchFrom": "ReportStudentAssessmentSummary.id","matchTo": "ReportStudentAssessmentSummary.id"}}}</t>
+  </si>
+  <si>
+    <t>${"match": {"displayValue": "ReportStudentAssessmentSummary.area_name","rows": {"matchFrom": "ReportStudentAssessmentSummary.id","matchTo": "ReportStudentAssessmentSummary.id"}}}</t>
+  </si>
+  <si>
+    <t>${"match": {"displayValue": "ReportStudentAssessmentSummary.institution_code","rows": {"matchFrom": "ReportStudentAssessmentSummary.id","matchTo": "ReportStudentAssessmentSummary.id"}}}</t>
+  </si>
+  <si>
+    <t>${"match": {"displayValue": "ReportStudentAssessmentSummary.institution_name","rows": {"matchFrom": "ReportStudentAssessmentSummary.id","matchTo": "ReportStudentAssessmentSummary.id"}}}</t>
+  </si>
+  <si>
+    <t>${"match": {"displayValue": "ReportStudentAssessmentSummary.grade_code","rows": {"matchFrom": "ReportStudentAssessmentSummary.id","matchTo": "ReportStudentAssessmentSummary.id"}}}</t>
+  </si>
+  <si>
+    <t>${"match": {"displayValue": "ReportStudentAssessmentSummary.grade_name","rows": {"matchFrom": "ReportStudentAssessmentSummary.id","matchTo": "ReportStudentAssessmentSummary.id"}}}</t>
+  </si>
+  <si>
+    <t>${"match": {"displayValue": "ReportStudentAssessmentSummary.subject_code","rows": {"matchFrom": "ReportStudentAssessmentSummary.id","matchTo": "ReportStudentAssessmentSummary.id"}}}</t>
+  </si>
+  <si>
+    <t>${"match": {"displayValue": "ReportStudentAssessmentSummary.subject_name","rows": {"matchFrom": "ReportStudentAssessmentSummary.id","matchTo": "ReportStudentAssessmentSummary.id"}}}</t>
+  </si>
+  <si>
+    <t>${"match": {"displayValue": "ReportStudentAssessmentSummary.subject_weight","rows": {"matchFrom": "ReportStudentAssessmentSummary.id","matchTo": "ReportStudentAssessmentSummary.id"}}}</t>
+  </si>
+  <si>
+    <t>${"match": {"displayValue": "ReportStudentAssessmentSummary.assessment_code","rows": {"matchFrom": "ReportStudentAssessmentSummary.id","matchTo": "ReportStudentAssessmentSummary.id"}}}</t>
+  </si>
+  <si>
+    <t>${"match": {"displayValue": "ReportStudentAssessmentSummary.assessment_name","rows": {"matchFrom": "ReportStudentAssessmentSummary.id","matchTo": "ReportStudentAssessmentSummary.id"}}}</t>
+  </si>
+  <si>
+    <t>${"match": {"displayValue": "ReportStudentAssessmentSummary.period_code","rows": {"matchFrom": "ReportStudentAssessmentSummary.id","matchTo": "ReportStudentAssessmentSummary.id"}}}</t>
+  </si>
+  <si>
+    <t>${"match": {"displayValue": "ReportStudentAssessmentSummary.period_name","rows": {"matchFrom": "ReportStudentAssessmentSummary.id","matchTo": "ReportStudentAssessmentSummary.id"}}}</t>
+  </si>
+  <si>
+    <t>${"match": {"displayValue": "ReportStudentAssessmentSummary.period_weight","rows": {"matchFrom": "ReportStudentAssessmentSummary.id","matchTo": "ReportStudentAssessmentSummary.id"}}}</t>
+  </si>
+  <si>
+    <t>${"match": {"displayValue": "ReportStudentAssessmentSummary.average_marks","rows": {"matchFrom": "ReportStudentAssessmentSummary.id","matchTo": "ReportStudentAssessmentSummary.id"}}}</t>
+  </si>
+  <si>
+    <t>Institution Room Code</t>
+  </si>
+  <si>
+    <t>Institution Room Name</t>
+  </si>
+  <si>
+    <t>Room Area</t>
+  </si>
+  <si>
+    <t>Room Type</t>
+  </si>
+  <si>
+    <t>Custom Field Name</t>
+  </si>
+  <si>
+    <t>Custom Field Value</t>
+  </si>
+  <si>
+    <t>${"match": {"displayValue": "InfrastructureRoomCustomFields.code","rows": {"matchFrom": "InfrastructureRoomCustomFields.id","matchTo": "InfrastructureRoomCustomFields.id"}}}</t>
+  </si>
+  <si>
+    <t>${"match": {"displayValue": "InfrastructureRoomCustomFields.name","rows": {"matchFrom": "InfrastructureRoomCustomFields.id","matchTo": "InfrastructureRoomCustomFields.id"}}}</t>
+  </si>
+  <si>
+    <t>${"match": {"displayValue": "InfrastructureRoomCustomFields.area","rows": {"matchFrom": "InfrastructureRoomCustomFields.id","matchTo": "InfrastructureRoomCustomFields.id"}}}</t>
+  </si>
+  <si>
+    <t>${"match": {"displayValue": "InfrastructureRoomCustomFields.room_type","rows": {"matchFrom": "InfrastructureRoomCustomFields.id","matchTo": "InfrastructureRoomCustomFields.id"}}}</t>
+  </si>
+  <si>
+    <t>${"match": {"displayValue": "InfrastructureRoomCustomFields.custom_field_name","rows": {"matchFrom": "InfrastructureRoomCustomFields.id","matchTo": "InfrastructureRoomCustomFields.id"}}}</t>
+  </si>
+  <si>
+    <t>${"match": {"displayValue": "InfrastructureRoomCustomFields.custom_field_value","rows": {"matchFrom": "InfrastructureRoomCustomFields.id","matchTo": "InfrastructureRoomCustomFields.id"}}}</t>
+  </si>
+  <si>
+    <t>Student Performance Summary</t>
+  </si>
+  <si>
     <t>Education Grade</t>
   </si>
   <si>
+    <t>Class Name</t>
+  </si>
+  <si>
     <t>Homeroom Teacher</t>
   </si>
   <si>
@@ -723,48 +882,42 @@
     <t>Number of Days Absence</t>
   </si>
   <si>
-    <t>Class Name</t>
-  </si>
-  <si>
-    <t>${"match": {"displayValue": "StudentDetails.openemis_no","rows": {"matchFrom": "StudentDetails.id","matchTo": "StudentDetails.id"}}}</t>
-  </si>
-  <si>
-    <t>${"match": {"displayValue": "StudentDetails.identity_number","rows": {"matchFrom": "StudentDetails.id","matchTo": "StudentDetails.id"}}}</t>
-  </si>
-  <si>
-    <t>${"match": {"displayValue": "StudentDetails.student_name","rows": {"matchFrom": "StudentDetails.id","matchTo": "StudentDetails.id"}}}</t>
+    <t>${"match": {"displayValue": "StudentDetails.grade_name","rows": {"matchFrom": "StudentDetails.id","matchTo": "StudentDetails.id"}}}</t>
   </si>
   <si>
     <t xml:space="preserve">${"match": {"displayValue": "StudentDetails.class_name","rows": {"matchFrom": "StudentDetails.id","matchTo": "StudentDetails.id"}}}
 </t>
   </si>
   <si>
-    <t>${"match": {"displayValue": "StudentDetails.grade_name","rows": {"matchFrom": "StudentDetails.id","matchTo": "StudentDetails.id"}}}</t>
-  </si>
-  <si>
     <t>${"match": {"displayValue": "StudentDetails.homeroom_teacher","rows": {"matchFrom": "StudentDetails.id","matchTo": "StudentDetails.id"}}}</t>
   </si>
   <si>
+    <t>${"match": {"displayValue": "StudentDetails.openemis_no","rows": {"matchFrom": "StudentDetails.id","matchTo": "StudentDetails.id"}}}</t>
+  </si>
+  <si>
+    <t>${"match": {"displayValue": "StudentDetails.identity_number","rows": {"matchFrom": "StudentDetails.id","matchTo": "StudentDetails.id"}}}</t>
+  </si>
+  <si>
+    <t>${"match": {"displayValue": "StudentDetails.student_name","rows": {"matchFrom": "StudentDetails.id","matchTo": "StudentDetails.id"}}}</t>
+  </si>
+  <si>
     <t>${"match": {"displayValue": "StudentDetails.subject_name","rows": {"matchFrom": "StudentDetails.id","matchTo": "StudentDetails.id"}}}</t>
   </si>
   <si>
+    <t>${"match": {"displayValue": "StudentDetails.average_marks","rows": {"matchFrom": "StudentDetails.id","matchTo": "StudentDetails.id"}}}</t>
+  </si>
+  <si>
+    <t>${"match": {"displayValue": "StudentDetails.individual_result","rows": {"matchFrom": "StudentDetails.id","matchTo": "StudentDetails.id"}}}</t>
+  </si>
+  <si>
     <t>${"match": {"displayValue": "StudentDetails.absence_day","rows": {"matchFrom": "StudentDetails.id","matchTo": "StudentDetails.id"}}}</t>
-  </si>
-  <si>
-    <t>${"match": {"displayValue": "StudentDetails.average_marks","rows": {"matchFrom": "StudentDetails.id","matchTo": "StudentDetails.id"}}}</t>
-  </si>
-  <si>
-    <t>${"match": {"displayValue": "StudentDetails.individual_result","rows": {"matchFrom": "StudentDetails.id","matchTo": "StudentDetails.id"}}}</t>
-  </si>
-  <si>
-    <t>Student Performance Summary</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -844,6 +997,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="9"/>
+      <color rgb="FF172B4D"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -855,19 +1015,6 @@
       <color rgb="FF000000"/>
       <name val="Tahoma"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="7"/>
-      <color rgb="FF172B4D"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF172B4D"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -992,7 +1139,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1096,12 +1243,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1126,22 +1267,22 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -1550,10 +1691,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:IV1048"/>
+  <dimension ref="A1:IV1041"/>
   <sheetViews>
-    <sheetView topLeftCell="B55" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="B60" sqref="B60"/>
+    <sheetView topLeftCell="A155" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="A168" sqref="A168"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1574,7 +1715,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4"/>
@@ -1595,13 +1736,13 @@
       <c r="Q1" s="7"/>
     </row>
     <row r="2" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="49"/>
-      <c r="B2" s="50" t="s">
+      <c r="A2" s="47"/>
+      <c r="B2" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
       <c r="F2" s="8"/>
       <c r="G2" s="9"/>
       <c r="H2" s="7"/>
@@ -1855,13 +1996,13 @@
       <c r="IV2" s="3"/>
     </row>
     <row r="3" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="49"/>
-      <c r="B3" s="51" t="s">
+      <c r="A3" s="47"/>
+      <c r="B3" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="51"/>
-      <c r="D3" s="51"/>
-      <c r="E3" s="51"/>
+      <c r="C3" s="49"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
       <c r="F3" s="9"/>
       <c r="G3" s="9"/>
       <c r="H3" s="7"/>
@@ -2115,7 +2256,7 @@
       <c r="IV3" s="3"/>
     </row>
     <row r="4" spans="1:256" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="49"/>
+      <c r="A4" s="47"/>
       <c r="B4" s="4"/>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
@@ -17940,8 +18081,10 @@
       <c r="IV71" s="3"/>
     </row>
     <row r="72" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A72" s="3"/>
-      <c r="B72" s="3"/>
+      <c r="A72" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B72" s="1"/>
       <c r="C72" s="3"/>
       <c r="E72" s="3"/>
       <c r="F72" s="3"/>
@@ -18197,8 +18340,12 @@
       <c r="IV72" s="3"/>
     </row>
     <row r="73" spans="1:256" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A73" s="3"/>
-      <c r="B73" s="3"/>
+      <c r="A73" s="23" t="s">
+        <v>196</v>
+      </c>
+      <c r="B73" s="24" t="s">
+        <v>197</v>
+      </c>
       <c r="C73" s="3"/>
       <c r="E73" s="3"/>
       <c r="F73" s="7"/>
@@ -18454,8 +18601,12 @@
       <c r="IV73" s="3"/>
     </row>
     <row r="74" spans="1:256" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A74" s="3"/>
-      <c r="B74" s="3"/>
+      <c r="A74" s="25" t="s">
+        <v>198</v>
+      </c>
+      <c r="B74" s="25" t="s">
+        <v>199</v>
+      </c>
       <c r="C74" s="3"/>
       <c r="E74" s="3"/>
       <c r="F74" s="7"/>
@@ -19252,22 +19403,139 @@
     <row r="94" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="95" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="96" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="97" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="98" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="99" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="100" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="101" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="102" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="103" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="104" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="105" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="106" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="107" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="108" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="109" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="110" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="111" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="112" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="97" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="98" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A98" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B98" s="1"/>
+      <c r="C98" s="1"/>
+      <c r="D98" s="1"/>
+      <c r="E98" s="1"/>
+      <c r="F98" s="1"/>
+      <c r="G98" s="1"/>
+      <c r="H98" s="1"/>
+      <c r="I98" s="1"/>
+      <c r="J98" s="1"/>
+      <c r="K98" s="1"/>
+      <c r="L98" s="1"/>
+      <c r="M98" s="1"/>
+      <c r="N98" s="1"/>
+      <c r="O98" s="1"/>
+      <c r="P98" s="1"/>
+    </row>
+    <row r="99" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A99" s="23" t="s">
+        <v>202</v>
+      </c>
+      <c r="B99" s="23" t="s">
+        <v>203</v>
+      </c>
+      <c r="C99" s="23" t="s">
+        <v>204</v>
+      </c>
+      <c r="D99" s="23" t="s">
+        <v>205</v>
+      </c>
+      <c r="E99" s="23" t="s">
+        <v>206</v>
+      </c>
+      <c r="F99" s="23" t="s">
+        <v>207</v>
+      </c>
+      <c r="G99" s="23" t="s">
+        <v>208</v>
+      </c>
+      <c r="H99" s="23" t="s">
+        <v>209</v>
+      </c>
+      <c r="I99" s="23" t="s">
+        <v>210</v>
+      </c>
+      <c r="J99" s="23" t="s">
+        <v>211</v>
+      </c>
+      <c r="K99" s="23" t="s">
+        <v>212</v>
+      </c>
+      <c r="L99" s="23" t="s">
+        <v>213</v>
+      </c>
+      <c r="M99" s="23" t="s">
+        <v>214</v>
+      </c>
+      <c r="N99" s="23" t="s">
+        <v>215</v>
+      </c>
+      <c r="O99" s="23" t="s">
+        <v>216</v>
+      </c>
+      <c r="P99" s="23" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="100" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A100" s="25" t="s">
+        <v>218</v>
+      </c>
+      <c r="B100" s="25" t="s">
+        <v>219</v>
+      </c>
+      <c r="C100" s="25" t="s">
+        <v>220</v>
+      </c>
+      <c r="D100" s="25" t="s">
+        <v>221</v>
+      </c>
+      <c r="E100" s="25" t="s">
+        <v>222</v>
+      </c>
+      <c r="F100" s="25" t="s">
+        <v>223</v>
+      </c>
+      <c r="G100" s="25" t="s">
+        <v>224</v>
+      </c>
+      <c r="H100" s="25" t="s">
+        <v>225</v>
+      </c>
+      <c r="I100" s="25" t="s">
+        <v>226</v>
+      </c>
+      <c r="J100" s="25" t="s">
+        <v>227</v>
+      </c>
+      <c r="K100" s="25" t="s">
+        <v>228</v>
+      </c>
+      <c r="L100" s="25" t="s">
+        <v>229</v>
+      </c>
+      <c r="M100" s="25" t="s">
+        <v>230</v>
+      </c>
+      <c r="N100" s="25" t="s">
+        <v>231</v>
+      </c>
+      <c r="O100" s="25" t="s">
+        <v>232</v>
+      </c>
+      <c r="P100" s="25" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="101" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="102" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="103" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="104" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="105" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="106" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="107" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="108" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="109" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="110" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="111" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="112" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="113" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="114" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="115" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -19316,22 +19584,69 @@
     <row r="158" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="159" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="160" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="161" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="162" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="163" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="164" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="165" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="166" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="167" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="168" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="169" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="170" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="171" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="172" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="173" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="174" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="175" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="176" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="161" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="162" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="163" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="164" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="165" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="166" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="167" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="168" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="169" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="170" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="171" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A171" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="B171" s="1"/>
+      <c r="C171" s="1"/>
+      <c r="D171" s="1"/>
+      <c r="E171" s="1"/>
+      <c r="F171" s="1"/>
+    </row>
+    <row r="172" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A172" s="23" t="s">
+        <v>234</v>
+      </c>
+      <c r="B172" s="23" t="s">
+        <v>235</v>
+      </c>
+      <c r="C172" s="23" t="s">
+        <v>236</v>
+      </c>
+      <c r="D172" s="23" t="s">
+        <v>237</v>
+      </c>
+      <c r="E172" s="23" t="s">
+        <v>238</v>
+      </c>
+      <c r="F172" s="23" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="173" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A173" s="25" t="s">
+        <v>240</v>
+      </c>
+      <c r="B173" s="25" t="s">
+        <v>241</v>
+      </c>
+      <c r="C173" s="25" t="s">
+        <v>242</v>
+      </c>
+      <c r="D173" s="25" t="s">
+        <v>243</v>
+      </c>
+      <c r="E173" s="25" t="s">
+        <v>244</v>
+      </c>
+      <c r="F173" s="25" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="174" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="175" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="176" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="177" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="178" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="179" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -20197,13 +20512,6 @@
     <row r="1039" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="1040" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="1041" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="1042" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="1043" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="1044" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="1045" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="1046" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="1047" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="1048" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:A4"/>
@@ -20224,7 +20532,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView zoomScale="98" zoomScaleNormal="98" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -20235,12 +20543,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="13" x14ac:dyDescent="0.3">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="50" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="26" t="s">
@@ -20288,7 +20596,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -20299,11 +20607,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="13" x14ac:dyDescent="0.3">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="51" t="s">
         <v>79</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="26" t="s">
@@ -20350,7 +20658,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -20361,11 +20669,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="52" t="s">
         <v>85</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="26" t="s">
@@ -20411,7 +20719,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView zoomScalePageLayoutView="60" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScalePageLayoutView="60" workbookViewId="0">
       <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
@@ -20423,11 +20731,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="52" t="s">
         <v>91</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="26" t="s">
@@ -20473,8 +20781,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -20485,11 +20793,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="52" t="s">
         <v>96</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
@@ -20535,8 +20843,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -20547,11 +20855,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="52" t="s">
         <v>101</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
@@ -20598,7 +20906,7 @@
   <dimension ref="A1:T94"/>
   <sheetViews>
     <sheetView zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection sqref="A1:K1"/>
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -20609,19 +20917,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="52" t="s">
         <v>106</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
-      <c r="K1" s="54"/>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="52"/>
+      <c r="H1" s="52"/>
+      <c r="I1" s="52"/>
+      <c r="J1" s="52"/>
+      <c r="K1" s="52"/>
       <c r="L1" s="30"/>
       <c r="M1" s="30"/>
       <c r="N1" s="30"/>
@@ -20867,10 +21175,10 @@
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" s="55" t="s">
+      <c r="A93" s="53" t="s">
         <v>192</v>
       </c>
-      <c r="B93" s="56"/>
+      <c r="B93" s="54"/>
       <c r="C93" s="42"/>
       <c r="D93" s="42"/>
     </row>
@@ -20897,117 +21205,112 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03DDC5C3-BD6D-444D-BAD4-1FA02546E2E3}">
-  <dimension ref="A1:L4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34BFAF30-6EFD-4A13-A39A-D09455CAAF60}">
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.453125" customWidth="1"/>
-    <col min="2" max="2" width="11.90625" customWidth="1"/>
-    <col min="3" max="3" width="17.81640625" customWidth="1"/>
-    <col min="4" max="4" width="13.08984375" customWidth="1"/>
-    <col min="5" max="5" width="19" customWidth="1"/>
-    <col min="6" max="6" width="15.1796875" customWidth="1"/>
-    <col min="7" max="7" width="21.7265625" customWidth="1"/>
-    <col min="8" max="8" width="14.6328125" customWidth="1"/>
-    <col min="9" max="9" width="14.36328125" customWidth="1"/>
-    <col min="10" max="10" width="20" customWidth="1"/>
+    <col min="1" max="1" width="14.08984375" customWidth="1"/>
+    <col min="2" max="2" width="12" customWidth="1"/>
+    <col min="3" max="3" width="15.36328125" customWidth="1"/>
+    <col min="4" max="4" width="13.6328125" customWidth="1"/>
+    <col min="5" max="5" width="19.81640625" customWidth="1"/>
+    <col min="6" max="6" width="14.453125" customWidth="1"/>
+    <col min="7" max="7" width="21.26953125" customWidth="1"/>
+    <col min="8" max="8" width="17.08984375" customWidth="1"/>
+    <col min="9" max="9" width="14.08984375" customWidth="1"/>
+    <col min="10" max="10" width="22.08984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="58" t="s">
-        <v>215</v>
-      </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-      <c r="E1" s="59"/>
-      <c r="F1" s="59"/>
-      <c r="G1" s="59"/>
-      <c r="H1" s="59"/>
-      <c r="I1" s="59"/>
-      <c r="J1" s="59"/>
+      <c r="A1" s="55" t="s">
+        <v>246</v>
+      </c>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
+      <c r="J1" s="56"/>
     </row>
     <row r="2" spans="1:12" ht="13" x14ac:dyDescent="0.3">
-      <c r="A2" s="47" t="s">
-        <v>195</v>
-      </c>
-      <c r="B2" s="47" t="s">
-        <v>204</v>
-      </c>
-      <c r="C2" s="47" t="s">
-        <v>196</v>
-      </c>
-      <c r="D2" s="47" t="s">
-        <v>197</v>
-      </c>
-      <c r="E2" s="47" t="s">
-        <v>198</v>
-      </c>
-      <c r="F2" s="47" t="s">
-        <v>199</v>
-      </c>
-      <c r="G2" s="47" t="s">
-        <v>200</v>
-      </c>
-      <c r="H2" s="47" t="s">
-        <v>201</v>
-      </c>
-      <c r="I2" s="47" t="s">
-        <v>202</v>
-      </c>
-      <c r="J2" s="47" t="s">
-        <v>203</v>
-      </c>
-      <c r="K2" s="47"/>
-      <c r="L2" s="47"/>
+      <c r="A2" s="57" t="s">
+        <v>247</v>
+      </c>
+      <c r="B2" s="57" t="s">
+        <v>248</v>
+      </c>
+      <c r="C2" s="57" t="s">
+        <v>249</v>
+      </c>
+      <c r="D2" s="57" t="s">
+        <v>250</v>
+      </c>
+      <c r="E2" s="57" t="s">
+        <v>251</v>
+      </c>
+      <c r="F2" s="57" t="s">
+        <v>252</v>
+      </c>
+      <c r="G2" s="57" t="s">
+        <v>253</v>
+      </c>
+      <c r="H2" s="57" t="s">
+        <v>254</v>
+      </c>
+      <c r="I2" s="57" t="s">
+        <v>255</v>
+      </c>
+      <c r="J2" s="57" t="s">
+        <v>256</v>
+      </c>
+      <c r="K2" s="57"/>
+      <c r="L2" s="57"/>
     </row>
     <row r="3" spans="1:12" ht="15.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="57" t="s">
-        <v>209</v>
-      </c>
-      <c r="B3" s="60" t="s">
-        <v>208</v>
-      </c>
-      <c r="C3" s="61" t="s">
-        <v>210</v>
-      </c>
-      <c r="D3" s="57" t="s">
-        <v>205</v>
-      </c>
-      <c r="E3" s="60" t="s">
-        <v>206</v>
-      </c>
-      <c r="F3" s="60" t="s">
-        <v>207</v>
-      </c>
-      <c r="G3" s="60" t="s">
-        <v>211</v>
-      </c>
-      <c r="H3" s="62" t="s">
-        <v>213</v>
-      </c>
-      <c r="I3" s="62" t="s">
-        <v>214</v>
-      </c>
-      <c r="J3" s="60" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="48"/>
-      <c r="D4" s="48"/>
+      <c r="A3" s="58" t="s">
+        <v>257</v>
+      </c>
+      <c r="B3" s="59" t="s">
+        <v>258</v>
+      </c>
+      <c r="C3" s="60" t="s">
+        <v>259</v>
+      </c>
+      <c r="D3" s="58" t="s">
+        <v>260</v>
+      </c>
+      <c r="E3" s="59" t="s">
+        <v>261</v>
+      </c>
+      <c r="F3" s="59" t="s">
+        <v>262</v>
+      </c>
+      <c r="G3" s="59" t="s">
+        <v>263</v>
+      </c>
+      <c r="H3" s="59" t="s">
+        <v>264</v>
+      </c>
+      <c r="I3" s="59" t="s">
+        <v>265</v>
+      </c>
+      <c r="J3" s="59" t="s">
+        <v>266</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:J1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
POCOR-6742|added extra columns into the profile template|status:ReadyToDeploy
</commit_message>
<xml_diff>
--- a/webroot/export/customexcel/default_templates/profile_template.xlsx
+++ b/webroot/export/customexcel/default_templates/profile_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\pocor-openemis-core\webroot\export\customexcel\default_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8157E890-A340-480A-9465-E098DB6A3348}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D45714BD-D685-4143-BC83-2815F86A7534}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="933" firstSheet="4" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="862" firstSheet="4" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -109,7 +109,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="280">
   <si>
     <t>${"image":{"displayValue":"Institutions.logo_content","imageWidth":"100","imageMarginLeft":"20","imageMarginTop":"5"}}</t>
   </si>
@@ -938,13 +938,25 @@
   </si>
   <si>
     <t xml:space="preserve">${"match": {"displayValue": "InstitutionRoomsArea.area_level:3","rows": {"matchFrom": "InstitutionRooms.id","matchTo": "InstitutionRooms.id"}}} </t>
+  </si>
+  <si>
+    <t>Institution Average Mark</t>
+  </si>
+  <si>
+    <t>Area Average Mark</t>
+  </si>
+  <si>
+    <t>${"match": {"displayValue": "StudentDetails.institution_average_mark","rows": {"matchFrom": "StudentDetails.id","matchTo": "StudentDetails.id"}}}</t>
+  </si>
+  <si>
+    <t>${"match": {"displayValue": "StudentDetails.area_average_mark","rows": {"matchFrom": "StudentDetails.id","matchTo": "StudentDetails.id"}}}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1039,6 +1051,28 @@
       <sz val="10"/>
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -1164,7 +1198,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1271,6 +1305,15 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1295,21 +1338,21 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1740,7 +1783,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="53" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4"/>
@@ -1761,13 +1804,13 @@
       <c r="Q1" s="7"/>
     </row>
     <row r="2" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="48"/>
-      <c r="B2" s="49" t="s">
+      <c r="A2" s="53"/>
+      <c r="B2" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
       <c r="F2" s="8"/>
       <c r="G2" s="9"/>
       <c r="H2" s="7"/>
@@ -2021,13 +2064,13 @@
       <c r="IV2" s="3"/>
     </row>
     <row r="3" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="48"/>
-      <c r="B3" s="50" t="s">
+      <c r="A3" s="53"/>
+      <c r="B3" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
-      <c r="E3" s="50"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="55"/>
       <c r="F3" s="9"/>
       <c r="G3" s="9"/>
       <c r="H3" s="7"/>
@@ -2281,7 +2324,7 @@
       <c r="IV3" s="3"/>
     </row>
     <row r="4" spans="1:256" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="48"/>
+      <c r="A4" s="53"/>
       <c r="B4" s="4"/>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
@@ -20568,12 +20611,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="13" x14ac:dyDescent="0.3">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="56" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="26" t="s">
@@ -20632,11 +20675,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="13" x14ac:dyDescent="0.3">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="57" t="s">
         <v>79</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="26" t="s">
@@ -20694,11 +20737,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="58" t="s">
         <v>85</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="26" t="s">
@@ -20756,11 +20799,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="58" t="s">
         <v>91</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="26" t="s">
@@ -20818,11 +20861,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="58" t="s">
         <v>96</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
@@ -20880,11 +20923,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="58" t="s">
         <v>101</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
@@ -20930,7 +20973,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:T125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" zoomScalePageLayoutView="60" workbookViewId="0">
+    <sheetView topLeftCell="A106" zoomScalePageLayoutView="60" workbookViewId="0">
       <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
@@ -20942,19 +20985,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="58" t="s">
         <v>106</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
-      <c r="I1" s="53"/>
-      <c r="J1" s="53"/>
-      <c r="K1" s="53"/>
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+      <c r="G1" s="58"/>
+      <c r="H1" s="58"/>
+      <c r="I1" s="58"/>
+      <c r="J1" s="58"/>
+      <c r="K1" s="58"/>
       <c r="L1" s="43"/>
       <c r="M1" s="43"/>
       <c r="N1" s="43"/>
@@ -21101,13 +21144,13 @@
       <c r="A16" s="41" t="s">
         <v>171</v>
       </c>
-      <c r="B16" s="58" t="s">
+      <c r="B16" s="48" t="s">
         <v>172</v>
       </c>
-      <c r="C16" s="58" t="s">
+      <c r="C16" s="48" t="s">
         <v>173</v>
       </c>
-      <c r="D16" s="58" t="s">
+      <c r="D16" s="48" t="s">
         <v>174</v>
       </c>
     </row>
@@ -21123,13 +21166,13 @@
       <c r="A29" s="41" t="s">
         <v>171</v>
       </c>
-      <c r="B29" s="58" t="s">
+      <c r="B29" s="48" t="s">
         <v>177</v>
       </c>
-      <c r="C29" s="58" t="s">
+      <c r="C29" s="48" t="s">
         <v>178</v>
       </c>
-      <c r="D29" s="58" t="s">
+      <c r="D29" s="48" t="s">
         <v>179</v>
       </c>
     </row>
@@ -21145,13 +21188,13 @@
       <c r="A45" s="41" t="s">
         <v>171</v>
       </c>
-      <c r="B45" s="58" t="s">
+      <c r="B45" s="48" t="s">
         <v>181</v>
       </c>
-      <c r="C45" s="58" t="s">
+      <c r="C45" s="48" t="s">
         <v>182</v>
       </c>
-      <c r="D45" s="58" t="s">
+      <c r="D45" s="48" t="s">
         <v>183</v>
       </c>
     </row>
@@ -21164,22 +21207,22 @@
       <c r="D58" s="40"/>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A59" s="59" t="s">
+      <c r="A59" s="49" t="s">
         <v>171</v>
       </c>
-      <c r="B59" s="60" t="s">
+      <c r="B59" s="50" t="s">
         <v>268</v>
       </c>
-      <c r="C59" s="60" t="s">
+      <c r="C59" s="50" t="s">
         <v>269</v>
       </c>
-      <c r="D59" s="60" t="s">
+      <c r="D59" s="50" t="s">
         <v>270</v>
       </c>
-      <c r="E59" s="61"/>
-      <c r="F59" s="61"/>
-      <c r="G59" s="61"/>
-      <c r="H59" s="61"/>
+      <c r="E59" s="51"/>
+      <c r="F59" s="51"/>
+      <c r="G59" s="51"/>
+      <c r="H59" s="51"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="40" t="s">
@@ -21193,13 +21236,13 @@
       <c r="A72" s="41" t="s">
         <v>171</v>
       </c>
-      <c r="B72" s="58" t="s">
+      <c r="B72" s="48" t="s">
         <v>184</v>
       </c>
-      <c r="C72" s="58" t="s">
+      <c r="C72" s="48" t="s">
         <v>185</v>
       </c>
-      <c r="D72" s="58" t="s">
+      <c r="D72" s="48" t="s">
         <v>186</v>
       </c>
     </row>
@@ -21215,13 +21258,13 @@
       <c r="A94" s="41" t="s">
         <v>188</v>
       </c>
-      <c r="B94" s="58" t="s">
+      <c r="B94" s="48" t="s">
         <v>189</v>
       </c>
-      <c r="C94" s="58" t="s">
+      <c r="C94" s="48" t="s">
         <v>190</v>
       </c>
-      <c r="D94" s="58" t="s">
+      <c r="D94" s="48" t="s">
         <v>191</v>
       </c>
     </row>
@@ -21233,29 +21276,29 @@
       <c r="C109" s="40"/>
       <c r="D109" s="40"/>
     </row>
-    <row r="110" spans="1:8" s="62" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="59" t="s">
+    <row r="110" spans="1:8" s="52" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A110" s="49" t="s">
         <v>272</v>
       </c>
-      <c r="B110" s="60" t="s">
+      <c r="B110" s="50" t="s">
         <v>273</v>
       </c>
-      <c r="C110" s="60" t="s">
+      <c r="C110" s="50" t="s">
         <v>274</v>
       </c>
-      <c r="D110" s="60" t="s">
+      <c r="D110" s="50" t="s">
         <v>275</v>
       </c>
-      <c r="E110" s="61"/>
-      <c r="F110" s="61"/>
-      <c r="G110" s="61"/>
-      <c r="H110" s="61"/>
+      <c r="E110" s="51"/>
+      <c r="F110" s="51"/>
+      <c r="G110" s="51"/>
+      <c r="H110" s="51"/>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A124" s="54" t="s">
+      <c r="A124" s="59" t="s">
         <v>192</v>
       </c>
-      <c r="B124" s="55"/>
+      <c r="B124" s="60"/>
       <c r="C124" s="40"/>
       <c r="D124" s="40"/>
     </row>
@@ -21285,8 +21328,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34BFAF30-6EFD-4A13-A39A-D09455CAAF60}">
   <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -21300,22 +21343,26 @@
     <col min="7" max="7" width="21.26953125" customWidth="1"/>
     <col min="8" max="8" width="17.08984375" customWidth="1"/>
     <col min="9" max="9" width="14.08984375" customWidth="1"/>
-    <col min="10" max="10" width="22.08984375" customWidth="1"/>
+    <col min="10" max="10" width="19" customWidth="1"/>
+    <col min="11" max="11" width="16.26953125" customWidth="1"/>
+    <col min="12" max="12" width="21.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="63" t="s">
         <v>246</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
-      <c r="F1" s="57"/>
-      <c r="G1" s="57"/>
-      <c r="H1" s="57"/>
-      <c r="I1" s="57"/>
-      <c r="J1" s="57"/>
+      <c r="B1" s="64"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="64"/>
+      <c r="F1" s="64"/>
+      <c r="G1" s="64"/>
+      <c r="H1" s="64"/>
+      <c r="I1" s="64"/>
+      <c r="J1" s="64"/>
+      <c r="K1" s="64"/>
+      <c r="L1" s="64"/>
     </row>
     <row r="2" spans="1:12" ht="13" x14ac:dyDescent="0.3">
       <c r="A2" s="44" t="s">
@@ -21345,11 +21392,15 @@
       <c r="I2" s="44" t="s">
         <v>255</v>
       </c>
-      <c r="J2" s="44" t="s">
+      <c r="J2" s="61" t="s">
+        <v>276</v>
+      </c>
+      <c r="K2" s="62" t="s">
+        <v>277</v>
+      </c>
+      <c r="L2" s="44" t="s">
         <v>256</v>
       </c>
-      <c r="K2" s="44"/>
-      <c r="L2" s="44"/>
     </row>
     <row r="3" spans="1:12" ht="15.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="45" t="s">
@@ -21380,12 +21431,18 @@
         <v>265</v>
       </c>
       <c r="J3" s="46" t="s">
+        <v>278</v>
+      </c>
+      <c r="K3" s="65" t="s">
+        <v>279</v>
+      </c>
+      <c r="L3" s="65" t="s">
         <v>266</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A1:L1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>

<commit_message>
POCOR-7272 \plugins>CustomExcel>src>Model>Table>InstitutionReportCardsTable.php worked on 2 placeholders(1 and 3) |Status:Inprogress
</commit_message>
<xml_diff>
--- a/webroot/export/customexcel/default_templates/profile_template.xlsx
+++ b/webroot/export/customexcel/default_templates/profile_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20361"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\pocor-openemis-core\webroot\export\customexcel\default_templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp2\htdocs\pocor-openemis-core\webroot\export\customexcel\default_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D45714BD-D685-4143-BC83-2815F86A7534}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C1E7BF6-5D52-4CA0-BB63-52E7AD6BD661}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="862" firstSheet="4" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10305" tabRatio="862" firstSheet="4" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -109,7 +109,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="282">
   <si>
     <t>${"image":{"displayValue":"Institutions.logo_content","imageWidth":"100","imageMarginLeft":"20","imageMarginTop":"5"}}</t>
   </si>
@@ -950,6 +950,13 @@
   </si>
   <si>
     <t>${"match": {"displayValue": "StudentDetails.area_average_mark","rows": {"matchFrom": "StudentDetails.id","matchTo": "StudentDetails.id"}}}</t>
+  </si>
+  <si>
+    <t>Percentage of Jordan Students</t>
+  </si>
+  <si>
+    <t>${"match": {"displayValue": "StudentFromEducationGrade.jordan_students","rows": {"matchFrom": "StudentFromEducationGrade.education_grade_id","matchTo": "StudentFromEducationGrade.education_grade_id"}
+}}</t>
   </si>
 </sst>
 </file>
@@ -1198,7 +1205,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1314,6 +1321,15 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1338,20 +1354,17 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1765,25 +1778,25 @@
       <selection activeCell="A168" sqref="A168"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="63.1796875" customWidth="1"/>
-    <col min="2" max="2" width="54.26953125" customWidth="1"/>
+    <col min="1" max="1" width="63.140625" customWidth="1"/>
+    <col min="2" max="2" width="54.28515625" customWidth="1"/>
     <col min="3" max="3" width="53" customWidth="1"/>
-    <col min="4" max="4" width="24.26953125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="61.26953125" customWidth="1"/>
-    <col min="6" max="6" width="51.81640625" customWidth="1"/>
+    <col min="4" max="4" width="24.28515625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="61.28515625" customWidth="1"/>
+    <col min="6" max="6" width="51.85546875" customWidth="1"/>
     <col min="7" max="7" width="58" customWidth="1"/>
     <col min="8" max="8" width="40" customWidth="1"/>
-    <col min="9" max="18" width="39.453125" customWidth="1"/>
-    <col min="19" max="27" width="41.81640625" customWidth="1"/>
-    <col min="28" max="256" width="39.7265625" customWidth="1"/>
-    <col min="257" max="1023" width="16.1796875" customWidth="1"/>
-    <col min="1024" max="1025" width="11.7265625" customWidth="1"/>
+    <col min="9" max="18" width="39.42578125" customWidth="1"/>
+    <col min="19" max="27" width="41.85546875" customWidth="1"/>
+    <col min="28" max="256" width="39.7109375" customWidth="1"/>
+    <col min="257" max="1023" width="16.140625" customWidth="1"/>
+    <col min="1024" max="1025" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="53" t="s">
+    <row r="1" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="56" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4"/>
@@ -1803,14 +1816,14 @@
       <c r="P1" s="7"/>
       <c r="Q1" s="7"/>
     </row>
-    <row r="2" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="53"/>
-      <c r="B2" s="54" t="s">
+    <row r="2" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="56"/>
+      <c r="B2" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
       <c r="F2" s="8"/>
       <c r="G2" s="9"/>
       <c r="H2" s="7"/>
@@ -2063,14 +2076,14 @@
       <c r="IU2" s="3"/>
       <c r="IV2" s="3"/>
     </row>
-    <row r="3" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="53"/>
-      <c r="B3" s="55" t="s">
+    <row r="3" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="56"/>
+      <c r="B3" s="58" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="55"/>
-      <c r="D3" s="55"/>
-      <c r="E3" s="55"/>
+      <c r="C3" s="58"/>
+      <c r="D3" s="58"/>
+      <c r="E3" s="58"/>
       <c r="F3" s="9"/>
       <c r="G3" s="9"/>
       <c r="H3" s="7"/>
@@ -2323,8 +2336,8 @@
       <c r="IU3" s="3"/>
       <c r="IV3" s="3"/>
     </row>
-    <row r="4" spans="1:256" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="53"/>
+    <row r="4" spans="1:256" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="56"/>
       <c r="B4" s="4"/>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
@@ -2342,7 +2355,7 @@
       <c r="P4" s="7"/>
       <c r="Q4" s="7"/>
     </row>
-    <row r="5" spans="1:256" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:256" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="10"/>
       <c r="B5" s="10"/>
       <c r="C5" s="10"/>
@@ -2362,7 +2375,7 @@
       <c r="Q5" s="7"/>
       <c r="R5" s="7"/>
     </row>
-    <row r="6" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>3</v>
       </c>
@@ -2386,7 +2399,7 @@
       <c r="Q6" s="7"/>
       <c r="R6" s="7"/>
     </row>
-    <row r="7" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>5</v>
       </c>
@@ -2410,7 +2423,7 @@
       <c r="Q7" s="7"/>
       <c r="R7" s="7"/>
     </row>
-    <row r="8" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>7</v>
       </c>
@@ -2434,7 +2447,7 @@
       <c r="Q8" s="7"/>
       <c r="R8" s="7"/>
     </row>
-    <row r="9" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>9</v>
       </c>
@@ -2458,7 +2471,7 @@
       <c r="Q9" s="7"/>
       <c r="R9" s="7"/>
     </row>
-    <row r="10" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>11</v>
       </c>
@@ -2482,7 +2495,7 @@
       <c r="Q10" s="7"/>
       <c r="R10" s="7"/>
     </row>
-    <row r="11" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
         <v>13</v>
       </c>
@@ -2744,7 +2757,7 @@
       <c r="IU11" s="3"/>
       <c r="IV11" s="3"/>
     </row>
-    <row r="12" spans="1:256" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:256" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="16"/>
       <c r="B12" s="16"/>
       <c r="C12" s="16"/>
@@ -3002,7 +3015,7 @@
       <c r="IU12" s="3"/>
       <c r="IV12" s="3"/>
     </row>
-    <row r="13" spans="1:256" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:256" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
         <v>15</v>
       </c>
@@ -3264,7 +3277,7 @@
       <c r="IU13" s="3"/>
       <c r="IV13" s="3"/>
     </row>
-    <row r="14" spans="1:256" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:256" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
         <v>17</v>
       </c>
@@ -3526,7 +3539,7 @@
       <c r="IU14" s="3"/>
       <c r="IV14" s="3"/>
     </row>
-    <row r="15" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
         <v>19</v>
       </c>
@@ -3788,7 +3801,7 @@
       <c r="IU15" s="3"/>
       <c r="IV15" s="3"/>
     </row>
-    <row r="16" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
         <v>21</v>
       </c>
@@ -4050,7 +4063,7 @@
       <c r="IU16" s="3"/>
       <c r="IV16" s="3"/>
     </row>
-    <row r="17" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
         <v>23</v>
       </c>
@@ -4312,7 +4325,7 @@
       <c r="IU17" s="3"/>
       <c r="IV17" s="3"/>
     </row>
-    <row r="18" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
         <v>25</v>
       </c>
@@ -4574,7 +4587,7 @@
       <c r="IU18" s="3"/>
       <c r="IV18" s="3"/>
     </row>
-    <row r="19" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
         <v>27</v>
       </c>
@@ -4836,7 +4849,7 @@
       <c r="IU19" s="3"/>
       <c r="IV19" s="3"/>
     </row>
-    <row r="20" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>15</v>
       </c>
@@ -5098,7 +5111,7 @@
       <c r="IU20" s="3"/>
       <c r="IV20" s="3"/>
     </row>
-    <row r="21" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
         <v>29</v>
       </c>
@@ -5360,7 +5373,7 @@
       <c r="IU21" s="3"/>
       <c r="IV21" s="3"/>
     </row>
-    <row r="22" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
         <v>164</v>
       </c>
@@ -5622,7 +5635,7 @@
       <c r="IU22" s="3"/>
       <c r="IV22" s="3"/>
     </row>
-    <row r="23" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
         <v>166</v>
       </c>
@@ -5884,7 +5897,7 @@
       <c r="IU23" s="3"/>
       <c r="IV23" s="3"/>
     </row>
-    <row r="24" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
         <v>168</v>
       </c>
@@ -6146,7 +6159,7 @@
       <c r="IU24" s="3"/>
       <c r="IV24" s="3"/>
     </row>
-    <row r="25" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="39"/>
       <c r="B25" s="39"/>
       <c r="C25" s="37"/>
@@ -6404,7 +6417,7 @@
       <c r="IU25" s="3"/>
       <c r="IV25" s="3"/>
     </row>
-    <row r="26" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="39"/>
       <c r="B26" s="39"/>
       <c r="C26" s="37"/>
@@ -6662,7 +6675,7 @@
       <c r="IU26" s="3"/>
       <c r="IV26" s="3"/>
     </row>
-    <row r="27" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>31</v>
       </c>
@@ -6922,7 +6935,7 @@
       <c r="IU27" s="3"/>
       <c r="IV27" s="3"/>
     </row>
-    <row r="28" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
         <v>32</v>
       </c>
@@ -7186,7 +7199,7 @@
       <c r="IU28" s="3"/>
       <c r="IV28" s="3"/>
     </row>
-    <row r="29" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
         <v>35</v>
       </c>
@@ -7450,7 +7463,7 @@
       <c r="IU29" s="3"/>
       <c r="IV29" s="3"/>
     </row>
-    <row r="30" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="7"/>
       <c r="B30" s="7"/>
       <c r="C30" s="7"/>
@@ -7708,7 +7721,7 @@
       <c r="IU30" s="3"/>
       <c r="IV30" s="3"/>
     </row>
-    <row r="31" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="7"/>
       <c r="B31" s="7"/>
       <c r="C31" s="7"/>
@@ -7966,7 +7979,7 @@
       <c r="IU31" s="3"/>
       <c r="IV31" s="3"/>
     </row>
-    <row r="32" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="20" t="s">
         <v>38</v>
       </c>
@@ -8228,7 +8241,7 @@
       <c r="IU32" s="3"/>
       <c r="IV32" s="3"/>
     </row>
-    <row r="33" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="20" t="s">
         <v>40</v>
       </c>
@@ -8490,7 +8503,7 @@
       <c r="IU33" s="3"/>
       <c r="IV33" s="3"/>
     </row>
-    <row r="34" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="17"/>
       <c r="B34" s="18"/>
       <c r="C34" s="18"/>
@@ -8748,7 +8761,7 @@
       <c r="IU34" s="3"/>
       <c r="IV34" s="3"/>
     </row>
-    <row r="35" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="17"/>
       <c r="B35" s="18"/>
       <c r="C35" s="18"/>
@@ -9006,7 +9019,7 @@
       <c r="IU35" s="3"/>
       <c r="IV35" s="3"/>
     </row>
-    <row r="36" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="20" t="s">
         <v>42</v>
       </c>
@@ -9268,7 +9281,7 @@
       <c r="IU36" s="3"/>
       <c r="IV36" s="3"/>
     </row>
-    <row r="37" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="20" t="s">
         <v>44</v>
       </c>
@@ -9530,7 +9543,7 @@
       <c r="IU37" s="3"/>
       <c r="IV37" s="3"/>
     </row>
-    <row r="38" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="17"/>
       <c r="B38" s="18"/>
       <c r="C38" s="18"/>
@@ -9788,7 +9801,7 @@
       <c r="IU38" s="3"/>
       <c r="IV38" s="3"/>
     </row>
-    <row r="39" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="17"/>
       <c r="B39" s="18"/>
       <c r="C39" s="18"/>
@@ -10046,7 +10059,7 @@
       <c r="IU39" s="3"/>
       <c r="IV39" s="3"/>
     </row>
-    <row r="40" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="21" t="s">
         <v>46</v>
       </c>
@@ -10308,7 +10321,7 @@
       <c r="IU40" s="3"/>
       <c r="IV40" s="3"/>
     </row>
-    <row r="41" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="21" t="s">
         <v>48</v>
       </c>
@@ -10570,7 +10583,7 @@
       <c r="IU41" s="3"/>
       <c r="IV41" s="3"/>
     </row>
-    <row r="42" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="17"/>
       <c r="B42" s="18"/>
       <c r="C42" s="18"/>
@@ -10828,7 +10841,7 @@
       <c r="IU42" s="3"/>
       <c r="IV42" s="3"/>
     </row>
-    <row r="43" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="17"/>
       <c r="B43" s="18"/>
       <c r="C43" s="18"/>
@@ -11086,7 +11099,7 @@
       <c r="IU43" s="3"/>
       <c r="IV43" s="3"/>
     </row>
-    <row r="44" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="11" t="s">
         <v>50</v>
       </c>
@@ -11348,7 +11361,7 @@
       <c r="IU44" s="3"/>
       <c r="IV44" s="3"/>
     </row>
-    <row r="45" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="11" t="s">
         <v>52</v>
       </c>
@@ -11610,7 +11623,7 @@
       <c r="IU45" s="3"/>
       <c r="IV45" s="3"/>
     </row>
-    <row r="46" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="11" t="s">
         <v>54</v>
       </c>
@@ -11872,7 +11885,7 @@
       <c r="IU46" s="3"/>
       <c r="IV46" s="3"/>
     </row>
-    <row r="47" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="11" t="s">
         <v>56</v>
       </c>
@@ -12134,7 +12147,7 @@
       <c r="IU47" s="3"/>
       <c r="IV47" s="3"/>
     </row>
-    <row r="48" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="11" t="s">
         <v>58</v>
       </c>
@@ -12396,7 +12409,7 @@
       <c r="IU48" s="3"/>
       <c r="IV48" s="3"/>
     </row>
-    <row r="49" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="11" t="s">
         <v>60</v>
       </c>
@@ -12658,7 +12671,7 @@
       <c r="IU49" s="3"/>
       <c r="IV49" s="3"/>
     </row>
-    <row r="50" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="11" t="s">
         <v>62</v>
       </c>
@@ -12920,7 +12933,7 @@
       <c r="IU50" s="3"/>
       <c r="IV50" s="3"/>
     </row>
-    <row r="51" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="11" t="s">
         <v>64</v>
       </c>
@@ -13180,7 +13193,7 @@
       <c r="IU51" s="3"/>
       <c r="IV51" s="3"/>
     </row>
-    <row r="52" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="11" t="s">
         <v>65</v>
       </c>
@@ -13442,7 +13455,7 @@
       <c r="IU52" s="3"/>
       <c r="IV52" s="3"/>
     </row>
-    <row r="53" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="17"/>
       <c r="B53" s="18"/>
       <c r="C53" s="18"/>
@@ -13700,7 +13713,7 @@
       <c r="IU53" s="3"/>
       <c r="IV53" s="3"/>
     </row>
-    <row r="54" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="17"/>
       <c r="B54" s="18"/>
       <c r="C54" s="18"/>
@@ -13958,7 +13971,7 @@
       <c r="IU54" s="3"/>
       <c r="IV54" s="3"/>
     </row>
-    <row r="55" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>142</v>
       </c>
@@ -14218,7 +14231,7 @@
       <c r="IU55" s="3"/>
       <c r="IV55" s="3"/>
     </row>
-    <row r="56" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="33" t="s">
         <v>143</v>
       </c>
@@ -14482,7 +14495,7 @@
       <c r="IU56" s="3"/>
       <c r="IV56" s="3"/>
     </row>
-    <row r="57" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="34" t="s">
         <v>146</v>
       </c>
@@ -14746,7 +14759,7 @@
       <c r="IU57" s="3"/>
       <c r="IV57" s="3"/>
     </row>
-    <row r="58" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="34" t="s">
         <v>149</v>
       </c>
@@ -15010,7 +15023,7 @@
       <c r="IU58" s="3"/>
       <c r="IV58" s="3"/>
     </row>
-    <row r="59" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="34" t="s">
         <v>152</v>
       </c>
@@ -15274,7 +15287,7 @@
       <c r="IU59" s="3"/>
       <c r="IV59" s="3"/>
     </row>
-    <row r="60" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="34" t="s">
         <v>155</v>
       </c>
@@ -15538,7 +15551,7 @@
       <c r="IU60" s="3"/>
       <c r="IV60" s="3"/>
     </row>
-    <row r="61" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="17"/>
       <c r="B61" s="18"/>
       <c r="C61" s="18"/>
@@ -15796,7 +15809,7 @@
       <c r="IU61" s="3"/>
       <c r="IV61" s="3"/>
     </row>
-    <row r="62" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>67</v>
       </c>
@@ -16056,7 +16069,7 @@
       <c r="IU62" s="3"/>
       <c r="IV62" s="3"/>
     </row>
-    <row r="63" spans="1:256" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:256" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="23" t="s">
         <v>68</v>
       </c>
@@ -16080,7 +16093,7 @@
       <c r="Q63" s="7"/>
       <c r="R63" s="7"/>
     </row>
-    <row r="64" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="25" t="s">
         <v>70</v>
       </c>
@@ -16342,7 +16355,7 @@
       <c r="IU64" s="3"/>
       <c r="IV64" s="3"/>
     </row>
-    <row r="65" spans="1:256" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:256" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="3"/>
       <c r="B65" s="3"/>
       <c r="C65" s="7"/>
@@ -16600,7 +16613,7 @@
       <c r="IU65" s="3"/>
       <c r="IV65" s="3"/>
     </row>
-    <row r="66" spans="1:256" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:256" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="3"/>
       <c r="B66" s="3"/>
       <c r="C66" s="7"/>
@@ -16858,7 +16871,7 @@
       <c r="IU66" s="3"/>
       <c r="IV66" s="3"/>
     </row>
-    <row r="67" spans="1:256" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:256" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="3"/>
       <c r="B67" s="3"/>
       <c r="C67" s="7"/>
@@ -17116,7 +17129,7 @@
       <c r="IU67" s="3"/>
       <c r="IV67" s="3"/>
     </row>
-    <row r="68" spans="1:256" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:256" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="3"/>
       <c r="B68" s="3"/>
       <c r="C68" s="7"/>
@@ -17374,7 +17387,7 @@
       <c r="IU68" s="3"/>
       <c r="IV68" s="3"/>
     </row>
-    <row r="69" spans="1:256" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:256" x14ac:dyDescent="0.25">
       <c r="A69" s="3"/>
       <c r="B69" s="3"/>
       <c r="C69" s="7"/>
@@ -17632,7 +17645,7 @@
       <c r="IU69" s="3"/>
       <c r="IV69" s="3"/>
     </row>
-    <row r="70" spans="1:256" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:256" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="3"/>
       <c r="B70" s="3"/>
       <c r="C70" s="7"/>
@@ -17890,7 +17903,7 @@
       <c r="IU70" s="3"/>
       <c r="IV70" s="3"/>
     </row>
-    <row r="71" spans="1:256" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:256" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="3"/>
       <c r="B71" s="3"/>
       <c r="C71" s="3"/>
@@ -18148,7 +18161,7 @@
       <c r="IU71" s="3"/>
       <c r="IV71" s="3"/>
     </row>
-    <row r="72" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>195</v>
       </c>
@@ -18407,7 +18420,7 @@
       <c r="IU72" s="3"/>
       <c r="IV72" s="3"/>
     </row>
-    <row r="73" spans="1:256" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:256" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="23" t="s">
         <v>196</v>
       </c>
@@ -18668,7 +18681,7 @@
       <c r="IU73" s="3"/>
       <c r="IV73" s="3"/>
     </row>
-    <row r="74" spans="1:256" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:256" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="25" t="s">
         <v>198</v>
       </c>
@@ -18929,7 +18942,7 @@
       <c r="IU74" s="3"/>
       <c r="IV74" s="3"/>
     </row>
-    <row r="75" spans="1:256" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:256" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="3"/>
       <c r="B75" s="3"/>
       <c r="C75" s="3"/>
@@ -19186,7 +19199,7 @@
       <c r="IU75" s="3"/>
       <c r="IV75" s="3"/>
     </row>
-    <row r="76" spans="1:256" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:256" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E76" s="3"/>
       <c r="F76" s="3"/>
       <c r="G76" s="3"/>
@@ -19440,7 +19453,7 @@
       <c r="IU76" s="3"/>
       <c r="IV76" s="3"/>
     </row>
-    <row r="77" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I77" s="7"/>
       <c r="J77" s="7"/>
       <c r="K77" s="7"/>
@@ -19452,27 +19465,27 @@
       <c r="Q77" s="7"/>
       <c r="R77" s="7"/>
     </row>
-    <row r="78" spans="1:256" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="79" spans="1:256" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="80" spans="1:256" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="81" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="82" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="83" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="84" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="85" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="86" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="87" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="88" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="89" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="90" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="91" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="92" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="93" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="94" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="95" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="96" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="97" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="98" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:256" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="79" spans="1:256" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="80" spans="1:256" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="81" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="82" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="83" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="84" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="85" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="86" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="87" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="88" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="89" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="90" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="91" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="92" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="93" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="94" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="95" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="96" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="97" spans="1:16" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="98" spans="1:16" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
         <v>201</v>
       </c>
@@ -19492,7 +19505,7 @@
       <c r="O98" s="1"/>
       <c r="P98" s="1"/>
     </row>
-    <row r="99" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:16" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="23" t="s">
         <v>202</v>
       </c>
@@ -19542,7 +19555,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="100" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:16" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="25" t="s">
         <v>218</v>
       </c>
@@ -19592,77 +19605,77 @@
         <v>233</v>
       </c>
     </row>
-    <row r="101" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="102" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="103" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="104" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="105" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="106" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="107" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="108" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="109" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="110" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="111" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="112" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="113" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="114" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="115" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="116" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="117" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="118" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="119" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="120" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="121" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="122" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="123" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="124" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="125" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="126" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="127" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="128" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="129" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="130" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="131" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="132" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="133" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="134" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="135" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="136" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="137" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="138" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="139" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="140" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="141" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="142" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="143" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="144" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="145" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="146" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="147" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="148" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="149" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="150" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="151" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="152" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="153" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="154" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="155" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="156" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="157" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="158" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="159" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="160" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="161" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="162" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="163" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="164" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="165" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="166" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="167" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="168" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="169" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="170" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="171" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:16" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="102" spans="1:16" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="103" spans="1:16" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="104" spans="1:16" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="105" spans="1:16" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="106" spans="1:16" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="107" spans="1:16" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="108" spans="1:16" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="109" spans="1:16" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="110" spans="1:16" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="111" spans="1:16" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="112" spans="1:16" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="113" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="114" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="115" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="116" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="117" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="118" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="119" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="120" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="121" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="122" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="123" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="124" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="125" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="126" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="127" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="128" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="129" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="130" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="131" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="132" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="133" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="134" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="135" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="136" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="137" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="138" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="139" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="140" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="141" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="142" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="143" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="144" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="145" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="146" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="147" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="148" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="149" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="150" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="151" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="152" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="153" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="154" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="155" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="156" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="157" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="158" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="159" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="160" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="161" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="162" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="163" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="164" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="165" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="166" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="167" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="168" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="169" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="170" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="171" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A171" s="1" t="s">
         <v>200</v>
       </c>
@@ -19672,7 +19685,7 @@
       <c r="E171" s="1"/>
       <c r="F171" s="1"/>
     </row>
-    <row r="172" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A172" s="23" t="s">
         <v>234</v>
       </c>
@@ -19692,7 +19705,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="173" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A173" s="25" t="s">
         <v>240</v>
       </c>
@@ -19712,874 +19725,874 @@
         <v>245</v>
       </c>
     </row>
-    <row r="174" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="175" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="176" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="177" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="178" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="179" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="180" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="181" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="182" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="183" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="184" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="185" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="186" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="187" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="188" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="189" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="190" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="191" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="192" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="193" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="194" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="195" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="196" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="197" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="198" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="199" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="200" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="201" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="202" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="203" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="204" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="205" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="206" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="207" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="208" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="209" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="210" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="211" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="212" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="213" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="214" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="215" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="216" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="217" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="218" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="219" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="220" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="221" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="222" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="223" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="224" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="225" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="226" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="227" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="228" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="229" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="230" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="231" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="232" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="233" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="234" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="235" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="236" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="237" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="238" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="239" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="240" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="241" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="242" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="243" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="244" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="245" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="246" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="247" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="248" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="249" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="250" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="251" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="252" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="253" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="254" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="255" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="256" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="257" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="258" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="259" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="260" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="261" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="262" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="263" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="264" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="265" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="266" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="267" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="268" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="269" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="270" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="271" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="272" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="273" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="274" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="275" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="276" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="277" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="278" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="279" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="280" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="281" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="282" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="283" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="284" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="285" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="286" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="287" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="288" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="289" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="290" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="291" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="292" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="293" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="294" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="295" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="296" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="297" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="298" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="299" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="300" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="301" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="302" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="303" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="304" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="305" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="306" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="307" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="308" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="309" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="310" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="311" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="312" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="313" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="314" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="315" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="316" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="317" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="318" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="319" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="320" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="321" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="322" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="323" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="324" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="325" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="326" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="327" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="328" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="329" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="330" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="331" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="332" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="333" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="334" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="335" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="336" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="337" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="338" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="339" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="340" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="341" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="342" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="343" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="344" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="345" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="346" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="347" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="348" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="349" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="350" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="351" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="352" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="353" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="354" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="355" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="356" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="357" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="358" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="359" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="360" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="361" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="362" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="363" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="364" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="365" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="366" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="367" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="368" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="369" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="370" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="371" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="372" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="373" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="374" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="375" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="376" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="377" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="378" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="379" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="380" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="381" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="382" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="383" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="384" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="385" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="386" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="387" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="388" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="389" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="390" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="391" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="392" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="393" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="394" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="395" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="396" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="397" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="398" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="399" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="400" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="401" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="402" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="403" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="404" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="405" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="406" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="407" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="408" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="409" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="410" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="411" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="412" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="413" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="414" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="415" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="416" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="417" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="418" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="419" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="420" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="421" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="422" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="423" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="424" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="425" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="426" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="427" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="428" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="429" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="430" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="431" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="432" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="433" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="434" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="435" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="436" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="437" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="438" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="439" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="440" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="441" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="442" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="443" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="444" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="445" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="446" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="447" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="448" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="449" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="450" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="451" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="452" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="453" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="454" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="455" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="456" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="457" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="458" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="459" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="460" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="461" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="462" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="463" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="464" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="465" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="466" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="467" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="468" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="469" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="470" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="471" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="472" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="473" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="474" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="475" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="476" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="477" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="478" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="479" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="480" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="481" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="482" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="483" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="484" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="485" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="486" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="487" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="488" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="489" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="490" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="491" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="492" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="493" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="494" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="495" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="496" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="497" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="498" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="499" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="500" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="501" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="502" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="503" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="504" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="505" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="506" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="507" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="508" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="509" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="510" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="511" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="512" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="513" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="514" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="515" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="516" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="517" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="518" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="519" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="520" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="521" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="522" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="523" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="524" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="525" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="526" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="527" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="528" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="529" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="530" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="531" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="532" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="533" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="534" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="535" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="536" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="537" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="538" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="539" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="540" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="541" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="542" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="543" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="544" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="545" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="546" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="547" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="548" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="549" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="550" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="551" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="552" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="553" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="554" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="555" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="556" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="557" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="558" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="559" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="560" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="561" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="562" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="563" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="564" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="565" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="566" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="567" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="568" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="569" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="570" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="571" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="572" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="573" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="574" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="575" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="576" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="577" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="578" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="579" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="580" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="581" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="582" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="583" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="584" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="585" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="586" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="587" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="588" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="589" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="590" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="591" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="592" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="593" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="594" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="595" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="596" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="597" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="598" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="599" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="600" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="601" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="602" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="603" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="604" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="605" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="606" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="607" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="608" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="609" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="610" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="611" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="612" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="613" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="614" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="615" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="616" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="617" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="618" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="619" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="620" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="621" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="622" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="623" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="624" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="625" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="626" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="627" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="628" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="629" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="630" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="631" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="632" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="633" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="634" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="635" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="636" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="637" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="638" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="639" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="640" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="641" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="642" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="643" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="644" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="645" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="646" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="647" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="648" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="649" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="650" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="651" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="652" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="653" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="654" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="655" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="656" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="657" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="658" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="659" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="660" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="661" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="662" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="663" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="664" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="665" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="666" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="667" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="668" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="669" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="670" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="671" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="672" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="673" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="674" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="675" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="676" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="677" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="678" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="679" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="680" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="681" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="682" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="683" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="684" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="685" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="686" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="687" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="688" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="689" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="690" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="691" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="692" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="693" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="694" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="695" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="696" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="697" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="698" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="699" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="700" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="701" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="702" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="703" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="704" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="705" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="706" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="707" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="708" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="709" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="710" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="711" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="712" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="713" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="714" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="715" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="716" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="717" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="718" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="719" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="720" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="721" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="722" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="723" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="724" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="725" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="726" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="727" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="728" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="729" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="730" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="731" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="732" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="733" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="734" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="735" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="736" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="737" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="738" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="739" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="740" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="741" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="742" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="743" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="744" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="745" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="746" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="747" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="748" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="749" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="750" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="751" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="752" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="753" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="754" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="755" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="756" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="757" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="758" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="759" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="760" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="761" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="762" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="763" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="764" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="765" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="766" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="767" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="768" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="769" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="770" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="771" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="772" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="773" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="774" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="775" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="776" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="777" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="778" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="779" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="780" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="781" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="782" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="783" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="784" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="785" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="786" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="787" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="788" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="789" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="790" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="791" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="792" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="793" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="794" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="795" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="796" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="797" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="798" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="799" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="800" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="801" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="802" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="803" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="804" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="805" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="806" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="807" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="808" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="809" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="810" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="811" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="812" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="813" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="814" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="815" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="816" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="817" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="818" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="819" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="820" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="821" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="822" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="823" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="824" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="825" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="826" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="827" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="828" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="829" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="830" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="831" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="832" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="833" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="834" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="835" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="836" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="837" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="838" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="839" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="840" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="841" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="842" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="843" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="844" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="845" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="846" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="847" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="848" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="849" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="850" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="851" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="852" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="853" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="854" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="855" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="856" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="857" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="858" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="859" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="860" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="861" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="862" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="863" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="864" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="865" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="866" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="867" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="868" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="869" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="870" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="871" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="872" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="873" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="874" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="875" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="876" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="877" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="878" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="879" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="880" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="881" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="882" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="883" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="884" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="885" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="886" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="887" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="888" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="889" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="890" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="891" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="892" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="893" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="894" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="895" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="896" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="897" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="898" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="899" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="900" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="901" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="902" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="903" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="904" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="905" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="906" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="907" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="908" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="909" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="910" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="911" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="912" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="913" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="914" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="915" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="916" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="917" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="918" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="919" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="920" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="921" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="922" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="923" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="924" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="925" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="926" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="927" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="928" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="929" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="930" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="931" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="932" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="933" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="934" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="935" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="936" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="937" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="938" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="939" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="940" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="941" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="942" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="943" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="944" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="945" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="946" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="947" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="948" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="949" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="950" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="951" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="952" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="953" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="954" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="955" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="956" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="957" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="958" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="959" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="960" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="961" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="962" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="963" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="964" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="965" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="966" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="967" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="968" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="969" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="970" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="971" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="972" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="973" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="974" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="975" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="976" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="977" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="978" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="979" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="980" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="981" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="982" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="983" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="984" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="985" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="986" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="987" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="988" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="989" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="990" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="991" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="992" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="993" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="994" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="995" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="996" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="997" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="998" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="999" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="1000" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="1001" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="1002" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="1003" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="1004" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="1005" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="1006" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="1007" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="1008" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="1009" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="1010" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="1011" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="1012" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="1013" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="1014" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="1015" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="1016" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="1017" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="1018" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="1019" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="1020" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="1021" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="1022" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="1023" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="1024" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="1025" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="1026" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="1027" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="1028" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="1029" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="1030" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="1031" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="1032" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="1033" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="1034" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="1035" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="1036" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="1037" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="1038" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="1039" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="1040" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="1041" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="174" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="175" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="176" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="177" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="178" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="179" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="180" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="181" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="182" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="183" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="184" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="185" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="186" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="187" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="188" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="189" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="190" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="191" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="192" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="193" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="194" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="195" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="196" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="197" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="198" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="199" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="200" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="201" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="202" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="203" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="204" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="205" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="206" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="207" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="208" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="209" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="210" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="211" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="212" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="213" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="214" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="215" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="216" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="217" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="218" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="219" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="220" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="221" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="222" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="223" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="224" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="225" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="226" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="227" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="228" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="229" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="230" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="231" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="232" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="233" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="234" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="235" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="236" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="237" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="238" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="239" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="240" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="241" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="242" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="243" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="244" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="245" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="246" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="247" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="248" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="249" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="250" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="251" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="252" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="253" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="254" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="255" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="256" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="257" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="258" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="259" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="260" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="261" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="262" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="263" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="264" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="265" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="266" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="267" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="268" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="269" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="270" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="271" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="272" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="273" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="274" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="275" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="276" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="277" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="278" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="279" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="280" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="281" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="282" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="283" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="284" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="285" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="286" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="287" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="288" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="289" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="290" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="291" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="292" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="293" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="294" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="295" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="296" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="297" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="298" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="299" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="300" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="301" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="302" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="303" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="304" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="305" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="306" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="307" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="308" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="309" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="310" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="311" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="312" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="313" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="314" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="315" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="316" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="317" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="318" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="319" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="320" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="321" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="322" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="323" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="324" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="325" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="326" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="327" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="328" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="329" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="330" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="331" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="332" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="333" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="334" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="335" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="336" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="337" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="338" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="339" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="340" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="341" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="342" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="343" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="344" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="345" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="346" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="347" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="348" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="349" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="350" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="351" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="352" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="353" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="354" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="355" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="356" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="357" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="358" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="359" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="360" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="361" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="362" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="363" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="364" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="365" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="366" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="367" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="368" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="369" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="370" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="371" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="372" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="373" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="374" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="375" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="376" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="377" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="378" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="379" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="380" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="381" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="382" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="383" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="384" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="385" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="386" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="387" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="388" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="389" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="390" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="391" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="392" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="393" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="394" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="395" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="396" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="397" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="398" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="399" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="400" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="401" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="402" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="403" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="404" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="405" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="406" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="407" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="408" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="409" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="410" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="411" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="412" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="413" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="414" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="415" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="416" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="417" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="418" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="419" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="420" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="421" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="422" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="423" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="424" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="425" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="426" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="427" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="428" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="429" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="430" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="431" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="432" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="433" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="434" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="435" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="436" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="437" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="438" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="439" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="440" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="441" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="442" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="443" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="444" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="445" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="446" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="447" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="448" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="449" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="450" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="451" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="452" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="453" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="454" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="455" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="456" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="457" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="458" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="459" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="460" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="461" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="462" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="463" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="464" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="465" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="466" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="467" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="468" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="469" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="470" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="471" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="472" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="473" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="474" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="475" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="476" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="477" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="478" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="479" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="480" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="481" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="482" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="483" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="484" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="485" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="486" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="487" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="488" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="489" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="490" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="491" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="492" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="493" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="494" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="495" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="496" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="497" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="498" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="499" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="500" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="501" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="502" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="503" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="504" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="505" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="506" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="507" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="508" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="509" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="510" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="511" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="512" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="513" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="514" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="515" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="516" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="517" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="518" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="519" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="520" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="521" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="522" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="523" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="524" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="525" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="526" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="527" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="528" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="529" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="530" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="531" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="532" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="533" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="534" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="535" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="536" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="537" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="538" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="539" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="540" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="541" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="542" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="543" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="544" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="545" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="546" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="547" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="548" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="549" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="550" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="551" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="552" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="553" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="554" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="555" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="556" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="557" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="558" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="559" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="560" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="561" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="562" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="563" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="564" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="565" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="566" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="567" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="568" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="569" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="570" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="571" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="572" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="573" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="574" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="575" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="576" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="577" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="578" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="579" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="580" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="581" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="582" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="583" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="584" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="585" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="586" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="587" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="588" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="589" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="590" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="591" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="592" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="593" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="594" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="595" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="596" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="597" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="598" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="599" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="600" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="601" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="602" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="603" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="604" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="605" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="606" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="607" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="608" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="609" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="610" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="611" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="612" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="613" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="614" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="615" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="616" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="617" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="618" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="619" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="620" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="621" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="622" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="623" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="624" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="625" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="626" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="627" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="628" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="629" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="630" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="631" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="632" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="633" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="634" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="635" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="636" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="637" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="638" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="639" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="640" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="641" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="642" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="643" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="644" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="645" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="646" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="647" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="648" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="649" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="650" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="651" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="652" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="653" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="654" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="655" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="656" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="657" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="658" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="659" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="660" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="661" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="662" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="663" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="664" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="665" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="666" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="667" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="668" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="669" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="670" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="671" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="672" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="673" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="674" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="675" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="676" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="677" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="678" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="679" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="680" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="681" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="682" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="683" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="684" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="685" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="686" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="687" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="688" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="689" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="690" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="691" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="692" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="693" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="694" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="695" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="696" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="697" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="698" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="699" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="700" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="701" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="702" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="703" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="704" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="705" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="706" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="707" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="708" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="709" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="710" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="711" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="712" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="713" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="714" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="715" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="716" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="717" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="718" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="719" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="720" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="721" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="722" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="723" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="724" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="725" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="726" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="727" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="728" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="729" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="730" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="731" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="732" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="733" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="734" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="735" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="736" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="737" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="738" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="739" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="740" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="741" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="742" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="743" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="744" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="745" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="746" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="747" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="748" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="749" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="750" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="751" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="752" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="753" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="754" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="755" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="756" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="757" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="758" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="759" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="760" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="761" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="762" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="763" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="764" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="765" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="766" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="767" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="768" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="769" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="770" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="771" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="772" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="773" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="774" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="775" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="776" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="777" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="778" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="779" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="780" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="781" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="782" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="783" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="784" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="785" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="786" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="787" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="788" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="789" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="790" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="791" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="792" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="793" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="794" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="795" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="796" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="797" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="798" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="799" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="800" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="801" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="802" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="803" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="804" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="805" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="806" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="807" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="808" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="809" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="810" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="811" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="812" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="813" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="814" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="815" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="816" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="817" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="818" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="819" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="820" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="821" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="822" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="823" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="824" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="825" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="826" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="827" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="828" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="829" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="830" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="831" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="832" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="833" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="834" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="835" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="836" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="837" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="838" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="839" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="840" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="841" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="842" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="843" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="844" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="845" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="846" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="847" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="848" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="849" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="850" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="851" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="852" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="853" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="854" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="855" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="856" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="857" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="858" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="859" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="860" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="861" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="862" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="863" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="864" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="865" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="866" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="867" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="868" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="869" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="870" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="871" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="872" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="873" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="874" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="875" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="876" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="877" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="878" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="879" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="880" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="881" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="882" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="883" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="884" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="885" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="886" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="887" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="888" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="889" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="890" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="891" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="892" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="893" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="894" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="895" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="896" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="897" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="898" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="899" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="900" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="901" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="902" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="903" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="904" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="905" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="906" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="907" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="908" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="909" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="910" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="911" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="912" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="913" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="914" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="915" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="916" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="917" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="918" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="919" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="920" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="921" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="922" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="923" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="924" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="925" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="926" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="927" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="928" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="929" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="930" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="931" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="932" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="933" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="934" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="935" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="936" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="937" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="938" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="939" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="940" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="941" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="942" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="943" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="944" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="945" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="946" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="947" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="948" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="949" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="950" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="951" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="952" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="953" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="954" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="955" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="956" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="957" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="958" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="959" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="960" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="961" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="962" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="963" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="964" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="965" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="966" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="967" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="968" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="969" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="970" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="971" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="972" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="973" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="974" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="975" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="976" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="977" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="978" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="979" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="980" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="981" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="982" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="983" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="984" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="985" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="986" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="987" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="988" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="989" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="990" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="991" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="992" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="993" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="994" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="995" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="996" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="997" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="998" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="999" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1000" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1001" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1002" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1003" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1004" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1005" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1006" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1007" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1008" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1009" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1010" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1011" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1012" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1013" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1014" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1015" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1016" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1017" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1018" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1019" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1020" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1021" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1022" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1023" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1024" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1025" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1026" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1027" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1028" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1029" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1030" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1031" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1032" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1033" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1034" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1035" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1036" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1037" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1038" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1039" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1040" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1041" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:A4"/>
@@ -20603,22 +20616,22 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="256" width="26.453125" customWidth="1"/>
-    <col min="257" max="1023" width="16.1796875" customWidth="1"/>
-    <col min="1024" max="1025" width="11.7265625" customWidth="1"/>
+    <col min="1" max="256" width="26.42578125" customWidth="1"/>
+    <col min="257" max="1023" width="16.140625" customWidth="1"/>
+    <col min="1024" max="1025" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="13" x14ac:dyDescent="0.3">
-      <c r="A1" s="56" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="59" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="26" t="s">
         <v>162</v>
       </c>
@@ -20632,7 +20645,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="27" t="s">
         <v>163</v>
       </c>
@@ -20667,21 +20680,21 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="256" width="24.453125" customWidth="1"/>
-    <col min="257" max="1023" width="16.1796875" customWidth="1"/>
-    <col min="1024" max="1025" width="11.7265625" customWidth="1"/>
+    <col min="1" max="256" width="24.42578125" customWidth="1"/>
+    <col min="257" max="1023" width="16.140625" customWidth="1"/>
+    <col min="1024" max="1025" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="13" x14ac:dyDescent="0.3">
-      <c r="A1" s="57" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="60" t="s">
         <v>79</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="26" t="s">
         <v>80</v>
       </c>
@@ -20692,7 +20705,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="27" t="s">
         <v>82</v>
       </c>
@@ -20703,7 +20716,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="28"/>
       <c r="B4" s="29"/>
       <c r="C4" s="29"/>
@@ -20729,21 +20742,21 @@
       <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="256" width="22.453125" customWidth="1"/>
-    <col min="257" max="1023" width="16.1796875" customWidth="1"/>
-    <col min="1024" max="1025" width="11.7265625" customWidth="1"/>
+    <col min="1" max="256" width="22.42578125" customWidth="1"/>
+    <col min="257" max="1023" width="16.140625" customWidth="1"/>
+    <col min="1024" max="1025" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="58" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="61" t="s">
         <v>85</v>
       </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="26" t="s">
         <v>86</v>
       </c>
@@ -20754,7 +20767,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
         <v>88</v>
       </c>
@@ -20765,7 +20778,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="12"/>
       <c r="B4" s="30"/>
       <c r="C4" s="30"/>
@@ -20791,21 +20804,21 @@
       <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="256" width="22.453125" customWidth="1"/>
-    <col min="257" max="1023" width="16.1796875" customWidth="1"/>
-    <col min="1024" max="1025" width="11.7265625" customWidth="1"/>
+    <col min="1" max="256" width="22.42578125" customWidth="1"/>
+    <col min="257" max="1023" width="16.140625" customWidth="1"/>
+    <col min="1024" max="1025" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="58" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="61" t="s">
         <v>91</v>
       </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="26" t="s">
         <v>86</v>
       </c>
@@ -20816,7 +20829,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
         <v>93</v>
       </c>
@@ -20827,7 +20840,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="28"/>
       <c r="B4" s="30"/>
       <c r="C4" s="30"/>
@@ -20853,21 +20866,21 @@
       <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="256" width="22.453125" customWidth="1"/>
-    <col min="257" max="1023" width="16.1796875" customWidth="1"/>
-    <col min="1024" max="1025" width="11.7265625" customWidth="1"/>
+    <col min="1" max="256" width="22.42578125" customWidth="1"/>
+    <col min="257" max="1023" width="16.140625" customWidth="1"/>
+    <col min="1024" max="1025" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="58" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="61" t="s">
         <v>96</v>
       </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
         <v>86</v>
       </c>
@@ -20878,7 +20891,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
         <v>98</v>
       </c>
@@ -20889,7 +20902,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="31"/>
       <c r="B4" s="9"/>
       <c r="C4" s="9"/>
@@ -20915,21 +20928,21 @@
       <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="256" width="22.453125" customWidth="1"/>
-    <col min="257" max="1023" width="16.1796875" customWidth="1"/>
-    <col min="1024" max="1025" width="11.7265625" customWidth="1"/>
+    <col min="1" max="256" width="22.42578125" customWidth="1"/>
+    <col min="257" max="1023" width="16.140625" customWidth="1"/>
+    <col min="1024" max="1025" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="58" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="61" t="s">
         <v>101</v>
       </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
         <v>86</v>
       </c>
@@ -20940,7 +20953,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
         <v>103</v>
       </c>
@@ -20951,7 +20964,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="31"/>
       <c r="B4" s="9"/>
       <c r="C4" s="9"/>
@@ -20971,33 +20984,35 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:T125"/>
+  <dimension ref="A1:U125"/>
   <sheetViews>
-    <sheetView topLeftCell="A106" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="U3" sqref="U3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.81640625" customWidth="1"/>
-    <col min="2" max="2" width="31.54296875" customWidth="1"/>
-    <col min="3" max="1023" width="12.453125" customWidth="1"/>
+    <col min="1" max="1" width="18.85546875" customWidth="1"/>
+    <col min="2" max="2" width="31.5703125" customWidth="1"/>
+    <col min="3" max="20" width="12.42578125" customWidth="1"/>
+    <col min="21" max="21" width="68.7109375" customWidth="1"/>
+    <col min="22" max="1023" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A1" s="58" t="s">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A1" s="61" t="s">
         <v>106</v>
       </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
-      <c r="F1" s="58"/>
-      <c r="G1" s="58"/>
-      <c r="H1" s="58"/>
-      <c r="I1" s="58"/>
-      <c r="J1" s="58"/>
-      <c r="K1" s="58"/>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="61"/>
+      <c r="G1" s="61"/>
+      <c r="H1" s="61"/>
+      <c r="I1" s="61"/>
+      <c r="J1" s="61"/>
+      <c r="K1" s="61"/>
       <c r="L1" s="43"/>
       <c r="M1" s="43"/>
       <c r="N1" s="43"/>
@@ -21008,7 +21023,7 @@
       <c r="S1" s="43"/>
       <c r="T1" s="43"/>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" s="29" t="s">
         <v>81</v>
       </c>
@@ -21069,8 +21084,11 @@
       <c r="T2" s="29" t="s">
         <v>123</v>
       </c>
+      <c r="U2" s="66" t="s">
+        <v>280</v>
+      </c>
     </row>
-    <row r="3" spans="1:20" ht="13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21" ht="48" x14ac:dyDescent="0.2">
       <c r="A3" s="32" t="s">
         <v>124</v>
       </c>
@@ -21131,8 +21149,11 @@
       <c r="T3" s="36" t="s">
         <v>141</v>
       </c>
+      <c r="U3" s="67" t="s">
+        <v>281</v>
+      </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A15" s="40" t="s">
         <v>176</v>
       </c>
@@ -21140,7 +21161,7 @@
       <c r="C15" s="40"/>
       <c r="D15" s="40"/>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A16" s="41" t="s">
         <v>171</v>
       </c>
@@ -21154,7 +21175,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="40" t="s">
         <v>175</v>
       </c>
@@ -21162,7 +21183,7 @@
       <c r="C28" s="40"/>
       <c r="D28" s="40"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="41" t="s">
         <v>171</v>
       </c>
@@ -21176,7 +21197,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" s="40" t="s">
         <v>180</v>
       </c>
@@ -21184,7 +21205,7 @@
       <c r="C44" s="40"/>
       <c r="D44" s="40"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" s="41" t="s">
         <v>171</v>
       </c>
@@ -21198,7 +21219,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" s="40" t="s">
         <v>267</v>
       </c>
@@ -21206,7 +21227,7 @@
       <c r="C58" s="40"/>
       <c r="D58" s="40"/>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" s="49" t="s">
         <v>171</v>
       </c>
@@ -21224,7 +21245,7 @@
       <c r="G59" s="51"/>
       <c r="H59" s="51"/>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" s="40" t="s">
         <v>170</v>
       </c>
@@ -21232,7 +21253,7 @@
       <c r="C71" s="40"/>
       <c r="D71" s="40"/>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" s="41" t="s">
         <v>171</v>
       </c>
@@ -21246,7 +21267,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" s="40" t="s">
         <v>187</v>
       </c>
@@ -21254,7 +21275,7 @@
       <c r="C93" s="40"/>
       <c r="D93" s="40"/>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" s="41" t="s">
         <v>188</v>
       </c>
@@ -21268,7 +21289,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A109" s="40" t="s">
         <v>271</v>
       </c>
@@ -21276,7 +21297,7 @@
       <c r="C109" s="40"/>
       <c r="D109" s="40"/>
     </row>
-    <row r="110" spans="1:8" s="52" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:8" s="52" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A110" s="49" t="s">
         <v>272</v>
       </c>
@@ -21294,15 +21315,15 @@
       <c r="G110" s="51"/>
       <c r="H110" s="51"/>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A124" s="59" t="s">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A124" s="62" t="s">
         <v>192</v>
       </c>
-      <c r="B124" s="60"/>
+      <c r="B124" s="63"/>
       <c r="C124" s="40"/>
       <c r="D124" s="40"/>
     </row>
-    <row r="125" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:4" ht="60" x14ac:dyDescent="0.2">
       <c r="A125" s="41" t="s">
         <v>193</v>
       </c>
@@ -21328,43 +21349,43 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34BFAF30-6EFD-4A13-A39A-D09455CAAF60}">
   <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.08984375" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
-    <col min="3" max="3" width="15.36328125" customWidth="1"/>
-    <col min="4" max="4" width="13.6328125" customWidth="1"/>
-    <col min="5" max="5" width="19.81640625" customWidth="1"/>
-    <col min="6" max="6" width="14.453125" customWidth="1"/>
-    <col min="7" max="7" width="21.26953125" customWidth="1"/>
-    <col min="8" max="8" width="17.08984375" customWidth="1"/>
-    <col min="9" max="9" width="14.08984375" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" customWidth="1"/>
+    <col min="5" max="5" width="19.85546875" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" customWidth="1"/>
+    <col min="7" max="7" width="21.28515625" customWidth="1"/>
+    <col min="8" max="8" width="17.140625" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" customWidth="1"/>
     <col min="10" max="10" width="19" customWidth="1"/>
-    <col min="11" max="11" width="16.26953125" customWidth="1"/>
-    <col min="12" max="12" width="21.7265625" customWidth="1"/>
+    <col min="11" max="11" width="16.28515625" customWidth="1"/>
+    <col min="12" max="12" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="63" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A1" s="64" t="s">
         <v>246</v>
       </c>
-      <c r="B1" s="64"/>
-      <c r="C1" s="64"/>
-      <c r="D1" s="64"/>
-      <c r="E1" s="64"/>
-      <c r="F1" s="64"/>
-      <c r="G1" s="64"/>
-      <c r="H1" s="64"/>
-      <c r="I1" s="64"/>
-      <c r="J1" s="64"/>
-      <c r="K1" s="64"/>
-      <c r="L1" s="64"/>
+      <c r="B1" s="65"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
+      <c r="E1" s="65"/>
+      <c r="F1" s="65"/>
+      <c r="G1" s="65"/>
+      <c r="H1" s="65"/>
+      <c r="I1" s="65"/>
+      <c r="J1" s="65"/>
+      <c r="K1" s="65"/>
+      <c r="L1" s="65"/>
     </row>
-    <row r="2" spans="1:12" ht="13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="44" t="s">
         <v>247</v>
       </c>
@@ -21392,17 +21413,17 @@
       <c r="I2" s="44" t="s">
         <v>255</v>
       </c>
-      <c r="J2" s="61" t="s">
+      <c r="J2" s="53" t="s">
         <v>276</v>
       </c>
-      <c r="K2" s="62" t="s">
+      <c r="K2" s="54" t="s">
         <v>277</v>
       </c>
       <c r="L2" s="44" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="15.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="45" t="s">
         <v>257</v>
       </c>
@@ -21433,10 +21454,10 @@
       <c r="J3" s="46" t="s">
         <v>278</v>
       </c>
-      <c r="K3" s="65" t="s">
+      <c r="K3" s="55" t="s">
         <v>279</v>
       </c>
-      <c r="L3" s="65" t="s">
+      <c r="L3" s="55" t="s">
         <v>266</v>
       </c>
     </row>

</xml_diff>

<commit_message>
POCOR-7272[Worked on Jordanian Student [Status Inprogress]]
</commit_message>
<xml_diff>
--- a/webroot/export/customexcel/default_templates/profile_template.xlsx
+++ b/webroot/export/customexcel/default_templates/profile_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp2\htdocs\pocor-openemis-core\webroot\export\customexcel\default_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C1E7BF6-5D52-4CA0-BB63-52E7AD6BD661}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AAD42A9-0B8A-4158-94F0-1B50EF1C3A9A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10305" tabRatio="862" firstSheet="4" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10305" tabRatio="862" firstSheet="3" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -183,9 +183,6 @@
     <t>Shift Type</t>
   </si>
   <si>
-    <t>${Institutions.shift_type_name}</t>
-  </si>
-  <si>
     <t>School Gender</t>
   </si>
   <si>
@@ -952,10 +949,13 @@
     <t>${"match": {"displayValue": "StudentDetails.area_average_mark","rows": {"matchFrom": "StudentDetails.id","matchTo": "StudentDetails.id"}}}</t>
   </si>
   <si>
-    <t>Percentage of Jordan Students</t>
-  </si>
-  <si>
-    <t>${"match": {"displayValue": "StudentFromEducationGrade.jordan_students","rows": {"matchFrom": "StudentFromEducationGrade.education_grade_id","matchTo": "StudentFromEducationGrade.education_grade_id"}
+    <t>${InstitutionShiftType.occupier}</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Jordanian Students</t>
+  </si>
+  <si>
+    <t>${"match": {"displayValue": "StudentFromEducationGrade.jordanian_students","rows": {"matchFrom": "StudentFromEducationGrade.education_grade_id","matchTo": "StudentFromEducationGrade.education_grade_id"}
 }}</t>
   </si>
 </sst>
@@ -1330,6 +1330,12 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1359,12 +1365,6 @@
     </xf>
     <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1774,8 +1774,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:IV1041"/>
   <sheetViews>
-    <sheetView topLeftCell="A155" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="A168" sqref="A168"/>
+    <sheetView topLeftCell="A17" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1796,7 +1796,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="58" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4"/>
@@ -1817,13 +1817,13 @@
       <c r="Q1" s="7"/>
     </row>
     <row r="2" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="56"/>
-      <c r="B2" s="57" t="s">
+      <c r="A2" s="58"/>
+      <c r="B2" s="59" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
       <c r="F2" s="8"/>
       <c r="G2" s="9"/>
       <c r="H2" s="7"/>
@@ -2077,13 +2077,13 @@
       <c r="IV2" s="3"/>
     </row>
     <row r="3" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="56"/>
-      <c r="B3" s="58" t="s">
+      <c r="A3" s="58"/>
+      <c r="B3" s="60" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="58"/>
-      <c r="D3" s="58"/>
-      <c r="E3" s="58"/>
+      <c r="C3" s="60"/>
+      <c r="D3" s="60"/>
+      <c r="E3" s="60"/>
       <c r="F3" s="9"/>
       <c r="G3" s="9"/>
       <c r="H3" s="7"/>
@@ -2337,7 +2337,7 @@
       <c r="IV3" s="3"/>
     </row>
     <row r="4" spans="1:256" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="56"/>
+      <c r="A4" s="58"/>
       <c r="B4" s="4"/>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
@@ -4068,7 +4068,7 @@
         <v>23</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>24</v>
+        <v>279</v>
       </c>
       <c r="C17" s="13"/>
       <c r="D17" s="5"/>
@@ -4327,10 +4327,10 @@
     </row>
     <row r="18" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" s="12" t="s">
         <v>25</v>
-      </c>
-      <c r="B18" s="12" t="s">
-        <v>26</v>
       </c>
       <c r="C18" s="13"/>
       <c r="D18" s="5"/>
@@ -4589,10 +4589,10 @@
     </row>
     <row r="19" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" s="12" t="s">
         <v>27</v>
-      </c>
-      <c r="B19" s="12" t="s">
-        <v>28</v>
       </c>
       <c r="C19" s="13"/>
       <c r="D19" s="5"/>
@@ -5113,10 +5113,10 @@
     </row>
     <row r="21" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" s="12" t="s">
         <v>29</v>
-      </c>
-      <c r="B21" s="12" t="s">
-        <v>30</v>
       </c>
       <c r="C21" s="13"/>
       <c r="D21" s="5"/>
@@ -5375,10 +5375,10 @@
     </row>
     <row r="22" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="B22" s="38" t="s">
         <v>164</v>
-      </c>
-      <c r="B22" s="38" t="s">
-        <v>165</v>
       </c>
       <c r="C22" s="13"/>
       <c r="D22" s="5"/>
@@ -5637,10 +5637,10 @@
     </row>
     <row r="23" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="B23" s="38" t="s">
         <v>166</v>
-      </c>
-      <c r="B23" s="38" t="s">
-        <v>167</v>
       </c>
       <c r="C23" s="13"/>
       <c r="D23" s="5"/>
@@ -5899,10 +5899,10 @@
     </row>
     <row r="24" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="B24" s="38" t="s">
         <v>168</v>
-      </c>
-      <c r="B24" s="38" t="s">
-        <v>169</v>
       </c>
       <c r="C24" s="13"/>
       <c r="D24" s="18"/>
@@ -6677,7 +6677,7 @@
     </row>
     <row r="27" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -6937,13 +6937,13 @@
     </row>
     <row r="28" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B28" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="B28" s="19" t="s">
+      <c r="C28" s="19" t="s">
         <v>33</v>
-      </c>
-      <c r="C28" s="19" t="s">
-        <v>34</v>
       </c>
       <c r="D28" s="18"/>
       <c r="E28" s="14"/>
@@ -7201,13 +7201,13 @@
     </row>
     <row r="29" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B29" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="B29" s="12" t="s">
+      <c r="C29" s="7" t="s">
         <v>36</v>
-      </c>
-      <c r="C29" s="7" t="s">
-        <v>37</v>
       </c>
       <c r="D29" s="18"/>
       <c r="E29" s="14"/>
@@ -7981,10 +7981,10 @@
     </row>
     <row r="32" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="B32" s="12" t="s">
         <v>38</v>
-      </c>
-      <c r="B32" s="12" t="s">
-        <v>39</v>
       </c>
       <c r="C32" s="18"/>
       <c r="D32" s="18"/>
@@ -8243,10 +8243,10 @@
     </row>
     <row r="33" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="B33" s="12" t="s">
         <v>40</v>
-      </c>
-      <c r="B33" s="12" t="s">
-        <v>41</v>
       </c>
       <c r="C33" s="18"/>
       <c r="D33" s="18"/>
@@ -9021,10 +9021,10 @@
     </row>
     <row r="36" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="B36" s="12" t="s">
         <v>42</v>
-      </c>
-      <c r="B36" s="12" t="s">
-        <v>43</v>
       </c>
       <c r="C36" s="18"/>
       <c r="D36" s="18"/>
@@ -9283,10 +9283,10 @@
     </row>
     <row r="37" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="B37" s="12" t="s">
         <v>44</v>
-      </c>
-      <c r="B37" s="12" t="s">
-        <v>45</v>
       </c>
       <c r="C37" s="18"/>
       <c r="D37" s="18"/>
@@ -10061,10 +10061,10 @@
     </row>
     <row r="40" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="B40" s="12" t="s">
         <v>46</v>
-      </c>
-      <c r="B40" s="12" t="s">
-        <v>47</v>
       </c>
       <c r="C40" s="18"/>
       <c r="D40" s="18"/>
@@ -10323,10 +10323,10 @@
     </row>
     <row r="41" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="B41" s="12" t="s">
         <v>48</v>
-      </c>
-      <c r="B41" s="12" t="s">
-        <v>49</v>
       </c>
       <c r="C41" s="18"/>
       <c r="D41" s="18"/>
@@ -11101,10 +11101,10 @@
     </row>
     <row r="44" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="B44" s="22" t="s">
         <v>50</v>
-      </c>
-      <c r="B44" s="22" t="s">
-        <v>51</v>
       </c>
       <c r="C44" s="18"/>
       <c r="D44" s="18"/>
@@ -11363,10 +11363,10 @@
     </row>
     <row r="45" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="B45" s="22" t="s">
         <v>52</v>
-      </c>
-      <c r="B45" s="22" t="s">
-        <v>53</v>
       </c>
       <c r="C45" s="18"/>
       <c r="D45" s="18"/>
@@ -11625,10 +11625,10 @@
     </row>
     <row r="46" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="B46" s="22" t="s">
         <v>54</v>
-      </c>
-      <c r="B46" s="22" t="s">
-        <v>55</v>
       </c>
       <c r="C46" s="18"/>
       <c r="D46" s="18"/>
@@ -11887,10 +11887,10 @@
     </row>
     <row r="47" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="B47" s="22" t="s">
         <v>56</v>
-      </c>
-      <c r="B47" s="22" t="s">
-        <v>57</v>
       </c>
       <c r="C47" s="18"/>
       <c r="D47" s="18"/>
@@ -12149,10 +12149,10 @@
     </row>
     <row r="48" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B48" s="22" t="s">
         <v>58</v>
-      </c>
-      <c r="B48" s="22" t="s">
-        <v>59</v>
       </c>
       <c r="C48" s="18"/>
       <c r="D48" s="18"/>
@@ -12411,10 +12411,10 @@
     </row>
     <row r="49" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B49" s="22" t="s">
         <v>60</v>
-      </c>
-      <c r="B49" s="22" t="s">
-        <v>61</v>
       </c>
       <c r="C49" s="18"/>
       <c r="D49" s="18"/>
@@ -12673,10 +12673,10 @@
     </row>
     <row r="50" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="B50" s="22" t="s">
         <v>62</v>
-      </c>
-      <c r="B50" s="22" t="s">
-        <v>63</v>
       </c>
       <c r="C50" s="18"/>
       <c r="D50" s="18"/>
@@ -12935,7 +12935,7 @@
     </row>
     <row r="51" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B51" s="22"/>
       <c r="C51" s="18"/>
@@ -13195,10 +13195,10 @@
     </row>
     <row r="52" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B52" s="22" t="s">
         <v>65</v>
-      </c>
-      <c r="B52" s="22" t="s">
-        <v>66</v>
       </c>
       <c r="C52" s="18"/>
       <c r="D52" s="18"/>
@@ -13973,7 +13973,7 @@
     </row>
     <row r="55" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
@@ -14233,13 +14233,13 @@
     </row>
     <row r="56" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="33" t="s">
+        <v>142</v>
+      </c>
+      <c r="B56" s="33" t="s">
         <v>143</v>
       </c>
-      <c r="B56" s="33" t="s">
+      <c r="C56" s="33" t="s">
         <v>144</v>
-      </c>
-      <c r="C56" s="33" t="s">
-        <v>145</v>
       </c>
       <c r="D56" s="18"/>
       <c r="E56" s="14"/>
@@ -14497,13 +14497,13 @@
     </row>
     <row r="57" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="34" t="s">
+        <v>145</v>
+      </c>
+      <c r="B57" s="35" t="s">
         <v>146</v>
       </c>
-      <c r="B57" s="35" t="s">
+      <c r="C57" s="35" t="s">
         <v>147</v>
-      </c>
-      <c r="C57" s="35" t="s">
-        <v>148</v>
       </c>
       <c r="D57" s="18"/>
       <c r="E57" s="14"/>
@@ -14761,13 +14761,13 @@
     </row>
     <row r="58" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="34" t="s">
+        <v>148</v>
+      </c>
+      <c r="B58" s="35" t="s">
         <v>149</v>
       </c>
-      <c r="B58" s="35" t="s">
+      <c r="C58" s="35" t="s">
         <v>150</v>
-      </c>
-      <c r="C58" s="35" t="s">
-        <v>151</v>
       </c>
       <c r="D58" s="18"/>
       <c r="E58" s="14"/>
@@ -15025,13 +15025,13 @@
     </row>
     <row r="59" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="34" t="s">
+        <v>151</v>
+      </c>
+      <c r="B59" s="35" t="s">
         <v>152</v>
       </c>
-      <c r="B59" s="35" t="s">
+      <c r="C59" s="35" t="s">
         <v>153</v>
-      </c>
-      <c r="C59" s="35" t="s">
-        <v>154</v>
       </c>
       <c r="D59" s="18"/>
       <c r="E59" s="14"/>
@@ -15289,13 +15289,13 @@
     </row>
     <row r="60" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="34" t="s">
+        <v>154</v>
+      </c>
+      <c r="B60" s="35" t="s">
         <v>155</v>
       </c>
-      <c r="B60" s="35" t="s">
+      <c r="C60" s="35" t="s">
         <v>156</v>
-      </c>
-      <c r="C60" s="35" t="s">
-        <v>157</v>
       </c>
       <c r="D60" s="18"/>
       <c r="E60" s="14"/>
@@ -15811,7 +15811,7 @@
     </row>
     <row r="62" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B62" s="1"/>
       <c r="C62" s="16"/>
@@ -16071,10 +16071,10 @@
     </row>
     <row r="63" spans="1:256" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="B63" s="24" t="s">
         <v>68</v>
-      </c>
-      <c r="B63" s="24" t="s">
-        <v>69</v>
       </c>
       <c r="C63" s="16"/>
       <c r="D63" s="16"/>
@@ -16095,10 +16095,10 @@
     </row>
     <row r="64" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="25" t="s">
+        <v>69</v>
+      </c>
+      <c r="B64" s="22" t="s">
         <v>70</v>
-      </c>
-      <c r="B64" s="22" t="s">
-        <v>71</v>
       </c>
       <c r="C64" s="7"/>
       <c r="D64" s="16"/>
@@ -18163,7 +18163,7 @@
     </row>
     <row r="72" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B72" s="1"/>
       <c r="C72" s="3"/>
@@ -18422,10 +18422,10 @@
     </row>
     <row r="73" spans="1:256" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="23" t="s">
+        <v>195</v>
+      </c>
+      <c r="B73" s="24" t="s">
         <v>196</v>
-      </c>
-      <c r="B73" s="24" t="s">
-        <v>197</v>
       </c>
       <c r="C73" s="3"/>
       <c r="E73" s="3"/>
@@ -18683,10 +18683,10 @@
     </row>
     <row r="74" spans="1:256" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="25" t="s">
+        <v>197</v>
+      </c>
+      <c r="B74" s="25" t="s">
         <v>198</v>
-      </c>
-      <c r="B74" s="25" t="s">
-        <v>199</v>
       </c>
       <c r="C74" s="3"/>
       <c r="E74" s="3"/>
@@ -19487,7 +19487,7 @@
     <row r="97" spans="1:16" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="98" spans="1:16" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B98" s="1"/>
       <c r="C98" s="1"/>
@@ -19507,102 +19507,102 @@
     </row>
     <row r="99" spans="1:16" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="23" t="s">
+        <v>201</v>
+      </c>
+      <c r="B99" s="23" t="s">
         <v>202</v>
       </c>
-      <c r="B99" s="23" t="s">
+      <c r="C99" s="23" t="s">
         <v>203</v>
       </c>
-      <c r="C99" s="23" t="s">
+      <c r="D99" s="23" t="s">
         <v>204</v>
       </c>
-      <c r="D99" s="23" t="s">
+      <c r="E99" s="23" t="s">
         <v>205</v>
       </c>
-      <c r="E99" s="23" t="s">
+      <c r="F99" s="23" t="s">
         <v>206</v>
       </c>
-      <c r="F99" s="23" t="s">
+      <c r="G99" s="23" t="s">
         <v>207</v>
       </c>
-      <c r="G99" s="23" t="s">
+      <c r="H99" s="23" t="s">
         <v>208</v>
       </c>
-      <c r="H99" s="23" t="s">
+      <c r="I99" s="23" t="s">
         <v>209</v>
       </c>
-      <c r="I99" s="23" t="s">
+      <c r="J99" s="23" t="s">
         <v>210</v>
       </c>
-      <c r="J99" s="23" t="s">
+      <c r="K99" s="23" t="s">
         <v>211</v>
       </c>
-      <c r="K99" s="23" t="s">
+      <c r="L99" s="23" t="s">
         <v>212</v>
       </c>
-      <c r="L99" s="23" t="s">
+      <c r="M99" s="23" t="s">
         <v>213</v>
       </c>
-      <c r="M99" s="23" t="s">
+      <c r="N99" s="23" t="s">
         <v>214</v>
       </c>
-      <c r="N99" s="23" t="s">
+      <c r="O99" s="23" t="s">
         <v>215</v>
       </c>
-      <c r="O99" s="23" t="s">
+      <c r="P99" s="23" t="s">
         <v>216</v>
-      </c>
-      <c r="P99" s="23" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="100" spans="1:16" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="25" t="s">
+        <v>217</v>
+      </c>
+      <c r="B100" s="25" t="s">
         <v>218</v>
       </c>
-      <c r="B100" s="25" t="s">
+      <c r="C100" s="25" t="s">
         <v>219</v>
       </c>
-      <c r="C100" s="25" t="s">
+      <c r="D100" s="25" t="s">
         <v>220</v>
       </c>
-      <c r="D100" s="25" t="s">
+      <c r="E100" s="25" t="s">
         <v>221</v>
       </c>
-      <c r="E100" s="25" t="s">
+      <c r="F100" s="25" t="s">
         <v>222</v>
       </c>
-      <c r="F100" s="25" t="s">
+      <c r="G100" s="25" t="s">
         <v>223</v>
       </c>
-      <c r="G100" s="25" t="s">
+      <c r="H100" s="25" t="s">
         <v>224</v>
       </c>
-      <c r="H100" s="25" t="s">
+      <c r="I100" s="25" t="s">
         <v>225</v>
       </c>
-      <c r="I100" s="25" t="s">
+      <c r="J100" s="25" t="s">
         <v>226</v>
       </c>
-      <c r="J100" s="25" t="s">
+      <c r="K100" s="25" t="s">
         <v>227</v>
       </c>
-      <c r="K100" s="25" t="s">
+      <c r="L100" s="25" t="s">
         <v>228</v>
       </c>
-      <c r="L100" s="25" t="s">
+      <c r="M100" s="25" t="s">
         <v>229</v>
       </c>
-      <c r="M100" s="25" t="s">
+      <c r="N100" s="25" t="s">
         <v>230</v>
       </c>
-      <c r="N100" s="25" t="s">
+      <c r="O100" s="25" t="s">
         <v>231</v>
       </c>
-      <c r="O100" s="25" t="s">
+      <c r="P100" s="25" t="s">
         <v>232</v>
-      </c>
-      <c r="P100" s="25" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="101" spans="1:16" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -19677,7 +19677,7 @@
     <row r="170" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="171" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A171" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B171" s="1"/>
       <c r="C171" s="1"/>
@@ -19687,42 +19687,42 @@
     </row>
     <row r="172" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A172" s="23" t="s">
+        <v>233</v>
+      </c>
+      <c r="B172" s="23" t="s">
         <v>234</v>
       </c>
-      <c r="B172" s="23" t="s">
+      <c r="C172" s="23" t="s">
         <v>235</v>
       </c>
-      <c r="C172" s="23" t="s">
+      <c r="D172" s="23" t="s">
         <v>236</v>
       </c>
-      <c r="D172" s="23" t="s">
+      <c r="E172" s="23" t="s">
         <v>237</v>
       </c>
-      <c r="E172" s="23" t="s">
+      <c r="F172" s="23" t="s">
         <v>238</v>
-      </c>
-      <c r="F172" s="23" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="173" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A173" s="25" t="s">
+        <v>239</v>
+      </c>
+      <c r="B173" s="25" t="s">
         <v>240</v>
       </c>
-      <c r="B173" s="25" t="s">
+      <c r="C173" s="25" t="s">
         <v>241</v>
       </c>
-      <c r="C173" s="25" t="s">
+      <c r="D173" s="25" t="s">
         <v>242</v>
       </c>
-      <c r="D173" s="25" t="s">
+      <c r="E173" s="25" t="s">
         <v>243</v>
       </c>
-      <c r="E173" s="25" t="s">
+      <c r="F173" s="25" t="s">
         <v>244</v>
-      </c>
-      <c r="F173" s="25" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="174" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -20624,39 +20624,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="59" t="s">
-        <v>72</v>
-      </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
+      <c r="A1" s="61" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="26" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B2" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="C2" s="26" t="s">
         <v>73</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="D2" s="26" t="s">
         <v>74</v>
-      </c>
-      <c r="D2" s="26" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="27" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B3" s="27" t="s">
+        <v>75</v>
+      </c>
+      <c r="C3" s="27" t="s">
         <v>76</v>
       </c>
-      <c r="C3" s="27" t="s">
+      <c r="D3" s="27" t="s">
         <v>77</v>
-      </c>
-      <c r="D3" s="27" t="s">
-        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -20688,32 +20688,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="60" t="s">
-        <v>79</v>
-      </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
+      <c r="A1" s="62" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="26" t="s">
+        <v>79</v>
+      </c>
+      <c r="B2" s="26" t="s">
         <v>80</v>
       </c>
-      <c r="B2" s="26" t="s">
-        <v>81</v>
-      </c>
       <c r="C2" s="26" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="27" t="s">
+        <v>81</v>
+      </c>
+      <c r="B3" s="27" t="s">
         <v>82</v>
       </c>
-      <c r="B3" s="27" t="s">
+      <c r="C3" s="27" t="s">
         <v>83</v>
-      </c>
-      <c r="C3" s="27" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -20750,32 +20750,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="61" t="s">
-        <v>85</v>
-      </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
+      <c r="A1" s="63" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="B2" s="26" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2" s="26" t="s">
         <v>86</v>
-      </c>
-      <c r="B2" s="26" t="s">
-        <v>80</v>
-      </c>
-      <c r="C2" s="26" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="B3" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="C3" s="22" t="s">
         <v>89</v>
-      </c>
-      <c r="C3" s="22" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -20812,32 +20812,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="61" t="s">
-        <v>91</v>
-      </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
+      <c r="A1" s="63" t="s">
+        <v>90</v>
+      </c>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="B2" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="C2" s="26" t="s">
         <v>86</v>
-      </c>
-      <c r="B2" s="26" t="s">
-        <v>92</v>
-      </c>
-      <c r="C2" s="26" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="B3" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="C3" s="22" t="s">
         <v>94</v>
-      </c>
-      <c r="C3" s="22" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -20863,7 +20863,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -20874,32 +20874,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="61" t="s">
-        <v>96</v>
-      </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
+      <c r="A1" s="63" t="s">
+        <v>95</v>
+      </c>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="C2" s="9" t="s">
         <v>86</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="B3" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="C3" s="22" t="s">
         <v>99</v>
-      </c>
-      <c r="C3" s="22" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -20936,32 +20936,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="61" t="s">
-        <v>101</v>
-      </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
+      <c r="A1" s="63" t="s">
+        <v>100</v>
+      </c>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="C2" s="9" t="s">
         <v>86</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="B3" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="C3" s="22" t="s">
         <v>104</v>
-      </c>
-      <c r="C3" s="22" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -21000,19 +21000,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A1" s="61" t="s">
-        <v>106</v>
-      </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
-      <c r="G1" s="61"/>
-      <c r="H1" s="61"/>
-      <c r="I1" s="61"/>
-      <c r="J1" s="61"/>
-      <c r="K1" s="61"/>
+      <c r="A1" s="63" t="s">
+        <v>105</v>
+      </c>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
+      <c r="H1" s="63"/>
+      <c r="I1" s="63"/>
+      <c r="J1" s="63"/>
+      <c r="K1" s="63"/>
       <c r="L1" s="43"/>
       <c r="M1" s="43"/>
       <c r="N1" s="43"/>
@@ -21025,137 +21025,137 @@
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" s="29" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B2" s="29" t="s">
+        <v>106</v>
+      </c>
+      <c r="C2" s="29" t="s">
         <v>107</v>
       </c>
-      <c r="C2" s="29" t="s">
+      <c r="D2" s="29" t="s">
         <v>108</v>
       </c>
-      <c r="D2" s="29" t="s">
+      <c r="E2" s="29" t="s">
         <v>109</v>
       </c>
-      <c r="E2" s="29" t="s">
+      <c r="F2" s="29" t="s">
         <v>110</v>
       </c>
-      <c r="F2" s="29" t="s">
+      <c r="G2" s="29" t="s">
         <v>111</v>
       </c>
-      <c r="G2" s="29" t="s">
+      <c r="H2" s="29" t="s">
         <v>112</v>
       </c>
-      <c r="H2" s="29" t="s">
+      <c r="I2" s="29" t="s">
         <v>113</v>
       </c>
-      <c r="I2" s="29" t="s">
+      <c r="J2" s="29" t="s">
         <v>114</v>
       </c>
-      <c r="J2" s="29" t="s">
+      <c r="K2" s="29" t="s">
         <v>115</v>
       </c>
-      <c r="K2" s="29" t="s">
+      <c r="L2" s="29" t="s">
         <v>116</v>
       </c>
-      <c r="L2" s="29" t="s">
+      <c r="M2" s="29" t="s">
         <v>117</v>
       </c>
-      <c r="M2" s="29" t="s">
+      <c r="N2" s="29" t="s">
         <v>118</v>
       </c>
-      <c r="N2" s="29" t="s">
+      <c r="O2" s="29" t="s">
         <v>119</v>
       </c>
-      <c r="O2" s="29" t="s">
+      <c r="P2" s="29" t="s">
         <v>120</v>
       </c>
-      <c r="P2" s="29" t="s">
+      <c r="Q2" s="29" t="s">
+        <v>157</v>
+      </c>
+      <c r="R2" s="29" t="s">
         <v>121</v>
       </c>
-      <c r="Q2" s="29" t="s">
+      <c r="S2" s="29" t="s">
+        <v>159</v>
+      </c>
+      <c r="T2" s="29" t="s">
+        <v>122</v>
+      </c>
+      <c r="U2" s="56" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" ht="60" x14ac:dyDescent="0.2">
+      <c r="A3" s="32" t="s">
+        <v>123</v>
+      </c>
+      <c r="B3" s="32" t="s">
+        <v>124</v>
+      </c>
+      <c r="C3" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="D3" s="32" t="s">
+        <v>126</v>
+      </c>
+      <c r="E3" s="32" t="s">
+        <v>127</v>
+      </c>
+      <c r="F3" s="32" t="s">
+        <v>128</v>
+      </c>
+      <c r="G3" s="32" t="s">
+        <v>129</v>
+      </c>
+      <c r="H3" s="32" t="s">
+        <v>130</v>
+      </c>
+      <c r="I3" s="32" t="s">
+        <v>131</v>
+      </c>
+      <c r="J3" s="32" t="s">
+        <v>132</v>
+      </c>
+      <c r="K3" s="32" t="s">
+        <v>133</v>
+      </c>
+      <c r="L3" s="36" t="s">
+        <v>134</v>
+      </c>
+      <c r="M3" s="36" t="s">
+        <v>135</v>
+      </c>
+      <c r="N3" s="36" t="s">
+        <v>136</v>
+      </c>
+      <c r="O3" s="36" t="s">
+        <v>137</v>
+      </c>
+      <c r="P3" s="36" t="s">
+        <v>138</v>
+      </c>
+      <c r="Q3" s="36" t="s">
         <v>158</v>
       </c>
-      <c r="R2" s="29" t="s">
-        <v>122</v>
-      </c>
-      <c r="S2" s="29" t="s">
+      <c r="R3" s="36" t="s">
+        <v>139</v>
+      </c>
+      <c r="S3" s="36" t="s">
         <v>160</v>
       </c>
-      <c r="T2" s="29" t="s">
-        <v>123</v>
-      </c>
-      <c r="U2" s="66" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21" ht="48" x14ac:dyDescent="0.2">
-      <c r="A3" s="32" t="s">
-        <v>124</v>
-      </c>
-      <c r="B3" s="32" t="s">
-        <v>125</v>
-      </c>
-      <c r="C3" s="32" t="s">
-        <v>126</v>
-      </c>
-      <c r="D3" s="32" t="s">
-        <v>127</v>
-      </c>
-      <c r="E3" s="32" t="s">
-        <v>128</v>
-      </c>
-      <c r="F3" s="32" t="s">
-        <v>129</v>
-      </c>
-      <c r="G3" s="32" t="s">
-        <v>130</v>
-      </c>
-      <c r="H3" s="32" t="s">
-        <v>131</v>
-      </c>
-      <c r="I3" s="32" t="s">
-        <v>132</v>
-      </c>
-      <c r="J3" s="32" t="s">
-        <v>133</v>
-      </c>
-      <c r="K3" s="32" t="s">
-        <v>134</v>
-      </c>
-      <c r="L3" s="36" t="s">
-        <v>135</v>
-      </c>
-      <c r="M3" s="36" t="s">
-        <v>136</v>
-      </c>
-      <c r="N3" s="36" t="s">
-        <v>137</v>
-      </c>
-      <c r="O3" s="36" t="s">
-        <v>138</v>
-      </c>
-      <c r="P3" s="36" t="s">
-        <v>139</v>
-      </c>
-      <c r="Q3" s="36" t="s">
-        <v>159</v>
-      </c>
-      <c r="R3" s="36" t="s">
+      <c r="T3" s="36" t="s">
         <v>140</v>
       </c>
-      <c r="S3" s="36" t="s">
-        <v>161</v>
-      </c>
-      <c r="T3" s="36" t="s">
-        <v>141</v>
-      </c>
-      <c r="U3" s="67" t="s">
+      <c r="U3" s="57" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A15" s="40" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B15" s="40"/>
       <c r="C15" s="40"/>
@@ -21163,21 +21163,21 @@
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A16" s="41" t="s">
+        <v>170</v>
+      </c>
+      <c r="B16" s="48" t="s">
         <v>171</v>
       </c>
-      <c r="B16" s="48" t="s">
+      <c r="C16" s="48" t="s">
         <v>172</v>
       </c>
-      <c r="C16" s="48" t="s">
+      <c r="D16" s="48" t="s">
         <v>173</v>
-      </c>
-      <c r="D16" s="48" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="40" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B28" s="40"/>
       <c r="C28" s="40"/>
@@ -21185,21 +21185,21 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="41" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B29" s="48" t="s">
+        <v>176</v>
+      </c>
+      <c r="C29" s="48" t="s">
         <v>177</v>
       </c>
-      <c r="C29" s="48" t="s">
+      <c r="D29" s="48" t="s">
         <v>178</v>
-      </c>
-      <c r="D29" s="48" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" s="40" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B44" s="40"/>
       <c r="C44" s="40"/>
@@ -21207,21 +21207,21 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" s="41" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B45" s="48" t="s">
+        <v>180</v>
+      </c>
+      <c r="C45" s="48" t="s">
         <v>181</v>
       </c>
-      <c r="C45" s="48" t="s">
+      <c r="D45" s="48" t="s">
         <v>182</v>
-      </c>
-      <c r="D45" s="48" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" s="40" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B58" s="40"/>
       <c r="C58" s="40"/>
@@ -21229,16 +21229,16 @@
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" s="49" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B59" s="50" t="s">
+        <v>267</v>
+      </c>
+      <c r="C59" s="50" t="s">
         <v>268</v>
       </c>
-      <c r="C59" s="50" t="s">
+      <c r="D59" s="50" t="s">
         <v>269</v>
-      </c>
-      <c r="D59" s="50" t="s">
-        <v>270</v>
       </c>
       <c r="E59" s="51"/>
       <c r="F59" s="51"/>
@@ -21247,7 +21247,7 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" s="40" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B71" s="40"/>
       <c r="C71" s="40"/>
@@ -21255,21 +21255,21 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" s="41" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B72" s="48" t="s">
+        <v>183</v>
+      </c>
+      <c r="C72" s="48" t="s">
         <v>184</v>
       </c>
-      <c r="C72" s="48" t="s">
+      <c r="D72" s="48" t="s">
         <v>185</v>
-      </c>
-      <c r="D72" s="48" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" s="40" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B93" s="40"/>
       <c r="C93" s="40"/>
@@ -21277,21 +21277,21 @@
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" s="41" t="s">
+        <v>187</v>
+      </c>
+      <c r="B94" s="48" t="s">
         <v>188</v>
       </c>
-      <c r="B94" s="48" t="s">
+      <c r="C94" s="48" t="s">
         <v>189</v>
       </c>
-      <c r="C94" s="48" t="s">
+      <c r="D94" s="48" t="s">
         <v>190</v>
-      </c>
-      <c r="D94" s="48" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A109" s="40" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B109" s="40"/>
       <c r="C109" s="40"/>
@@ -21299,16 +21299,16 @@
     </row>
     <row r="110" spans="1:8" s="52" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A110" s="49" t="s">
+        <v>271</v>
+      </c>
+      <c r="B110" s="50" t="s">
         <v>272</v>
       </c>
-      <c r="B110" s="50" t="s">
+      <c r="C110" s="50" t="s">
         <v>273</v>
       </c>
-      <c r="C110" s="50" t="s">
+      <c r="D110" s="50" t="s">
         <v>274</v>
-      </c>
-      <c r="D110" s="50" t="s">
-        <v>275</v>
       </c>
       <c r="E110" s="51"/>
       <c r="F110" s="51"/>
@@ -21316,19 +21316,19 @@
       <c r="H110" s="51"/>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A124" s="62" t="s">
-        <v>192</v>
-      </c>
-      <c r="B124" s="63"/>
+      <c r="A124" s="64" t="s">
+        <v>191</v>
+      </c>
+      <c r="B124" s="65"/>
       <c r="C124" s="40"/>
       <c r="D124" s="40"/>
     </row>
     <row r="125" spans="1:4" ht="60" x14ac:dyDescent="0.2">
       <c r="A125" s="41" t="s">
+        <v>192</v>
+      </c>
+      <c r="B125" s="42" t="s">
         <v>193</v>
-      </c>
-      <c r="B125" s="42" t="s">
-        <v>194</v>
       </c>
     </row>
   </sheetData>
@@ -21370,95 +21370,95 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A1" s="64" t="s">
-        <v>246</v>
-      </c>
-      <c r="B1" s="65"/>
-      <c r="C1" s="65"/>
-      <c r="D1" s="65"/>
-      <c r="E1" s="65"/>
-      <c r="F1" s="65"/>
-      <c r="G1" s="65"/>
-      <c r="H1" s="65"/>
-      <c r="I1" s="65"/>
-      <c r="J1" s="65"/>
-      <c r="K1" s="65"/>
-      <c r="L1" s="65"/>
+      <c r="A1" s="66" t="s">
+        <v>245</v>
+      </c>
+      <c r="B1" s="67"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="67"/>
+      <c r="G1" s="67"/>
+      <c r="H1" s="67"/>
+      <c r="I1" s="67"/>
+      <c r="J1" s="67"/>
+      <c r="K1" s="67"/>
+      <c r="L1" s="67"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="44" t="s">
+        <v>246</v>
+      </c>
+      <c r="B2" s="44" t="s">
         <v>247</v>
       </c>
-      <c r="B2" s="44" t="s">
+      <c r="C2" s="44" t="s">
         <v>248</v>
       </c>
-      <c r="C2" s="44" t="s">
+      <c r="D2" s="44" t="s">
         <v>249</v>
       </c>
-      <c r="D2" s="44" t="s">
+      <c r="E2" s="44" t="s">
         <v>250</v>
       </c>
-      <c r="E2" s="44" t="s">
+      <c r="F2" s="44" t="s">
         <v>251</v>
       </c>
-      <c r="F2" s="44" t="s">
+      <c r="G2" s="44" t="s">
         <v>252</v>
       </c>
-      <c r="G2" s="44" t="s">
+      <c r="H2" s="44" t="s">
         <v>253</v>
       </c>
-      <c r="H2" s="44" t="s">
+      <c r="I2" s="44" t="s">
         <v>254</v>
       </c>
-      <c r="I2" s="44" t="s">
+      <c r="J2" s="53" t="s">
+        <v>275</v>
+      </c>
+      <c r="K2" s="54" t="s">
+        <v>276</v>
+      </c>
+      <c r="L2" s="44" t="s">
         <v>255</v>
-      </c>
-      <c r="J2" s="53" t="s">
-        <v>276</v>
-      </c>
-      <c r="K2" s="54" t="s">
-        <v>277</v>
-      </c>
-      <c r="L2" s="44" t="s">
-        <v>256</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="45" t="s">
+        <v>256</v>
+      </c>
+      <c r="B3" s="46" t="s">
         <v>257</v>
       </c>
-      <c r="B3" s="46" t="s">
+      <c r="C3" s="47" t="s">
         <v>258</v>
       </c>
-      <c r="C3" s="47" t="s">
+      <c r="D3" s="45" t="s">
         <v>259</v>
       </c>
-      <c r="D3" s="45" t="s">
+      <c r="E3" s="46" t="s">
         <v>260</v>
       </c>
-      <c r="E3" s="46" t="s">
+      <c r="F3" s="46" t="s">
         <v>261</v>
       </c>
-      <c r="F3" s="46" t="s">
+      <c r="G3" s="46" t="s">
         <v>262</v>
       </c>
-      <c r="G3" s="46" t="s">
+      <c r="H3" s="46" t="s">
         <v>263</v>
       </c>
-      <c r="H3" s="46" t="s">
+      <c r="I3" s="46" t="s">
         <v>264</v>
       </c>
-      <c r="I3" s="46" t="s">
+      <c r="J3" s="46" t="s">
+        <v>277</v>
+      </c>
+      <c r="K3" s="55" t="s">
+        <v>278</v>
+      </c>
+      <c r="L3" s="55" t="s">
         <v>265</v>
-      </c>
-      <c r="J3" s="46" t="s">
-        <v>278</v>
-      </c>
-      <c r="K3" s="55" t="s">
-        <v>279</v>
-      </c>
-      <c r="L3" s="55" t="s">
-        <v>266</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
POCOR-7272: code enhancement for instituion report card new placeholder | Status: Done
</commit_message>
<xml_diff>
--- a/webroot/export/customexcel/default_templates/profile_template.xlsx
+++ b/webroot/export/customexcel/default_templates/profile_template.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20361"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp2\htdocs\pocor-openemis-core\webroot\export\customexcel\default_templates\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AAD42A9-0B8A-4158-94F0-1B50EF1C3A9A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10305" tabRatio="862" firstSheet="3" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10305" tabRatio="862"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -24,6 +18,7 @@
     <sheet name="Student Performance Summary" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="124519"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
@@ -32,84 +27,8 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>Microsoft Office User</author>
-  </authors>
-  <commentList>
-    <comment ref="F2" authorId="0" shapeId="0" xr:uid="{F01695D2-B671-4E84-9F87-A62CD3489B50}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Microsoft Office User:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>First Name + Middle Name + Third Name + Last Name</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H2" authorId="0" shapeId="0" xr:uid="{1D9C0F74-2025-4507-A482-610EFCC338CD}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Microsoft Office User:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Please account for case when subjects can have different weights. Simple average may not always work</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="288">
   <si>
     <t>${"image":{"displayValue":"Institutions.logo_content","imageWidth":"100","imageMarginLeft":"20","imageMarginTop":"5"}}</t>
   </si>
@@ -952,18 +871,36 @@
     <t>${InstitutionShiftType.occupier}</t>
   </si>
   <si>
-    <t xml:space="preserve"> Jordanian Students</t>
-  </si>
-  <si>
     <t>${"match": {"displayValue": "StudentFromEducationGrade.jordanian_students","rows": {"matchFrom": "StudentFromEducationGrade.education_grade_id","matchTo": "StudentFromEducationGrade.education_grade_id"}
 }}</t>
+  </si>
+  <si>
+    <t>Jordanian Students</t>
+  </si>
+  <si>
+    <t>${"match": {"displayValue": "StudentFromEducationGrade.male_student_promotion","rows": {"matchFrom": "StudentFromEducationGrade.education_grade_id","matchTo": "StudentFromEducationGrade.education_grade_id"}}}</t>
+  </si>
+  <si>
+    <t>${"match": {"displayValue": "StudentFromEducationGrade.female_student_promotion","rows": {"matchFrom": "StudentFromEducationGrade.education_grade_id","matchTo": "StudentFromEducationGrade.education_grade_id"}}}</t>
+  </si>
+  <si>
+    <t>${"match": {"displayValue": "StudentFromEducationGrade.total_student_promotion","rows": {"matchFrom": "StudentFromEducationGrade.education_grade_id","matchTo": "StudentFromEducationGrade.education_grade_id"}}}</t>
+  </si>
+  <si>
+    <t>Male Student Promotion Rate</t>
+  </si>
+  <si>
+    <t>Female Student Promotion Rate</t>
+  </si>
+  <si>
+    <t>Total Student Promotion Rate</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="16">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1037,19 +974,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -1083,7 +1007,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1094,6 +1018,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF0077D4"/>
         <bgColor rgb="FF008080"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1205,7 +1135,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1297,9 +1227,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1315,26 +1242,23 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -1360,11 +1284,20 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1494,7 +1427,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1526,27 +1459,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1578,24 +1493,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1771,14 +1668,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:IV1041"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" zoomScalePageLayoutView="60" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScalePageLayoutView="60" workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="63.140625" customWidth="1"/>
     <col min="2" max="2" width="54.28515625" customWidth="1"/>
@@ -1795,8 +1692,8 @@
     <col min="1024" max="1025" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="58" t="s">
+    <row r="1" spans="1:256" ht="15" customHeight="1">
+      <c r="A1" s="56" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4"/>
@@ -1816,14 +1713,14 @@
       <c r="P1" s="7"/>
       <c r="Q1" s="7"/>
     </row>
-    <row r="2" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="58"/>
-      <c r="B2" s="59" t="s">
+    <row r="2" spans="1:256" ht="25.5" customHeight="1">
+      <c r="A2" s="56"/>
+      <c r="B2" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="59"/>
-      <c r="D2" s="59"/>
-      <c r="E2" s="59"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
       <c r="F2" s="8"/>
       <c r="G2" s="9"/>
       <c r="H2" s="7"/>
@@ -2076,14 +1973,14 @@
       <c r="IU2" s="3"/>
       <c r="IV2" s="3"/>
     </row>
-    <row r="3" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="58"/>
-      <c r="B3" s="60" t="s">
+    <row r="3" spans="1:256" ht="25.5" customHeight="1">
+      <c r="A3" s="56"/>
+      <c r="B3" s="58" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="60"/>
-      <c r="D3" s="60"/>
-      <c r="E3" s="60"/>
+      <c r="C3" s="58"/>
+      <c r="D3" s="58"/>
+      <c r="E3" s="58"/>
       <c r="F3" s="9"/>
       <c r="G3" s="9"/>
       <c r="H3" s="7"/>
@@ -2336,8 +2233,8 @@
       <c r="IU3" s="3"/>
       <c r="IV3" s="3"/>
     </row>
-    <row r="4" spans="1:256" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="58"/>
+    <row r="4" spans="1:256" ht="22.5" customHeight="1">
+      <c r="A4" s="56"/>
       <c r="B4" s="4"/>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
@@ -2355,7 +2252,7 @@
       <c r="P4" s="7"/>
       <c r="Q4" s="7"/>
     </row>
-    <row r="5" spans="1:256" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:256" ht="15.75" customHeight="1">
       <c r="A5" s="10"/>
       <c r="B5" s="10"/>
       <c r="C5" s="10"/>
@@ -2375,7 +2272,7 @@
       <c r="Q5" s="7"/>
       <c r="R5" s="7"/>
     </row>
-    <row r="6" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:256" ht="12" customHeight="1">
       <c r="A6" s="11" t="s">
         <v>3</v>
       </c>
@@ -2399,7 +2296,7 @@
       <c r="Q6" s="7"/>
       <c r="R6" s="7"/>
     </row>
-    <row r="7" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:256" ht="12" customHeight="1">
       <c r="A7" s="11" t="s">
         <v>5</v>
       </c>
@@ -2423,7 +2320,7 @@
       <c r="Q7" s="7"/>
       <c r="R7" s="7"/>
     </row>
-    <row r="8" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:256" ht="12" customHeight="1">
       <c r="A8" s="11" t="s">
         <v>7</v>
       </c>
@@ -2447,7 +2344,7 @@
       <c r="Q8" s="7"/>
       <c r="R8" s="7"/>
     </row>
-    <row r="9" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:256" ht="12" customHeight="1">
       <c r="A9" s="11" t="s">
         <v>9</v>
       </c>
@@ -2471,7 +2368,7 @@
       <c r="Q9" s="7"/>
       <c r="R9" s="7"/>
     </row>
-    <row r="10" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:256" ht="12" customHeight="1">
       <c r="A10" s="11" t="s">
         <v>11</v>
       </c>
@@ -2495,7 +2392,7 @@
       <c r="Q10" s="7"/>
       <c r="R10" s="7"/>
     </row>
-    <row r="11" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:256" ht="12" customHeight="1">
       <c r="A11" s="11" t="s">
         <v>13</v>
       </c>
@@ -2757,7 +2654,7 @@
       <c r="IU11" s="3"/>
       <c r="IV11" s="3"/>
     </row>
-    <row r="12" spans="1:256" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:256" ht="16.5" customHeight="1">
       <c r="A12" s="16"/>
       <c r="B12" s="16"/>
       <c r="C12" s="16"/>
@@ -3015,7 +2912,7 @@
       <c r="IU12" s="3"/>
       <c r="IV12" s="3"/>
     </row>
-    <row r="13" spans="1:256" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:256" ht="16.5" customHeight="1">
       <c r="A13" s="11" t="s">
         <v>15</v>
       </c>
@@ -3277,7 +3174,7 @@
       <c r="IU13" s="3"/>
       <c r="IV13" s="3"/>
     </row>
-    <row r="14" spans="1:256" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:256" ht="16.5" customHeight="1">
       <c r="A14" s="11" t="s">
         <v>17</v>
       </c>
@@ -3539,7 +3436,7 @@
       <c r="IU14" s="3"/>
       <c r="IV14" s="3"/>
     </row>
-    <row r="15" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:256" ht="12" customHeight="1">
       <c r="A15" s="11" t="s">
         <v>19</v>
       </c>
@@ -3801,7 +3698,7 @@
       <c r="IU15" s="3"/>
       <c r="IV15" s="3"/>
     </row>
-    <row r="16" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:256" ht="12" customHeight="1">
       <c r="A16" s="11" t="s">
         <v>21</v>
       </c>
@@ -4063,7 +3960,7 @@
       <c r="IU16" s="3"/>
       <c r="IV16" s="3"/>
     </row>
-    <row r="17" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:256" ht="12" customHeight="1">
       <c r="A17" s="11" t="s">
         <v>23</v>
       </c>
@@ -4325,7 +4222,7 @@
       <c r="IU17" s="3"/>
       <c r="IV17" s="3"/>
     </row>
-    <row r="18" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:256" ht="12" customHeight="1">
       <c r="A18" s="11" t="s">
         <v>24</v>
       </c>
@@ -4587,7 +4484,7 @@
       <c r="IU18" s="3"/>
       <c r="IV18" s="3"/>
     </row>
-    <row r="19" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:256" ht="12" customHeight="1">
       <c r="A19" s="11" t="s">
         <v>26</v>
       </c>
@@ -4849,7 +4746,7 @@
       <c r="IU19" s="3"/>
       <c r="IV19" s="3"/>
     </row>
-    <row r="20" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:256" ht="12" customHeight="1">
       <c r="A20" s="11" t="s">
         <v>15</v>
       </c>
@@ -5111,7 +5008,7 @@
       <c r="IU20" s="3"/>
       <c r="IV20" s="3"/>
     </row>
-    <row r="21" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:256" ht="12" customHeight="1">
       <c r="A21" s="11" t="s">
         <v>28</v>
       </c>
@@ -5373,7 +5270,7 @@
       <c r="IU21" s="3"/>
       <c r="IV21" s="3"/>
     </row>
-    <row r="22" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:256" ht="12" customHeight="1">
       <c r="A22" s="11" t="s">
         <v>163</v>
       </c>
@@ -5635,7 +5532,7 @@
       <c r="IU22" s="3"/>
       <c r="IV22" s="3"/>
     </row>
-    <row r="23" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:256" ht="12" customHeight="1">
       <c r="A23" s="11" t="s">
         <v>165</v>
       </c>
@@ -5897,7 +5794,7 @@
       <c r="IU23" s="3"/>
       <c r="IV23" s="3"/>
     </row>
-    <row r="24" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:256" ht="12" customHeight="1">
       <c r="A24" s="11" t="s">
         <v>167</v>
       </c>
@@ -6159,7 +6056,7 @@
       <c r="IU24" s="3"/>
       <c r="IV24" s="3"/>
     </row>
-    <row r="25" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:256" ht="12" customHeight="1">
       <c r="A25" s="39"/>
       <c r="B25" s="39"/>
       <c r="C25" s="37"/>
@@ -6417,7 +6314,7 @@
       <c r="IU25" s="3"/>
       <c r="IV25" s="3"/>
     </row>
-    <row r="26" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:256" ht="12" customHeight="1">
       <c r="A26" s="39"/>
       <c r="B26" s="39"/>
       <c r="C26" s="37"/>
@@ -6675,7 +6572,7 @@
       <c r="IU26" s="3"/>
       <c r="IV26" s="3"/>
     </row>
-    <row r="27" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:256" ht="12" customHeight="1">
       <c r="A27" s="2" t="s">
         <v>30</v>
       </c>
@@ -6935,7 +6832,7 @@
       <c r="IU27" s="3"/>
       <c r="IV27" s="3"/>
     </row>
-    <row r="28" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:256" ht="12" customHeight="1">
       <c r="A28" s="9" t="s">
         <v>31</v>
       </c>
@@ -7199,7 +7096,7 @@
       <c r="IU28" s="3"/>
       <c r="IV28" s="3"/>
     </row>
-    <row r="29" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:256" ht="12" customHeight="1">
       <c r="A29" s="12" t="s">
         <v>34</v>
       </c>
@@ -7463,7 +7360,7 @@
       <c r="IU29" s="3"/>
       <c r="IV29" s="3"/>
     </row>
-    <row r="30" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:256" ht="12" customHeight="1">
       <c r="A30" s="7"/>
       <c r="B30" s="7"/>
       <c r="C30" s="7"/>
@@ -7721,7 +7618,7 @@
       <c r="IU30" s="3"/>
       <c r="IV30" s="3"/>
     </row>
-    <row r="31" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:256" ht="12" customHeight="1">
       <c r="A31" s="7"/>
       <c r="B31" s="7"/>
       <c r="C31" s="7"/>
@@ -7979,7 +7876,7 @@
       <c r="IU31" s="3"/>
       <c r="IV31" s="3"/>
     </row>
-    <row r="32" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:256" ht="12" customHeight="1">
       <c r="A32" s="20" t="s">
         <v>37</v>
       </c>
@@ -8241,7 +8138,7 @@
       <c r="IU32" s="3"/>
       <c r="IV32" s="3"/>
     </row>
-    <row r="33" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:256" ht="12" customHeight="1">
       <c r="A33" s="20" t="s">
         <v>39</v>
       </c>
@@ -8503,7 +8400,7 @@
       <c r="IU33" s="3"/>
       <c r="IV33" s="3"/>
     </row>
-    <row r="34" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:256" ht="12" customHeight="1">
       <c r="A34" s="17"/>
       <c r="B34" s="18"/>
       <c r="C34" s="18"/>
@@ -8761,7 +8658,7 @@
       <c r="IU34" s="3"/>
       <c r="IV34" s="3"/>
     </row>
-    <row r="35" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:256" ht="12" customHeight="1">
       <c r="A35" s="17"/>
       <c r="B35" s="18"/>
       <c r="C35" s="18"/>
@@ -9019,7 +8916,7 @@
       <c r="IU35" s="3"/>
       <c r="IV35" s="3"/>
     </row>
-    <row r="36" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:256" ht="12" customHeight="1">
       <c r="A36" s="20" t="s">
         <v>41</v>
       </c>
@@ -9281,7 +9178,7 @@
       <c r="IU36" s="3"/>
       <c r="IV36" s="3"/>
     </row>
-    <row r="37" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:256" ht="12" customHeight="1">
       <c r="A37" s="20" t="s">
         <v>43</v>
       </c>
@@ -9543,7 +9440,7 @@
       <c r="IU37" s="3"/>
       <c r="IV37" s="3"/>
     </row>
-    <row r="38" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:256" ht="12" customHeight="1">
       <c r="A38" s="17"/>
       <c r="B38" s="18"/>
       <c r="C38" s="18"/>
@@ -9801,7 +9698,7 @@
       <c r="IU38" s="3"/>
       <c r="IV38" s="3"/>
     </row>
-    <row r="39" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:256" ht="12" customHeight="1">
       <c r="A39" s="17"/>
       <c r="B39" s="18"/>
       <c r="C39" s="18"/>
@@ -10059,7 +9956,7 @@
       <c r="IU39" s="3"/>
       <c r="IV39" s="3"/>
     </row>
-    <row r="40" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:256" ht="12" customHeight="1">
       <c r="A40" s="21" t="s">
         <v>45</v>
       </c>
@@ -10321,7 +10218,7 @@
       <c r="IU40" s="3"/>
       <c r="IV40" s="3"/>
     </row>
-    <row r="41" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:256" ht="12" customHeight="1">
       <c r="A41" s="21" t="s">
         <v>47</v>
       </c>
@@ -10583,7 +10480,7 @@
       <c r="IU41" s="3"/>
       <c r="IV41" s="3"/>
     </row>
-    <row r="42" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:256" ht="12" customHeight="1">
       <c r="A42" s="17"/>
       <c r="B42" s="18"/>
       <c r="C42" s="18"/>
@@ -10841,7 +10738,7 @@
       <c r="IU42" s="3"/>
       <c r="IV42" s="3"/>
     </row>
-    <row r="43" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:256" ht="12" customHeight="1">
       <c r="A43" s="17"/>
       <c r="B43" s="18"/>
       <c r="C43" s="18"/>
@@ -11099,7 +10996,7 @@
       <c r="IU43" s="3"/>
       <c r="IV43" s="3"/>
     </row>
-    <row r="44" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:256" ht="12" customHeight="1">
       <c r="A44" s="11" t="s">
         <v>49</v>
       </c>
@@ -11361,7 +11258,7 @@
       <c r="IU44" s="3"/>
       <c r="IV44" s="3"/>
     </row>
-    <row r="45" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:256" ht="12" customHeight="1">
       <c r="A45" s="11" t="s">
         <v>51</v>
       </c>
@@ -11623,7 +11520,7 @@
       <c r="IU45" s="3"/>
       <c r="IV45" s="3"/>
     </row>
-    <row r="46" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:256" ht="12" customHeight="1">
       <c r="A46" s="11" t="s">
         <v>53</v>
       </c>
@@ -11885,7 +11782,7 @@
       <c r="IU46" s="3"/>
       <c r="IV46" s="3"/>
     </row>
-    <row r="47" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:256" ht="12" customHeight="1">
       <c r="A47" s="11" t="s">
         <v>55</v>
       </c>
@@ -12147,7 +12044,7 @@
       <c r="IU47" s="3"/>
       <c r="IV47" s="3"/>
     </row>
-    <row r="48" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:256" ht="12" customHeight="1">
       <c r="A48" s="11" t="s">
         <v>57</v>
       </c>
@@ -12409,7 +12306,7 @@
       <c r="IU48" s="3"/>
       <c r="IV48" s="3"/>
     </row>
-    <row r="49" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:256" ht="12" customHeight="1">
       <c r="A49" s="11" t="s">
         <v>59</v>
       </c>
@@ -12671,7 +12568,7 @@
       <c r="IU49" s="3"/>
       <c r="IV49" s="3"/>
     </row>
-    <row r="50" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:256" ht="12" customHeight="1">
       <c r="A50" s="11" t="s">
         <v>61</v>
       </c>
@@ -12933,7 +12830,7 @@
       <c r="IU50" s="3"/>
       <c r="IV50" s="3"/>
     </row>
-    <row r="51" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:256" ht="12" customHeight="1">
       <c r="A51" s="11" t="s">
         <v>63</v>
       </c>
@@ -13193,7 +13090,7 @@
       <c r="IU51" s="3"/>
       <c r="IV51" s="3"/>
     </row>
-    <row r="52" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:256" ht="12" customHeight="1">
       <c r="A52" s="11" t="s">
         <v>64</v>
       </c>
@@ -13455,7 +13352,7 @@
       <c r="IU52" s="3"/>
       <c r="IV52" s="3"/>
     </row>
-    <row r="53" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:256" ht="12" customHeight="1">
       <c r="A53" s="17"/>
       <c r="B53" s="18"/>
       <c r="C53" s="18"/>
@@ -13713,7 +13610,7 @@
       <c r="IU53" s="3"/>
       <c r="IV53" s="3"/>
     </row>
-    <row r="54" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:256" ht="12" customHeight="1">
       <c r="A54" s="17"/>
       <c r="B54" s="18"/>
       <c r="C54" s="18"/>
@@ -13971,7 +13868,7 @@
       <c r="IU54" s="3"/>
       <c r="IV54" s="3"/>
     </row>
-    <row r="55" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:256" ht="12" customHeight="1">
       <c r="A55" s="2" t="s">
         <v>141</v>
       </c>
@@ -14231,7 +14128,7 @@
       <c r="IU55" s="3"/>
       <c r="IV55" s="3"/>
     </row>
-    <row r="56" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:256" ht="12" customHeight="1">
       <c r="A56" s="33" t="s">
         <v>142</v>
       </c>
@@ -14495,7 +14392,7 @@
       <c r="IU56" s="3"/>
       <c r="IV56" s="3"/>
     </row>
-    <row r="57" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:256" ht="12" customHeight="1">
       <c r="A57" s="34" t="s">
         <v>145</v>
       </c>
@@ -14759,7 +14656,7 @@
       <c r="IU57" s="3"/>
       <c r="IV57" s="3"/>
     </row>
-    <row r="58" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:256" ht="12" customHeight="1">
       <c r="A58" s="34" t="s">
         <v>148</v>
       </c>
@@ -15023,7 +14920,7 @@
       <c r="IU58" s="3"/>
       <c r="IV58" s="3"/>
     </row>
-    <row r="59" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:256" ht="12" customHeight="1">
       <c r="A59" s="34" t="s">
         <v>151</v>
       </c>
@@ -15287,7 +15184,7 @@
       <c r="IU59" s="3"/>
       <c r="IV59" s="3"/>
     </row>
-    <row r="60" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:256" ht="12" customHeight="1">
       <c r="A60" s="34" t="s">
         <v>154</v>
       </c>
@@ -15551,7 +15448,7 @@
       <c r="IU60" s="3"/>
       <c r="IV60" s="3"/>
     </row>
-    <row r="61" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:256" ht="12" customHeight="1">
       <c r="A61" s="17"/>
       <c r="B61" s="18"/>
       <c r="C61" s="18"/>
@@ -15809,7 +15706,7 @@
       <c r="IU61" s="3"/>
       <c r="IV61" s="3"/>
     </row>
-    <row r="62" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:256" ht="12" customHeight="1">
       <c r="A62" s="1" t="s">
         <v>66</v>
       </c>
@@ -16069,7 +15966,7 @@
       <c r="IU62" s="3"/>
       <c r="IV62" s="3"/>
     </row>
-    <row r="63" spans="1:256" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:256" ht="16.5" customHeight="1">
       <c r="A63" s="23" t="s">
         <v>67</v>
       </c>
@@ -16093,7 +15990,7 @@
       <c r="Q63" s="7"/>
       <c r="R63" s="7"/>
     </row>
-    <row r="64" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:256" ht="12" customHeight="1">
       <c r="A64" s="25" t="s">
         <v>69</v>
       </c>
@@ -16355,7 +16252,7 @@
       <c r="IU64" s="3"/>
       <c r="IV64" s="3"/>
     </row>
-    <row r="65" spans="1:256" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:256" ht="15.95" customHeight="1">
       <c r="A65" s="3"/>
       <c r="B65" s="3"/>
       <c r="C65" s="7"/>
@@ -16613,7 +16510,7 @@
       <c r="IU65" s="3"/>
       <c r="IV65" s="3"/>
     </row>
-    <row r="66" spans="1:256" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:256" ht="15.95" customHeight="1">
       <c r="A66" s="3"/>
       <c r="B66" s="3"/>
       <c r="C66" s="7"/>
@@ -16871,7 +16768,7 @@
       <c r="IU66" s="3"/>
       <c r="IV66" s="3"/>
     </row>
-    <row r="67" spans="1:256" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:256" ht="15.95" customHeight="1">
       <c r="A67" s="3"/>
       <c r="B67" s="3"/>
       <c r="C67" s="7"/>
@@ -17129,7 +17026,7 @@
       <c r="IU67" s="3"/>
       <c r="IV67" s="3"/>
     </row>
-    <row r="68" spans="1:256" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:256" ht="15.95" customHeight="1">
       <c r="A68" s="3"/>
       <c r="B68" s="3"/>
       <c r="C68" s="7"/>
@@ -17387,7 +17284,7 @@
       <c r="IU68" s="3"/>
       <c r="IV68" s="3"/>
     </row>
-    <row r="69" spans="1:256" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:256">
       <c r="A69" s="3"/>
       <c r="B69" s="3"/>
       <c r="C69" s="7"/>
@@ -17645,7 +17542,7 @@
       <c r="IU69" s="3"/>
       <c r="IV69" s="3"/>
     </row>
-    <row r="70" spans="1:256" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:256" ht="15.75" customHeight="1">
       <c r="A70" s="3"/>
       <c r="B70" s="3"/>
       <c r="C70" s="7"/>
@@ -17903,7 +17800,7 @@
       <c r="IU70" s="3"/>
       <c r="IV70" s="3"/>
     </row>
-    <row r="71" spans="1:256" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:256" ht="15.75" customHeight="1">
       <c r="A71" s="3"/>
       <c r="B71" s="3"/>
       <c r="C71" s="3"/>
@@ -18161,7 +18058,7 @@
       <c r="IU71" s="3"/>
       <c r="IV71" s="3"/>
     </row>
-    <row r="72" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:256" ht="12" customHeight="1">
       <c r="A72" s="1" t="s">
         <v>194</v>
       </c>
@@ -18420,7 +18317,7 @@
       <c r="IU72" s="3"/>
       <c r="IV72" s="3"/>
     </row>
-    <row r="73" spans="1:256" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:256" ht="15.75" customHeight="1">
       <c r="A73" s="23" t="s">
         <v>195</v>
       </c>
@@ -18681,7 +18578,7 @@
       <c r="IU73" s="3"/>
       <c r="IV73" s="3"/>
     </row>
-    <row r="74" spans="1:256" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:256" ht="15.75" customHeight="1">
       <c r="A74" s="25" t="s">
         <v>197</v>
       </c>
@@ -18942,7 +18839,7 @@
       <c r="IU74" s="3"/>
       <c r="IV74" s="3"/>
     </row>
-    <row r="75" spans="1:256" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:256" ht="15.75" customHeight="1">
       <c r="A75" s="3"/>
       <c r="B75" s="3"/>
       <c r="C75" s="3"/>
@@ -19199,7 +19096,7 @@
       <c r="IU75" s="3"/>
       <c r="IV75" s="3"/>
     </row>
-    <row r="76" spans="1:256" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:256" ht="15.75" customHeight="1">
       <c r="E76" s="3"/>
       <c r="F76" s="3"/>
       <c r="G76" s="3"/>
@@ -19453,7 +19350,7 @@
       <c r="IU76" s="3"/>
       <c r="IV76" s="3"/>
     </row>
-    <row r="77" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:256" ht="12" customHeight="1">
       <c r="I77" s="7"/>
       <c r="J77" s="7"/>
       <c r="K77" s="7"/>
@@ -19465,27 +19362,27 @@
       <c r="Q77" s="7"/>
       <c r="R77" s="7"/>
     </row>
-    <row r="78" spans="1:256" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="79" spans="1:256" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="80" spans="1:256" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="81" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="82" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="83" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="84" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="85" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="86" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="87" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="88" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="89" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="90" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="91" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="92" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="93" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="94" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="95" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="96" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="97" spans="1:16" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="98" spans="1:16" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:256" ht="15.95" customHeight="1"/>
+    <row r="79" spans="1:256" ht="15.95" customHeight="1"/>
+    <row r="80" spans="1:256" ht="15.95" customHeight="1"/>
+    <row r="81" ht="15.95" customHeight="1"/>
+    <row r="82" ht="15.95" customHeight="1"/>
+    <row r="83" ht="15.95" customHeight="1"/>
+    <row r="84" ht="15.95" customHeight="1"/>
+    <row r="85" ht="15.95" customHeight="1"/>
+    <row r="86" ht="15.95" customHeight="1"/>
+    <row r="87" ht="15.95" customHeight="1"/>
+    <row r="88" ht="15.95" customHeight="1"/>
+    <row r="89" ht="15.95" customHeight="1"/>
+    <row r="90" ht="15.95" customHeight="1"/>
+    <row r="91" ht="15.95" customHeight="1"/>
+    <row r="92" ht="15.95" customHeight="1"/>
+    <row r="93" ht="15.95" customHeight="1"/>
+    <row r="94" ht="15.95" customHeight="1"/>
+    <row r="95" ht="15.95" customHeight="1"/>
+    <row r="96" ht="15.95" customHeight="1"/>
+    <row r="97" spans="1:16" ht="15.95" customHeight="1"/>
+    <row r="98" spans="1:16" ht="15.95" customHeight="1">
       <c r="A98" s="1" t="s">
         <v>200</v>
       </c>
@@ -19505,7 +19402,7 @@
       <c r="O98" s="1"/>
       <c r="P98" s="1"/>
     </row>
-    <row r="99" spans="1:16" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:16" ht="15.95" customHeight="1">
       <c r="A99" s="23" t="s">
         <v>201</v>
       </c>
@@ -19555,7 +19452,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="100" spans="1:16" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:16" ht="15.95" customHeight="1">
       <c r="A100" s="25" t="s">
         <v>217</v>
       </c>
@@ -19605,77 +19502,77 @@
         <v>232</v>
       </c>
     </row>
-    <row r="101" spans="1:16" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="102" spans="1:16" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="103" spans="1:16" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="104" spans="1:16" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="105" spans="1:16" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="106" spans="1:16" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="107" spans="1:16" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="108" spans="1:16" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="109" spans="1:16" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="110" spans="1:16" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="111" spans="1:16" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="112" spans="1:16" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="113" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="114" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="115" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="116" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="117" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="118" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="119" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="120" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="121" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="122" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="123" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="124" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="125" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="126" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="127" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="128" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="129" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="130" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="131" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="132" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="133" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="134" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="135" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="136" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="137" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="138" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="139" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="140" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="141" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="142" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="143" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="144" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="145" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="146" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="147" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="148" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="149" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="150" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="151" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="152" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="153" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="154" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="155" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="156" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="157" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="158" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="159" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="160" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="161" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="162" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="163" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="164" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="165" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="166" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="167" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="168" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="169" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="170" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="171" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:16" ht="15.95" customHeight="1"/>
+    <row r="102" spans="1:16" ht="15.95" customHeight="1"/>
+    <row r="103" spans="1:16" ht="15.95" customHeight="1"/>
+    <row r="104" spans="1:16" ht="15.95" customHeight="1"/>
+    <row r="105" spans="1:16" ht="15.95" customHeight="1"/>
+    <row r="106" spans="1:16" ht="15.95" customHeight="1"/>
+    <row r="107" spans="1:16" ht="15.95" customHeight="1"/>
+    <row r="108" spans="1:16" ht="15.95" customHeight="1"/>
+    <row r="109" spans="1:16" ht="15.95" customHeight="1"/>
+    <row r="110" spans="1:16" ht="15.95" customHeight="1"/>
+    <row r="111" spans="1:16" ht="15.95" customHeight="1"/>
+    <row r="112" spans="1:16" ht="15.95" customHeight="1"/>
+    <row r="113" ht="15.95" customHeight="1"/>
+    <row r="114" ht="15.95" customHeight="1"/>
+    <row r="115" ht="15.95" customHeight="1"/>
+    <row r="116" ht="15.95" customHeight="1"/>
+    <row r="117" ht="15.95" customHeight="1"/>
+    <row r="118" ht="15.95" customHeight="1"/>
+    <row r="119" ht="15.95" customHeight="1"/>
+    <row r="120" ht="15.95" customHeight="1"/>
+    <row r="121" ht="15.95" customHeight="1"/>
+    <row r="122" ht="15.95" customHeight="1"/>
+    <row r="123" ht="15.95" customHeight="1"/>
+    <row r="124" ht="15.95" customHeight="1"/>
+    <row r="125" ht="15.95" customHeight="1"/>
+    <row r="126" ht="15.95" customHeight="1"/>
+    <row r="127" ht="15.95" customHeight="1"/>
+    <row r="128" ht="15.95" customHeight="1"/>
+    <row r="129" ht="15.95" customHeight="1"/>
+    <row r="130" ht="15.95" customHeight="1"/>
+    <row r="131" ht="15.95" customHeight="1"/>
+    <row r="132" ht="15.95" customHeight="1"/>
+    <row r="133" ht="15.95" customHeight="1"/>
+    <row r="134" ht="15.95" customHeight="1"/>
+    <row r="135" ht="15.95" customHeight="1"/>
+    <row r="136" ht="15.95" customHeight="1"/>
+    <row r="137" ht="15.95" customHeight="1"/>
+    <row r="138" ht="15.95" customHeight="1"/>
+    <row r="139" ht="15.95" customHeight="1"/>
+    <row r="140" ht="15.95" customHeight="1"/>
+    <row r="141" ht="15.95" customHeight="1"/>
+    <row r="142" ht="15.95" customHeight="1"/>
+    <row r="143" ht="15.95" customHeight="1"/>
+    <row r="144" ht="15.95" customHeight="1"/>
+    <row r="145" ht="15.95" customHeight="1"/>
+    <row r="146" ht="15.95" customHeight="1"/>
+    <row r="147" ht="15.95" customHeight="1"/>
+    <row r="148" ht="15.95" customHeight="1"/>
+    <row r="149" ht="15.95" customHeight="1"/>
+    <row r="150" ht="15.95" customHeight="1"/>
+    <row r="151" ht="15.95" customHeight="1"/>
+    <row r="152" ht="15.95" customHeight="1"/>
+    <row r="153" ht="15.95" customHeight="1"/>
+    <row r="154" ht="15.95" customHeight="1"/>
+    <row r="155" ht="15.95" customHeight="1"/>
+    <row r="156" ht="15.95" customHeight="1"/>
+    <row r="157" ht="15.95" customHeight="1"/>
+    <row r="158" ht="15.95" customHeight="1"/>
+    <row r="159" ht="15.95" customHeight="1"/>
+    <row r="160" ht="15.95" customHeight="1"/>
+    <row r="161" spans="1:6" ht="15.95" customHeight="1"/>
+    <row r="162" spans="1:6" ht="15.95" customHeight="1"/>
+    <row r="163" spans="1:6" ht="15.95" customHeight="1"/>
+    <row r="164" spans="1:6" ht="15.95" customHeight="1"/>
+    <row r="165" spans="1:6" ht="15.95" customHeight="1"/>
+    <row r="166" spans="1:6" ht="15.95" customHeight="1"/>
+    <row r="167" spans="1:6" ht="15.95" customHeight="1"/>
+    <row r="168" spans="1:6" ht="15.95" customHeight="1"/>
+    <row r="169" spans="1:6" ht="15.95" customHeight="1"/>
+    <row r="170" spans="1:6" ht="15.95" customHeight="1"/>
+    <row r="171" spans="1:6" ht="15.95" customHeight="1">
       <c r="A171" s="1" t="s">
         <v>199</v>
       </c>
@@ -19685,7 +19582,7 @@
       <c r="E171" s="1"/>
       <c r="F171" s="1"/>
     </row>
-    <row r="172" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:6" ht="15.95" customHeight="1">
       <c r="A172" s="23" t="s">
         <v>233</v>
       </c>
@@ -19705,7 +19602,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="173" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:6" ht="15.95" customHeight="1">
       <c r="A173" s="25" t="s">
         <v>239</v>
       </c>
@@ -19725,874 +19622,874 @@
         <v>244</v>
       </c>
     </row>
-    <row r="174" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="175" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="176" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="177" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="178" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="179" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="180" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="181" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="182" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="183" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="184" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="185" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="186" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="187" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="188" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="189" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="190" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="191" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="192" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="193" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="194" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="195" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="196" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="197" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="198" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="199" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="200" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="201" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="202" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="203" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="204" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="205" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="206" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="207" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="208" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="209" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="210" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="211" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="212" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="213" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="214" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="215" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="216" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="217" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="218" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="219" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="220" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="221" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="222" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="223" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="224" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="225" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="226" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="227" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="228" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="229" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="230" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="231" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="232" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="233" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="234" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="235" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="236" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="237" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="238" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="239" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="240" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="241" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="242" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="243" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="244" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="245" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="246" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="247" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="248" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="249" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="250" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="251" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="252" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="253" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="254" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="255" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="256" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="257" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="258" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="259" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="260" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="261" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="262" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="263" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="264" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="265" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="266" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="267" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="268" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="269" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="270" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="271" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="272" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="273" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="274" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="275" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="276" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="277" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="278" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="279" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="280" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="281" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="282" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="283" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="284" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="285" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="286" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="287" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="288" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="289" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="290" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="291" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="292" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="293" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="294" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="295" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="296" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="297" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="298" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="299" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="300" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="301" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="302" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="303" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="304" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="305" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="306" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="307" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="308" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="309" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="310" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="311" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="312" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="313" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="314" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="315" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="316" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="317" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="318" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="319" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="320" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="321" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="322" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="323" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="324" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="325" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="326" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="327" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="328" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="329" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="330" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="331" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="332" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="333" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="334" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="335" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="336" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="337" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="338" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="339" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="340" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="341" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="342" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="343" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="344" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="345" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="346" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="347" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="348" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="349" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="350" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="351" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="352" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="353" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="354" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="355" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="356" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="357" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="358" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="359" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="360" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="361" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="362" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="363" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="364" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="365" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="366" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="367" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="368" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="369" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="370" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="371" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="372" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="373" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="374" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="375" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="376" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="377" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="378" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="379" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="380" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="381" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="382" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="383" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="384" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="385" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="386" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="387" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="388" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="389" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="390" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="391" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="392" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="393" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="394" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="395" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="396" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="397" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="398" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="399" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="400" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="401" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="402" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="403" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="404" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="405" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="406" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="407" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="408" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="409" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="410" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="411" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="412" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="413" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="414" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="415" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="416" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="417" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="418" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="419" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="420" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="421" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="422" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="423" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="424" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="425" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="426" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="427" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="428" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="429" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="430" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="431" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="432" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="433" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="434" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="435" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="436" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="437" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="438" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="439" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="440" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="441" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="442" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="443" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="444" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="445" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="446" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="447" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="448" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="449" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="450" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="451" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="452" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="453" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="454" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="455" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="456" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="457" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="458" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="459" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="460" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="461" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="462" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="463" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="464" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="465" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="466" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="467" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="468" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="469" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="470" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="471" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="472" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="473" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="474" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="475" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="476" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="477" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="478" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="479" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="480" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="481" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="482" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="483" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="484" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="485" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="486" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="487" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="488" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="489" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="490" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="491" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="492" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="493" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="494" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="495" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="496" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="497" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="498" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="499" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="500" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="501" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="502" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="503" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="504" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="505" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="506" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="507" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="508" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="509" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="510" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="511" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="512" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="513" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="514" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="515" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="516" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="517" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="518" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="519" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="520" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="521" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="522" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="523" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="524" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="525" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="526" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="527" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="528" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="529" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="530" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="531" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="532" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="533" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="534" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="535" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="536" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="537" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="538" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="539" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="540" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="541" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="542" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="543" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="544" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="545" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="546" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="547" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="548" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="549" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="550" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="551" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="552" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="553" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="554" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="555" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="556" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="557" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="558" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="559" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="560" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="561" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="562" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="563" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="564" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="565" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="566" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="567" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="568" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="569" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="570" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="571" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="572" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="573" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="574" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="575" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="576" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="577" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="578" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="579" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="580" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="581" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="582" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="583" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="584" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="585" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="586" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="587" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="588" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="589" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="590" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="591" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="592" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="593" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="594" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="595" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="596" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="597" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="598" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="599" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="600" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="601" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="602" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="603" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="604" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="605" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="606" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="607" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="608" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="609" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="610" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="611" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="612" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="613" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="614" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="615" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="616" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="617" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="618" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="619" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="620" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="621" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="622" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="623" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="624" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="625" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="626" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="627" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="628" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="629" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="630" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="631" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="632" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="633" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="634" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="635" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="636" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="637" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="638" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="639" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="640" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="641" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="642" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="643" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="644" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="645" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="646" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="647" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="648" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="649" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="650" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="651" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="652" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="653" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="654" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="655" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="656" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="657" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="658" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="659" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="660" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="661" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="662" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="663" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="664" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="665" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="666" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="667" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="668" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="669" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="670" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="671" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="672" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="673" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="674" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="675" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="676" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="677" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="678" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="679" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="680" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="681" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="682" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="683" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="684" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="685" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="686" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="687" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="688" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="689" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="690" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="691" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="692" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="693" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="694" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="695" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="696" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="697" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="698" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="699" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="700" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="701" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="702" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="703" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="704" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="705" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="706" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="707" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="708" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="709" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="710" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="711" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="712" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="713" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="714" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="715" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="716" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="717" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="718" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="719" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="720" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="721" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="722" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="723" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="724" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="725" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="726" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="727" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="728" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="729" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="730" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="731" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="732" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="733" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="734" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="735" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="736" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="737" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="738" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="739" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="740" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="741" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="742" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="743" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="744" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="745" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="746" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="747" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="748" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="749" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="750" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="751" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="752" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="753" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="754" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="755" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="756" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="757" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="758" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="759" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="760" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="761" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="762" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="763" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="764" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="765" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="766" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="767" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="768" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="769" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="770" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="771" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="772" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="773" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="774" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="775" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="776" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="777" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="778" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="779" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="780" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="781" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="782" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="783" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="784" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="785" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="786" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="787" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="788" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="789" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="790" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="791" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="792" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="793" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="794" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="795" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="796" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="797" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="798" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="799" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="800" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="801" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="802" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="803" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="804" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="805" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="806" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="807" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="808" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="809" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="810" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="811" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="812" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="813" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="814" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="815" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="816" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="817" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="818" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="819" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="820" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="821" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="822" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="823" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="824" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="825" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="826" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="827" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="828" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="829" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="830" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="831" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="832" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="833" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="834" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="835" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="836" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="837" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="838" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="839" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="840" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="841" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="842" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="843" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="844" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="845" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="846" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="847" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="848" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="849" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="850" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="851" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="852" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="853" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="854" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="855" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="856" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="857" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="858" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="859" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="860" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="861" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="862" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="863" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="864" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="865" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="866" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="867" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="868" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="869" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="870" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="871" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="872" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="873" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="874" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="875" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="876" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="877" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="878" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="879" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="880" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="881" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="882" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="883" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="884" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="885" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="886" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="887" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="888" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="889" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="890" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="891" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="892" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="893" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="894" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="895" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="896" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="897" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="898" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="899" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="900" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="901" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="902" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="903" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="904" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="905" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="906" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="907" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="908" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="909" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="910" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="911" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="912" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="913" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="914" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="915" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="916" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="917" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="918" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="919" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="920" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="921" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="922" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="923" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="924" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="925" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="926" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="927" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="928" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="929" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="930" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="931" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="932" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="933" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="934" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="935" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="936" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="937" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="938" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="939" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="940" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="941" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="942" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="943" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="944" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="945" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="946" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="947" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="948" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="949" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="950" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="951" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="952" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="953" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="954" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="955" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="956" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="957" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="958" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="959" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="960" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="961" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="962" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="963" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="964" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="965" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="966" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="967" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="968" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="969" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="970" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="971" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="972" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="973" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="974" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="975" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="976" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="977" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="978" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="979" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="980" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="981" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="982" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="983" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="984" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="985" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="986" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="987" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="988" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="989" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="990" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="991" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="992" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="993" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="994" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="995" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="996" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="997" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="998" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="999" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1000" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1001" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1002" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1003" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1004" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1005" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1006" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1007" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1008" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1009" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1010" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1011" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1012" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1013" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1014" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1015" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1016" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1017" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1018" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1019" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1020" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1021" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1022" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1023" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1024" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1025" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1026" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1027" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1028" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1029" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1030" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1031" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1032" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1033" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1034" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1035" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1036" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1037" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1038" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1039" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1040" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1041" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="174" spans="1:6" ht="15.95" customHeight="1"/>
+    <row r="175" spans="1:6" ht="15.95" customHeight="1"/>
+    <row r="176" spans="1:6" ht="15.95" customHeight="1"/>
+    <row r="177" ht="15.95" customHeight="1"/>
+    <row r="178" ht="15.95" customHeight="1"/>
+    <row r="179" ht="15.95" customHeight="1"/>
+    <row r="180" ht="15.95" customHeight="1"/>
+    <row r="181" ht="15.95" customHeight="1"/>
+    <row r="182" ht="15.95" customHeight="1"/>
+    <row r="183" ht="15.95" customHeight="1"/>
+    <row r="184" ht="15.95" customHeight="1"/>
+    <row r="185" ht="15.95" customHeight="1"/>
+    <row r="186" ht="15.95" customHeight="1"/>
+    <row r="187" ht="15.95" customHeight="1"/>
+    <row r="188" ht="15.95" customHeight="1"/>
+    <row r="189" ht="15.95" customHeight="1"/>
+    <row r="190" ht="15.95" customHeight="1"/>
+    <row r="191" ht="15.95" customHeight="1"/>
+    <row r="192" ht="15.95" customHeight="1"/>
+    <row r="193" ht="15.95" customHeight="1"/>
+    <row r="194" ht="15.95" customHeight="1"/>
+    <row r="195" ht="15.95" customHeight="1"/>
+    <row r="196" ht="15.95" customHeight="1"/>
+    <row r="197" ht="15.95" customHeight="1"/>
+    <row r="198" ht="15.95" customHeight="1"/>
+    <row r="199" ht="15.95" customHeight="1"/>
+    <row r="200" ht="15.95" customHeight="1"/>
+    <row r="201" ht="15.95" customHeight="1"/>
+    <row r="202" ht="15.95" customHeight="1"/>
+    <row r="203" ht="15.95" customHeight="1"/>
+    <row r="204" ht="15.95" customHeight="1"/>
+    <row r="205" ht="15.95" customHeight="1"/>
+    <row r="206" ht="15.95" customHeight="1"/>
+    <row r="207" ht="15.95" customHeight="1"/>
+    <row r="208" ht="15.95" customHeight="1"/>
+    <row r="209" ht="15.95" customHeight="1"/>
+    <row r="210" ht="15.95" customHeight="1"/>
+    <row r="211" ht="15.95" customHeight="1"/>
+    <row r="212" ht="15.95" customHeight="1"/>
+    <row r="213" ht="15.95" customHeight="1"/>
+    <row r="214" ht="15.95" customHeight="1"/>
+    <row r="215" ht="15.95" customHeight="1"/>
+    <row r="216" ht="15.95" customHeight="1"/>
+    <row r="217" ht="15.95" customHeight="1"/>
+    <row r="218" ht="15.95" customHeight="1"/>
+    <row r="219" ht="15.95" customHeight="1"/>
+    <row r="220" ht="15.95" customHeight="1"/>
+    <row r="221" ht="15.95" customHeight="1"/>
+    <row r="222" ht="15.95" customHeight="1"/>
+    <row r="223" ht="15.95" customHeight="1"/>
+    <row r="224" ht="15.95" customHeight="1"/>
+    <row r="225" ht="15.95" customHeight="1"/>
+    <row r="226" ht="15.95" customHeight="1"/>
+    <row r="227" ht="15.95" customHeight="1"/>
+    <row r="228" ht="15.95" customHeight="1"/>
+    <row r="229" ht="15.95" customHeight="1"/>
+    <row r="230" ht="15.95" customHeight="1"/>
+    <row r="231" ht="15.95" customHeight="1"/>
+    <row r="232" ht="15.95" customHeight="1"/>
+    <row r="233" ht="15.95" customHeight="1"/>
+    <row r="234" ht="15.95" customHeight="1"/>
+    <row r="235" ht="15.95" customHeight="1"/>
+    <row r="236" ht="15.95" customHeight="1"/>
+    <row r="237" ht="15.95" customHeight="1"/>
+    <row r="238" ht="15.95" customHeight="1"/>
+    <row r="239" ht="15.95" customHeight="1"/>
+    <row r="240" ht="15.95" customHeight="1"/>
+    <row r="241" ht="15.95" customHeight="1"/>
+    <row r="242" ht="15.95" customHeight="1"/>
+    <row r="243" ht="15.95" customHeight="1"/>
+    <row r="244" ht="15.95" customHeight="1"/>
+    <row r="245" ht="15.95" customHeight="1"/>
+    <row r="246" ht="15.95" customHeight="1"/>
+    <row r="247" ht="15.95" customHeight="1"/>
+    <row r="248" ht="15.95" customHeight="1"/>
+    <row r="249" ht="15.95" customHeight="1"/>
+    <row r="250" ht="15.95" customHeight="1"/>
+    <row r="251" ht="15.95" customHeight="1"/>
+    <row r="252" ht="15.95" customHeight="1"/>
+    <row r="253" ht="15.95" customHeight="1"/>
+    <row r="254" ht="15.95" customHeight="1"/>
+    <row r="255" ht="15.95" customHeight="1"/>
+    <row r="256" ht="15.95" customHeight="1"/>
+    <row r="257" ht="15.95" customHeight="1"/>
+    <row r="258" ht="15.95" customHeight="1"/>
+    <row r="259" ht="15.95" customHeight="1"/>
+    <row r="260" ht="15.95" customHeight="1"/>
+    <row r="261" ht="15.95" customHeight="1"/>
+    <row r="262" ht="15.95" customHeight="1"/>
+    <row r="263" ht="15.95" customHeight="1"/>
+    <row r="264" ht="15.95" customHeight="1"/>
+    <row r="265" ht="15.95" customHeight="1"/>
+    <row r="266" ht="15.95" customHeight="1"/>
+    <row r="267" ht="15.95" customHeight="1"/>
+    <row r="268" ht="15.95" customHeight="1"/>
+    <row r="269" ht="15.95" customHeight="1"/>
+    <row r="270" ht="15.95" customHeight="1"/>
+    <row r="271" ht="15.95" customHeight="1"/>
+    <row r="272" ht="15.95" customHeight="1"/>
+    <row r="273" ht="15.95" customHeight="1"/>
+    <row r="274" ht="15.95" customHeight="1"/>
+    <row r="275" ht="15.95" customHeight="1"/>
+    <row r="276" ht="15.95" customHeight="1"/>
+    <row r="277" ht="15.95" customHeight="1"/>
+    <row r="278" ht="15.95" customHeight="1"/>
+    <row r="279" ht="15.95" customHeight="1"/>
+    <row r="280" ht="15.95" customHeight="1"/>
+    <row r="281" ht="15.95" customHeight="1"/>
+    <row r="282" ht="15.95" customHeight="1"/>
+    <row r="283" ht="15.95" customHeight="1"/>
+    <row r="284" ht="15.95" customHeight="1"/>
+    <row r="285" ht="15.95" customHeight="1"/>
+    <row r="286" ht="15.95" customHeight="1"/>
+    <row r="287" ht="15.95" customHeight="1"/>
+    <row r="288" ht="15.95" customHeight="1"/>
+    <row r="289" ht="15.95" customHeight="1"/>
+    <row r="290" ht="15.95" customHeight="1"/>
+    <row r="291" ht="15.95" customHeight="1"/>
+    <row r="292" ht="15.95" customHeight="1"/>
+    <row r="293" ht="15.95" customHeight="1"/>
+    <row r="294" ht="15.95" customHeight="1"/>
+    <row r="295" ht="15.95" customHeight="1"/>
+    <row r="296" ht="15.95" customHeight="1"/>
+    <row r="297" ht="15.95" customHeight="1"/>
+    <row r="298" ht="15.95" customHeight="1"/>
+    <row r="299" ht="15.95" customHeight="1"/>
+    <row r="300" ht="15.95" customHeight="1"/>
+    <row r="301" ht="15.95" customHeight="1"/>
+    <row r="302" ht="15.95" customHeight="1"/>
+    <row r="303" ht="15.95" customHeight="1"/>
+    <row r="304" ht="15.95" customHeight="1"/>
+    <row r="305" ht="15.95" customHeight="1"/>
+    <row r="306" ht="15.95" customHeight="1"/>
+    <row r="307" ht="15.95" customHeight="1"/>
+    <row r="308" ht="15.95" customHeight="1"/>
+    <row r="309" ht="15.95" customHeight="1"/>
+    <row r="310" ht="15.95" customHeight="1"/>
+    <row r="311" ht="15.95" customHeight="1"/>
+    <row r="312" ht="15.95" customHeight="1"/>
+    <row r="313" ht="15.95" customHeight="1"/>
+    <row r="314" ht="15.95" customHeight="1"/>
+    <row r="315" ht="15.95" customHeight="1"/>
+    <row r="316" ht="15.95" customHeight="1"/>
+    <row r="317" ht="15.95" customHeight="1"/>
+    <row r="318" ht="15.95" customHeight="1"/>
+    <row r="319" ht="15.95" customHeight="1"/>
+    <row r="320" ht="15.95" customHeight="1"/>
+    <row r="321" ht="15.95" customHeight="1"/>
+    <row r="322" ht="15.95" customHeight="1"/>
+    <row r="323" ht="15.95" customHeight="1"/>
+    <row r="324" ht="15.95" customHeight="1"/>
+    <row r="325" ht="15.95" customHeight="1"/>
+    <row r="326" ht="15.95" customHeight="1"/>
+    <row r="327" ht="15.95" customHeight="1"/>
+    <row r="328" ht="15.95" customHeight="1"/>
+    <row r="329" ht="15.95" customHeight="1"/>
+    <row r="330" ht="15.95" customHeight="1"/>
+    <row r="331" ht="15.95" customHeight="1"/>
+    <row r="332" ht="15.95" customHeight="1"/>
+    <row r="333" ht="15.95" customHeight="1"/>
+    <row r="334" ht="15.95" customHeight="1"/>
+    <row r="335" ht="15.95" customHeight="1"/>
+    <row r="336" ht="15.95" customHeight="1"/>
+    <row r="337" ht="15.95" customHeight="1"/>
+    <row r="338" ht="15.95" customHeight="1"/>
+    <row r="339" ht="15.95" customHeight="1"/>
+    <row r="340" ht="15.95" customHeight="1"/>
+    <row r="341" ht="15.95" customHeight="1"/>
+    <row r="342" ht="15.95" customHeight="1"/>
+    <row r="343" ht="15.95" customHeight="1"/>
+    <row r="344" ht="15.95" customHeight="1"/>
+    <row r="345" ht="15.95" customHeight="1"/>
+    <row r="346" ht="15.95" customHeight="1"/>
+    <row r="347" ht="15.95" customHeight="1"/>
+    <row r="348" ht="15.95" customHeight="1"/>
+    <row r="349" ht="15.95" customHeight="1"/>
+    <row r="350" ht="15.95" customHeight="1"/>
+    <row r="351" ht="15.95" customHeight="1"/>
+    <row r="352" ht="15.95" customHeight="1"/>
+    <row r="353" ht="15.95" customHeight="1"/>
+    <row r="354" ht="15.95" customHeight="1"/>
+    <row r="355" ht="15.95" customHeight="1"/>
+    <row r="356" ht="15.95" customHeight="1"/>
+    <row r="357" ht="15.95" customHeight="1"/>
+    <row r="358" ht="15.95" customHeight="1"/>
+    <row r="359" ht="15.95" customHeight="1"/>
+    <row r="360" ht="15.95" customHeight="1"/>
+    <row r="361" ht="15.95" customHeight="1"/>
+    <row r="362" ht="15.95" customHeight="1"/>
+    <row r="363" ht="15.95" customHeight="1"/>
+    <row r="364" ht="15.95" customHeight="1"/>
+    <row r="365" ht="15.95" customHeight="1"/>
+    <row r="366" ht="15.95" customHeight="1"/>
+    <row r="367" ht="15.95" customHeight="1"/>
+    <row r="368" ht="15.95" customHeight="1"/>
+    <row r="369" ht="15.95" customHeight="1"/>
+    <row r="370" ht="15.95" customHeight="1"/>
+    <row r="371" ht="15.95" customHeight="1"/>
+    <row r="372" ht="15.95" customHeight="1"/>
+    <row r="373" ht="15.95" customHeight="1"/>
+    <row r="374" ht="15.95" customHeight="1"/>
+    <row r="375" ht="15.95" customHeight="1"/>
+    <row r="376" ht="15.95" customHeight="1"/>
+    <row r="377" ht="15.95" customHeight="1"/>
+    <row r="378" ht="15.95" customHeight="1"/>
+    <row r="379" ht="15.95" customHeight="1"/>
+    <row r="380" ht="15.95" customHeight="1"/>
+    <row r="381" ht="15.95" customHeight="1"/>
+    <row r="382" ht="15.95" customHeight="1"/>
+    <row r="383" ht="15.95" customHeight="1"/>
+    <row r="384" ht="15.95" customHeight="1"/>
+    <row r="385" ht="15.95" customHeight="1"/>
+    <row r="386" ht="15.95" customHeight="1"/>
+    <row r="387" ht="15.95" customHeight="1"/>
+    <row r="388" ht="15.95" customHeight="1"/>
+    <row r="389" ht="15.95" customHeight="1"/>
+    <row r="390" ht="15.95" customHeight="1"/>
+    <row r="391" ht="15.95" customHeight="1"/>
+    <row r="392" ht="15.95" customHeight="1"/>
+    <row r="393" ht="15.95" customHeight="1"/>
+    <row r="394" ht="15.95" customHeight="1"/>
+    <row r="395" ht="15.95" customHeight="1"/>
+    <row r="396" ht="15.95" customHeight="1"/>
+    <row r="397" ht="15.95" customHeight="1"/>
+    <row r="398" ht="15.95" customHeight="1"/>
+    <row r="399" ht="15.95" customHeight="1"/>
+    <row r="400" ht="15.95" customHeight="1"/>
+    <row r="401" ht="15.95" customHeight="1"/>
+    <row r="402" ht="15.95" customHeight="1"/>
+    <row r="403" ht="15.95" customHeight="1"/>
+    <row r="404" ht="15.95" customHeight="1"/>
+    <row r="405" ht="15.95" customHeight="1"/>
+    <row r="406" ht="15.95" customHeight="1"/>
+    <row r="407" ht="15.95" customHeight="1"/>
+    <row r="408" ht="15.95" customHeight="1"/>
+    <row r="409" ht="15.95" customHeight="1"/>
+    <row r="410" ht="15.95" customHeight="1"/>
+    <row r="411" ht="15.95" customHeight="1"/>
+    <row r="412" ht="15.95" customHeight="1"/>
+    <row r="413" ht="15.95" customHeight="1"/>
+    <row r="414" ht="15.95" customHeight="1"/>
+    <row r="415" ht="15.95" customHeight="1"/>
+    <row r="416" ht="15.95" customHeight="1"/>
+    <row r="417" ht="15.95" customHeight="1"/>
+    <row r="418" ht="15.95" customHeight="1"/>
+    <row r="419" ht="15.95" customHeight="1"/>
+    <row r="420" ht="15.95" customHeight="1"/>
+    <row r="421" ht="15.95" customHeight="1"/>
+    <row r="422" ht="15.95" customHeight="1"/>
+    <row r="423" ht="15.95" customHeight="1"/>
+    <row r="424" ht="15.95" customHeight="1"/>
+    <row r="425" ht="15.95" customHeight="1"/>
+    <row r="426" ht="15.95" customHeight="1"/>
+    <row r="427" ht="15.95" customHeight="1"/>
+    <row r="428" ht="15.95" customHeight="1"/>
+    <row r="429" ht="15.95" customHeight="1"/>
+    <row r="430" ht="15.95" customHeight="1"/>
+    <row r="431" ht="15.95" customHeight="1"/>
+    <row r="432" ht="15.95" customHeight="1"/>
+    <row r="433" ht="15.95" customHeight="1"/>
+    <row r="434" ht="15.95" customHeight="1"/>
+    <row r="435" ht="15.95" customHeight="1"/>
+    <row r="436" ht="15.95" customHeight="1"/>
+    <row r="437" ht="15.95" customHeight="1"/>
+    <row r="438" ht="15.95" customHeight="1"/>
+    <row r="439" ht="15.95" customHeight="1"/>
+    <row r="440" ht="15.95" customHeight="1"/>
+    <row r="441" ht="15.95" customHeight="1"/>
+    <row r="442" ht="15.95" customHeight="1"/>
+    <row r="443" ht="15.95" customHeight="1"/>
+    <row r="444" ht="15.95" customHeight="1"/>
+    <row r="445" ht="15.95" customHeight="1"/>
+    <row r="446" ht="15.95" customHeight="1"/>
+    <row r="447" ht="15.95" customHeight="1"/>
+    <row r="448" ht="15.95" customHeight="1"/>
+    <row r="449" ht="15.95" customHeight="1"/>
+    <row r="450" ht="15.95" customHeight="1"/>
+    <row r="451" ht="15.95" customHeight="1"/>
+    <row r="452" ht="15.95" customHeight="1"/>
+    <row r="453" ht="15.95" customHeight="1"/>
+    <row r="454" ht="15.95" customHeight="1"/>
+    <row r="455" ht="15.95" customHeight="1"/>
+    <row r="456" ht="15.95" customHeight="1"/>
+    <row r="457" ht="15.95" customHeight="1"/>
+    <row r="458" ht="15.95" customHeight="1"/>
+    <row r="459" ht="15.95" customHeight="1"/>
+    <row r="460" ht="15.95" customHeight="1"/>
+    <row r="461" ht="15.95" customHeight="1"/>
+    <row r="462" ht="15.95" customHeight="1"/>
+    <row r="463" ht="15.95" customHeight="1"/>
+    <row r="464" ht="15.95" customHeight="1"/>
+    <row r="465" ht="15.95" customHeight="1"/>
+    <row r="466" ht="15.95" customHeight="1"/>
+    <row r="467" ht="15.95" customHeight="1"/>
+    <row r="468" ht="15.95" customHeight="1"/>
+    <row r="469" ht="15.95" customHeight="1"/>
+    <row r="470" ht="15.95" customHeight="1"/>
+    <row r="471" ht="15.95" customHeight="1"/>
+    <row r="472" ht="15.95" customHeight="1"/>
+    <row r="473" ht="15.95" customHeight="1"/>
+    <row r="474" ht="15.95" customHeight="1"/>
+    <row r="475" ht="15.95" customHeight="1"/>
+    <row r="476" ht="15.95" customHeight="1"/>
+    <row r="477" ht="15.95" customHeight="1"/>
+    <row r="478" ht="15.95" customHeight="1"/>
+    <row r="479" ht="15.95" customHeight="1"/>
+    <row r="480" ht="15.95" customHeight="1"/>
+    <row r="481" ht="15.95" customHeight="1"/>
+    <row r="482" ht="15.95" customHeight="1"/>
+    <row r="483" ht="15.95" customHeight="1"/>
+    <row r="484" ht="15.95" customHeight="1"/>
+    <row r="485" ht="15.95" customHeight="1"/>
+    <row r="486" ht="15.95" customHeight="1"/>
+    <row r="487" ht="15.95" customHeight="1"/>
+    <row r="488" ht="15.95" customHeight="1"/>
+    <row r="489" ht="15.95" customHeight="1"/>
+    <row r="490" ht="15.95" customHeight="1"/>
+    <row r="491" ht="15.95" customHeight="1"/>
+    <row r="492" ht="15.95" customHeight="1"/>
+    <row r="493" ht="15.95" customHeight="1"/>
+    <row r="494" ht="15.95" customHeight="1"/>
+    <row r="495" ht="15.95" customHeight="1"/>
+    <row r="496" ht="15.95" customHeight="1"/>
+    <row r="497" ht="15.95" customHeight="1"/>
+    <row r="498" ht="15.95" customHeight="1"/>
+    <row r="499" ht="15.95" customHeight="1"/>
+    <row r="500" ht="15.95" customHeight="1"/>
+    <row r="501" ht="15.95" customHeight="1"/>
+    <row r="502" ht="15.95" customHeight="1"/>
+    <row r="503" ht="15.95" customHeight="1"/>
+    <row r="504" ht="15.95" customHeight="1"/>
+    <row r="505" ht="15.95" customHeight="1"/>
+    <row r="506" ht="15.95" customHeight="1"/>
+    <row r="507" ht="15.95" customHeight="1"/>
+    <row r="508" ht="15.95" customHeight="1"/>
+    <row r="509" ht="15.95" customHeight="1"/>
+    <row r="510" ht="15.95" customHeight="1"/>
+    <row r="511" ht="15.95" customHeight="1"/>
+    <row r="512" ht="15.95" customHeight="1"/>
+    <row r="513" ht="15.95" customHeight="1"/>
+    <row r="514" ht="15.95" customHeight="1"/>
+    <row r="515" ht="15.95" customHeight="1"/>
+    <row r="516" ht="15.95" customHeight="1"/>
+    <row r="517" ht="15.95" customHeight="1"/>
+    <row r="518" ht="15.95" customHeight="1"/>
+    <row r="519" ht="15.95" customHeight="1"/>
+    <row r="520" ht="15.95" customHeight="1"/>
+    <row r="521" ht="15.95" customHeight="1"/>
+    <row r="522" ht="15.95" customHeight="1"/>
+    <row r="523" ht="15.95" customHeight="1"/>
+    <row r="524" ht="15.95" customHeight="1"/>
+    <row r="525" ht="15.95" customHeight="1"/>
+    <row r="526" ht="15.95" customHeight="1"/>
+    <row r="527" ht="15.95" customHeight="1"/>
+    <row r="528" ht="15.95" customHeight="1"/>
+    <row r="529" ht="15.95" customHeight="1"/>
+    <row r="530" ht="15.95" customHeight="1"/>
+    <row r="531" ht="15.95" customHeight="1"/>
+    <row r="532" ht="15.95" customHeight="1"/>
+    <row r="533" ht="15.95" customHeight="1"/>
+    <row r="534" ht="15.95" customHeight="1"/>
+    <row r="535" ht="15.95" customHeight="1"/>
+    <row r="536" ht="15.95" customHeight="1"/>
+    <row r="537" ht="15.95" customHeight="1"/>
+    <row r="538" ht="15.95" customHeight="1"/>
+    <row r="539" ht="15.95" customHeight="1"/>
+    <row r="540" ht="15.95" customHeight="1"/>
+    <row r="541" ht="15.95" customHeight="1"/>
+    <row r="542" ht="15.95" customHeight="1"/>
+    <row r="543" ht="15.95" customHeight="1"/>
+    <row r="544" ht="15.95" customHeight="1"/>
+    <row r="545" ht="15.95" customHeight="1"/>
+    <row r="546" ht="15.95" customHeight="1"/>
+    <row r="547" ht="15.95" customHeight="1"/>
+    <row r="548" ht="15.95" customHeight="1"/>
+    <row r="549" ht="15.95" customHeight="1"/>
+    <row r="550" ht="15.95" customHeight="1"/>
+    <row r="551" ht="15.95" customHeight="1"/>
+    <row r="552" ht="15.95" customHeight="1"/>
+    <row r="553" ht="15.95" customHeight="1"/>
+    <row r="554" ht="15.95" customHeight="1"/>
+    <row r="555" ht="15.95" customHeight="1"/>
+    <row r="556" ht="15.95" customHeight="1"/>
+    <row r="557" ht="15.95" customHeight="1"/>
+    <row r="558" ht="15.95" customHeight="1"/>
+    <row r="559" ht="15.95" customHeight="1"/>
+    <row r="560" ht="15.95" customHeight="1"/>
+    <row r="561" ht="15.95" customHeight="1"/>
+    <row r="562" ht="15.95" customHeight="1"/>
+    <row r="563" ht="15.95" customHeight="1"/>
+    <row r="564" ht="15.95" customHeight="1"/>
+    <row r="565" ht="15.95" customHeight="1"/>
+    <row r="566" ht="15.95" customHeight="1"/>
+    <row r="567" ht="15.95" customHeight="1"/>
+    <row r="568" ht="15.95" customHeight="1"/>
+    <row r="569" ht="15.95" customHeight="1"/>
+    <row r="570" ht="15.95" customHeight="1"/>
+    <row r="571" ht="15.95" customHeight="1"/>
+    <row r="572" ht="15.95" customHeight="1"/>
+    <row r="573" ht="15.95" customHeight="1"/>
+    <row r="574" ht="15.95" customHeight="1"/>
+    <row r="575" ht="15.95" customHeight="1"/>
+    <row r="576" ht="15.95" customHeight="1"/>
+    <row r="577" ht="15.95" customHeight="1"/>
+    <row r="578" ht="15.95" customHeight="1"/>
+    <row r="579" ht="15.95" customHeight="1"/>
+    <row r="580" ht="15.95" customHeight="1"/>
+    <row r="581" ht="15.95" customHeight="1"/>
+    <row r="582" ht="15.95" customHeight="1"/>
+    <row r="583" ht="15.95" customHeight="1"/>
+    <row r="584" ht="15.95" customHeight="1"/>
+    <row r="585" ht="15.95" customHeight="1"/>
+    <row r="586" ht="15.95" customHeight="1"/>
+    <row r="587" ht="15.95" customHeight="1"/>
+    <row r="588" ht="15.95" customHeight="1"/>
+    <row r="589" ht="15.95" customHeight="1"/>
+    <row r="590" ht="15.95" customHeight="1"/>
+    <row r="591" ht="15.95" customHeight="1"/>
+    <row r="592" ht="15.95" customHeight="1"/>
+    <row r="593" ht="15.95" customHeight="1"/>
+    <row r="594" ht="15.95" customHeight="1"/>
+    <row r="595" ht="15.95" customHeight="1"/>
+    <row r="596" ht="15.95" customHeight="1"/>
+    <row r="597" ht="15.95" customHeight="1"/>
+    <row r="598" ht="15.95" customHeight="1"/>
+    <row r="599" ht="15.95" customHeight="1"/>
+    <row r="600" ht="15.95" customHeight="1"/>
+    <row r="601" ht="15.95" customHeight="1"/>
+    <row r="602" ht="15.95" customHeight="1"/>
+    <row r="603" ht="15.95" customHeight="1"/>
+    <row r="604" ht="15.95" customHeight="1"/>
+    <row r="605" ht="15.95" customHeight="1"/>
+    <row r="606" ht="15.95" customHeight="1"/>
+    <row r="607" ht="15.95" customHeight="1"/>
+    <row r="608" ht="15.95" customHeight="1"/>
+    <row r="609" ht="15.95" customHeight="1"/>
+    <row r="610" ht="15.95" customHeight="1"/>
+    <row r="611" ht="15.95" customHeight="1"/>
+    <row r="612" ht="15.95" customHeight="1"/>
+    <row r="613" ht="15.95" customHeight="1"/>
+    <row r="614" ht="15.95" customHeight="1"/>
+    <row r="615" ht="15.95" customHeight="1"/>
+    <row r="616" ht="15.95" customHeight="1"/>
+    <row r="617" ht="15.95" customHeight="1"/>
+    <row r="618" ht="15.95" customHeight="1"/>
+    <row r="619" ht="15.95" customHeight="1"/>
+    <row r="620" ht="15.95" customHeight="1"/>
+    <row r="621" ht="15.95" customHeight="1"/>
+    <row r="622" ht="15.95" customHeight="1"/>
+    <row r="623" ht="15.95" customHeight="1"/>
+    <row r="624" ht="15.95" customHeight="1"/>
+    <row r="625" ht="15.95" customHeight="1"/>
+    <row r="626" ht="15.95" customHeight="1"/>
+    <row r="627" ht="15.95" customHeight="1"/>
+    <row r="628" ht="15.95" customHeight="1"/>
+    <row r="629" ht="15.95" customHeight="1"/>
+    <row r="630" ht="15.95" customHeight="1"/>
+    <row r="631" ht="15.95" customHeight="1"/>
+    <row r="632" ht="15.95" customHeight="1"/>
+    <row r="633" ht="15.95" customHeight="1"/>
+    <row r="634" ht="15.95" customHeight="1"/>
+    <row r="635" ht="15.95" customHeight="1"/>
+    <row r="636" ht="15.95" customHeight="1"/>
+    <row r="637" ht="15.95" customHeight="1"/>
+    <row r="638" ht="15.95" customHeight="1"/>
+    <row r="639" ht="15.95" customHeight="1"/>
+    <row r="640" ht="15.95" customHeight="1"/>
+    <row r="641" ht="15.95" customHeight="1"/>
+    <row r="642" ht="15.95" customHeight="1"/>
+    <row r="643" ht="15.95" customHeight="1"/>
+    <row r="644" ht="15.95" customHeight="1"/>
+    <row r="645" ht="15.95" customHeight="1"/>
+    <row r="646" ht="15.95" customHeight="1"/>
+    <row r="647" ht="15.95" customHeight="1"/>
+    <row r="648" ht="15.95" customHeight="1"/>
+    <row r="649" ht="15.95" customHeight="1"/>
+    <row r="650" ht="15.95" customHeight="1"/>
+    <row r="651" ht="15.95" customHeight="1"/>
+    <row r="652" ht="15.95" customHeight="1"/>
+    <row r="653" ht="15.95" customHeight="1"/>
+    <row r="654" ht="15.95" customHeight="1"/>
+    <row r="655" ht="15.95" customHeight="1"/>
+    <row r="656" ht="15.95" customHeight="1"/>
+    <row r="657" ht="15.95" customHeight="1"/>
+    <row r="658" ht="15.95" customHeight="1"/>
+    <row r="659" ht="15.95" customHeight="1"/>
+    <row r="660" ht="15.95" customHeight="1"/>
+    <row r="661" ht="15.95" customHeight="1"/>
+    <row r="662" ht="15.95" customHeight="1"/>
+    <row r="663" ht="15.95" customHeight="1"/>
+    <row r="664" ht="15.95" customHeight="1"/>
+    <row r="665" ht="15.95" customHeight="1"/>
+    <row r="666" ht="15.95" customHeight="1"/>
+    <row r="667" ht="15.95" customHeight="1"/>
+    <row r="668" ht="15.95" customHeight="1"/>
+    <row r="669" ht="15.95" customHeight="1"/>
+    <row r="670" ht="15.95" customHeight="1"/>
+    <row r="671" ht="15.95" customHeight="1"/>
+    <row r="672" ht="15.95" customHeight="1"/>
+    <row r="673" ht="15.95" customHeight="1"/>
+    <row r="674" ht="15.95" customHeight="1"/>
+    <row r="675" ht="15.95" customHeight="1"/>
+    <row r="676" ht="15.95" customHeight="1"/>
+    <row r="677" ht="15.95" customHeight="1"/>
+    <row r="678" ht="15.95" customHeight="1"/>
+    <row r="679" ht="15.95" customHeight="1"/>
+    <row r="680" ht="15.95" customHeight="1"/>
+    <row r="681" ht="15.95" customHeight="1"/>
+    <row r="682" ht="15.95" customHeight="1"/>
+    <row r="683" ht="15.95" customHeight="1"/>
+    <row r="684" ht="15.95" customHeight="1"/>
+    <row r="685" ht="15.95" customHeight="1"/>
+    <row r="686" ht="15.95" customHeight="1"/>
+    <row r="687" ht="15.95" customHeight="1"/>
+    <row r="688" ht="15.95" customHeight="1"/>
+    <row r="689" ht="15.95" customHeight="1"/>
+    <row r="690" ht="15.95" customHeight="1"/>
+    <row r="691" ht="15.95" customHeight="1"/>
+    <row r="692" ht="15.95" customHeight="1"/>
+    <row r="693" ht="15.95" customHeight="1"/>
+    <row r="694" ht="15.95" customHeight="1"/>
+    <row r="695" ht="15.95" customHeight="1"/>
+    <row r="696" ht="15.95" customHeight="1"/>
+    <row r="697" ht="15.95" customHeight="1"/>
+    <row r="698" ht="15.95" customHeight="1"/>
+    <row r="699" ht="15.95" customHeight="1"/>
+    <row r="700" ht="15.95" customHeight="1"/>
+    <row r="701" ht="15.95" customHeight="1"/>
+    <row r="702" ht="15.95" customHeight="1"/>
+    <row r="703" ht="15.95" customHeight="1"/>
+    <row r="704" ht="15.95" customHeight="1"/>
+    <row r="705" ht="15.95" customHeight="1"/>
+    <row r="706" ht="15.95" customHeight="1"/>
+    <row r="707" ht="15.95" customHeight="1"/>
+    <row r="708" ht="15.95" customHeight="1"/>
+    <row r="709" ht="15.95" customHeight="1"/>
+    <row r="710" ht="15.95" customHeight="1"/>
+    <row r="711" ht="15.95" customHeight="1"/>
+    <row r="712" ht="15.95" customHeight="1"/>
+    <row r="713" ht="15.95" customHeight="1"/>
+    <row r="714" ht="15.95" customHeight="1"/>
+    <row r="715" ht="15.95" customHeight="1"/>
+    <row r="716" ht="15.95" customHeight="1"/>
+    <row r="717" ht="15.95" customHeight="1"/>
+    <row r="718" ht="15.95" customHeight="1"/>
+    <row r="719" ht="15.95" customHeight="1"/>
+    <row r="720" ht="15.95" customHeight="1"/>
+    <row r="721" ht="15.95" customHeight="1"/>
+    <row r="722" ht="15.95" customHeight="1"/>
+    <row r="723" ht="15.95" customHeight="1"/>
+    <row r="724" ht="15.95" customHeight="1"/>
+    <row r="725" ht="15.95" customHeight="1"/>
+    <row r="726" ht="15.95" customHeight="1"/>
+    <row r="727" ht="15.95" customHeight="1"/>
+    <row r="728" ht="15.95" customHeight="1"/>
+    <row r="729" ht="15.95" customHeight="1"/>
+    <row r="730" ht="15.95" customHeight="1"/>
+    <row r="731" ht="15.95" customHeight="1"/>
+    <row r="732" ht="15.95" customHeight="1"/>
+    <row r="733" ht="15.95" customHeight="1"/>
+    <row r="734" ht="15.95" customHeight="1"/>
+    <row r="735" ht="15.95" customHeight="1"/>
+    <row r="736" ht="15.95" customHeight="1"/>
+    <row r="737" ht="15.95" customHeight="1"/>
+    <row r="738" ht="15.95" customHeight="1"/>
+    <row r="739" ht="15.95" customHeight="1"/>
+    <row r="740" ht="15.95" customHeight="1"/>
+    <row r="741" ht="15.95" customHeight="1"/>
+    <row r="742" ht="15.95" customHeight="1"/>
+    <row r="743" ht="15.95" customHeight="1"/>
+    <row r="744" ht="15.95" customHeight="1"/>
+    <row r="745" ht="15.95" customHeight="1"/>
+    <row r="746" ht="15.95" customHeight="1"/>
+    <row r="747" ht="15.95" customHeight="1"/>
+    <row r="748" ht="15.95" customHeight="1"/>
+    <row r="749" ht="15.95" customHeight="1"/>
+    <row r="750" ht="15.95" customHeight="1"/>
+    <row r="751" ht="15.95" customHeight="1"/>
+    <row r="752" ht="15.95" customHeight="1"/>
+    <row r="753" ht="15.95" customHeight="1"/>
+    <row r="754" ht="15.95" customHeight="1"/>
+    <row r="755" ht="15.95" customHeight="1"/>
+    <row r="756" ht="15.95" customHeight="1"/>
+    <row r="757" ht="15.95" customHeight="1"/>
+    <row r="758" ht="15.95" customHeight="1"/>
+    <row r="759" ht="15.95" customHeight="1"/>
+    <row r="760" ht="15.95" customHeight="1"/>
+    <row r="761" ht="15.95" customHeight="1"/>
+    <row r="762" ht="15.95" customHeight="1"/>
+    <row r="763" ht="15.95" customHeight="1"/>
+    <row r="764" ht="15.95" customHeight="1"/>
+    <row r="765" ht="15.95" customHeight="1"/>
+    <row r="766" ht="15.95" customHeight="1"/>
+    <row r="767" ht="15.95" customHeight="1"/>
+    <row r="768" ht="15.95" customHeight="1"/>
+    <row r="769" ht="15.95" customHeight="1"/>
+    <row r="770" ht="15.95" customHeight="1"/>
+    <row r="771" ht="15.95" customHeight="1"/>
+    <row r="772" ht="15.95" customHeight="1"/>
+    <row r="773" ht="15.95" customHeight="1"/>
+    <row r="774" ht="15.95" customHeight="1"/>
+    <row r="775" ht="15.95" customHeight="1"/>
+    <row r="776" ht="15.95" customHeight="1"/>
+    <row r="777" ht="15.95" customHeight="1"/>
+    <row r="778" ht="15.95" customHeight="1"/>
+    <row r="779" ht="15.95" customHeight="1"/>
+    <row r="780" ht="15.95" customHeight="1"/>
+    <row r="781" ht="15.95" customHeight="1"/>
+    <row r="782" ht="15.95" customHeight="1"/>
+    <row r="783" ht="15.95" customHeight="1"/>
+    <row r="784" ht="15.95" customHeight="1"/>
+    <row r="785" ht="15.95" customHeight="1"/>
+    <row r="786" ht="15.95" customHeight="1"/>
+    <row r="787" ht="15.95" customHeight="1"/>
+    <row r="788" ht="15.95" customHeight="1"/>
+    <row r="789" ht="15.95" customHeight="1"/>
+    <row r="790" ht="15.95" customHeight="1"/>
+    <row r="791" ht="15.95" customHeight="1"/>
+    <row r="792" ht="15.95" customHeight="1"/>
+    <row r="793" ht="15.95" customHeight="1"/>
+    <row r="794" ht="15.95" customHeight="1"/>
+    <row r="795" ht="15.95" customHeight="1"/>
+    <row r="796" ht="15.95" customHeight="1"/>
+    <row r="797" ht="15.95" customHeight="1"/>
+    <row r="798" ht="15.95" customHeight="1"/>
+    <row r="799" ht="15.95" customHeight="1"/>
+    <row r="800" ht="15.95" customHeight="1"/>
+    <row r="801" ht="15.95" customHeight="1"/>
+    <row r="802" ht="15.95" customHeight="1"/>
+    <row r="803" ht="15.95" customHeight="1"/>
+    <row r="804" ht="15.95" customHeight="1"/>
+    <row r="805" ht="15.95" customHeight="1"/>
+    <row r="806" ht="15.95" customHeight="1"/>
+    <row r="807" ht="15.95" customHeight="1"/>
+    <row r="808" ht="15.95" customHeight="1"/>
+    <row r="809" ht="15.95" customHeight="1"/>
+    <row r="810" ht="15.95" customHeight="1"/>
+    <row r="811" ht="15.95" customHeight="1"/>
+    <row r="812" ht="15.95" customHeight="1"/>
+    <row r="813" ht="15.95" customHeight="1"/>
+    <row r="814" ht="15.95" customHeight="1"/>
+    <row r="815" ht="15.95" customHeight="1"/>
+    <row r="816" ht="15.95" customHeight="1"/>
+    <row r="817" ht="15.95" customHeight="1"/>
+    <row r="818" ht="15.95" customHeight="1"/>
+    <row r="819" ht="15.95" customHeight="1"/>
+    <row r="820" ht="15.95" customHeight="1"/>
+    <row r="821" ht="15.95" customHeight="1"/>
+    <row r="822" ht="15.95" customHeight="1"/>
+    <row r="823" ht="15.95" customHeight="1"/>
+    <row r="824" ht="15.95" customHeight="1"/>
+    <row r="825" ht="15.95" customHeight="1"/>
+    <row r="826" ht="15.95" customHeight="1"/>
+    <row r="827" ht="15.95" customHeight="1"/>
+    <row r="828" ht="15.95" customHeight="1"/>
+    <row r="829" ht="15.95" customHeight="1"/>
+    <row r="830" ht="15.95" customHeight="1"/>
+    <row r="831" ht="15.95" customHeight="1"/>
+    <row r="832" ht="15.95" customHeight="1"/>
+    <row r="833" ht="15.95" customHeight="1"/>
+    <row r="834" ht="15.95" customHeight="1"/>
+    <row r="835" ht="15.95" customHeight="1"/>
+    <row r="836" ht="15.95" customHeight="1"/>
+    <row r="837" ht="15.95" customHeight="1"/>
+    <row r="838" ht="15.95" customHeight="1"/>
+    <row r="839" ht="15.95" customHeight="1"/>
+    <row r="840" ht="15.95" customHeight="1"/>
+    <row r="841" ht="15.95" customHeight="1"/>
+    <row r="842" ht="15.95" customHeight="1"/>
+    <row r="843" ht="15.95" customHeight="1"/>
+    <row r="844" ht="15.95" customHeight="1"/>
+    <row r="845" ht="15.95" customHeight="1"/>
+    <row r="846" ht="15.95" customHeight="1"/>
+    <row r="847" ht="15.95" customHeight="1"/>
+    <row r="848" ht="15.95" customHeight="1"/>
+    <row r="849" ht="15.95" customHeight="1"/>
+    <row r="850" ht="15.95" customHeight="1"/>
+    <row r="851" ht="15.95" customHeight="1"/>
+    <row r="852" ht="15.95" customHeight="1"/>
+    <row r="853" ht="15.95" customHeight="1"/>
+    <row r="854" ht="15.95" customHeight="1"/>
+    <row r="855" ht="15.95" customHeight="1"/>
+    <row r="856" ht="15.95" customHeight="1"/>
+    <row r="857" ht="15.95" customHeight="1"/>
+    <row r="858" ht="15.95" customHeight="1"/>
+    <row r="859" ht="15.95" customHeight="1"/>
+    <row r="860" ht="15.95" customHeight="1"/>
+    <row r="861" ht="15.95" customHeight="1"/>
+    <row r="862" ht="15.95" customHeight="1"/>
+    <row r="863" ht="15.95" customHeight="1"/>
+    <row r="864" ht="15.95" customHeight="1"/>
+    <row r="865" ht="15.95" customHeight="1"/>
+    <row r="866" ht="15.95" customHeight="1"/>
+    <row r="867" ht="15.95" customHeight="1"/>
+    <row r="868" ht="15.95" customHeight="1"/>
+    <row r="869" ht="15.95" customHeight="1"/>
+    <row r="870" ht="15.95" customHeight="1"/>
+    <row r="871" ht="15.95" customHeight="1"/>
+    <row r="872" ht="15.95" customHeight="1"/>
+    <row r="873" ht="15.95" customHeight="1"/>
+    <row r="874" ht="15.95" customHeight="1"/>
+    <row r="875" ht="15.95" customHeight="1"/>
+    <row r="876" ht="15.95" customHeight="1"/>
+    <row r="877" ht="15.95" customHeight="1"/>
+    <row r="878" ht="15.95" customHeight="1"/>
+    <row r="879" ht="15.95" customHeight="1"/>
+    <row r="880" ht="15.95" customHeight="1"/>
+    <row r="881" ht="15.95" customHeight="1"/>
+    <row r="882" ht="15.95" customHeight="1"/>
+    <row r="883" ht="15.95" customHeight="1"/>
+    <row r="884" ht="15.95" customHeight="1"/>
+    <row r="885" ht="15.95" customHeight="1"/>
+    <row r="886" ht="15.95" customHeight="1"/>
+    <row r="887" ht="15.95" customHeight="1"/>
+    <row r="888" ht="15.95" customHeight="1"/>
+    <row r="889" ht="15.95" customHeight="1"/>
+    <row r="890" ht="15.95" customHeight="1"/>
+    <row r="891" ht="15.95" customHeight="1"/>
+    <row r="892" ht="15.95" customHeight="1"/>
+    <row r="893" ht="15.95" customHeight="1"/>
+    <row r="894" ht="15.95" customHeight="1"/>
+    <row r="895" ht="15.95" customHeight="1"/>
+    <row r="896" ht="15.95" customHeight="1"/>
+    <row r="897" ht="15.95" customHeight="1"/>
+    <row r="898" ht="15.95" customHeight="1"/>
+    <row r="899" ht="15.95" customHeight="1"/>
+    <row r="900" ht="15.95" customHeight="1"/>
+    <row r="901" ht="15.95" customHeight="1"/>
+    <row r="902" ht="15.95" customHeight="1"/>
+    <row r="903" ht="15.95" customHeight="1"/>
+    <row r="904" ht="15.95" customHeight="1"/>
+    <row r="905" ht="15.95" customHeight="1"/>
+    <row r="906" ht="15.95" customHeight="1"/>
+    <row r="907" ht="15.95" customHeight="1"/>
+    <row r="908" ht="15.95" customHeight="1"/>
+    <row r="909" ht="15.95" customHeight="1"/>
+    <row r="910" ht="15.95" customHeight="1"/>
+    <row r="911" ht="15.95" customHeight="1"/>
+    <row r="912" ht="15.95" customHeight="1"/>
+    <row r="913" ht="15.95" customHeight="1"/>
+    <row r="914" ht="15.95" customHeight="1"/>
+    <row r="915" ht="15.95" customHeight="1"/>
+    <row r="916" ht="15.95" customHeight="1"/>
+    <row r="917" ht="15.95" customHeight="1"/>
+    <row r="918" ht="15.95" customHeight="1"/>
+    <row r="919" ht="15.95" customHeight="1"/>
+    <row r="920" ht="15.95" customHeight="1"/>
+    <row r="921" ht="15.95" customHeight="1"/>
+    <row r="922" ht="15.95" customHeight="1"/>
+    <row r="923" ht="15.95" customHeight="1"/>
+    <row r="924" ht="15.95" customHeight="1"/>
+    <row r="925" ht="15.95" customHeight="1"/>
+    <row r="926" ht="15.95" customHeight="1"/>
+    <row r="927" ht="15.95" customHeight="1"/>
+    <row r="928" ht="15.95" customHeight="1"/>
+    <row r="929" ht="15.95" customHeight="1"/>
+    <row r="930" ht="15.95" customHeight="1"/>
+    <row r="931" ht="15.95" customHeight="1"/>
+    <row r="932" ht="15.95" customHeight="1"/>
+    <row r="933" ht="15.95" customHeight="1"/>
+    <row r="934" ht="15.95" customHeight="1"/>
+    <row r="935" ht="15.95" customHeight="1"/>
+    <row r="936" ht="15.95" customHeight="1"/>
+    <row r="937" ht="15.95" customHeight="1"/>
+    <row r="938" ht="15.95" customHeight="1"/>
+    <row r="939" ht="15.95" customHeight="1"/>
+    <row r="940" ht="15.95" customHeight="1"/>
+    <row r="941" ht="15.95" customHeight="1"/>
+    <row r="942" ht="15.95" customHeight="1"/>
+    <row r="943" ht="15.95" customHeight="1"/>
+    <row r="944" ht="15.95" customHeight="1"/>
+    <row r="945" ht="15.95" customHeight="1"/>
+    <row r="946" ht="15.95" customHeight="1"/>
+    <row r="947" ht="15.95" customHeight="1"/>
+    <row r="948" ht="15.95" customHeight="1"/>
+    <row r="949" ht="15.95" customHeight="1"/>
+    <row r="950" ht="15.95" customHeight="1"/>
+    <row r="951" ht="15.95" customHeight="1"/>
+    <row r="952" ht="15.95" customHeight="1"/>
+    <row r="953" ht="15.95" customHeight="1"/>
+    <row r="954" ht="15.95" customHeight="1"/>
+    <row r="955" ht="15.95" customHeight="1"/>
+    <row r="956" ht="15.95" customHeight="1"/>
+    <row r="957" ht="15.95" customHeight="1"/>
+    <row r="958" ht="15.95" customHeight="1"/>
+    <row r="959" ht="15.95" customHeight="1"/>
+    <row r="960" ht="15.95" customHeight="1"/>
+    <row r="961" ht="15.95" customHeight="1"/>
+    <row r="962" ht="15.95" customHeight="1"/>
+    <row r="963" ht="15.95" customHeight="1"/>
+    <row r="964" ht="15.95" customHeight="1"/>
+    <row r="965" ht="15.95" customHeight="1"/>
+    <row r="966" ht="15.95" customHeight="1"/>
+    <row r="967" ht="15.95" customHeight="1"/>
+    <row r="968" ht="15.95" customHeight="1"/>
+    <row r="969" ht="15.95" customHeight="1"/>
+    <row r="970" ht="15.95" customHeight="1"/>
+    <row r="971" ht="15.95" customHeight="1"/>
+    <row r="972" ht="15.95" customHeight="1"/>
+    <row r="973" ht="15.95" customHeight="1"/>
+    <row r="974" ht="15.95" customHeight="1"/>
+    <row r="975" ht="15.95" customHeight="1"/>
+    <row r="976" ht="15.95" customHeight="1"/>
+    <row r="977" ht="15.95" customHeight="1"/>
+    <row r="978" ht="15.95" customHeight="1"/>
+    <row r="979" ht="15.95" customHeight="1"/>
+    <row r="980" ht="15.95" customHeight="1"/>
+    <row r="981" ht="15.95" customHeight="1"/>
+    <row r="982" ht="15.95" customHeight="1"/>
+    <row r="983" ht="15.95" customHeight="1"/>
+    <row r="984" ht="15.95" customHeight="1"/>
+    <row r="985" ht="15.95" customHeight="1"/>
+    <row r="986" ht="15.95" customHeight="1"/>
+    <row r="987" ht="15.95" customHeight="1"/>
+    <row r="988" ht="15.95" customHeight="1"/>
+    <row r="989" ht="15.95" customHeight="1"/>
+    <row r="990" ht="15.95" customHeight="1"/>
+    <row r="991" ht="15.95" customHeight="1"/>
+    <row r="992" ht="15.95" customHeight="1"/>
+    <row r="993" ht="15.95" customHeight="1"/>
+    <row r="994" ht="15.95" customHeight="1"/>
+    <row r="995" ht="15.95" customHeight="1"/>
+    <row r="996" ht="15.95" customHeight="1"/>
+    <row r="997" ht="15.95" customHeight="1"/>
+    <row r="998" ht="15.95" customHeight="1"/>
+    <row r="999" ht="15.95" customHeight="1"/>
+    <row r="1000" ht="15.95" customHeight="1"/>
+    <row r="1001" ht="15.95" customHeight="1"/>
+    <row r="1002" ht="15.95" customHeight="1"/>
+    <row r="1003" ht="15.95" customHeight="1"/>
+    <row r="1004" ht="15.95" customHeight="1"/>
+    <row r="1005" ht="15.95" customHeight="1"/>
+    <row r="1006" ht="15.95" customHeight="1"/>
+    <row r="1007" ht="15.95" customHeight="1"/>
+    <row r="1008" ht="15.95" customHeight="1"/>
+    <row r="1009" ht="15.95" customHeight="1"/>
+    <row r="1010" ht="15.95" customHeight="1"/>
+    <row r="1011" ht="15.95" customHeight="1"/>
+    <row r="1012" ht="15.95" customHeight="1"/>
+    <row r="1013" ht="15.95" customHeight="1"/>
+    <row r="1014" ht="15.95" customHeight="1"/>
+    <row r="1015" ht="15.95" customHeight="1"/>
+    <row r="1016" ht="15.95" customHeight="1"/>
+    <row r="1017" ht="15.95" customHeight="1"/>
+    <row r="1018" ht="15.95" customHeight="1"/>
+    <row r="1019" ht="15.95" customHeight="1"/>
+    <row r="1020" ht="15.95" customHeight="1"/>
+    <row r="1021" ht="15.95" customHeight="1"/>
+    <row r="1022" ht="15.95" customHeight="1"/>
+    <row r="1023" ht="15.95" customHeight="1"/>
+    <row r="1024" ht="15.95" customHeight="1"/>
+    <row r="1025" ht="15.95" customHeight="1"/>
+    <row r="1026" ht="15.95" customHeight="1"/>
+    <row r="1027" ht="15.95" customHeight="1"/>
+    <row r="1028" ht="15.95" customHeight="1"/>
+    <row r="1029" ht="15.95" customHeight="1"/>
+    <row r="1030" ht="15.95" customHeight="1"/>
+    <row r="1031" ht="15.95" customHeight="1"/>
+    <row r="1032" ht="15.95" customHeight="1"/>
+    <row r="1033" ht="15.95" customHeight="1"/>
+    <row r="1034" ht="15.95" customHeight="1"/>
+    <row r="1035" ht="15.95" customHeight="1"/>
+    <row r="1036" ht="15.95" customHeight="1"/>
+    <row r="1037" ht="15.95" customHeight="1"/>
+    <row r="1038" ht="15.95" customHeight="1"/>
+    <row r="1039" ht="15.95" customHeight="1"/>
+    <row r="1040" ht="15.95" customHeight="1"/>
+    <row r="1041" ht="15.95" customHeight="1"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:A4"/>
@@ -20609,29 +20506,29 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView zoomScale="98" zoomScaleNormal="98" zoomScalePageLayoutView="60" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="256" width="26.42578125" customWidth="1"/>
     <col min="257" max="1023" width="16.140625" customWidth="1"/>
     <col min="1024" max="1025" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="61" t="s">
+    <row r="1" spans="1:4">
+      <c r="A1" s="59" t="s">
         <v>71</v>
       </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2" s="26" t="s">
         <v>161</v>
       </c>
@@ -20645,7 +20542,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4">
       <c r="A3" s="27" t="s">
         <v>162</v>
       </c>
@@ -20673,28 +20570,28 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView zoomScalePageLayoutView="60" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="256" width="24.42578125" customWidth="1"/>
     <col min="257" max="1023" width="16.140625" customWidth="1"/>
     <col min="1024" max="1025" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="62" t="s">
+    <row r="1" spans="1:3">
+      <c r="A1" s="60" t="s">
         <v>78</v>
       </c>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3">
       <c r="A2" s="26" t="s">
         <v>79</v>
       </c>
@@ -20705,7 +20602,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3">
       <c r="A3" s="27" t="s">
         <v>81</v>
       </c>
@@ -20716,7 +20613,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3">
       <c r="A4" s="28"/>
       <c r="B4" s="29"/>
       <c r="C4" s="29"/>
@@ -20735,28 +20632,28 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView zoomScalePageLayoutView="60" workbookViewId="0">
       <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="256" width="22.42578125" customWidth="1"/>
     <col min="257" max="1023" width="16.140625" customWidth="1"/>
     <col min="1024" max="1025" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="63" t="s">
+    <row r="1" spans="1:3">
+      <c r="A1" s="61" t="s">
         <v>84</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3">
       <c r="A2" s="26" t="s">
         <v>85</v>
       </c>
@@ -20767,7 +20664,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3">
       <c r="A3" s="12" t="s">
         <v>87</v>
       </c>
@@ -20778,7 +20675,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3">
       <c r="A4" s="12"/>
       <c r="B4" s="30"/>
       <c r="C4" s="30"/>
@@ -20797,28 +20694,28 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView topLeftCell="A13" zoomScalePageLayoutView="60" workbookViewId="0">
       <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="256" width="22.42578125" customWidth="1"/>
     <col min="257" max="1023" width="16.140625" customWidth="1"/>
     <col min="1024" max="1025" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="63" t="s">
+    <row r="1" spans="1:3">
+      <c r="A1" s="61" t="s">
         <v>90</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3">
       <c r="A2" s="26" t="s">
         <v>85</v>
       </c>
@@ -20829,7 +20726,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3">
       <c r="A3" s="12" t="s">
         <v>92</v>
       </c>
@@ -20840,7 +20737,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3">
       <c r="A4" s="28"/>
       <c r="B4" s="30"/>
       <c r="C4" s="30"/>
@@ -20859,28 +20756,28 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView zoomScalePageLayoutView="60" workbookViewId="0">
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="256" width="22.42578125" customWidth="1"/>
     <col min="257" max="1023" width="16.140625" customWidth="1"/>
     <col min="1024" max="1025" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="63" t="s">
+    <row r="1" spans="1:3">
+      <c r="A1" s="61" t="s">
         <v>95</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3">
       <c r="A2" s="9" t="s">
         <v>85</v>
       </c>
@@ -20891,7 +20788,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3">
       <c r="A3" s="12" t="s">
         <v>97</v>
       </c>
@@ -20902,7 +20799,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3">
       <c r="A4" s="31"/>
       <c r="B4" s="9"/>
       <c r="C4" s="9"/>
@@ -20921,28 +20818,28 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView zoomScalePageLayoutView="60" workbookViewId="0">
       <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="256" width="22.42578125" customWidth="1"/>
     <col min="257" max="1023" width="16.140625" customWidth="1"/>
     <col min="1024" max="1025" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="63" t="s">
+    <row r="1" spans="1:3">
+      <c r="A1" s="61" t="s">
         <v>100</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3">
       <c r="A2" s="9" t="s">
         <v>85</v>
       </c>
@@ -20953,7 +20850,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3">
       <c r="A3" s="12" t="s">
         <v>102</v>
       </c>
@@ -20964,7 +20861,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3">
       <c r="A4" s="31"/>
       <c r="B4" s="9"/>
       <c r="C4" s="9"/>
@@ -20983,47 +20880,53 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:U125"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:X121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="U3" sqref="U3"/>
+    <sheetView zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="18.85546875" customWidth="1"/>
     <col min="2" max="2" width="31.5703125" customWidth="1"/>
     <col min="3" max="20" width="12.42578125" customWidth="1"/>
-    <col min="21" max="21" width="68.7109375" customWidth="1"/>
-    <col min="22" max="1023" width="12.42578125" customWidth="1"/>
+    <col min="21" max="21" width="12.85546875" customWidth="1"/>
+    <col min="22" max="23" width="12.42578125" customWidth="1"/>
+    <col min="24" max="24" width="14.5703125" customWidth="1"/>
+    <col min="25" max="1023" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A1" s="63" t="s">
+    <row r="1" spans="1:24">
+      <c r="A1" s="61" t="s">
         <v>105</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
-      <c r="G1" s="63"/>
-      <c r="H1" s="63"/>
-      <c r="I1" s="63"/>
-      <c r="J1" s="63"/>
-      <c r="K1" s="63"/>
-      <c r="L1" s="43"/>
-      <c r="M1" s="43"/>
-      <c r="N1" s="43"/>
-      <c r="O1" s="43"/>
-      <c r="P1" s="43"/>
-      <c r="Q1" s="43"/>
-      <c r="R1" s="43"/>
-      <c r="S1" s="43"/>
-      <c r="T1" s="43"/>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="61"/>
+      <c r="G1" s="61"/>
+      <c r="H1" s="61"/>
+      <c r="I1" s="61"/>
+      <c r="J1" s="61"/>
+      <c r="K1" s="61"/>
+      <c r="L1" s="61"/>
+      <c r="M1" s="61"/>
+      <c r="N1" s="61"/>
+      <c r="O1" s="55"/>
+      <c r="P1" s="55"/>
+      <c r="Q1" s="55"/>
+      <c r="R1" s="55"/>
+      <c r="S1" s="55"/>
+      <c r="T1" s="55"/>
+      <c r="U1" s="55"/>
+      <c r="V1" s="55"/>
+      <c r="W1" s="55"/>
+      <c r="X1" s="55"/>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:24">
       <c r="A2" s="29" t="s">
         <v>80</v>
       </c>
@@ -21045,50 +20948,59 @@
       <c r="G2" s="29" t="s">
         <v>111</v>
       </c>
-      <c r="H2" s="29" t="s">
+      <c r="H2" s="66" t="s">
+        <v>285</v>
+      </c>
+      <c r="I2" s="66" t="s">
+        <v>286</v>
+      </c>
+      <c r="J2" s="66" t="s">
+        <v>287</v>
+      </c>
+      <c r="K2" s="29" t="s">
         <v>112</v>
       </c>
-      <c r="I2" s="29" t="s">
+      <c r="L2" s="29" t="s">
         <v>113</v>
       </c>
-      <c r="J2" s="29" t="s">
+      <c r="M2" s="29" t="s">
         <v>114</v>
       </c>
-      <c r="K2" s="29" t="s">
+      <c r="N2" s="29" t="s">
         <v>115</v>
       </c>
-      <c r="L2" s="29" t="s">
+      <c r="O2" s="29" t="s">
         <v>116</v>
       </c>
-      <c r="M2" s="29" t="s">
+      <c r="P2" s="29" t="s">
         <v>117</v>
       </c>
-      <c r="N2" s="29" t="s">
+      <c r="Q2" s="29" t="s">
         <v>118</v>
       </c>
-      <c r="O2" s="29" t="s">
+      <c r="R2" s="29" t="s">
         <v>119</v>
       </c>
-      <c r="P2" s="29" t="s">
+      <c r="S2" s="29" t="s">
         <v>120</v>
       </c>
-      <c r="Q2" s="29" t="s">
+      <c r="T2" s="29" t="s">
         <v>157</v>
       </c>
-      <c r="R2" s="29" t="s">
+      <c r="U2" s="29" t="s">
         <v>121</v>
       </c>
-      <c r="S2" s="29" t="s">
+      <c r="V2" s="29" t="s">
         <v>159</v>
       </c>
-      <c r="T2" s="29" t="s">
+      <c r="W2" s="29" t="s">
         <v>122</v>
       </c>
-      <c r="U2" s="56" t="s">
-        <v>280</v>
+      <c r="X2" s="66" t="s">
+        <v>281</v>
       </c>
     </row>
-    <row r="3" spans="1:21" ht="60" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:24">
       <c r="A3" s="32" t="s">
         <v>123</v>
       </c>
@@ -21110,231 +21022,240 @@
       <c r="G3" s="32" t="s">
         <v>129</v>
       </c>
-      <c r="H3" s="32" t="s">
+      <c r="H3" s="67" t="s">
+        <v>282</v>
+      </c>
+      <c r="I3" s="67" t="s">
+        <v>283</v>
+      </c>
+      <c r="J3" s="67" t="s">
+        <v>284</v>
+      </c>
+      <c r="K3" s="32" t="s">
         <v>130</v>
       </c>
-      <c r="I3" s="32" t="s">
+      <c r="L3" s="32" t="s">
         <v>131</v>
       </c>
-      <c r="J3" s="32" t="s">
+      <c r="M3" s="32" t="s">
         <v>132</v>
       </c>
-      <c r="K3" s="32" t="s">
+      <c r="N3" s="32" t="s">
         <v>133</v>
       </c>
-      <c r="L3" s="36" t="s">
+      <c r="O3" s="36" t="s">
         <v>134</v>
       </c>
-      <c r="M3" s="36" t="s">
+      <c r="P3" s="36" t="s">
         <v>135</v>
       </c>
-      <c r="N3" s="36" t="s">
+      <c r="Q3" s="36" t="s">
         <v>136</v>
       </c>
-      <c r="O3" s="36" t="s">
+      <c r="R3" s="36" t="s">
         <v>137</v>
       </c>
-      <c r="P3" s="36" t="s">
+      <c r="S3" s="36" t="s">
         <v>138</v>
       </c>
-      <c r="Q3" s="36" t="s">
+      <c r="T3" s="36" t="s">
         <v>158</v>
       </c>
-      <c r="R3" s="36" t="s">
+      <c r="U3" s="36" t="s">
         <v>139</v>
       </c>
-      <c r="S3" s="36" t="s">
+      <c r="V3" s="36" t="s">
         <v>160</v>
       </c>
-      <c r="T3" s="36" t="s">
+      <c r="W3" s="36" t="s">
         <v>140</v>
       </c>
-      <c r="U3" s="57" t="s">
-        <v>281</v>
+      <c r="X3" s="68" t="s">
+        <v>280</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A15" s="40" t="s">
+    <row r="11" spans="1:24">
+      <c r="A11" s="40" t="s">
         <v>175</v>
       </c>
-      <c r="B15" s="40"/>
-      <c r="C15" s="40"/>
-      <c r="D15" s="40"/>
+      <c r="B11" s="40"/>
+      <c r="C11" s="40"/>
+      <c r="D11" s="40"/>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A16" s="41" t="s">
+    <row r="12" spans="1:24">
+      <c r="A12" s="41" t="s">
         <v>170</v>
       </c>
-      <c r="B16" s="48" t="s">
+      <c r="B12" s="47" t="s">
         <v>171</v>
       </c>
-      <c r="C16" s="48" t="s">
+      <c r="C12" s="47" t="s">
         <v>172</v>
       </c>
-      <c r="D16" s="48" t="s">
+      <c r="D12" s="47" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="40" t="s">
+    <row r="24" spans="1:4">
+      <c r="A24" s="40" t="s">
         <v>174</v>
       </c>
-      <c r="B28" s="40"/>
-      <c r="C28" s="40"/>
-      <c r="D28" s="40"/>
+      <c r="B24" s="40"/>
+      <c r="C24" s="40"/>
+      <c r="D24" s="40"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="41" t="s">
+    <row r="25" spans="1:4">
+      <c r="A25" s="41" t="s">
         <v>170</v>
       </c>
-      <c r="B29" s="48" t="s">
+      <c r="B25" s="47" t="s">
         <v>176</v>
       </c>
-      <c r="C29" s="48" t="s">
+      <c r="C25" s="47" t="s">
         <v>177</v>
       </c>
-      <c r="D29" s="48" t="s">
+      <c r="D25" s="47" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44" s="40" t="s">
+    <row r="40" spans="1:4">
+      <c r="A40" s="40" t="s">
         <v>179</v>
       </c>
-      <c r="B44" s="40"/>
-      <c r="C44" s="40"/>
-      <c r="D44" s="40"/>
+      <c r="B40" s="40"/>
+      <c r="C40" s="40"/>
+      <c r="D40" s="40"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" s="41" t="s">
+    <row r="41" spans="1:4">
+      <c r="A41" s="41" t="s">
         <v>170</v>
       </c>
-      <c r="B45" s="48" t="s">
+      <c r="B41" s="47" t="s">
         <v>180</v>
       </c>
-      <c r="C45" s="48" t="s">
+      <c r="C41" s="47" t="s">
         <v>181</v>
       </c>
-      <c r="D45" s="48" t="s">
+      <c r="D41" s="47" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A58" s="40" t="s">
+    <row r="54" spans="1:8">
+      <c r="A54" s="40" t="s">
         <v>266</v>
       </c>
-      <c r="B58" s="40"/>
-      <c r="C58" s="40"/>
-      <c r="D58" s="40"/>
+      <c r="B54" s="40"/>
+      <c r="C54" s="40"/>
+      <c r="D54" s="40"/>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A59" s="49" t="s">
+    <row r="55" spans="1:8">
+      <c r="A55" s="48" t="s">
         <v>170</v>
       </c>
-      <c r="B59" s="50" t="s">
+      <c r="B55" s="49" t="s">
         <v>267</v>
       </c>
-      <c r="C59" s="50" t="s">
+      <c r="C55" s="49" t="s">
         <v>268</v>
       </c>
-      <c r="D59" s="50" t="s">
+      <c r="D55" s="49" t="s">
         <v>269</v>
       </c>
-      <c r="E59" s="51"/>
-      <c r="F59" s="51"/>
-      <c r="G59" s="51"/>
-      <c r="H59" s="51"/>
+      <c r="E55" s="50"/>
+      <c r="F55" s="50"/>
+      <c r="G55" s="50"/>
+      <c r="H55" s="50"/>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A71" s="40" t="s">
+    <row r="67" spans="1:4">
+      <c r="A67" s="40" t="s">
         <v>169</v>
       </c>
-      <c r="B71" s="40"/>
-      <c r="C71" s="40"/>
-      <c r="D71" s="40"/>
+      <c r="B67" s="40"/>
+      <c r="C67" s="40"/>
+      <c r="D67" s="40"/>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A72" s="41" t="s">
+    <row r="68" spans="1:4">
+      <c r="A68" s="41" t="s">
         <v>170</v>
       </c>
-      <c r="B72" s="48" t="s">
+      <c r="B68" s="47" t="s">
         <v>183</v>
       </c>
-      <c r="C72" s="48" t="s">
+      <c r="C68" s="47" t="s">
         <v>184</v>
       </c>
-      <c r="D72" s="48" t="s">
+      <c r="D68" s="47" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A93" s="40" t="s">
+    <row r="89" spans="1:4">
+      <c r="A89" s="40" t="s">
         <v>186</v>
       </c>
-      <c r="B93" s="40"/>
-      <c r="C93" s="40"/>
-      <c r="D93" s="40"/>
+      <c r="B89" s="40"/>
+      <c r="C89" s="40"/>
+      <c r="D89" s="40"/>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A94" s="41" t="s">
+    <row r="90" spans="1:4">
+      <c r="A90" s="41" t="s">
         <v>187</v>
       </c>
-      <c r="B94" s="48" t="s">
+      <c r="B90" s="47" t="s">
         <v>188</v>
       </c>
-      <c r="C94" s="48" t="s">
+      <c r="C90" s="47" t="s">
         <v>189</v>
       </c>
-      <c r="D94" s="48" t="s">
+      <c r="D90" s="47" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A109" s="40" t="s">
+    <row r="105" spans="1:8">
+      <c r="A105" s="40" t="s">
         <v>270</v>
       </c>
-      <c r="B109" s="40"/>
-      <c r="C109" s="40"/>
-      <c r="D109" s="40"/>
+      <c r="B105" s="40"/>
+      <c r="C105" s="40"/>
+      <c r="D105" s="40"/>
     </row>
-    <row r="110" spans="1:8" s="52" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A110" s="49" t="s">
+    <row r="106" spans="1:8" s="51" customFormat="1">
+      <c r="A106" s="48" t="s">
         <v>271</v>
       </c>
-      <c r="B110" s="50" t="s">
+      <c r="B106" s="49" t="s">
         <v>272</v>
       </c>
-      <c r="C110" s="50" t="s">
+      <c r="C106" s="49" t="s">
         <v>273</v>
       </c>
-      <c r="D110" s="50" t="s">
+      <c r="D106" s="49" t="s">
         <v>274</v>
       </c>
-      <c r="E110" s="51"/>
-      <c r="F110" s="51"/>
-      <c r="G110" s="51"/>
-      <c r="H110" s="51"/>
+      <c r="E106" s="50"/>
+      <c r="F106" s="50"/>
+      <c r="G106" s="50"/>
+      <c r="H106" s="50"/>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A124" s="64" t="s">
+    <row r="120" spans="1:4">
+      <c r="A120" s="62" t="s">
         <v>191</v>
       </c>
-      <c r="B124" s="65"/>
-      <c r="C124" s="40"/>
-      <c r="D124" s="40"/>
+      <c r="B120" s="63"/>
+      <c r="C120" s="40"/>
+      <c r="D120" s="40"/>
     </row>
-    <row r="125" spans="1:4" ht="60" x14ac:dyDescent="0.2">
-      <c r="A125" s="41" t="s">
+    <row r="121" spans="1:4" ht="60">
+      <c r="A121" s="41" t="s">
         <v>192</v>
       </c>
-      <c r="B125" s="42" t="s">
+      <c r="B121" s="42" t="s">
         <v>193</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A124:B124"/>
+    <mergeCell ref="A120:B120"/>
+    <mergeCell ref="A1:N1"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -21346,14 +21267,14 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34BFAF30-6EFD-4A13-A39A-D09455CAAF60}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="14.140625" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
@@ -21369,95 +21290,95 @@
     <col min="12" max="12" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A1" s="66" t="s">
+    <row r="1" spans="1:12">
+      <c r="A1" s="64" t="s">
         <v>245</v>
       </c>
-      <c r="B1" s="67"/>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67"/>
-      <c r="G1" s="67"/>
-      <c r="H1" s="67"/>
-      <c r="I1" s="67"/>
-      <c r="J1" s="67"/>
-      <c r="K1" s="67"/>
-      <c r="L1" s="67"/>
+      <c r="B1" s="65"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
+      <c r="E1" s="65"/>
+      <c r="F1" s="65"/>
+      <c r="G1" s="65"/>
+      <c r="H1" s="65"/>
+      <c r="I1" s="65"/>
+      <c r="J1" s="65"/>
+      <c r="K1" s="65"/>
+      <c r="L1" s="65"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2" s="44" t="s">
+    <row r="2" spans="1:12">
+      <c r="A2" s="43" t="s">
         <v>246</v>
       </c>
-      <c r="B2" s="44" t="s">
+      <c r="B2" s="43" t="s">
         <v>247</v>
       </c>
-      <c r="C2" s="44" t="s">
+      <c r="C2" s="43" t="s">
         <v>248</v>
       </c>
-      <c r="D2" s="44" t="s">
+      <c r="D2" s="43" t="s">
         <v>249</v>
       </c>
-      <c r="E2" s="44" t="s">
+      <c r="E2" s="43" t="s">
         <v>250</v>
       </c>
-      <c r="F2" s="44" t="s">
+      <c r="F2" s="43" t="s">
         <v>251</v>
       </c>
-      <c r="G2" s="44" t="s">
+      <c r="G2" s="43" t="s">
         <v>252</v>
       </c>
-      <c r="H2" s="44" t="s">
+      <c r="H2" s="43" t="s">
         <v>253</v>
       </c>
-      <c r="I2" s="44" t="s">
+      <c r="I2" s="43" t="s">
         <v>254</v>
       </c>
-      <c r="J2" s="53" t="s">
+      <c r="J2" s="52" t="s">
         <v>275</v>
       </c>
-      <c r="K2" s="54" t="s">
+      <c r="K2" s="53" t="s">
         <v>276</v>
       </c>
-      <c r="L2" s="44" t="s">
+      <c r="L2" s="43" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="45" t="s">
+    <row r="3" spans="1:12" ht="15.6" customHeight="1">
+      <c r="A3" s="44" t="s">
         <v>256</v>
       </c>
-      <c r="B3" s="46" t="s">
+      <c r="B3" s="45" t="s">
         <v>257</v>
       </c>
-      <c r="C3" s="47" t="s">
+      <c r="C3" s="46" t="s">
         <v>258</v>
       </c>
-      <c r="D3" s="45" t="s">
+      <c r="D3" s="44" t="s">
         <v>259</v>
       </c>
-      <c r="E3" s="46" t="s">
+      <c r="E3" s="45" t="s">
         <v>260</v>
       </c>
-      <c r="F3" s="46" t="s">
+      <c r="F3" s="45" t="s">
         <v>261</v>
       </c>
-      <c r="G3" s="46" t="s">
+      <c r="G3" s="45" t="s">
         <v>262</v>
       </c>
-      <c r="H3" s="46" t="s">
+      <c r="H3" s="45" t="s">
         <v>263</v>
       </c>
-      <c r="I3" s="46" t="s">
+      <c r="I3" s="45" t="s">
         <v>264</v>
       </c>
-      <c r="J3" s="46" t="s">
+      <c r="J3" s="45" t="s">
         <v>277</v>
       </c>
-      <c r="K3" s="55" t="s">
+      <c r="K3" s="54" t="s">
         <v>278</v>
       </c>
-      <c r="L3" s="55" t="s">
+      <c r="L3" s="54" t="s">
         <v>265</v>
       </c>
     </row>
@@ -21466,6 +21387,5 @@
     <mergeCell ref="A1:L1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
POCOR-7328: code enhancement for institution report cards | Status: Done
</commit_message>
<xml_diff>
--- a/webroot/export/customexcel/default_templates/profile_template.xlsx
+++ b/webroot/export/customexcel/default_templates/profile_template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10305" tabRatio="862"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10305" tabRatio="862" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,6 @@
     <sheet name="Student Performance Summary" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="293">
   <si>
     <t>${"image":{"displayValue":"Institutions.logo_content","imageWidth":"100","imageMarginLeft":"20","imageMarginTop":"5"}}</t>
   </si>
@@ -565,18 +564,6 @@
   </si>
   <si>
     <t xml:space="preserve">${"match": {"displayValue": "InstitutionStudentWithdrawn.area_level:3","rows": {"matchFrom": "InstitutionEducationGrade.id","matchTo": "InstitutionEducationGrade.id"}}} </t>
-  </si>
-  <si>
-    <t>Count of Transferred students</t>
-  </si>
-  <si>
-    <t xml:space="preserve">${"match": {"displayValue": "InstitutionStudentTransferred.area_level:1","rows": {"matchFrom": "InstitutionEducationGrade.id","matchTo": "InstitutionEducationGrade.id"}}} </t>
-  </si>
-  <si>
-    <t xml:space="preserve">${"match": {"displayValue": "InstitutionStudentTransferred.area_level:2","rows": {"matchFrom": "InstitutionEducationGrade.id","matchTo": "InstitutionEducationGrade.id"}}} </t>
-  </si>
-  <si>
-    <t xml:space="preserve">${"match": {"displayValue": "InstitutionStudentTransferred.area_level:3","rows": {"matchFrom": "InstitutionEducationGrade.id","matchTo": "InstitutionEducationGrade.id"}}} </t>
   </si>
   <si>
     <t xml:space="preserve">${"match": {"displayValue": "InstitutionStaffCount.area_level:1","rows": {"matchFrom": "InstitutionEducationGrade.id","matchTo": "InstitutionEducationGrade.id"}}} </t>
@@ -894,6 +881,33 @@
   </si>
   <si>
     <t>Total Student Promotion Rate</t>
+  </si>
+  <si>
+    <t>Shift Association</t>
+  </si>
+  <si>
+    <t>Owner</t>
+  </si>
+  <si>
+    <t>Occupier</t>
+  </si>
+  <si>
+    <t>${"match": {"displayValue": "InstitutionOwnerOccupier.owner_name","rows": {"matchFrom": "InstitutionOwnerOccupier.id","matchTo": "InstitutionOwnerOccupier.id"}}}</t>
+  </si>
+  <si>
+    <t>${"match": {"displayValue": "InstitutionOwnerOccupier.occupier_name","rows": {"matchFrom": "InstitutionOwnerOccupier.id","matchTo": "InstitutionOwnerOccupier.id"}}}</t>
+  </si>
+  <si>
+    <t>Count of Promoted Students</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${"match": {"displayValue": "InstitutionStudentPromoted.area_level:1","rows": {"matchFrom": "InstitutionEducationGrade.id","matchTo": "InstitutionEducationGrade.id"}}} </t>
+  </si>
+  <si>
+    <t xml:space="preserve">${"match": {"displayValue": "InstitutionStudentPromoted.area_level:2","rows": {"matchFrom": "InstitutionEducationGrade.id","matchTo": "InstitutionEducationGrade.id"}}} </t>
+  </si>
+  <si>
+    <t xml:space="preserve">${"match": {"displayValue": "InstitutionStudentPromoted.area_level:3","rows": {"matchFrom": "InstitutionEducationGrade.id","matchTo": "InstitutionEducationGrade.id"}}} </t>
   </si>
 </sst>
 </file>
@@ -1027,7 +1041,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -1131,11 +1145,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1260,6 +1283,15 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1290,13 +1322,7 @@
     <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1671,8 +1697,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:IV1041"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView topLeftCell="A58" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="B64" sqref="B64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75"/>
@@ -1693,7 +1719,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:256" ht="15" customHeight="1">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="59" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4"/>
@@ -1714,13 +1740,13 @@
       <c r="Q1" s="7"/>
     </row>
     <row r="2" spans="1:256" ht="25.5" customHeight="1">
-      <c r="A2" s="56"/>
-      <c r="B2" s="57" t="s">
+      <c r="A2" s="59"/>
+      <c r="B2" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57"/>
+      <c r="C2" s="60"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
       <c r="F2" s="8"/>
       <c r="G2" s="9"/>
       <c r="H2" s="7"/>
@@ -1974,13 +2000,13 @@
       <c r="IV2" s="3"/>
     </row>
     <row r="3" spans="1:256" ht="25.5" customHeight="1">
-      <c r="A3" s="56"/>
-      <c r="B3" s="58" t="s">
+      <c r="A3" s="59"/>
+      <c r="B3" s="61" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="58"/>
-      <c r="D3" s="58"/>
-      <c r="E3" s="58"/>
+      <c r="C3" s="61"/>
+      <c r="D3" s="61"/>
+      <c r="E3" s="61"/>
       <c r="F3" s="9"/>
       <c r="G3" s="9"/>
       <c r="H3" s="7"/>
@@ -2234,7 +2260,7 @@
       <c r="IV3" s="3"/>
     </row>
     <row r="4" spans="1:256" ht="22.5" customHeight="1">
-      <c r="A4" s="56"/>
+      <c r="A4" s="59"/>
       <c r="B4" s="4"/>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
@@ -3965,7 +3991,7 @@
         <v>23</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="C17" s="13"/>
       <c r="D17" s="5"/>
@@ -18060,7 +18086,7 @@
     </row>
     <row r="72" spans="1:256" ht="12" customHeight="1">
       <c r="A72" s="1" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="B72" s="1"/>
       <c r="C72" s="3"/>
@@ -18319,10 +18345,10 @@
     </row>
     <row r="73" spans="1:256" ht="15.75" customHeight="1">
       <c r="A73" s="23" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="B73" s="24" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="C73" s="3"/>
       <c r="E73" s="3"/>
@@ -18580,10 +18606,10 @@
     </row>
     <row r="74" spans="1:256" ht="15.75" customHeight="1">
       <c r="A74" s="25" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="B74" s="25" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="C74" s="3"/>
       <c r="E74" s="3"/>
@@ -19384,7 +19410,7 @@
     <row r="97" spans="1:16" ht="15.95" customHeight="1"/>
     <row r="98" spans="1:16" ht="15.95" customHeight="1">
       <c r="A98" s="1" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="B98" s="1"/>
       <c r="C98" s="1"/>
@@ -19404,102 +19430,102 @@
     </row>
     <row r="99" spans="1:16" ht="15.95" customHeight="1">
       <c r="A99" s="23" t="s">
+        <v>197</v>
+      </c>
+      <c r="B99" s="23" t="s">
+        <v>198</v>
+      </c>
+      <c r="C99" s="23" t="s">
+        <v>199</v>
+      </c>
+      <c r="D99" s="23" t="s">
+        <v>200</v>
+      </c>
+      <c r="E99" s="23" t="s">
         <v>201</v>
       </c>
-      <c r="B99" s="23" t="s">
+      <c r="F99" s="23" t="s">
         <v>202</v>
       </c>
-      <c r="C99" s="23" t="s">
+      <c r="G99" s="23" t="s">
         <v>203</v>
       </c>
-      <c r="D99" s="23" t="s">
+      <c r="H99" s="23" t="s">
         <v>204</v>
       </c>
-      <c r="E99" s="23" t="s">
+      <c r="I99" s="23" t="s">
         <v>205</v>
       </c>
-      <c r="F99" s="23" t="s">
+      <c r="J99" s="23" t="s">
         <v>206</v>
       </c>
-      <c r="G99" s="23" t="s">
+      <c r="K99" s="23" t="s">
         <v>207</v>
       </c>
-      <c r="H99" s="23" t="s">
+      <c r="L99" s="23" t="s">
         <v>208</v>
       </c>
-      <c r="I99" s="23" t="s">
+      <c r="M99" s="23" t="s">
         <v>209</v>
       </c>
-      <c r="J99" s="23" t="s">
+      <c r="N99" s="23" t="s">
         <v>210</v>
       </c>
-      <c r="K99" s="23" t="s">
+      <c r="O99" s="23" t="s">
         <v>211</v>
       </c>
-      <c r="L99" s="23" t="s">
+      <c r="P99" s="23" t="s">
         <v>212</v>
-      </c>
-      <c r="M99" s="23" t="s">
-        <v>213</v>
-      </c>
-      <c r="N99" s="23" t="s">
-        <v>214</v>
-      </c>
-      <c r="O99" s="23" t="s">
-        <v>215</v>
-      </c>
-      <c r="P99" s="23" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="100" spans="1:16" ht="15.95" customHeight="1">
       <c r="A100" s="25" t="s">
+        <v>213</v>
+      </c>
+      <c r="B100" s="25" t="s">
+        <v>214</v>
+      </c>
+      <c r="C100" s="25" t="s">
+        <v>215</v>
+      </c>
+      <c r="D100" s="25" t="s">
+        <v>216</v>
+      </c>
+      <c r="E100" s="25" t="s">
         <v>217</v>
       </c>
-      <c r="B100" s="25" t="s">
+      <c r="F100" s="25" t="s">
         <v>218</v>
       </c>
-      <c r="C100" s="25" t="s">
+      <c r="G100" s="25" t="s">
         <v>219</v>
       </c>
-      <c r="D100" s="25" t="s">
+      <c r="H100" s="25" t="s">
         <v>220</v>
       </c>
-      <c r="E100" s="25" t="s">
+      <c r="I100" s="25" t="s">
         <v>221</v>
       </c>
-      <c r="F100" s="25" t="s">
+      <c r="J100" s="25" t="s">
         <v>222</v>
       </c>
-      <c r="G100" s="25" t="s">
+      <c r="K100" s="25" t="s">
         <v>223</v>
       </c>
-      <c r="H100" s="25" t="s">
+      <c r="L100" s="25" t="s">
         <v>224</v>
       </c>
-      <c r="I100" s="25" t="s">
+      <c r="M100" s="25" t="s">
         <v>225</v>
       </c>
-      <c r="J100" s="25" t="s">
+      <c r="N100" s="25" t="s">
         <v>226</v>
       </c>
-      <c r="K100" s="25" t="s">
+      <c r="O100" s="25" t="s">
         <v>227</v>
       </c>
-      <c r="L100" s="25" t="s">
+      <c r="P100" s="25" t="s">
         <v>228</v>
-      </c>
-      <c r="M100" s="25" t="s">
-        <v>229</v>
-      </c>
-      <c r="N100" s="25" t="s">
-        <v>230</v>
-      </c>
-      <c r="O100" s="25" t="s">
-        <v>231</v>
-      </c>
-      <c r="P100" s="25" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="101" spans="1:16" ht="15.95" customHeight="1"/>
@@ -19574,7 +19600,7 @@
     <row r="170" spans="1:6" ht="15.95" customHeight="1"/>
     <row r="171" spans="1:6" ht="15.95" customHeight="1">
       <c r="A171" s="1" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="B171" s="1"/>
       <c r="C171" s="1"/>
@@ -19584,42 +19610,42 @@
     </row>
     <row r="172" spans="1:6" ht="15.95" customHeight="1">
       <c r="A172" s="23" t="s">
+        <v>229</v>
+      </c>
+      <c r="B172" s="23" t="s">
+        <v>230</v>
+      </c>
+      <c r="C172" s="23" t="s">
+        <v>231</v>
+      </c>
+      <c r="D172" s="23" t="s">
+        <v>232</v>
+      </c>
+      <c r="E172" s="23" t="s">
         <v>233</v>
       </c>
-      <c r="B172" s="23" t="s">
+      <c r="F172" s="23" t="s">
         <v>234</v>
-      </c>
-      <c r="C172" s="23" t="s">
-        <v>235</v>
-      </c>
-      <c r="D172" s="23" t="s">
-        <v>236</v>
-      </c>
-      <c r="E172" s="23" t="s">
-        <v>237</v>
-      </c>
-      <c r="F172" s="23" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="173" spans="1:6" ht="15.95" customHeight="1">
       <c r="A173" s="25" t="s">
+        <v>235</v>
+      </c>
+      <c r="B173" s="25" t="s">
+        <v>236</v>
+      </c>
+      <c r="C173" s="25" t="s">
+        <v>237</v>
+      </c>
+      <c r="D173" s="25" t="s">
+        <v>238</v>
+      </c>
+      <c r="E173" s="25" t="s">
         <v>239</v>
       </c>
-      <c r="B173" s="25" t="s">
+      <c r="F173" s="25" t="s">
         <v>240</v>
-      </c>
-      <c r="C173" s="25" t="s">
-        <v>241</v>
-      </c>
-      <c r="D173" s="25" t="s">
-        <v>242</v>
-      </c>
-      <c r="E173" s="25" t="s">
-        <v>243</v>
-      </c>
-      <c r="F173" s="25" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="174" spans="1:6" ht="15.95" customHeight="1"/>
@@ -19737,22 +19763,41 @@
     <row r="286" ht="15.95" customHeight="1"/>
     <row r="287" ht="15.95" customHeight="1"/>
     <row r="288" ht="15.95" customHeight="1"/>
-    <row r="289" ht="15.95" customHeight="1"/>
-    <row r="290" ht="15.95" customHeight="1"/>
-    <row r="291" ht="15.95" customHeight="1"/>
-    <row r="292" ht="15.95" customHeight="1"/>
-    <row r="293" ht="15.95" customHeight="1"/>
-    <row r="294" ht="15.95" customHeight="1"/>
-    <row r="295" ht="15.95" customHeight="1"/>
-    <row r="296" ht="15.95" customHeight="1"/>
-    <row r="297" ht="15.95" customHeight="1"/>
-    <row r="298" ht="15.95" customHeight="1"/>
-    <row r="299" ht="15.95" customHeight="1"/>
-    <row r="300" ht="15.95" customHeight="1"/>
-    <row r="301" ht="15.95" customHeight="1"/>
-    <row r="302" ht="15.95" customHeight="1"/>
-    <row r="303" ht="15.95" customHeight="1"/>
-    <row r="304" ht="15.95" customHeight="1"/>
+    <row r="289" spans="1:2" ht="15.95" customHeight="1"/>
+    <row r="290" spans="1:2" ht="15.95" customHeight="1"/>
+    <row r="291" spans="1:2" ht="15.95" customHeight="1">
+      <c r="A291" s="69" t="s">
+        <v>284</v>
+      </c>
+      <c r="B291" s="69"/>
+    </row>
+    <row r="292" spans="1:2" ht="15.95" customHeight="1">
+      <c r="A292" s="23" t="s">
+        <v>285</v>
+      </c>
+      <c r="B292" s="24" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="293" spans="1:2" ht="15.95" customHeight="1">
+      <c r="A293" s="25" t="s">
+        <v>287</v>
+      </c>
+      <c r="B293" s="25" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="294" spans="1:2" ht="15.95" customHeight="1"/>
+    <row r="295" spans="1:2" ht="15.95" customHeight="1"/>
+    <row r="296" spans="1:2" ht="15.95" customHeight="1"/>
+    <row r="297" spans="1:2" ht="15.95" customHeight="1"/>
+    <row r="298" spans="1:2" ht="15.95" customHeight="1"/>
+    <row r="299" spans="1:2" ht="15.95" customHeight="1"/>
+    <row r="300" spans="1:2" ht="15.95" customHeight="1"/>
+    <row r="301" spans="1:2" ht="15.95" customHeight="1"/>
+    <row r="302" spans="1:2" ht="15.95" customHeight="1"/>
+    <row r="303" spans="1:2" ht="15.95" customHeight="1"/>
+    <row r="304" spans="1:2" ht="15.95" customHeight="1"/>
     <row r="305" ht="15.95" customHeight="1"/>
     <row r="306" ht="15.95" customHeight="1"/>
     <row r="307" ht="15.95" customHeight="1"/>
@@ -20491,10 +20536,11 @@
     <row r="1040" ht="15.95" customHeight="1"/>
     <row r="1041" ht="15.95" customHeight="1"/>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A1:A4"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="B3:E3"/>
+    <mergeCell ref="A291:B291"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
@@ -20521,12 +20567,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="62" t="s">
         <v>71</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="26" t="s">
@@ -20585,11 +20631,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="63" t="s">
         <v>78</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="26" t="s">
@@ -20647,11 +20693,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="64" t="s">
         <v>84</v>
       </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
+      <c r="B1" s="64"/>
+      <c r="C1" s="64"/>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="26" t="s">
@@ -20709,11 +20755,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="64" t="s">
         <v>90</v>
       </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
+      <c r="B1" s="64"/>
+      <c r="C1" s="64"/>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="26" t="s">
@@ -20771,11 +20817,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="64" t="s">
         <v>95</v>
       </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
+      <c r="B1" s="64"/>
+      <c r="C1" s="64"/>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="9" t="s">
@@ -20833,11 +20879,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="64" t="s">
         <v>100</v>
       </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
+      <c r="B1" s="64"/>
+      <c r="C1" s="64"/>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="9" t="s">
@@ -20883,8 +20929,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:X121"/>
   <sheetViews>
-    <sheetView zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
@@ -20899,22 +20945,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="64" t="s">
         <v>105</v>
       </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
-      <c r="G1" s="61"/>
-      <c r="H1" s="61"/>
-      <c r="I1" s="61"/>
-      <c r="J1" s="61"/>
-      <c r="K1" s="61"/>
-      <c r="L1" s="61"/>
-      <c r="M1" s="61"/>
-      <c r="N1" s="61"/>
+      <c r="B1" s="64"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="64"/>
+      <c r="F1" s="64"/>
+      <c r="G1" s="64"/>
+      <c r="H1" s="64"/>
+      <c r="I1" s="64"/>
+      <c r="J1" s="64"/>
+      <c r="K1" s="64"/>
+      <c r="L1" s="64"/>
+      <c r="M1" s="64"/>
+      <c r="N1" s="64"/>
       <c r="O1" s="55"/>
       <c r="P1" s="55"/>
       <c r="Q1" s="55"/>
@@ -20948,14 +20994,14 @@
       <c r="G2" s="29" t="s">
         <v>111</v>
       </c>
-      <c r="H2" s="66" t="s">
-        <v>285</v>
-      </c>
-      <c r="I2" s="66" t="s">
-        <v>286</v>
-      </c>
-      <c r="J2" s="66" t="s">
-        <v>287</v>
+      <c r="H2" s="56" t="s">
+        <v>281</v>
+      </c>
+      <c r="I2" s="56" t="s">
+        <v>282</v>
+      </c>
+      <c r="J2" s="56" t="s">
+        <v>283</v>
       </c>
       <c r="K2" s="29" t="s">
         <v>112</v>
@@ -20996,8 +21042,8 @@
       <c r="W2" s="29" t="s">
         <v>122</v>
       </c>
-      <c r="X2" s="66" t="s">
-        <v>281</v>
+      <c r="X2" s="56" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="3" spans="1:24">
@@ -21022,14 +21068,14 @@
       <c r="G3" s="32" t="s">
         <v>129</v>
       </c>
-      <c r="H3" s="67" t="s">
-        <v>282</v>
-      </c>
-      <c r="I3" s="67" t="s">
-        <v>283</v>
-      </c>
-      <c r="J3" s="67" t="s">
-        <v>284</v>
+      <c r="H3" s="57" t="s">
+        <v>278</v>
+      </c>
+      <c r="I3" s="57" t="s">
+        <v>279</v>
+      </c>
+      <c r="J3" s="57" t="s">
+        <v>280</v>
       </c>
       <c r="K3" s="32" t="s">
         <v>130</v>
@@ -21070,8 +21116,8 @@
       <c r="W3" s="36" t="s">
         <v>140</v>
       </c>
-      <c r="X3" s="68" t="s">
-        <v>280</v>
+      <c r="X3" s="58" t="s">
+        <v>276</v>
       </c>
     </row>
     <row r="11" spans="1:24">
@@ -21118,31 +21164,31 @@
         <v>178</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
-      <c r="A40" s="40" t="s">
-        <v>179</v>
-      </c>
-      <c r="B40" s="40"/>
-      <c r="C40" s="40"/>
-      <c r="D40" s="40"/>
+    <row r="38" spans="1:4">
+      <c r="A38" s="40" t="s">
+        <v>289</v>
+      </c>
+      <c r="B38" s="40"/>
+      <c r="C38" s="40"/>
+      <c r="D38" s="40"/>
     </row>
-    <row r="41" spans="1:4">
-      <c r="A41" s="41" t="s">
+    <row r="39" spans="1:4">
+      <c r="A39" s="41" t="s">
         <v>170</v>
       </c>
-      <c r="B41" s="47" t="s">
-        <v>180</v>
-      </c>
-      <c r="C41" s="47" t="s">
-        <v>181</v>
-      </c>
-      <c r="D41" s="47" t="s">
-        <v>182</v>
+      <c r="B39" s="47" t="s">
+        <v>290</v>
+      </c>
+      <c r="C39" s="47" t="s">
+        <v>291</v>
+      </c>
+      <c r="D39" s="47" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="54" spans="1:8">
       <c r="A54" s="40" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="B54" s="40"/>
       <c r="C54" s="40"/>
@@ -21153,13 +21199,13 @@
         <v>170</v>
       </c>
       <c r="B55" s="49" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="C55" s="49" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="D55" s="49" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="E55" s="50"/>
       <c r="F55" s="50"/>
@@ -21179,18 +21225,18 @@
         <v>170</v>
       </c>
       <c r="B68" s="47" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="C68" s="47" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="D68" s="47" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
     </row>
     <row r="89" spans="1:4">
       <c r="A89" s="40" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="B89" s="40"/>
       <c r="C89" s="40"/>
@@ -21198,21 +21244,21 @@
     </row>
     <row r="90" spans="1:4">
       <c r="A90" s="41" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="B90" s="47" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="C90" s="47" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="D90" s="47" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="105" spans="1:8">
       <c r="A105" s="40" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="B105" s="40"/>
       <c r="C105" s="40"/>
@@ -21220,16 +21266,16 @@
     </row>
     <row r="106" spans="1:8" s="51" customFormat="1">
       <c r="A106" s="48" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="B106" s="49" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="C106" s="49" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="D106" s="49" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="E106" s="50"/>
       <c r="F106" s="50"/>
@@ -21237,19 +21283,19 @@
       <c r="H106" s="50"/>
     </row>
     <row r="120" spans="1:4">
-      <c r="A120" s="62" t="s">
-        <v>191</v>
-      </c>
-      <c r="B120" s="63"/>
+      <c r="A120" s="65" t="s">
+        <v>187</v>
+      </c>
+      <c r="B120" s="66"/>
       <c r="C120" s="40"/>
       <c r="D120" s="40"/>
     </row>
     <row r="121" spans="1:4" ht="60">
       <c r="A121" s="41" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="B121" s="42" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
     </row>
   </sheetData>
@@ -21291,95 +21337,95 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
-      <c r="A1" s="64" t="s">
-        <v>245</v>
-      </c>
-      <c r="B1" s="65"/>
-      <c r="C1" s="65"/>
-      <c r="D1" s="65"/>
-      <c r="E1" s="65"/>
-      <c r="F1" s="65"/>
-      <c r="G1" s="65"/>
-      <c r="H1" s="65"/>
-      <c r="I1" s="65"/>
-      <c r="J1" s="65"/>
-      <c r="K1" s="65"/>
-      <c r="L1" s="65"/>
+      <c r="A1" s="67" t="s">
+        <v>241</v>
+      </c>
+      <c r="B1" s="68"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="68"/>
+      <c r="G1" s="68"/>
+      <c r="H1" s="68"/>
+      <c r="I1" s="68"/>
+      <c r="J1" s="68"/>
+      <c r="K1" s="68"/>
+      <c r="L1" s="68"/>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="43" t="s">
+        <v>242</v>
+      </c>
+      <c r="B2" s="43" t="s">
+        <v>243</v>
+      </c>
+      <c r="C2" s="43" t="s">
+        <v>244</v>
+      </c>
+      <c r="D2" s="43" t="s">
+        <v>245</v>
+      </c>
+      <c r="E2" s="43" t="s">
         <v>246</v>
       </c>
-      <c r="B2" s="43" t="s">
+      <c r="F2" s="43" t="s">
         <v>247</v>
       </c>
-      <c r="C2" s="43" t="s">
+      <c r="G2" s="43" t="s">
         <v>248</v>
       </c>
-      <c r="D2" s="43" t="s">
+      <c r="H2" s="43" t="s">
         <v>249</v>
       </c>
-      <c r="E2" s="43" t="s">
+      <c r="I2" s="43" t="s">
         <v>250</v>
       </c>
-      <c r="F2" s="43" t="s">
+      <c r="J2" s="52" t="s">
+        <v>271</v>
+      </c>
+      <c r="K2" s="53" t="s">
+        <v>272</v>
+      </c>
+      <c r="L2" s="43" t="s">
         <v>251</v>
-      </c>
-      <c r="G2" s="43" t="s">
-        <v>252</v>
-      </c>
-      <c r="H2" s="43" t="s">
-        <v>253</v>
-      </c>
-      <c r="I2" s="43" t="s">
-        <v>254</v>
-      </c>
-      <c r="J2" s="52" t="s">
-        <v>275</v>
-      </c>
-      <c r="K2" s="53" t="s">
-        <v>276</v>
-      </c>
-      <c r="L2" s="43" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="15.6" customHeight="1">
       <c r="A3" s="44" t="s">
+        <v>252</v>
+      </c>
+      <c r="B3" s="45" t="s">
+        <v>253</v>
+      </c>
+      <c r="C3" s="46" t="s">
+        <v>254</v>
+      </c>
+      <c r="D3" s="44" t="s">
+        <v>255</v>
+      </c>
+      <c r="E3" s="45" t="s">
         <v>256</v>
       </c>
-      <c r="B3" s="45" t="s">
+      <c r="F3" s="45" t="s">
         <v>257</v>
       </c>
-      <c r="C3" s="46" t="s">
+      <c r="G3" s="45" t="s">
         <v>258</v>
       </c>
-      <c r="D3" s="44" t="s">
+      <c r="H3" s="45" t="s">
         <v>259</v>
       </c>
-      <c r="E3" s="45" t="s">
+      <c r="I3" s="45" t="s">
         <v>260</v>
       </c>
-      <c r="F3" s="45" t="s">
+      <c r="J3" s="45" t="s">
+        <v>273</v>
+      </c>
+      <c r="K3" s="54" t="s">
+        <v>274</v>
+      </c>
+      <c r="L3" s="54" t="s">
         <v>261</v>
-      </c>
-      <c r="G3" s="45" t="s">
-        <v>262</v>
-      </c>
-      <c r="H3" s="45" t="s">
-        <v>263</v>
-      </c>
-      <c r="I3" s="45" t="s">
-        <v>264</v>
-      </c>
-      <c r="J3" s="45" t="s">
-        <v>277</v>
-      </c>
-      <c r="K3" s="54" t="s">
-        <v>278</v>
-      </c>
-      <c r="L3" s="54" t="s">
-        <v>265</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
POCOR-7378: code enhance for count staff in Institution Report Cards | Status: Done
</commit_message>
<xml_diff>
--- a/webroot/export/customexcel/default_templates/profile_template.xlsx
+++ b/webroot/export/customexcel/default_templates/profile_template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10305" tabRatio="862"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10305" tabRatio="862" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="304">
   <si>
     <t>${"image":{"displayValue":"Institutions.logo_content","imageWidth":"100","imageMarginLeft":"20","imageMarginTop":"5"}}</t>
   </si>
@@ -908,6 +908,39 @@
   </si>
   <si>
     <t xml:space="preserve">${"match": {"displayValue": "InstitutionStudentPromoted.area_level:3","rows": {"matchFrom": "InstitutionEducationGrade.id","matchTo": "InstitutionEducationGrade.id"}}} </t>
+  </si>
+  <si>
+    <t>Count of  Institution Subject Staff Per Education Programme</t>
+  </si>
+  <si>
+    <t>Education Programme</t>
+  </si>
+  <si>
+    <t>Total Teaching Staff</t>
+  </si>
+  <si>
+    <t>Total Teaching Male Staff</t>
+  </si>
+  <si>
+    <t>Total Teaching Female Staff</t>
+  </si>
+  <si>
+    <t>Total Temporary Teaching Staff</t>
+  </si>
+  <si>
+    <t>${"match": {"displayValue": "InstitutionEducationProgramme.programme_name","rows": {"matchFrom": "InstitutionEducationProgramme.programme_id","matchTo": "InstitutionEducationProgramme.programme_id"}}}</t>
+  </si>
+  <si>
+    <t>${"match": {"displayValue": "StaffFromEducationProgramme.subject_staff","rows": {"matchFrom": "StaffFromEducationProgramme.programme_id","matchTo": "StaffFromEducationProgramme.programme_id"}}}</t>
+  </si>
+  <si>
+    <t>${"match": {"displayValue": "StaffFromEducationProgramme.male_subject_staff","rows": {"matchFrom": "StaffFromEducationProgramme.programme_id","matchTo": "StaffFromEducationProgramme.programme_id"}}}</t>
+  </si>
+  <si>
+    <t>${"match": {"displayValue": "StaffFromEducationProgramme.female_subject_staff","rows": {"matchFrom": "StaffFromEducationProgramme.programme_id","matchTo": "StaffFromEducationProgramme.programme_id"}}}</t>
+  </si>
+  <si>
+    <t>${"match": {"displayValue": "StaffFromEducationProgramme.subject_staff_type_temporary","rows": {"matchFrom": "StaffFromEducationProgramme.programme_id","matchTo": "StaffFromEducationProgramme.programme_id"}}}</t>
   </si>
 </sst>
 </file>
@@ -1180,7 +1213,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1302,6 +1335,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1314,6 +1348,12 @@
     <xf numFmtId="49" fontId="5" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1322,18 +1362,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1354,6 +1382,18 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1728,7 +1768,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:IV1041"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A121" zoomScalePageLayoutView="60" workbookViewId="0">
+    <sheetView topLeftCell="A121" zoomScalePageLayoutView="60" workbookViewId="0">
       <selection activeCell="B309" sqref="B309"/>
     </sheetView>
   </sheetViews>
@@ -1750,7 +1790,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:256" ht="15" customHeight="1">
-      <c r="A1" s="55" t="s">
+      <c r="A1" s="56" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2"/>
@@ -1771,13 +1811,13 @@
       <c r="Q1" s="5"/>
     </row>
     <row r="2" spans="1:256" ht="25.5" customHeight="1">
-      <c r="A2" s="55"/>
-      <c r="B2" s="56" t="s">
+      <c r="A2" s="56"/>
+      <c r="B2" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="56"/>
-      <c r="D2" s="56"/>
-      <c r="E2" s="56"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
       <c r="F2" s="6"/>
       <c r="G2" s="7"/>
       <c r="H2" s="5"/>
@@ -2031,13 +2071,13 @@
       <c r="IV2" s="1"/>
     </row>
     <row r="3" spans="1:256" ht="25.5" customHeight="1">
-      <c r="A3" s="55"/>
-      <c r="B3" s="57" t="s">
+      <c r="A3" s="56"/>
+      <c r="B3" s="58" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="57"/>
-      <c r="D3" s="57"/>
-      <c r="E3" s="57"/>
+      <c r="C3" s="58"/>
+      <c r="D3" s="58"/>
+      <c r="E3" s="58"/>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
       <c r="H3" s="5"/>
@@ -2291,7 +2331,7 @@
       <c r="IV3" s="1"/>
     </row>
     <row r="4" spans="1:256" ht="22.5" customHeight="1">
-      <c r="A4" s="55"/>
+      <c r="A4" s="56"/>
       <c r="B4" s="2"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
@@ -6630,11 +6670,11 @@
       <c r="IV26" s="1"/>
     </row>
     <row r="27" spans="1:256" ht="12" customHeight="1">
-      <c r="A27" s="64" t="s">
+      <c r="A27" s="60" t="s">
         <v>30</v>
       </c>
-      <c r="B27" s="65"/>
-      <c r="C27" s="65"/>
+      <c r="B27" s="61"/>
+      <c r="C27" s="61"/>
       <c r="D27" s="16"/>
       <c r="E27" s="12"/>
       <c r="F27" s="12"/>
@@ -13926,11 +13966,11 @@
       <c r="IV54" s="1"/>
     </row>
     <row r="55" spans="1:256" ht="12" customHeight="1">
-      <c r="A55" s="64" t="s">
+      <c r="A55" s="60" t="s">
         <v>141</v>
       </c>
-      <c r="B55" s="65"/>
-      <c r="C55" s="65"/>
+      <c r="B55" s="61"/>
+      <c r="C55" s="61"/>
       <c r="D55" s="16"/>
       <c r="E55" s="12"/>
       <c r="F55" s="12"/>
@@ -15764,10 +15804,10 @@
       <c r="IV61" s="1"/>
     </row>
     <row r="62" spans="1:256" ht="12" customHeight="1">
-      <c r="A62" s="58" t="s">
+      <c r="A62" s="59" t="s">
         <v>66</v>
       </c>
-      <c r="B62" s="58"/>
+      <c r="B62" s="59"/>
       <c r="C62" s="14"/>
       <c r="D62" s="16"/>
       <c r="E62" s="12"/>
@@ -18116,10 +18156,10 @@
       <c r="IV71" s="1"/>
     </row>
     <row r="72" spans="1:256" ht="12" customHeight="1">
-      <c r="A72" s="58" t="s">
+      <c r="A72" s="59" t="s">
         <v>190</v>
       </c>
-      <c r="B72" s="58"/>
+      <c r="B72" s="59"/>
       <c r="C72" s="1"/>
       <c r="E72" s="1"/>
       <c r="F72" s="1"/>
@@ -19440,24 +19480,24 @@
     <row r="96" ht="15.95" customHeight="1"/>
     <row r="97" spans="1:16" ht="15.95" customHeight="1"/>
     <row r="98" spans="1:16" ht="15.95" customHeight="1">
-      <c r="A98" s="58" t="s">
+      <c r="A98" s="59" t="s">
         <v>196</v>
       </c>
-      <c r="B98" s="58"/>
-      <c r="C98" s="58"/>
-      <c r="D98" s="58"/>
-      <c r="E98" s="58"/>
-      <c r="F98" s="58"/>
-      <c r="G98" s="58"/>
-      <c r="H98" s="58"/>
-      <c r="I98" s="58"/>
-      <c r="J98" s="58"/>
-      <c r="K98" s="58"/>
-      <c r="L98" s="58"/>
-      <c r="M98" s="58"/>
-      <c r="N98" s="58"/>
-      <c r="O98" s="58"/>
-      <c r="P98" s="58"/>
+      <c r="B98" s="59"/>
+      <c r="C98" s="59"/>
+      <c r="D98" s="59"/>
+      <c r="E98" s="59"/>
+      <c r="F98" s="59"/>
+      <c r="G98" s="59"/>
+      <c r="H98" s="59"/>
+      <c r="I98" s="59"/>
+      <c r="J98" s="59"/>
+      <c r="K98" s="59"/>
+      <c r="L98" s="59"/>
+      <c r="M98" s="59"/>
+      <c r="N98" s="59"/>
+      <c r="O98" s="59"/>
+      <c r="P98" s="59"/>
     </row>
     <row r="99" spans="1:16" ht="15.95" customHeight="1">
       <c r="A99" s="21" t="s">
@@ -19630,14 +19670,14 @@
     <row r="169" spans="1:6" ht="15.95" customHeight="1"/>
     <row r="170" spans="1:6" ht="15.95" customHeight="1"/>
     <row r="171" spans="1:6" ht="15.95" customHeight="1">
-      <c r="A171" s="58" t="s">
+      <c r="A171" s="59" t="s">
         <v>195</v>
       </c>
-      <c r="B171" s="58"/>
-      <c r="C171" s="58"/>
-      <c r="D171" s="58"/>
-      <c r="E171" s="58"/>
-      <c r="F171" s="58"/>
+      <c r="B171" s="59"/>
+      <c r="C171" s="59"/>
+      <c r="D171" s="59"/>
+      <c r="E171" s="59"/>
+      <c r="F171" s="59"/>
     </row>
     <row r="172" spans="1:6" ht="15.95" customHeight="1">
       <c r="A172" s="21" t="s">
@@ -19797,10 +19837,10 @@
     <row r="289" spans="1:2" ht="15.95" customHeight="1"/>
     <row r="290" spans="1:2" ht="15.95" customHeight="1"/>
     <row r="291" spans="1:2" ht="15.95" customHeight="1">
-      <c r="A291" s="58" t="s">
+      <c r="A291" s="59" t="s">
         <v>284</v>
       </c>
-      <c r="B291" s="58"/>
+      <c r="B291" s="59"/>
     </row>
     <row r="292" spans="1:2" ht="15.95" customHeight="1">
       <c r="A292" s="21" t="s">
@@ -20604,12 +20644,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="62" t="s">
         <v>71</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="24" t="s">
@@ -20668,11 +20708,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="63" t="s">
         <v>78</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="24" t="s">
@@ -20730,11 +20770,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="64" t="s">
         <v>84</v>
       </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
+      <c r="B1" s="64"/>
+      <c r="C1" s="64"/>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="24" t="s">
@@ -20792,11 +20832,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="64" t="s">
         <v>90</v>
       </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
+      <c r="B1" s="64"/>
+      <c r="C1" s="64"/>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="24" t="s">
@@ -20854,11 +20894,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="64" t="s">
         <v>95</v>
       </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
+      <c r="B1" s="64"/>
+      <c r="C1" s="64"/>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="7" t="s">
@@ -20916,11 +20956,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="64" t="s">
         <v>100</v>
       </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
+      <c r="B1" s="64"/>
+      <c r="C1" s="64"/>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="7" t="s">
@@ -20964,10 +21004,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:X121"/>
+  <dimension ref="A1:X144"/>
   <sheetViews>
-    <sheetView topLeftCell="A100" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+    <sheetView tabSelected="1" topLeftCell="A119" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="B147" sqref="B147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
@@ -20982,32 +21022,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="64" t="s">
         <v>105</v>
       </c>
-      <c r="B1" s="72"/>
-      <c r="C1" s="72"/>
-      <c r="D1" s="72"/>
-      <c r="E1" s="72"/>
-      <c r="F1" s="72"/>
-      <c r="G1" s="72"/>
-      <c r="H1" s="72"/>
-      <c r="I1" s="72"/>
-      <c r="J1" s="72"/>
-      <c r="K1" s="72"/>
-      <c r="L1" s="72"/>
-      <c r="M1" s="72"/>
-      <c r="N1" s="72"/>
-      <c r="O1" s="72"/>
-      <c r="P1" s="72"/>
-      <c r="Q1" s="72"/>
-      <c r="R1" s="72"/>
-      <c r="S1" s="72"/>
-      <c r="T1" s="72"/>
-      <c r="U1" s="72"/>
-      <c r="V1" s="72"/>
-      <c r="W1" s="72"/>
-      <c r="X1" s="72"/>
+      <c r="B1" s="71"/>
+      <c r="C1" s="71"/>
+      <c r="D1" s="71"/>
+      <c r="E1" s="71"/>
+      <c r="F1" s="71"/>
+      <c r="G1" s="71"/>
+      <c r="H1" s="71"/>
+      <c r="I1" s="71"/>
+      <c r="J1" s="71"/>
+      <c r="K1" s="71"/>
+      <c r="L1" s="71"/>
+      <c r="M1" s="71"/>
+      <c r="N1" s="71"/>
+      <c r="O1" s="71"/>
+      <c r="P1" s="71"/>
+      <c r="Q1" s="71"/>
+      <c r="R1" s="71"/>
+      <c r="S1" s="71"/>
+      <c r="T1" s="71"/>
+      <c r="U1" s="71"/>
+      <c r="V1" s="71"/>
+      <c r="W1" s="71"/>
+      <c r="X1" s="71"/>
     </row>
     <row r="2" spans="1:24">
       <c r="A2" s="27" t="s">
@@ -21158,12 +21198,12 @@
       </c>
     </row>
     <row r="11" spans="1:24">
-      <c r="A11" s="66" t="s">
+      <c r="A11" s="65" t="s">
         <v>175</v>
       </c>
-      <c r="B11" s="67"/>
-      <c r="C11" s="67"/>
-      <c r="D11" s="68"/>
+      <c r="B11" s="66"/>
+      <c r="C11" s="66"/>
+      <c r="D11" s="67"/>
     </row>
     <row r="12" spans="1:24">
       <c r="A12" s="38" t="s">
@@ -21180,12 +21220,12 @@
       </c>
     </row>
     <row r="24" spans="1:4">
-      <c r="A24" s="66" t="s">
+      <c r="A24" s="65" t="s">
         <v>174</v>
       </c>
-      <c r="B24" s="67"/>
-      <c r="C24" s="67"/>
-      <c r="D24" s="68"/>
+      <c r="B24" s="66"/>
+      <c r="C24" s="66"/>
+      <c r="D24" s="67"/>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="38" t="s">
@@ -21202,12 +21242,12 @@
       </c>
     </row>
     <row r="38" spans="1:4">
-      <c r="A38" s="66" t="s">
+      <c r="A38" s="65" t="s">
         <v>289</v>
       </c>
-      <c r="B38" s="67"/>
-      <c r="C38" s="67"/>
-      <c r="D38" s="68"/>
+      <c r="B38" s="66"/>
+      <c r="C38" s="66"/>
+      <c r="D38" s="67"/>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="38" t="s">
@@ -21224,12 +21264,12 @@
       </c>
     </row>
     <row r="54" spans="1:8">
-      <c r="A54" s="66" t="s">
+      <c r="A54" s="65" t="s">
         <v>262</v>
       </c>
-      <c r="B54" s="67"/>
-      <c r="C54" s="67"/>
-      <c r="D54" s="68"/>
+      <c r="B54" s="66"/>
+      <c r="C54" s="66"/>
+      <c r="D54" s="67"/>
     </row>
     <row r="55" spans="1:8">
       <c r="A55" s="45" t="s">
@@ -21250,12 +21290,12 @@
       <c r="H55" s="47"/>
     </row>
     <row r="67" spans="1:4">
-      <c r="A67" s="66" t="s">
+      <c r="A67" s="65" t="s">
         <v>169</v>
       </c>
-      <c r="B67" s="67"/>
-      <c r="C67" s="67"/>
-      <c r="D67" s="68"/>
+      <c r="B67" s="66"/>
+      <c r="C67" s="66"/>
+      <c r="D67" s="67"/>
     </row>
     <row r="68" spans="1:4">
       <c r="A68" s="38" t="s">
@@ -21272,12 +21312,12 @@
       </c>
     </row>
     <row r="89" spans="1:4">
-      <c r="A89" s="66" t="s">
+      <c r="A89" s="65" t="s">
         <v>182</v>
       </c>
-      <c r="B89" s="67"/>
-      <c r="C89" s="67"/>
-      <c r="D89" s="68"/>
+      <c r="B89" s="66"/>
+      <c r="C89" s="66"/>
+      <c r="D89" s="67"/>
     </row>
     <row r="90" spans="1:4">
       <c r="A90" s="38" t="s">
@@ -21294,12 +21334,12 @@
       </c>
     </row>
     <row r="105" spans="1:8">
-      <c r="A105" s="66" t="s">
+      <c r="A105" s="65" t="s">
         <v>266</v>
       </c>
-      <c r="B105" s="67"/>
-      <c r="C105" s="67"/>
-      <c r="D105" s="68"/>
+      <c r="B105" s="66"/>
+      <c r="C105" s="66"/>
+      <c r="D105" s="67"/>
     </row>
     <row r="106" spans="1:8" s="48" customFormat="1">
       <c r="A106" s="45" t="s">
@@ -21320,12 +21360,12 @@
       <c r="H106" s="47"/>
     </row>
     <row r="120" spans="1:4">
-      <c r="A120" s="69" t="s">
+      <c r="A120" s="68" t="s">
         <v>187</v>
       </c>
-      <c r="B120" s="70"/>
-      <c r="C120" s="70"/>
-      <c r="D120" s="71"/>
+      <c r="B120" s="69"/>
+      <c r="C120" s="69"/>
+      <c r="D120" s="70"/>
     </row>
     <row r="121" spans="1:4" ht="60">
       <c r="A121" s="38" t="s">
@@ -21335,17 +21375,61 @@
         <v>189</v>
       </c>
     </row>
+    <row r="142" spans="1:5">
+      <c r="A142" s="72" t="s">
+        <v>293</v>
+      </c>
+      <c r="B142" s="73"/>
+      <c r="C142" s="73"/>
+      <c r="D142" s="73"/>
+      <c r="E142" s="73"/>
+    </row>
+    <row r="143" spans="1:5">
+      <c r="A143" s="52" t="s">
+        <v>294</v>
+      </c>
+      <c r="B143" s="52" t="s">
+        <v>295</v>
+      </c>
+      <c r="C143" s="52" t="s">
+        <v>296</v>
+      </c>
+      <c r="D143" s="52" t="s">
+        <v>297</v>
+      </c>
+      <c r="E143" s="52" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5">
+      <c r="A144" s="55" t="s">
+        <v>299</v>
+      </c>
+      <c r="B144" t="s">
+        <v>300</v>
+      </c>
+      <c r="C144" t="s">
+        <v>301</v>
+      </c>
+      <c r="D144" t="s">
+        <v>302</v>
+      </c>
+      <c r="E144" t="s">
+        <v>303</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="10">
+    <mergeCell ref="A89:D89"/>
+    <mergeCell ref="A105:D105"/>
+    <mergeCell ref="A120:D120"/>
+    <mergeCell ref="A1:X1"/>
+    <mergeCell ref="A142:E142"/>
     <mergeCell ref="A11:D11"/>
     <mergeCell ref="A38:D38"/>
     <mergeCell ref="A24:D24"/>
     <mergeCell ref="A54:D54"/>
     <mergeCell ref="A67:D67"/>
-    <mergeCell ref="A89:D89"/>
-    <mergeCell ref="A105:D105"/>
-    <mergeCell ref="A120:D120"/>
-    <mergeCell ref="A1:X1"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -21381,20 +21465,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
-      <c r="A1" s="62" t="s">
+      <c r="A1" s="74" t="s">
         <v>241</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
-      <c r="G1" s="63"/>
-      <c r="H1" s="63"/>
-      <c r="I1" s="63"/>
-      <c r="J1" s="63"/>
-      <c r="K1" s="63"/>
-      <c r="L1" s="63"/>
+      <c r="B1" s="75"/>
+      <c r="C1" s="75"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="75"/>
+      <c r="F1" s="75"/>
+      <c r="G1" s="75"/>
+      <c r="H1" s="75"/>
+      <c r="I1" s="75"/>
+      <c r="J1" s="75"/>
+      <c r="K1" s="75"/>
+      <c r="L1" s="75"/>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="40" t="s">

</xml_diff>

<commit_message>
POCOR-7411: add placeholders in institution report cards | Status: Done
</commit_message>
<xml_diff>
--- a/webroot/export/customexcel/default_templates/profile_template.xlsx
+++ b/webroot/export/customexcel/default_templates/profile_template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10305" tabRatio="862" activeTab="7"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10305" tabRatio="862"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="308">
   <si>
     <t>${"image":{"displayValue":"Institutions.logo_content","imageWidth":"100","imageMarginLeft":"20","imageMarginTop":"5"}}</t>
   </si>
@@ -941,6 +941,18 @@
   </si>
   <si>
     <t>${"match": {"displayValue": "StaffFromEducationProgramme.subject_staff_type_temporary","rows": {"matchFrom": "StaffFromEducationProgramme.programme_id","matchTo": "StaffFromEducationProgramme.programme_id"}}}</t>
+  </si>
+  <si>
+    <t>Jordon Shift</t>
+  </si>
+  <si>
+    <t>${JordonSchoolShifts.jordan_shift}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total Non Teaching Staff : </t>
+  </si>
+  <si>
+    <t>${TotalNonTeachingStaffs}</t>
   </si>
 </sst>
 </file>
@@ -1766,10 +1778,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:IV1041"/>
+  <dimension ref="A1:IV1043"/>
   <sheetViews>
-    <sheetView topLeftCell="A121" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="B309" sqref="B309"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75"/>
@@ -9277,10 +9289,10 @@
     </row>
     <row r="37" spans="1:256" ht="12" customHeight="1">
       <c r="A37" s="18" t="s">
-        <v>43</v>
+        <v>306</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>44</v>
+        <v>307</v>
       </c>
       <c r="C37" s="16"/>
       <c r="D37" s="16"/>
@@ -9538,8 +9550,12 @@
       <c r="IV37" s="1"/>
     </row>
     <row r="38" spans="1:256" ht="12" customHeight="1">
-      <c r="A38" s="15"/>
-      <c r="B38" s="16"/>
+      <c r="A38" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="B38" s="10" t="s">
+        <v>44</v>
+      </c>
       <c r="C38" s="16"/>
       <c r="D38" s="16"/>
       <c r="E38" s="12"/>
@@ -10054,12 +10070,8 @@
       <c r="IV39" s="1"/>
     </row>
     <row r="40" spans="1:256" ht="12" customHeight="1">
-      <c r="A40" s="19" t="s">
-        <v>45</v>
-      </c>
-      <c r="B40" s="10" t="s">
-        <v>46</v>
-      </c>
+      <c r="A40" s="15"/>
+      <c r="B40" s="16"/>
       <c r="C40" s="16"/>
       <c r="D40" s="16"/>
       <c r="E40" s="12"/>
@@ -10317,10 +10329,10 @@
     </row>
     <row r="41" spans="1:256" ht="12" customHeight="1">
       <c r="A41" s="19" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B41" s="10" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C41" s="16"/>
       <c r="D41" s="16"/>
@@ -10578,8 +10590,12 @@
       <c r="IV41" s="1"/>
     </row>
     <row r="42" spans="1:256" ht="12" customHeight="1">
-      <c r="A42" s="15"/>
-      <c r="B42" s="16"/>
+      <c r="A42" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="B42" s="10" t="s">
+        <v>48</v>
+      </c>
       <c r="C42" s="16"/>
       <c r="D42" s="16"/>
       <c r="E42" s="12"/>
@@ -11094,12 +11110,8 @@
       <c r="IV43" s="1"/>
     </row>
     <row r="44" spans="1:256" ht="12" customHeight="1">
-      <c r="A44" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="B44" s="20" t="s">
-        <v>50</v>
-      </c>
+      <c r="A44" s="15"/>
+      <c r="B44" s="16"/>
       <c r="C44" s="16"/>
       <c r="D44" s="16"/>
       <c r="E44" s="12"/>
@@ -11357,10 +11369,10 @@
     </row>
     <row r="45" spans="1:256" ht="12" customHeight="1">
       <c r="A45" s="9" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B45" s="20" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C45" s="16"/>
       <c r="D45" s="16"/>
@@ -11619,10 +11631,10 @@
     </row>
     <row r="46" spans="1:256" ht="12" customHeight="1">
       <c r="A46" s="9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B46" s="20" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C46" s="16"/>
       <c r="D46" s="16"/>
@@ -11881,10 +11893,10 @@
     </row>
     <row r="47" spans="1:256" ht="12" customHeight="1">
       <c r="A47" s="9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B47" s="20" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C47" s="16"/>
       <c r="D47" s="16"/>
@@ -12143,10 +12155,10 @@
     </row>
     <row r="48" spans="1:256" ht="12" customHeight="1">
       <c r="A48" s="9" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B48" s="20" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C48" s="16"/>
       <c r="D48" s="16"/>
@@ -12405,10 +12417,10 @@
     </row>
     <row r="49" spans="1:256" ht="12" customHeight="1">
       <c r="A49" s="9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B49" s="20" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C49" s="16"/>
       <c r="D49" s="16"/>
@@ -12667,10 +12679,10 @@
     </row>
     <row r="50" spans="1:256" ht="12" customHeight="1">
       <c r="A50" s="9" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B50" s="20" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C50" s="16"/>
       <c r="D50" s="16"/>
@@ -12929,9 +12941,11 @@
     </row>
     <row r="51" spans="1:256" ht="12" customHeight="1">
       <c r="A51" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="B51" s="20"/>
+        <v>61</v>
+      </c>
+      <c r="B51" s="20" t="s">
+        <v>62</v>
+      </c>
       <c r="C51" s="16"/>
       <c r="D51" s="16"/>
       <c r="E51" s="12"/>
@@ -13189,11 +13203,9 @@
     </row>
     <row r="52" spans="1:256" ht="12" customHeight="1">
       <c r="A52" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="B52" s="20" t="s">
-        <v>65</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="B52" s="20"/>
       <c r="C52" s="16"/>
       <c r="D52" s="16"/>
       <c r="E52" s="12"/>
@@ -13450,8 +13462,12 @@
       <c r="IV52" s="1"/>
     </row>
     <row r="53" spans="1:256" ht="12" customHeight="1">
-      <c r="A53" s="15"/>
-      <c r="B53" s="16"/>
+      <c r="A53" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="B53" s="20" t="s">
+        <v>65</v>
+      </c>
       <c r="C53" s="16"/>
       <c r="D53" s="16"/>
       <c r="E53" s="12"/>
@@ -13708,8 +13724,12 @@
       <c r="IV53" s="1"/>
     </row>
     <row r="54" spans="1:256" ht="12" customHeight="1">
-      <c r="A54" s="15"/>
-      <c r="B54" s="16"/>
+      <c r="A54" s="9" t="s">
+        <v>304</v>
+      </c>
+      <c r="B54" s="20" t="s">
+        <v>305</v>
+      </c>
       <c r="C54" s="16"/>
       <c r="D54" s="16"/>
       <c r="E54" s="12"/>
@@ -13966,275 +13986,12 @@
       <c r="IV54" s="1"/>
     </row>
     <row r="55" spans="1:256" ht="12" customHeight="1">
-      <c r="A55" s="60" t="s">
-        <v>141</v>
-      </c>
-      <c r="B55" s="61"/>
-      <c r="C55" s="61"/>
-      <c r="D55" s="16"/>
-      <c r="E55" s="12"/>
-      <c r="F55" s="12"/>
-      <c r="G55" s="12"/>
-      <c r="H55" s="12"/>
-      <c r="I55" s="5"/>
-      <c r="J55" s="5"/>
-      <c r="K55" s="5"/>
-      <c r="L55" s="5"/>
-      <c r="M55" s="5"/>
-      <c r="N55" s="5"/>
-      <c r="O55" s="5"/>
-      <c r="P55" s="5"/>
-      <c r="Q55" s="5"/>
-      <c r="R55" s="5"/>
-      <c r="S55" s="1"/>
-      <c r="T55" s="1"/>
-      <c r="U55" s="1"/>
-      <c r="V55" s="1"/>
-      <c r="W55" s="1"/>
-      <c r="X55" s="1"/>
-      <c r="Y55" s="1"/>
-      <c r="Z55" s="1"/>
-      <c r="AA55" s="1"/>
-      <c r="AB55" s="1"/>
-      <c r="AC55" s="1"/>
-      <c r="AD55" s="1"/>
-      <c r="AE55" s="1"/>
-      <c r="AF55" s="1"/>
-      <c r="AG55" s="1"/>
-      <c r="AH55" s="1"/>
-      <c r="AI55" s="1"/>
-      <c r="AJ55" s="1"/>
-      <c r="AK55" s="1"/>
-      <c r="AL55" s="1"/>
-      <c r="AM55" s="1"/>
-      <c r="AN55" s="1"/>
-      <c r="AO55" s="1"/>
-      <c r="AP55" s="1"/>
-      <c r="AQ55" s="1"/>
-      <c r="AR55" s="1"/>
-      <c r="AS55" s="1"/>
-      <c r="AT55" s="1"/>
-      <c r="AU55" s="1"/>
-      <c r="AV55" s="1"/>
-      <c r="AW55" s="1"/>
-      <c r="AX55" s="1"/>
-      <c r="AY55" s="1"/>
-      <c r="AZ55" s="1"/>
-      <c r="BA55" s="1"/>
-      <c r="BB55" s="1"/>
-      <c r="BC55" s="1"/>
-      <c r="BD55" s="1"/>
-      <c r="BE55" s="1"/>
-      <c r="BF55" s="1"/>
-      <c r="BG55" s="1"/>
-      <c r="BH55" s="1"/>
-      <c r="BI55" s="1"/>
-      <c r="BJ55" s="1"/>
-      <c r="BK55" s="1"/>
-      <c r="BL55" s="1"/>
-      <c r="BM55" s="1"/>
-      <c r="BN55" s="1"/>
-      <c r="BO55" s="1"/>
-      <c r="BP55" s="1"/>
-      <c r="BQ55" s="1"/>
-      <c r="BR55" s="1"/>
-      <c r="BS55" s="1"/>
-      <c r="BT55" s="1"/>
-      <c r="BU55" s="1"/>
-      <c r="BV55" s="1"/>
-      <c r="BW55" s="1"/>
-      <c r="BX55" s="1"/>
-      <c r="BY55" s="1"/>
-      <c r="BZ55" s="1"/>
-      <c r="CA55" s="1"/>
-      <c r="CB55" s="1"/>
-      <c r="CC55" s="1"/>
-      <c r="CD55" s="1"/>
-      <c r="CE55" s="1"/>
-      <c r="CF55" s="1"/>
-      <c r="CG55" s="1"/>
-      <c r="CH55" s="1"/>
-      <c r="CI55" s="1"/>
-      <c r="CJ55" s="1"/>
-      <c r="CK55" s="1"/>
-      <c r="CL55" s="1"/>
-      <c r="CM55" s="1"/>
-      <c r="CN55" s="1"/>
-      <c r="CO55" s="1"/>
-      <c r="CP55" s="1"/>
-      <c r="CQ55" s="1"/>
-      <c r="CR55" s="1"/>
-      <c r="CS55" s="1"/>
-      <c r="CT55" s="1"/>
-      <c r="CU55" s="1"/>
-      <c r="CV55" s="1"/>
-      <c r="CW55" s="1"/>
-      <c r="CX55" s="1"/>
-      <c r="CY55" s="1"/>
-      <c r="CZ55" s="1"/>
-      <c r="DA55" s="1"/>
-      <c r="DB55" s="1"/>
-      <c r="DC55" s="1"/>
-      <c r="DD55" s="1"/>
-      <c r="DE55" s="1"/>
-      <c r="DF55" s="1"/>
-      <c r="DG55" s="1"/>
-      <c r="DH55" s="1"/>
-      <c r="DI55" s="1"/>
-      <c r="DJ55" s="1"/>
-      <c r="DK55" s="1"/>
-      <c r="DL55" s="1"/>
-      <c r="DM55" s="1"/>
-      <c r="DN55" s="1"/>
-      <c r="DO55" s="1"/>
-      <c r="DP55" s="1"/>
-      <c r="DQ55" s="1"/>
-      <c r="DR55" s="1"/>
-      <c r="DS55" s="1"/>
-      <c r="DT55" s="1"/>
-      <c r="DU55" s="1"/>
-      <c r="DV55" s="1"/>
-      <c r="DW55" s="1"/>
-      <c r="DX55" s="1"/>
-      <c r="DY55" s="1"/>
-      <c r="DZ55" s="1"/>
-      <c r="EA55" s="1"/>
-      <c r="EB55" s="1"/>
-      <c r="EC55" s="1"/>
-      <c r="ED55" s="1"/>
-      <c r="EE55" s="1"/>
-      <c r="EF55" s="1"/>
-      <c r="EG55" s="1"/>
-      <c r="EH55" s="1"/>
-      <c r="EI55" s="1"/>
-      <c r="EJ55" s="1"/>
-      <c r="EK55" s="1"/>
-      <c r="EL55" s="1"/>
-      <c r="EM55" s="1"/>
-      <c r="EN55" s="1"/>
-      <c r="EO55" s="1"/>
-      <c r="EP55" s="1"/>
-      <c r="EQ55" s="1"/>
-      <c r="ER55" s="1"/>
-      <c r="ES55" s="1"/>
-      <c r="ET55" s="1"/>
-      <c r="EU55" s="1"/>
-      <c r="EV55" s="1"/>
-      <c r="EW55" s="1"/>
-      <c r="EX55" s="1"/>
-      <c r="EY55" s="1"/>
-      <c r="EZ55" s="1"/>
-      <c r="FA55" s="1"/>
-      <c r="FB55" s="1"/>
-      <c r="FC55" s="1"/>
-      <c r="FD55" s="1"/>
-      <c r="FE55" s="1"/>
-      <c r="FF55" s="1"/>
-      <c r="FG55" s="1"/>
-      <c r="FH55" s="1"/>
-      <c r="FI55" s="1"/>
-      <c r="FJ55" s="1"/>
-      <c r="FK55" s="1"/>
-      <c r="FL55" s="1"/>
-      <c r="FM55" s="1"/>
-      <c r="FN55" s="1"/>
-      <c r="FO55" s="1"/>
-      <c r="FP55" s="1"/>
-      <c r="FQ55" s="1"/>
-      <c r="FR55" s="1"/>
-      <c r="FS55" s="1"/>
-      <c r="FT55" s="1"/>
-      <c r="FU55" s="1"/>
-      <c r="FV55" s="1"/>
-      <c r="FW55" s="1"/>
-      <c r="FX55" s="1"/>
-      <c r="FY55" s="1"/>
-      <c r="FZ55" s="1"/>
-      <c r="GA55" s="1"/>
-      <c r="GB55" s="1"/>
-      <c r="GC55" s="1"/>
-      <c r="GD55" s="1"/>
-      <c r="GE55" s="1"/>
-      <c r="GF55" s="1"/>
-      <c r="GG55" s="1"/>
-      <c r="GH55" s="1"/>
-      <c r="GI55" s="1"/>
-      <c r="GJ55" s="1"/>
-      <c r="GK55" s="1"/>
-      <c r="GL55" s="1"/>
-      <c r="GM55" s="1"/>
-      <c r="GN55" s="1"/>
-      <c r="GO55" s="1"/>
-      <c r="GP55" s="1"/>
-      <c r="GQ55" s="1"/>
-      <c r="GR55" s="1"/>
-      <c r="GS55" s="1"/>
-      <c r="GT55" s="1"/>
-      <c r="GU55" s="1"/>
-      <c r="GV55" s="1"/>
-      <c r="GW55" s="1"/>
-      <c r="GX55" s="1"/>
-      <c r="GY55" s="1"/>
-      <c r="GZ55" s="1"/>
-      <c r="HA55" s="1"/>
-      <c r="HB55" s="1"/>
-      <c r="HC55" s="1"/>
-      <c r="HD55" s="1"/>
-      <c r="HE55" s="1"/>
-      <c r="HF55" s="1"/>
-      <c r="HG55" s="1"/>
-      <c r="HH55" s="1"/>
-      <c r="HI55" s="1"/>
-      <c r="HJ55" s="1"/>
-      <c r="HK55" s="1"/>
-      <c r="HL55" s="1"/>
-      <c r="HM55" s="1"/>
-      <c r="HN55" s="1"/>
-      <c r="HO55" s="1"/>
-      <c r="HP55" s="1"/>
-      <c r="HQ55" s="1"/>
-      <c r="HR55" s="1"/>
-      <c r="HS55" s="1"/>
-      <c r="HT55" s="1"/>
-      <c r="HU55" s="1"/>
-      <c r="HV55" s="1"/>
-      <c r="HW55" s="1"/>
-      <c r="HX55" s="1"/>
-      <c r="HY55" s="1"/>
-      <c r="HZ55" s="1"/>
-      <c r="IA55" s="1"/>
-      <c r="IB55" s="1"/>
-      <c r="IC55" s="1"/>
-      <c r="ID55" s="1"/>
-      <c r="IE55" s="1"/>
-      <c r="IF55" s="1"/>
-      <c r="IG55" s="1"/>
-      <c r="IH55" s="1"/>
-      <c r="II55" s="1"/>
-      <c r="IJ55" s="1"/>
-      <c r="IK55" s="1"/>
-      <c r="IL55" s="1"/>
-      <c r="IM55" s="1"/>
-      <c r="IN55" s="1"/>
-      <c r="IO55" s="1"/>
-      <c r="IP55" s="1"/>
-      <c r="IQ55" s="1"/>
-      <c r="IR55" s="1"/>
-      <c r="IS55" s="1"/>
-      <c r="IT55" s="1"/>
-      <c r="IU55" s="1"/>
-      <c r="IV55" s="1"/>
+      <c r="D55"/>
     </row>
     <row r="56" spans="1:256" ht="12" customHeight="1">
-      <c r="A56" s="31" t="s">
-        <v>142</v>
-      </c>
-      <c r="B56" s="31" t="s">
-        <v>143</v>
-      </c>
-      <c r="C56" s="31" t="s">
-        <v>144</v>
-      </c>
+      <c r="A56" s="15"/>
+      <c r="B56" s="16"/>
+      <c r="C56" s="16"/>
       <c r="D56" s="16"/>
       <c r="E56" s="12"/>
       <c r="F56" s="12"/>
@@ -14490,15 +14247,11 @@
       <c r="IV56" s="1"/>
     </row>
     <row r="57" spans="1:256" ht="12" customHeight="1">
-      <c r="A57" s="32" t="s">
-        <v>145</v>
-      </c>
-      <c r="B57" s="33" t="s">
-        <v>146</v>
-      </c>
-      <c r="C57" s="33" t="s">
-        <v>147</v>
-      </c>
+      <c r="A57" s="60" t="s">
+        <v>141</v>
+      </c>
+      <c r="B57" s="61"/>
+      <c r="C57" s="61"/>
       <c r="D57" s="16"/>
       <c r="E57" s="12"/>
       <c r="F57" s="12"/>
@@ -14754,14 +14507,14 @@
       <c r="IV57" s="1"/>
     </row>
     <row r="58" spans="1:256" ht="12" customHeight="1">
-      <c r="A58" s="32" t="s">
-        <v>148</v>
-      </c>
-      <c r="B58" s="33" t="s">
-        <v>149</v>
-      </c>
-      <c r="C58" s="33" t="s">
-        <v>150</v>
+      <c r="A58" s="31" t="s">
+        <v>142</v>
+      </c>
+      <c r="B58" s="31" t="s">
+        <v>143</v>
+      </c>
+      <c r="C58" s="31" t="s">
+        <v>144</v>
       </c>
       <c r="D58" s="16"/>
       <c r="E58" s="12"/>
@@ -15019,13 +14772,13 @@
     </row>
     <row r="59" spans="1:256" ht="12" customHeight="1">
       <c r="A59" s="32" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="B59" s="33" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="C59" s="33" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="D59" s="16"/>
       <c r="E59" s="12"/>
@@ -15283,13 +15036,13 @@
     </row>
     <row r="60" spans="1:256" ht="12" customHeight="1">
       <c r="A60" s="32" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="B60" s="33" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="C60" s="33" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="D60" s="16"/>
       <c r="E60" s="12"/>
@@ -15546,9 +15299,15 @@
       <c r="IV60" s="1"/>
     </row>
     <row r="61" spans="1:256" ht="12" customHeight="1">
-      <c r="A61" s="15"/>
-      <c r="B61" s="16"/>
-      <c r="C61" s="16"/>
+      <c r="A61" s="32" t="s">
+        <v>151</v>
+      </c>
+      <c r="B61" s="33" t="s">
+        <v>152</v>
+      </c>
+      <c r="C61" s="33" t="s">
+        <v>153</v>
+      </c>
       <c r="D61" s="16"/>
       <c r="E61" s="12"/>
       <c r="F61" s="12"/>
@@ -15804,11 +15563,15 @@
       <c r="IV61" s="1"/>
     </row>
     <row r="62" spans="1:256" ht="12" customHeight="1">
-      <c r="A62" s="59" t="s">
-        <v>66</v>
-      </c>
-      <c r="B62" s="59"/>
-      <c r="C62" s="14"/>
+      <c r="A62" s="32" t="s">
+        <v>154</v>
+      </c>
+      <c r="B62" s="33" t="s">
+        <v>155</v>
+      </c>
+      <c r="C62" s="33" t="s">
+        <v>156</v>
+      </c>
       <c r="D62" s="16"/>
       <c r="E62" s="12"/>
       <c r="F62" s="12"/>
@@ -16063,19 +15826,15 @@
       <c r="IU62" s="1"/>
       <c r="IV62" s="1"/>
     </row>
-    <row r="63" spans="1:256" ht="16.5" customHeight="1">
-      <c r="A63" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="B63" s="22" t="s">
-        <v>68</v>
-      </c>
-      <c r="C63" s="14"/>
-      <c r="D63" s="14"/>
-      <c r="E63" s="5"/>
-      <c r="F63" s="5"/>
-      <c r="G63" s="14"/>
-      <c r="H63" s="14"/>
+    <row r="63" spans="1:256" ht="12" customHeight="1">
+      <c r="A63" s="15"/>
+      <c r="B63" s="16"/>
+      <c r="C63" s="16"/>
+      <c r="D63" s="16"/>
+      <c r="E63" s="12"/>
+      <c r="F63" s="12"/>
+      <c r="G63" s="12"/>
+      <c r="H63" s="12"/>
       <c r="I63" s="5"/>
       <c r="J63" s="5"/>
       <c r="K63" s="5"/>
@@ -16086,20 +15845,256 @@
       <c r="P63" s="5"/>
       <c r="Q63" s="5"/>
       <c r="R63" s="5"/>
+      <c r="S63" s="1"/>
+      <c r="T63" s="1"/>
+      <c r="U63" s="1"/>
+      <c r="V63" s="1"/>
+      <c r="W63" s="1"/>
+      <c r="X63" s="1"/>
+      <c r="Y63" s="1"/>
+      <c r="Z63" s="1"/>
+      <c r="AA63" s="1"/>
+      <c r="AB63" s="1"/>
+      <c r="AC63" s="1"/>
+      <c r="AD63" s="1"/>
+      <c r="AE63" s="1"/>
+      <c r="AF63" s="1"/>
+      <c r="AG63" s="1"/>
+      <c r="AH63" s="1"/>
+      <c r="AI63" s="1"/>
+      <c r="AJ63" s="1"/>
+      <c r="AK63" s="1"/>
+      <c r="AL63" s="1"/>
+      <c r="AM63" s="1"/>
+      <c r="AN63" s="1"/>
+      <c r="AO63" s="1"/>
+      <c r="AP63" s="1"/>
+      <c r="AQ63" s="1"/>
+      <c r="AR63" s="1"/>
+      <c r="AS63" s="1"/>
+      <c r="AT63" s="1"/>
+      <c r="AU63" s="1"/>
+      <c r="AV63" s="1"/>
+      <c r="AW63" s="1"/>
+      <c r="AX63" s="1"/>
+      <c r="AY63" s="1"/>
+      <c r="AZ63" s="1"/>
+      <c r="BA63" s="1"/>
+      <c r="BB63" s="1"/>
+      <c r="BC63" s="1"/>
+      <c r="BD63" s="1"/>
+      <c r="BE63" s="1"/>
+      <c r="BF63" s="1"/>
+      <c r="BG63" s="1"/>
+      <c r="BH63" s="1"/>
+      <c r="BI63" s="1"/>
+      <c r="BJ63" s="1"/>
+      <c r="BK63" s="1"/>
+      <c r="BL63" s="1"/>
+      <c r="BM63" s="1"/>
+      <c r="BN63" s="1"/>
+      <c r="BO63" s="1"/>
+      <c r="BP63" s="1"/>
+      <c r="BQ63" s="1"/>
+      <c r="BR63" s="1"/>
+      <c r="BS63" s="1"/>
+      <c r="BT63" s="1"/>
+      <c r="BU63" s="1"/>
+      <c r="BV63" s="1"/>
+      <c r="BW63" s="1"/>
+      <c r="BX63" s="1"/>
+      <c r="BY63" s="1"/>
+      <c r="BZ63" s="1"/>
+      <c r="CA63" s="1"/>
+      <c r="CB63" s="1"/>
+      <c r="CC63" s="1"/>
+      <c r="CD63" s="1"/>
+      <c r="CE63" s="1"/>
+      <c r="CF63" s="1"/>
+      <c r="CG63" s="1"/>
+      <c r="CH63" s="1"/>
+      <c r="CI63" s="1"/>
+      <c r="CJ63" s="1"/>
+      <c r="CK63" s="1"/>
+      <c r="CL63" s="1"/>
+      <c r="CM63" s="1"/>
+      <c r="CN63" s="1"/>
+      <c r="CO63" s="1"/>
+      <c r="CP63" s="1"/>
+      <c r="CQ63" s="1"/>
+      <c r="CR63" s="1"/>
+      <c r="CS63" s="1"/>
+      <c r="CT63" s="1"/>
+      <c r="CU63" s="1"/>
+      <c r="CV63" s="1"/>
+      <c r="CW63" s="1"/>
+      <c r="CX63" s="1"/>
+      <c r="CY63" s="1"/>
+      <c r="CZ63" s="1"/>
+      <c r="DA63" s="1"/>
+      <c r="DB63" s="1"/>
+      <c r="DC63" s="1"/>
+      <c r="DD63" s="1"/>
+      <c r="DE63" s="1"/>
+      <c r="DF63" s="1"/>
+      <c r="DG63" s="1"/>
+      <c r="DH63" s="1"/>
+      <c r="DI63" s="1"/>
+      <c r="DJ63" s="1"/>
+      <c r="DK63" s="1"/>
+      <c r="DL63" s="1"/>
+      <c r="DM63" s="1"/>
+      <c r="DN63" s="1"/>
+      <c r="DO63" s="1"/>
+      <c r="DP63" s="1"/>
+      <c r="DQ63" s="1"/>
+      <c r="DR63" s="1"/>
+      <c r="DS63" s="1"/>
+      <c r="DT63" s="1"/>
+      <c r="DU63" s="1"/>
+      <c r="DV63" s="1"/>
+      <c r="DW63" s="1"/>
+      <c r="DX63" s="1"/>
+      <c r="DY63" s="1"/>
+      <c r="DZ63" s="1"/>
+      <c r="EA63" s="1"/>
+      <c r="EB63" s="1"/>
+      <c r="EC63" s="1"/>
+      <c r="ED63" s="1"/>
+      <c r="EE63" s="1"/>
+      <c r="EF63" s="1"/>
+      <c r="EG63" s="1"/>
+      <c r="EH63" s="1"/>
+      <c r="EI63" s="1"/>
+      <c r="EJ63" s="1"/>
+      <c r="EK63" s="1"/>
+      <c r="EL63" s="1"/>
+      <c r="EM63" s="1"/>
+      <c r="EN63" s="1"/>
+      <c r="EO63" s="1"/>
+      <c r="EP63" s="1"/>
+      <c r="EQ63" s="1"/>
+      <c r="ER63" s="1"/>
+      <c r="ES63" s="1"/>
+      <c r="ET63" s="1"/>
+      <c r="EU63" s="1"/>
+      <c r="EV63" s="1"/>
+      <c r="EW63" s="1"/>
+      <c r="EX63" s="1"/>
+      <c r="EY63" s="1"/>
+      <c r="EZ63" s="1"/>
+      <c r="FA63" s="1"/>
+      <c r="FB63" s="1"/>
+      <c r="FC63" s="1"/>
+      <c r="FD63" s="1"/>
+      <c r="FE63" s="1"/>
+      <c r="FF63" s="1"/>
+      <c r="FG63" s="1"/>
+      <c r="FH63" s="1"/>
+      <c r="FI63" s="1"/>
+      <c r="FJ63" s="1"/>
+      <c r="FK63" s="1"/>
+      <c r="FL63" s="1"/>
+      <c r="FM63" s="1"/>
+      <c r="FN63" s="1"/>
+      <c r="FO63" s="1"/>
+      <c r="FP63" s="1"/>
+      <c r="FQ63" s="1"/>
+      <c r="FR63" s="1"/>
+      <c r="FS63" s="1"/>
+      <c r="FT63" s="1"/>
+      <c r="FU63" s="1"/>
+      <c r="FV63" s="1"/>
+      <c r="FW63" s="1"/>
+      <c r="FX63" s="1"/>
+      <c r="FY63" s="1"/>
+      <c r="FZ63" s="1"/>
+      <c r="GA63" s="1"/>
+      <c r="GB63" s="1"/>
+      <c r="GC63" s="1"/>
+      <c r="GD63" s="1"/>
+      <c r="GE63" s="1"/>
+      <c r="GF63" s="1"/>
+      <c r="GG63" s="1"/>
+      <c r="GH63" s="1"/>
+      <c r="GI63" s="1"/>
+      <c r="GJ63" s="1"/>
+      <c r="GK63" s="1"/>
+      <c r="GL63" s="1"/>
+      <c r="GM63" s="1"/>
+      <c r="GN63" s="1"/>
+      <c r="GO63" s="1"/>
+      <c r="GP63" s="1"/>
+      <c r="GQ63" s="1"/>
+      <c r="GR63" s="1"/>
+      <c r="GS63" s="1"/>
+      <c r="GT63" s="1"/>
+      <c r="GU63" s="1"/>
+      <c r="GV63" s="1"/>
+      <c r="GW63" s="1"/>
+      <c r="GX63" s="1"/>
+      <c r="GY63" s="1"/>
+      <c r="GZ63" s="1"/>
+      <c r="HA63" s="1"/>
+      <c r="HB63" s="1"/>
+      <c r="HC63" s="1"/>
+      <c r="HD63" s="1"/>
+      <c r="HE63" s="1"/>
+      <c r="HF63" s="1"/>
+      <c r="HG63" s="1"/>
+      <c r="HH63" s="1"/>
+      <c r="HI63" s="1"/>
+      <c r="HJ63" s="1"/>
+      <c r="HK63" s="1"/>
+      <c r="HL63" s="1"/>
+      <c r="HM63" s="1"/>
+      <c r="HN63" s="1"/>
+      <c r="HO63" s="1"/>
+      <c r="HP63" s="1"/>
+      <c r="HQ63" s="1"/>
+      <c r="HR63" s="1"/>
+      <c r="HS63" s="1"/>
+      <c r="HT63" s="1"/>
+      <c r="HU63" s="1"/>
+      <c r="HV63" s="1"/>
+      <c r="HW63" s="1"/>
+      <c r="HX63" s="1"/>
+      <c r="HY63" s="1"/>
+      <c r="HZ63" s="1"/>
+      <c r="IA63" s="1"/>
+      <c r="IB63" s="1"/>
+      <c r="IC63" s="1"/>
+      <c r="ID63" s="1"/>
+      <c r="IE63" s="1"/>
+      <c r="IF63" s="1"/>
+      <c r="IG63" s="1"/>
+      <c r="IH63" s="1"/>
+      <c r="II63" s="1"/>
+      <c r="IJ63" s="1"/>
+      <c r="IK63" s="1"/>
+      <c r="IL63" s="1"/>
+      <c r="IM63" s="1"/>
+      <c r="IN63" s="1"/>
+      <c r="IO63" s="1"/>
+      <c r="IP63" s="1"/>
+      <c r="IQ63" s="1"/>
+      <c r="IR63" s="1"/>
+      <c r="IS63" s="1"/>
+      <c r="IT63" s="1"/>
+      <c r="IU63" s="1"/>
+      <c r="IV63" s="1"/>
     </row>
     <row r="64" spans="1:256" ht="12" customHeight="1">
-      <c r="A64" s="23" t="s">
-        <v>69</v>
-      </c>
-      <c r="B64" s="20" t="s">
-        <v>70</v>
-      </c>
-      <c r="C64" s="5"/>
-      <c r="D64" s="14"/>
-      <c r="E64" s="5"/>
-      <c r="F64" s="5"/>
-      <c r="G64" s="14"/>
-      <c r="H64" s="14"/>
+      <c r="A64" s="59" t="s">
+        <v>66</v>
+      </c>
+      <c r="B64" s="59"/>
+      <c r="C64" s="14"/>
+      <c r="D64" s="16"/>
+      <c r="E64" s="12"/>
+      <c r="F64" s="12"/>
+      <c r="G64" s="12"/>
+      <c r="H64" s="12"/>
       <c r="I64" s="5"/>
       <c r="J64" s="5"/>
       <c r="K64" s="5"/>
@@ -16349,15 +16344,19 @@
       <c r="IU64" s="1"/>
       <c r="IV64" s="1"/>
     </row>
-    <row r="65" spans="1:256" ht="15.95" customHeight="1">
-      <c r="A65" s="1"/>
-      <c r="B65" s="1"/>
-      <c r="C65" s="5"/>
-      <c r="D65" s="5"/>
+    <row r="65" spans="1:256" ht="16.5" customHeight="1">
+      <c r="A65" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="B65" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="C65" s="14"/>
+      <c r="D65" s="14"/>
       <c r="E65" s="5"/>
       <c r="F65" s="5"/>
-      <c r="G65" s="5"/>
-      <c r="H65" s="5"/>
+      <c r="G65" s="14"/>
+      <c r="H65" s="14"/>
       <c r="I65" s="5"/>
       <c r="J65" s="5"/>
       <c r="K65" s="5"/>
@@ -16368,254 +16367,20 @@
       <c r="P65" s="5"/>
       <c r="Q65" s="5"/>
       <c r="R65" s="5"/>
-      <c r="S65" s="1"/>
-      <c r="T65" s="1"/>
-      <c r="U65" s="1"/>
-      <c r="V65" s="1"/>
-      <c r="W65" s="1"/>
-      <c r="X65" s="1"/>
-      <c r="Y65" s="1"/>
-      <c r="Z65" s="1"/>
-      <c r="AA65" s="1"/>
-      <c r="AB65" s="1"/>
-      <c r="AC65" s="1"/>
-      <c r="AD65" s="1"/>
-      <c r="AE65" s="1"/>
-      <c r="AF65" s="1"/>
-      <c r="AG65" s="1"/>
-      <c r="AH65" s="1"/>
-      <c r="AI65" s="1"/>
-      <c r="AJ65" s="1"/>
-      <c r="AK65" s="1"/>
-      <c r="AL65" s="1"/>
-      <c r="AM65" s="1"/>
-      <c r="AN65" s="1"/>
-      <c r="AO65" s="1"/>
-      <c r="AP65" s="1"/>
-      <c r="AQ65" s="1"/>
-      <c r="AR65" s="1"/>
-      <c r="AS65" s="1"/>
-      <c r="AT65" s="1"/>
-      <c r="AU65" s="1"/>
-      <c r="AV65" s="1"/>
-      <c r="AW65" s="1"/>
-      <c r="AX65" s="1"/>
-      <c r="AY65" s="1"/>
-      <c r="AZ65" s="1"/>
-      <c r="BA65" s="1"/>
-      <c r="BB65" s="1"/>
-      <c r="BC65" s="1"/>
-      <c r="BD65" s="1"/>
-      <c r="BE65" s="1"/>
-      <c r="BF65" s="1"/>
-      <c r="BG65" s="1"/>
-      <c r="BH65" s="1"/>
-      <c r="BI65" s="1"/>
-      <c r="BJ65" s="1"/>
-      <c r="BK65" s="1"/>
-      <c r="BL65" s="1"/>
-      <c r="BM65" s="1"/>
-      <c r="BN65" s="1"/>
-      <c r="BO65" s="1"/>
-      <c r="BP65" s="1"/>
-      <c r="BQ65" s="1"/>
-      <c r="BR65" s="1"/>
-      <c r="BS65" s="1"/>
-      <c r="BT65" s="1"/>
-      <c r="BU65" s="1"/>
-      <c r="BV65" s="1"/>
-      <c r="BW65" s="1"/>
-      <c r="BX65" s="1"/>
-      <c r="BY65" s="1"/>
-      <c r="BZ65" s="1"/>
-      <c r="CA65" s="1"/>
-      <c r="CB65" s="1"/>
-      <c r="CC65" s="1"/>
-      <c r="CD65" s="1"/>
-      <c r="CE65" s="1"/>
-      <c r="CF65" s="1"/>
-      <c r="CG65" s="1"/>
-      <c r="CH65" s="1"/>
-      <c r="CI65" s="1"/>
-      <c r="CJ65" s="1"/>
-      <c r="CK65" s="1"/>
-      <c r="CL65" s="1"/>
-      <c r="CM65" s="1"/>
-      <c r="CN65" s="1"/>
-      <c r="CO65" s="1"/>
-      <c r="CP65" s="1"/>
-      <c r="CQ65" s="1"/>
-      <c r="CR65" s="1"/>
-      <c r="CS65" s="1"/>
-      <c r="CT65" s="1"/>
-      <c r="CU65" s="1"/>
-      <c r="CV65" s="1"/>
-      <c r="CW65" s="1"/>
-      <c r="CX65" s="1"/>
-      <c r="CY65" s="1"/>
-      <c r="CZ65" s="1"/>
-      <c r="DA65" s="1"/>
-      <c r="DB65" s="1"/>
-      <c r="DC65" s="1"/>
-      <c r="DD65" s="1"/>
-      <c r="DE65" s="1"/>
-      <c r="DF65" s="1"/>
-      <c r="DG65" s="1"/>
-      <c r="DH65" s="1"/>
-      <c r="DI65" s="1"/>
-      <c r="DJ65" s="1"/>
-      <c r="DK65" s="1"/>
-      <c r="DL65" s="1"/>
-      <c r="DM65" s="1"/>
-      <c r="DN65" s="1"/>
-      <c r="DO65" s="1"/>
-      <c r="DP65" s="1"/>
-      <c r="DQ65" s="1"/>
-      <c r="DR65" s="1"/>
-      <c r="DS65" s="1"/>
-      <c r="DT65" s="1"/>
-      <c r="DU65" s="1"/>
-      <c r="DV65" s="1"/>
-      <c r="DW65" s="1"/>
-      <c r="DX65" s="1"/>
-      <c r="DY65" s="1"/>
-      <c r="DZ65" s="1"/>
-      <c r="EA65" s="1"/>
-      <c r="EB65" s="1"/>
-      <c r="EC65" s="1"/>
-      <c r="ED65" s="1"/>
-      <c r="EE65" s="1"/>
-      <c r="EF65" s="1"/>
-      <c r="EG65" s="1"/>
-      <c r="EH65" s="1"/>
-      <c r="EI65" s="1"/>
-      <c r="EJ65" s="1"/>
-      <c r="EK65" s="1"/>
-      <c r="EL65" s="1"/>
-      <c r="EM65" s="1"/>
-      <c r="EN65" s="1"/>
-      <c r="EO65" s="1"/>
-      <c r="EP65" s="1"/>
-      <c r="EQ65" s="1"/>
-      <c r="ER65" s="1"/>
-      <c r="ES65" s="1"/>
-      <c r="ET65" s="1"/>
-      <c r="EU65" s="1"/>
-      <c r="EV65" s="1"/>
-      <c r="EW65" s="1"/>
-      <c r="EX65" s="1"/>
-      <c r="EY65" s="1"/>
-      <c r="EZ65" s="1"/>
-      <c r="FA65" s="1"/>
-      <c r="FB65" s="1"/>
-      <c r="FC65" s="1"/>
-      <c r="FD65" s="1"/>
-      <c r="FE65" s="1"/>
-      <c r="FF65" s="1"/>
-      <c r="FG65" s="1"/>
-      <c r="FH65" s="1"/>
-      <c r="FI65" s="1"/>
-      <c r="FJ65" s="1"/>
-      <c r="FK65" s="1"/>
-      <c r="FL65" s="1"/>
-      <c r="FM65" s="1"/>
-      <c r="FN65" s="1"/>
-      <c r="FO65" s="1"/>
-      <c r="FP65" s="1"/>
-      <c r="FQ65" s="1"/>
-      <c r="FR65" s="1"/>
-      <c r="FS65" s="1"/>
-      <c r="FT65" s="1"/>
-      <c r="FU65" s="1"/>
-      <c r="FV65" s="1"/>
-      <c r="FW65" s="1"/>
-      <c r="FX65" s="1"/>
-      <c r="FY65" s="1"/>
-      <c r="FZ65" s="1"/>
-      <c r="GA65" s="1"/>
-      <c r="GB65" s="1"/>
-      <c r="GC65" s="1"/>
-      <c r="GD65" s="1"/>
-      <c r="GE65" s="1"/>
-      <c r="GF65" s="1"/>
-      <c r="GG65" s="1"/>
-      <c r="GH65" s="1"/>
-      <c r="GI65" s="1"/>
-      <c r="GJ65" s="1"/>
-      <c r="GK65" s="1"/>
-      <c r="GL65" s="1"/>
-      <c r="GM65" s="1"/>
-      <c r="GN65" s="1"/>
-      <c r="GO65" s="1"/>
-      <c r="GP65" s="1"/>
-      <c r="GQ65" s="1"/>
-      <c r="GR65" s="1"/>
-      <c r="GS65" s="1"/>
-      <c r="GT65" s="1"/>
-      <c r="GU65" s="1"/>
-      <c r="GV65" s="1"/>
-      <c r="GW65" s="1"/>
-      <c r="GX65" s="1"/>
-      <c r="GY65" s="1"/>
-      <c r="GZ65" s="1"/>
-      <c r="HA65" s="1"/>
-      <c r="HB65" s="1"/>
-      <c r="HC65" s="1"/>
-      <c r="HD65" s="1"/>
-      <c r="HE65" s="1"/>
-      <c r="HF65" s="1"/>
-      <c r="HG65" s="1"/>
-      <c r="HH65" s="1"/>
-      <c r="HI65" s="1"/>
-      <c r="HJ65" s="1"/>
-      <c r="HK65" s="1"/>
-      <c r="HL65" s="1"/>
-      <c r="HM65" s="1"/>
-      <c r="HN65" s="1"/>
-      <c r="HO65" s="1"/>
-      <c r="HP65" s="1"/>
-      <c r="HQ65" s="1"/>
-      <c r="HR65" s="1"/>
-      <c r="HS65" s="1"/>
-      <c r="HT65" s="1"/>
-      <c r="HU65" s="1"/>
-      <c r="HV65" s="1"/>
-      <c r="HW65" s="1"/>
-      <c r="HX65" s="1"/>
-      <c r="HY65" s="1"/>
-      <c r="HZ65" s="1"/>
-      <c r="IA65" s="1"/>
-      <c r="IB65" s="1"/>
-      <c r="IC65" s="1"/>
-      <c r="ID65" s="1"/>
-      <c r="IE65" s="1"/>
-      <c r="IF65" s="1"/>
-      <c r="IG65" s="1"/>
-      <c r="IH65" s="1"/>
-      <c r="II65" s="1"/>
-      <c r="IJ65" s="1"/>
-      <c r="IK65" s="1"/>
-      <c r="IL65" s="1"/>
-      <c r="IM65" s="1"/>
-      <c r="IN65" s="1"/>
-      <c r="IO65" s="1"/>
-      <c r="IP65" s="1"/>
-      <c r="IQ65" s="1"/>
-      <c r="IR65" s="1"/>
-      <c r="IS65" s="1"/>
-      <c r="IT65" s="1"/>
-      <c r="IU65" s="1"/>
-      <c r="IV65" s="1"/>
     </row>
-    <row r="66" spans="1:256" ht="15.95" customHeight="1">
-      <c r="A66" s="1"/>
-      <c r="B66" s="1"/>
+    <row r="66" spans="1:256" ht="12" customHeight="1">
+      <c r="A66" s="23" t="s">
+        <v>69</v>
+      </c>
+      <c r="B66" s="20" t="s">
+        <v>70</v>
+      </c>
       <c r="C66" s="5"/>
-      <c r="D66" s="5"/>
+      <c r="D66" s="14"/>
       <c r="E66" s="5"/>
       <c r="F66" s="5"/>
-      <c r="G66" s="5"/>
-      <c r="H66" s="5"/>
+      <c r="G66" s="14"/>
+      <c r="H66" s="14"/>
       <c r="I66" s="5"/>
       <c r="J66" s="5"/>
       <c r="K66" s="5"/>
@@ -16878,12 +16643,12 @@
       <c r="J67" s="5"/>
       <c r="K67" s="5"/>
       <c r="L67" s="5"/>
-      <c r="M67" s="1"/>
-      <c r="N67" s="1"/>
-      <c r="O67" s="1"/>
-      <c r="P67" s="1"/>
-      <c r="Q67" s="1"/>
-      <c r="R67" s="1"/>
+      <c r="M67" s="5"/>
+      <c r="N67" s="5"/>
+      <c r="O67" s="5"/>
+      <c r="P67" s="5"/>
+      <c r="Q67" s="5"/>
+      <c r="R67" s="5"/>
       <c r="S67" s="1"/>
       <c r="T67" s="1"/>
       <c r="U67" s="1"/>
@@ -17136,12 +16901,12 @@
       <c r="J68" s="5"/>
       <c r="K68" s="5"/>
       <c r="L68" s="5"/>
-      <c r="M68" s="1"/>
-      <c r="N68" s="1"/>
-      <c r="O68" s="1"/>
-      <c r="P68" s="1"/>
-      <c r="Q68" s="1"/>
-      <c r="R68" s="1"/>
+      <c r="M68" s="5"/>
+      <c r="N68" s="5"/>
+      <c r="O68" s="5"/>
+      <c r="P68" s="5"/>
+      <c r="Q68" s="5"/>
+      <c r="R68" s="5"/>
       <c r="S68" s="1"/>
       <c r="T68" s="1"/>
       <c r="U68" s="1"/>
@@ -17381,7 +17146,7 @@
       <c r="IU68" s="1"/>
       <c r="IV68" s="1"/>
     </row>
-    <row r="69" spans="1:256">
+    <row r="69" spans="1:256" ht="15.95" customHeight="1">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
       <c r="C69" s="5"/>
@@ -17639,7 +17404,7 @@
       <c r="IU69" s="1"/>
       <c r="IV69" s="1"/>
     </row>
-    <row r="70" spans="1:256" ht="15.75" customHeight="1">
+    <row r="70" spans="1:256" ht="15.95" customHeight="1">
       <c r="A70" s="1"/>
       <c r="B70" s="1"/>
       <c r="C70" s="5"/>
@@ -17897,10 +17662,10 @@
       <c r="IU70" s="1"/>
       <c r="IV70" s="1"/>
     </row>
-    <row r="71" spans="1:256" ht="15.75" customHeight="1">
+    <row r="71" spans="1:256">
       <c r="A71" s="1"/>
       <c r="B71" s="1"/>
-      <c r="C71" s="1"/>
+      <c r="C71" s="5"/>
       <c r="D71" s="5"/>
       <c r="E71" s="5"/>
       <c r="F71" s="5"/>
@@ -18155,26 +17920,25 @@
       <c r="IU71" s="1"/>
       <c r="IV71" s="1"/>
     </row>
-    <row r="72" spans="1:256" ht="12" customHeight="1">
-      <c r="A72" s="59" t="s">
-        <v>190</v>
-      </c>
-      <c r="B72" s="59"/>
-      <c r="C72" s="1"/>
-      <c r="E72" s="1"/>
-      <c r="F72" s="1"/>
-      <c r="G72" s="1"/>
-      <c r="H72" s="1"/>
+    <row r="72" spans="1:256" ht="15.75" customHeight="1">
+      <c r="A72" s="1"/>
+      <c r="B72" s="1"/>
+      <c r="C72" s="5"/>
+      <c r="D72" s="5"/>
+      <c r="E72" s="5"/>
+      <c r="F72" s="5"/>
+      <c r="G72" s="5"/>
+      <c r="H72" s="5"/>
       <c r="I72" s="5"/>
       <c r="J72" s="5"/>
       <c r="K72" s="5"/>
       <c r="L72" s="5"/>
-      <c r="M72" s="5"/>
-      <c r="N72" s="5"/>
-      <c r="O72" s="5"/>
-      <c r="P72" s="5"/>
-      <c r="Q72" s="5"/>
-      <c r="R72" s="5"/>
+      <c r="M72" s="1"/>
+      <c r="N72" s="1"/>
+      <c r="O72" s="1"/>
+      <c r="P72" s="1"/>
+      <c r="Q72" s="1"/>
+      <c r="R72" s="1"/>
       <c r="S72" s="1"/>
       <c r="T72" s="1"/>
       <c r="U72" s="1"/>
@@ -18415,14 +18179,11 @@
       <c r="IV72" s="1"/>
     </row>
     <row r="73" spans="1:256" ht="15.75" customHeight="1">
-      <c r="A73" s="21" t="s">
-        <v>191</v>
-      </c>
-      <c r="B73" s="22" t="s">
-        <v>192</v>
-      </c>
+      <c r="A73" s="1"/>
+      <c r="B73" s="1"/>
       <c r="C73" s="1"/>
-      <c r="E73" s="1"/>
+      <c r="D73" s="5"/>
+      <c r="E73" s="5"/>
       <c r="F73" s="5"/>
       <c r="G73" s="5"/>
       <c r="H73" s="5"/>
@@ -18430,9 +18191,9 @@
       <c r="J73" s="5"/>
       <c r="K73" s="5"/>
       <c r="L73" s="5"/>
-      <c r="M73" s="5"/>
-      <c r="N73" s="5"/>
-      <c r="O73" s="5"/>
+      <c r="M73" s="1"/>
+      <c r="N73" s="1"/>
+      <c r="O73" s="1"/>
       <c r="P73" s="1"/>
       <c r="Q73" s="1"/>
       <c r="R73" s="1"/>
@@ -18675,18 +18436,16 @@
       <c r="IU73" s="1"/>
       <c r="IV73" s="1"/>
     </row>
-    <row r="74" spans="1:256" ht="15.75" customHeight="1">
-      <c r="A74" s="23" t="s">
-        <v>193</v>
-      </c>
-      <c r="B74" s="23" t="s">
-        <v>194</v>
-      </c>
+    <row r="74" spans="1:256" ht="12" customHeight="1">
+      <c r="A74" s="59" t="s">
+        <v>190</v>
+      </c>
+      <c r="B74" s="59"/>
       <c r="C74" s="1"/>
       <c r="E74" s="1"/>
-      <c r="F74" s="5"/>
-      <c r="G74" s="5"/>
-      <c r="H74" s="5"/>
+      <c r="F74" s="1"/>
+      <c r="G74" s="1"/>
+      <c r="H74" s="1"/>
       <c r="I74" s="5"/>
       <c r="J74" s="5"/>
       <c r="K74" s="5"/>
@@ -18694,9 +18453,9 @@
       <c r="M74" s="5"/>
       <c r="N74" s="5"/>
       <c r="O74" s="5"/>
-      <c r="P74" s="1"/>
-      <c r="Q74" s="1"/>
-      <c r="R74" s="1"/>
+      <c r="P74" s="5"/>
+      <c r="Q74" s="5"/>
+      <c r="R74" s="5"/>
       <c r="S74" s="1"/>
       <c r="T74" s="1"/>
       <c r="U74" s="1"/>
@@ -18937,8 +18696,12 @@
       <c r="IV74" s="1"/>
     </row>
     <row r="75" spans="1:256" ht="15.75" customHeight="1">
-      <c r="A75" s="1"/>
-      <c r="B75" s="1"/>
+      <c r="A75" s="21" t="s">
+        <v>191</v>
+      </c>
+      <c r="B75" s="22" t="s">
+        <v>192</v>
+      </c>
       <c r="C75" s="1"/>
       <c r="E75" s="1"/>
       <c r="F75" s="5"/>
@@ -19194,10 +18957,17 @@
       <c r="IV75" s="1"/>
     </row>
     <row r="76" spans="1:256" ht="15.75" customHeight="1">
+      <c r="A76" s="23" t="s">
+        <v>193</v>
+      </c>
+      <c r="B76" s="23" t="s">
+        <v>194</v>
+      </c>
+      <c r="C76" s="1"/>
       <c r="E76" s="1"/>
-      <c r="F76" s="1"/>
-      <c r="G76" s="1"/>
-      <c r="H76" s="1"/>
+      <c r="F76" s="5"/>
+      <c r="G76" s="5"/>
+      <c r="H76" s="5"/>
       <c r="I76" s="5"/>
       <c r="J76" s="5"/>
       <c r="K76" s="5"/>
@@ -19205,9 +18975,9 @@
       <c r="M76" s="5"/>
       <c r="N76" s="5"/>
       <c r="O76" s="5"/>
-      <c r="P76" s="5"/>
-      <c r="Q76" s="5"/>
-      <c r="R76" s="5"/>
+      <c r="P76" s="1"/>
+      <c r="Q76" s="1"/>
+      <c r="R76" s="1"/>
       <c r="S76" s="1"/>
       <c r="T76" s="1"/>
       <c r="U76" s="1"/>
@@ -19447,7 +19217,14 @@
       <c r="IU76" s="1"/>
       <c r="IV76" s="1"/>
     </row>
-    <row r="77" spans="1:256" ht="12" customHeight="1">
+    <row r="77" spans="1:256" ht="15.75" customHeight="1">
+      <c r="A77" s="1"/>
+      <c r="B77" s="1"/>
+      <c r="C77" s="1"/>
+      <c r="E77" s="1"/>
+      <c r="F77" s="5"/>
+      <c r="G77" s="5"/>
+      <c r="H77" s="5"/>
       <c r="I77" s="5"/>
       <c r="J77" s="5"/>
       <c r="K77" s="5"/>
@@ -19455,12 +19232,514 @@
       <c r="M77" s="5"/>
       <c r="N77" s="5"/>
       <c r="O77" s="5"/>
-      <c r="P77" s="5"/>
-      <c r="Q77" s="5"/>
-      <c r="R77" s="5"/>
+      <c r="P77" s="1"/>
+      <c r="Q77" s="1"/>
+      <c r="R77" s="1"/>
+      <c r="S77" s="1"/>
+      <c r="T77" s="1"/>
+      <c r="U77" s="1"/>
+      <c r="V77" s="1"/>
+      <c r="W77" s="1"/>
+      <c r="X77" s="1"/>
+      <c r="Y77" s="1"/>
+      <c r="Z77" s="1"/>
+      <c r="AA77" s="1"/>
+      <c r="AB77" s="1"/>
+      <c r="AC77" s="1"/>
+      <c r="AD77" s="1"/>
+      <c r="AE77" s="1"/>
+      <c r="AF77" s="1"/>
+      <c r="AG77" s="1"/>
+      <c r="AH77" s="1"/>
+      <c r="AI77" s="1"/>
+      <c r="AJ77" s="1"/>
+      <c r="AK77" s="1"/>
+      <c r="AL77" s="1"/>
+      <c r="AM77" s="1"/>
+      <c r="AN77" s="1"/>
+      <c r="AO77" s="1"/>
+      <c r="AP77" s="1"/>
+      <c r="AQ77" s="1"/>
+      <c r="AR77" s="1"/>
+      <c r="AS77" s="1"/>
+      <c r="AT77" s="1"/>
+      <c r="AU77" s="1"/>
+      <c r="AV77" s="1"/>
+      <c r="AW77" s="1"/>
+      <c r="AX77" s="1"/>
+      <c r="AY77" s="1"/>
+      <c r="AZ77" s="1"/>
+      <c r="BA77" s="1"/>
+      <c r="BB77" s="1"/>
+      <c r="BC77" s="1"/>
+      <c r="BD77" s="1"/>
+      <c r="BE77" s="1"/>
+      <c r="BF77" s="1"/>
+      <c r="BG77" s="1"/>
+      <c r="BH77" s="1"/>
+      <c r="BI77" s="1"/>
+      <c r="BJ77" s="1"/>
+      <c r="BK77" s="1"/>
+      <c r="BL77" s="1"/>
+      <c r="BM77" s="1"/>
+      <c r="BN77" s="1"/>
+      <c r="BO77" s="1"/>
+      <c r="BP77" s="1"/>
+      <c r="BQ77" s="1"/>
+      <c r="BR77" s="1"/>
+      <c r="BS77" s="1"/>
+      <c r="BT77" s="1"/>
+      <c r="BU77" s="1"/>
+      <c r="BV77" s="1"/>
+      <c r="BW77" s="1"/>
+      <c r="BX77" s="1"/>
+      <c r="BY77" s="1"/>
+      <c r="BZ77" s="1"/>
+      <c r="CA77" s="1"/>
+      <c r="CB77" s="1"/>
+      <c r="CC77" s="1"/>
+      <c r="CD77" s="1"/>
+      <c r="CE77" s="1"/>
+      <c r="CF77" s="1"/>
+      <c r="CG77" s="1"/>
+      <c r="CH77" s="1"/>
+      <c r="CI77" s="1"/>
+      <c r="CJ77" s="1"/>
+      <c r="CK77" s="1"/>
+      <c r="CL77" s="1"/>
+      <c r="CM77" s="1"/>
+      <c r="CN77" s="1"/>
+      <c r="CO77" s="1"/>
+      <c r="CP77" s="1"/>
+      <c r="CQ77" s="1"/>
+      <c r="CR77" s="1"/>
+      <c r="CS77" s="1"/>
+      <c r="CT77" s="1"/>
+      <c r="CU77" s="1"/>
+      <c r="CV77" s="1"/>
+      <c r="CW77" s="1"/>
+      <c r="CX77" s="1"/>
+      <c r="CY77" s="1"/>
+      <c r="CZ77" s="1"/>
+      <c r="DA77" s="1"/>
+      <c r="DB77" s="1"/>
+      <c r="DC77" s="1"/>
+      <c r="DD77" s="1"/>
+      <c r="DE77" s="1"/>
+      <c r="DF77" s="1"/>
+      <c r="DG77" s="1"/>
+      <c r="DH77" s="1"/>
+      <c r="DI77" s="1"/>
+      <c r="DJ77" s="1"/>
+      <c r="DK77" s="1"/>
+      <c r="DL77" s="1"/>
+      <c r="DM77" s="1"/>
+      <c r="DN77" s="1"/>
+      <c r="DO77" s="1"/>
+      <c r="DP77" s="1"/>
+      <c r="DQ77" s="1"/>
+      <c r="DR77" s="1"/>
+      <c r="DS77" s="1"/>
+      <c r="DT77" s="1"/>
+      <c r="DU77" s="1"/>
+      <c r="DV77" s="1"/>
+      <c r="DW77" s="1"/>
+      <c r="DX77" s="1"/>
+      <c r="DY77" s="1"/>
+      <c r="DZ77" s="1"/>
+      <c r="EA77" s="1"/>
+      <c r="EB77" s="1"/>
+      <c r="EC77" s="1"/>
+      <c r="ED77" s="1"/>
+      <c r="EE77" s="1"/>
+      <c r="EF77" s="1"/>
+      <c r="EG77" s="1"/>
+      <c r="EH77" s="1"/>
+      <c r="EI77" s="1"/>
+      <c r="EJ77" s="1"/>
+      <c r="EK77" s="1"/>
+      <c r="EL77" s="1"/>
+      <c r="EM77" s="1"/>
+      <c r="EN77" s="1"/>
+      <c r="EO77" s="1"/>
+      <c r="EP77" s="1"/>
+      <c r="EQ77" s="1"/>
+      <c r="ER77" s="1"/>
+      <c r="ES77" s="1"/>
+      <c r="ET77" s="1"/>
+      <c r="EU77" s="1"/>
+      <c r="EV77" s="1"/>
+      <c r="EW77" s="1"/>
+      <c r="EX77" s="1"/>
+      <c r="EY77" s="1"/>
+      <c r="EZ77" s="1"/>
+      <c r="FA77" s="1"/>
+      <c r="FB77" s="1"/>
+      <c r="FC77" s="1"/>
+      <c r="FD77" s="1"/>
+      <c r="FE77" s="1"/>
+      <c r="FF77" s="1"/>
+      <c r="FG77" s="1"/>
+      <c r="FH77" s="1"/>
+      <c r="FI77" s="1"/>
+      <c r="FJ77" s="1"/>
+      <c r="FK77" s="1"/>
+      <c r="FL77" s="1"/>
+      <c r="FM77" s="1"/>
+      <c r="FN77" s="1"/>
+      <c r="FO77" s="1"/>
+      <c r="FP77" s="1"/>
+      <c r="FQ77" s="1"/>
+      <c r="FR77" s="1"/>
+      <c r="FS77" s="1"/>
+      <c r="FT77" s="1"/>
+      <c r="FU77" s="1"/>
+      <c r="FV77" s="1"/>
+      <c r="FW77" s="1"/>
+      <c r="FX77" s="1"/>
+      <c r="FY77" s="1"/>
+      <c r="FZ77" s="1"/>
+      <c r="GA77" s="1"/>
+      <c r="GB77" s="1"/>
+      <c r="GC77" s="1"/>
+      <c r="GD77" s="1"/>
+      <c r="GE77" s="1"/>
+      <c r="GF77" s="1"/>
+      <c r="GG77" s="1"/>
+      <c r="GH77" s="1"/>
+      <c r="GI77" s="1"/>
+      <c r="GJ77" s="1"/>
+      <c r="GK77" s="1"/>
+      <c r="GL77" s="1"/>
+      <c r="GM77" s="1"/>
+      <c r="GN77" s="1"/>
+      <c r="GO77" s="1"/>
+      <c r="GP77" s="1"/>
+      <c r="GQ77" s="1"/>
+      <c r="GR77" s="1"/>
+      <c r="GS77" s="1"/>
+      <c r="GT77" s="1"/>
+      <c r="GU77" s="1"/>
+      <c r="GV77" s="1"/>
+      <c r="GW77" s="1"/>
+      <c r="GX77" s="1"/>
+      <c r="GY77" s="1"/>
+      <c r="GZ77" s="1"/>
+      <c r="HA77" s="1"/>
+      <c r="HB77" s="1"/>
+      <c r="HC77" s="1"/>
+      <c r="HD77" s="1"/>
+      <c r="HE77" s="1"/>
+      <c r="HF77" s="1"/>
+      <c r="HG77" s="1"/>
+      <c r="HH77" s="1"/>
+      <c r="HI77" s="1"/>
+      <c r="HJ77" s="1"/>
+      <c r="HK77" s="1"/>
+      <c r="HL77" s="1"/>
+      <c r="HM77" s="1"/>
+      <c r="HN77" s="1"/>
+      <c r="HO77" s="1"/>
+      <c r="HP77" s="1"/>
+      <c r="HQ77" s="1"/>
+      <c r="HR77" s="1"/>
+      <c r="HS77" s="1"/>
+      <c r="HT77" s="1"/>
+      <c r="HU77" s="1"/>
+      <c r="HV77" s="1"/>
+      <c r="HW77" s="1"/>
+      <c r="HX77" s="1"/>
+      <c r="HY77" s="1"/>
+      <c r="HZ77" s="1"/>
+      <c r="IA77" s="1"/>
+      <c r="IB77" s="1"/>
+      <c r="IC77" s="1"/>
+      <c r="ID77" s="1"/>
+      <c r="IE77" s="1"/>
+      <c r="IF77" s="1"/>
+      <c r="IG77" s="1"/>
+      <c r="IH77" s="1"/>
+      <c r="II77" s="1"/>
+      <c r="IJ77" s="1"/>
+      <c r="IK77" s="1"/>
+      <c r="IL77" s="1"/>
+      <c r="IM77" s="1"/>
+      <c r="IN77" s="1"/>
+      <c r="IO77" s="1"/>
+      <c r="IP77" s="1"/>
+      <c r="IQ77" s="1"/>
+      <c r="IR77" s="1"/>
+      <c r="IS77" s="1"/>
+      <c r="IT77" s="1"/>
+      <c r="IU77" s="1"/>
+      <c r="IV77" s="1"/>
     </row>
-    <row r="78" spans="1:256" ht="15.95" customHeight="1"/>
-    <row r="79" spans="1:256" ht="15.95" customHeight="1"/>
+    <row r="78" spans="1:256" ht="15.75" customHeight="1">
+      <c r="E78" s="1"/>
+      <c r="F78" s="1"/>
+      <c r="G78" s="1"/>
+      <c r="H78" s="1"/>
+      <c r="I78" s="5"/>
+      <c r="J78" s="5"/>
+      <c r="K78" s="5"/>
+      <c r="L78" s="5"/>
+      <c r="M78" s="5"/>
+      <c r="N78" s="5"/>
+      <c r="O78" s="5"/>
+      <c r="P78" s="5"/>
+      <c r="Q78" s="5"/>
+      <c r="R78" s="5"/>
+      <c r="S78" s="1"/>
+      <c r="T78" s="1"/>
+      <c r="U78" s="1"/>
+      <c r="V78" s="1"/>
+      <c r="W78" s="1"/>
+      <c r="X78" s="1"/>
+      <c r="Y78" s="1"/>
+      <c r="Z78" s="1"/>
+      <c r="AA78" s="1"/>
+      <c r="AB78" s="1"/>
+      <c r="AC78" s="1"/>
+      <c r="AD78" s="1"/>
+      <c r="AE78" s="1"/>
+      <c r="AF78" s="1"/>
+      <c r="AG78" s="1"/>
+      <c r="AH78" s="1"/>
+      <c r="AI78" s="1"/>
+      <c r="AJ78" s="1"/>
+      <c r="AK78" s="1"/>
+      <c r="AL78" s="1"/>
+      <c r="AM78" s="1"/>
+      <c r="AN78" s="1"/>
+      <c r="AO78" s="1"/>
+      <c r="AP78" s="1"/>
+      <c r="AQ78" s="1"/>
+      <c r="AR78" s="1"/>
+      <c r="AS78" s="1"/>
+      <c r="AT78" s="1"/>
+      <c r="AU78" s="1"/>
+      <c r="AV78" s="1"/>
+      <c r="AW78" s="1"/>
+      <c r="AX78" s="1"/>
+      <c r="AY78" s="1"/>
+      <c r="AZ78" s="1"/>
+      <c r="BA78" s="1"/>
+      <c r="BB78" s="1"/>
+      <c r="BC78" s="1"/>
+      <c r="BD78" s="1"/>
+      <c r="BE78" s="1"/>
+      <c r="BF78" s="1"/>
+      <c r="BG78" s="1"/>
+      <c r="BH78" s="1"/>
+      <c r="BI78" s="1"/>
+      <c r="BJ78" s="1"/>
+      <c r="BK78" s="1"/>
+      <c r="BL78" s="1"/>
+      <c r="BM78" s="1"/>
+      <c r="BN78" s="1"/>
+      <c r="BO78" s="1"/>
+      <c r="BP78" s="1"/>
+      <c r="BQ78" s="1"/>
+      <c r="BR78" s="1"/>
+      <c r="BS78" s="1"/>
+      <c r="BT78" s="1"/>
+      <c r="BU78" s="1"/>
+      <c r="BV78" s="1"/>
+      <c r="BW78" s="1"/>
+      <c r="BX78" s="1"/>
+      <c r="BY78" s="1"/>
+      <c r="BZ78" s="1"/>
+      <c r="CA78" s="1"/>
+      <c r="CB78" s="1"/>
+      <c r="CC78" s="1"/>
+      <c r="CD78" s="1"/>
+      <c r="CE78" s="1"/>
+      <c r="CF78" s="1"/>
+      <c r="CG78" s="1"/>
+      <c r="CH78" s="1"/>
+      <c r="CI78" s="1"/>
+      <c r="CJ78" s="1"/>
+      <c r="CK78" s="1"/>
+      <c r="CL78" s="1"/>
+      <c r="CM78" s="1"/>
+      <c r="CN78" s="1"/>
+      <c r="CO78" s="1"/>
+      <c r="CP78" s="1"/>
+      <c r="CQ78" s="1"/>
+      <c r="CR78" s="1"/>
+      <c r="CS78" s="1"/>
+      <c r="CT78" s="1"/>
+      <c r="CU78" s="1"/>
+      <c r="CV78" s="1"/>
+      <c r="CW78" s="1"/>
+      <c r="CX78" s="1"/>
+      <c r="CY78" s="1"/>
+      <c r="CZ78" s="1"/>
+      <c r="DA78" s="1"/>
+      <c r="DB78" s="1"/>
+      <c r="DC78" s="1"/>
+      <c r="DD78" s="1"/>
+      <c r="DE78" s="1"/>
+      <c r="DF78" s="1"/>
+      <c r="DG78" s="1"/>
+      <c r="DH78" s="1"/>
+      <c r="DI78" s="1"/>
+      <c r="DJ78" s="1"/>
+      <c r="DK78" s="1"/>
+      <c r="DL78" s="1"/>
+      <c r="DM78" s="1"/>
+      <c r="DN78" s="1"/>
+      <c r="DO78" s="1"/>
+      <c r="DP78" s="1"/>
+      <c r="DQ78" s="1"/>
+      <c r="DR78" s="1"/>
+      <c r="DS78" s="1"/>
+      <c r="DT78" s="1"/>
+      <c r="DU78" s="1"/>
+      <c r="DV78" s="1"/>
+      <c r="DW78" s="1"/>
+      <c r="DX78" s="1"/>
+      <c r="DY78" s="1"/>
+      <c r="DZ78" s="1"/>
+      <c r="EA78" s="1"/>
+      <c r="EB78" s="1"/>
+      <c r="EC78" s="1"/>
+      <c r="ED78" s="1"/>
+      <c r="EE78" s="1"/>
+      <c r="EF78" s="1"/>
+      <c r="EG78" s="1"/>
+      <c r="EH78" s="1"/>
+      <c r="EI78" s="1"/>
+      <c r="EJ78" s="1"/>
+      <c r="EK78" s="1"/>
+      <c r="EL78" s="1"/>
+      <c r="EM78" s="1"/>
+      <c r="EN78" s="1"/>
+      <c r="EO78" s="1"/>
+      <c r="EP78" s="1"/>
+      <c r="EQ78" s="1"/>
+      <c r="ER78" s="1"/>
+      <c r="ES78" s="1"/>
+      <c r="ET78" s="1"/>
+      <c r="EU78" s="1"/>
+      <c r="EV78" s="1"/>
+      <c r="EW78" s="1"/>
+      <c r="EX78" s="1"/>
+      <c r="EY78" s="1"/>
+      <c r="EZ78" s="1"/>
+      <c r="FA78" s="1"/>
+      <c r="FB78" s="1"/>
+      <c r="FC78" s="1"/>
+      <c r="FD78" s="1"/>
+      <c r="FE78" s="1"/>
+      <c r="FF78" s="1"/>
+      <c r="FG78" s="1"/>
+      <c r="FH78" s="1"/>
+      <c r="FI78" s="1"/>
+      <c r="FJ78" s="1"/>
+      <c r="FK78" s="1"/>
+      <c r="FL78" s="1"/>
+      <c r="FM78" s="1"/>
+      <c r="FN78" s="1"/>
+      <c r="FO78" s="1"/>
+      <c r="FP78" s="1"/>
+      <c r="FQ78" s="1"/>
+      <c r="FR78" s="1"/>
+      <c r="FS78" s="1"/>
+      <c r="FT78" s="1"/>
+      <c r="FU78" s="1"/>
+      <c r="FV78" s="1"/>
+      <c r="FW78" s="1"/>
+      <c r="FX78" s="1"/>
+      <c r="FY78" s="1"/>
+      <c r="FZ78" s="1"/>
+      <c r="GA78" s="1"/>
+      <c r="GB78" s="1"/>
+      <c r="GC78" s="1"/>
+      <c r="GD78" s="1"/>
+      <c r="GE78" s="1"/>
+      <c r="GF78" s="1"/>
+      <c r="GG78" s="1"/>
+      <c r="GH78" s="1"/>
+      <c r="GI78" s="1"/>
+      <c r="GJ78" s="1"/>
+      <c r="GK78" s="1"/>
+      <c r="GL78" s="1"/>
+      <c r="GM78" s="1"/>
+      <c r="GN78" s="1"/>
+      <c r="GO78" s="1"/>
+      <c r="GP78" s="1"/>
+      <c r="GQ78" s="1"/>
+      <c r="GR78" s="1"/>
+      <c r="GS78" s="1"/>
+      <c r="GT78" s="1"/>
+      <c r="GU78" s="1"/>
+      <c r="GV78" s="1"/>
+      <c r="GW78" s="1"/>
+      <c r="GX78" s="1"/>
+      <c r="GY78" s="1"/>
+      <c r="GZ78" s="1"/>
+      <c r="HA78" s="1"/>
+      <c r="HB78" s="1"/>
+      <c r="HC78" s="1"/>
+      <c r="HD78" s="1"/>
+      <c r="HE78" s="1"/>
+      <c r="HF78" s="1"/>
+      <c r="HG78" s="1"/>
+      <c r="HH78" s="1"/>
+      <c r="HI78" s="1"/>
+      <c r="HJ78" s="1"/>
+      <c r="HK78" s="1"/>
+      <c r="HL78" s="1"/>
+      <c r="HM78" s="1"/>
+      <c r="HN78" s="1"/>
+      <c r="HO78" s="1"/>
+      <c r="HP78" s="1"/>
+      <c r="HQ78" s="1"/>
+      <c r="HR78" s="1"/>
+      <c r="HS78" s="1"/>
+      <c r="HT78" s="1"/>
+      <c r="HU78" s="1"/>
+      <c r="HV78" s="1"/>
+      <c r="HW78" s="1"/>
+      <c r="HX78" s="1"/>
+      <c r="HY78" s="1"/>
+      <c r="HZ78" s="1"/>
+      <c r="IA78" s="1"/>
+      <c r="IB78" s="1"/>
+      <c r="IC78" s="1"/>
+      <c r="ID78" s="1"/>
+      <c r="IE78" s="1"/>
+      <c r="IF78" s="1"/>
+      <c r="IG78" s="1"/>
+      <c r="IH78" s="1"/>
+      <c r="II78" s="1"/>
+      <c r="IJ78" s="1"/>
+      <c r="IK78" s="1"/>
+      <c r="IL78" s="1"/>
+      <c r="IM78" s="1"/>
+      <c r="IN78" s="1"/>
+      <c r="IO78" s="1"/>
+      <c r="IP78" s="1"/>
+      <c r="IQ78" s="1"/>
+      <c r="IR78" s="1"/>
+      <c r="IS78" s="1"/>
+      <c r="IT78" s="1"/>
+      <c r="IU78" s="1"/>
+      <c r="IV78" s="1"/>
+    </row>
+    <row r="79" spans="1:256" ht="12" customHeight="1">
+      <c r="I79" s="5"/>
+      <c r="J79" s="5"/>
+      <c r="K79" s="5"/>
+      <c r="L79" s="5"/>
+      <c r="M79" s="5"/>
+      <c r="N79" s="5"/>
+      <c r="O79" s="5"/>
+      <c r="P79" s="5"/>
+      <c r="Q79" s="5"/>
+      <c r="R79" s="5"/>
+    </row>
     <row r="80" spans="1:256" ht="15.95" customHeight="1"/>
     <row r="81" ht="15.95" customHeight="1"/>
     <row r="82" ht="15.95" customHeight="1"/>
@@ -19479,128 +19758,128 @@
     <row r="95" ht="15.95" customHeight="1"/>
     <row r="96" ht="15.95" customHeight="1"/>
     <row r="97" spans="1:16" ht="15.95" customHeight="1"/>
-    <row r="98" spans="1:16" ht="15.95" customHeight="1">
-      <c r="A98" s="59" t="s">
+    <row r="98" spans="1:16" ht="15.95" customHeight="1"/>
+    <row r="99" spans="1:16" ht="15.95" customHeight="1"/>
+    <row r="100" spans="1:16" ht="15.95" customHeight="1">
+      <c r="A100" s="59" t="s">
         <v>196</v>
       </c>
-      <c r="B98" s="59"/>
-      <c r="C98" s="59"/>
-      <c r="D98" s="59"/>
-      <c r="E98" s="59"/>
-      <c r="F98" s="59"/>
-      <c r="G98" s="59"/>
-      <c r="H98" s="59"/>
-      <c r="I98" s="59"/>
-      <c r="J98" s="59"/>
-      <c r="K98" s="59"/>
-      <c r="L98" s="59"/>
-      <c r="M98" s="59"/>
-      <c r="N98" s="59"/>
-      <c r="O98" s="59"/>
-      <c r="P98" s="59"/>
+      <c r="B100" s="59"/>
+      <c r="C100" s="59"/>
+      <c r="D100" s="59"/>
+      <c r="E100" s="59"/>
+      <c r="F100" s="59"/>
+      <c r="G100" s="59"/>
+      <c r="H100" s="59"/>
+      <c r="I100" s="59"/>
+      <c r="J100" s="59"/>
+      <c r="K100" s="59"/>
+      <c r="L100" s="59"/>
+      <c r="M100" s="59"/>
+      <c r="N100" s="59"/>
+      <c r="O100" s="59"/>
+      <c r="P100" s="59"/>
     </row>
-    <row r="99" spans="1:16" ht="15.95" customHeight="1">
-      <c r="A99" s="21" t="s">
+    <row r="101" spans="1:16" ht="15.95" customHeight="1">
+      <c r="A101" s="21" t="s">
         <v>197</v>
       </c>
-      <c r="B99" s="21" t="s">
+      <c r="B101" s="21" t="s">
         <v>198</v>
       </c>
-      <c r="C99" s="21" t="s">
+      <c r="C101" s="21" t="s">
         <v>199</v>
       </c>
-      <c r="D99" s="21" t="s">
+      <c r="D101" s="21" t="s">
         <v>200</v>
       </c>
-      <c r="E99" s="21" t="s">
+      <c r="E101" s="21" t="s">
         <v>201</v>
       </c>
-      <c r="F99" s="21" t="s">
+      <c r="F101" s="21" t="s">
         <v>202</v>
       </c>
-      <c r="G99" s="21" t="s">
+      <c r="G101" s="21" t="s">
         <v>203</v>
       </c>
-      <c r="H99" s="21" t="s">
+      <c r="H101" s="21" t="s">
         <v>204</v>
       </c>
-      <c r="I99" s="21" t="s">
+      <c r="I101" s="21" t="s">
         <v>205</v>
       </c>
-      <c r="J99" s="21" t="s">
+      <c r="J101" s="21" t="s">
         <v>206</v>
       </c>
-      <c r="K99" s="21" t="s">
+      <c r="K101" s="21" t="s">
         <v>207</v>
       </c>
-      <c r="L99" s="21" t="s">
+      <c r="L101" s="21" t="s">
         <v>208</v>
       </c>
-      <c r="M99" s="21" t="s">
+      <c r="M101" s="21" t="s">
         <v>209</v>
       </c>
-      <c r="N99" s="21" t="s">
+      <c r="N101" s="21" t="s">
         <v>210</v>
       </c>
-      <c r="O99" s="21" t="s">
+      <c r="O101" s="21" t="s">
         <v>211</v>
       </c>
-      <c r="P99" s="21" t="s">
+      <c r="P101" s="21" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="100" spans="1:16" ht="15.95" customHeight="1">
-      <c r="A100" s="23" t="s">
+    <row r="102" spans="1:16" ht="15.95" customHeight="1">
+      <c r="A102" s="23" t="s">
         <v>213</v>
       </c>
-      <c r="B100" s="23" t="s">
+      <c r="B102" s="23" t="s">
         <v>214</v>
       </c>
-      <c r="C100" s="23" t="s">
+      <c r="C102" s="23" t="s">
         <v>215</v>
       </c>
-      <c r="D100" s="23" t="s">
+      <c r="D102" s="23" t="s">
         <v>216</v>
       </c>
-      <c r="E100" s="23" t="s">
+      <c r="E102" s="23" t="s">
         <v>217</v>
       </c>
-      <c r="F100" s="23" t="s">
+      <c r="F102" s="23" t="s">
         <v>218</v>
       </c>
-      <c r="G100" s="23" t="s">
+      <c r="G102" s="23" t="s">
         <v>219</v>
       </c>
-      <c r="H100" s="23" t="s">
+      <c r="H102" s="23" t="s">
         <v>220</v>
       </c>
-      <c r="I100" s="23" t="s">
+      <c r="I102" s="23" t="s">
         <v>221</v>
       </c>
-      <c r="J100" s="23" t="s">
+      <c r="J102" s="23" t="s">
         <v>222</v>
       </c>
-      <c r="K100" s="23" t="s">
+      <c r="K102" s="23" t="s">
         <v>223</v>
       </c>
-      <c r="L100" s="23" t="s">
+      <c r="L102" s="23" t="s">
         <v>224</v>
       </c>
-      <c r="M100" s="23" t="s">
+      <c r="M102" s="23" t="s">
         <v>225</v>
       </c>
-      <c r="N100" s="23" t="s">
+      <c r="N102" s="23" t="s">
         <v>226</v>
       </c>
-      <c r="O100" s="23" t="s">
+      <c r="O102" s="23" t="s">
         <v>227</v>
       </c>
-      <c r="P100" s="23" t="s">
+      <c r="P102" s="23" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="101" spans="1:16" ht="15.95" customHeight="1"/>
-    <row r="102" spans="1:16" ht="15.95" customHeight="1"/>
     <row r="103" spans="1:16" ht="15.95" customHeight="1"/>
     <row r="104" spans="1:16" ht="15.95" customHeight="1"/>
     <row r="105" spans="1:16" ht="15.95" customHeight="1"/>
@@ -19669,58 +19948,58 @@
     <row r="168" spans="1:6" ht="15.95" customHeight="1"/>
     <row r="169" spans="1:6" ht="15.95" customHeight="1"/>
     <row r="170" spans="1:6" ht="15.95" customHeight="1"/>
-    <row r="171" spans="1:6" ht="15.95" customHeight="1">
-      <c r="A171" s="59" t="s">
+    <row r="171" spans="1:6" ht="15.95" customHeight="1"/>
+    <row r="172" spans="1:6" ht="15.95" customHeight="1"/>
+    <row r="173" spans="1:6" ht="15.95" customHeight="1">
+      <c r="A173" s="59" t="s">
         <v>195</v>
       </c>
-      <c r="B171" s="59"/>
-      <c r="C171" s="59"/>
-      <c r="D171" s="59"/>
-      <c r="E171" s="59"/>
-      <c r="F171" s="59"/>
+      <c r="B173" s="59"/>
+      <c r="C173" s="59"/>
+      <c r="D173" s="59"/>
+      <c r="E173" s="59"/>
+      <c r="F173" s="59"/>
     </row>
-    <row r="172" spans="1:6" ht="15.95" customHeight="1">
-      <c r="A172" s="21" t="s">
+    <row r="174" spans="1:6" ht="15.95" customHeight="1">
+      <c r="A174" s="21" t="s">
         <v>229</v>
       </c>
-      <c r="B172" s="21" t="s">
+      <c r="B174" s="21" t="s">
         <v>230</v>
       </c>
-      <c r="C172" s="21" t="s">
+      <c r="C174" s="21" t="s">
         <v>231</v>
       </c>
-      <c r="D172" s="21" t="s">
+      <c r="D174" s="21" t="s">
         <v>232</v>
       </c>
-      <c r="E172" s="21" t="s">
+      <c r="E174" s="21" t="s">
         <v>233</v>
       </c>
-      <c r="F172" s="21" t="s">
+      <c r="F174" s="21" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="173" spans="1:6" ht="15.95" customHeight="1">
-      <c r="A173" s="23" t="s">
+    <row r="175" spans="1:6" ht="15.95" customHeight="1">
+      <c r="A175" s="23" t="s">
         <v>235</v>
       </c>
-      <c r="B173" s="23" t="s">
+      <c r="B175" s="23" t="s">
         <v>236</v>
       </c>
-      <c r="C173" s="23" t="s">
+      <c r="C175" s="23" t="s">
         <v>237</v>
       </c>
-      <c r="D173" s="23" t="s">
+      <c r="D175" s="23" t="s">
         <v>238</v>
       </c>
-      <c r="E173" s="23" t="s">
+      <c r="E175" s="23" t="s">
         <v>239</v>
       </c>
-      <c r="F173" s="23" t="s">
+      <c r="F175" s="23" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="174" spans="1:6" ht="15.95" customHeight="1"/>
-    <row r="175" spans="1:6" ht="15.95" customHeight="1"/>
     <row r="176" spans="1:6" ht="15.95" customHeight="1"/>
     <row r="177" ht="15.95" customHeight="1"/>
     <row r="178" ht="15.95" customHeight="1"/>
@@ -19836,30 +20115,30 @@
     <row r="288" ht="15.95" customHeight="1"/>
     <row r="289" spans="1:2" ht="15.95" customHeight="1"/>
     <row r="290" spans="1:2" ht="15.95" customHeight="1"/>
-    <row r="291" spans="1:2" ht="15.95" customHeight="1">
-      <c r="A291" s="59" t="s">
+    <row r="291" spans="1:2" ht="15.95" customHeight="1"/>
+    <row r="292" spans="1:2" ht="15.95" customHeight="1"/>
+    <row r="293" spans="1:2" ht="15.95" customHeight="1">
+      <c r="A293" s="59" t="s">
         <v>284</v>
       </c>
-      <c r="B291" s="59"/>
+      <c r="B293" s="59"/>
     </row>
-    <row r="292" spans="1:2" ht="15.95" customHeight="1">
-      <c r="A292" s="21" t="s">
+    <row r="294" spans="1:2" ht="15.95" customHeight="1">
+      <c r="A294" s="21" t="s">
         <v>285</v>
       </c>
-      <c r="B292" s="22" t="s">
+      <c r="B294" s="22" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="293" spans="1:2" ht="15.95" customHeight="1">
-      <c r="A293" s="23" t="s">
+    <row r="295" spans="1:2" ht="15.95" customHeight="1">
+      <c r="A295" s="23" t="s">
         <v>287</v>
       </c>
-      <c r="B293" s="23" t="s">
+      <c r="B295" s="23" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="294" spans="1:2" ht="15.95" customHeight="1"/>
-    <row r="295" spans="1:2" ht="15.95" customHeight="1"/>
     <row r="296" spans="1:2" ht="15.95" customHeight="1"/>
     <row r="297" spans="1:2" ht="15.95" customHeight="1"/>
     <row r="298" spans="1:2" ht="15.95" customHeight="1"/>
@@ -20606,17 +20885,19 @@
     <row r="1039" ht="15.95" customHeight="1"/>
     <row r="1040" ht="15.95" customHeight="1"/>
     <row r="1041" ht="15.95" customHeight="1"/>
+    <row r="1042" ht="15.95" customHeight="1"/>
+    <row r="1043" ht="15.95" customHeight="1"/>
   </sheetData>
   <mergeCells count="10">
     <mergeCell ref="A1:A4"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="B3:E3"/>
-    <mergeCell ref="A291:B291"/>
-    <mergeCell ref="A171:F171"/>
-    <mergeCell ref="A98:P98"/>
-    <mergeCell ref="A72:B72"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="A55:C55"/>
+    <mergeCell ref="A293:B293"/>
+    <mergeCell ref="A173:F173"/>
+    <mergeCell ref="A100:P100"/>
+    <mergeCell ref="A74:B74"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="A57:C57"/>
     <mergeCell ref="A27:C27"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
@@ -21006,7 +21287,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:X144"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A119" zoomScalePageLayoutView="60" workbookViewId="0">
+    <sheetView topLeftCell="A128" zoomScalePageLayoutView="60" workbookViewId="0">
       <selection activeCell="B147" sqref="B147"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
POCOR-7421: code enhance update institution report cards | Status: Done
</commit_message>
<xml_diff>
--- a/webroot/export/customexcel/default_templates/profile_template.xlsx
+++ b/webroot/export/customexcel/default_templates/profile_template.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="342">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="346">
   <si>
     <t>${"image":{"displayValue":"Institutions.logo_content","imageWidth":"100","imageMarginLeft":"20","imageMarginTop":"5"}}</t>
   </si>
@@ -1055,6 +1055,18 @@
   </si>
   <si>
     <t>${"match": {"displayValue": "StudentFromEducationGrade.total_student_withdrawn_last_year","rows": {"matchFrom": "StudentFromEducationGrade.education_grade_id","matchTo": "StudentFromEducationGrade.education_grade_id"}}}</t>
+  </si>
+  <si>
+    <t>Count of  Withdrawn students Last Year</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${"match": {"displayValue": "LasrYearInstitutionStudentWithdrawn.area_level:1","rows": {"matchFrom": "InstitutionEducationGrade.id","matchTo": "InstitutionEducationGrade.id"}}} </t>
+  </si>
+  <si>
+    <t xml:space="preserve">${"match": {"displayValue": "LasrYearInstitutionStudentWithdrawn.area_level:2","rows": {"matchFrom": "InstitutionEducationGrade.id","matchTo": "InstitutionEducationGrade.id"}}} </t>
+  </si>
+  <si>
+    <t xml:space="preserve">${"match": {"displayValue": "LasrYearInstitutionStudentWithdrawn.area_level:3","rows": {"matchFrom": "InstitutionEducationGrade.id","matchTo": "InstitutionEducationGrade.id"}}} </t>
   </si>
 </sst>
 </file>
@@ -1458,6 +1470,17 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1494,6 +1517,12 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -1503,27 +1532,10 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1920,7 +1932,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:256" ht="15" customHeight="1">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="61" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2"/>
@@ -1941,13 +1953,13 @@
       <c r="Q1" s="5"/>
     </row>
     <row r="2" spans="1:256" ht="25.5" customHeight="1">
-      <c r="A2" s="56"/>
-      <c r="B2" s="57" t="s">
+      <c r="A2" s="61"/>
+      <c r="B2" s="62" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
       <c r="F2" s="6"/>
       <c r="G2" s="7"/>
       <c r="H2" s="5"/>
@@ -2201,13 +2213,13 @@
       <c r="IV2" s="1"/>
     </row>
     <row r="3" spans="1:256" ht="25.5" customHeight="1">
-      <c r="A3" s="56"/>
-      <c r="B3" s="58" t="s">
+      <c r="A3" s="61"/>
+      <c r="B3" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="58"/>
-      <c r="D3" s="58"/>
-      <c r="E3" s="58"/>
+      <c r="C3" s="63"/>
+      <c r="D3" s="63"/>
+      <c r="E3" s="63"/>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
       <c r="H3" s="5"/>
@@ -2461,7 +2473,7 @@
       <c r="IV3" s="1"/>
     </row>
     <row r="4" spans="1:256" ht="22.5" customHeight="1">
-      <c r="A4" s="56"/>
+      <c r="A4" s="61"/>
       <c r="B4" s="2"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
@@ -6800,11 +6812,11 @@
       <c r="IV26" s="1"/>
     </row>
     <row r="27" spans="1:256" ht="12" customHeight="1">
-      <c r="A27" s="60" t="s">
+      <c r="A27" s="65" t="s">
         <v>30</v>
       </c>
-      <c r="B27" s="61"/>
-      <c r="C27" s="61"/>
+      <c r="B27" s="66"/>
+      <c r="C27" s="66"/>
       <c r="D27" s="16"/>
       <c r="E27" s="12"/>
       <c r="F27" s="12"/>
@@ -10446,10 +10458,10 @@
       <c r="IV40" s="1"/>
     </row>
     <row r="41" spans="1:256" ht="12" customHeight="1">
-      <c r="A41" s="76" t="s">
+      <c r="A41" s="57" t="s">
         <v>45</v>
       </c>
-      <c r="B41" s="75" t="s">
+      <c r="B41" s="56" t="s">
         <v>46</v>
       </c>
       <c r="C41" s="16"/>
@@ -10708,10 +10720,10 @@
       <c r="IV41" s="1"/>
     </row>
     <row r="42" spans="1:256" ht="12" customHeight="1">
-      <c r="A42" s="76" t="s">
+      <c r="A42" s="57" t="s">
         <v>47</v>
       </c>
-      <c r="B42" s="75" t="s">
+      <c r="B42" s="56" t="s">
         <v>48</v>
       </c>
       <c r="C42" s="16"/>
@@ -10970,10 +10982,10 @@
       <c r="IV42" s="1"/>
     </row>
     <row r="43" spans="1:256" ht="12" customHeight="1">
-      <c r="A43" s="76" t="s">
+      <c r="A43" s="57" t="s">
         <v>321</v>
       </c>
-      <c r="B43" s="75" t="s">
+      <c r="B43" s="56" t="s">
         <v>48</v>
       </c>
       <c r="C43" s="16"/>
@@ -11232,10 +11244,10 @@
       <c r="IV43" s="1"/>
     </row>
     <row r="44" spans="1:256" ht="12" customHeight="1">
-      <c r="A44" s="76" t="s">
+      <c r="A44" s="57" t="s">
         <v>322</v>
       </c>
-      <c r="B44" s="75" t="s">
+      <c r="B44" s="56" t="s">
         <v>325</v>
       </c>
       <c r="C44" s="16"/>
@@ -11494,10 +11506,10 @@
       <c r="IV44" s="1"/>
     </row>
     <row r="45" spans="1:256" ht="12" customHeight="1">
-      <c r="A45" s="76" t="s">
+      <c r="A45" s="57" t="s">
         <v>323</v>
       </c>
-      <c r="B45" s="75" t="s">
+      <c r="B45" s="56" t="s">
         <v>326</v>
       </c>
       <c r="C45" s="16"/>
@@ -11756,10 +11768,10 @@
       <c r="IV45" s="1"/>
     </row>
     <row r="46" spans="1:256" ht="12" customHeight="1">
-      <c r="A46" s="76" t="s">
+      <c r="A46" s="57" t="s">
         <v>324</v>
       </c>
-      <c r="B46" s="74" t="s">
+      <c r="B46" s="55" t="s">
         <v>327</v>
       </c>
       <c r="C46" s="16"/>
@@ -15422,11 +15434,11 @@
       <c r="IV61" s="1"/>
     </row>
     <row r="62" spans="1:256" ht="12" customHeight="1">
-      <c r="A62" s="60" t="s">
+      <c r="A62" s="65" t="s">
         <v>136</v>
       </c>
-      <c r="B62" s="61"/>
-      <c r="C62" s="61"/>
+      <c r="B62" s="66"/>
+      <c r="C62" s="66"/>
       <c r="D62" s="16"/>
       <c r="E62" s="12"/>
       <c r="F62" s="12"/>
@@ -17260,10 +17272,10 @@
       <c r="IV68" s="1"/>
     </row>
     <row r="69" spans="1:256" ht="12" customHeight="1">
-      <c r="A69" s="59" t="s">
+      <c r="A69" s="64" t="s">
         <v>66</v>
       </c>
-      <c r="B69" s="59"/>
+      <c r="B69" s="64"/>
       <c r="C69" s="14"/>
       <c r="D69" s="16"/>
       <c r="E69" s="12"/>
@@ -19612,10 +19624,10 @@
       <c r="IV78" s="1"/>
     </row>
     <row r="79" spans="1:256" ht="12" customHeight="1">
-      <c r="A79" s="59" t="s">
+      <c r="A79" s="64" t="s">
         <v>184</v>
       </c>
-      <c r="B79" s="59"/>
+      <c r="B79" s="64"/>
       <c r="C79" s="1"/>
       <c r="E79" s="1"/>
       <c r="F79" s="1"/>
@@ -20936,24 +20948,24 @@
     <row r="103" spans="1:16" ht="15.95" customHeight="1"/>
     <row r="104" spans="1:16" ht="15.95" customHeight="1"/>
     <row r="105" spans="1:16" ht="15.95" customHeight="1">
-      <c r="A105" s="59" t="s">
+      <c r="A105" s="64" t="s">
         <v>190</v>
       </c>
-      <c r="B105" s="59"/>
-      <c r="C105" s="59"/>
-      <c r="D105" s="59"/>
-      <c r="E105" s="59"/>
-      <c r="F105" s="59"/>
-      <c r="G105" s="59"/>
-      <c r="H105" s="59"/>
-      <c r="I105" s="59"/>
-      <c r="J105" s="59"/>
-      <c r="K105" s="59"/>
-      <c r="L105" s="59"/>
-      <c r="M105" s="59"/>
-      <c r="N105" s="59"/>
-      <c r="O105" s="59"/>
-      <c r="P105" s="59"/>
+      <c r="B105" s="64"/>
+      <c r="C105" s="64"/>
+      <c r="D105" s="64"/>
+      <c r="E105" s="64"/>
+      <c r="F105" s="64"/>
+      <c r="G105" s="64"/>
+      <c r="H105" s="64"/>
+      <c r="I105" s="64"/>
+      <c r="J105" s="64"/>
+      <c r="K105" s="64"/>
+      <c r="L105" s="64"/>
+      <c r="M105" s="64"/>
+      <c r="N105" s="64"/>
+      <c r="O105" s="64"/>
+      <c r="P105" s="64"/>
     </row>
     <row r="106" spans="1:16" ht="15.95" customHeight="1">
       <c r="A106" s="20" t="s">
@@ -21126,14 +21138,14 @@
     <row r="176" ht="15.95" customHeight="1"/>
     <row r="177" spans="1:6" ht="15.95" customHeight="1"/>
     <row r="178" spans="1:6" ht="15.95" customHeight="1">
-      <c r="A178" s="59" t="s">
+      <c r="A178" s="64" t="s">
         <v>189</v>
       </c>
-      <c r="B178" s="59"/>
-      <c r="C178" s="59"/>
-      <c r="D178" s="59"/>
-      <c r="E178" s="59"/>
-      <c r="F178" s="59"/>
+      <c r="B178" s="64"/>
+      <c r="C178" s="64"/>
+      <c r="D178" s="64"/>
+      <c r="E178" s="64"/>
+      <c r="F178" s="64"/>
     </row>
     <row r="179" spans="1:6" ht="15.95" customHeight="1">
       <c r="A179" s="20" t="s">
@@ -21293,10 +21305,10 @@
     <row r="296" spans="1:2" ht="15.95" customHeight="1"/>
     <row r="297" spans="1:2" ht="15.95" customHeight="1"/>
     <row r="298" spans="1:2" ht="15.95" customHeight="1">
-      <c r="A298" s="59" t="s">
+      <c r="A298" s="64" t="s">
         <v>278</v>
       </c>
-      <c r="B298" s="59"/>
+      <c r="B298" s="64"/>
     </row>
     <row r="299" spans="1:2" ht="15.95" customHeight="1">
       <c r="A299" s="20" t="s">
@@ -21339,14 +21351,14 @@
     <row r="323" spans="1:6" ht="15.95" customHeight="1"/>
     <row r="324" spans="1:6" ht="15.95" customHeight="1"/>
     <row r="325" spans="1:6" ht="15.95" customHeight="1">
-      <c r="A325" s="55" t="s">
+      <c r="A325" s="60" t="s">
         <v>318</v>
       </c>
-      <c r="B325" s="55"/>
-      <c r="C325" s="55"/>
-      <c r="D325" s="55"/>
-      <c r="E325" s="55"/>
-      <c r="F325" s="55"/>
+      <c r="B325" s="60"/>
+      <c r="C325" s="60"/>
+      <c r="D325" s="60"/>
+      <c r="E325" s="60"/>
+      <c r="F325" s="60"/>
     </row>
     <row r="326" spans="1:6" ht="15.95" customHeight="1">
       <c r="A326" s="23" t="s">
@@ -22148,12 +22160,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="55" t="s">
+      <c r="A1" s="60" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="23" t="s">
@@ -22212,11 +22224,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="62" t="s">
+      <c r="A1" s="67" t="s">
         <v>73</v>
       </c>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
+      <c r="B1" s="67"/>
+      <c r="C1" s="67"/>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="23" t="s">
@@ -22274,11 +22286,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="63" t="s">
+      <c r="A1" s="68" t="s">
         <v>79</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
+      <c r="B1" s="68"/>
+      <c r="C1" s="68"/>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="23" t="s">
@@ -22336,11 +22348,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="63" t="s">
+      <c r="A1" s="68" t="s">
         <v>85</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
+      <c r="B1" s="68"/>
+      <c r="C1" s="68"/>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="23" t="s">
@@ -22398,11 +22410,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="63" t="s">
+      <c r="A1" s="68" t="s">
         <v>90</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
+      <c r="B1" s="68"/>
+      <c r="C1" s="68"/>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="7" t="s">
@@ -22460,11 +22472,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="63" t="s">
+      <c r="A1" s="68" t="s">
         <v>95</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
+      <c r="B1" s="68"/>
+      <c r="C1" s="68"/>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="7" t="s">
@@ -22508,10 +22520,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AA191"/>
+  <dimension ref="A1:AA221"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="Z3" sqref="Z3"/>
+    <sheetView tabSelected="1" topLeftCell="A189" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="D221" sqref="D221"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
@@ -22526,35 +22538,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27">
-      <c r="A1" s="70" t="s">
+      <c r="A1" s="72" t="s">
         <v>100</v>
       </c>
-      <c r="B1" s="71"/>
-      <c r="C1" s="71"/>
-      <c r="D1" s="71"/>
-      <c r="E1" s="71"/>
-      <c r="F1" s="71"/>
-      <c r="G1" s="71"/>
-      <c r="H1" s="71"/>
-      <c r="I1" s="71"/>
-      <c r="J1" s="71"/>
-      <c r="K1" s="71"/>
-      <c r="L1" s="71"/>
-      <c r="M1" s="71"/>
-      <c r="N1" s="71"/>
-      <c r="O1" s="71"/>
-      <c r="P1" s="71"/>
-      <c r="Q1" s="71"/>
-      <c r="R1" s="71"/>
-      <c r="S1" s="71"/>
-      <c r="T1" s="71"/>
-      <c r="U1" s="71"/>
-      <c r="V1" s="71"/>
-      <c r="W1" s="71"/>
-      <c r="X1" s="71"/>
-      <c r="Y1" s="71"/>
-      <c r="Z1" s="71"/>
-      <c r="AA1" s="71"/>
+      <c r="B1" s="73"/>
+      <c r="C1" s="73"/>
+      <c r="D1" s="73"/>
+      <c r="E1" s="73"/>
+      <c r="F1" s="73"/>
+      <c r="G1" s="73"/>
+      <c r="H1" s="73"/>
+      <c r="I1" s="73"/>
+      <c r="J1" s="73"/>
+      <c r="K1" s="73"/>
+      <c r="L1" s="73"/>
+      <c r="M1" s="73"/>
+      <c r="N1" s="73"/>
+      <c r="O1" s="73"/>
+      <c r="P1" s="73"/>
+      <c r="Q1" s="73"/>
+      <c r="R1" s="73"/>
+      <c r="S1" s="73"/>
+      <c r="T1" s="73"/>
+      <c r="U1" s="73"/>
+      <c r="V1" s="73"/>
+      <c r="W1" s="73"/>
+      <c r="X1" s="73"/>
+      <c r="Y1" s="73"/>
+      <c r="Z1" s="73"/>
+      <c r="AA1" s="73"/>
     </row>
     <row r="2" spans="1:27">
       <c r="A2" s="26" t="s">
@@ -22632,10 +22644,10 @@
       <c r="Y2" s="51" t="s">
         <v>328</v>
       </c>
-      <c r="Z2" s="78" t="s">
+      <c r="Z2" s="59" t="s">
         <v>338</v>
       </c>
-      <c r="AA2" s="78" t="s">
+      <c r="AA2" s="59" t="s">
         <v>339</v>
       </c>
     </row>
@@ -22712,23 +22724,23 @@
       <c r="X3" s="53" t="s">
         <v>270</v>
       </c>
-      <c r="Y3" s="77" t="s">
+      <c r="Y3" s="58" t="s">
         <v>329</v>
       </c>
-      <c r="Z3" s="77" t="s">
+      <c r="Z3" s="58" t="s">
         <v>340</v>
       </c>
-      <c r="AA3" s="77" t="s">
+      <c r="AA3" s="58" t="s">
         <v>341</v>
       </c>
     </row>
     <row r="11" spans="1:27">
-      <c r="A11" s="64" t="s">
+      <c r="A11" s="69" t="s">
         <v>169</v>
       </c>
-      <c r="B11" s="65"/>
-      <c r="C11" s="65"/>
-      <c r="D11" s="66"/>
+      <c r="B11" s="70"/>
+      <c r="C11" s="70"/>
+      <c r="D11" s="71"/>
     </row>
     <row r="12" spans="1:27">
       <c r="A12" s="37" t="s">
@@ -22745,12 +22757,12 @@
       </c>
     </row>
     <row r="24" spans="1:4">
-      <c r="A24" s="64" t="s">
+      <c r="A24" s="69" t="s">
         <v>168</v>
       </c>
-      <c r="B24" s="65"/>
-      <c r="C24" s="65"/>
-      <c r="D24" s="66"/>
+      <c r="B24" s="70"/>
+      <c r="C24" s="70"/>
+      <c r="D24" s="71"/>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="37" t="s">
@@ -22767,12 +22779,12 @@
       </c>
     </row>
     <row r="38" spans="1:4">
-      <c r="A38" s="64" t="s">
+      <c r="A38" s="69" t="s">
         <v>283</v>
       </c>
-      <c r="B38" s="65"/>
-      <c r="C38" s="65"/>
-      <c r="D38" s="66"/>
+      <c r="B38" s="70"/>
+      <c r="C38" s="70"/>
+      <c r="D38" s="71"/>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="37" t="s">
@@ -22789,12 +22801,12 @@
       </c>
     </row>
     <row r="54" spans="1:8">
-      <c r="A54" s="64" t="s">
+      <c r="A54" s="69" t="s">
         <v>256</v>
       </c>
-      <c r="B54" s="65"/>
-      <c r="C54" s="65"/>
-      <c r="D54" s="66"/>
+      <c r="B54" s="70"/>
+      <c r="C54" s="70"/>
+      <c r="D54" s="71"/>
     </row>
     <row r="55" spans="1:8">
       <c r="A55" s="44" t="s">
@@ -22815,12 +22827,12 @@
       <c r="H55" s="46"/>
     </row>
     <row r="67" spans="1:4">
-      <c r="A67" s="64" t="s">
+      <c r="A67" s="69" t="s">
         <v>163</v>
       </c>
-      <c r="B67" s="65"/>
-      <c r="C67" s="65"/>
-      <c r="D67" s="66"/>
+      <c r="B67" s="70"/>
+      <c r="C67" s="70"/>
+      <c r="D67" s="71"/>
     </row>
     <row r="68" spans="1:4">
       <c r="A68" s="37" t="s">
@@ -22837,12 +22849,12 @@
       </c>
     </row>
     <row r="89" spans="1:4">
-      <c r="A89" s="64" t="s">
+      <c r="A89" s="69" t="s">
         <v>176</v>
       </c>
-      <c r="B89" s="65"/>
-      <c r="C89" s="65"/>
-      <c r="D89" s="66"/>
+      <c r="B89" s="70"/>
+      <c r="C89" s="70"/>
+      <c r="D89" s="71"/>
     </row>
     <row r="90" spans="1:4">
       <c r="A90" s="37" t="s">
@@ -22859,12 +22871,12 @@
       </c>
     </row>
     <row r="105" spans="1:8">
-      <c r="A105" s="64" t="s">
+      <c r="A105" s="69" t="s">
         <v>260</v>
       </c>
-      <c r="B105" s="65"/>
-      <c r="C105" s="65"/>
-      <c r="D105" s="66"/>
+      <c r="B105" s="70"/>
+      <c r="C105" s="70"/>
+      <c r="D105" s="71"/>
     </row>
     <row r="106" spans="1:8" s="47" customFormat="1">
       <c r="A106" s="44" t="s">
@@ -22885,12 +22897,12 @@
       <c r="H106" s="46"/>
     </row>
     <row r="120" spans="1:4">
-      <c r="A120" s="67" t="s">
+      <c r="A120" s="74" t="s">
         <v>181</v>
       </c>
-      <c r="B120" s="68"/>
-      <c r="C120" s="68"/>
-      <c r="D120" s="69"/>
+      <c r="B120" s="75"/>
+      <c r="C120" s="75"/>
+      <c r="D120" s="76"/>
     </row>
     <row r="121" spans="1:4" ht="60">
       <c r="A121" s="37" t="s">
@@ -22901,13 +22913,13 @@
       </c>
     </row>
     <row r="142" spans="1:5">
-      <c r="A142" s="70" t="s">
+      <c r="A142" s="72" t="s">
         <v>287</v>
       </c>
-      <c r="B142" s="71"/>
-      <c r="C142" s="71"/>
-      <c r="D142" s="71"/>
-      <c r="E142" s="71"/>
+      <c r="B142" s="73"/>
+      <c r="C142" s="73"/>
+      <c r="D142" s="73"/>
+      <c r="E142" s="73"/>
     </row>
     <row r="143" spans="1:5">
       <c r="A143" s="51" t="s">
@@ -22944,12 +22956,12 @@
       </c>
     </row>
     <row r="167" spans="1:4">
-      <c r="A167" s="64" t="s">
+      <c r="A167" s="69" t="s">
         <v>330</v>
       </c>
-      <c r="B167" s="65"/>
-      <c r="C167" s="65"/>
-      <c r="D167" s="66"/>
+      <c r="B167" s="70"/>
+      <c r="C167" s="70"/>
+      <c r="D167" s="71"/>
     </row>
     <row r="168" spans="1:4">
       <c r="A168" s="37" t="s">
@@ -22966,12 +22978,12 @@
       </c>
     </row>
     <row r="190" spans="1:4">
-      <c r="A190" s="64" t="s">
+      <c r="A190" s="69" t="s">
         <v>334</v>
       </c>
-      <c r="B190" s="65"/>
-      <c r="C190" s="65"/>
-      <c r="D190" s="66"/>
+      <c r="B190" s="70"/>
+      <c r="C190" s="70"/>
+      <c r="D190" s="71"/>
     </row>
     <row r="191" spans="1:4">
       <c r="A191" s="37" t="s">
@@ -22987,8 +22999,31 @@
         <v>337</v>
       </c>
     </row>
+    <row r="220" spans="1:4">
+      <c r="A220" s="69" t="s">
+        <v>342</v>
+      </c>
+      <c r="B220" s="70"/>
+      <c r="C220" s="70"/>
+      <c r="D220" s="71"/>
+    </row>
+    <row r="221" spans="1:4">
+      <c r="A221" s="37" t="s">
+        <v>164</v>
+      </c>
+      <c r="B221" s="43" t="s">
+        <v>343</v>
+      </c>
+      <c r="C221" s="43" t="s">
+        <v>344</v>
+      </c>
+      <c r="D221" s="43" t="s">
+        <v>345</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="13">
+    <mergeCell ref="A220:D220"/>
     <mergeCell ref="A167:D167"/>
     <mergeCell ref="A190:D190"/>
     <mergeCell ref="A1:AA1"/>
@@ -23036,20 +23071,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
-      <c r="A1" s="72" t="s">
+      <c r="A1" s="77" t="s">
         <v>235</v>
       </c>
-      <c r="B1" s="73"/>
-      <c r="C1" s="73"/>
-      <c r="D1" s="73"/>
-      <c r="E1" s="73"/>
-      <c r="F1" s="73"/>
-      <c r="G1" s="73"/>
-      <c r="H1" s="73"/>
-      <c r="I1" s="73"/>
-      <c r="J1" s="73"/>
-      <c r="K1" s="73"/>
-      <c r="L1" s="73"/>
+      <c r="B1" s="78"/>
+      <c r="C1" s="78"/>
+      <c r="D1" s="78"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="78"/>
+      <c r="G1" s="78"/>
+      <c r="H1" s="78"/>
+      <c r="I1" s="78"/>
+      <c r="J1" s="78"/>
+      <c r="K1" s="78"/>
+      <c r="L1" s="78"/>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="39" t="s">

</xml_diff>

<commit_message>
POCOR-7421: code enhance for enrolled promoted withdrawn last year student | Status: Done
</commit_message>
<xml_diff>
--- a/webroot/export/customexcel/default_templates/profile_template.xlsx
+++ b/webroot/export/customexcel/default_templates/profile_template.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="346">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="349">
   <si>
     <t>${"image":{"displayValue":"Institutions.logo_content","imageWidth":"100","imageMarginLeft":"20","imageMarginTop":"5"}}</t>
   </si>
@@ -1067,6 +1067,15 @@
   </si>
   <si>
     <t xml:space="preserve">${"match": {"displayValue": "LasrYearInstitutionStudentWithdrawn.area_level:3","rows": {"matchFrom": "InstitutionEducationGrade.id","matchTo": "InstitutionEducationGrade.id"}}} </t>
+  </si>
+  <si>
+    <t>Last Year Total Student Enrolled/Promoted/Withdrawn Rate</t>
+  </si>
+  <si>
+    <t>Education Grades</t>
+  </si>
+  <si>
+    <t>${"match": {"displayValue": "LastYearEducationGrade.education_grade_name","rows": {"matchFrom": "StudentFromEducationGrade.education_grade_id","matchTo": "StudentFromEducationGrade.education_grade_id"}}}</t>
   </si>
 </sst>
 </file>
@@ -1200,7 +1209,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -1346,11 +1355,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1536,6 +1556,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -22520,10 +22546,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AA221"/>
+  <dimension ref="A1:X252"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A189" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="D221" sqref="D221"/>
+    <sheetView tabSelected="1" topLeftCell="A139" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="E263" sqref="E263"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
@@ -22534,10 +22560,10 @@
     <col min="21" max="21" width="12.85546875" customWidth="1"/>
     <col min="22" max="23" width="12.42578125" customWidth="1"/>
     <col min="24" max="24" width="14.5703125" customWidth="1"/>
-    <col min="25" max="1023" width="12.42578125" customWidth="1"/>
+    <col min="25" max="1020" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27">
+    <row r="1" spans="1:24">
       <c r="A1" s="72" t="s">
         <v>100</v>
       </c>
@@ -22564,11 +22590,8 @@
       <c r="V1" s="73"/>
       <c r="W1" s="73"/>
       <c r="X1" s="73"/>
-      <c r="Y1" s="73"/>
-      <c r="Z1" s="73"/>
-      <c r="AA1" s="73"/>
     </row>
-    <row r="2" spans="1:27">
+    <row r="2" spans="1:24">
       <c r="A2" s="26" t="s">
         <v>75</v>
       </c>
@@ -22641,17 +22664,8 @@
       <c r="X2" s="51" t="s">
         <v>271</v>
       </c>
-      <c r="Y2" s="51" t="s">
-        <v>328</v>
-      </c>
-      <c r="Z2" s="59" t="s">
-        <v>338</v>
-      </c>
-      <c r="AA2" s="59" t="s">
-        <v>339</v>
-      </c>
     </row>
-    <row r="3" spans="1:27">
+    <row r="3" spans="1:24">
       <c r="A3" s="29" t="s">
         <v>118</v>
       </c>
@@ -22724,17 +22738,8 @@
       <c r="X3" s="53" t="s">
         <v>270</v>
       </c>
-      <c r="Y3" s="58" t="s">
-        <v>329</v>
-      </c>
-      <c r="Z3" s="58" t="s">
-        <v>340</v>
-      </c>
-      <c r="AA3" s="58" t="s">
-        <v>341</v>
-      </c>
     </row>
-    <row r="11" spans="1:27">
+    <row r="11" spans="1:24">
       <c r="A11" s="69" t="s">
         <v>169</v>
       </c>
@@ -22742,7 +22747,7 @@
       <c r="C11" s="70"/>
       <c r="D11" s="71"/>
     </row>
-    <row r="12" spans="1:27">
+    <row r="12" spans="1:24">
       <c r="A12" s="37" t="s">
         <v>164</v>
       </c>
@@ -22913,13 +22918,13 @@
       </c>
     </row>
     <row r="142" spans="1:5">
-      <c r="A142" s="72" t="s">
+      <c r="A142" s="79" t="s">
         <v>287</v>
       </c>
-      <c r="B142" s="73"/>
-      <c r="C142" s="73"/>
-      <c r="D142" s="73"/>
-      <c r="E142" s="73"/>
+      <c r="B142" s="80"/>
+      <c r="C142" s="80"/>
+      <c r="D142" s="80"/>
+      <c r="E142" s="80"/>
     </row>
     <row r="143" spans="1:5">
       <c r="A143" s="51" t="s">
@@ -23021,12 +23026,49 @@
         <v>345</v>
       </c>
     </row>
+    <row r="250" spans="1:4">
+      <c r="A250" s="74" t="s">
+        <v>346</v>
+      </c>
+      <c r="B250" s="75"/>
+      <c r="C250" s="75"/>
+      <c r="D250" s="76"/>
+    </row>
+    <row r="251" spans="1:4">
+      <c r="A251" s="51" t="s">
+        <v>347</v>
+      </c>
+      <c r="B251" s="51" t="s">
+        <v>328</v>
+      </c>
+      <c r="C251" s="59" t="s">
+        <v>338</v>
+      </c>
+      <c r="D251" s="59" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="252" spans="1:4">
+      <c r="A252" t="s">
+        <v>348</v>
+      </c>
+      <c r="B252" s="58" t="s">
+        <v>329</v>
+      </c>
+      <c r="C252" s="58" t="s">
+        <v>340</v>
+      </c>
+      <c r="D252" s="58" t="s">
+        <v>341</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="14">
+    <mergeCell ref="A250:D250"/>
     <mergeCell ref="A220:D220"/>
     <mergeCell ref="A167:D167"/>
     <mergeCell ref="A190:D190"/>
-    <mergeCell ref="A1:AA1"/>
+    <mergeCell ref="A1:X1"/>
     <mergeCell ref="A89:D89"/>
     <mergeCell ref="A105:D105"/>
     <mergeCell ref="A120:D120"/>

</xml_diff>

<commit_message>
POCOR-7421: code enhance for last year related functions | Status: Done
</commit_message>
<xml_diff>
--- a/webroot/export/customexcel/default_templates/profile_template.xlsx
+++ b/webroot/export/customexcel/default_templates/profile_template.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="350">
   <si>
     <t>${"image":{"displayValue":"Institutions.logo_content","imageWidth":"100","imageMarginLeft":"20","imageMarginTop":"5"}}</t>
   </si>
@@ -1024,15 +1024,6 @@
     <t>Count of  Enrolled students Last Year</t>
   </si>
   <si>
-    <t xml:space="preserve">${"match": {"displayValue": "LasrYearInstitutionStudentEnrolled.area_level:1","rows": {"matchFrom": "InstitutionEducationGrade.id","matchTo": "InstitutionEducationGrade.id"}}} </t>
-  </si>
-  <si>
-    <t xml:space="preserve">${"match": {"displayValue": "LasrYearInstitutionStudentEnrolled.area_level:2","rows": {"matchFrom": "InstitutionEducationGrade.id","matchTo": "InstitutionEducationGrade.id"}}} </t>
-  </si>
-  <si>
-    <t xml:space="preserve">${"match": {"displayValue": "LasrYearInstitutionStudentEnrolled.area_level:3","rows": {"matchFrom": "InstitutionEducationGrade.id","matchTo": "InstitutionEducationGrade.id"}}} </t>
-  </si>
-  <si>
     <t>Count of  Promoted students Last Year</t>
   </si>
   <si>
@@ -1076,6 +1067,18 @@
   </si>
   <si>
     <t>${"match": {"displayValue": "LastYearEducationGrade.education_grade_name","rows": {"matchFrom": "StudentFromEducationGrade.education_grade_id","matchTo": "StudentFromEducationGrade.education_grade_id"}}}</t>
+  </si>
+  <si>
+    <t>${"match": {"displayValue": "LastYearInstitutionEducationGrade.name","rows": {"matchFrom": "LastYearInstitutionEducationGrade.id","matchTo": "LastYearInstitutionEducationGrade.id"}}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${"match": {"displayValue": "LasrYearInstitutionStudentEnrolled.area_level:1","rows": {"matchFrom": "LastYearInstitutionEducationGrade.id","matchTo": "LastYearInstitutionEducationGrade.id"}}} </t>
+  </si>
+  <si>
+    <t xml:space="preserve">${"match": {"displayValue": "LasrYearInstitutionStudentEnrolled.area_level:2","rows": {"matchFrom": "LastYearInstitutionEducationGrade.id","matchTo": "LastYearInstitutionEducationGrade.id"}}} </t>
+  </si>
+  <si>
+    <t xml:space="preserve">${"match": {"displayValue": "LasrYearInstitutionStudentEnrolled.area_level:3","rows": {"matchFrom": "LastYearInstitutionEducationGrade.id","matchTo": "LastYearInstitutionEducationGrade.id"}}} </t>
   </si>
 </sst>
 </file>
@@ -1529,6 +1532,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1543,25 +1555,16 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -22548,8 +22551,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:X252"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A139" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="E263" sqref="E263"/>
+    <sheetView tabSelected="1" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="A67" sqref="A67:E68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
@@ -22564,32 +22567,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24">
-      <c r="A1" s="72" t="s">
+      <c r="A1" s="75" t="s">
         <v>100</v>
       </c>
-      <c r="B1" s="73"/>
-      <c r="C1" s="73"/>
-      <c r="D1" s="73"/>
-      <c r="E1" s="73"/>
-      <c r="F1" s="73"/>
-      <c r="G1" s="73"/>
-      <c r="H1" s="73"/>
-      <c r="I1" s="73"/>
-      <c r="J1" s="73"/>
-      <c r="K1" s="73"/>
-      <c r="L1" s="73"/>
-      <c r="M1" s="73"/>
-      <c r="N1" s="73"/>
-      <c r="O1" s="73"/>
-      <c r="P1" s="73"/>
-      <c r="Q1" s="73"/>
-      <c r="R1" s="73"/>
-      <c r="S1" s="73"/>
-      <c r="T1" s="73"/>
-      <c r="U1" s="73"/>
-      <c r="V1" s="73"/>
-      <c r="W1" s="73"/>
-      <c r="X1" s="73"/>
+      <c r="B1" s="76"/>
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
+      <c r="F1" s="76"/>
+      <c r="G1" s="76"/>
+      <c r="H1" s="76"/>
+      <c r="I1" s="76"/>
+      <c r="J1" s="76"/>
+      <c r="K1" s="76"/>
+      <c r="L1" s="76"/>
+      <c r="M1" s="76"/>
+      <c r="N1" s="76"/>
+      <c r="O1" s="76"/>
+      <c r="P1" s="76"/>
+      <c r="Q1" s="76"/>
+      <c r="R1" s="76"/>
+      <c r="S1" s="76"/>
+      <c r="T1" s="76"/>
+      <c r="U1" s="76"/>
+      <c r="V1" s="76"/>
+      <c r="W1" s="76"/>
+      <c r="X1" s="76"/>
     </row>
     <row r="2" spans="1:24">
       <c r="A2" s="26" t="s">
@@ -22740,12 +22743,12 @@
       </c>
     </row>
     <row r="11" spans="1:24">
-      <c r="A11" s="69" t="s">
+      <c r="A11" s="72" t="s">
         <v>169</v>
       </c>
-      <c r="B11" s="70"/>
-      <c r="C11" s="70"/>
-      <c r="D11" s="71"/>
+      <c r="B11" s="73"/>
+      <c r="C11" s="73"/>
+      <c r="D11" s="74"/>
     </row>
     <row r="12" spans="1:24">
       <c r="A12" s="37" t="s">
@@ -22762,12 +22765,12 @@
       </c>
     </row>
     <row r="24" spans="1:4">
-      <c r="A24" s="69" t="s">
+      <c r="A24" s="72" t="s">
         <v>168</v>
       </c>
-      <c r="B24" s="70"/>
-      <c r="C24" s="70"/>
-      <c r="D24" s="71"/>
+      <c r="B24" s="73"/>
+      <c r="C24" s="73"/>
+      <c r="D24" s="74"/>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="37" t="s">
@@ -22784,12 +22787,12 @@
       </c>
     </row>
     <row r="38" spans="1:4">
-      <c r="A38" s="69" t="s">
+      <c r="A38" s="72" t="s">
         <v>283</v>
       </c>
-      <c r="B38" s="70"/>
-      <c r="C38" s="70"/>
-      <c r="D38" s="71"/>
+      <c r="B38" s="73"/>
+      <c r="C38" s="73"/>
+      <c r="D38" s="74"/>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="37" t="s">
@@ -22806,12 +22809,12 @@
       </c>
     </row>
     <row r="54" spans="1:8">
-      <c r="A54" s="69" t="s">
+      <c r="A54" s="72" t="s">
         <v>256</v>
       </c>
-      <c r="B54" s="70"/>
-      <c r="C54" s="70"/>
-      <c r="D54" s="71"/>
+      <c r="B54" s="73"/>
+      <c r="C54" s="73"/>
+      <c r="D54" s="74"/>
     </row>
     <row r="55" spans="1:8">
       <c r="A55" s="44" t="s">
@@ -22832,12 +22835,12 @@
       <c r="H55" s="46"/>
     </row>
     <row r="67" spans="1:4">
-      <c r="A67" s="69" t="s">
+      <c r="A67" s="72" t="s">
         <v>163</v>
       </c>
-      <c r="B67" s="70"/>
-      <c r="C67" s="70"/>
-      <c r="D67" s="71"/>
+      <c r="B67" s="73"/>
+      <c r="C67" s="73"/>
+      <c r="D67" s="74"/>
     </row>
     <row r="68" spans="1:4">
       <c r="A68" s="37" t="s">
@@ -22854,12 +22857,12 @@
       </c>
     </row>
     <row r="89" spans="1:4">
-      <c r="A89" s="69" t="s">
+      <c r="A89" s="72" t="s">
         <v>176</v>
       </c>
-      <c r="B89" s="70"/>
-      <c r="C89" s="70"/>
-      <c r="D89" s="71"/>
+      <c r="B89" s="73"/>
+      <c r="C89" s="73"/>
+      <c r="D89" s="74"/>
     </row>
     <row r="90" spans="1:4">
       <c r="A90" s="37" t="s">
@@ -22876,12 +22879,12 @@
       </c>
     </row>
     <row r="105" spans="1:8">
-      <c r="A105" s="69" t="s">
+      <c r="A105" s="72" t="s">
         <v>260</v>
       </c>
-      <c r="B105" s="70"/>
-      <c r="C105" s="70"/>
-      <c r="D105" s="71"/>
+      <c r="B105" s="73"/>
+      <c r="C105" s="73"/>
+      <c r="D105" s="74"/>
     </row>
     <row r="106" spans="1:8" s="47" customFormat="1">
       <c r="A106" s="44" t="s">
@@ -22902,12 +22905,12 @@
       <c r="H106" s="46"/>
     </row>
     <row r="120" spans="1:4">
-      <c r="A120" s="74" t="s">
+      <c r="A120" s="69" t="s">
         <v>181</v>
       </c>
-      <c r="B120" s="75"/>
-      <c r="C120" s="75"/>
-      <c r="D120" s="76"/>
+      <c r="B120" s="70"/>
+      <c r="C120" s="70"/>
+      <c r="D120" s="71"/>
     </row>
     <row r="121" spans="1:4" ht="60">
       <c r="A121" s="37" t="s">
@@ -22918,13 +22921,13 @@
       </c>
     </row>
     <row r="142" spans="1:5">
-      <c r="A142" s="79" t="s">
+      <c r="A142" s="77" t="s">
         <v>287</v>
       </c>
-      <c r="B142" s="80"/>
-      <c r="C142" s="80"/>
-      <c r="D142" s="80"/>
-      <c r="E142" s="80"/>
+      <c r="B142" s="78"/>
+      <c r="C142" s="78"/>
+      <c r="D142" s="78"/>
+      <c r="E142" s="78"/>
     </row>
     <row r="143" spans="1:5">
       <c r="A143" s="51" t="s">
@@ -22961,105 +22964,105 @@
       </c>
     </row>
     <row r="167" spans="1:4">
-      <c r="A167" s="69" t="s">
+      <c r="A167" s="72" t="s">
         <v>330</v>
       </c>
-      <c r="B167" s="70"/>
-      <c r="C167" s="70"/>
-      <c r="D167" s="71"/>
+      <c r="B167" s="73"/>
+      <c r="C167" s="73"/>
+      <c r="D167" s="74"/>
     </row>
     <row r="168" spans="1:4">
       <c r="A168" s="37" t="s">
-        <v>164</v>
+        <v>346</v>
       </c>
       <c r="B168" s="43" t="s">
-        <v>331</v>
+        <v>347</v>
       </c>
       <c r="C168" s="43" t="s">
-        <v>332</v>
+        <v>348</v>
       </c>
       <c r="D168" s="43" t="s">
-        <v>333</v>
+        <v>349</v>
       </c>
     </row>
     <row r="190" spans="1:4">
-      <c r="A190" s="69" t="s">
-        <v>334</v>
-      </c>
-      <c r="B190" s="70"/>
-      <c r="C190" s="70"/>
-      <c r="D190" s="71"/>
+      <c r="A190" s="72" t="s">
+        <v>331</v>
+      </c>
+      <c r="B190" s="73"/>
+      <c r="C190" s="73"/>
+      <c r="D190" s="74"/>
     </row>
     <row r="191" spans="1:4">
       <c r="A191" s="37" t="s">
-        <v>164</v>
+        <v>346</v>
       </c>
       <c r="B191" s="43" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="C191" s="43" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="D191" s="43" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="220" spans="1:4">
-      <c r="A220" s="69" t="s">
-        <v>342</v>
-      </c>
-      <c r="B220" s="70"/>
-      <c r="C220" s="70"/>
-      <c r="D220" s="71"/>
+      <c r="A220" s="72" t="s">
+        <v>339</v>
+      </c>
+      <c r="B220" s="73"/>
+      <c r="C220" s="73"/>
+      <c r="D220" s="74"/>
     </row>
     <row r="221" spans="1:4">
       <c r="A221" s="37" t="s">
-        <v>164</v>
+        <v>346</v>
       </c>
       <c r="B221" s="43" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="C221" s="43" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="D221" s="43" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
     </row>
     <row r="250" spans="1:4">
-      <c r="A250" s="74" t="s">
-        <v>346</v>
-      </c>
-      <c r="B250" s="75"/>
-      <c r="C250" s="75"/>
-      <c r="D250" s="76"/>
+      <c r="A250" s="69" t="s">
+        <v>343</v>
+      </c>
+      <c r="B250" s="70"/>
+      <c r="C250" s="70"/>
+      <c r="D250" s="71"/>
     </row>
     <row r="251" spans="1:4">
       <c r="A251" s="51" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="B251" s="51" t="s">
         <v>328</v>
       </c>
       <c r="C251" s="59" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="D251" s="59" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
     </row>
     <row r="252" spans="1:4">
       <c r="A252" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="B252" s="58" t="s">
         <v>329</v>
       </c>
       <c r="C252" s="58" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="D252" s="58" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
     </row>
   </sheetData>
@@ -23113,20 +23116,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="79" t="s">
         <v>235</v>
       </c>
-      <c r="B1" s="78"/>
-      <c r="C1" s="78"/>
-      <c r="D1" s="78"/>
-      <c r="E1" s="78"/>
-      <c r="F1" s="78"/>
-      <c r="G1" s="78"/>
-      <c r="H1" s="78"/>
-      <c r="I1" s="78"/>
-      <c r="J1" s="78"/>
-      <c r="K1" s="78"/>
-      <c r="L1" s="78"/>
+      <c r="B1" s="80"/>
+      <c r="C1" s="80"/>
+      <c r="D1" s="80"/>
+      <c r="E1" s="80"/>
+      <c r="F1" s="80"/>
+      <c r="G1" s="80"/>
+      <c r="H1" s="80"/>
+      <c r="I1" s="80"/>
+      <c r="J1" s="80"/>
+      <c r="K1" s="80"/>
+      <c r="L1" s="80"/>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="39" t="s">

</xml_diff>

<commit_message>
POCOR-7421: code enhance for last year student all status related count | Status: Done
</commit_message>
<xml_diff>
--- a/webroot/export/customexcel/default_templates/profile_template.xlsx
+++ b/webroot/export/customexcel/default_templates/profile_template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10305" tabRatio="862" activeTab="7"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="7890" tabRatio="862" firstSheet="2" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="350">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="369">
   <si>
     <t>${"image":{"displayValue":"Institutions.logo_content","imageWidth":"100","imageMarginLeft":"20","imageMarginTop":"5"}}</t>
   </si>
@@ -1018,48 +1018,12 @@
     <t>Last Year Total Student Enrolment Rate</t>
   </si>
   <si>
-    <t>${"match": {"displayValue": "StudentFromEducationGrade.total_student_enrolment_last_year","rows": {"matchFrom": "StudentFromEducationGrade.education_grade_id","matchTo": "StudentFromEducationGrade.education_grade_id"}}}</t>
-  </si>
-  <si>
-    <t>Count of  Enrolled students Last Year</t>
-  </si>
-  <si>
-    <t>Count of  Promoted students Last Year</t>
-  </si>
-  <si>
-    <t xml:space="preserve">${"match": {"displayValue": "LasrYearInstitutionStudentPromoted.area_level:1","rows": {"matchFrom": "InstitutionEducationGrade.id","matchTo": "InstitutionEducationGrade.id"}}} </t>
-  </si>
-  <si>
-    <t xml:space="preserve">${"match": {"displayValue": "LasrYearInstitutionStudentPromoted.area_level:2","rows": {"matchFrom": "InstitutionEducationGrade.id","matchTo": "InstitutionEducationGrade.id"}}} </t>
-  </si>
-  <si>
-    <t xml:space="preserve">${"match": {"displayValue": "LasrYearInstitutionStudentPromoted.area_level:3","rows": {"matchFrom": "InstitutionEducationGrade.id","matchTo": "InstitutionEducationGrade.id"}}} </t>
-  </si>
-  <si>
     <t>Last Year Total Student Promoted Rate</t>
   </si>
   <si>
     <t>Last Year Total Student Withdrawn Rate</t>
   </si>
   <si>
-    <t>${"match": {"displayValue": "StudentFromEducationGrade.total_student_promoted_last_year","rows": {"matchFrom": "StudentFromEducationGrade.education_grade_id","matchTo": "StudentFromEducationGrade.education_grade_id"}}}</t>
-  </si>
-  <si>
-    <t>${"match": {"displayValue": "StudentFromEducationGrade.total_student_withdrawn_last_year","rows": {"matchFrom": "StudentFromEducationGrade.education_grade_id","matchTo": "StudentFromEducationGrade.education_grade_id"}}}</t>
-  </si>
-  <si>
-    <t>Count of  Withdrawn students Last Year</t>
-  </si>
-  <si>
-    <t xml:space="preserve">${"match": {"displayValue": "LasrYearInstitutionStudentWithdrawn.area_level:1","rows": {"matchFrom": "InstitutionEducationGrade.id","matchTo": "InstitutionEducationGrade.id"}}} </t>
-  </si>
-  <si>
-    <t xml:space="preserve">${"match": {"displayValue": "LasrYearInstitutionStudentWithdrawn.area_level:2","rows": {"matchFrom": "InstitutionEducationGrade.id","matchTo": "InstitutionEducationGrade.id"}}} </t>
-  </si>
-  <si>
-    <t xml:space="preserve">${"match": {"displayValue": "LasrYearInstitutionStudentWithdrawn.area_level:3","rows": {"matchFrom": "InstitutionEducationGrade.id","matchTo": "InstitutionEducationGrade.id"}}} </t>
-  </si>
-  <si>
     <t>Last Year Total Student Enrolled/Promoted/Withdrawn Rate</t>
   </si>
   <si>
@@ -1069,16 +1033,109 @@
     <t>${"match": {"displayValue": "LastYearEducationGrade.education_grade_name","rows": {"matchFrom": "StudentFromEducationGrade.education_grade_id","matchTo": "StudentFromEducationGrade.education_grade_id"}}}</t>
   </si>
   <si>
-    <t>${"match": {"displayValue": "LastYearInstitutionEducationGrade.name","rows": {"matchFrom": "LastYearInstitutionEducationGrade.id","matchTo": "LastYearInstitutionEducationGrade.id"}}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">${"match": {"displayValue": "LasrYearInstitutionStudentEnrolled.area_level:1","rows": {"matchFrom": "LastYearInstitutionEducationGrade.id","matchTo": "LastYearInstitutionEducationGrade.id"}}} </t>
-  </si>
-  <si>
-    <t xml:space="preserve">${"match": {"displayValue": "LasrYearInstitutionStudentEnrolled.area_level:2","rows": {"matchFrom": "LastYearInstitutionEducationGrade.id","matchTo": "LastYearInstitutionEducationGrade.id"}}} </t>
-  </si>
-  <si>
-    <t xml:space="preserve">${"match": {"displayValue": "LasrYearInstitutionStudentEnrolled.area_level:3","rows": {"matchFrom": "LastYearInstitutionEducationGrade.id","matchTo": "LastYearInstitutionEducationGrade.id"}}} </t>
+    <t>Count of  Enrolled students in the current school Last Year</t>
+  </si>
+  <si>
+    <t>${"match": {"displayValue": "LastYearInstitutionStudentEnrolled.education_grade_name","rows": {"matchFrom": "LastYearInstitutionStudentEnrolled.id","matchTo": "LastYearInstitutionStudentEnrolled.id"}}}</t>
+  </si>
+  <si>
+    <t>${"match": {"displayValue": "LastYearInstitutionStudentEnrolled.last_year_enrolled_students","rows": {"matchFrom": "LastYearInstitutionStudentEnrolled.id","matchTo": "LastYearInstitutionStudentEnrolled.id"}}}</t>
+  </si>
+  <si>
+    <t>Count of  Promoted students in the current school Last Year</t>
+  </si>
+  <si>
+    <t>${"match": {"displayValue": "LastYearInstitutionStudentPromoted.education_grade_name","rows": {"matchFrom": "LastYearInstitutionStudentPromoted.id","matchTo": "LastYearInstitutionStudentPromoted.id"}}}</t>
+  </si>
+  <si>
+    <t>${"match": {"displayValue": "LastYearInstitutionStudentPromoted.last_year_promoted_students","rows": {"matchFrom": "LastYearInstitutionStudentPromoted.id","matchTo": "LastYearInstitutionStudentPromoted.id"}}}</t>
+  </si>
+  <si>
+    <t>Count of  Withdrawn students in the current school Last Year</t>
+  </si>
+  <si>
+    <t>${"match": {"displayValue": "LastYearInstitutionStudentWithdrawn.education_grade_name","rows": {"matchFrom": "LastYearInstitutionStudentWithdrawn.id","matchTo": "LastYearInstitutionStudentWithdrawn.id"}}}</t>
+  </si>
+  <si>
+    <t>${"match": {"displayValue": "LastYearInstitutionStudentWithdrawn.last_year_withdrawn_students","rows": {"matchFrom": "LastYearInstitutionStudentWithdrawn.id","matchTo": "LastYearInstitutionStudentWithdrawn.id"}}}</t>
+  </si>
+  <si>
+    <t>Count of  Repeated students in the current school Last Year</t>
+  </si>
+  <si>
+    <t>${"match": {"displayValue": "LastYearInstitutionStudentRepeated.education_grade_name","rows": {"matchFrom": "LastYearInstitutionStudentRepeated.id","matchTo": "LastYearInstitutionStudentRepeated.id"}}}</t>
+  </si>
+  <si>
+    <t>${"match": {"displayValue": "LastYearInstitutionStudentRepeated.last_year_repeated_students","rows": {"matchFrom": "LastYearInstitutionStudentRepeated.id","matchTo": "LastYearInstitutionStudentRepeated.id"}}}</t>
+  </si>
+  <si>
+    <t>Count of  Enrolled students per Area Last Year</t>
+  </si>
+  <si>
+    <t>${"match": {"displayValue": "LastYearStudentEnrolledByArea.name","rows": {"matchFrom": "LastYearStudentEnrolledByArea.id","matchTo": "LastYearStudentEnrolledByArea.id"}}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${"match": {"displayValue": "LastYearStudentEnrolledByArea.area_level:1","rows": {"matchFrom": "LastYearStudentEnrolledByArea.id","matchTo": "LastYearStudentEnrolledByArea.id"}}} </t>
+  </si>
+  <si>
+    <t xml:space="preserve">${"match": {"displayValue": "LastYearStudentEnrolledByArea.area_level:2","rows": {"matchFrom": "LastYearStudentEnrolledByArea.id","matchTo": "LastYearStudentEnrolledByArea.id"}}} </t>
+  </si>
+  <si>
+    <t xml:space="preserve">${"match": {"displayValue": "LastYearStudentEnrolledByArea.area_level:3","rows": {"matchFrom": "LastYearStudentEnrolledByArea.id","matchTo": "LastYearStudentEnrolledByArea.id"}}} </t>
+  </si>
+  <si>
+    <t>${"match": {"displayValue": "LastYearStudentPromotedByArea.name","rows": {"matchFrom": "LastYearStudentPromotedByArea.id","matchTo": "LastYearStudentPromotedByArea.id"}}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${"match": {"displayValue": "LastYearStudentPromotedByArea.area_level:1","rows": {"matchFrom": "LastYearStudentPromotedByArea.id","matchTo": "LastYearStudentPromotedByArea.id"}}} </t>
+  </si>
+  <si>
+    <t xml:space="preserve">${"match": {"displayValue": "LastYearStudentPromotedByArea.area_level:2","rows": {"matchFrom": "LastYearStudentPromotedByArea.id","matchTo": "LastYearStudentPromotedByArea.id"}}} </t>
+  </si>
+  <si>
+    <t xml:space="preserve">${"match": {"displayValue": "LastYearStudentPromotedByArea.area_level:3","rows": {"matchFrom": "LastYearStudentPromotedByArea.id","matchTo": "LastYearStudentPromotedByArea.id"}}} </t>
+  </si>
+  <si>
+    <t>${"match": {"displayValue": "LastYearStudentWithdrawnByArea.name","rows": {"matchFrom": "LastYearStudentWithdrawnByArea.id","matchTo": "LastYearStudentWithdrawnByArea.id"}}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${"match": {"displayValue": "LastYearStudentWithdrawnByArea.area_level:1","rows": {"matchFrom": "LastYearStudentWithdrawnByArea.id","matchTo": "LastYearStudentWithdrawnByArea.id"}}} </t>
+  </si>
+  <si>
+    <t xml:space="preserve">${"match": {"displayValue": "LastYearStudentWithdrawnByArea.area_level:2","rows": {"matchFrom": "LastYearStudentWithdrawnByArea.id","matchTo": "LastYearStudentWithdrawnByArea.id"}}} </t>
+  </si>
+  <si>
+    <t xml:space="preserve">${"match": {"displayValue": "LastYearStudentWithdrawnByArea.area_level:3","rows": {"matchFrom": "LastYearStudentWithdrawnByArea.id","matchTo": "LastYearStudentWithdrawnByArea.id"}}} </t>
+  </si>
+  <si>
+    <t>Count of  Promoted students per Area Last Year</t>
+  </si>
+  <si>
+    <t>Count of  Withdrawn students per Area Last Year</t>
+  </si>
+  <si>
+    <t>Count of Repeated students per Area Last Year</t>
+  </si>
+  <si>
+    <t>${"match": {"displayValue": "LastYearStudentRepeatedByArea.name","rows": {"matchFrom": "LastYearStudentRepeatedByArea.id","matchTo": "LastYearStudentRepeatedByArea.id"}}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${"match": {"displayValue": "LastYearStudentRepeatedByArea.area_level:1","rows": {"matchFrom": "LastYearStudentRepeatedByArea.id","matchTo": "LastYearStudentRepeatedByArea.id"}}} </t>
+  </si>
+  <si>
+    <t xml:space="preserve">${"match": {"displayValue": "LastYearStudentRepeatedByArea.area_level:2","rows": {"matchFrom": "LastYearStudentRepeatedByArea.id","matchTo": "LastYearStudentRepeatedByArea.id"}}} </t>
+  </si>
+  <si>
+    <t xml:space="preserve">${"match": {"displayValue": "LastYearStudentRepeatedByArea.area_level:3","rows": {"matchFrom": "LastYearStudentRepeatedByArea.id","matchTo": "LastYearStudentRepeatedByArea.id"}}} </t>
+  </si>
+  <si>
+    <t>${"match": {"displayValue": "LastYearEducationGrade.total_student_enrolment_last_year","rows": {"matchFrom": "LastYearEducationGrade.education_grade_id","matchTo": "LastYearEducationGrade.education_grade_id"}}}</t>
+  </si>
+  <si>
+    <t>${"match": {"displayValue": "LastYearEducationGrade.total_student_promoted_last_year","rows": {"matchFrom": "LastYearEducationGrade.education_grade_id","matchTo": "LastYearEducationGrade.education_grade_id"}}}</t>
+  </si>
+  <si>
+    <t>${"match": {"displayValue": "LastYearEducationGrade.total_student_withdrawn_last_year","rows": {"matchFrom": "LastYearEducationGrade.education_grade_id","matchTo": "LastYearEducationGrade.education_grade_id"}}}</t>
   </si>
 </sst>
 </file>
@@ -1532,6 +1589,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1539,12 +1602,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -22549,10 +22606,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:X252"/>
+  <dimension ref="A1:X357"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="A67" sqref="A67:E68"/>
+    <sheetView tabSelected="1" topLeftCell="A244" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="D266" sqref="D266"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
@@ -22743,11 +22800,11 @@
       </c>
     </row>
     <row r="11" spans="1:24">
-      <c r="A11" s="72" t="s">
+      <c r="A11" s="69" t="s">
         <v>169</v>
       </c>
-      <c r="B11" s="73"/>
-      <c r="C11" s="73"/>
+      <c r="B11" s="70"/>
+      <c r="C11" s="70"/>
       <c r="D11" s="74"/>
     </row>
     <row r="12" spans="1:24">
@@ -22765,11 +22822,11 @@
       </c>
     </row>
     <row r="24" spans="1:4">
-      <c r="A24" s="72" t="s">
+      <c r="A24" s="69" t="s">
         <v>168</v>
       </c>
-      <c r="B24" s="73"/>
-      <c r="C24" s="73"/>
+      <c r="B24" s="70"/>
+      <c r="C24" s="70"/>
       <c r="D24" s="74"/>
     </row>
     <row r="25" spans="1:4">
@@ -22787,11 +22844,11 @@
       </c>
     </row>
     <row r="38" spans="1:4">
-      <c r="A38" s="72" t="s">
+      <c r="A38" s="69" t="s">
         <v>283</v>
       </c>
-      <c r="B38" s="73"/>
-      <c r="C38" s="73"/>
+      <c r="B38" s="70"/>
+      <c r="C38" s="70"/>
       <c r="D38" s="74"/>
     </row>
     <row r="39" spans="1:4">
@@ -22809,11 +22866,11 @@
       </c>
     </row>
     <row r="54" spans="1:8">
-      <c r="A54" s="72" t="s">
+      <c r="A54" s="69" t="s">
         <v>256</v>
       </c>
-      <c r="B54" s="73"/>
-      <c r="C54" s="73"/>
+      <c r="B54" s="70"/>
+      <c r="C54" s="70"/>
       <c r="D54" s="74"/>
     </row>
     <row r="55" spans="1:8">
@@ -22835,11 +22892,11 @@
       <c r="H55" s="46"/>
     </row>
     <row r="67" spans="1:4">
-      <c r="A67" s="72" t="s">
+      <c r="A67" s="69" t="s">
         <v>163</v>
       </c>
-      <c r="B67" s="73"/>
-      <c r="C67" s="73"/>
+      <c r="B67" s="70"/>
+      <c r="C67" s="70"/>
       <c r="D67" s="74"/>
     </row>
     <row r="68" spans="1:4">
@@ -22857,11 +22914,11 @@
       </c>
     </row>
     <row r="89" spans="1:4">
-      <c r="A89" s="72" t="s">
+      <c r="A89" s="69" t="s">
         <v>176</v>
       </c>
-      <c r="B89" s="73"/>
-      <c r="C89" s="73"/>
+      <c r="B89" s="70"/>
+      <c r="C89" s="70"/>
       <c r="D89" s="74"/>
     </row>
     <row r="90" spans="1:4">
@@ -22879,11 +22936,11 @@
       </c>
     </row>
     <row r="105" spans="1:8">
-      <c r="A105" s="72" t="s">
+      <c r="A105" s="69" t="s">
         <v>260</v>
       </c>
-      <c r="B105" s="73"/>
-      <c r="C105" s="73"/>
+      <c r="B105" s="70"/>
+      <c r="C105" s="70"/>
       <c r="D105" s="74"/>
     </row>
     <row r="106" spans="1:8" s="47" customFormat="1">
@@ -22905,12 +22962,12 @@
       <c r="H106" s="46"/>
     </row>
     <row r="120" spans="1:4">
-      <c r="A120" s="69" t="s">
+      <c r="A120" s="71" t="s">
         <v>181</v>
       </c>
-      <c r="B120" s="70"/>
-      <c r="C120" s="70"/>
-      <c r="D120" s="71"/>
+      <c r="B120" s="72"/>
+      <c r="C120" s="72"/>
+      <c r="D120" s="73"/>
     </row>
     <row r="121" spans="1:4" ht="60">
       <c r="A121" s="37" t="s">
@@ -22964,110 +23021,224 @@
       </c>
     </row>
     <row r="167" spans="1:4">
-      <c r="A167" s="72" t="s">
-        <v>330</v>
-      </c>
-      <c r="B167" s="73"/>
-      <c r="C167" s="73"/>
+      <c r="A167" s="69" t="s">
+        <v>346</v>
+      </c>
+      <c r="B167" s="70"/>
+      <c r="C167" s="70"/>
       <c r="D167" s="74"/>
     </row>
     <row r="168" spans="1:4">
       <c r="A168" s="37" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B168" s="43" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="C168" s="43" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="D168" s="43" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="190" spans="1:4">
-      <c r="A190" s="72" t="s">
-        <v>331</v>
-      </c>
-      <c r="B190" s="73"/>
-      <c r="C190" s="73"/>
+      <c r="A190" s="69" t="s">
+        <v>359</v>
+      </c>
+      <c r="B190" s="70"/>
+      <c r="C190" s="70"/>
       <c r="D190" s="74"/>
     </row>
     <row r="191" spans="1:4">
       <c r="A191" s="37" t="s">
-        <v>346</v>
+        <v>351</v>
       </c>
       <c r="B191" s="43" t="s">
-        <v>332</v>
+        <v>352</v>
       </c>
       <c r="C191" s="43" t="s">
-        <v>333</v>
+        <v>353</v>
       </c>
       <c r="D191" s="43" t="s">
-        <v>334</v>
+        <v>354</v>
       </c>
     </row>
     <row r="220" spans="1:4">
-      <c r="A220" s="72" t="s">
-        <v>339</v>
-      </c>
-      <c r="B220" s="73"/>
-      <c r="C220" s="73"/>
+      <c r="A220" s="69" t="s">
+        <v>360</v>
+      </c>
+      <c r="B220" s="70"/>
+      <c r="C220" s="70"/>
       <c r="D220" s="74"/>
     </row>
     <row r="221" spans="1:4">
       <c r="A221" s="37" t="s">
-        <v>346</v>
+        <v>355</v>
       </c>
       <c r="B221" s="43" t="s">
+        <v>356</v>
+      </c>
+      <c r="C221" s="43" t="s">
+        <v>357</v>
+      </c>
+      <c r="D221" s="43" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="239" spans="1:4">
+      <c r="A239" s="71" t="s">
+        <v>361</v>
+      </c>
+      <c r="B239" s="72"/>
+      <c r="C239" s="72"/>
+      <c r="D239" s="73"/>
+    </row>
+    <row r="240" spans="1:4">
+      <c r="A240" s="37" t="s">
+        <v>362</v>
+      </c>
+      <c r="B240" s="43" t="s">
+        <v>363</v>
+      </c>
+      <c r="C240" s="43" t="s">
+        <v>364</v>
+      </c>
+      <c r="D240" s="43" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="241" spans="2:4">
+      <c r="B241" s="58"/>
+      <c r="C241" s="58"/>
+      <c r="D241" s="58"/>
+    </row>
+    <row r="264" spans="1:4">
+      <c r="A264" s="71" t="s">
+        <v>331</v>
+      </c>
+      <c r="B264" s="72"/>
+      <c r="C264" s="72"/>
+      <c r="D264" s="73"/>
+    </row>
+    <row r="265" spans="1:4">
+      <c r="A265" s="51" t="s">
+        <v>332</v>
+      </c>
+      <c r="B265" s="51" t="s">
+        <v>328</v>
+      </c>
+      <c r="C265" s="59" t="s">
+        <v>329</v>
+      </c>
+      <c r="D265" s="59" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="266" spans="1:4">
+      <c r="A266" t="s">
+        <v>333</v>
+      </c>
+      <c r="B266" s="58" t="s">
+        <v>366</v>
+      </c>
+      <c r="C266" s="58" t="s">
+        <v>367</v>
+      </c>
+      <c r="D266" s="58" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="300" spans="1:2">
+      <c r="A300" s="69" t="s">
+        <v>334</v>
+      </c>
+      <c r="B300" s="70"/>
+    </row>
+    <row r="301" spans="1:2">
+      <c r="A301" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="B301" s="26" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="302" spans="1:2">
+      <c r="A302" s="37" t="s">
+        <v>335</v>
+      </c>
+      <c r="B302" s="43" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="320" spans="1:2">
+      <c r="A320" s="69" t="s">
+        <v>337</v>
+      </c>
+      <c r="B320" s="70"/>
+    </row>
+    <row r="321" spans="1:2">
+      <c r="A321" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="B321" s="26" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="322" spans="1:2">
+      <c r="A322" s="37" t="s">
+        <v>338</v>
+      </c>
+      <c r="B322" s="43" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="340" spans="1:2">
+      <c r="A340" s="69" t="s">
         <v>340</v>
       </c>
-      <c r="C221" s="43" t="s">
+      <c r="B340" s="70"/>
+    </row>
+    <row r="341" spans="1:2">
+      <c r="A341" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="B341" s="26" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="342" spans="1:2">
+      <c r="A342" s="37" t="s">
         <v>341</v>
       </c>
-      <c r="D221" s="43" t="s">
+      <c r="B342" s="43" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="250" spans="1:4">
-      <c r="A250" s="69" t="s">
+    <row r="355" spans="1:2">
+      <c r="A355" s="69" t="s">
         <v>343</v>
       </c>
-      <c r="B250" s="70"/>
-      <c r="C250" s="70"/>
-      <c r="D250" s="71"/>
+      <c r="B355" s="70"/>
     </row>
-    <row r="251" spans="1:4">
-      <c r="A251" s="51" t="s">
+    <row r="356" spans="1:2">
+      <c r="A356" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="B356" s="26" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="357" spans="1:2">
+      <c r="A357" s="37" t="s">
         <v>344</v>
       </c>
-      <c r="B251" s="51" t="s">
-        <v>328</v>
-      </c>
-      <c r="C251" s="59" t="s">
-        <v>335</v>
-      </c>
-      <c r="D251" s="59" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="252" spans="1:4">
-      <c r="A252" t="s">
+      <c r="B357" s="43" t="s">
         <v>345</v>
-      </c>
-      <c r="B252" s="58" t="s">
-        <v>329</v>
-      </c>
-      <c r="C252" s="58" t="s">
-        <v>337</v>
-      </c>
-      <c r="D252" s="58" t="s">
-        <v>338</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="14">
-    <mergeCell ref="A250:D250"/>
+  <mergeCells count="19">
     <mergeCell ref="A220:D220"/>
     <mergeCell ref="A167:D167"/>
     <mergeCell ref="A190:D190"/>
@@ -23081,6 +23252,12 @@
     <mergeCell ref="A24:D24"/>
     <mergeCell ref="A54:D54"/>
     <mergeCell ref="A67:D67"/>
+    <mergeCell ref="A300:B300"/>
+    <mergeCell ref="A320:B320"/>
+    <mergeCell ref="A340:B340"/>
+    <mergeCell ref="A355:B355"/>
+    <mergeCell ref="A239:D239"/>
+    <mergeCell ref="A264:D264"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
POCOR-7449: code enhance for correct result | Status: Done
</commit_message>
<xml_diff>
--- a/webroot/export/customexcel/default_templates/profile_template.xlsx
+++ b/webroot/export/customexcel/default_templates/profile_template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="7890" tabRatio="862" firstSheet="2" activeTab="7"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="7890" tabRatio="862"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -1594,6 +1594,15 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -1602,15 +1611,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1996,8 +1996,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:IV1048"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75"/>
@@ -11072,7 +11072,7 @@
         <v>321</v>
       </c>
       <c r="B43" s="56" t="s">
-        <v>48</v>
+        <v>325</v>
       </c>
       <c r="C43" s="16"/>
       <c r="D43" s="16"/>
@@ -11334,7 +11334,7 @@
         <v>322</v>
       </c>
       <c r="B44" s="56" t="s">
-        <v>325</v>
+        <v>48</v>
       </c>
       <c r="C44" s="16"/>
       <c r="D44" s="16"/>
@@ -22608,7 +22608,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:X357"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A244" zoomScalePageLayoutView="60" workbookViewId="0">
+    <sheetView topLeftCell="A244" zoomScalePageLayoutView="60" workbookViewId="0">
       <selection activeCell="D266" sqref="D266"/>
     </sheetView>
   </sheetViews>
@@ -22624,32 +22624,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24">
-      <c r="A1" s="75" t="s">
+      <c r="A1" s="72" t="s">
         <v>100</v>
       </c>
-      <c r="B1" s="76"/>
-      <c r="C1" s="76"/>
-      <c r="D1" s="76"/>
-      <c r="E1" s="76"/>
-      <c r="F1" s="76"/>
-      <c r="G1" s="76"/>
-      <c r="H1" s="76"/>
-      <c r="I1" s="76"/>
-      <c r="J1" s="76"/>
-      <c r="K1" s="76"/>
-      <c r="L1" s="76"/>
-      <c r="M1" s="76"/>
-      <c r="N1" s="76"/>
-      <c r="O1" s="76"/>
-      <c r="P1" s="76"/>
-      <c r="Q1" s="76"/>
-      <c r="R1" s="76"/>
-      <c r="S1" s="76"/>
-      <c r="T1" s="76"/>
-      <c r="U1" s="76"/>
-      <c r="V1" s="76"/>
-      <c r="W1" s="76"/>
-      <c r="X1" s="76"/>
+      <c r="B1" s="73"/>
+      <c r="C1" s="73"/>
+      <c r="D1" s="73"/>
+      <c r="E1" s="73"/>
+      <c r="F1" s="73"/>
+      <c r="G1" s="73"/>
+      <c r="H1" s="73"/>
+      <c r="I1" s="73"/>
+      <c r="J1" s="73"/>
+      <c r="K1" s="73"/>
+      <c r="L1" s="73"/>
+      <c r="M1" s="73"/>
+      <c r="N1" s="73"/>
+      <c r="O1" s="73"/>
+      <c r="P1" s="73"/>
+      <c r="Q1" s="73"/>
+      <c r="R1" s="73"/>
+      <c r="S1" s="73"/>
+      <c r="T1" s="73"/>
+      <c r="U1" s="73"/>
+      <c r="V1" s="73"/>
+      <c r="W1" s="73"/>
+      <c r="X1" s="73"/>
     </row>
     <row r="2" spans="1:24">
       <c r="A2" s="26" t="s">
@@ -22805,7 +22805,7 @@
       </c>
       <c r="B11" s="70"/>
       <c r="C11" s="70"/>
-      <c r="D11" s="74"/>
+      <c r="D11" s="71"/>
     </row>
     <row r="12" spans="1:24">
       <c r="A12" s="37" t="s">
@@ -22827,7 +22827,7 @@
       </c>
       <c r="B24" s="70"/>
       <c r="C24" s="70"/>
-      <c r="D24" s="74"/>
+      <c r="D24" s="71"/>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="37" t="s">
@@ -22849,7 +22849,7 @@
       </c>
       <c r="B38" s="70"/>
       <c r="C38" s="70"/>
-      <c r="D38" s="74"/>
+      <c r="D38" s="71"/>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="37" t="s">
@@ -22871,7 +22871,7 @@
       </c>
       <c r="B54" s="70"/>
       <c r="C54" s="70"/>
-      <c r="D54" s="74"/>
+      <c r="D54" s="71"/>
     </row>
     <row r="55" spans="1:8">
       <c r="A55" s="44" t="s">
@@ -22897,7 +22897,7 @@
       </c>
       <c r="B67" s="70"/>
       <c r="C67" s="70"/>
-      <c r="D67" s="74"/>
+      <c r="D67" s="71"/>
     </row>
     <row r="68" spans="1:4">
       <c r="A68" s="37" t="s">
@@ -22919,7 +22919,7 @@
       </c>
       <c r="B89" s="70"/>
       <c r="C89" s="70"/>
-      <c r="D89" s="74"/>
+      <c r="D89" s="71"/>
     </row>
     <row r="90" spans="1:4">
       <c r="A90" s="37" t="s">
@@ -22941,7 +22941,7 @@
       </c>
       <c r="B105" s="70"/>
       <c r="C105" s="70"/>
-      <c r="D105" s="74"/>
+      <c r="D105" s="71"/>
     </row>
     <row r="106" spans="1:8" s="47" customFormat="1">
       <c r="A106" s="44" t="s">
@@ -22962,12 +22962,12 @@
       <c r="H106" s="46"/>
     </row>
     <row r="120" spans="1:4">
-      <c r="A120" s="71" t="s">
+      <c r="A120" s="74" t="s">
         <v>181</v>
       </c>
-      <c r="B120" s="72"/>
-      <c r="C120" s="72"/>
-      <c r="D120" s="73"/>
+      <c r="B120" s="75"/>
+      <c r="C120" s="75"/>
+      <c r="D120" s="76"/>
     </row>
     <row r="121" spans="1:4" ht="60">
       <c r="A121" s="37" t="s">
@@ -23026,7 +23026,7 @@
       </c>
       <c r="B167" s="70"/>
       <c r="C167" s="70"/>
-      <c r="D167" s="74"/>
+      <c r="D167" s="71"/>
     </row>
     <row r="168" spans="1:4">
       <c r="A168" s="37" t="s">
@@ -23048,7 +23048,7 @@
       </c>
       <c r="B190" s="70"/>
       <c r="C190" s="70"/>
-      <c r="D190" s="74"/>
+      <c r="D190" s="71"/>
     </row>
     <row r="191" spans="1:4">
       <c r="A191" s="37" t="s">
@@ -23070,7 +23070,7 @@
       </c>
       <c r="B220" s="70"/>
       <c r="C220" s="70"/>
-      <c r="D220" s="74"/>
+      <c r="D220" s="71"/>
     </row>
     <row r="221" spans="1:4">
       <c r="A221" s="37" t="s">
@@ -23087,12 +23087,12 @@
       </c>
     </row>
     <row r="239" spans="1:4">
-      <c r="A239" s="71" t="s">
+      <c r="A239" s="74" t="s">
         <v>361</v>
       </c>
-      <c r="B239" s="72"/>
-      <c r="C239" s="72"/>
-      <c r="D239" s="73"/>
+      <c r="B239" s="75"/>
+      <c r="C239" s="75"/>
+      <c r="D239" s="76"/>
     </row>
     <row r="240" spans="1:4">
       <c r="A240" s="37" t="s">
@@ -23114,12 +23114,12 @@
       <c r="D241" s="58"/>
     </row>
     <row r="264" spans="1:4">
-      <c r="A264" s="71" t="s">
+      <c r="A264" s="74" t="s">
         <v>331</v>
       </c>
-      <c r="B264" s="72"/>
-      <c r="C264" s="72"/>
-      <c r="D264" s="73"/>
+      <c r="B264" s="75"/>
+      <c r="C264" s="75"/>
+      <c r="D264" s="76"/>
     </row>
     <row r="265" spans="1:4">
       <c r="A265" s="51" t="s">
@@ -23239,6 +23239,12 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="A300:B300"/>
+    <mergeCell ref="A320:B320"/>
+    <mergeCell ref="A340:B340"/>
+    <mergeCell ref="A355:B355"/>
+    <mergeCell ref="A239:D239"/>
+    <mergeCell ref="A264:D264"/>
     <mergeCell ref="A220:D220"/>
     <mergeCell ref="A167:D167"/>
     <mergeCell ref="A190:D190"/>
@@ -23252,12 +23258,6 @@
     <mergeCell ref="A24:D24"/>
     <mergeCell ref="A54:D54"/>
     <mergeCell ref="A67:D67"/>
-    <mergeCell ref="A300:B300"/>
-    <mergeCell ref="A320:B320"/>
-    <mergeCell ref="A340:B340"/>
-    <mergeCell ref="A355:B355"/>
-    <mergeCell ref="A239:D239"/>
-    <mergeCell ref="A264:D264"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
POCOR-7449: code enhance add new placeholders | Status: In review
</commit_message>
<xml_diff>
--- a/webroot/export/customexcel/default_templates/profile_template.xlsx
+++ b/webroot/export/customexcel/default_templates/profile_template.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="369">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="373">
   <si>
     <t>${"image":{"displayValue":"Institutions.logo_content","imageWidth":"100","imageMarginLeft":"20","imageMarginTop":"5"}}</t>
   </si>
@@ -1136,6 +1136,18 @@
   </si>
   <si>
     <t>${"match": {"displayValue": "LastYearEducationGrade.total_student_withdrawn_last_year","rows": {"matchFrom": "LastYearEducationGrade.education_grade_id","matchTo": "LastYearEducationGrade.education_grade_id"}}}</t>
+  </si>
+  <si>
+    <t>Area Teaching Staff Absence Days</t>
+  </si>
+  <si>
+    <t>${AreaTeachingStaffTotalAbsenceDays}</t>
+  </si>
+  <si>
+    <t>School Teaching Staff Absence Days</t>
+  </si>
+  <si>
+    <t>${TeachingStaffTotalAbsences}</t>
   </si>
 </sst>
 </file>
@@ -1430,7 +1442,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1550,8 +1562,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1594,6 +1604,15 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1602,15 +1621,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1994,10 +2004,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:IV1048"/>
+  <dimension ref="A1:IV1050"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75"/>
@@ -2018,7 +2028,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:256" ht="15" customHeight="1">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="59" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2"/>
@@ -2039,13 +2049,13 @@
       <c r="Q1" s="5"/>
     </row>
     <row r="2" spans="1:256" ht="25.5" customHeight="1">
-      <c r="A2" s="61"/>
-      <c r="B2" s="62" t="s">
+      <c r="A2" s="59"/>
+      <c r="B2" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="62"/>
-      <c r="D2" s="62"/>
-      <c r="E2" s="62"/>
+      <c r="C2" s="60"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
       <c r="F2" s="6"/>
       <c r="G2" s="7"/>
       <c r="H2" s="5"/>
@@ -2299,13 +2309,13 @@
       <c r="IV2" s="1"/>
     </row>
     <row r="3" spans="1:256" ht="25.5" customHeight="1">
-      <c r="A3" s="61"/>
-      <c r="B3" s="63" t="s">
+      <c r="A3" s="59"/>
+      <c r="B3" s="61" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="63"/>
-      <c r="D3" s="63"/>
-      <c r="E3" s="63"/>
+      <c r="C3" s="61"/>
+      <c r="D3" s="61"/>
+      <c r="E3" s="61"/>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
       <c r="H3" s="5"/>
@@ -2559,7 +2569,7 @@
       <c r="IV3" s="1"/>
     </row>
     <row r="4" spans="1:256" ht="22.5" customHeight="1">
-      <c r="A4" s="61"/>
+      <c r="A4" s="59"/>
       <c r="B4" s="2"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
@@ -6898,11 +6908,11 @@
       <c r="IV26" s="1"/>
     </row>
     <row r="27" spans="1:256" ht="12" customHeight="1">
-      <c r="A27" s="65" t="s">
+      <c r="A27" s="63" t="s">
         <v>30</v>
       </c>
-      <c r="B27" s="66"/>
-      <c r="C27" s="66"/>
+      <c r="B27" s="64"/>
+      <c r="C27" s="64"/>
       <c r="D27" s="16"/>
       <c r="E27" s="12"/>
       <c r="F27" s="12"/>
@@ -10544,10 +10554,10 @@
       <c r="IV40" s="1"/>
     </row>
     <row r="41" spans="1:256" ht="12" customHeight="1">
-      <c r="A41" s="57" t="s">
+      <c r="A41" s="55" t="s">
         <v>45</v>
       </c>
-      <c r="B41" s="56" t="s">
+      <c r="B41" s="19" t="s">
         <v>46</v>
       </c>
       <c r="C41" s="16"/>
@@ -10806,10 +10816,10 @@
       <c r="IV41" s="1"/>
     </row>
     <row r="42" spans="1:256" ht="12" customHeight="1">
-      <c r="A42" s="57" t="s">
+      <c r="A42" s="55" t="s">
         <v>47</v>
       </c>
-      <c r="B42" s="56" t="s">
+      <c r="B42" s="19" t="s">
         <v>48</v>
       </c>
       <c r="C42" s="16"/>
@@ -11068,10 +11078,10 @@
       <c r="IV42" s="1"/>
     </row>
     <row r="43" spans="1:256" ht="12" customHeight="1">
-      <c r="A43" s="57" t="s">
+      <c r="A43" s="55" t="s">
         <v>321</v>
       </c>
-      <c r="B43" s="56" t="s">
+      <c r="B43" s="19" t="s">
         <v>325</v>
       </c>
       <c r="C43" s="16"/>
@@ -11330,10 +11340,10 @@
       <c r="IV43" s="1"/>
     </row>
     <row r="44" spans="1:256" ht="12" customHeight="1">
-      <c r="A44" s="57" t="s">
+      <c r="A44" s="55" t="s">
         <v>322</v>
       </c>
-      <c r="B44" s="56" t="s">
+      <c r="B44" s="19" t="s">
         <v>48</v>
       </c>
       <c r="C44" s="16"/>
@@ -11592,11 +11602,11 @@
       <c r="IV44" s="1"/>
     </row>
     <row r="45" spans="1:256" ht="12" customHeight="1">
-      <c r="A45" s="57" t="s">
-        <v>323</v>
-      </c>
-      <c r="B45" s="56" t="s">
-        <v>326</v>
+      <c r="A45" s="55" t="s">
+        <v>371</v>
+      </c>
+      <c r="B45" s="19" t="s">
+        <v>372</v>
       </c>
       <c r="C45" s="16"/>
       <c r="D45" s="16"/>
@@ -11854,11 +11864,11 @@
       <c r="IV45" s="1"/>
     </row>
     <row r="46" spans="1:256" ht="12" customHeight="1">
-      <c r="A46" s="57" t="s">
-        <v>324</v>
-      </c>
-      <c r="B46" s="55" t="s">
-        <v>327</v>
+      <c r="A46" s="55" t="s">
+        <v>323</v>
+      </c>
+      <c r="B46" s="19" t="s">
+        <v>326</v>
       </c>
       <c r="C46" s="16"/>
       <c r="D46" s="16"/>
@@ -12116,8 +12126,12 @@
       <c r="IV46" s="1"/>
     </row>
     <row r="47" spans="1:256" ht="12" customHeight="1">
-      <c r="A47" s="15"/>
-      <c r="B47" s="16"/>
+      <c r="A47" s="55" t="s">
+        <v>324</v>
+      </c>
+      <c r="B47" s="19" t="s">
+        <v>327</v>
+      </c>
       <c r="C47" s="16"/>
       <c r="D47" s="16"/>
       <c r="E47" s="12"/>
@@ -12374,8 +12388,12 @@
       <c r="IV47" s="1"/>
     </row>
     <row r="48" spans="1:256" ht="12" customHeight="1">
-      <c r="A48" s="15"/>
-      <c r="B48" s="16"/>
+      <c r="A48" s="55" t="s">
+        <v>369</v>
+      </c>
+      <c r="B48" s="19" t="s">
+        <v>370</v>
+      </c>
       <c r="C48" s="16"/>
       <c r="D48" s="16"/>
       <c r="E48" s="12"/>
@@ -12632,12 +12650,8 @@
       <c r="IV48" s="1"/>
     </row>
     <row r="49" spans="1:256" ht="12" customHeight="1">
-      <c r="A49" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="B49" s="19" t="s">
-        <v>50</v>
-      </c>
+      <c r="A49" s="15"/>
+      <c r="B49" s="16"/>
       <c r="C49" s="16"/>
       <c r="D49" s="16"/>
       <c r="E49" s="12"/>
@@ -12894,12 +12908,8 @@
       <c r="IV49" s="1"/>
     </row>
     <row r="50" spans="1:256" ht="12" customHeight="1">
-      <c r="A50" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="B50" s="19" t="s">
-        <v>52</v>
-      </c>
+      <c r="A50" s="15"/>
+      <c r="B50" s="16"/>
       <c r="C50" s="16"/>
       <c r="D50" s="16"/>
       <c r="E50" s="12"/>
@@ -13157,10 +13167,10 @@
     </row>
     <row r="51" spans="1:256" ht="12" customHeight="1">
       <c r="A51" s="9" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B51" s="19" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C51" s="16"/>
       <c r="D51" s="16"/>
@@ -13419,10 +13429,10 @@
     </row>
     <row r="52" spans="1:256" ht="12" customHeight="1">
       <c r="A52" s="9" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B52" s="19" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C52" s="16"/>
       <c r="D52" s="16"/>
@@ -13681,10 +13691,10 @@
     </row>
     <row r="53" spans="1:256" ht="12" customHeight="1">
       <c r="A53" s="9" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B53" s="19" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C53" s="16"/>
       <c r="D53" s="16"/>
@@ -13943,10 +13953,10 @@
     </row>
     <row r="54" spans="1:256" ht="12" customHeight="1">
       <c r="A54" s="9" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B54" s="19" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C54" s="16"/>
       <c r="D54" s="16"/>
@@ -14205,10 +14215,10 @@
     </row>
     <row r="55" spans="1:256" ht="12" customHeight="1">
       <c r="A55" s="9" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B55" s="19" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C55" s="16"/>
       <c r="D55" s="16"/>
@@ -14467,9 +14477,11 @@
     </row>
     <row r="56" spans="1:256" ht="12" customHeight="1">
       <c r="A56" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="B56" s="19"/>
+        <v>59</v>
+      </c>
+      <c r="B56" s="19" t="s">
+        <v>60</v>
+      </c>
       <c r="C56" s="16"/>
       <c r="D56" s="16"/>
       <c r="E56" s="12"/>
@@ -14727,10 +14739,10 @@
     </row>
     <row r="57" spans="1:256" ht="12" customHeight="1">
       <c r="A57" s="9" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B57" s="19" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C57" s="16"/>
       <c r="D57" s="16"/>
@@ -14989,11 +15001,9 @@
     </row>
     <row r="58" spans="1:256" ht="12" customHeight="1">
       <c r="A58" s="9" t="s">
-        <v>297</v>
-      </c>
-      <c r="B58" s="19" t="s">
-        <v>298</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="B58" s="19"/>
       <c r="C58" s="16"/>
       <c r="D58" s="16"/>
       <c r="E58" s="12"/>
@@ -15251,544 +15261,544 @@
     </row>
     <row r="59" spans="1:256" ht="12" customHeight="1">
       <c r="A59" s="9" t="s">
-        <v>317</v>
+        <v>64</v>
       </c>
       <c r="B59" s="19" t="s">
-        <v>319</v>
-      </c>
-      <c r="D59"/>
+        <v>65</v>
+      </c>
+      <c r="C59" s="16"/>
+      <c r="D59" s="16"/>
+      <c r="E59" s="12"/>
+      <c r="F59" s="12"/>
+      <c r="G59" s="12"/>
+      <c r="H59" s="12"/>
+      <c r="I59" s="5"/>
+      <c r="J59" s="5"/>
+      <c r="K59" s="5"/>
+      <c r="L59" s="5"/>
+      <c r="M59" s="5"/>
+      <c r="N59" s="5"/>
+      <c r="O59" s="5"/>
+      <c r="P59" s="5"/>
+      <c r="Q59" s="5"/>
+      <c r="R59" s="5"/>
+      <c r="S59" s="1"/>
+      <c r="T59" s="1"/>
+      <c r="U59" s="1"/>
+      <c r="V59" s="1"/>
+      <c r="W59" s="1"/>
+      <c r="X59" s="1"/>
+      <c r="Y59" s="1"/>
+      <c r="Z59" s="1"/>
+      <c r="AA59" s="1"/>
+      <c r="AB59" s="1"/>
+      <c r="AC59" s="1"/>
+      <c r="AD59" s="1"/>
+      <c r="AE59" s="1"/>
+      <c r="AF59" s="1"/>
+      <c r="AG59" s="1"/>
+      <c r="AH59" s="1"/>
+      <c r="AI59" s="1"/>
+      <c r="AJ59" s="1"/>
+      <c r="AK59" s="1"/>
+      <c r="AL59" s="1"/>
+      <c r="AM59" s="1"/>
+      <c r="AN59" s="1"/>
+      <c r="AO59" s="1"/>
+      <c r="AP59" s="1"/>
+      <c r="AQ59" s="1"/>
+      <c r="AR59" s="1"/>
+      <c r="AS59" s="1"/>
+      <c r="AT59" s="1"/>
+      <c r="AU59" s="1"/>
+      <c r="AV59" s="1"/>
+      <c r="AW59" s="1"/>
+      <c r="AX59" s="1"/>
+      <c r="AY59" s="1"/>
+      <c r="AZ59" s="1"/>
+      <c r="BA59" s="1"/>
+      <c r="BB59" s="1"/>
+      <c r="BC59" s="1"/>
+      <c r="BD59" s="1"/>
+      <c r="BE59" s="1"/>
+      <c r="BF59" s="1"/>
+      <c r="BG59" s="1"/>
+      <c r="BH59" s="1"/>
+      <c r="BI59" s="1"/>
+      <c r="BJ59" s="1"/>
+      <c r="BK59" s="1"/>
+      <c r="BL59" s="1"/>
+      <c r="BM59" s="1"/>
+      <c r="BN59" s="1"/>
+      <c r="BO59" s="1"/>
+      <c r="BP59" s="1"/>
+      <c r="BQ59" s="1"/>
+      <c r="BR59" s="1"/>
+      <c r="BS59" s="1"/>
+      <c r="BT59" s="1"/>
+      <c r="BU59" s="1"/>
+      <c r="BV59" s="1"/>
+      <c r="BW59" s="1"/>
+      <c r="BX59" s="1"/>
+      <c r="BY59" s="1"/>
+      <c r="BZ59" s="1"/>
+      <c r="CA59" s="1"/>
+      <c r="CB59" s="1"/>
+      <c r="CC59" s="1"/>
+      <c r="CD59" s="1"/>
+      <c r="CE59" s="1"/>
+      <c r="CF59" s="1"/>
+      <c r="CG59" s="1"/>
+      <c r="CH59" s="1"/>
+      <c r="CI59" s="1"/>
+      <c r="CJ59" s="1"/>
+      <c r="CK59" s="1"/>
+      <c r="CL59" s="1"/>
+      <c r="CM59" s="1"/>
+      <c r="CN59" s="1"/>
+      <c r="CO59" s="1"/>
+      <c r="CP59" s="1"/>
+      <c r="CQ59" s="1"/>
+      <c r="CR59" s="1"/>
+      <c r="CS59" s="1"/>
+      <c r="CT59" s="1"/>
+      <c r="CU59" s="1"/>
+      <c r="CV59" s="1"/>
+      <c r="CW59" s="1"/>
+      <c r="CX59" s="1"/>
+      <c r="CY59" s="1"/>
+      <c r="CZ59" s="1"/>
+      <c r="DA59" s="1"/>
+      <c r="DB59" s="1"/>
+      <c r="DC59" s="1"/>
+      <c r="DD59" s="1"/>
+      <c r="DE59" s="1"/>
+      <c r="DF59" s="1"/>
+      <c r="DG59" s="1"/>
+      <c r="DH59" s="1"/>
+      <c r="DI59" s="1"/>
+      <c r="DJ59" s="1"/>
+      <c r="DK59" s="1"/>
+      <c r="DL59" s="1"/>
+      <c r="DM59" s="1"/>
+      <c r="DN59" s="1"/>
+      <c r="DO59" s="1"/>
+      <c r="DP59" s="1"/>
+      <c r="DQ59" s="1"/>
+      <c r="DR59" s="1"/>
+      <c r="DS59" s="1"/>
+      <c r="DT59" s="1"/>
+      <c r="DU59" s="1"/>
+      <c r="DV59" s="1"/>
+      <c r="DW59" s="1"/>
+      <c r="DX59" s="1"/>
+      <c r="DY59" s="1"/>
+      <c r="DZ59" s="1"/>
+      <c r="EA59" s="1"/>
+      <c r="EB59" s="1"/>
+      <c r="EC59" s="1"/>
+      <c r="ED59" s="1"/>
+      <c r="EE59" s="1"/>
+      <c r="EF59" s="1"/>
+      <c r="EG59" s="1"/>
+      <c r="EH59" s="1"/>
+      <c r="EI59" s="1"/>
+      <c r="EJ59" s="1"/>
+      <c r="EK59" s="1"/>
+      <c r="EL59" s="1"/>
+      <c r="EM59" s="1"/>
+      <c r="EN59" s="1"/>
+      <c r="EO59" s="1"/>
+      <c r="EP59" s="1"/>
+      <c r="EQ59" s="1"/>
+      <c r="ER59" s="1"/>
+      <c r="ES59" s="1"/>
+      <c r="ET59" s="1"/>
+      <c r="EU59" s="1"/>
+      <c r="EV59" s="1"/>
+      <c r="EW59" s="1"/>
+      <c r="EX59" s="1"/>
+      <c r="EY59" s="1"/>
+      <c r="EZ59" s="1"/>
+      <c r="FA59" s="1"/>
+      <c r="FB59" s="1"/>
+      <c r="FC59" s="1"/>
+      <c r="FD59" s="1"/>
+      <c r="FE59" s="1"/>
+      <c r="FF59" s="1"/>
+      <c r="FG59" s="1"/>
+      <c r="FH59" s="1"/>
+      <c r="FI59" s="1"/>
+      <c r="FJ59" s="1"/>
+      <c r="FK59" s="1"/>
+      <c r="FL59" s="1"/>
+      <c r="FM59" s="1"/>
+      <c r="FN59" s="1"/>
+      <c r="FO59" s="1"/>
+      <c r="FP59" s="1"/>
+      <c r="FQ59" s="1"/>
+      <c r="FR59" s="1"/>
+      <c r="FS59" s="1"/>
+      <c r="FT59" s="1"/>
+      <c r="FU59" s="1"/>
+      <c r="FV59" s="1"/>
+      <c r="FW59" s="1"/>
+      <c r="FX59" s="1"/>
+      <c r="FY59" s="1"/>
+      <c r="FZ59" s="1"/>
+      <c r="GA59" s="1"/>
+      <c r="GB59" s="1"/>
+      <c r="GC59" s="1"/>
+      <c r="GD59" s="1"/>
+      <c r="GE59" s="1"/>
+      <c r="GF59" s="1"/>
+      <c r="GG59" s="1"/>
+      <c r="GH59" s="1"/>
+      <c r="GI59" s="1"/>
+      <c r="GJ59" s="1"/>
+      <c r="GK59" s="1"/>
+      <c r="GL59" s="1"/>
+      <c r="GM59" s="1"/>
+      <c r="GN59" s="1"/>
+      <c r="GO59" s="1"/>
+      <c r="GP59" s="1"/>
+      <c r="GQ59" s="1"/>
+      <c r="GR59" s="1"/>
+      <c r="GS59" s="1"/>
+      <c r="GT59" s="1"/>
+      <c r="GU59" s="1"/>
+      <c r="GV59" s="1"/>
+      <c r="GW59" s="1"/>
+      <c r="GX59" s="1"/>
+      <c r="GY59" s="1"/>
+      <c r="GZ59" s="1"/>
+      <c r="HA59" s="1"/>
+      <c r="HB59" s="1"/>
+      <c r="HC59" s="1"/>
+      <c r="HD59" s="1"/>
+      <c r="HE59" s="1"/>
+      <c r="HF59" s="1"/>
+      <c r="HG59" s="1"/>
+      <c r="HH59" s="1"/>
+      <c r="HI59" s="1"/>
+      <c r="HJ59" s="1"/>
+      <c r="HK59" s="1"/>
+      <c r="HL59" s="1"/>
+      <c r="HM59" s="1"/>
+      <c r="HN59" s="1"/>
+      <c r="HO59" s="1"/>
+      <c r="HP59" s="1"/>
+      <c r="HQ59" s="1"/>
+      <c r="HR59" s="1"/>
+      <c r="HS59" s="1"/>
+      <c r="HT59" s="1"/>
+      <c r="HU59" s="1"/>
+      <c r="HV59" s="1"/>
+      <c r="HW59" s="1"/>
+      <c r="HX59" s="1"/>
+      <c r="HY59" s="1"/>
+      <c r="HZ59" s="1"/>
+      <c r="IA59" s="1"/>
+      <c r="IB59" s="1"/>
+      <c r="IC59" s="1"/>
+      <c r="ID59" s="1"/>
+      <c r="IE59" s="1"/>
+      <c r="IF59" s="1"/>
+      <c r="IG59" s="1"/>
+      <c r="IH59" s="1"/>
+      <c r="II59" s="1"/>
+      <c r="IJ59" s="1"/>
+      <c r="IK59" s="1"/>
+      <c r="IL59" s="1"/>
+      <c r="IM59" s="1"/>
+      <c r="IN59" s="1"/>
+      <c r="IO59" s="1"/>
+      <c r="IP59" s="1"/>
+      <c r="IQ59" s="1"/>
+      <c r="IR59" s="1"/>
+      <c r="IS59" s="1"/>
+      <c r="IT59" s="1"/>
+      <c r="IU59" s="1"/>
+      <c r="IV59" s="1"/>
     </row>
     <row r="60" spans="1:256" ht="12" customHeight="1">
-      <c r="D60"/>
+      <c r="A60" s="9" t="s">
+        <v>297</v>
+      </c>
+      <c r="B60" s="19" t="s">
+        <v>298</v>
+      </c>
+      <c r="C60" s="16"/>
+      <c r="D60" s="16"/>
+      <c r="E60" s="12"/>
+      <c r="F60" s="12"/>
+      <c r="G60" s="12"/>
+      <c r="H60" s="12"/>
+      <c r="I60" s="5"/>
+      <c r="J60" s="5"/>
+      <c r="K60" s="5"/>
+      <c r="L60" s="5"/>
+      <c r="M60" s="5"/>
+      <c r="N60" s="5"/>
+      <c r="O60" s="5"/>
+      <c r="P60" s="5"/>
+      <c r="Q60" s="5"/>
+      <c r="R60" s="5"/>
+      <c r="S60" s="1"/>
+      <c r="T60" s="1"/>
+      <c r="U60" s="1"/>
+      <c r="V60" s="1"/>
+      <c r="W60" s="1"/>
+      <c r="X60" s="1"/>
+      <c r="Y60" s="1"/>
+      <c r="Z60" s="1"/>
+      <c r="AA60" s="1"/>
+      <c r="AB60" s="1"/>
+      <c r="AC60" s="1"/>
+      <c r="AD60" s="1"/>
+      <c r="AE60" s="1"/>
+      <c r="AF60" s="1"/>
+      <c r="AG60" s="1"/>
+      <c r="AH60" s="1"/>
+      <c r="AI60" s="1"/>
+      <c r="AJ60" s="1"/>
+      <c r="AK60" s="1"/>
+      <c r="AL60" s="1"/>
+      <c r="AM60" s="1"/>
+      <c r="AN60" s="1"/>
+      <c r="AO60" s="1"/>
+      <c r="AP60" s="1"/>
+      <c r="AQ60" s="1"/>
+      <c r="AR60" s="1"/>
+      <c r="AS60" s="1"/>
+      <c r="AT60" s="1"/>
+      <c r="AU60" s="1"/>
+      <c r="AV60" s="1"/>
+      <c r="AW60" s="1"/>
+      <c r="AX60" s="1"/>
+      <c r="AY60" s="1"/>
+      <c r="AZ60" s="1"/>
+      <c r="BA60" s="1"/>
+      <c r="BB60" s="1"/>
+      <c r="BC60" s="1"/>
+      <c r="BD60" s="1"/>
+      <c r="BE60" s="1"/>
+      <c r="BF60" s="1"/>
+      <c r="BG60" s="1"/>
+      <c r="BH60" s="1"/>
+      <c r="BI60" s="1"/>
+      <c r="BJ60" s="1"/>
+      <c r="BK60" s="1"/>
+      <c r="BL60" s="1"/>
+      <c r="BM60" s="1"/>
+      <c r="BN60" s="1"/>
+      <c r="BO60" s="1"/>
+      <c r="BP60" s="1"/>
+      <c r="BQ60" s="1"/>
+      <c r="BR60" s="1"/>
+      <c r="BS60" s="1"/>
+      <c r="BT60" s="1"/>
+      <c r="BU60" s="1"/>
+      <c r="BV60" s="1"/>
+      <c r="BW60" s="1"/>
+      <c r="BX60" s="1"/>
+      <c r="BY60" s="1"/>
+      <c r="BZ60" s="1"/>
+      <c r="CA60" s="1"/>
+      <c r="CB60" s="1"/>
+      <c r="CC60" s="1"/>
+      <c r="CD60" s="1"/>
+      <c r="CE60" s="1"/>
+      <c r="CF60" s="1"/>
+      <c r="CG60" s="1"/>
+      <c r="CH60" s="1"/>
+      <c r="CI60" s="1"/>
+      <c r="CJ60" s="1"/>
+      <c r="CK60" s="1"/>
+      <c r="CL60" s="1"/>
+      <c r="CM60" s="1"/>
+      <c r="CN60" s="1"/>
+      <c r="CO60" s="1"/>
+      <c r="CP60" s="1"/>
+      <c r="CQ60" s="1"/>
+      <c r="CR60" s="1"/>
+      <c r="CS60" s="1"/>
+      <c r="CT60" s="1"/>
+      <c r="CU60" s="1"/>
+      <c r="CV60" s="1"/>
+      <c r="CW60" s="1"/>
+      <c r="CX60" s="1"/>
+      <c r="CY60" s="1"/>
+      <c r="CZ60" s="1"/>
+      <c r="DA60" s="1"/>
+      <c r="DB60" s="1"/>
+      <c r="DC60" s="1"/>
+      <c r="DD60" s="1"/>
+      <c r="DE60" s="1"/>
+      <c r="DF60" s="1"/>
+      <c r="DG60" s="1"/>
+      <c r="DH60" s="1"/>
+      <c r="DI60" s="1"/>
+      <c r="DJ60" s="1"/>
+      <c r="DK60" s="1"/>
+      <c r="DL60" s="1"/>
+      <c r="DM60" s="1"/>
+      <c r="DN60" s="1"/>
+      <c r="DO60" s="1"/>
+      <c r="DP60" s="1"/>
+      <c r="DQ60" s="1"/>
+      <c r="DR60" s="1"/>
+      <c r="DS60" s="1"/>
+      <c r="DT60" s="1"/>
+      <c r="DU60" s="1"/>
+      <c r="DV60" s="1"/>
+      <c r="DW60" s="1"/>
+      <c r="DX60" s="1"/>
+      <c r="DY60" s="1"/>
+      <c r="DZ60" s="1"/>
+      <c r="EA60" s="1"/>
+      <c r="EB60" s="1"/>
+      <c r="EC60" s="1"/>
+      <c r="ED60" s="1"/>
+      <c r="EE60" s="1"/>
+      <c r="EF60" s="1"/>
+      <c r="EG60" s="1"/>
+      <c r="EH60" s="1"/>
+      <c r="EI60" s="1"/>
+      <c r="EJ60" s="1"/>
+      <c r="EK60" s="1"/>
+      <c r="EL60" s="1"/>
+      <c r="EM60" s="1"/>
+      <c r="EN60" s="1"/>
+      <c r="EO60" s="1"/>
+      <c r="EP60" s="1"/>
+      <c r="EQ60" s="1"/>
+      <c r="ER60" s="1"/>
+      <c r="ES60" s="1"/>
+      <c r="ET60" s="1"/>
+      <c r="EU60" s="1"/>
+      <c r="EV60" s="1"/>
+      <c r="EW60" s="1"/>
+      <c r="EX60" s="1"/>
+      <c r="EY60" s="1"/>
+      <c r="EZ60" s="1"/>
+      <c r="FA60" s="1"/>
+      <c r="FB60" s="1"/>
+      <c r="FC60" s="1"/>
+      <c r="FD60" s="1"/>
+      <c r="FE60" s="1"/>
+      <c r="FF60" s="1"/>
+      <c r="FG60" s="1"/>
+      <c r="FH60" s="1"/>
+      <c r="FI60" s="1"/>
+      <c r="FJ60" s="1"/>
+      <c r="FK60" s="1"/>
+      <c r="FL60" s="1"/>
+      <c r="FM60" s="1"/>
+      <c r="FN60" s="1"/>
+      <c r="FO60" s="1"/>
+      <c r="FP60" s="1"/>
+      <c r="FQ60" s="1"/>
+      <c r="FR60" s="1"/>
+      <c r="FS60" s="1"/>
+      <c r="FT60" s="1"/>
+      <c r="FU60" s="1"/>
+      <c r="FV60" s="1"/>
+      <c r="FW60" s="1"/>
+      <c r="FX60" s="1"/>
+      <c r="FY60" s="1"/>
+      <c r="FZ60" s="1"/>
+      <c r="GA60" s="1"/>
+      <c r="GB60" s="1"/>
+      <c r="GC60" s="1"/>
+      <c r="GD60" s="1"/>
+      <c r="GE60" s="1"/>
+      <c r="GF60" s="1"/>
+      <c r="GG60" s="1"/>
+      <c r="GH60" s="1"/>
+      <c r="GI60" s="1"/>
+      <c r="GJ60" s="1"/>
+      <c r="GK60" s="1"/>
+      <c r="GL60" s="1"/>
+      <c r="GM60" s="1"/>
+      <c r="GN60" s="1"/>
+      <c r="GO60" s="1"/>
+      <c r="GP60" s="1"/>
+      <c r="GQ60" s="1"/>
+      <c r="GR60" s="1"/>
+      <c r="GS60" s="1"/>
+      <c r="GT60" s="1"/>
+      <c r="GU60" s="1"/>
+      <c r="GV60" s="1"/>
+      <c r="GW60" s="1"/>
+      <c r="GX60" s="1"/>
+      <c r="GY60" s="1"/>
+      <c r="GZ60" s="1"/>
+      <c r="HA60" s="1"/>
+      <c r="HB60" s="1"/>
+      <c r="HC60" s="1"/>
+      <c r="HD60" s="1"/>
+      <c r="HE60" s="1"/>
+      <c r="HF60" s="1"/>
+      <c r="HG60" s="1"/>
+      <c r="HH60" s="1"/>
+      <c r="HI60" s="1"/>
+      <c r="HJ60" s="1"/>
+      <c r="HK60" s="1"/>
+      <c r="HL60" s="1"/>
+      <c r="HM60" s="1"/>
+      <c r="HN60" s="1"/>
+      <c r="HO60" s="1"/>
+      <c r="HP60" s="1"/>
+      <c r="HQ60" s="1"/>
+      <c r="HR60" s="1"/>
+      <c r="HS60" s="1"/>
+      <c r="HT60" s="1"/>
+      <c r="HU60" s="1"/>
+      <c r="HV60" s="1"/>
+      <c r="HW60" s="1"/>
+      <c r="HX60" s="1"/>
+      <c r="HY60" s="1"/>
+      <c r="HZ60" s="1"/>
+      <c r="IA60" s="1"/>
+      <c r="IB60" s="1"/>
+      <c r="IC60" s="1"/>
+      <c r="ID60" s="1"/>
+      <c r="IE60" s="1"/>
+      <c r="IF60" s="1"/>
+      <c r="IG60" s="1"/>
+      <c r="IH60" s="1"/>
+      <c r="II60" s="1"/>
+      <c r="IJ60" s="1"/>
+      <c r="IK60" s="1"/>
+      <c r="IL60" s="1"/>
+      <c r="IM60" s="1"/>
+      <c r="IN60" s="1"/>
+      <c r="IO60" s="1"/>
+      <c r="IP60" s="1"/>
+      <c r="IQ60" s="1"/>
+      <c r="IR60" s="1"/>
+      <c r="IS60" s="1"/>
+      <c r="IT60" s="1"/>
+      <c r="IU60" s="1"/>
+      <c r="IV60" s="1"/>
     </row>
     <row r="61" spans="1:256" ht="12" customHeight="1">
-      <c r="A61" s="15"/>
-      <c r="B61" s="16"/>
-      <c r="C61" s="16"/>
-      <c r="D61" s="16"/>
-      <c r="E61" s="12"/>
-      <c r="F61" s="12"/>
-      <c r="G61" s="12"/>
-      <c r="H61" s="12"/>
-      <c r="I61" s="5"/>
-      <c r="J61" s="5"/>
-      <c r="K61" s="5"/>
-      <c r="L61" s="5"/>
-      <c r="M61" s="5"/>
-      <c r="N61" s="5"/>
-      <c r="O61" s="5"/>
-      <c r="P61" s="5"/>
-      <c r="Q61" s="5"/>
-      <c r="R61" s="5"/>
-      <c r="S61" s="1"/>
-      <c r="T61" s="1"/>
-      <c r="U61" s="1"/>
-      <c r="V61" s="1"/>
-      <c r="W61" s="1"/>
-      <c r="X61" s="1"/>
-      <c r="Y61" s="1"/>
-      <c r="Z61" s="1"/>
-      <c r="AA61" s="1"/>
-      <c r="AB61" s="1"/>
-      <c r="AC61" s="1"/>
-      <c r="AD61" s="1"/>
-      <c r="AE61" s="1"/>
-      <c r="AF61" s="1"/>
-      <c r="AG61" s="1"/>
-      <c r="AH61" s="1"/>
-      <c r="AI61" s="1"/>
-      <c r="AJ61" s="1"/>
-      <c r="AK61" s="1"/>
-      <c r="AL61" s="1"/>
-      <c r="AM61" s="1"/>
-      <c r="AN61" s="1"/>
-      <c r="AO61" s="1"/>
-      <c r="AP61" s="1"/>
-      <c r="AQ61" s="1"/>
-      <c r="AR61" s="1"/>
-      <c r="AS61" s="1"/>
-      <c r="AT61" s="1"/>
-      <c r="AU61" s="1"/>
-      <c r="AV61" s="1"/>
-      <c r="AW61" s="1"/>
-      <c r="AX61" s="1"/>
-      <c r="AY61" s="1"/>
-      <c r="AZ61" s="1"/>
-      <c r="BA61" s="1"/>
-      <c r="BB61" s="1"/>
-      <c r="BC61" s="1"/>
-      <c r="BD61" s="1"/>
-      <c r="BE61" s="1"/>
-      <c r="BF61" s="1"/>
-      <c r="BG61" s="1"/>
-      <c r="BH61" s="1"/>
-      <c r="BI61" s="1"/>
-      <c r="BJ61" s="1"/>
-      <c r="BK61" s="1"/>
-      <c r="BL61" s="1"/>
-      <c r="BM61" s="1"/>
-      <c r="BN61" s="1"/>
-      <c r="BO61" s="1"/>
-      <c r="BP61" s="1"/>
-      <c r="BQ61" s="1"/>
-      <c r="BR61" s="1"/>
-      <c r="BS61" s="1"/>
-      <c r="BT61" s="1"/>
-      <c r="BU61" s="1"/>
-      <c r="BV61" s="1"/>
-      <c r="BW61" s="1"/>
-      <c r="BX61" s="1"/>
-      <c r="BY61" s="1"/>
-      <c r="BZ61" s="1"/>
-      <c r="CA61" s="1"/>
-      <c r="CB61" s="1"/>
-      <c r="CC61" s="1"/>
-      <c r="CD61" s="1"/>
-      <c r="CE61" s="1"/>
-      <c r="CF61" s="1"/>
-      <c r="CG61" s="1"/>
-      <c r="CH61" s="1"/>
-      <c r="CI61" s="1"/>
-      <c r="CJ61" s="1"/>
-      <c r="CK61" s="1"/>
-      <c r="CL61" s="1"/>
-      <c r="CM61" s="1"/>
-      <c r="CN61" s="1"/>
-      <c r="CO61" s="1"/>
-      <c r="CP61" s="1"/>
-      <c r="CQ61" s="1"/>
-      <c r="CR61" s="1"/>
-      <c r="CS61" s="1"/>
-      <c r="CT61" s="1"/>
-      <c r="CU61" s="1"/>
-      <c r="CV61" s="1"/>
-      <c r="CW61" s="1"/>
-      <c r="CX61" s="1"/>
-      <c r="CY61" s="1"/>
-      <c r="CZ61" s="1"/>
-      <c r="DA61" s="1"/>
-      <c r="DB61" s="1"/>
-      <c r="DC61" s="1"/>
-      <c r="DD61" s="1"/>
-      <c r="DE61" s="1"/>
-      <c r="DF61" s="1"/>
-      <c r="DG61" s="1"/>
-      <c r="DH61" s="1"/>
-      <c r="DI61" s="1"/>
-      <c r="DJ61" s="1"/>
-      <c r="DK61" s="1"/>
-      <c r="DL61" s="1"/>
-      <c r="DM61" s="1"/>
-      <c r="DN61" s="1"/>
-      <c r="DO61" s="1"/>
-      <c r="DP61" s="1"/>
-      <c r="DQ61" s="1"/>
-      <c r="DR61" s="1"/>
-      <c r="DS61" s="1"/>
-      <c r="DT61" s="1"/>
-      <c r="DU61" s="1"/>
-      <c r="DV61" s="1"/>
-      <c r="DW61" s="1"/>
-      <c r="DX61" s="1"/>
-      <c r="DY61" s="1"/>
-      <c r="DZ61" s="1"/>
-      <c r="EA61" s="1"/>
-      <c r="EB61" s="1"/>
-      <c r="EC61" s="1"/>
-      <c r="ED61" s="1"/>
-      <c r="EE61" s="1"/>
-      <c r="EF61" s="1"/>
-      <c r="EG61" s="1"/>
-      <c r="EH61" s="1"/>
-      <c r="EI61" s="1"/>
-      <c r="EJ61" s="1"/>
-      <c r="EK61" s="1"/>
-      <c r="EL61" s="1"/>
-      <c r="EM61" s="1"/>
-      <c r="EN61" s="1"/>
-      <c r="EO61" s="1"/>
-      <c r="EP61" s="1"/>
-      <c r="EQ61" s="1"/>
-      <c r="ER61" s="1"/>
-      <c r="ES61" s="1"/>
-      <c r="ET61" s="1"/>
-      <c r="EU61" s="1"/>
-      <c r="EV61" s="1"/>
-      <c r="EW61" s="1"/>
-      <c r="EX61" s="1"/>
-      <c r="EY61" s="1"/>
-      <c r="EZ61" s="1"/>
-      <c r="FA61" s="1"/>
-      <c r="FB61" s="1"/>
-      <c r="FC61" s="1"/>
-      <c r="FD61" s="1"/>
-      <c r="FE61" s="1"/>
-      <c r="FF61" s="1"/>
-      <c r="FG61" s="1"/>
-      <c r="FH61" s="1"/>
-      <c r="FI61" s="1"/>
-      <c r="FJ61" s="1"/>
-      <c r="FK61" s="1"/>
-      <c r="FL61" s="1"/>
-      <c r="FM61" s="1"/>
-      <c r="FN61" s="1"/>
-      <c r="FO61" s="1"/>
-      <c r="FP61" s="1"/>
-      <c r="FQ61" s="1"/>
-      <c r="FR61" s="1"/>
-      <c r="FS61" s="1"/>
-      <c r="FT61" s="1"/>
-      <c r="FU61" s="1"/>
-      <c r="FV61" s="1"/>
-      <c r="FW61" s="1"/>
-      <c r="FX61" s="1"/>
-      <c r="FY61" s="1"/>
-      <c r="FZ61" s="1"/>
-      <c r="GA61" s="1"/>
-      <c r="GB61" s="1"/>
-      <c r="GC61" s="1"/>
-      <c r="GD61" s="1"/>
-      <c r="GE61" s="1"/>
-      <c r="GF61" s="1"/>
-      <c r="GG61" s="1"/>
-      <c r="GH61" s="1"/>
-      <c r="GI61" s="1"/>
-      <c r="GJ61" s="1"/>
-      <c r="GK61" s="1"/>
-      <c r="GL61" s="1"/>
-      <c r="GM61" s="1"/>
-      <c r="GN61" s="1"/>
-      <c r="GO61" s="1"/>
-      <c r="GP61" s="1"/>
-      <c r="GQ61" s="1"/>
-      <c r="GR61" s="1"/>
-      <c r="GS61" s="1"/>
-      <c r="GT61" s="1"/>
-      <c r="GU61" s="1"/>
-      <c r="GV61" s="1"/>
-      <c r="GW61" s="1"/>
-      <c r="GX61" s="1"/>
-      <c r="GY61" s="1"/>
-      <c r="GZ61" s="1"/>
-      <c r="HA61" s="1"/>
-      <c r="HB61" s="1"/>
-      <c r="HC61" s="1"/>
-      <c r="HD61" s="1"/>
-      <c r="HE61" s="1"/>
-      <c r="HF61" s="1"/>
-      <c r="HG61" s="1"/>
-      <c r="HH61" s="1"/>
-      <c r="HI61" s="1"/>
-      <c r="HJ61" s="1"/>
-      <c r="HK61" s="1"/>
-      <c r="HL61" s="1"/>
-      <c r="HM61" s="1"/>
-      <c r="HN61" s="1"/>
-      <c r="HO61" s="1"/>
-      <c r="HP61" s="1"/>
-      <c r="HQ61" s="1"/>
-      <c r="HR61" s="1"/>
-      <c r="HS61" s="1"/>
-      <c r="HT61" s="1"/>
-      <c r="HU61" s="1"/>
-      <c r="HV61" s="1"/>
-      <c r="HW61" s="1"/>
-      <c r="HX61" s="1"/>
-      <c r="HY61" s="1"/>
-      <c r="HZ61" s="1"/>
-      <c r="IA61" s="1"/>
-      <c r="IB61" s="1"/>
-      <c r="IC61" s="1"/>
-      <c r="ID61" s="1"/>
-      <c r="IE61" s="1"/>
-      <c r="IF61" s="1"/>
-      <c r="IG61" s="1"/>
-      <c r="IH61" s="1"/>
-      <c r="II61" s="1"/>
-      <c r="IJ61" s="1"/>
-      <c r="IK61" s="1"/>
-      <c r="IL61" s="1"/>
-      <c r="IM61" s="1"/>
-      <c r="IN61" s="1"/>
-      <c r="IO61" s="1"/>
-      <c r="IP61" s="1"/>
-      <c r="IQ61" s="1"/>
-      <c r="IR61" s="1"/>
-      <c r="IS61" s="1"/>
-      <c r="IT61" s="1"/>
-      <c r="IU61" s="1"/>
-      <c r="IV61" s="1"/>
+      <c r="A61" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="B61" s="19" t="s">
+        <v>319</v>
+      </c>
+      <c r="D61"/>
     </row>
     <row r="62" spans="1:256" ht="12" customHeight="1">
-      <c r="A62" s="65" t="s">
-        <v>136</v>
-      </c>
-      <c r="B62" s="66"/>
-      <c r="C62" s="66"/>
-      <c r="D62" s="16"/>
-      <c r="E62" s="12"/>
-      <c r="F62" s="12"/>
-      <c r="G62" s="12"/>
-      <c r="H62" s="12"/>
-      <c r="I62" s="5"/>
-      <c r="J62" s="5"/>
-      <c r="K62" s="5"/>
-      <c r="L62" s="5"/>
-      <c r="M62" s="5"/>
-      <c r="N62" s="5"/>
-      <c r="O62" s="5"/>
-      <c r="P62" s="5"/>
-      <c r="Q62" s="5"/>
-      <c r="R62" s="5"/>
-      <c r="S62" s="1"/>
-      <c r="T62" s="1"/>
-      <c r="U62" s="1"/>
-      <c r="V62" s="1"/>
-      <c r="W62" s="1"/>
-      <c r="X62" s="1"/>
-      <c r="Y62" s="1"/>
-      <c r="Z62" s="1"/>
-      <c r="AA62" s="1"/>
-      <c r="AB62" s="1"/>
-      <c r="AC62" s="1"/>
-      <c r="AD62" s="1"/>
-      <c r="AE62" s="1"/>
-      <c r="AF62" s="1"/>
-      <c r="AG62" s="1"/>
-      <c r="AH62" s="1"/>
-      <c r="AI62" s="1"/>
-      <c r="AJ62" s="1"/>
-      <c r="AK62" s="1"/>
-      <c r="AL62" s="1"/>
-      <c r="AM62" s="1"/>
-      <c r="AN62" s="1"/>
-      <c r="AO62" s="1"/>
-      <c r="AP62" s="1"/>
-      <c r="AQ62" s="1"/>
-      <c r="AR62" s="1"/>
-      <c r="AS62" s="1"/>
-      <c r="AT62" s="1"/>
-      <c r="AU62" s="1"/>
-      <c r="AV62" s="1"/>
-      <c r="AW62" s="1"/>
-      <c r="AX62" s="1"/>
-      <c r="AY62" s="1"/>
-      <c r="AZ62" s="1"/>
-      <c r="BA62" s="1"/>
-      <c r="BB62" s="1"/>
-      <c r="BC62" s="1"/>
-      <c r="BD62" s="1"/>
-      <c r="BE62" s="1"/>
-      <c r="BF62" s="1"/>
-      <c r="BG62" s="1"/>
-      <c r="BH62" s="1"/>
-      <c r="BI62" s="1"/>
-      <c r="BJ62" s="1"/>
-      <c r="BK62" s="1"/>
-      <c r="BL62" s="1"/>
-      <c r="BM62" s="1"/>
-      <c r="BN62" s="1"/>
-      <c r="BO62" s="1"/>
-      <c r="BP62" s="1"/>
-      <c r="BQ62" s="1"/>
-      <c r="BR62" s="1"/>
-      <c r="BS62" s="1"/>
-      <c r="BT62" s="1"/>
-      <c r="BU62" s="1"/>
-      <c r="BV62" s="1"/>
-      <c r="BW62" s="1"/>
-      <c r="BX62" s="1"/>
-      <c r="BY62" s="1"/>
-      <c r="BZ62" s="1"/>
-      <c r="CA62" s="1"/>
-      <c r="CB62" s="1"/>
-      <c r="CC62" s="1"/>
-      <c r="CD62" s="1"/>
-      <c r="CE62" s="1"/>
-      <c r="CF62" s="1"/>
-      <c r="CG62" s="1"/>
-      <c r="CH62" s="1"/>
-      <c r="CI62" s="1"/>
-      <c r="CJ62" s="1"/>
-      <c r="CK62" s="1"/>
-      <c r="CL62" s="1"/>
-      <c r="CM62" s="1"/>
-      <c r="CN62" s="1"/>
-      <c r="CO62" s="1"/>
-      <c r="CP62" s="1"/>
-      <c r="CQ62" s="1"/>
-      <c r="CR62" s="1"/>
-      <c r="CS62" s="1"/>
-      <c r="CT62" s="1"/>
-      <c r="CU62" s="1"/>
-      <c r="CV62" s="1"/>
-      <c r="CW62" s="1"/>
-      <c r="CX62" s="1"/>
-      <c r="CY62" s="1"/>
-      <c r="CZ62" s="1"/>
-      <c r="DA62" s="1"/>
-      <c r="DB62" s="1"/>
-      <c r="DC62" s="1"/>
-      <c r="DD62" s="1"/>
-      <c r="DE62" s="1"/>
-      <c r="DF62" s="1"/>
-      <c r="DG62" s="1"/>
-      <c r="DH62" s="1"/>
-      <c r="DI62" s="1"/>
-      <c r="DJ62" s="1"/>
-      <c r="DK62" s="1"/>
-      <c r="DL62" s="1"/>
-      <c r="DM62" s="1"/>
-      <c r="DN62" s="1"/>
-      <c r="DO62" s="1"/>
-      <c r="DP62" s="1"/>
-      <c r="DQ62" s="1"/>
-      <c r="DR62" s="1"/>
-      <c r="DS62" s="1"/>
-      <c r="DT62" s="1"/>
-      <c r="DU62" s="1"/>
-      <c r="DV62" s="1"/>
-      <c r="DW62" s="1"/>
-      <c r="DX62" s="1"/>
-      <c r="DY62" s="1"/>
-      <c r="DZ62" s="1"/>
-      <c r="EA62" s="1"/>
-      <c r="EB62" s="1"/>
-      <c r="EC62" s="1"/>
-      <c r="ED62" s="1"/>
-      <c r="EE62" s="1"/>
-      <c r="EF62" s="1"/>
-      <c r="EG62" s="1"/>
-      <c r="EH62" s="1"/>
-      <c r="EI62" s="1"/>
-      <c r="EJ62" s="1"/>
-      <c r="EK62" s="1"/>
-      <c r="EL62" s="1"/>
-      <c r="EM62" s="1"/>
-      <c r="EN62" s="1"/>
-      <c r="EO62" s="1"/>
-      <c r="EP62" s="1"/>
-      <c r="EQ62" s="1"/>
-      <c r="ER62" s="1"/>
-      <c r="ES62" s="1"/>
-      <c r="ET62" s="1"/>
-      <c r="EU62" s="1"/>
-      <c r="EV62" s="1"/>
-      <c r="EW62" s="1"/>
-      <c r="EX62" s="1"/>
-      <c r="EY62" s="1"/>
-      <c r="EZ62" s="1"/>
-      <c r="FA62" s="1"/>
-      <c r="FB62" s="1"/>
-      <c r="FC62" s="1"/>
-      <c r="FD62" s="1"/>
-      <c r="FE62" s="1"/>
-      <c r="FF62" s="1"/>
-      <c r="FG62" s="1"/>
-      <c r="FH62" s="1"/>
-      <c r="FI62" s="1"/>
-      <c r="FJ62" s="1"/>
-      <c r="FK62" s="1"/>
-      <c r="FL62" s="1"/>
-      <c r="FM62" s="1"/>
-      <c r="FN62" s="1"/>
-      <c r="FO62" s="1"/>
-      <c r="FP62" s="1"/>
-      <c r="FQ62" s="1"/>
-      <c r="FR62" s="1"/>
-      <c r="FS62" s="1"/>
-      <c r="FT62" s="1"/>
-      <c r="FU62" s="1"/>
-      <c r="FV62" s="1"/>
-      <c r="FW62" s="1"/>
-      <c r="FX62" s="1"/>
-      <c r="FY62" s="1"/>
-      <c r="FZ62" s="1"/>
-      <c r="GA62" s="1"/>
-      <c r="GB62" s="1"/>
-      <c r="GC62" s="1"/>
-      <c r="GD62" s="1"/>
-      <c r="GE62" s="1"/>
-      <c r="GF62" s="1"/>
-      <c r="GG62" s="1"/>
-      <c r="GH62" s="1"/>
-      <c r="GI62" s="1"/>
-      <c r="GJ62" s="1"/>
-      <c r="GK62" s="1"/>
-      <c r="GL62" s="1"/>
-      <c r="GM62" s="1"/>
-      <c r="GN62" s="1"/>
-      <c r="GO62" s="1"/>
-      <c r="GP62" s="1"/>
-      <c r="GQ62" s="1"/>
-      <c r="GR62" s="1"/>
-      <c r="GS62" s="1"/>
-      <c r="GT62" s="1"/>
-      <c r="GU62" s="1"/>
-      <c r="GV62" s="1"/>
-      <c r="GW62" s="1"/>
-      <c r="GX62" s="1"/>
-      <c r="GY62" s="1"/>
-      <c r="GZ62" s="1"/>
-      <c r="HA62" s="1"/>
-      <c r="HB62" s="1"/>
-      <c r="HC62" s="1"/>
-      <c r="HD62" s="1"/>
-      <c r="HE62" s="1"/>
-      <c r="HF62" s="1"/>
-      <c r="HG62" s="1"/>
-      <c r="HH62" s="1"/>
-      <c r="HI62" s="1"/>
-      <c r="HJ62" s="1"/>
-      <c r="HK62" s="1"/>
-      <c r="HL62" s="1"/>
-      <c r="HM62" s="1"/>
-      <c r="HN62" s="1"/>
-      <c r="HO62" s="1"/>
-      <c r="HP62" s="1"/>
-      <c r="HQ62" s="1"/>
-      <c r="HR62" s="1"/>
-      <c r="HS62" s="1"/>
-      <c r="HT62" s="1"/>
-      <c r="HU62" s="1"/>
-      <c r="HV62" s="1"/>
-      <c r="HW62" s="1"/>
-      <c r="HX62" s="1"/>
-      <c r="HY62" s="1"/>
-      <c r="HZ62" s="1"/>
-      <c r="IA62" s="1"/>
-      <c r="IB62" s="1"/>
-      <c r="IC62" s="1"/>
-      <c r="ID62" s="1"/>
-      <c r="IE62" s="1"/>
-      <c r="IF62" s="1"/>
-      <c r="IG62" s="1"/>
-      <c r="IH62" s="1"/>
-      <c r="II62" s="1"/>
-      <c r="IJ62" s="1"/>
-      <c r="IK62" s="1"/>
-      <c r="IL62" s="1"/>
-      <c r="IM62" s="1"/>
-      <c r="IN62" s="1"/>
-      <c r="IO62" s="1"/>
-      <c r="IP62" s="1"/>
-      <c r="IQ62" s="1"/>
-      <c r="IR62" s="1"/>
-      <c r="IS62" s="1"/>
-      <c r="IT62" s="1"/>
-      <c r="IU62" s="1"/>
-      <c r="IV62" s="1"/>
+      <c r="D62"/>
     </row>
     <row r="63" spans="1:256" ht="12" customHeight="1">
-      <c r="A63" s="30" t="s">
-        <v>137</v>
-      </c>
-      <c r="B63" s="30" t="s">
-        <v>138</v>
-      </c>
-      <c r="C63" s="30" t="s">
-        <v>139</v>
-      </c>
+      <c r="A63" s="15"/>
+      <c r="B63" s="16"/>
+      <c r="C63" s="16"/>
       <c r="D63" s="16"/>
       <c r="E63" s="12"/>
       <c r="F63" s="12"/>
@@ -16044,15 +16054,11 @@
       <c r="IV63" s="1"/>
     </row>
     <row r="64" spans="1:256" ht="12" customHeight="1">
-      <c r="A64" s="31" t="s">
-        <v>140</v>
-      </c>
-      <c r="B64" s="32" t="s">
-        <v>141</v>
-      </c>
-      <c r="C64" s="32" t="s">
-        <v>142</v>
-      </c>
+      <c r="A64" s="63" t="s">
+        <v>136</v>
+      </c>
+      <c r="B64" s="64"/>
+      <c r="C64" s="64"/>
       <c r="D64" s="16"/>
       <c r="E64" s="12"/>
       <c r="F64" s="12"/>
@@ -16308,14 +16314,14 @@
       <c r="IV64" s="1"/>
     </row>
     <row r="65" spans="1:256" ht="12" customHeight="1">
-      <c r="A65" s="31" t="s">
-        <v>143</v>
-      </c>
-      <c r="B65" s="32" t="s">
-        <v>144</v>
-      </c>
-      <c r="C65" s="32" t="s">
-        <v>145</v>
+      <c r="A65" s="30" t="s">
+        <v>137</v>
+      </c>
+      <c r="B65" s="30" t="s">
+        <v>138</v>
+      </c>
+      <c r="C65" s="30" t="s">
+        <v>139</v>
       </c>
       <c r="D65" s="16"/>
       <c r="E65" s="12"/>
@@ -16573,13 +16579,13 @@
     </row>
     <row r="66" spans="1:256" ht="12" customHeight="1">
       <c r="A66" s="31" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="B66" s="32" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="C66" s="32" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="D66" s="16"/>
       <c r="E66" s="12"/>
@@ -16837,13 +16843,13 @@
     </row>
     <row r="67" spans="1:256" ht="12" customHeight="1">
       <c r="A67" s="31" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="B67" s="32" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="C67" s="32" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="D67" s="16"/>
       <c r="E67" s="12"/>
@@ -17100,9 +17106,15 @@
       <c r="IV67" s="1"/>
     </row>
     <row r="68" spans="1:256" ht="12" customHeight="1">
-      <c r="A68" s="15"/>
-      <c r="B68" s="16"/>
-      <c r="C68" s="16"/>
+      <c r="A68" s="31" t="s">
+        <v>146</v>
+      </c>
+      <c r="B68" s="32" t="s">
+        <v>147</v>
+      </c>
+      <c r="C68" s="32" t="s">
+        <v>148</v>
+      </c>
       <c r="D68" s="16"/>
       <c r="E68" s="12"/>
       <c r="F68" s="12"/>
@@ -17358,11 +17370,15 @@
       <c r="IV68" s="1"/>
     </row>
     <row r="69" spans="1:256" ht="12" customHeight="1">
-      <c r="A69" s="64" t="s">
-        <v>66</v>
-      </c>
-      <c r="B69" s="64"/>
-      <c r="C69" s="14"/>
+      <c r="A69" s="31" t="s">
+        <v>149</v>
+      </c>
+      <c r="B69" s="32" t="s">
+        <v>150</v>
+      </c>
+      <c r="C69" s="32" t="s">
+        <v>151</v>
+      </c>
       <c r="D69" s="16"/>
       <c r="E69" s="12"/>
       <c r="F69" s="12"/>
@@ -17617,19 +17633,15 @@
       <c r="IU69" s="1"/>
       <c r="IV69" s="1"/>
     </row>
-    <row r="70" spans="1:256" ht="16.5" customHeight="1">
-      <c r="A70" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="B70" s="21" t="s">
-        <v>68</v>
-      </c>
-      <c r="C70" s="14"/>
-      <c r="D70" s="14"/>
-      <c r="E70" s="5"/>
-      <c r="F70" s="5"/>
-      <c r="G70" s="14"/>
-      <c r="H70" s="14"/>
+    <row r="70" spans="1:256" ht="12" customHeight="1">
+      <c r="A70" s="15"/>
+      <c r="B70" s="16"/>
+      <c r="C70" s="16"/>
+      <c r="D70" s="16"/>
+      <c r="E70" s="12"/>
+      <c r="F70" s="12"/>
+      <c r="G70" s="12"/>
+      <c r="H70" s="12"/>
       <c r="I70" s="5"/>
       <c r="J70" s="5"/>
       <c r="K70" s="5"/>
@@ -17640,20 +17652,256 @@
       <c r="P70" s="5"/>
       <c r="Q70" s="5"/>
       <c r="R70" s="5"/>
+      <c r="S70" s="1"/>
+      <c r="T70" s="1"/>
+      <c r="U70" s="1"/>
+      <c r="V70" s="1"/>
+      <c r="W70" s="1"/>
+      <c r="X70" s="1"/>
+      <c r="Y70" s="1"/>
+      <c r="Z70" s="1"/>
+      <c r="AA70" s="1"/>
+      <c r="AB70" s="1"/>
+      <c r="AC70" s="1"/>
+      <c r="AD70" s="1"/>
+      <c r="AE70" s="1"/>
+      <c r="AF70" s="1"/>
+      <c r="AG70" s="1"/>
+      <c r="AH70" s="1"/>
+      <c r="AI70" s="1"/>
+      <c r="AJ70" s="1"/>
+      <c r="AK70" s="1"/>
+      <c r="AL70" s="1"/>
+      <c r="AM70" s="1"/>
+      <c r="AN70" s="1"/>
+      <c r="AO70" s="1"/>
+      <c r="AP70" s="1"/>
+      <c r="AQ70" s="1"/>
+      <c r="AR70" s="1"/>
+      <c r="AS70" s="1"/>
+      <c r="AT70" s="1"/>
+      <c r="AU70" s="1"/>
+      <c r="AV70" s="1"/>
+      <c r="AW70" s="1"/>
+      <c r="AX70" s="1"/>
+      <c r="AY70" s="1"/>
+      <c r="AZ70" s="1"/>
+      <c r="BA70" s="1"/>
+      <c r="BB70" s="1"/>
+      <c r="BC70" s="1"/>
+      <c r="BD70" s="1"/>
+      <c r="BE70" s="1"/>
+      <c r="BF70" s="1"/>
+      <c r="BG70" s="1"/>
+      <c r="BH70" s="1"/>
+      <c r="BI70" s="1"/>
+      <c r="BJ70" s="1"/>
+      <c r="BK70" s="1"/>
+      <c r="BL70" s="1"/>
+      <c r="BM70" s="1"/>
+      <c r="BN70" s="1"/>
+      <c r="BO70" s="1"/>
+      <c r="BP70" s="1"/>
+      <c r="BQ70" s="1"/>
+      <c r="BR70" s="1"/>
+      <c r="BS70" s="1"/>
+      <c r="BT70" s="1"/>
+      <c r="BU70" s="1"/>
+      <c r="BV70" s="1"/>
+      <c r="BW70" s="1"/>
+      <c r="BX70" s="1"/>
+      <c r="BY70" s="1"/>
+      <c r="BZ70" s="1"/>
+      <c r="CA70" s="1"/>
+      <c r="CB70" s="1"/>
+      <c r="CC70" s="1"/>
+      <c r="CD70" s="1"/>
+      <c r="CE70" s="1"/>
+      <c r="CF70" s="1"/>
+      <c r="CG70" s="1"/>
+      <c r="CH70" s="1"/>
+      <c r="CI70" s="1"/>
+      <c r="CJ70" s="1"/>
+      <c r="CK70" s="1"/>
+      <c r="CL70" s="1"/>
+      <c r="CM70" s="1"/>
+      <c r="CN70" s="1"/>
+      <c r="CO70" s="1"/>
+      <c r="CP70" s="1"/>
+      <c r="CQ70" s="1"/>
+      <c r="CR70" s="1"/>
+      <c r="CS70" s="1"/>
+      <c r="CT70" s="1"/>
+      <c r="CU70" s="1"/>
+      <c r="CV70" s="1"/>
+      <c r="CW70" s="1"/>
+      <c r="CX70" s="1"/>
+      <c r="CY70" s="1"/>
+      <c r="CZ70" s="1"/>
+      <c r="DA70" s="1"/>
+      <c r="DB70" s="1"/>
+      <c r="DC70" s="1"/>
+      <c r="DD70" s="1"/>
+      <c r="DE70" s="1"/>
+      <c r="DF70" s="1"/>
+      <c r="DG70" s="1"/>
+      <c r="DH70" s="1"/>
+      <c r="DI70" s="1"/>
+      <c r="DJ70" s="1"/>
+      <c r="DK70" s="1"/>
+      <c r="DL70" s="1"/>
+      <c r="DM70" s="1"/>
+      <c r="DN70" s="1"/>
+      <c r="DO70" s="1"/>
+      <c r="DP70" s="1"/>
+      <c r="DQ70" s="1"/>
+      <c r="DR70" s="1"/>
+      <c r="DS70" s="1"/>
+      <c r="DT70" s="1"/>
+      <c r="DU70" s="1"/>
+      <c r="DV70" s="1"/>
+      <c r="DW70" s="1"/>
+      <c r="DX70" s="1"/>
+      <c r="DY70" s="1"/>
+      <c r="DZ70" s="1"/>
+      <c r="EA70" s="1"/>
+      <c r="EB70" s="1"/>
+      <c r="EC70" s="1"/>
+      <c r="ED70" s="1"/>
+      <c r="EE70" s="1"/>
+      <c r="EF70" s="1"/>
+      <c r="EG70" s="1"/>
+      <c r="EH70" s="1"/>
+      <c r="EI70" s="1"/>
+      <c r="EJ70" s="1"/>
+      <c r="EK70" s="1"/>
+      <c r="EL70" s="1"/>
+      <c r="EM70" s="1"/>
+      <c r="EN70" s="1"/>
+      <c r="EO70" s="1"/>
+      <c r="EP70" s="1"/>
+      <c r="EQ70" s="1"/>
+      <c r="ER70" s="1"/>
+      <c r="ES70" s="1"/>
+      <c r="ET70" s="1"/>
+      <c r="EU70" s="1"/>
+      <c r="EV70" s="1"/>
+      <c r="EW70" s="1"/>
+      <c r="EX70" s="1"/>
+      <c r="EY70" s="1"/>
+      <c r="EZ70" s="1"/>
+      <c r="FA70" s="1"/>
+      <c r="FB70" s="1"/>
+      <c r="FC70" s="1"/>
+      <c r="FD70" s="1"/>
+      <c r="FE70" s="1"/>
+      <c r="FF70" s="1"/>
+      <c r="FG70" s="1"/>
+      <c r="FH70" s="1"/>
+      <c r="FI70" s="1"/>
+      <c r="FJ70" s="1"/>
+      <c r="FK70" s="1"/>
+      <c r="FL70" s="1"/>
+      <c r="FM70" s="1"/>
+      <c r="FN70" s="1"/>
+      <c r="FO70" s="1"/>
+      <c r="FP70" s="1"/>
+      <c r="FQ70" s="1"/>
+      <c r="FR70" s="1"/>
+      <c r="FS70" s="1"/>
+      <c r="FT70" s="1"/>
+      <c r="FU70" s="1"/>
+      <c r="FV70" s="1"/>
+      <c r="FW70" s="1"/>
+      <c r="FX70" s="1"/>
+      <c r="FY70" s="1"/>
+      <c r="FZ70" s="1"/>
+      <c r="GA70" s="1"/>
+      <c r="GB70" s="1"/>
+      <c r="GC70" s="1"/>
+      <c r="GD70" s="1"/>
+      <c r="GE70" s="1"/>
+      <c r="GF70" s="1"/>
+      <c r="GG70" s="1"/>
+      <c r="GH70" s="1"/>
+      <c r="GI70" s="1"/>
+      <c r="GJ70" s="1"/>
+      <c r="GK70" s="1"/>
+      <c r="GL70" s="1"/>
+      <c r="GM70" s="1"/>
+      <c r="GN70" s="1"/>
+      <c r="GO70" s="1"/>
+      <c r="GP70" s="1"/>
+      <c r="GQ70" s="1"/>
+      <c r="GR70" s="1"/>
+      <c r="GS70" s="1"/>
+      <c r="GT70" s="1"/>
+      <c r="GU70" s="1"/>
+      <c r="GV70" s="1"/>
+      <c r="GW70" s="1"/>
+      <c r="GX70" s="1"/>
+      <c r="GY70" s="1"/>
+      <c r="GZ70" s="1"/>
+      <c r="HA70" s="1"/>
+      <c r="HB70" s="1"/>
+      <c r="HC70" s="1"/>
+      <c r="HD70" s="1"/>
+      <c r="HE70" s="1"/>
+      <c r="HF70" s="1"/>
+      <c r="HG70" s="1"/>
+      <c r="HH70" s="1"/>
+      <c r="HI70" s="1"/>
+      <c r="HJ70" s="1"/>
+      <c r="HK70" s="1"/>
+      <c r="HL70" s="1"/>
+      <c r="HM70" s="1"/>
+      <c r="HN70" s="1"/>
+      <c r="HO70" s="1"/>
+      <c r="HP70" s="1"/>
+      <c r="HQ70" s="1"/>
+      <c r="HR70" s="1"/>
+      <c r="HS70" s="1"/>
+      <c r="HT70" s="1"/>
+      <c r="HU70" s="1"/>
+      <c r="HV70" s="1"/>
+      <c r="HW70" s="1"/>
+      <c r="HX70" s="1"/>
+      <c r="HY70" s="1"/>
+      <c r="HZ70" s="1"/>
+      <c r="IA70" s="1"/>
+      <c r="IB70" s="1"/>
+      <c r="IC70" s="1"/>
+      <c r="ID70" s="1"/>
+      <c r="IE70" s="1"/>
+      <c r="IF70" s="1"/>
+      <c r="IG70" s="1"/>
+      <c r="IH70" s="1"/>
+      <c r="II70" s="1"/>
+      <c r="IJ70" s="1"/>
+      <c r="IK70" s="1"/>
+      <c r="IL70" s="1"/>
+      <c r="IM70" s="1"/>
+      <c r="IN70" s="1"/>
+      <c r="IO70" s="1"/>
+      <c r="IP70" s="1"/>
+      <c r="IQ70" s="1"/>
+      <c r="IR70" s="1"/>
+      <c r="IS70" s="1"/>
+      <c r="IT70" s="1"/>
+      <c r="IU70" s="1"/>
+      <c r="IV70" s="1"/>
     </row>
     <row r="71" spans="1:256" ht="12" customHeight="1">
-      <c r="A71" s="22" t="s">
-        <v>305</v>
-      </c>
-      <c r="B71" s="19" t="s">
-        <v>306</v>
-      </c>
-      <c r="C71" s="5"/>
-      <c r="D71" s="14"/>
-      <c r="E71" s="5"/>
-      <c r="F71" s="5"/>
-      <c r="G71" s="14"/>
-      <c r="H71" s="14"/>
+      <c r="A71" s="62" t="s">
+        <v>66</v>
+      </c>
+      <c r="B71" s="62"/>
+      <c r="C71" s="14"/>
+      <c r="D71" s="16"/>
+      <c r="E71" s="12"/>
+      <c r="F71" s="12"/>
+      <c r="G71" s="12"/>
+      <c r="H71" s="12"/>
       <c r="I71" s="5"/>
       <c r="J71" s="5"/>
       <c r="K71" s="5"/>
@@ -17903,15 +18151,19 @@
       <c r="IU71" s="1"/>
       <c r="IV71" s="1"/>
     </row>
-    <row r="72" spans="1:256" ht="15.95" customHeight="1">
-      <c r="A72" s="1"/>
-      <c r="B72" s="1"/>
-      <c r="C72" s="5"/>
-      <c r="D72" s="5"/>
+    <row r="72" spans="1:256" ht="16.5" customHeight="1">
+      <c r="A72" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="B72" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="C72" s="14"/>
+      <c r="D72" s="14"/>
       <c r="E72" s="5"/>
       <c r="F72" s="5"/>
-      <c r="G72" s="5"/>
-      <c r="H72" s="5"/>
+      <c r="G72" s="14"/>
+      <c r="H72" s="14"/>
       <c r="I72" s="5"/>
       <c r="J72" s="5"/>
       <c r="K72" s="5"/>
@@ -17922,254 +18174,20 @@
       <c r="P72" s="5"/>
       <c r="Q72" s="5"/>
       <c r="R72" s="5"/>
-      <c r="S72" s="1"/>
-      <c r="T72" s="1"/>
-      <c r="U72" s="1"/>
-      <c r="V72" s="1"/>
-      <c r="W72" s="1"/>
-      <c r="X72" s="1"/>
-      <c r="Y72" s="1"/>
-      <c r="Z72" s="1"/>
-      <c r="AA72" s="1"/>
-      <c r="AB72" s="1"/>
-      <c r="AC72" s="1"/>
-      <c r="AD72" s="1"/>
-      <c r="AE72" s="1"/>
-      <c r="AF72" s="1"/>
-      <c r="AG72" s="1"/>
-      <c r="AH72" s="1"/>
-      <c r="AI72" s="1"/>
-      <c r="AJ72" s="1"/>
-      <c r="AK72" s="1"/>
-      <c r="AL72" s="1"/>
-      <c r="AM72" s="1"/>
-      <c r="AN72" s="1"/>
-      <c r="AO72" s="1"/>
-      <c r="AP72" s="1"/>
-      <c r="AQ72" s="1"/>
-      <c r="AR72" s="1"/>
-      <c r="AS72" s="1"/>
-      <c r="AT72" s="1"/>
-      <c r="AU72" s="1"/>
-      <c r="AV72" s="1"/>
-      <c r="AW72" s="1"/>
-      <c r="AX72" s="1"/>
-      <c r="AY72" s="1"/>
-      <c r="AZ72" s="1"/>
-      <c r="BA72" s="1"/>
-      <c r="BB72" s="1"/>
-      <c r="BC72" s="1"/>
-      <c r="BD72" s="1"/>
-      <c r="BE72" s="1"/>
-      <c r="BF72" s="1"/>
-      <c r="BG72" s="1"/>
-      <c r="BH72" s="1"/>
-      <c r="BI72" s="1"/>
-      <c r="BJ72" s="1"/>
-      <c r="BK72" s="1"/>
-      <c r="BL72" s="1"/>
-      <c r="BM72" s="1"/>
-      <c r="BN72" s="1"/>
-      <c r="BO72" s="1"/>
-      <c r="BP72" s="1"/>
-      <c r="BQ72" s="1"/>
-      <c r="BR72" s="1"/>
-      <c r="BS72" s="1"/>
-      <c r="BT72" s="1"/>
-      <c r="BU72" s="1"/>
-      <c r="BV72" s="1"/>
-      <c r="BW72" s="1"/>
-      <c r="BX72" s="1"/>
-      <c r="BY72" s="1"/>
-      <c r="BZ72" s="1"/>
-      <c r="CA72" s="1"/>
-      <c r="CB72" s="1"/>
-      <c r="CC72" s="1"/>
-      <c r="CD72" s="1"/>
-      <c r="CE72" s="1"/>
-      <c r="CF72" s="1"/>
-      <c r="CG72" s="1"/>
-      <c r="CH72" s="1"/>
-      <c r="CI72" s="1"/>
-      <c r="CJ72" s="1"/>
-      <c r="CK72" s="1"/>
-      <c r="CL72" s="1"/>
-      <c r="CM72" s="1"/>
-      <c r="CN72" s="1"/>
-      <c r="CO72" s="1"/>
-      <c r="CP72" s="1"/>
-      <c r="CQ72" s="1"/>
-      <c r="CR72" s="1"/>
-      <c r="CS72" s="1"/>
-      <c r="CT72" s="1"/>
-      <c r="CU72" s="1"/>
-      <c r="CV72" s="1"/>
-      <c r="CW72" s="1"/>
-      <c r="CX72" s="1"/>
-      <c r="CY72" s="1"/>
-      <c r="CZ72" s="1"/>
-      <c r="DA72" s="1"/>
-      <c r="DB72" s="1"/>
-      <c r="DC72" s="1"/>
-      <c r="DD72" s="1"/>
-      <c r="DE72" s="1"/>
-      <c r="DF72" s="1"/>
-      <c r="DG72" s="1"/>
-      <c r="DH72" s="1"/>
-      <c r="DI72" s="1"/>
-      <c r="DJ72" s="1"/>
-      <c r="DK72" s="1"/>
-      <c r="DL72" s="1"/>
-      <c r="DM72" s="1"/>
-      <c r="DN72" s="1"/>
-      <c r="DO72" s="1"/>
-      <c r="DP72" s="1"/>
-      <c r="DQ72" s="1"/>
-      <c r="DR72" s="1"/>
-      <c r="DS72" s="1"/>
-      <c r="DT72" s="1"/>
-      <c r="DU72" s="1"/>
-      <c r="DV72" s="1"/>
-      <c r="DW72" s="1"/>
-      <c r="DX72" s="1"/>
-      <c r="DY72" s="1"/>
-      <c r="DZ72" s="1"/>
-      <c r="EA72" s="1"/>
-      <c r="EB72" s="1"/>
-      <c r="EC72" s="1"/>
-      <c r="ED72" s="1"/>
-      <c r="EE72" s="1"/>
-      <c r="EF72" s="1"/>
-      <c r="EG72" s="1"/>
-      <c r="EH72" s="1"/>
-      <c r="EI72" s="1"/>
-      <c r="EJ72" s="1"/>
-      <c r="EK72" s="1"/>
-      <c r="EL72" s="1"/>
-      <c r="EM72" s="1"/>
-      <c r="EN72" s="1"/>
-      <c r="EO72" s="1"/>
-      <c r="EP72" s="1"/>
-      <c r="EQ72" s="1"/>
-      <c r="ER72" s="1"/>
-      <c r="ES72" s="1"/>
-      <c r="ET72" s="1"/>
-      <c r="EU72" s="1"/>
-      <c r="EV72" s="1"/>
-      <c r="EW72" s="1"/>
-      <c r="EX72" s="1"/>
-      <c r="EY72" s="1"/>
-      <c r="EZ72" s="1"/>
-      <c r="FA72" s="1"/>
-      <c r="FB72" s="1"/>
-      <c r="FC72" s="1"/>
-      <c r="FD72" s="1"/>
-      <c r="FE72" s="1"/>
-      <c r="FF72" s="1"/>
-      <c r="FG72" s="1"/>
-      <c r="FH72" s="1"/>
-      <c r="FI72" s="1"/>
-      <c r="FJ72" s="1"/>
-      <c r="FK72" s="1"/>
-      <c r="FL72" s="1"/>
-      <c r="FM72" s="1"/>
-      <c r="FN72" s="1"/>
-      <c r="FO72" s="1"/>
-      <c r="FP72" s="1"/>
-      <c r="FQ72" s="1"/>
-      <c r="FR72" s="1"/>
-      <c r="FS72" s="1"/>
-      <c r="FT72" s="1"/>
-      <c r="FU72" s="1"/>
-      <c r="FV72" s="1"/>
-      <c r="FW72" s="1"/>
-      <c r="FX72" s="1"/>
-      <c r="FY72" s="1"/>
-      <c r="FZ72" s="1"/>
-      <c r="GA72" s="1"/>
-      <c r="GB72" s="1"/>
-      <c r="GC72" s="1"/>
-      <c r="GD72" s="1"/>
-      <c r="GE72" s="1"/>
-      <c r="GF72" s="1"/>
-      <c r="GG72" s="1"/>
-      <c r="GH72" s="1"/>
-      <c r="GI72" s="1"/>
-      <c r="GJ72" s="1"/>
-      <c r="GK72" s="1"/>
-      <c r="GL72" s="1"/>
-      <c r="GM72" s="1"/>
-      <c r="GN72" s="1"/>
-      <c r="GO72" s="1"/>
-      <c r="GP72" s="1"/>
-      <c r="GQ72" s="1"/>
-      <c r="GR72" s="1"/>
-      <c r="GS72" s="1"/>
-      <c r="GT72" s="1"/>
-      <c r="GU72" s="1"/>
-      <c r="GV72" s="1"/>
-      <c r="GW72" s="1"/>
-      <c r="GX72" s="1"/>
-      <c r="GY72" s="1"/>
-      <c r="GZ72" s="1"/>
-      <c r="HA72" s="1"/>
-      <c r="HB72" s="1"/>
-      <c r="HC72" s="1"/>
-      <c r="HD72" s="1"/>
-      <c r="HE72" s="1"/>
-      <c r="HF72" s="1"/>
-      <c r="HG72" s="1"/>
-      <c r="HH72" s="1"/>
-      <c r="HI72" s="1"/>
-      <c r="HJ72" s="1"/>
-      <c r="HK72" s="1"/>
-      <c r="HL72" s="1"/>
-      <c r="HM72" s="1"/>
-      <c r="HN72" s="1"/>
-      <c r="HO72" s="1"/>
-      <c r="HP72" s="1"/>
-      <c r="HQ72" s="1"/>
-      <c r="HR72" s="1"/>
-      <c r="HS72" s="1"/>
-      <c r="HT72" s="1"/>
-      <c r="HU72" s="1"/>
-      <c r="HV72" s="1"/>
-      <c r="HW72" s="1"/>
-      <c r="HX72" s="1"/>
-      <c r="HY72" s="1"/>
-      <c r="HZ72" s="1"/>
-      <c r="IA72" s="1"/>
-      <c r="IB72" s="1"/>
-      <c r="IC72" s="1"/>
-      <c r="ID72" s="1"/>
-      <c r="IE72" s="1"/>
-      <c r="IF72" s="1"/>
-      <c r="IG72" s="1"/>
-      <c r="IH72" s="1"/>
-      <c r="II72" s="1"/>
-      <c r="IJ72" s="1"/>
-      <c r="IK72" s="1"/>
-      <c r="IL72" s="1"/>
-      <c r="IM72" s="1"/>
-      <c r="IN72" s="1"/>
-      <c r="IO72" s="1"/>
-      <c r="IP72" s="1"/>
-      <c r="IQ72" s="1"/>
-      <c r="IR72" s="1"/>
-      <c r="IS72" s="1"/>
-      <c r="IT72" s="1"/>
-      <c r="IU72" s="1"/>
-      <c r="IV72" s="1"/>
     </row>
-    <row r="73" spans="1:256" ht="15.95" customHeight="1">
-      <c r="A73" s="1"/>
-      <c r="B73" s="1"/>
+    <row r="73" spans="1:256" ht="12" customHeight="1">
+      <c r="A73" s="22" t="s">
+        <v>305</v>
+      </c>
+      <c r="B73" s="19" t="s">
+        <v>306</v>
+      </c>
       <c r="C73" s="5"/>
-      <c r="D73" s="5"/>
+      <c r="D73" s="14"/>
       <c r="E73" s="5"/>
       <c r="F73" s="5"/>
-      <c r="G73" s="5"/>
-      <c r="H73" s="5"/>
+      <c r="G73" s="14"/>
+      <c r="H73" s="14"/>
       <c r="I73" s="5"/>
       <c r="J73" s="5"/>
       <c r="K73" s="5"/>
@@ -18432,12 +18450,12 @@
       <c r="J74" s="5"/>
       <c r="K74" s="5"/>
       <c r="L74" s="5"/>
-      <c r="M74" s="1"/>
-      <c r="N74" s="1"/>
-      <c r="O74" s="1"/>
-      <c r="P74" s="1"/>
-      <c r="Q74" s="1"/>
-      <c r="R74" s="1"/>
+      <c r="M74" s="5"/>
+      <c r="N74" s="5"/>
+      <c r="O74" s="5"/>
+      <c r="P74" s="5"/>
+      <c r="Q74" s="5"/>
+      <c r="R74" s="5"/>
       <c r="S74" s="1"/>
       <c r="T74" s="1"/>
       <c r="U74" s="1"/>
@@ -18690,12 +18708,12 @@
       <c r="J75" s="5"/>
       <c r="K75" s="5"/>
       <c r="L75" s="5"/>
-      <c r="M75" s="1"/>
-      <c r="N75" s="1"/>
-      <c r="O75" s="1"/>
-      <c r="P75" s="1"/>
-      <c r="Q75" s="1"/>
-      <c r="R75" s="1"/>
+      <c r="M75" s="5"/>
+      <c r="N75" s="5"/>
+      <c r="O75" s="5"/>
+      <c r="P75" s="5"/>
+      <c r="Q75" s="5"/>
+      <c r="R75" s="5"/>
       <c r="S75" s="1"/>
       <c r="T75" s="1"/>
       <c r="U75" s="1"/>
@@ -18935,7 +18953,7 @@
       <c r="IU75" s="1"/>
       <c r="IV75" s="1"/>
     </row>
-    <row r="76" spans="1:256">
+    <row r="76" spans="1:256" ht="15.95" customHeight="1">
       <c r="A76" s="1"/>
       <c r="B76" s="1"/>
       <c r="C76" s="5"/>
@@ -19193,7 +19211,7 @@
       <c r="IU76" s="1"/>
       <c r="IV76" s="1"/>
     </row>
-    <row r="77" spans="1:256" ht="15.75" customHeight="1">
+    <row r="77" spans="1:256" ht="15.95" customHeight="1">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
       <c r="C77" s="5"/>
@@ -19451,10 +19469,10 @@
       <c r="IU77" s="1"/>
       <c r="IV77" s="1"/>
     </row>
-    <row r="78" spans="1:256" ht="15.75" customHeight="1">
+    <row r="78" spans="1:256">
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
-      <c r="C78" s="1"/>
+      <c r="C78" s="5"/>
       <c r="D78" s="5"/>
       <c r="E78" s="5"/>
       <c r="F78" s="5"/>
@@ -19709,26 +19727,25 @@
       <c r="IU78" s="1"/>
       <c r="IV78" s="1"/>
     </row>
-    <row r="79" spans="1:256" ht="12" customHeight="1">
-      <c r="A79" s="64" t="s">
-        <v>184</v>
-      </c>
-      <c r="B79" s="64"/>
-      <c r="C79" s="1"/>
-      <c r="E79" s="1"/>
-      <c r="F79" s="1"/>
-      <c r="G79" s="1"/>
-      <c r="H79" s="1"/>
+    <row r="79" spans="1:256" ht="15.75" customHeight="1">
+      <c r="A79" s="1"/>
+      <c r="B79" s="1"/>
+      <c r="C79" s="5"/>
+      <c r="D79" s="5"/>
+      <c r="E79" s="5"/>
+      <c r="F79" s="5"/>
+      <c r="G79" s="5"/>
+      <c r="H79" s="5"/>
       <c r="I79" s="5"/>
       <c r="J79" s="5"/>
       <c r="K79" s="5"/>
       <c r="L79" s="5"/>
-      <c r="M79" s="5"/>
-      <c r="N79" s="5"/>
-      <c r="O79" s="5"/>
-      <c r="P79" s="5"/>
-      <c r="Q79" s="5"/>
-      <c r="R79" s="5"/>
+      <c r="M79" s="1"/>
+      <c r="N79" s="1"/>
+      <c r="O79" s="1"/>
+      <c r="P79" s="1"/>
+      <c r="Q79" s="1"/>
+      <c r="R79" s="1"/>
       <c r="S79" s="1"/>
       <c r="T79" s="1"/>
       <c r="U79" s="1"/>
@@ -19969,14 +19986,11 @@
       <c r="IV79" s="1"/>
     </row>
     <row r="80" spans="1:256" ht="15.75" customHeight="1">
-      <c r="A80" s="20" t="s">
-        <v>185</v>
-      </c>
-      <c r="B80" s="21" t="s">
-        <v>186</v>
-      </c>
+      <c r="A80" s="1"/>
+      <c r="B80" s="1"/>
       <c r="C80" s="1"/>
-      <c r="E80" s="1"/>
+      <c r="D80" s="5"/>
+      <c r="E80" s="5"/>
       <c r="F80" s="5"/>
       <c r="G80" s="5"/>
       <c r="H80" s="5"/>
@@ -19984,9 +19998,9 @@
       <c r="J80" s="5"/>
       <c r="K80" s="5"/>
       <c r="L80" s="5"/>
-      <c r="M80" s="5"/>
-      <c r="N80" s="5"/>
-      <c r="O80" s="5"/>
+      <c r="M80" s="1"/>
+      <c r="N80" s="1"/>
+      <c r="O80" s="1"/>
       <c r="P80" s="1"/>
       <c r="Q80" s="1"/>
       <c r="R80" s="1"/>
@@ -20229,18 +20243,16 @@
       <c r="IU80" s="1"/>
       <c r="IV80" s="1"/>
     </row>
-    <row r="81" spans="1:256" ht="15.75" customHeight="1">
-      <c r="A81" s="22" t="s">
-        <v>187</v>
-      </c>
-      <c r="B81" s="22" t="s">
-        <v>188</v>
-      </c>
+    <row r="81" spans="1:256" ht="12" customHeight="1">
+      <c r="A81" s="62" t="s">
+        <v>184</v>
+      </c>
+      <c r="B81" s="62"/>
       <c r="C81" s="1"/>
       <c r="E81" s="1"/>
-      <c r="F81" s="5"/>
-      <c r="G81" s="5"/>
-      <c r="H81" s="5"/>
+      <c r="F81" s="1"/>
+      <c r="G81" s="1"/>
+      <c r="H81" s="1"/>
       <c r="I81" s="5"/>
       <c r="J81" s="5"/>
       <c r="K81" s="5"/>
@@ -20248,9 +20260,9 @@
       <c r="M81" s="5"/>
       <c r="N81" s="5"/>
       <c r="O81" s="5"/>
-      <c r="P81" s="1"/>
-      <c r="Q81" s="1"/>
-      <c r="R81" s="1"/>
+      <c r="P81" s="5"/>
+      <c r="Q81" s="5"/>
+      <c r="R81" s="5"/>
       <c r="S81" s="1"/>
       <c r="T81" s="1"/>
       <c r="U81" s="1"/>
@@ -20491,8 +20503,12 @@
       <c r="IV81" s="1"/>
     </row>
     <row r="82" spans="1:256" ht="15.75" customHeight="1">
-      <c r="A82" s="1"/>
-      <c r="B82" s="1"/>
+      <c r="A82" s="20" t="s">
+        <v>185</v>
+      </c>
+      <c r="B82" s="21" t="s">
+        <v>186</v>
+      </c>
       <c r="C82" s="1"/>
       <c r="E82" s="1"/>
       <c r="F82" s="5"/>
@@ -20748,10 +20764,17 @@
       <c r="IV82" s="1"/>
     </row>
     <row r="83" spans="1:256" ht="15.75" customHeight="1">
+      <c r="A83" s="22" t="s">
+        <v>187</v>
+      </c>
+      <c r="B83" s="22" t="s">
+        <v>188</v>
+      </c>
+      <c r="C83" s="1"/>
       <c r="E83" s="1"/>
-      <c r="F83" s="1"/>
-      <c r="G83" s="1"/>
-      <c r="H83" s="1"/>
+      <c r="F83" s="5"/>
+      <c r="G83" s="5"/>
+      <c r="H83" s="5"/>
       <c r="I83" s="5"/>
       <c r="J83" s="5"/>
       <c r="K83" s="5"/>
@@ -20759,9 +20782,9 @@
       <c r="M83" s="5"/>
       <c r="N83" s="5"/>
       <c r="O83" s="5"/>
-      <c r="P83" s="5"/>
-      <c r="Q83" s="5"/>
-      <c r="R83" s="5"/>
+      <c r="P83" s="1"/>
+      <c r="Q83" s="1"/>
+      <c r="R83" s="1"/>
       <c r="S83" s="1"/>
       <c r="T83" s="1"/>
       <c r="U83" s="1"/>
@@ -21001,7 +21024,14 @@
       <c r="IU83" s="1"/>
       <c r="IV83" s="1"/>
     </row>
-    <row r="84" spans="1:256" ht="12" customHeight="1">
+    <row r="84" spans="1:256" ht="15.75" customHeight="1">
+      <c r="A84" s="1"/>
+      <c r="B84" s="1"/>
+      <c r="C84" s="1"/>
+      <c r="E84" s="1"/>
+      <c r="F84" s="5"/>
+      <c r="G84" s="5"/>
+      <c r="H84" s="5"/>
       <c r="I84" s="5"/>
       <c r="J84" s="5"/>
       <c r="K84" s="5"/>
@@ -21009,12 +21039,514 @@
       <c r="M84" s="5"/>
       <c r="N84" s="5"/>
       <c r="O84" s="5"/>
-      <c r="P84" s="5"/>
-      <c r="Q84" s="5"/>
-      <c r="R84" s="5"/>
+      <c r="P84" s="1"/>
+      <c r="Q84" s="1"/>
+      <c r="R84" s="1"/>
+      <c r="S84" s="1"/>
+      <c r="T84" s="1"/>
+      <c r="U84" s="1"/>
+      <c r="V84" s="1"/>
+      <c r="W84" s="1"/>
+      <c r="X84" s="1"/>
+      <c r="Y84" s="1"/>
+      <c r="Z84" s="1"/>
+      <c r="AA84" s="1"/>
+      <c r="AB84" s="1"/>
+      <c r="AC84" s="1"/>
+      <c r="AD84" s="1"/>
+      <c r="AE84" s="1"/>
+      <c r="AF84" s="1"/>
+      <c r="AG84" s="1"/>
+      <c r="AH84" s="1"/>
+      <c r="AI84" s="1"/>
+      <c r="AJ84" s="1"/>
+      <c r="AK84" s="1"/>
+      <c r="AL84" s="1"/>
+      <c r="AM84" s="1"/>
+      <c r="AN84" s="1"/>
+      <c r="AO84" s="1"/>
+      <c r="AP84" s="1"/>
+      <c r="AQ84" s="1"/>
+      <c r="AR84" s="1"/>
+      <c r="AS84" s="1"/>
+      <c r="AT84" s="1"/>
+      <c r="AU84" s="1"/>
+      <c r="AV84" s="1"/>
+      <c r="AW84" s="1"/>
+      <c r="AX84" s="1"/>
+      <c r="AY84" s="1"/>
+      <c r="AZ84" s="1"/>
+      <c r="BA84" s="1"/>
+      <c r="BB84" s="1"/>
+      <c r="BC84" s="1"/>
+      <c r="BD84" s="1"/>
+      <c r="BE84" s="1"/>
+      <c r="BF84" s="1"/>
+      <c r="BG84" s="1"/>
+      <c r="BH84" s="1"/>
+      <c r="BI84" s="1"/>
+      <c r="BJ84" s="1"/>
+      <c r="BK84" s="1"/>
+      <c r="BL84" s="1"/>
+      <c r="BM84" s="1"/>
+      <c r="BN84" s="1"/>
+      <c r="BO84" s="1"/>
+      <c r="BP84" s="1"/>
+      <c r="BQ84" s="1"/>
+      <c r="BR84" s="1"/>
+      <c r="BS84" s="1"/>
+      <c r="BT84" s="1"/>
+      <c r="BU84" s="1"/>
+      <c r="BV84" s="1"/>
+      <c r="BW84" s="1"/>
+      <c r="BX84" s="1"/>
+      <c r="BY84" s="1"/>
+      <c r="BZ84" s="1"/>
+      <c r="CA84" s="1"/>
+      <c r="CB84" s="1"/>
+      <c r="CC84" s="1"/>
+      <c r="CD84" s="1"/>
+      <c r="CE84" s="1"/>
+      <c r="CF84" s="1"/>
+      <c r="CG84" s="1"/>
+      <c r="CH84" s="1"/>
+      <c r="CI84" s="1"/>
+      <c r="CJ84" s="1"/>
+      <c r="CK84" s="1"/>
+      <c r="CL84" s="1"/>
+      <c r="CM84" s="1"/>
+      <c r="CN84" s="1"/>
+      <c r="CO84" s="1"/>
+      <c r="CP84" s="1"/>
+      <c r="CQ84" s="1"/>
+      <c r="CR84" s="1"/>
+      <c r="CS84" s="1"/>
+      <c r="CT84" s="1"/>
+      <c r="CU84" s="1"/>
+      <c r="CV84" s="1"/>
+      <c r="CW84" s="1"/>
+      <c r="CX84" s="1"/>
+      <c r="CY84" s="1"/>
+      <c r="CZ84" s="1"/>
+      <c r="DA84" s="1"/>
+      <c r="DB84" s="1"/>
+      <c r="DC84" s="1"/>
+      <c r="DD84" s="1"/>
+      <c r="DE84" s="1"/>
+      <c r="DF84" s="1"/>
+      <c r="DG84" s="1"/>
+      <c r="DH84" s="1"/>
+      <c r="DI84" s="1"/>
+      <c r="DJ84" s="1"/>
+      <c r="DK84" s="1"/>
+      <c r="DL84" s="1"/>
+      <c r="DM84" s="1"/>
+      <c r="DN84" s="1"/>
+      <c r="DO84" s="1"/>
+      <c r="DP84" s="1"/>
+      <c r="DQ84" s="1"/>
+      <c r="DR84" s="1"/>
+      <c r="DS84" s="1"/>
+      <c r="DT84" s="1"/>
+      <c r="DU84" s="1"/>
+      <c r="DV84" s="1"/>
+      <c r="DW84" s="1"/>
+      <c r="DX84" s="1"/>
+      <c r="DY84" s="1"/>
+      <c r="DZ84" s="1"/>
+      <c r="EA84" s="1"/>
+      <c r="EB84" s="1"/>
+      <c r="EC84" s="1"/>
+      <c r="ED84" s="1"/>
+      <c r="EE84" s="1"/>
+      <c r="EF84" s="1"/>
+      <c r="EG84" s="1"/>
+      <c r="EH84" s="1"/>
+      <c r="EI84" s="1"/>
+      <c r="EJ84" s="1"/>
+      <c r="EK84" s="1"/>
+      <c r="EL84" s="1"/>
+      <c r="EM84" s="1"/>
+      <c r="EN84" s="1"/>
+      <c r="EO84" s="1"/>
+      <c r="EP84" s="1"/>
+      <c r="EQ84" s="1"/>
+      <c r="ER84" s="1"/>
+      <c r="ES84" s="1"/>
+      <c r="ET84" s="1"/>
+      <c r="EU84" s="1"/>
+      <c r="EV84" s="1"/>
+      <c r="EW84" s="1"/>
+      <c r="EX84" s="1"/>
+      <c r="EY84" s="1"/>
+      <c r="EZ84" s="1"/>
+      <c r="FA84" s="1"/>
+      <c r="FB84" s="1"/>
+      <c r="FC84" s="1"/>
+      <c r="FD84" s="1"/>
+      <c r="FE84" s="1"/>
+      <c r="FF84" s="1"/>
+      <c r="FG84" s="1"/>
+      <c r="FH84" s="1"/>
+      <c r="FI84" s="1"/>
+      <c r="FJ84" s="1"/>
+      <c r="FK84" s="1"/>
+      <c r="FL84" s="1"/>
+      <c r="FM84" s="1"/>
+      <c r="FN84" s="1"/>
+      <c r="FO84" s="1"/>
+      <c r="FP84" s="1"/>
+      <c r="FQ84" s="1"/>
+      <c r="FR84" s="1"/>
+      <c r="FS84" s="1"/>
+      <c r="FT84" s="1"/>
+      <c r="FU84" s="1"/>
+      <c r="FV84" s="1"/>
+      <c r="FW84" s="1"/>
+      <c r="FX84" s="1"/>
+      <c r="FY84" s="1"/>
+      <c r="FZ84" s="1"/>
+      <c r="GA84" s="1"/>
+      <c r="GB84" s="1"/>
+      <c r="GC84" s="1"/>
+      <c r="GD84" s="1"/>
+      <c r="GE84" s="1"/>
+      <c r="GF84" s="1"/>
+      <c r="GG84" s="1"/>
+      <c r="GH84" s="1"/>
+      <c r="GI84" s="1"/>
+      <c r="GJ84" s="1"/>
+      <c r="GK84" s="1"/>
+      <c r="GL84" s="1"/>
+      <c r="GM84" s="1"/>
+      <c r="GN84" s="1"/>
+      <c r="GO84" s="1"/>
+      <c r="GP84" s="1"/>
+      <c r="GQ84" s="1"/>
+      <c r="GR84" s="1"/>
+      <c r="GS84" s="1"/>
+      <c r="GT84" s="1"/>
+      <c r="GU84" s="1"/>
+      <c r="GV84" s="1"/>
+      <c r="GW84" s="1"/>
+      <c r="GX84" s="1"/>
+      <c r="GY84" s="1"/>
+      <c r="GZ84" s="1"/>
+      <c r="HA84" s="1"/>
+      <c r="HB84" s="1"/>
+      <c r="HC84" s="1"/>
+      <c r="HD84" s="1"/>
+      <c r="HE84" s="1"/>
+      <c r="HF84" s="1"/>
+      <c r="HG84" s="1"/>
+      <c r="HH84" s="1"/>
+      <c r="HI84" s="1"/>
+      <c r="HJ84" s="1"/>
+      <c r="HK84" s="1"/>
+      <c r="HL84" s="1"/>
+      <c r="HM84" s="1"/>
+      <c r="HN84" s="1"/>
+      <c r="HO84" s="1"/>
+      <c r="HP84" s="1"/>
+      <c r="HQ84" s="1"/>
+      <c r="HR84" s="1"/>
+      <c r="HS84" s="1"/>
+      <c r="HT84" s="1"/>
+      <c r="HU84" s="1"/>
+      <c r="HV84" s="1"/>
+      <c r="HW84" s="1"/>
+      <c r="HX84" s="1"/>
+      <c r="HY84" s="1"/>
+      <c r="HZ84" s="1"/>
+      <c r="IA84" s="1"/>
+      <c r="IB84" s="1"/>
+      <c r="IC84" s="1"/>
+      <c r="ID84" s="1"/>
+      <c r="IE84" s="1"/>
+      <c r="IF84" s="1"/>
+      <c r="IG84" s="1"/>
+      <c r="IH84" s="1"/>
+      <c r="II84" s="1"/>
+      <c r="IJ84" s="1"/>
+      <c r="IK84" s="1"/>
+      <c r="IL84" s="1"/>
+      <c r="IM84" s="1"/>
+      <c r="IN84" s="1"/>
+      <c r="IO84" s="1"/>
+      <c r="IP84" s="1"/>
+      <c r="IQ84" s="1"/>
+      <c r="IR84" s="1"/>
+      <c r="IS84" s="1"/>
+      <c r="IT84" s="1"/>
+      <c r="IU84" s="1"/>
+      <c r="IV84" s="1"/>
     </row>
-    <row r="85" spans="1:256" ht="15.95" customHeight="1"/>
-    <row r="86" spans="1:256" ht="15.95" customHeight="1"/>
+    <row r="85" spans="1:256" ht="15.75" customHeight="1">
+      <c r="E85" s="1"/>
+      <c r="F85" s="1"/>
+      <c r="G85" s="1"/>
+      <c r="H85" s="1"/>
+      <c r="I85" s="5"/>
+      <c r="J85" s="5"/>
+      <c r="K85" s="5"/>
+      <c r="L85" s="5"/>
+      <c r="M85" s="5"/>
+      <c r="N85" s="5"/>
+      <c r="O85" s="5"/>
+      <c r="P85" s="5"/>
+      <c r="Q85" s="5"/>
+      <c r="R85" s="5"/>
+      <c r="S85" s="1"/>
+      <c r="T85" s="1"/>
+      <c r="U85" s="1"/>
+      <c r="V85" s="1"/>
+      <c r="W85" s="1"/>
+      <c r="X85" s="1"/>
+      <c r="Y85" s="1"/>
+      <c r="Z85" s="1"/>
+      <c r="AA85" s="1"/>
+      <c r="AB85" s="1"/>
+      <c r="AC85" s="1"/>
+      <c r="AD85" s="1"/>
+      <c r="AE85" s="1"/>
+      <c r="AF85" s="1"/>
+      <c r="AG85" s="1"/>
+      <c r="AH85" s="1"/>
+      <c r="AI85" s="1"/>
+      <c r="AJ85" s="1"/>
+      <c r="AK85" s="1"/>
+      <c r="AL85" s="1"/>
+      <c r="AM85" s="1"/>
+      <c r="AN85" s="1"/>
+      <c r="AO85" s="1"/>
+      <c r="AP85" s="1"/>
+      <c r="AQ85" s="1"/>
+      <c r="AR85" s="1"/>
+      <c r="AS85" s="1"/>
+      <c r="AT85" s="1"/>
+      <c r="AU85" s="1"/>
+      <c r="AV85" s="1"/>
+      <c r="AW85" s="1"/>
+      <c r="AX85" s="1"/>
+      <c r="AY85" s="1"/>
+      <c r="AZ85" s="1"/>
+      <c r="BA85" s="1"/>
+      <c r="BB85" s="1"/>
+      <c r="BC85" s="1"/>
+      <c r="BD85" s="1"/>
+      <c r="BE85" s="1"/>
+      <c r="BF85" s="1"/>
+      <c r="BG85" s="1"/>
+      <c r="BH85" s="1"/>
+      <c r="BI85" s="1"/>
+      <c r="BJ85" s="1"/>
+      <c r="BK85" s="1"/>
+      <c r="BL85" s="1"/>
+      <c r="BM85" s="1"/>
+      <c r="BN85" s="1"/>
+      <c r="BO85" s="1"/>
+      <c r="BP85" s="1"/>
+      <c r="BQ85" s="1"/>
+      <c r="BR85" s="1"/>
+      <c r="BS85" s="1"/>
+      <c r="BT85" s="1"/>
+      <c r="BU85" s="1"/>
+      <c r="BV85" s="1"/>
+      <c r="BW85" s="1"/>
+      <c r="BX85" s="1"/>
+      <c r="BY85" s="1"/>
+      <c r="BZ85" s="1"/>
+      <c r="CA85" s="1"/>
+      <c r="CB85" s="1"/>
+      <c r="CC85" s="1"/>
+      <c r="CD85" s="1"/>
+      <c r="CE85" s="1"/>
+      <c r="CF85" s="1"/>
+      <c r="CG85" s="1"/>
+      <c r="CH85" s="1"/>
+      <c r="CI85" s="1"/>
+      <c r="CJ85" s="1"/>
+      <c r="CK85" s="1"/>
+      <c r="CL85" s="1"/>
+      <c r="CM85" s="1"/>
+      <c r="CN85" s="1"/>
+      <c r="CO85" s="1"/>
+      <c r="CP85" s="1"/>
+      <c r="CQ85" s="1"/>
+      <c r="CR85" s="1"/>
+      <c r="CS85" s="1"/>
+      <c r="CT85" s="1"/>
+      <c r="CU85" s="1"/>
+      <c r="CV85" s="1"/>
+      <c r="CW85" s="1"/>
+      <c r="CX85" s="1"/>
+      <c r="CY85" s="1"/>
+      <c r="CZ85" s="1"/>
+      <c r="DA85" s="1"/>
+      <c r="DB85" s="1"/>
+      <c r="DC85" s="1"/>
+      <c r="DD85" s="1"/>
+      <c r="DE85" s="1"/>
+      <c r="DF85" s="1"/>
+      <c r="DG85" s="1"/>
+      <c r="DH85" s="1"/>
+      <c r="DI85" s="1"/>
+      <c r="DJ85" s="1"/>
+      <c r="DK85" s="1"/>
+      <c r="DL85" s="1"/>
+      <c r="DM85" s="1"/>
+      <c r="DN85" s="1"/>
+      <c r="DO85" s="1"/>
+      <c r="DP85" s="1"/>
+      <c r="DQ85" s="1"/>
+      <c r="DR85" s="1"/>
+      <c r="DS85" s="1"/>
+      <c r="DT85" s="1"/>
+      <c r="DU85" s="1"/>
+      <c r="DV85" s="1"/>
+      <c r="DW85" s="1"/>
+      <c r="DX85" s="1"/>
+      <c r="DY85" s="1"/>
+      <c r="DZ85" s="1"/>
+      <c r="EA85" s="1"/>
+      <c r="EB85" s="1"/>
+      <c r="EC85" s="1"/>
+      <c r="ED85" s="1"/>
+      <c r="EE85" s="1"/>
+      <c r="EF85" s="1"/>
+      <c r="EG85" s="1"/>
+      <c r="EH85" s="1"/>
+      <c r="EI85" s="1"/>
+      <c r="EJ85" s="1"/>
+      <c r="EK85" s="1"/>
+      <c r="EL85" s="1"/>
+      <c r="EM85" s="1"/>
+      <c r="EN85" s="1"/>
+      <c r="EO85" s="1"/>
+      <c r="EP85" s="1"/>
+      <c r="EQ85" s="1"/>
+      <c r="ER85" s="1"/>
+      <c r="ES85" s="1"/>
+      <c r="ET85" s="1"/>
+      <c r="EU85" s="1"/>
+      <c r="EV85" s="1"/>
+      <c r="EW85" s="1"/>
+      <c r="EX85" s="1"/>
+      <c r="EY85" s="1"/>
+      <c r="EZ85" s="1"/>
+      <c r="FA85" s="1"/>
+      <c r="FB85" s="1"/>
+      <c r="FC85" s="1"/>
+      <c r="FD85" s="1"/>
+      <c r="FE85" s="1"/>
+      <c r="FF85" s="1"/>
+      <c r="FG85" s="1"/>
+      <c r="FH85" s="1"/>
+      <c r="FI85" s="1"/>
+      <c r="FJ85" s="1"/>
+      <c r="FK85" s="1"/>
+      <c r="FL85" s="1"/>
+      <c r="FM85" s="1"/>
+      <c r="FN85" s="1"/>
+      <c r="FO85" s="1"/>
+      <c r="FP85" s="1"/>
+      <c r="FQ85" s="1"/>
+      <c r="FR85" s="1"/>
+      <c r="FS85" s="1"/>
+      <c r="FT85" s="1"/>
+      <c r="FU85" s="1"/>
+      <c r="FV85" s="1"/>
+      <c r="FW85" s="1"/>
+      <c r="FX85" s="1"/>
+      <c r="FY85" s="1"/>
+      <c r="FZ85" s="1"/>
+      <c r="GA85" s="1"/>
+      <c r="GB85" s="1"/>
+      <c r="GC85" s="1"/>
+      <c r="GD85" s="1"/>
+      <c r="GE85" s="1"/>
+      <c r="GF85" s="1"/>
+      <c r="GG85" s="1"/>
+      <c r="GH85" s="1"/>
+      <c r="GI85" s="1"/>
+      <c r="GJ85" s="1"/>
+      <c r="GK85" s="1"/>
+      <c r="GL85" s="1"/>
+      <c r="GM85" s="1"/>
+      <c r="GN85" s="1"/>
+      <c r="GO85" s="1"/>
+      <c r="GP85" s="1"/>
+      <c r="GQ85" s="1"/>
+      <c r="GR85" s="1"/>
+      <c r="GS85" s="1"/>
+      <c r="GT85" s="1"/>
+      <c r="GU85" s="1"/>
+      <c r="GV85" s="1"/>
+      <c r="GW85" s="1"/>
+      <c r="GX85" s="1"/>
+      <c r="GY85" s="1"/>
+      <c r="GZ85" s="1"/>
+      <c r="HA85" s="1"/>
+      <c r="HB85" s="1"/>
+      <c r="HC85" s="1"/>
+      <c r="HD85" s="1"/>
+      <c r="HE85" s="1"/>
+      <c r="HF85" s="1"/>
+      <c r="HG85" s="1"/>
+      <c r="HH85" s="1"/>
+      <c r="HI85" s="1"/>
+      <c r="HJ85" s="1"/>
+      <c r="HK85" s="1"/>
+      <c r="HL85" s="1"/>
+      <c r="HM85" s="1"/>
+      <c r="HN85" s="1"/>
+      <c r="HO85" s="1"/>
+      <c r="HP85" s="1"/>
+      <c r="HQ85" s="1"/>
+      <c r="HR85" s="1"/>
+      <c r="HS85" s="1"/>
+      <c r="HT85" s="1"/>
+      <c r="HU85" s="1"/>
+      <c r="HV85" s="1"/>
+      <c r="HW85" s="1"/>
+      <c r="HX85" s="1"/>
+      <c r="HY85" s="1"/>
+      <c r="HZ85" s="1"/>
+      <c r="IA85" s="1"/>
+      <c r="IB85" s="1"/>
+      <c r="IC85" s="1"/>
+      <c r="ID85" s="1"/>
+      <c r="IE85" s="1"/>
+      <c r="IF85" s="1"/>
+      <c r="IG85" s="1"/>
+      <c r="IH85" s="1"/>
+      <c r="II85" s="1"/>
+      <c r="IJ85" s="1"/>
+      <c r="IK85" s="1"/>
+      <c r="IL85" s="1"/>
+      <c r="IM85" s="1"/>
+      <c r="IN85" s="1"/>
+      <c r="IO85" s="1"/>
+      <c r="IP85" s="1"/>
+      <c r="IQ85" s="1"/>
+      <c r="IR85" s="1"/>
+      <c r="IS85" s="1"/>
+      <c r="IT85" s="1"/>
+      <c r="IU85" s="1"/>
+      <c r="IV85" s="1"/>
+    </row>
+    <row r="86" spans="1:256" ht="12" customHeight="1">
+      <c r="I86" s="5"/>
+      <c r="J86" s="5"/>
+      <c r="K86" s="5"/>
+      <c r="L86" s="5"/>
+      <c r="M86" s="5"/>
+      <c r="N86" s="5"/>
+      <c r="O86" s="5"/>
+      <c r="P86" s="5"/>
+      <c r="Q86" s="5"/>
+      <c r="R86" s="5"/>
+    </row>
     <row r="87" spans="1:256" ht="15.95" customHeight="1"/>
     <row r="88" spans="1:256" ht="15.95" customHeight="1"/>
     <row r="89" spans="1:256" ht="15.95" customHeight="1"/>
@@ -21033,128 +21565,128 @@
     <row r="102" spans="1:16" ht="15.95" customHeight="1"/>
     <row r="103" spans="1:16" ht="15.95" customHeight="1"/>
     <row r="104" spans="1:16" ht="15.95" customHeight="1"/>
-    <row r="105" spans="1:16" ht="15.95" customHeight="1">
-      <c r="A105" s="64" t="s">
+    <row r="105" spans="1:16" ht="15.95" customHeight="1"/>
+    <row r="106" spans="1:16" ht="15.95" customHeight="1"/>
+    <row r="107" spans="1:16" ht="15.95" customHeight="1">
+      <c r="A107" s="62" t="s">
         <v>190</v>
       </c>
-      <c r="B105" s="64"/>
-      <c r="C105" s="64"/>
-      <c r="D105" s="64"/>
-      <c r="E105" s="64"/>
-      <c r="F105" s="64"/>
-      <c r="G105" s="64"/>
-      <c r="H105" s="64"/>
-      <c r="I105" s="64"/>
-      <c r="J105" s="64"/>
-      <c r="K105" s="64"/>
-      <c r="L105" s="64"/>
-      <c r="M105" s="64"/>
-      <c r="N105" s="64"/>
-      <c r="O105" s="64"/>
-      <c r="P105" s="64"/>
+      <c r="B107" s="62"/>
+      <c r="C107" s="62"/>
+      <c r="D107" s="62"/>
+      <c r="E107" s="62"/>
+      <c r="F107" s="62"/>
+      <c r="G107" s="62"/>
+      <c r="H107" s="62"/>
+      <c r="I107" s="62"/>
+      <c r="J107" s="62"/>
+      <c r="K107" s="62"/>
+      <c r="L107" s="62"/>
+      <c r="M107" s="62"/>
+      <c r="N107" s="62"/>
+      <c r="O107" s="62"/>
+      <c r="P107" s="62"/>
     </row>
-    <row r="106" spans="1:16" ht="15.95" customHeight="1">
-      <c r="A106" s="20" t="s">
+    <row r="108" spans="1:16" ht="15.95" customHeight="1">
+      <c r="A108" s="20" t="s">
         <v>191</v>
       </c>
-      <c r="B106" s="20" t="s">
+      <c r="B108" s="20" t="s">
         <v>192</v>
       </c>
-      <c r="C106" s="20" t="s">
+      <c r="C108" s="20" t="s">
         <v>193</v>
       </c>
-      <c r="D106" s="20" t="s">
+      <c r="D108" s="20" t="s">
         <v>194</v>
       </c>
-      <c r="E106" s="20" t="s">
+      <c r="E108" s="20" t="s">
         <v>195</v>
       </c>
-      <c r="F106" s="20" t="s">
+      <c r="F108" s="20" t="s">
         <v>196</v>
       </c>
-      <c r="G106" s="20" t="s">
+      <c r="G108" s="20" t="s">
         <v>197</v>
       </c>
-      <c r="H106" s="20" t="s">
+      <c r="H108" s="20" t="s">
         <v>198</v>
       </c>
-      <c r="I106" s="20" t="s">
+      <c r="I108" s="20" t="s">
         <v>199</v>
       </c>
-      <c r="J106" s="20" t="s">
+      <c r="J108" s="20" t="s">
         <v>200</v>
       </c>
-      <c r="K106" s="20" t="s">
+      <c r="K108" s="20" t="s">
         <v>201</v>
       </c>
-      <c r="L106" s="20" t="s">
+      <c r="L108" s="20" t="s">
         <v>202</v>
       </c>
-      <c r="M106" s="20" t="s">
+      <c r="M108" s="20" t="s">
         <v>203</v>
       </c>
-      <c r="N106" s="20" t="s">
+      <c r="N108" s="20" t="s">
         <v>204</v>
       </c>
-      <c r="O106" s="20" t="s">
+      <c r="O108" s="20" t="s">
         <v>205</v>
       </c>
-      <c r="P106" s="20" t="s">
+      <c r="P108" s="20" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="107" spans="1:16" ht="15.95" customHeight="1">
-      <c r="A107" s="22" t="s">
+    <row r="109" spans="1:16" ht="15.95" customHeight="1">
+      <c r="A109" s="22" t="s">
         <v>207</v>
       </c>
-      <c r="B107" s="22" t="s">
+      <c r="B109" s="22" t="s">
         <v>208</v>
       </c>
-      <c r="C107" s="22" t="s">
+      <c r="C109" s="22" t="s">
         <v>209</v>
       </c>
-      <c r="D107" s="22" t="s">
+      <c r="D109" s="22" t="s">
         <v>210</v>
       </c>
-      <c r="E107" s="22" t="s">
+      <c r="E109" s="22" t="s">
         <v>211</v>
       </c>
-      <c r="F107" s="22" t="s">
+      <c r="F109" s="22" t="s">
         <v>212</v>
       </c>
-      <c r="G107" s="22" t="s">
+      <c r="G109" s="22" t="s">
         <v>213</v>
       </c>
-      <c r="H107" s="22" t="s">
+      <c r="H109" s="22" t="s">
         <v>214</v>
       </c>
-      <c r="I107" s="22" t="s">
+      <c r="I109" s="22" t="s">
         <v>215</v>
       </c>
-      <c r="J107" s="22" t="s">
+      <c r="J109" s="22" t="s">
         <v>216</v>
       </c>
-      <c r="K107" s="22" t="s">
+      <c r="K109" s="22" t="s">
         <v>217</v>
       </c>
-      <c r="L107" s="22" t="s">
+      <c r="L109" s="22" t="s">
         <v>218</v>
       </c>
-      <c r="M107" s="22" t="s">
+      <c r="M109" s="22" t="s">
         <v>219</v>
       </c>
-      <c r="N107" s="22" t="s">
+      <c r="N109" s="22" t="s">
         <v>220</v>
       </c>
-      <c r="O107" s="22" t="s">
+      <c r="O109" s="22" t="s">
         <v>221</v>
       </c>
-      <c r="P107" s="22" t="s">
+      <c r="P109" s="22" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="108" spans="1:16" ht="15.95" customHeight="1"/>
-    <row r="109" spans="1:16" ht="15.95" customHeight="1"/>
     <row r="110" spans="1:16" ht="15.95" customHeight="1"/>
     <row r="111" spans="1:16" ht="15.95" customHeight="1"/>
     <row r="112" spans="1:16" ht="15.95" customHeight="1"/>
@@ -21223,58 +21755,58 @@
     <row r="175" ht="15.95" customHeight="1"/>
     <row r="176" ht="15.95" customHeight="1"/>
     <row r="177" spans="1:6" ht="15.95" customHeight="1"/>
-    <row r="178" spans="1:6" ht="15.95" customHeight="1">
-      <c r="A178" s="64" t="s">
+    <row r="178" spans="1:6" ht="15.95" customHeight="1"/>
+    <row r="179" spans="1:6" ht="15.95" customHeight="1"/>
+    <row r="180" spans="1:6" ht="15.95" customHeight="1">
+      <c r="A180" s="62" t="s">
         <v>189</v>
       </c>
-      <c r="B178" s="64"/>
-      <c r="C178" s="64"/>
-      <c r="D178" s="64"/>
-      <c r="E178" s="64"/>
-      <c r="F178" s="64"/>
+      <c r="B180" s="62"/>
+      <c r="C180" s="62"/>
+      <c r="D180" s="62"/>
+      <c r="E180" s="62"/>
+      <c r="F180" s="62"/>
     </row>
-    <row r="179" spans="1:6" ht="15.95" customHeight="1">
-      <c r="A179" s="20" t="s">
+    <row r="181" spans="1:6" ht="15.95" customHeight="1">
+      <c r="A181" s="20" t="s">
         <v>223</v>
       </c>
-      <c r="B179" s="20" t="s">
+      <c r="B181" s="20" t="s">
         <v>224</v>
       </c>
-      <c r="C179" s="20" t="s">
+      <c r="C181" s="20" t="s">
         <v>225</v>
       </c>
-      <c r="D179" s="20" t="s">
+      <c r="D181" s="20" t="s">
         <v>226</v>
       </c>
-      <c r="E179" s="20" t="s">
+      <c r="E181" s="20" t="s">
         <v>227</v>
       </c>
-      <c r="F179" s="20" t="s">
+      <c r="F181" s="20" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="180" spans="1:6" ht="15.95" customHeight="1">
-      <c r="A180" s="22" t="s">
+    <row r="182" spans="1:6" ht="15.95" customHeight="1">
+      <c r="A182" s="22" t="s">
         <v>229</v>
       </c>
-      <c r="B180" s="22" t="s">
+      <c r="B182" s="22" t="s">
         <v>230</v>
       </c>
-      <c r="C180" s="22" t="s">
+      <c r="C182" s="22" t="s">
         <v>231</v>
       </c>
-      <c r="D180" s="22" t="s">
+      <c r="D182" s="22" t="s">
         <v>232</v>
       </c>
-      <c r="E180" s="22" t="s">
+      <c r="E182" s="22" t="s">
         <v>233</v>
       </c>
-      <c r="F180" s="22" t="s">
+      <c r="F182" s="22" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="181" spans="1:6" ht="15.95" customHeight="1"/>
-    <row r="182" spans="1:6" ht="15.95" customHeight="1"/>
     <row r="183" spans="1:6" ht="15.95" customHeight="1"/>
     <row r="184" spans="1:6" ht="15.95" customHeight="1"/>
     <row r="185" spans="1:6" ht="15.95" customHeight="1"/>
@@ -21390,30 +21922,30 @@
     <row r="295" spans="1:2" ht="15.95" customHeight="1"/>
     <row r="296" spans="1:2" ht="15.95" customHeight="1"/>
     <row r="297" spans="1:2" ht="15.95" customHeight="1"/>
-    <row r="298" spans="1:2" ht="15.95" customHeight="1">
-      <c r="A298" s="64" t="s">
+    <row r="298" spans="1:2" ht="15.95" customHeight="1"/>
+    <row r="299" spans="1:2" ht="15.95" customHeight="1"/>
+    <row r="300" spans="1:2" ht="15.95" customHeight="1">
+      <c r="A300" s="62" t="s">
         <v>278</v>
       </c>
-      <c r="B298" s="64"/>
+      <c r="B300" s="62"/>
     </row>
-    <row r="299" spans="1:2" ht="15.95" customHeight="1">
-      <c r="A299" s="20" t="s">
+    <row r="301" spans="1:2" ht="15.95" customHeight="1">
+      <c r="A301" s="20" t="s">
         <v>279</v>
       </c>
-      <c r="B299" s="21" t="s">
+      <c r="B301" s="21" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="300" spans="1:2" ht="15.95" customHeight="1">
-      <c r="A300" s="22" t="s">
+    <row r="302" spans="1:2" ht="15.95" customHeight="1">
+      <c r="A302" s="22" t="s">
         <v>281</v>
       </c>
-      <c r="B300" s="22" t="s">
+      <c r="B302" s="22" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="301" spans="1:2" ht="15.95" customHeight="1"/>
-    <row r="302" spans="1:2" ht="15.95" customHeight="1"/>
     <row r="303" spans="1:2" ht="15.95" customHeight="1"/>
     <row r="304" spans="1:2" ht="15.95" customHeight="1"/>
     <row r="305" ht="15.95" customHeight="1"/>
@@ -21436,58 +21968,58 @@
     <row r="322" spans="1:6" ht="15.95" customHeight="1"/>
     <row r="323" spans="1:6" ht="15.95" customHeight="1"/>
     <row r="324" spans="1:6" ht="15.95" customHeight="1"/>
-    <row r="325" spans="1:6" ht="15.95" customHeight="1">
-      <c r="A325" s="60" t="s">
+    <row r="325" spans="1:6" ht="15.95" customHeight="1"/>
+    <row r="326" spans="1:6" ht="15.95" customHeight="1"/>
+    <row r="327" spans="1:6" ht="15.95" customHeight="1">
+      <c r="A327" s="58" t="s">
         <v>318</v>
       </c>
-      <c r="B325" s="60"/>
-      <c r="C325" s="60"/>
-      <c r="D325" s="60"/>
-      <c r="E325" s="60"/>
-      <c r="F325" s="60"/>
+      <c r="B327" s="58"/>
+      <c r="C327" s="58"/>
+      <c r="D327" s="58"/>
+      <c r="E327" s="58"/>
+      <c r="F327" s="58"/>
     </row>
-    <row r="326" spans="1:6" ht="15.95" customHeight="1">
-      <c r="A326" s="23" t="s">
+    <row r="328" spans="1:6" ht="15.95" customHeight="1">
+      <c r="A328" s="23" t="s">
         <v>307</v>
       </c>
-      <c r="B326" s="23" t="s">
+      <c r="B328" s="23" t="s">
         <v>308</v>
       </c>
-      <c r="C326" s="23" t="s">
+      <c r="C328" s="23" t="s">
         <v>309</v>
       </c>
-      <c r="D326" s="23" t="s">
+      <c r="D328" s="23" t="s">
         <v>310</v>
       </c>
-      <c r="E326" s="26" t="s">
+      <c r="E328" s="26" t="s">
         <v>227</v>
       </c>
-      <c r="F326" s="26" t="s">
+      <c r="F328" s="26" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="327" spans="1:6" ht="15.95" customHeight="1">
-      <c r="A327" s="24" t="s">
+    <row r="329" spans="1:6" ht="15.95" customHeight="1">
+      <c r="A329" s="24" t="s">
         <v>311</v>
       </c>
-      <c r="B327" s="24" t="s">
+      <c r="B329" s="24" t="s">
         <v>312</v>
       </c>
-      <c r="C327" s="24" t="s">
+      <c r="C329" s="24" t="s">
         <v>313</v>
       </c>
-      <c r="D327" s="24" t="s">
+      <c r="D329" s="24" t="s">
         <v>314</v>
       </c>
-      <c r="E327" s="24" t="s">
+      <c r="E329" s="24" t="s">
         <v>315</v>
       </c>
-      <c r="F327" s="24" t="s">
+      <c r="F329" s="24" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="328" spans="1:6" ht="15.95" customHeight="1"/>
-    <row r="329" spans="1:6" ht="15.95" customHeight="1"/>
     <row r="330" spans="1:6" ht="15.95" customHeight="1"/>
     <row r="331" spans="1:6" ht="15.95" customHeight="1"/>
     <row r="332" spans="1:6" ht="15.95" customHeight="1"/>
@@ -22207,18 +22739,20 @@
     <row r="1046" ht="15.95" customHeight="1"/>
     <row r="1047" ht="15.95" customHeight="1"/>
     <row r="1048" ht="15.95" customHeight="1"/>
+    <row r="1049" ht="15.95" customHeight="1"/>
+    <row r="1050" ht="15.95" customHeight="1"/>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A325:F325"/>
+    <mergeCell ref="A327:F327"/>
     <mergeCell ref="A1:A4"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="B3:E3"/>
-    <mergeCell ref="A298:B298"/>
-    <mergeCell ref="A178:F178"/>
-    <mergeCell ref="A105:P105"/>
-    <mergeCell ref="A79:B79"/>
-    <mergeCell ref="A69:B69"/>
-    <mergeCell ref="A62:C62"/>
+    <mergeCell ref="A300:B300"/>
+    <mergeCell ref="A180:F180"/>
+    <mergeCell ref="A107:P107"/>
+    <mergeCell ref="A81:B81"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="A64:C64"/>
     <mergeCell ref="A27:C27"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
@@ -22246,12 +22780,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="58" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="23" t="s">
@@ -22310,11 +22844,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="67" t="s">
+      <c r="A1" s="65" t="s">
         <v>73</v>
       </c>
-      <c r="B1" s="67"/>
-      <c r="C1" s="67"/>
+      <c r="B1" s="65"/>
+      <c r="C1" s="65"/>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="23" t="s">
@@ -22372,11 +22906,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="66" t="s">
         <v>79</v>
       </c>
-      <c r="B1" s="68"/>
-      <c r="C1" s="68"/>
+      <c r="B1" s="66"/>
+      <c r="C1" s="66"/>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="23" t="s">
@@ -22434,11 +22968,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="66" t="s">
         <v>85</v>
       </c>
-      <c r="B1" s="68"/>
-      <c r="C1" s="68"/>
+      <c r="B1" s="66"/>
+      <c r="C1" s="66"/>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="23" t="s">
@@ -22496,11 +23030,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="66" t="s">
         <v>90</v>
       </c>
-      <c r="B1" s="68"/>
-      <c r="C1" s="68"/>
+      <c r="B1" s="66"/>
+      <c r="C1" s="66"/>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="7" t="s">
@@ -22558,11 +23092,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="66" t="s">
         <v>95</v>
       </c>
-      <c r="B1" s="68"/>
-      <c r="C1" s="68"/>
+      <c r="B1" s="66"/>
+      <c r="C1" s="66"/>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="7" t="s">
@@ -22624,32 +23158,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24">
-      <c r="A1" s="72" t="s">
+      <c r="A1" s="73" t="s">
         <v>100</v>
       </c>
-      <c r="B1" s="73"/>
-      <c r="C1" s="73"/>
-      <c r="D1" s="73"/>
-      <c r="E1" s="73"/>
-      <c r="F1" s="73"/>
-      <c r="G1" s="73"/>
-      <c r="H1" s="73"/>
-      <c r="I1" s="73"/>
-      <c r="J1" s="73"/>
-      <c r="K1" s="73"/>
-      <c r="L1" s="73"/>
-      <c r="M1" s="73"/>
-      <c r="N1" s="73"/>
-      <c r="O1" s="73"/>
-      <c r="P1" s="73"/>
-      <c r="Q1" s="73"/>
-      <c r="R1" s="73"/>
-      <c r="S1" s="73"/>
-      <c r="T1" s="73"/>
-      <c r="U1" s="73"/>
-      <c r="V1" s="73"/>
-      <c r="W1" s="73"/>
-      <c r="X1" s="73"/>
+      <c r="B1" s="74"/>
+      <c r="C1" s="74"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
+      <c r="F1" s="74"/>
+      <c r="G1" s="74"/>
+      <c r="H1" s="74"/>
+      <c r="I1" s="74"/>
+      <c r="J1" s="74"/>
+      <c r="K1" s="74"/>
+      <c r="L1" s="74"/>
+      <c r="M1" s="74"/>
+      <c r="N1" s="74"/>
+      <c r="O1" s="74"/>
+      <c r="P1" s="74"/>
+      <c r="Q1" s="74"/>
+      <c r="R1" s="74"/>
+      <c r="S1" s="74"/>
+      <c r="T1" s="74"/>
+      <c r="U1" s="74"/>
+      <c r="V1" s="74"/>
+      <c r="W1" s="74"/>
+      <c r="X1" s="74"/>
     </row>
     <row r="2" spans="1:24">
       <c r="A2" s="26" t="s">
@@ -22800,12 +23334,12 @@
       </c>
     </row>
     <row r="11" spans="1:24">
-      <c r="A11" s="69" t="s">
+      <c r="A11" s="67" t="s">
         <v>169</v>
       </c>
-      <c r="B11" s="70"/>
-      <c r="C11" s="70"/>
-      <c r="D11" s="71"/>
+      <c r="B11" s="68"/>
+      <c r="C11" s="68"/>
+      <c r="D11" s="72"/>
     </row>
     <row r="12" spans="1:24">
       <c r="A12" s="37" t="s">
@@ -22822,12 +23356,12 @@
       </c>
     </row>
     <row r="24" spans="1:4">
-      <c r="A24" s="69" t="s">
+      <c r="A24" s="67" t="s">
         <v>168</v>
       </c>
-      <c r="B24" s="70"/>
-      <c r="C24" s="70"/>
-      <c r="D24" s="71"/>
+      <c r="B24" s="68"/>
+      <c r="C24" s="68"/>
+      <c r="D24" s="72"/>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="37" t="s">
@@ -22844,12 +23378,12 @@
       </c>
     </row>
     <row r="38" spans="1:4">
-      <c r="A38" s="69" t="s">
+      <c r="A38" s="67" t="s">
         <v>283</v>
       </c>
-      <c r="B38" s="70"/>
-      <c r="C38" s="70"/>
-      <c r="D38" s="71"/>
+      <c r="B38" s="68"/>
+      <c r="C38" s="68"/>
+      <c r="D38" s="72"/>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="37" t="s">
@@ -22866,12 +23400,12 @@
       </c>
     </row>
     <row r="54" spans="1:8">
-      <c r="A54" s="69" t="s">
+      <c r="A54" s="67" t="s">
         <v>256</v>
       </c>
-      <c r="B54" s="70"/>
-      <c r="C54" s="70"/>
-      <c r="D54" s="71"/>
+      <c r="B54" s="68"/>
+      <c r="C54" s="68"/>
+      <c r="D54" s="72"/>
     </row>
     <row r="55" spans="1:8">
       <c r="A55" s="44" t="s">
@@ -22892,12 +23426,12 @@
       <c r="H55" s="46"/>
     </row>
     <row r="67" spans="1:4">
-      <c r="A67" s="69" t="s">
+      <c r="A67" s="67" t="s">
         <v>163</v>
       </c>
-      <c r="B67" s="70"/>
-      <c r="C67" s="70"/>
-      <c r="D67" s="71"/>
+      <c r="B67" s="68"/>
+      <c r="C67" s="68"/>
+      <c r="D67" s="72"/>
     </row>
     <row r="68" spans="1:4">
       <c r="A68" s="37" t="s">
@@ -22914,12 +23448,12 @@
       </c>
     </row>
     <row r="89" spans="1:4">
-      <c r="A89" s="69" t="s">
+      <c r="A89" s="67" t="s">
         <v>176</v>
       </c>
-      <c r="B89" s="70"/>
-      <c r="C89" s="70"/>
-      <c r="D89" s="71"/>
+      <c r="B89" s="68"/>
+      <c r="C89" s="68"/>
+      <c r="D89" s="72"/>
     </row>
     <row r="90" spans="1:4">
       <c r="A90" s="37" t="s">
@@ -22936,12 +23470,12 @@
       </c>
     </row>
     <row r="105" spans="1:8">
-      <c r="A105" s="69" t="s">
+      <c r="A105" s="67" t="s">
         <v>260</v>
       </c>
-      <c r="B105" s="70"/>
-      <c r="C105" s="70"/>
-      <c r="D105" s="71"/>
+      <c r="B105" s="68"/>
+      <c r="C105" s="68"/>
+      <c r="D105" s="72"/>
     </row>
     <row r="106" spans="1:8" s="47" customFormat="1">
       <c r="A106" s="44" t="s">
@@ -22962,12 +23496,12 @@
       <c r="H106" s="46"/>
     </row>
     <row r="120" spans="1:4">
-      <c r="A120" s="74" t="s">
+      <c r="A120" s="69" t="s">
         <v>181</v>
       </c>
-      <c r="B120" s="75"/>
-      <c r="C120" s="75"/>
-      <c r="D120" s="76"/>
+      <c r="B120" s="70"/>
+      <c r="C120" s="70"/>
+      <c r="D120" s="71"/>
     </row>
     <row r="121" spans="1:4" ht="60">
       <c r="A121" s="37" t="s">
@@ -22978,13 +23512,13 @@
       </c>
     </row>
     <row r="142" spans="1:5">
-      <c r="A142" s="77" t="s">
+      <c r="A142" s="75" t="s">
         <v>287</v>
       </c>
-      <c r="B142" s="78"/>
-      <c r="C142" s="78"/>
-      <c r="D142" s="78"/>
-      <c r="E142" s="78"/>
+      <c r="B142" s="76"/>
+      <c r="C142" s="76"/>
+      <c r="D142" s="76"/>
+      <c r="E142" s="76"/>
     </row>
     <row r="143" spans="1:5">
       <c r="A143" s="51" t="s">
@@ -23021,12 +23555,12 @@
       </c>
     </row>
     <row r="167" spans="1:4">
-      <c r="A167" s="69" t="s">
+      <c r="A167" s="67" t="s">
         <v>346</v>
       </c>
-      <c r="B167" s="70"/>
-      <c r="C167" s="70"/>
-      <c r="D167" s="71"/>
+      <c r="B167" s="68"/>
+      <c r="C167" s="68"/>
+      <c r="D167" s="72"/>
     </row>
     <row r="168" spans="1:4">
       <c r="A168" s="37" t="s">
@@ -23043,12 +23577,12 @@
       </c>
     </row>
     <row r="190" spans="1:4">
-      <c r="A190" s="69" t="s">
+      <c r="A190" s="67" t="s">
         <v>359</v>
       </c>
-      <c r="B190" s="70"/>
-      <c r="C190" s="70"/>
-      <c r="D190" s="71"/>
+      <c r="B190" s="68"/>
+      <c r="C190" s="68"/>
+      <c r="D190" s="72"/>
     </row>
     <row r="191" spans="1:4">
       <c r="A191" s="37" t="s">
@@ -23065,12 +23599,12 @@
       </c>
     </row>
     <row r="220" spans="1:4">
-      <c r="A220" s="69" t="s">
+      <c r="A220" s="67" t="s">
         <v>360</v>
       </c>
-      <c r="B220" s="70"/>
-      <c r="C220" s="70"/>
-      <c r="D220" s="71"/>
+      <c r="B220" s="68"/>
+      <c r="C220" s="68"/>
+      <c r="D220" s="72"/>
     </row>
     <row r="221" spans="1:4">
       <c r="A221" s="37" t="s">
@@ -23087,12 +23621,12 @@
       </c>
     </row>
     <row r="239" spans="1:4">
-      <c r="A239" s="74" t="s">
+      <c r="A239" s="69" t="s">
         <v>361</v>
       </c>
-      <c r="B239" s="75"/>
-      <c r="C239" s="75"/>
-      <c r="D239" s="76"/>
+      <c r="B239" s="70"/>
+      <c r="C239" s="70"/>
+      <c r="D239" s="71"/>
     </row>
     <row r="240" spans="1:4">
       <c r="A240" s="37" t="s">
@@ -23109,17 +23643,17 @@
       </c>
     </row>
     <row r="241" spans="2:4">
-      <c r="B241" s="58"/>
-      <c r="C241" s="58"/>
-      <c r="D241" s="58"/>
+      <c r="B241" s="56"/>
+      <c r="C241" s="56"/>
+      <c r="D241" s="56"/>
     </row>
     <row r="264" spans="1:4">
-      <c r="A264" s="74" t="s">
+      <c r="A264" s="69" t="s">
         <v>331</v>
       </c>
-      <c r="B264" s="75"/>
-      <c r="C264" s="75"/>
-      <c r="D264" s="76"/>
+      <c r="B264" s="70"/>
+      <c r="C264" s="70"/>
+      <c r="D264" s="71"/>
     </row>
     <row r="265" spans="1:4">
       <c r="A265" s="51" t="s">
@@ -23128,10 +23662,10 @@
       <c r="B265" s="51" t="s">
         <v>328</v>
       </c>
-      <c r="C265" s="59" t="s">
+      <c r="C265" s="57" t="s">
         <v>329</v>
       </c>
-      <c r="D265" s="59" t="s">
+      <c r="D265" s="57" t="s">
         <v>330</v>
       </c>
     </row>
@@ -23139,21 +23673,21 @@
       <c r="A266" t="s">
         <v>333</v>
       </c>
-      <c r="B266" s="58" t="s">
+      <c r="B266" s="56" t="s">
         <v>366</v>
       </c>
-      <c r="C266" s="58" t="s">
+      <c r="C266" s="56" t="s">
         <v>367</v>
       </c>
-      <c r="D266" s="58" t="s">
+      <c r="D266" s="56" t="s">
         <v>368</v>
       </c>
     </row>
     <row r="300" spans="1:2">
-      <c r="A300" s="69" t="s">
+      <c r="A300" s="67" t="s">
         <v>334</v>
       </c>
-      <c r="B300" s="70"/>
+      <c r="B300" s="68"/>
     </row>
     <row r="301" spans="1:2">
       <c r="A301" s="26" t="s">
@@ -23172,10 +23706,10 @@
       </c>
     </row>
     <row r="320" spans="1:2">
-      <c r="A320" s="69" t="s">
+      <c r="A320" s="67" t="s">
         <v>337</v>
       </c>
-      <c r="B320" s="70"/>
+      <c r="B320" s="68"/>
     </row>
     <row r="321" spans="1:2">
       <c r="A321" s="26" t="s">
@@ -23194,10 +23728,10 @@
       </c>
     </row>
     <row r="340" spans="1:2">
-      <c r="A340" s="69" t="s">
+      <c r="A340" s="67" t="s">
         <v>340</v>
       </c>
-      <c r="B340" s="70"/>
+      <c r="B340" s="68"/>
     </row>
     <row r="341" spans="1:2">
       <c r="A341" s="26" t="s">
@@ -23216,10 +23750,10 @@
       </c>
     </row>
     <row r="355" spans="1:2">
-      <c r="A355" s="69" t="s">
+      <c r="A355" s="67" t="s">
         <v>343</v>
       </c>
-      <c r="B355" s="70"/>
+      <c r="B355" s="68"/>
     </row>
     <row r="356" spans="1:2">
       <c r="A356" s="26" t="s">
@@ -23239,12 +23773,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="A300:B300"/>
-    <mergeCell ref="A320:B320"/>
-    <mergeCell ref="A340:B340"/>
-    <mergeCell ref="A355:B355"/>
-    <mergeCell ref="A239:D239"/>
-    <mergeCell ref="A264:D264"/>
     <mergeCell ref="A220:D220"/>
     <mergeCell ref="A167:D167"/>
     <mergeCell ref="A190:D190"/>
@@ -23258,6 +23786,12 @@
     <mergeCell ref="A24:D24"/>
     <mergeCell ref="A54:D54"/>
     <mergeCell ref="A67:D67"/>
+    <mergeCell ref="A300:B300"/>
+    <mergeCell ref="A320:B320"/>
+    <mergeCell ref="A340:B340"/>
+    <mergeCell ref="A355:B355"/>
+    <mergeCell ref="A239:D239"/>
+    <mergeCell ref="A264:D264"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -23293,20 +23827,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
-      <c r="A1" s="79" t="s">
+      <c r="A1" s="77" t="s">
         <v>235</v>
       </c>
-      <c r="B1" s="80"/>
-      <c r="C1" s="80"/>
-      <c r="D1" s="80"/>
-      <c r="E1" s="80"/>
-      <c r="F1" s="80"/>
-      <c r="G1" s="80"/>
-      <c r="H1" s="80"/>
-      <c r="I1" s="80"/>
-      <c r="J1" s="80"/>
-      <c r="K1" s="80"/>
-      <c r="L1" s="80"/>
+      <c r="B1" s="78"/>
+      <c r="C1" s="78"/>
+      <c r="D1" s="78"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="78"/>
+      <c r="G1" s="78"/>
+      <c r="H1" s="78"/>
+      <c r="I1" s="78"/>
+      <c r="J1" s="78"/>
+      <c r="K1" s="78"/>
+      <c r="L1" s="78"/>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="39" t="s">

</xml_diff>

<commit_message>
POCOR-7449: updated excel pushed | Status: Done
</commit_message>
<xml_diff>
--- a/webroot/export/customexcel/default_templates/profile_template.xlsx
+++ b/webroot/export/customexcel/default_templates/profile_template.xlsx
@@ -1604,6 +1604,15 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -1612,15 +1621,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2007,7 +2007,7 @@
   <dimension ref="A1:IV1050"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="C54" sqref="C54"/>
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75"/>
@@ -23158,32 +23158,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24">
-      <c r="A1" s="73" t="s">
+      <c r="A1" s="70" t="s">
         <v>100</v>
       </c>
-      <c r="B1" s="74"/>
-      <c r="C1" s="74"/>
-      <c r="D1" s="74"/>
-      <c r="E1" s="74"/>
-      <c r="F1" s="74"/>
-      <c r="G1" s="74"/>
-      <c r="H1" s="74"/>
-      <c r="I1" s="74"/>
-      <c r="J1" s="74"/>
-      <c r="K1" s="74"/>
-      <c r="L1" s="74"/>
-      <c r="M1" s="74"/>
-      <c r="N1" s="74"/>
-      <c r="O1" s="74"/>
-      <c r="P1" s="74"/>
-      <c r="Q1" s="74"/>
-      <c r="R1" s="74"/>
-      <c r="S1" s="74"/>
-      <c r="T1" s="74"/>
-      <c r="U1" s="74"/>
-      <c r="V1" s="74"/>
-      <c r="W1" s="74"/>
-      <c r="X1" s="74"/>
+      <c r="B1" s="71"/>
+      <c r="C1" s="71"/>
+      <c r="D1" s="71"/>
+      <c r="E1" s="71"/>
+      <c r="F1" s="71"/>
+      <c r="G1" s="71"/>
+      <c r="H1" s="71"/>
+      <c r="I1" s="71"/>
+      <c r="J1" s="71"/>
+      <c r="K1" s="71"/>
+      <c r="L1" s="71"/>
+      <c r="M1" s="71"/>
+      <c r="N1" s="71"/>
+      <c r="O1" s="71"/>
+      <c r="P1" s="71"/>
+      <c r="Q1" s="71"/>
+      <c r="R1" s="71"/>
+      <c r="S1" s="71"/>
+      <c r="T1" s="71"/>
+      <c r="U1" s="71"/>
+      <c r="V1" s="71"/>
+      <c r="W1" s="71"/>
+      <c r="X1" s="71"/>
     </row>
     <row r="2" spans="1:24">
       <c r="A2" s="26" t="s">
@@ -23339,7 +23339,7 @@
       </c>
       <c r="B11" s="68"/>
       <c r="C11" s="68"/>
-      <c r="D11" s="72"/>
+      <c r="D11" s="69"/>
     </row>
     <row r="12" spans="1:24">
       <c r="A12" s="37" t="s">
@@ -23361,7 +23361,7 @@
       </c>
       <c r="B24" s="68"/>
       <c r="C24" s="68"/>
-      <c r="D24" s="72"/>
+      <c r="D24" s="69"/>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="37" t="s">
@@ -23383,7 +23383,7 @@
       </c>
       <c r="B38" s="68"/>
       <c r="C38" s="68"/>
-      <c r="D38" s="72"/>
+      <c r="D38" s="69"/>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="37" t="s">
@@ -23405,7 +23405,7 @@
       </c>
       <c r="B54" s="68"/>
       <c r="C54" s="68"/>
-      <c r="D54" s="72"/>
+      <c r="D54" s="69"/>
     </row>
     <row r="55" spans="1:8">
       <c r="A55" s="44" t="s">
@@ -23431,7 +23431,7 @@
       </c>
       <c r="B67" s="68"/>
       <c r="C67" s="68"/>
-      <c r="D67" s="72"/>
+      <c r="D67" s="69"/>
     </row>
     <row r="68" spans="1:4">
       <c r="A68" s="37" t="s">
@@ -23453,7 +23453,7 @@
       </c>
       <c r="B89" s="68"/>
       <c r="C89" s="68"/>
-      <c r="D89" s="72"/>
+      <c r="D89" s="69"/>
     </row>
     <row r="90" spans="1:4">
       <c r="A90" s="37" t="s">
@@ -23475,7 +23475,7 @@
       </c>
       <c r="B105" s="68"/>
       <c r="C105" s="68"/>
-      <c r="D105" s="72"/>
+      <c r="D105" s="69"/>
     </row>
     <row r="106" spans="1:8" s="47" customFormat="1">
       <c r="A106" s="44" t="s">
@@ -23496,12 +23496,12 @@
       <c r="H106" s="46"/>
     </row>
     <row r="120" spans="1:4">
-      <c r="A120" s="69" t="s">
+      <c r="A120" s="72" t="s">
         <v>181</v>
       </c>
-      <c r="B120" s="70"/>
-      <c r="C120" s="70"/>
-      <c r="D120" s="71"/>
+      <c r="B120" s="73"/>
+      <c r="C120" s="73"/>
+      <c r="D120" s="74"/>
     </row>
     <row r="121" spans="1:4" ht="60">
       <c r="A121" s="37" t="s">
@@ -23560,7 +23560,7 @@
       </c>
       <c r="B167" s="68"/>
       <c r="C167" s="68"/>
-      <c r="D167" s="72"/>
+      <c r="D167" s="69"/>
     </row>
     <row r="168" spans="1:4">
       <c r="A168" s="37" t="s">
@@ -23582,7 +23582,7 @@
       </c>
       <c r="B190" s="68"/>
       <c r="C190" s="68"/>
-      <c r="D190" s="72"/>
+      <c r="D190" s="69"/>
     </row>
     <row r="191" spans="1:4">
       <c r="A191" s="37" t="s">
@@ -23604,7 +23604,7 @@
       </c>
       <c r="B220" s="68"/>
       <c r="C220" s="68"/>
-      <c r="D220" s="72"/>
+      <c r="D220" s="69"/>
     </row>
     <row r="221" spans="1:4">
       <c r="A221" s="37" t="s">
@@ -23621,12 +23621,12 @@
       </c>
     </row>
     <row r="239" spans="1:4">
-      <c r="A239" s="69" t="s">
+      <c r="A239" s="72" t="s">
         <v>361</v>
       </c>
-      <c r="B239" s="70"/>
-      <c r="C239" s="70"/>
-      <c r="D239" s="71"/>
+      <c r="B239" s="73"/>
+      <c r="C239" s="73"/>
+      <c r="D239" s="74"/>
     </row>
     <row r="240" spans="1:4">
       <c r="A240" s="37" t="s">
@@ -23648,12 +23648,12 @@
       <c r="D241" s="56"/>
     </row>
     <row r="264" spans="1:4">
-      <c r="A264" s="69" t="s">
+      <c r="A264" s="72" t="s">
         <v>331</v>
       </c>
-      <c r="B264" s="70"/>
-      <c r="C264" s="70"/>
-      <c r="D264" s="71"/>
+      <c r="B264" s="73"/>
+      <c r="C264" s="73"/>
+      <c r="D264" s="74"/>
     </row>
     <row r="265" spans="1:4">
       <c r="A265" s="51" t="s">
@@ -23773,6 +23773,12 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="A300:B300"/>
+    <mergeCell ref="A320:B320"/>
+    <mergeCell ref="A340:B340"/>
+    <mergeCell ref="A355:B355"/>
+    <mergeCell ref="A239:D239"/>
+    <mergeCell ref="A264:D264"/>
     <mergeCell ref="A220:D220"/>
     <mergeCell ref="A167:D167"/>
     <mergeCell ref="A190:D190"/>
@@ -23786,12 +23792,6 @@
     <mergeCell ref="A24:D24"/>
     <mergeCell ref="A54:D54"/>
     <mergeCell ref="A67:D67"/>
-    <mergeCell ref="A300:B300"/>
-    <mergeCell ref="A320:B320"/>
-    <mergeCell ref="A340:B340"/>
-    <mergeCell ref="A355:B355"/>
-    <mergeCell ref="A239:D239"/>
-    <mergeCell ref="A264:D264"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
POCOR-7694: code enhance for adding public holiday | Status: Done
</commit_message>
<xml_diff>
--- a/webroot/export/customexcel/default_templates/profile_template.xlsx
+++ b/webroot/export/customexcel/default_templates/profile_template.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="373">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="375">
   <si>
     <t>${"image":{"displayValue":"Institutions.logo_content","imageWidth":"100","imageMarginLeft":"20","imageMarginTop":"5"}}</t>
   </si>
@@ -1148,6 +1148,12 @@
   </si>
   <si>
     <t>${TeachingStaffTotalAbsences}</t>
+  </si>
+  <si>
+    <t>Public Holidays</t>
+  </si>
+  <si>
+    <t>${PublicHolidays}</t>
   </si>
 </sst>
 </file>
@@ -1604,6 +1610,15 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1612,15 +1627,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2004,10 +2010,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:IV1050"/>
+  <dimension ref="A1:IV1051"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75"/>
@@ -12650,8 +12656,12 @@
       <c r="IV48" s="1"/>
     </row>
     <row r="49" spans="1:256" ht="12" customHeight="1">
-      <c r="A49" s="15"/>
-      <c r="B49" s="16"/>
+      <c r="A49" s="55" t="s">
+        <v>373</v>
+      </c>
+      <c r="B49" s="19" t="s">
+        <v>374</v>
+      </c>
       <c r="C49" s="16"/>
       <c r="D49" s="16"/>
       <c r="E49" s="12"/>
@@ -12908,270 +12918,11 @@
       <c r="IV49" s="1"/>
     </row>
     <row r="50" spans="1:256" ht="12" customHeight="1">
-      <c r="A50" s="15"/>
-      <c r="B50" s="16"/>
-      <c r="C50" s="16"/>
-      <c r="D50" s="16"/>
-      <c r="E50" s="12"/>
-      <c r="F50" s="12"/>
-      <c r="G50" s="12"/>
-      <c r="H50" s="12"/>
-      <c r="I50" s="5"/>
-      <c r="J50" s="5"/>
-      <c r="K50" s="5"/>
-      <c r="L50" s="5"/>
-      <c r="M50" s="5"/>
-      <c r="N50" s="5"/>
-      <c r="O50" s="5"/>
-      <c r="P50" s="5"/>
-      <c r="Q50" s="5"/>
-      <c r="R50" s="5"/>
-      <c r="S50" s="1"/>
-      <c r="T50" s="1"/>
-      <c r="U50" s="1"/>
-      <c r="V50" s="1"/>
-      <c r="W50" s="1"/>
-      <c r="X50" s="1"/>
-      <c r="Y50" s="1"/>
-      <c r="Z50" s="1"/>
-      <c r="AA50" s="1"/>
-      <c r="AB50" s="1"/>
-      <c r="AC50" s="1"/>
-      <c r="AD50" s="1"/>
-      <c r="AE50" s="1"/>
-      <c r="AF50" s="1"/>
-      <c r="AG50" s="1"/>
-      <c r="AH50" s="1"/>
-      <c r="AI50" s="1"/>
-      <c r="AJ50" s="1"/>
-      <c r="AK50" s="1"/>
-      <c r="AL50" s="1"/>
-      <c r="AM50" s="1"/>
-      <c r="AN50" s="1"/>
-      <c r="AO50" s="1"/>
-      <c r="AP50" s="1"/>
-      <c r="AQ50" s="1"/>
-      <c r="AR50" s="1"/>
-      <c r="AS50" s="1"/>
-      <c r="AT50" s="1"/>
-      <c r="AU50" s="1"/>
-      <c r="AV50" s="1"/>
-      <c r="AW50" s="1"/>
-      <c r="AX50" s="1"/>
-      <c r="AY50" s="1"/>
-      <c r="AZ50" s="1"/>
-      <c r="BA50" s="1"/>
-      <c r="BB50" s="1"/>
-      <c r="BC50" s="1"/>
-      <c r="BD50" s="1"/>
-      <c r="BE50" s="1"/>
-      <c r="BF50" s="1"/>
-      <c r="BG50" s="1"/>
-      <c r="BH50" s="1"/>
-      <c r="BI50" s="1"/>
-      <c r="BJ50" s="1"/>
-      <c r="BK50" s="1"/>
-      <c r="BL50" s="1"/>
-      <c r="BM50" s="1"/>
-      <c r="BN50" s="1"/>
-      <c r="BO50" s="1"/>
-      <c r="BP50" s="1"/>
-      <c r="BQ50" s="1"/>
-      <c r="BR50" s="1"/>
-      <c r="BS50" s="1"/>
-      <c r="BT50" s="1"/>
-      <c r="BU50" s="1"/>
-      <c r="BV50" s="1"/>
-      <c r="BW50" s="1"/>
-      <c r="BX50" s="1"/>
-      <c r="BY50" s="1"/>
-      <c r="BZ50" s="1"/>
-      <c r="CA50" s="1"/>
-      <c r="CB50" s="1"/>
-      <c r="CC50" s="1"/>
-      <c r="CD50" s="1"/>
-      <c r="CE50" s="1"/>
-      <c r="CF50" s="1"/>
-      <c r="CG50" s="1"/>
-      <c r="CH50" s="1"/>
-      <c r="CI50" s="1"/>
-      <c r="CJ50" s="1"/>
-      <c r="CK50" s="1"/>
-      <c r="CL50" s="1"/>
-      <c r="CM50" s="1"/>
-      <c r="CN50" s="1"/>
-      <c r="CO50" s="1"/>
-      <c r="CP50" s="1"/>
-      <c r="CQ50" s="1"/>
-      <c r="CR50" s="1"/>
-      <c r="CS50" s="1"/>
-      <c r="CT50" s="1"/>
-      <c r="CU50" s="1"/>
-      <c r="CV50" s="1"/>
-      <c r="CW50" s="1"/>
-      <c r="CX50" s="1"/>
-      <c r="CY50" s="1"/>
-      <c r="CZ50" s="1"/>
-      <c r="DA50" s="1"/>
-      <c r="DB50" s="1"/>
-      <c r="DC50" s="1"/>
-      <c r="DD50" s="1"/>
-      <c r="DE50" s="1"/>
-      <c r="DF50" s="1"/>
-      <c r="DG50" s="1"/>
-      <c r="DH50" s="1"/>
-      <c r="DI50" s="1"/>
-      <c r="DJ50" s="1"/>
-      <c r="DK50" s="1"/>
-      <c r="DL50" s="1"/>
-      <c r="DM50" s="1"/>
-      <c r="DN50" s="1"/>
-      <c r="DO50" s="1"/>
-      <c r="DP50" s="1"/>
-      <c r="DQ50" s="1"/>
-      <c r="DR50" s="1"/>
-      <c r="DS50" s="1"/>
-      <c r="DT50" s="1"/>
-      <c r="DU50" s="1"/>
-      <c r="DV50" s="1"/>
-      <c r="DW50" s="1"/>
-      <c r="DX50" s="1"/>
-      <c r="DY50" s="1"/>
-      <c r="DZ50" s="1"/>
-      <c r="EA50" s="1"/>
-      <c r="EB50" s="1"/>
-      <c r="EC50" s="1"/>
-      <c r="ED50" s="1"/>
-      <c r="EE50" s="1"/>
-      <c r="EF50" s="1"/>
-      <c r="EG50" s="1"/>
-      <c r="EH50" s="1"/>
-      <c r="EI50" s="1"/>
-      <c r="EJ50" s="1"/>
-      <c r="EK50" s="1"/>
-      <c r="EL50" s="1"/>
-      <c r="EM50" s="1"/>
-      <c r="EN50" s="1"/>
-      <c r="EO50" s="1"/>
-      <c r="EP50" s="1"/>
-      <c r="EQ50" s="1"/>
-      <c r="ER50" s="1"/>
-      <c r="ES50" s="1"/>
-      <c r="ET50" s="1"/>
-      <c r="EU50" s="1"/>
-      <c r="EV50" s="1"/>
-      <c r="EW50" s="1"/>
-      <c r="EX50" s="1"/>
-      <c r="EY50" s="1"/>
-      <c r="EZ50" s="1"/>
-      <c r="FA50" s="1"/>
-      <c r="FB50" s="1"/>
-      <c r="FC50" s="1"/>
-      <c r="FD50" s="1"/>
-      <c r="FE50" s="1"/>
-      <c r="FF50" s="1"/>
-      <c r="FG50" s="1"/>
-      <c r="FH50" s="1"/>
-      <c r="FI50" s="1"/>
-      <c r="FJ50" s="1"/>
-      <c r="FK50" s="1"/>
-      <c r="FL50" s="1"/>
-      <c r="FM50" s="1"/>
-      <c r="FN50" s="1"/>
-      <c r="FO50" s="1"/>
-      <c r="FP50" s="1"/>
-      <c r="FQ50" s="1"/>
-      <c r="FR50" s="1"/>
-      <c r="FS50" s="1"/>
-      <c r="FT50" s="1"/>
-      <c r="FU50" s="1"/>
-      <c r="FV50" s="1"/>
-      <c r="FW50" s="1"/>
-      <c r="FX50" s="1"/>
-      <c r="FY50" s="1"/>
-      <c r="FZ50" s="1"/>
-      <c r="GA50" s="1"/>
-      <c r="GB50" s="1"/>
-      <c r="GC50" s="1"/>
-      <c r="GD50" s="1"/>
-      <c r="GE50" s="1"/>
-      <c r="GF50" s="1"/>
-      <c r="GG50" s="1"/>
-      <c r="GH50" s="1"/>
-      <c r="GI50" s="1"/>
-      <c r="GJ50" s="1"/>
-      <c r="GK50" s="1"/>
-      <c r="GL50" s="1"/>
-      <c r="GM50" s="1"/>
-      <c r="GN50" s="1"/>
-      <c r="GO50" s="1"/>
-      <c r="GP50" s="1"/>
-      <c r="GQ50" s="1"/>
-      <c r="GR50" s="1"/>
-      <c r="GS50" s="1"/>
-      <c r="GT50" s="1"/>
-      <c r="GU50" s="1"/>
-      <c r="GV50" s="1"/>
-      <c r="GW50" s="1"/>
-      <c r="GX50" s="1"/>
-      <c r="GY50" s="1"/>
-      <c r="GZ50" s="1"/>
-      <c r="HA50" s="1"/>
-      <c r="HB50" s="1"/>
-      <c r="HC50" s="1"/>
-      <c r="HD50" s="1"/>
-      <c r="HE50" s="1"/>
-      <c r="HF50" s="1"/>
-      <c r="HG50" s="1"/>
-      <c r="HH50" s="1"/>
-      <c r="HI50" s="1"/>
-      <c r="HJ50" s="1"/>
-      <c r="HK50" s="1"/>
-      <c r="HL50" s="1"/>
-      <c r="HM50" s="1"/>
-      <c r="HN50" s="1"/>
-      <c r="HO50" s="1"/>
-      <c r="HP50" s="1"/>
-      <c r="HQ50" s="1"/>
-      <c r="HR50" s="1"/>
-      <c r="HS50" s="1"/>
-      <c r="HT50" s="1"/>
-      <c r="HU50" s="1"/>
-      <c r="HV50" s="1"/>
-      <c r="HW50" s="1"/>
-      <c r="HX50" s="1"/>
-      <c r="HY50" s="1"/>
-      <c r="HZ50" s="1"/>
-      <c r="IA50" s="1"/>
-      <c r="IB50" s="1"/>
-      <c r="IC50" s="1"/>
-      <c r="ID50" s="1"/>
-      <c r="IE50" s="1"/>
-      <c r="IF50" s="1"/>
-      <c r="IG50" s="1"/>
-      <c r="IH50" s="1"/>
-      <c r="II50" s="1"/>
-      <c r="IJ50" s="1"/>
-      <c r="IK50" s="1"/>
-      <c r="IL50" s="1"/>
-      <c r="IM50" s="1"/>
-      <c r="IN50" s="1"/>
-      <c r="IO50" s="1"/>
-      <c r="IP50" s="1"/>
-      <c r="IQ50" s="1"/>
-      <c r="IR50" s="1"/>
-      <c r="IS50" s="1"/>
-      <c r="IT50" s="1"/>
-      <c r="IU50" s="1"/>
-      <c r="IV50" s="1"/>
+      <c r="D50"/>
     </row>
     <row r="51" spans="1:256" ht="12" customHeight="1">
-      <c r="A51" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="B51" s="19" t="s">
-        <v>50</v>
-      </c>
+      <c r="A51" s="15"/>
+      <c r="B51" s="16"/>
       <c r="C51" s="16"/>
       <c r="D51" s="16"/>
       <c r="E51" s="12"/>
@@ -13429,10 +13180,10 @@
     </row>
     <row r="52" spans="1:256" ht="12" customHeight="1">
       <c r="A52" s="9" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B52" s="19" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C52" s="16"/>
       <c r="D52" s="16"/>
@@ -13691,10 +13442,10 @@
     </row>
     <row r="53" spans="1:256" ht="12" customHeight="1">
       <c r="A53" s="9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B53" s="19" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C53" s="16"/>
       <c r="D53" s="16"/>
@@ -13953,10 +13704,10 @@
     </row>
     <row r="54" spans="1:256" ht="12" customHeight="1">
       <c r="A54" s="9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B54" s="19" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C54" s="16"/>
       <c r="D54" s="16"/>
@@ -14215,10 +13966,10 @@
     </row>
     <row r="55" spans="1:256" ht="12" customHeight="1">
       <c r="A55" s="9" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B55" s="19" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C55" s="16"/>
       <c r="D55" s="16"/>
@@ -14477,10 +14228,10 @@
     </row>
     <row r="56" spans="1:256" ht="12" customHeight="1">
       <c r="A56" s="9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B56" s="19" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C56" s="16"/>
       <c r="D56" s="16"/>
@@ -14739,10 +14490,10 @@
     </row>
     <row r="57" spans="1:256" ht="12" customHeight="1">
       <c r="A57" s="9" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B57" s="19" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C57" s="16"/>
       <c r="D57" s="16"/>
@@ -15001,9 +14752,11 @@
     </row>
     <row r="58" spans="1:256" ht="12" customHeight="1">
       <c r="A58" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="B58" s="19"/>
+        <v>61</v>
+      </c>
+      <c r="B58" s="19" t="s">
+        <v>62</v>
+      </c>
       <c r="C58" s="16"/>
       <c r="D58" s="16"/>
       <c r="E58" s="12"/>
@@ -15261,11 +15014,9 @@
     </row>
     <row r="59" spans="1:256" ht="12" customHeight="1">
       <c r="A59" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="B59" s="19" t="s">
-        <v>65</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="B59" s="19"/>
       <c r="C59" s="16"/>
       <c r="D59" s="16"/>
       <c r="E59" s="12"/>
@@ -15523,10 +15274,10 @@
     </row>
     <row r="60" spans="1:256" ht="12" customHeight="1">
       <c r="A60" s="9" t="s">
-        <v>297</v>
+        <v>64</v>
       </c>
       <c r="B60" s="19" t="s">
-        <v>298</v>
+        <v>65</v>
       </c>
       <c r="C60" s="16"/>
       <c r="D60" s="16"/>
@@ -15785,280 +15536,282 @@
     </row>
     <row r="61" spans="1:256" ht="12" customHeight="1">
       <c r="A61" s="9" t="s">
-        <v>317</v>
+        <v>297</v>
       </c>
       <c r="B61" s="19" t="s">
-        <v>319</v>
-      </c>
-      <c r="D61"/>
+        <v>298</v>
+      </c>
+      <c r="C61" s="16"/>
+      <c r="D61" s="16"/>
+      <c r="E61" s="12"/>
+      <c r="F61" s="12"/>
+      <c r="G61" s="12"/>
+      <c r="H61" s="12"/>
+      <c r="I61" s="5"/>
+      <c r="J61" s="5"/>
+      <c r="K61" s="5"/>
+      <c r="L61" s="5"/>
+      <c r="M61" s="5"/>
+      <c r="N61" s="5"/>
+      <c r="O61" s="5"/>
+      <c r="P61" s="5"/>
+      <c r="Q61" s="5"/>
+      <c r="R61" s="5"/>
+      <c r="S61" s="1"/>
+      <c r="T61" s="1"/>
+      <c r="U61" s="1"/>
+      <c r="V61" s="1"/>
+      <c r="W61" s="1"/>
+      <c r="X61" s="1"/>
+      <c r="Y61" s="1"/>
+      <c r="Z61" s="1"/>
+      <c r="AA61" s="1"/>
+      <c r="AB61" s="1"/>
+      <c r="AC61" s="1"/>
+      <c r="AD61" s="1"/>
+      <c r="AE61" s="1"/>
+      <c r="AF61" s="1"/>
+      <c r="AG61" s="1"/>
+      <c r="AH61" s="1"/>
+      <c r="AI61" s="1"/>
+      <c r="AJ61" s="1"/>
+      <c r="AK61" s="1"/>
+      <c r="AL61" s="1"/>
+      <c r="AM61" s="1"/>
+      <c r="AN61" s="1"/>
+      <c r="AO61" s="1"/>
+      <c r="AP61" s="1"/>
+      <c r="AQ61" s="1"/>
+      <c r="AR61" s="1"/>
+      <c r="AS61" s="1"/>
+      <c r="AT61" s="1"/>
+      <c r="AU61" s="1"/>
+      <c r="AV61" s="1"/>
+      <c r="AW61" s="1"/>
+      <c r="AX61" s="1"/>
+      <c r="AY61" s="1"/>
+      <c r="AZ61" s="1"/>
+      <c r="BA61" s="1"/>
+      <c r="BB61" s="1"/>
+      <c r="BC61" s="1"/>
+      <c r="BD61" s="1"/>
+      <c r="BE61" s="1"/>
+      <c r="BF61" s="1"/>
+      <c r="BG61" s="1"/>
+      <c r="BH61" s="1"/>
+      <c r="BI61" s="1"/>
+      <c r="BJ61" s="1"/>
+      <c r="BK61" s="1"/>
+      <c r="BL61" s="1"/>
+      <c r="BM61" s="1"/>
+      <c r="BN61" s="1"/>
+      <c r="BO61" s="1"/>
+      <c r="BP61" s="1"/>
+      <c r="BQ61" s="1"/>
+      <c r="BR61" s="1"/>
+      <c r="BS61" s="1"/>
+      <c r="BT61" s="1"/>
+      <c r="BU61" s="1"/>
+      <c r="BV61" s="1"/>
+      <c r="BW61" s="1"/>
+      <c r="BX61" s="1"/>
+      <c r="BY61" s="1"/>
+      <c r="BZ61" s="1"/>
+      <c r="CA61" s="1"/>
+      <c r="CB61" s="1"/>
+      <c r="CC61" s="1"/>
+      <c r="CD61" s="1"/>
+      <c r="CE61" s="1"/>
+      <c r="CF61" s="1"/>
+      <c r="CG61" s="1"/>
+      <c r="CH61" s="1"/>
+      <c r="CI61" s="1"/>
+      <c r="CJ61" s="1"/>
+      <c r="CK61" s="1"/>
+      <c r="CL61" s="1"/>
+      <c r="CM61" s="1"/>
+      <c r="CN61" s="1"/>
+      <c r="CO61" s="1"/>
+      <c r="CP61" s="1"/>
+      <c r="CQ61" s="1"/>
+      <c r="CR61" s="1"/>
+      <c r="CS61" s="1"/>
+      <c r="CT61" s="1"/>
+      <c r="CU61" s="1"/>
+      <c r="CV61" s="1"/>
+      <c r="CW61" s="1"/>
+      <c r="CX61" s="1"/>
+      <c r="CY61" s="1"/>
+      <c r="CZ61" s="1"/>
+      <c r="DA61" s="1"/>
+      <c r="DB61" s="1"/>
+      <c r="DC61" s="1"/>
+      <c r="DD61" s="1"/>
+      <c r="DE61" s="1"/>
+      <c r="DF61" s="1"/>
+      <c r="DG61" s="1"/>
+      <c r="DH61" s="1"/>
+      <c r="DI61" s="1"/>
+      <c r="DJ61" s="1"/>
+      <c r="DK61" s="1"/>
+      <c r="DL61" s="1"/>
+      <c r="DM61" s="1"/>
+      <c r="DN61" s="1"/>
+      <c r="DO61" s="1"/>
+      <c r="DP61" s="1"/>
+      <c r="DQ61" s="1"/>
+      <c r="DR61" s="1"/>
+      <c r="DS61" s="1"/>
+      <c r="DT61" s="1"/>
+      <c r="DU61" s="1"/>
+      <c r="DV61" s="1"/>
+      <c r="DW61" s="1"/>
+      <c r="DX61" s="1"/>
+      <c r="DY61" s="1"/>
+      <c r="DZ61" s="1"/>
+      <c r="EA61" s="1"/>
+      <c r="EB61" s="1"/>
+      <c r="EC61" s="1"/>
+      <c r="ED61" s="1"/>
+      <c r="EE61" s="1"/>
+      <c r="EF61" s="1"/>
+      <c r="EG61" s="1"/>
+      <c r="EH61" s="1"/>
+      <c r="EI61" s="1"/>
+      <c r="EJ61" s="1"/>
+      <c r="EK61" s="1"/>
+      <c r="EL61" s="1"/>
+      <c r="EM61" s="1"/>
+      <c r="EN61" s="1"/>
+      <c r="EO61" s="1"/>
+      <c r="EP61" s="1"/>
+      <c r="EQ61" s="1"/>
+      <c r="ER61" s="1"/>
+      <c r="ES61" s="1"/>
+      <c r="ET61" s="1"/>
+      <c r="EU61" s="1"/>
+      <c r="EV61" s="1"/>
+      <c r="EW61" s="1"/>
+      <c r="EX61" s="1"/>
+      <c r="EY61" s="1"/>
+      <c r="EZ61" s="1"/>
+      <c r="FA61" s="1"/>
+      <c r="FB61" s="1"/>
+      <c r="FC61" s="1"/>
+      <c r="FD61" s="1"/>
+      <c r="FE61" s="1"/>
+      <c r="FF61" s="1"/>
+      <c r="FG61" s="1"/>
+      <c r="FH61" s="1"/>
+      <c r="FI61" s="1"/>
+      <c r="FJ61" s="1"/>
+      <c r="FK61" s="1"/>
+      <c r="FL61" s="1"/>
+      <c r="FM61" s="1"/>
+      <c r="FN61" s="1"/>
+      <c r="FO61" s="1"/>
+      <c r="FP61" s="1"/>
+      <c r="FQ61" s="1"/>
+      <c r="FR61" s="1"/>
+      <c r="FS61" s="1"/>
+      <c r="FT61" s="1"/>
+      <c r="FU61" s="1"/>
+      <c r="FV61" s="1"/>
+      <c r="FW61" s="1"/>
+      <c r="FX61" s="1"/>
+      <c r="FY61" s="1"/>
+      <c r="FZ61" s="1"/>
+      <c r="GA61" s="1"/>
+      <c r="GB61" s="1"/>
+      <c r="GC61" s="1"/>
+      <c r="GD61" s="1"/>
+      <c r="GE61" s="1"/>
+      <c r="GF61" s="1"/>
+      <c r="GG61" s="1"/>
+      <c r="GH61" s="1"/>
+      <c r="GI61" s="1"/>
+      <c r="GJ61" s="1"/>
+      <c r="GK61" s="1"/>
+      <c r="GL61" s="1"/>
+      <c r="GM61" s="1"/>
+      <c r="GN61" s="1"/>
+      <c r="GO61" s="1"/>
+      <c r="GP61" s="1"/>
+      <c r="GQ61" s="1"/>
+      <c r="GR61" s="1"/>
+      <c r="GS61" s="1"/>
+      <c r="GT61" s="1"/>
+      <c r="GU61" s="1"/>
+      <c r="GV61" s="1"/>
+      <c r="GW61" s="1"/>
+      <c r="GX61" s="1"/>
+      <c r="GY61" s="1"/>
+      <c r="GZ61" s="1"/>
+      <c r="HA61" s="1"/>
+      <c r="HB61" s="1"/>
+      <c r="HC61" s="1"/>
+      <c r="HD61" s="1"/>
+      <c r="HE61" s="1"/>
+      <c r="HF61" s="1"/>
+      <c r="HG61" s="1"/>
+      <c r="HH61" s="1"/>
+      <c r="HI61" s="1"/>
+      <c r="HJ61" s="1"/>
+      <c r="HK61" s="1"/>
+      <c r="HL61" s="1"/>
+      <c r="HM61" s="1"/>
+      <c r="HN61" s="1"/>
+      <c r="HO61" s="1"/>
+      <c r="HP61" s="1"/>
+      <c r="HQ61" s="1"/>
+      <c r="HR61" s="1"/>
+      <c r="HS61" s="1"/>
+      <c r="HT61" s="1"/>
+      <c r="HU61" s="1"/>
+      <c r="HV61" s="1"/>
+      <c r="HW61" s="1"/>
+      <c r="HX61" s="1"/>
+      <c r="HY61" s="1"/>
+      <c r="HZ61" s="1"/>
+      <c r="IA61" s="1"/>
+      <c r="IB61" s="1"/>
+      <c r="IC61" s="1"/>
+      <c r="ID61" s="1"/>
+      <c r="IE61" s="1"/>
+      <c r="IF61" s="1"/>
+      <c r="IG61" s="1"/>
+      <c r="IH61" s="1"/>
+      <c r="II61" s="1"/>
+      <c r="IJ61" s="1"/>
+      <c r="IK61" s="1"/>
+      <c r="IL61" s="1"/>
+      <c r="IM61" s="1"/>
+      <c r="IN61" s="1"/>
+      <c r="IO61" s="1"/>
+      <c r="IP61" s="1"/>
+      <c r="IQ61" s="1"/>
+      <c r="IR61" s="1"/>
+      <c r="IS61" s="1"/>
+      <c r="IT61" s="1"/>
+      <c r="IU61" s="1"/>
+      <c r="IV61" s="1"/>
     </row>
     <row r="62" spans="1:256" ht="12" customHeight="1">
+      <c r="A62" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="B62" s="19" t="s">
+        <v>319</v>
+      </c>
       <c r="D62"/>
     </row>
     <row r="63" spans="1:256" ht="12" customHeight="1">
-      <c r="A63" s="15"/>
-      <c r="B63" s="16"/>
-      <c r="C63" s="16"/>
-      <c r="D63" s="16"/>
-      <c r="E63" s="12"/>
-      <c r="F63" s="12"/>
-      <c r="G63" s="12"/>
-      <c r="H63" s="12"/>
-      <c r="I63" s="5"/>
-      <c r="J63" s="5"/>
-      <c r="K63" s="5"/>
-      <c r="L63" s="5"/>
-      <c r="M63" s="5"/>
-      <c r="N63" s="5"/>
-      <c r="O63" s="5"/>
-      <c r="P63" s="5"/>
-      <c r="Q63" s="5"/>
-      <c r="R63" s="5"/>
-      <c r="S63" s="1"/>
-      <c r="T63" s="1"/>
-      <c r="U63" s="1"/>
-      <c r="V63" s="1"/>
-      <c r="W63" s="1"/>
-      <c r="X63" s="1"/>
-      <c r="Y63" s="1"/>
-      <c r="Z63" s="1"/>
-      <c r="AA63" s="1"/>
-      <c r="AB63" s="1"/>
-      <c r="AC63" s="1"/>
-      <c r="AD63" s="1"/>
-      <c r="AE63" s="1"/>
-      <c r="AF63" s="1"/>
-      <c r="AG63" s="1"/>
-      <c r="AH63" s="1"/>
-      <c r="AI63" s="1"/>
-      <c r="AJ63" s="1"/>
-      <c r="AK63" s="1"/>
-      <c r="AL63" s="1"/>
-      <c r="AM63" s="1"/>
-      <c r="AN63" s="1"/>
-      <c r="AO63" s="1"/>
-      <c r="AP63" s="1"/>
-      <c r="AQ63" s="1"/>
-      <c r="AR63" s="1"/>
-      <c r="AS63" s="1"/>
-      <c r="AT63" s="1"/>
-      <c r="AU63" s="1"/>
-      <c r="AV63" s="1"/>
-      <c r="AW63" s="1"/>
-      <c r="AX63" s="1"/>
-      <c r="AY63" s="1"/>
-      <c r="AZ63" s="1"/>
-      <c r="BA63" s="1"/>
-      <c r="BB63" s="1"/>
-      <c r="BC63" s="1"/>
-      <c r="BD63" s="1"/>
-      <c r="BE63" s="1"/>
-      <c r="BF63" s="1"/>
-      <c r="BG63" s="1"/>
-      <c r="BH63" s="1"/>
-      <c r="BI63" s="1"/>
-      <c r="BJ63" s="1"/>
-      <c r="BK63" s="1"/>
-      <c r="BL63" s="1"/>
-      <c r="BM63" s="1"/>
-      <c r="BN63" s="1"/>
-      <c r="BO63" s="1"/>
-      <c r="BP63" s="1"/>
-      <c r="BQ63" s="1"/>
-      <c r="BR63" s="1"/>
-      <c r="BS63" s="1"/>
-      <c r="BT63" s="1"/>
-      <c r="BU63" s="1"/>
-      <c r="BV63" s="1"/>
-      <c r="BW63" s="1"/>
-      <c r="BX63" s="1"/>
-      <c r="BY63" s="1"/>
-      <c r="BZ63" s="1"/>
-      <c r="CA63" s="1"/>
-      <c r="CB63" s="1"/>
-      <c r="CC63" s="1"/>
-      <c r="CD63" s="1"/>
-      <c r="CE63" s="1"/>
-      <c r="CF63" s="1"/>
-      <c r="CG63" s="1"/>
-      <c r="CH63" s="1"/>
-      <c r="CI63" s="1"/>
-      <c r="CJ63" s="1"/>
-      <c r="CK63" s="1"/>
-      <c r="CL63" s="1"/>
-      <c r="CM63" s="1"/>
-      <c r="CN63" s="1"/>
-      <c r="CO63" s="1"/>
-      <c r="CP63" s="1"/>
-      <c r="CQ63" s="1"/>
-      <c r="CR63" s="1"/>
-      <c r="CS63" s="1"/>
-      <c r="CT63" s="1"/>
-      <c r="CU63" s="1"/>
-      <c r="CV63" s="1"/>
-      <c r="CW63" s="1"/>
-      <c r="CX63" s="1"/>
-      <c r="CY63" s="1"/>
-      <c r="CZ63" s="1"/>
-      <c r="DA63" s="1"/>
-      <c r="DB63" s="1"/>
-      <c r="DC63" s="1"/>
-      <c r="DD63" s="1"/>
-      <c r="DE63" s="1"/>
-      <c r="DF63" s="1"/>
-      <c r="DG63" s="1"/>
-      <c r="DH63" s="1"/>
-      <c r="DI63" s="1"/>
-      <c r="DJ63" s="1"/>
-      <c r="DK63" s="1"/>
-      <c r="DL63" s="1"/>
-      <c r="DM63" s="1"/>
-      <c r="DN63" s="1"/>
-      <c r="DO63" s="1"/>
-      <c r="DP63" s="1"/>
-      <c r="DQ63" s="1"/>
-      <c r="DR63" s="1"/>
-      <c r="DS63" s="1"/>
-      <c r="DT63" s="1"/>
-      <c r="DU63" s="1"/>
-      <c r="DV63" s="1"/>
-      <c r="DW63" s="1"/>
-      <c r="DX63" s="1"/>
-      <c r="DY63" s="1"/>
-      <c r="DZ63" s="1"/>
-      <c r="EA63" s="1"/>
-      <c r="EB63" s="1"/>
-      <c r="EC63" s="1"/>
-      <c r="ED63" s="1"/>
-      <c r="EE63" s="1"/>
-      <c r="EF63" s="1"/>
-      <c r="EG63" s="1"/>
-      <c r="EH63" s="1"/>
-      <c r="EI63" s="1"/>
-      <c r="EJ63" s="1"/>
-      <c r="EK63" s="1"/>
-      <c r="EL63" s="1"/>
-      <c r="EM63" s="1"/>
-      <c r="EN63" s="1"/>
-      <c r="EO63" s="1"/>
-      <c r="EP63" s="1"/>
-      <c r="EQ63" s="1"/>
-      <c r="ER63" s="1"/>
-      <c r="ES63" s="1"/>
-      <c r="ET63" s="1"/>
-      <c r="EU63" s="1"/>
-      <c r="EV63" s="1"/>
-      <c r="EW63" s="1"/>
-      <c r="EX63" s="1"/>
-      <c r="EY63" s="1"/>
-      <c r="EZ63" s="1"/>
-      <c r="FA63" s="1"/>
-      <c r="FB63" s="1"/>
-      <c r="FC63" s="1"/>
-      <c r="FD63" s="1"/>
-      <c r="FE63" s="1"/>
-      <c r="FF63" s="1"/>
-      <c r="FG63" s="1"/>
-      <c r="FH63" s="1"/>
-      <c r="FI63" s="1"/>
-      <c r="FJ63" s="1"/>
-      <c r="FK63" s="1"/>
-      <c r="FL63" s="1"/>
-      <c r="FM63" s="1"/>
-      <c r="FN63" s="1"/>
-      <c r="FO63" s="1"/>
-      <c r="FP63" s="1"/>
-      <c r="FQ63" s="1"/>
-      <c r="FR63" s="1"/>
-      <c r="FS63" s="1"/>
-      <c r="FT63" s="1"/>
-      <c r="FU63" s="1"/>
-      <c r="FV63" s="1"/>
-      <c r="FW63" s="1"/>
-      <c r="FX63" s="1"/>
-      <c r="FY63" s="1"/>
-      <c r="FZ63" s="1"/>
-      <c r="GA63" s="1"/>
-      <c r="GB63" s="1"/>
-      <c r="GC63" s="1"/>
-      <c r="GD63" s="1"/>
-      <c r="GE63" s="1"/>
-      <c r="GF63" s="1"/>
-      <c r="GG63" s="1"/>
-      <c r="GH63" s="1"/>
-      <c r="GI63" s="1"/>
-      <c r="GJ63" s="1"/>
-      <c r="GK63" s="1"/>
-      <c r="GL63" s="1"/>
-      <c r="GM63" s="1"/>
-      <c r="GN63" s="1"/>
-      <c r="GO63" s="1"/>
-      <c r="GP63" s="1"/>
-      <c r="GQ63" s="1"/>
-      <c r="GR63" s="1"/>
-      <c r="GS63" s="1"/>
-      <c r="GT63" s="1"/>
-      <c r="GU63" s="1"/>
-      <c r="GV63" s="1"/>
-      <c r="GW63" s="1"/>
-      <c r="GX63" s="1"/>
-      <c r="GY63" s="1"/>
-      <c r="GZ63" s="1"/>
-      <c r="HA63" s="1"/>
-      <c r="HB63" s="1"/>
-      <c r="HC63" s="1"/>
-      <c r="HD63" s="1"/>
-      <c r="HE63" s="1"/>
-      <c r="HF63" s="1"/>
-      <c r="HG63" s="1"/>
-      <c r="HH63" s="1"/>
-      <c r="HI63" s="1"/>
-      <c r="HJ63" s="1"/>
-      <c r="HK63" s="1"/>
-      <c r="HL63" s="1"/>
-      <c r="HM63" s="1"/>
-      <c r="HN63" s="1"/>
-      <c r="HO63" s="1"/>
-      <c r="HP63" s="1"/>
-      <c r="HQ63" s="1"/>
-      <c r="HR63" s="1"/>
-      <c r="HS63" s="1"/>
-      <c r="HT63" s="1"/>
-      <c r="HU63" s="1"/>
-      <c r="HV63" s="1"/>
-      <c r="HW63" s="1"/>
-      <c r="HX63" s="1"/>
-      <c r="HY63" s="1"/>
-      <c r="HZ63" s="1"/>
-      <c r="IA63" s="1"/>
-      <c r="IB63" s="1"/>
-      <c r="IC63" s="1"/>
-      <c r="ID63" s="1"/>
-      <c r="IE63" s="1"/>
-      <c r="IF63" s="1"/>
-      <c r="IG63" s="1"/>
-      <c r="IH63" s="1"/>
-      <c r="II63" s="1"/>
-      <c r="IJ63" s="1"/>
-      <c r="IK63" s="1"/>
-      <c r="IL63" s="1"/>
-      <c r="IM63" s="1"/>
-      <c r="IN63" s="1"/>
-      <c r="IO63" s="1"/>
-      <c r="IP63" s="1"/>
-      <c r="IQ63" s="1"/>
-      <c r="IR63" s="1"/>
-      <c r="IS63" s="1"/>
-      <c r="IT63" s="1"/>
-      <c r="IU63" s="1"/>
-      <c r="IV63" s="1"/>
+      <c r="D63"/>
     </row>
     <row r="64" spans="1:256" ht="12" customHeight="1">
-      <c r="A64" s="63" t="s">
-        <v>136</v>
-      </c>
-      <c r="B64" s="64"/>
-      <c r="C64" s="64"/>
+      <c r="A64" s="15"/>
+      <c r="B64" s="16"/>
+      <c r="C64" s="16"/>
       <c r="D64" s="16"/>
       <c r="E64" s="12"/>
       <c r="F64" s="12"/>
@@ -16314,15 +16067,11 @@
       <c r="IV64" s="1"/>
     </row>
     <row r="65" spans="1:256" ht="12" customHeight="1">
-      <c r="A65" s="30" t="s">
-        <v>137</v>
-      </c>
-      <c r="B65" s="30" t="s">
-        <v>138</v>
-      </c>
-      <c r="C65" s="30" t="s">
-        <v>139</v>
-      </c>
+      <c r="A65" s="63" t="s">
+        <v>136</v>
+      </c>
+      <c r="B65" s="64"/>
+      <c r="C65" s="64"/>
       <c r="D65" s="16"/>
       <c r="E65" s="12"/>
       <c r="F65" s="12"/>
@@ -16578,14 +16327,14 @@
       <c r="IV65" s="1"/>
     </row>
     <row r="66" spans="1:256" ht="12" customHeight="1">
-      <c r="A66" s="31" t="s">
-        <v>140</v>
-      </c>
-      <c r="B66" s="32" t="s">
-        <v>141</v>
-      </c>
-      <c r="C66" s="32" t="s">
-        <v>142</v>
+      <c r="A66" s="30" t="s">
+        <v>137</v>
+      </c>
+      <c r="B66" s="30" t="s">
+        <v>138</v>
+      </c>
+      <c r="C66" s="30" t="s">
+        <v>139</v>
       </c>
       <c r="D66" s="16"/>
       <c r="E66" s="12"/>
@@ -16843,13 +16592,13 @@
     </row>
     <row r="67" spans="1:256" ht="12" customHeight="1">
       <c r="A67" s="31" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B67" s="32" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C67" s="32" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D67" s="16"/>
       <c r="E67" s="12"/>
@@ -17107,13 +16856,13 @@
     </row>
     <row r="68" spans="1:256" ht="12" customHeight="1">
       <c r="A68" s="31" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B68" s="32" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C68" s="32" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="D68" s="16"/>
       <c r="E68" s="12"/>
@@ -17371,13 +17120,13 @@
     </row>
     <row r="69" spans="1:256" ht="12" customHeight="1">
       <c r="A69" s="31" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B69" s="32" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C69" s="32" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="D69" s="16"/>
       <c r="E69" s="12"/>
@@ -17634,9 +17383,15 @@
       <c r="IV69" s="1"/>
     </row>
     <row r="70" spans="1:256" ht="12" customHeight="1">
-      <c r="A70" s="15"/>
-      <c r="B70" s="16"/>
-      <c r="C70" s="16"/>
+      <c r="A70" s="31" t="s">
+        <v>149</v>
+      </c>
+      <c r="B70" s="32" t="s">
+        <v>150</v>
+      </c>
+      <c r="C70" s="32" t="s">
+        <v>151</v>
+      </c>
       <c r="D70" s="16"/>
       <c r="E70" s="12"/>
       <c r="F70" s="12"/>
@@ -17892,11 +17647,9 @@
       <c r="IV70" s="1"/>
     </row>
     <row r="71" spans="1:256" ht="12" customHeight="1">
-      <c r="A71" s="62" t="s">
-        <v>66</v>
-      </c>
-      <c r="B71" s="62"/>
-      <c r="C71" s="14"/>
+      <c r="A71" s="15"/>
+      <c r="B71" s="16"/>
+      <c r="C71" s="16"/>
       <c r="D71" s="16"/>
       <c r="E71" s="12"/>
       <c r="F71" s="12"/>
@@ -18151,19 +17904,17 @@
       <c r="IU71" s="1"/>
       <c r="IV71" s="1"/>
     </row>
-    <row r="72" spans="1:256" ht="16.5" customHeight="1">
-      <c r="A72" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="B72" s="21" t="s">
-        <v>68</v>
-      </c>
+    <row r="72" spans="1:256" ht="12" customHeight="1">
+      <c r="A72" s="62" t="s">
+        <v>66</v>
+      </c>
+      <c r="B72" s="62"/>
       <c r="C72" s="14"/>
-      <c r="D72" s="14"/>
-      <c r="E72" s="5"/>
-      <c r="F72" s="5"/>
-      <c r="G72" s="14"/>
-      <c r="H72" s="14"/>
+      <c r="D72" s="16"/>
+      <c r="E72" s="12"/>
+      <c r="F72" s="12"/>
+      <c r="G72" s="12"/>
+      <c r="H72" s="12"/>
       <c r="I72" s="5"/>
       <c r="J72" s="5"/>
       <c r="K72" s="5"/>
@@ -18174,15 +17925,253 @@
       <c r="P72" s="5"/>
       <c r="Q72" s="5"/>
       <c r="R72" s="5"/>
+      <c r="S72" s="1"/>
+      <c r="T72" s="1"/>
+      <c r="U72" s="1"/>
+      <c r="V72" s="1"/>
+      <c r="W72" s="1"/>
+      <c r="X72" s="1"/>
+      <c r="Y72" s="1"/>
+      <c r="Z72" s="1"/>
+      <c r="AA72" s="1"/>
+      <c r="AB72" s="1"/>
+      <c r="AC72" s="1"/>
+      <c r="AD72" s="1"/>
+      <c r="AE72" s="1"/>
+      <c r="AF72" s="1"/>
+      <c r="AG72" s="1"/>
+      <c r="AH72" s="1"/>
+      <c r="AI72" s="1"/>
+      <c r="AJ72" s="1"/>
+      <c r="AK72" s="1"/>
+      <c r="AL72" s="1"/>
+      <c r="AM72" s="1"/>
+      <c r="AN72" s="1"/>
+      <c r="AO72" s="1"/>
+      <c r="AP72" s="1"/>
+      <c r="AQ72" s="1"/>
+      <c r="AR72" s="1"/>
+      <c r="AS72" s="1"/>
+      <c r="AT72" s="1"/>
+      <c r="AU72" s="1"/>
+      <c r="AV72" s="1"/>
+      <c r="AW72" s="1"/>
+      <c r="AX72" s="1"/>
+      <c r="AY72" s="1"/>
+      <c r="AZ72" s="1"/>
+      <c r="BA72" s="1"/>
+      <c r="BB72" s="1"/>
+      <c r="BC72" s="1"/>
+      <c r="BD72" s="1"/>
+      <c r="BE72" s="1"/>
+      <c r="BF72" s="1"/>
+      <c r="BG72" s="1"/>
+      <c r="BH72" s="1"/>
+      <c r="BI72" s="1"/>
+      <c r="BJ72" s="1"/>
+      <c r="BK72" s="1"/>
+      <c r="BL72" s="1"/>
+      <c r="BM72" s="1"/>
+      <c r="BN72" s="1"/>
+      <c r="BO72" s="1"/>
+      <c r="BP72" s="1"/>
+      <c r="BQ72" s="1"/>
+      <c r="BR72" s="1"/>
+      <c r="BS72" s="1"/>
+      <c r="BT72" s="1"/>
+      <c r="BU72" s="1"/>
+      <c r="BV72" s="1"/>
+      <c r="BW72" s="1"/>
+      <c r="BX72" s="1"/>
+      <c r="BY72" s="1"/>
+      <c r="BZ72" s="1"/>
+      <c r="CA72" s="1"/>
+      <c r="CB72" s="1"/>
+      <c r="CC72" s="1"/>
+      <c r="CD72" s="1"/>
+      <c r="CE72" s="1"/>
+      <c r="CF72" s="1"/>
+      <c r="CG72" s="1"/>
+      <c r="CH72" s="1"/>
+      <c r="CI72" s="1"/>
+      <c r="CJ72" s="1"/>
+      <c r="CK72" s="1"/>
+      <c r="CL72" s="1"/>
+      <c r="CM72" s="1"/>
+      <c r="CN72" s="1"/>
+      <c r="CO72" s="1"/>
+      <c r="CP72" s="1"/>
+      <c r="CQ72" s="1"/>
+      <c r="CR72" s="1"/>
+      <c r="CS72" s="1"/>
+      <c r="CT72" s="1"/>
+      <c r="CU72" s="1"/>
+      <c r="CV72" s="1"/>
+      <c r="CW72" s="1"/>
+      <c r="CX72" s="1"/>
+      <c r="CY72" s="1"/>
+      <c r="CZ72" s="1"/>
+      <c r="DA72" s="1"/>
+      <c r="DB72" s="1"/>
+      <c r="DC72" s="1"/>
+      <c r="DD72" s="1"/>
+      <c r="DE72" s="1"/>
+      <c r="DF72" s="1"/>
+      <c r="DG72" s="1"/>
+      <c r="DH72" s="1"/>
+      <c r="DI72" s="1"/>
+      <c r="DJ72" s="1"/>
+      <c r="DK72" s="1"/>
+      <c r="DL72" s="1"/>
+      <c r="DM72" s="1"/>
+      <c r="DN72" s="1"/>
+      <c r="DO72" s="1"/>
+      <c r="DP72" s="1"/>
+      <c r="DQ72" s="1"/>
+      <c r="DR72" s="1"/>
+      <c r="DS72" s="1"/>
+      <c r="DT72" s="1"/>
+      <c r="DU72" s="1"/>
+      <c r="DV72" s="1"/>
+      <c r="DW72" s="1"/>
+      <c r="DX72" s="1"/>
+      <c r="DY72" s="1"/>
+      <c r="DZ72" s="1"/>
+      <c r="EA72" s="1"/>
+      <c r="EB72" s="1"/>
+      <c r="EC72" s="1"/>
+      <c r="ED72" s="1"/>
+      <c r="EE72" s="1"/>
+      <c r="EF72" s="1"/>
+      <c r="EG72" s="1"/>
+      <c r="EH72" s="1"/>
+      <c r="EI72" s="1"/>
+      <c r="EJ72" s="1"/>
+      <c r="EK72" s="1"/>
+      <c r="EL72" s="1"/>
+      <c r="EM72" s="1"/>
+      <c r="EN72" s="1"/>
+      <c r="EO72" s="1"/>
+      <c r="EP72" s="1"/>
+      <c r="EQ72" s="1"/>
+      <c r="ER72" s="1"/>
+      <c r="ES72" s="1"/>
+      <c r="ET72" s="1"/>
+      <c r="EU72" s="1"/>
+      <c r="EV72" s="1"/>
+      <c r="EW72" s="1"/>
+      <c r="EX72" s="1"/>
+      <c r="EY72" s="1"/>
+      <c r="EZ72" s="1"/>
+      <c r="FA72" s="1"/>
+      <c r="FB72" s="1"/>
+      <c r="FC72" s="1"/>
+      <c r="FD72" s="1"/>
+      <c r="FE72" s="1"/>
+      <c r="FF72" s="1"/>
+      <c r="FG72" s="1"/>
+      <c r="FH72" s="1"/>
+      <c r="FI72" s="1"/>
+      <c r="FJ72" s="1"/>
+      <c r="FK72" s="1"/>
+      <c r="FL72" s="1"/>
+      <c r="FM72" s="1"/>
+      <c r="FN72" s="1"/>
+      <c r="FO72" s="1"/>
+      <c r="FP72" s="1"/>
+      <c r="FQ72" s="1"/>
+      <c r="FR72" s="1"/>
+      <c r="FS72" s="1"/>
+      <c r="FT72" s="1"/>
+      <c r="FU72" s="1"/>
+      <c r="FV72" s="1"/>
+      <c r="FW72" s="1"/>
+      <c r="FX72" s="1"/>
+      <c r="FY72" s="1"/>
+      <c r="FZ72" s="1"/>
+      <c r="GA72" s="1"/>
+      <c r="GB72" s="1"/>
+      <c r="GC72" s="1"/>
+      <c r="GD72" s="1"/>
+      <c r="GE72" s="1"/>
+      <c r="GF72" s="1"/>
+      <c r="GG72" s="1"/>
+      <c r="GH72" s="1"/>
+      <c r="GI72" s="1"/>
+      <c r="GJ72" s="1"/>
+      <c r="GK72" s="1"/>
+      <c r="GL72" s="1"/>
+      <c r="GM72" s="1"/>
+      <c r="GN72" s="1"/>
+      <c r="GO72" s="1"/>
+      <c r="GP72" s="1"/>
+      <c r="GQ72" s="1"/>
+      <c r="GR72" s="1"/>
+      <c r="GS72" s="1"/>
+      <c r="GT72" s="1"/>
+      <c r="GU72" s="1"/>
+      <c r="GV72" s="1"/>
+      <c r="GW72" s="1"/>
+      <c r="GX72" s="1"/>
+      <c r="GY72" s="1"/>
+      <c r="GZ72" s="1"/>
+      <c r="HA72" s="1"/>
+      <c r="HB72" s="1"/>
+      <c r="HC72" s="1"/>
+      <c r="HD72" s="1"/>
+      <c r="HE72" s="1"/>
+      <c r="HF72" s="1"/>
+      <c r="HG72" s="1"/>
+      <c r="HH72" s="1"/>
+      <c r="HI72" s="1"/>
+      <c r="HJ72" s="1"/>
+      <c r="HK72" s="1"/>
+      <c r="HL72" s="1"/>
+      <c r="HM72" s="1"/>
+      <c r="HN72" s="1"/>
+      <c r="HO72" s="1"/>
+      <c r="HP72" s="1"/>
+      <c r="HQ72" s="1"/>
+      <c r="HR72" s="1"/>
+      <c r="HS72" s="1"/>
+      <c r="HT72" s="1"/>
+      <c r="HU72" s="1"/>
+      <c r="HV72" s="1"/>
+      <c r="HW72" s="1"/>
+      <c r="HX72" s="1"/>
+      <c r="HY72" s="1"/>
+      <c r="HZ72" s="1"/>
+      <c r="IA72" s="1"/>
+      <c r="IB72" s="1"/>
+      <c r="IC72" s="1"/>
+      <c r="ID72" s="1"/>
+      <c r="IE72" s="1"/>
+      <c r="IF72" s="1"/>
+      <c r="IG72" s="1"/>
+      <c r="IH72" s="1"/>
+      <c r="II72" s="1"/>
+      <c r="IJ72" s="1"/>
+      <c r="IK72" s="1"/>
+      <c r="IL72" s="1"/>
+      <c r="IM72" s="1"/>
+      <c r="IN72" s="1"/>
+      <c r="IO72" s="1"/>
+      <c r="IP72" s="1"/>
+      <c r="IQ72" s="1"/>
+      <c r="IR72" s="1"/>
+      <c r="IS72" s="1"/>
+      <c r="IT72" s="1"/>
+      <c r="IU72" s="1"/>
+      <c r="IV72" s="1"/>
     </row>
-    <row r="73" spans="1:256" ht="12" customHeight="1">
-      <c r="A73" s="22" t="s">
-        <v>305</v>
-      </c>
-      <c r="B73" s="19" t="s">
-        <v>306</v>
-      </c>
-      <c r="C73" s="5"/>
+    <row r="73" spans="1:256" ht="16.5" customHeight="1">
+      <c r="A73" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="B73" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="C73" s="14"/>
       <c r="D73" s="14"/>
       <c r="E73" s="5"/>
       <c r="F73" s="5"/>
@@ -18198,254 +18187,20 @@
       <c r="P73" s="5"/>
       <c r="Q73" s="5"/>
       <c r="R73" s="5"/>
-      <c r="S73" s="1"/>
-      <c r="T73" s="1"/>
-      <c r="U73" s="1"/>
-      <c r="V73" s="1"/>
-      <c r="W73" s="1"/>
-      <c r="X73" s="1"/>
-      <c r="Y73" s="1"/>
-      <c r="Z73" s="1"/>
-      <c r="AA73" s="1"/>
-      <c r="AB73" s="1"/>
-      <c r="AC73" s="1"/>
-      <c r="AD73" s="1"/>
-      <c r="AE73" s="1"/>
-      <c r="AF73" s="1"/>
-      <c r="AG73" s="1"/>
-      <c r="AH73" s="1"/>
-      <c r="AI73" s="1"/>
-      <c r="AJ73" s="1"/>
-      <c r="AK73" s="1"/>
-      <c r="AL73" s="1"/>
-      <c r="AM73" s="1"/>
-      <c r="AN73" s="1"/>
-      <c r="AO73" s="1"/>
-      <c r="AP73" s="1"/>
-      <c r="AQ73" s="1"/>
-      <c r="AR73" s="1"/>
-      <c r="AS73" s="1"/>
-      <c r="AT73" s="1"/>
-      <c r="AU73" s="1"/>
-      <c r="AV73" s="1"/>
-      <c r="AW73" s="1"/>
-      <c r="AX73" s="1"/>
-      <c r="AY73" s="1"/>
-      <c r="AZ73" s="1"/>
-      <c r="BA73" s="1"/>
-      <c r="BB73" s="1"/>
-      <c r="BC73" s="1"/>
-      <c r="BD73" s="1"/>
-      <c r="BE73" s="1"/>
-      <c r="BF73" s="1"/>
-      <c r="BG73" s="1"/>
-      <c r="BH73" s="1"/>
-      <c r="BI73" s="1"/>
-      <c r="BJ73" s="1"/>
-      <c r="BK73" s="1"/>
-      <c r="BL73" s="1"/>
-      <c r="BM73" s="1"/>
-      <c r="BN73" s="1"/>
-      <c r="BO73" s="1"/>
-      <c r="BP73" s="1"/>
-      <c r="BQ73" s="1"/>
-      <c r="BR73" s="1"/>
-      <c r="BS73" s="1"/>
-      <c r="BT73" s="1"/>
-      <c r="BU73" s="1"/>
-      <c r="BV73" s="1"/>
-      <c r="BW73" s="1"/>
-      <c r="BX73" s="1"/>
-      <c r="BY73" s="1"/>
-      <c r="BZ73" s="1"/>
-      <c r="CA73" s="1"/>
-      <c r="CB73" s="1"/>
-      <c r="CC73" s="1"/>
-      <c r="CD73" s="1"/>
-      <c r="CE73" s="1"/>
-      <c r="CF73" s="1"/>
-      <c r="CG73" s="1"/>
-      <c r="CH73" s="1"/>
-      <c r="CI73" s="1"/>
-      <c r="CJ73" s="1"/>
-      <c r="CK73" s="1"/>
-      <c r="CL73" s="1"/>
-      <c r="CM73" s="1"/>
-      <c r="CN73" s="1"/>
-      <c r="CO73" s="1"/>
-      <c r="CP73" s="1"/>
-      <c r="CQ73" s="1"/>
-      <c r="CR73" s="1"/>
-      <c r="CS73" s="1"/>
-      <c r="CT73" s="1"/>
-      <c r="CU73" s="1"/>
-      <c r="CV73" s="1"/>
-      <c r="CW73" s="1"/>
-      <c r="CX73" s="1"/>
-      <c r="CY73" s="1"/>
-      <c r="CZ73" s="1"/>
-      <c r="DA73" s="1"/>
-      <c r="DB73" s="1"/>
-      <c r="DC73" s="1"/>
-      <c r="DD73" s="1"/>
-      <c r="DE73" s="1"/>
-      <c r="DF73" s="1"/>
-      <c r="DG73" s="1"/>
-      <c r="DH73" s="1"/>
-      <c r="DI73" s="1"/>
-      <c r="DJ73" s="1"/>
-      <c r="DK73" s="1"/>
-      <c r="DL73" s="1"/>
-      <c r="DM73" s="1"/>
-      <c r="DN73" s="1"/>
-      <c r="DO73" s="1"/>
-      <c r="DP73" s="1"/>
-      <c r="DQ73" s="1"/>
-      <c r="DR73" s="1"/>
-      <c r="DS73" s="1"/>
-      <c r="DT73" s="1"/>
-      <c r="DU73" s="1"/>
-      <c r="DV73" s="1"/>
-      <c r="DW73" s="1"/>
-      <c r="DX73" s="1"/>
-      <c r="DY73" s="1"/>
-      <c r="DZ73" s="1"/>
-      <c r="EA73" s="1"/>
-      <c r="EB73" s="1"/>
-      <c r="EC73" s="1"/>
-      <c r="ED73" s="1"/>
-      <c r="EE73" s="1"/>
-      <c r="EF73" s="1"/>
-      <c r="EG73" s="1"/>
-      <c r="EH73" s="1"/>
-      <c r="EI73" s="1"/>
-      <c r="EJ73" s="1"/>
-      <c r="EK73" s="1"/>
-      <c r="EL73" s="1"/>
-      <c r="EM73" s="1"/>
-      <c r="EN73" s="1"/>
-      <c r="EO73" s="1"/>
-      <c r="EP73" s="1"/>
-      <c r="EQ73" s="1"/>
-      <c r="ER73" s="1"/>
-      <c r="ES73" s="1"/>
-      <c r="ET73" s="1"/>
-      <c r="EU73" s="1"/>
-      <c r="EV73" s="1"/>
-      <c r="EW73" s="1"/>
-      <c r="EX73" s="1"/>
-      <c r="EY73" s="1"/>
-      <c r="EZ73" s="1"/>
-      <c r="FA73" s="1"/>
-      <c r="FB73" s="1"/>
-      <c r="FC73" s="1"/>
-      <c r="FD73" s="1"/>
-      <c r="FE73" s="1"/>
-      <c r="FF73" s="1"/>
-      <c r="FG73" s="1"/>
-      <c r="FH73" s="1"/>
-      <c r="FI73" s="1"/>
-      <c r="FJ73" s="1"/>
-      <c r="FK73" s="1"/>
-      <c r="FL73" s="1"/>
-      <c r="FM73" s="1"/>
-      <c r="FN73" s="1"/>
-      <c r="FO73" s="1"/>
-      <c r="FP73" s="1"/>
-      <c r="FQ73" s="1"/>
-      <c r="FR73" s="1"/>
-      <c r="FS73" s="1"/>
-      <c r="FT73" s="1"/>
-      <c r="FU73" s="1"/>
-      <c r="FV73" s="1"/>
-      <c r="FW73" s="1"/>
-      <c r="FX73" s="1"/>
-      <c r="FY73" s="1"/>
-      <c r="FZ73" s="1"/>
-      <c r="GA73" s="1"/>
-      <c r="GB73" s="1"/>
-      <c r="GC73" s="1"/>
-      <c r="GD73" s="1"/>
-      <c r="GE73" s="1"/>
-      <c r="GF73" s="1"/>
-      <c r="GG73" s="1"/>
-      <c r="GH73" s="1"/>
-      <c r="GI73" s="1"/>
-      <c r="GJ73" s="1"/>
-      <c r="GK73" s="1"/>
-      <c r="GL73" s="1"/>
-      <c r="GM73" s="1"/>
-      <c r="GN73" s="1"/>
-      <c r="GO73" s="1"/>
-      <c r="GP73" s="1"/>
-      <c r="GQ73" s="1"/>
-      <c r="GR73" s="1"/>
-      <c r="GS73" s="1"/>
-      <c r="GT73" s="1"/>
-      <c r="GU73" s="1"/>
-      <c r="GV73" s="1"/>
-      <c r="GW73" s="1"/>
-      <c r="GX73" s="1"/>
-      <c r="GY73" s="1"/>
-      <c r="GZ73" s="1"/>
-      <c r="HA73" s="1"/>
-      <c r="HB73" s="1"/>
-      <c r="HC73" s="1"/>
-      <c r="HD73" s="1"/>
-      <c r="HE73" s="1"/>
-      <c r="HF73" s="1"/>
-      <c r="HG73" s="1"/>
-      <c r="HH73" s="1"/>
-      <c r="HI73" s="1"/>
-      <c r="HJ73" s="1"/>
-      <c r="HK73" s="1"/>
-      <c r="HL73" s="1"/>
-      <c r="HM73" s="1"/>
-      <c r="HN73" s="1"/>
-      <c r="HO73" s="1"/>
-      <c r="HP73" s="1"/>
-      <c r="HQ73" s="1"/>
-      <c r="HR73" s="1"/>
-      <c r="HS73" s="1"/>
-      <c r="HT73" s="1"/>
-      <c r="HU73" s="1"/>
-      <c r="HV73" s="1"/>
-      <c r="HW73" s="1"/>
-      <c r="HX73" s="1"/>
-      <c r="HY73" s="1"/>
-      <c r="HZ73" s="1"/>
-      <c r="IA73" s="1"/>
-      <c r="IB73" s="1"/>
-      <c r="IC73" s="1"/>
-      <c r="ID73" s="1"/>
-      <c r="IE73" s="1"/>
-      <c r="IF73" s="1"/>
-      <c r="IG73" s="1"/>
-      <c r="IH73" s="1"/>
-      <c r="II73" s="1"/>
-      <c r="IJ73" s="1"/>
-      <c r="IK73" s="1"/>
-      <c r="IL73" s="1"/>
-      <c r="IM73" s="1"/>
-      <c r="IN73" s="1"/>
-      <c r="IO73" s="1"/>
-      <c r="IP73" s="1"/>
-      <c r="IQ73" s="1"/>
-      <c r="IR73" s="1"/>
-      <c r="IS73" s="1"/>
-      <c r="IT73" s="1"/>
-      <c r="IU73" s="1"/>
-      <c r="IV73" s="1"/>
     </row>
-    <row r="74" spans="1:256" ht="15.95" customHeight="1">
-      <c r="A74" s="1"/>
-      <c r="B74" s="1"/>
+    <row r="74" spans="1:256" ht="12" customHeight="1">
+      <c r="A74" s="22" t="s">
+        <v>305</v>
+      </c>
+      <c r="B74" s="19" t="s">
+        <v>306</v>
+      </c>
       <c r="C74" s="5"/>
-      <c r="D74" s="5"/>
+      <c r="D74" s="14"/>
       <c r="E74" s="5"/>
       <c r="F74" s="5"/>
-      <c r="G74" s="5"/>
-      <c r="H74" s="5"/>
+      <c r="G74" s="14"/>
+      <c r="H74" s="14"/>
       <c r="I74" s="5"/>
       <c r="J74" s="5"/>
       <c r="K74" s="5"/>
@@ -18966,12 +18721,12 @@
       <c r="J76" s="5"/>
       <c r="K76" s="5"/>
       <c r="L76" s="5"/>
-      <c r="M76" s="1"/>
-      <c r="N76" s="1"/>
-      <c r="O76" s="1"/>
-      <c r="P76" s="1"/>
-      <c r="Q76" s="1"/>
-      <c r="R76" s="1"/>
+      <c r="M76" s="5"/>
+      <c r="N76" s="5"/>
+      <c r="O76" s="5"/>
+      <c r="P76" s="5"/>
+      <c r="Q76" s="5"/>
+      <c r="R76" s="5"/>
       <c r="S76" s="1"/>
       <c r="T76" s="1"/>
       <c r="U76" s="1"/>
@@ -19469,7 +19224,7 @@
       <c r="IU77" s="1"/>
       <c r="IV77" s="1"/>
     </row>
-    <row r="78" spans="1:256">
+    <row r="78" spans="1:256" ht="15.95" customHeight="1">
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
       <c r="C78" s="5"/>
@@ -19727,7 +19482,7 @@
       <c r="IU78" s="1"/>
       <c r="IV78" s="1"/>
     </row>
-    <row r="79" spans="1:256" ht="15.75" customHeight="1">
+    <row r="79" spans="1:256">
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
       <c r="C79" s="5"/>
@@ -19988,7 +19743,7 @@
     <row r="80" spans="1:256" ht="15.75" customHeight="1">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
-      <c r="C80" s="1"/>
+      <c r="C80" s="5"/>
       <c r="D80" s="5"/>
       <c r="E80" s="5"/>
       <c r="F80" s="5"/>
@@ -20243,26 +19998,25 @@
       <c r="IU80" s="1"/>
       <c r="IV80" s="1"/>
     </row>
-    <row r="81" spans="1:256" ht="12" customHeight="1">
-      <c r="A81" s="62" t="s">
-        <v>184</v>
-      </c>
-      <c r="B81" s="62"/>
+    <row r="81" spans="1:256" ht="15.75" customHeight="1">
+      <c r="A81" s="1"/>
+      <c r="B81" s="1"/>
       <c r="C81" s="1"/>
-      <c r="E81" s="1"/>
-      <c r="F81" s="1"/>
-      <c r="G81" s="1"/>
-      <c r="H81" s="1"/>
+      <c r="D81" s="5"/>
+      <c r="E81" s="5"/>
+      <c r="F81" s="5"/>
+      <c r="G81" s="5"/>
+      <c r="H81" s="5"/>
       <c r="I81" s="5"/>
       <c r="J81" s="5"/>
       <c r="K81" s="5"/>
       <c r="L81" s="5"/>
-      <c r="M81" s="5"/>
-      <c r="N81" s="5"/>
-      <c r="O81" s="5"/>
-      <c r="P81" s="5"/>
-      <c r="Q81" s="5"/>
-      <c r="R81" s="5"/>
+      <c r="M81" s="1"/>
+      <c r="N81" s="1"/>
+      <c r="O81" s="1"/>
+      <c r="P81" s="1"/>
+      <c r="Q81" s="1"/>
+      <c r="R81" s="1"/>
       <c r="S81" s="1"/>
       <c r="T81" s="1"/>
       <c r="U81" s="1"/>
@@ -20502,18 +20256,16 @@
       <c r="IU81" s="1"/>
       <c r="IV81" s="1"/>
     </row>
-    <row r="82" spans="1:256" ht="15.75" customHeight="1">
-      <c r="A82" s="20" t="s">
-        <v>185</v>
-      </c>
-      <c r="B82" s="21" t="s">
-        <v>186</v>
-      </c>
+    <row r="82" spans="1:256" ht="12" customHeight="1">
+      <c r="A82" s="62" t="s">
+        <v>184</v>
+      </c>
+      <c r="B82" s="62"/>
       <c r="C82" s="1"/>
       <c r="E82" s="1"/>
-      <c r="F82" s="5"/>
-      <c r="G82" s="5"/>
-      <c r="H82" s="5"/>
+      <c r="F82" s="1"/>
+      <c r="G82" s="1"/>
+      <c r="H82" s="1"/>
       <c r="I82" s="5"/>
       <c r="J82" s="5"/>
       <c r="K82" s="5"/>
@@ -20521,9 +20273,9 @@
       <c r="M82" s="5"/>
       <c r="N82" s="5"/>
       <c r="O82" s="5"/>
-      <c r="P82" s="1"/>
-      <c r="Q82" s="1"/>
-      <c r="R82" s="1"/>
+      <c r="P82" s="5"/>
+      <c r="Q82" s="5"/>
+      <c r="R82" s="5"/>
       <c r="S82" s="1"/>
       <c r="T82" s="1"/>
       <c r="U82" s="1"/>
@@ -20764,11 +20516,11 @@
       <c r="IV82" s="1"/>
     </row>
     <row r="83" spans="1:256" ht="15.75" customHeight="1">
-      <c r="A83" s="22" t="s">
-        <v>187</v>
-      </c>
-      <c r="B83" s="22" t="s">
-        <v>188</v>
+      <c r="A83" s="20" t="s">
+        <v>185</v>
+      </c>
+      <c r="B83" s="21" t="s">
+        <v>186</v>
       </c>
       <c r="C83" s="1"/>
       <c r="E83" s="1"/>
@@ -21025,8 +20777,12 @@
       <c r="IV83" s="1"/>
     </row>
     <row r="84" spans="1:256" ht="15.75" customHeight="1">
-      <c r="A84" s="1"/>
-      <c r="B84" s="1"/>
+      <c r="A84" s="22" t="s">
+        <v>187</v>
+      </c>
+      <c r="B84" s="22" t="s">
+        <v>188</v>
+      </c>
       <c r="C84" s="1"/>
       <c r="E84" s="1"/>
       <c r="F84" s="5"/>
@@ -21282,10 +21038,13 @@
       <c r="IV84" s="1"/>
     </row>
     <row r="85" spans="1:256" ht="15.75" customHeight="1">
+      <c r="A85" s="1"/>
+      <c r="B85" s="1"/>
+      <c r="C85" s="1"/>
       <c r="E85" s="1"/>
-      <c r="F85" s="1"/>
-      <c r="G85" s="1"/>
-      <c r="H85" s="1"/>
+      <c r="F85" s="5"/>
+      <c r="G85" s="5"/>
+      <c r="H85" s="5"/>
       <c r="I85" s="5"/>
       <c r="J85" s="5"/>
       <c r="K85" s="5"/>
@@ -21293,9 +21052,9 @@
       <c r="M85" s="5"/>
       <c r="N85" s="5"/>
       <c r="O85" s="5"/>
-      <c r="P85" s="5"/>
-      <c r="Q85" s="5"/>
-      <c r="R85" s="5"/>
+      <c r="P85" s="1"/>
+      <c r="Q85" s="1"/>
+      <c r="R85" s="1"/>
       <c r="S85" s="1"/>
       <c r="T85" s="1"/>
       <c r="U85" s="1"/>
@@ -21535,7 +21294,11 @@
       <c r="IU85" s="1"/>
       <c r="IV85" s="1"/>
     </row>
-    <row r="86" spans="1:256" ht="12" customHeight="1">
+    <row r="86" spans="1:256" ht="15.75" customHeight="1">
+      <c r="E86" s="1"/>
+      <c r="F86" s="1"/>
+      <c r="G86" s="1"/>
+      <c r="H86" s="1"/>
       <c r="I86" s="5"/>
       <c r="J86" s="5"/>
       <c r="K86" s="5"/>
@@ -21546,8 +21309,257 @@
       <c r="P86" s="5"/>
       <c r="Q86" s="5"/>
       <c r="R86" s="5"/>
+      <c r="S86" s="1"/>
+      <c r="T86" s="1"/>
+      <c r="U86" s="1"/>
+      <c r="V86" s="1"/>
+      <c r="W86" s="1"/>
+      <c r="X86" s="1"/>
+      <c r="Y86" s="1"/>
+      <c r="Z86" s="1"/>
+      <c r="AA86" s="1"/>
+      <c r="AB86" s="1"/>
+      <c r="AC86" s="1"/>
+      <c r="AD86" s="1"/>
+      <c r="AE86" s="1"/>
+      <c r="AF86" s="1"/>
+      <c r="AG86" s="1"/>
+      <c r="AH86" s="1"/>
+      <c r="AI86" s="1"/>
+      <c r="AJ86" s="1"/>
+      <c r="AK86" s="1"/>
+      <c r="AL86" s="1"/>
+      <c r="AM86" s="1"/>
+      <c r="AN86" s="1"/>
+      <c r="AO86" s="1"/>
+      <c r="AP86" s="1"/>
+      <c r="AQ86" s="1"/>
+      <c r="AR86" s="1"/>
+      <c r="AS86" s="1"/>
+      <c r="AT86" s="1"/>
+      <c r="AU86" s="1"/>
+      <c r="AV86" s="1"/>
+      <c r="AW86" s="1"/>
+      <c r="AX86" s="1"/>
+      <c r="AY86" s="1"/>
+      <c r="AZ86" s="1"/>
+      <c r="BA86" s="1"/>
+      <c r="BB86" s="1"/>
+      <c r="BC86" s="1"/>
+      <c r="BD86" s="1"/>
+      <c r="BE86" s="1"/>
+      <c r="BF86" s="1"/>
+      <c r="BG86" s="1"/>
+      <c r="BH86" s="1"/>
+      <c r="BI86" s="1"/>
+      <c r="BJ86" s="1"/>
+      <c r="BK86" s="1"/>
+      <c r="BL86" s="1"/>
+      <c r="BM86" s="1"/>
+      <c r="BN86" s="1"/>
+      <c r="BO86" s="1"/>
+      <c r="BP86" s="1"/>
+      <c r="BQ86" s="1"/>
+      <c r="BR86" s="1"/>
+      <c r="BS86" s="1"/>
+      <c r="BT86" s="1"/>
+      <c r="BU86" s="1"/>
+      <c r="BV86" s="1"/>
+      <c r="BW86" s="1"/>
+      <c r="BX86" s="1"/>
+      <c r="BY86" s="1"/>
+      <c r="BZ86" s="1"/>
+      <c r="CA86" s="1"/>
+      <c r="CB86" s="1"/>
+      <c r="CC86" s="1"/>
+      <c r="CD86" s="1"/>
+      <c r="CE86" s="1"/>
+      <c r="CF86" s="1"/>
+      <c r="CG86" s="1"/>
+      <c r="CH86" s="1"/>
+      <c r="CI86" s="1"/>
+      <c r="CJ86" s="1"/>
+      <c r="CK86" s="1"/>
+      <c r="CL86" s="1"/>
+      <c r="CM86" s="1"/>
+      <c r="CN86" s="1"/>
+      <c r="CO86" s="1"/>
+      <c r="CP86" s="1"/>
+      <c r="CQ86" s="1"/>
+      <c r="CR86" s="1"/>
+      <c r="CS86" s="1"/>
+      <c r="CT86" s="1"/>
+      <c r="CU86" s="1"/>
+      <c r="CV86" s="1"/>
+      <c r="CW86" s="1"/>
+      <c r="CX86" s="1"/>
+      <c r="CY86" s="1"/>
+      <c r="CZ86" s="1"/>
+      <c r="DA86" s="1"/>
+      <c r="DB86" s="1"/>
+      <c r="DC86" s="1"/>
+      <c r="DD86" s="1"/>
+      <c r="DE86" s="1"/>
+      <c r="DF86" s="1"/>
+      <c r="DG86" s="1"/>
+      <c r="DH86" s="1"/>
+      <c r="DI86" s="1"/>
+      <c r="DJ86" s="1"/>
+      <c r="DK86" s="1"/>
+      <c r="DL86" s="1"/>
+      <c r="DM86" s="1"/>
+      <c r="DN86" s="1"/>
+      <c r="DO86" s="1"/>
+      <c r="DP86" s="1"/>
+      <c r="DQ86" s="1"/>
+      <c r="DR86" s="1"/>
+      <c r="DS86" s="1"/>
+      <c r="DT86" s="1"/>
+      <c r="DU86" s="1"/>
+      <c r="DV86" s="1"/>
+      <c r="DW86" s="1"/>
+      <c r="DX86" s="1"/>
+      <c r="DY86" s="1"/>
+      <c r="DZ86" s="1"/>
+      <c r="EA86" s="1"/>
+      <c r="EB86" s="1"/>
+      <c r="EC86" s="1"/>
+      <c r="ED86" s="1"/>
+      <c r="EE86" s="1"/>
+      <c r="EF86" s="1"/>
+      <c r="EG86" s="1"/>
+      <c r="EH86" s="1"/>
+      <c r="EI86" s="1"/>
+      <c r="EJ86" s="1"/>
+      <c r="EK86" s="1"/>
+      <c r="EL86" s="1"/>
+      <c r="EM86" s="1"/>
+      <c r="EN86" s="1"/>
+      <c r="EO86" s="1"/>
+      <c r="EP86" s="1"/>
+      <c r="EQ86" s="1"/>
+      <c r="ER86" s="1"/>
+      <c r="ES86" s="1"/>
+      <c r="ET86" s="1"/>
+      <c r="EU86" s="1"/>
+      <c r="EV86" s="1"/>
+      <c r="EW86" s="1"/>
+      <c r="EX86" s="1"/>
+      <c r="EY86" s="1"/>
+      <c r="EZ86" s="1"/>
+      <c r="FA86" s="1"/>
+      <c r="FB86" s="1"/>
+      <c r="FC86" s="1"/>
+      <c r="FD86" s="1"/>
+      <c r="FE86" s="1"/>
+      <c r="FF86" s="1"/>
+      <c r="FG86" s="1"/>
+      <c r="FH86" s="1"/>
+      <c r="FI86" s="1"/>
+      <c r="FJ86" s="1"/>
+      <c r="FK86" s="1"/>
+      <c r="FL86" s="1"/>
+      <c r="FM86" s="1"/>
+      <c r="FN86" s="1"/>
+      <c r="FO86" s="1"/>
+      <c r="FP86" s="1"/>
+      <c r="FQ86" s="1"/>
+      <c r="FR86" s="1"/>
+      <c r="FS86" s="1"/>
+      <c r="FT86" s="1"/>
+      <c r="FU86" s="1"/>
+      <c r="FV86" s="1"/>
+      <c r="FW86" s="1"/>
+      <c r="FX86" s="1"/>
+      <c r="FY86" s="1"/>
+      <c r="FZ86" s="1"/>
+      <c r="GA86" s="1"/>
+      <c r="GB86" s="1"/>
+      <c r="GC86" s="1"/>
+      <c r="GD86" s="1"/>
+      <c r="GE86" s="1"/>
+      <c r="GF86" s="1"/>
+      <c r="GG86" s="1"/>
+      <c r="GH86" s="1"/>
+      <c r="GI86" s="1"/>
+      <c r="GJ86" s="1"/>
+      <c r="GK86" s="1"/>
+      <c r="GL86" s="1"/>
+      <c r="GM86" s="1"/>
+      <c r="GN86" s="1"/>
+      <c r="GO86" s="1"/>
+      <c r="GP86" s="1"/>
+      <c r="GQ86" s="1"/>
+      <c r="GR86" s="1"/>
+      <c r="GS86" s="1"/>
+      <c r="GT86" s="1"/>
+      <c r="GU86" s="1"/>
+      <c r="GV86" s="1"/>
+      <c r="GW86" s="1"/>
+      <c r="GX86" s="1"/>
+      <c r="GY86" s="1"/>
+      <c r="GZ86" s="1"/>
+      <c r="HA86" s="1"/>
+      <c r="HB86" s="1"/>
+      <c r="HC86" s="1"/>
+      <c r="HD86" s="1"/>
+      <c r="HE86" s="1"/>
+      <c r="HF86" s="1"/>
+      <c r="HG86" s="1"/>
+      <c r="HH86" s="1"/>
+      <c r="HI86" s="1"/>
+      <c r="HJ86" s="1"/>
+      <c r="HK86" s="1"/>
+      <c r="HL86" s="1"/>
+      <c r="HM86" s="1"/>
+      <c r="HN86" s="1"/>
+      <c r="HO86" s="1"/>
+      <c r="HP86" s="1"/>
+      <c r="HQ86" s="1"/>
+      <c r="HR86" s="1"/>
+      <c r="HS86" s="1"/>
+      <c r="HT86" s="1"/>
+      <c r="HU86" s="1"/>
+      <c r="HV86" s="1"/>
+      <c r="HW86" s="1"/>
+      <c r="HX86" s="1"/>
+      <c r="HY86" s="1"/>
+      <c r="HZ86" s="1"/>
+      <c r="IA86" s="1"/>
+      <c r="IB86" s="1"/>
+      <c r="IC86" s="1"/>
+      <c r="ID86" s="1"/>
+      <c r="IE86" s="1"/>
+      <c r="IF86" s="1"/>
+      <c r="IG86" s="1"/>
+      <c r="IH86" s="1"/>
+      <c r="II86" s="1"/>
+      <c r="IJ86" s="1"/>
+      <c r="IK86" s="1"/>
+      <c r="IL86" s="1"/>
+      <c r="IM86" s="1"/>
+      <c r="IN86" s="1"/>
+      <c r="IO86" s="1"/>
+      <c r="IP86" s="1"/>
+      <c r="IQ86" s="1"/>
+      <c r="IR86" s="1"/>
+      <c r="IS86" s="1"/>
+      <c r="IT86" s="1"/>
+      <c r="IU86" s="1"/>
+      <c r="IV86" s="1"/>
     </row>
-    <row r="87" spans="1:256" ht="15.95" customHeight="1"/>
+    <row r="87" spans="1:256" ht="12" customHeight="1">
+      <c r="I87" s="5"/>
+      <c r="J87" s="5"/>
+      <c r="K87" s="5"/>
+      <c r="L87" s="5"/>
+      <c r="M87" s="5"/>
+      <c r="N87" s="5"/>
+      <c r="O87" s="5"/>
+      <c r="P87" s="5"/>
+      <c r="Q87" s="5"/>
+      <c r="R87" s="5"/>
+    </row>
     <row r="88" spans="1:256" ht="15.95" customHeight="1"/>
     <row r="89" spans="1:256" ht="15.95" customHeight="1"/>
     <row r="90" spans="1:256" ht="15.95" customHeight="1"/>
@@ -21567,127 +21579,127 @@
     <row r="104" spans="1:16" ht="15.95" customHeight="1"/>
     <row r="105" spans="1:16" ht="15.95" customHeight="1"/>
     <row r="106" spans="1:16" ht="15.95" customHeight="1"/>
-    <row r="107" spans="1:16" ht="15.95" customHeight="1">
-      <c r="A107" s="62" t="s">
+    <row r="107" spans="1:16" ht="15.95" customHeight="1"/>
+    <row r="108" spans="1:16" ht="15.95" customHeight="1">
+      <c r="A108" s="62" t="s">
         <v>190</v>
       </c>
-      <c r="B107" s="62"/>
-      <c r="C107" s="62"/>
-      <c r="D107" s="62"/>
-      <c r="E107" s="62"/>
-      <c r="F107" s="62"/>
-      <c r="G107" s="62"/>
-      <c r="H107" s="62"/>
-      <c r="I107" s="62"/>
-      <c r="J107" s="62"/>
-      <c r="K107" s="62"/>
-      <c r="L107" s="62"/>
-      <c r="M107" s="62"/>
-      <c r="N107" s="62"/>
-      <c r="O107" s="62"/>
-      <c r="P107" s="62"/>
-    </row>
-    <row r="108" spans="1:16" ht="15.95" customHeight="1">
-      <c r="A108" s="20" t="s">
-        <v>191</v>
-      </c>
-      <c r="B108" s="20" t="s">
-        <v>192</v>
-      </c>
-      <c r="C108" s="20" t="s">
-        <v>193</v>
-      </c>
-      <c r="D108" s="20" t="s">
-        <v>194</v>
-      </c>
-      <c r="E108" s="20" t="s">
-        <v>195</v>
-      </c>
-      <c r="F108" s="20" t="s">
-        <v>196</v>
-      </c>
-      <c r="G108" s="20" t="s">
-        <v>197</v>
-      </c>
-      <c r="H108" s="20" t="s">
-        <v>198</v>
-      </c>
-      <c r="I108" s="20" t="s">
-        <v>199</v>
-      </c>
-      <c r="J108" s="20" t="s">
-        <v>200</v>
-      </c>
-      <c r="K108" s="20" t="s">
-        <v>201</v>
-      </c>
-      <c r="L108" s="20" t="s">
-        <v>202</v>
-      </c>
-      <c r="M108" s="20" t="s">
-        <v>203</v>
-      </c>
-      <c r="N108" s="20" t="s">
-        <v>204</v>
-      </c>
-      <c r="O108" s="20" t="s">
-        <v>205</v>
-      </c>
-      <c r="P108" s="20" t="s">
-        <v>206</v>
-      </c>
+      <c r="B108" s="62"/>
+      <c r="C108" s="62"/>
+      <c r="D108" s="62"/>
+      <c r="E108" s="62"/>
+      <c r="F108" s="62"/>
+      <c r="G108" s="62"/>
+      <c r="H108" s="62"/>
+      <c r="I108" s="62"/>
+      <c r="J108" s="62"/>
+      <c r="K108" s="62"/>
+      <c r="L108" s="62"/>
+      <c r="M108" s="62"/>
+      <c r="N108" s="62"/>
+      <c r="O108" s="62"/>
+      <c r="P108" s="62"/>
     </row>
     <row r="109" spans="1:16" ht="15.95" customHeight="1">
-      <c r="A109" s="22" t="s">
+      <c r="A109" s="20" t="s">
+        <v>191</v>
+      </c>
+      <c r="B109" s="20" t="s">
+        <v>192</v>
+      </c>
+      <c r="C109" s="20" t="s">
+        <v>193</v>
+      </c>
+      <c r="D109" s="20" t="s">
+        <v>194</v>
+      </c>
+      <c r="E109" s="20" t="s">
+        <v>195</v>
+      </c>
+      <c r="F109" s="20" t="s">
+        <v>196</v>
+      </c>
+      <c r="G109" s="20" t="s">
+        <v>197</v>
+      </c>
+      <c r="H109" s="20" t="s">
+        <v>198</v>
+      </c>
+      <c r="I109" s="20" t="s">
+        <v>199</v>
+      </c>
+      <c r="J109" s="20" t="s">
+        <v>200</v>
+      </c>
+      <c r="K109" s="20" t="s">
+        <v>201</v>
+      </c>
+      <c r="L109" s="20" t="s">
+        <v>202</v>
+      </c>
+      <c r="M109" s="20" t="s">
+        <v>203</v>
+      </c>
+      <c r="N109" s="20" t="s">
+        <v>204</v>
+      </c>
+      <c r="O109" s="20" t="s">
+        <v>205</v>
+      </c>
+      <c r="P109" s="20" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="110" spans="1:16" ht="15.95" customHeight="1">
+      <c r="A110" s="22" t="s">
         <v>207</v>
       </c>
-      <c r="B109" s="22" t="s">
+      <c r="B110" s="22" t="s">
         <v>208</v>
       </c>
-      <c r="C109" s="22" t="s">
+      <c r="C110" s="22" t="s">
         <v>209</v>
       </c>
-      <c r="D109" s="22" t="s">
+      <c r="D110" s="22" t="s">
         <v>210</v>
       </c>
-      <c r="E109" s="22" t="s">
+      <c r="E110" s="22" t="s">
         <v>211</v>
       </c>
-      <c r="F109" s="22" t="s">
+      <c r="F110" s="22" t="s">
         <v>212</v>
       </c>
-      <c r="G109" s="22" t="s">
+      <c r="G110" s="22" t="s">
         <v>213</v>
       </c>
-      <c r="H109" s="22" t="s">
+      <c r="H110" s="22" t="s">
         <v>214</v>
       </c>
-      <c r="I109" s="22" t="s">
+      <c r="I110" s="22" t="s">
         <v>215</v>
       </c>
-      <c r="J109" s="22" t="s">
+      <c r="J110" s="22" t="s">
         <v>216</v>
       </c>
-      <c r="K109" s="22" t="s">
+      <c r="K110" s="22" t="s">
         <v>217</v>
       </c>
-      <c r="L109" s="22" t="s">
+      <c r="L110" s="22" t="s">
         <v>218</v>
       </c>
-      <c r="M109" s="22" t="s">
+      <c r="M110" s="22" t="s">
         <v>219</v>
       </c>
-      <c r="N109" s="22" t="s">
+      <c r="N110" s="22" t="s">
         <v>220</v>
       </c>
-      <c r="O109" s="22" t="s">
+      <c r="O110" s="22" t="s">
         <v>221</v>
       </c>
-      <c r="P109" s="22" t="s">
+      <c r="P110" s="22" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="110" spans="1:16" ht="15.95" customHeight="1"/>
     <row r="111" spans="1:16" ht="15.95" customHeight="1"/>
     <row r="112" spans="1:16" ht="15.95" customHeight="1"/>
     <row r="113" ht="15.95" customHeight="1"/>
@@ -21757,57 +21769,57 @@
     <row r="177" spans="1:6" ht="15.95" customHeight="1"/>
     <row r="178" spans="1:6" ht="15.95" customHeight="1"/>
     <row r="179" spans="1:6" ht="15.95" customHeight="1"/>
-    <row r="180" spans="1:6" ht="15.95" customHeight="1">
-      <c r="A180" s="62" t="s">
+    <row r="180" spans="1:6" ht="15.95" customHeight="1"/>
+    <row r="181" spans="1:6" ht="15.95" customHeight="1">
+      <c r="A181" s="62" t="s">
         <v>189</v>
       </c>
-      <c r="B180" s="62"/>
-      <c r="C180" s="62"/>
-      <c r="D180" s="62"/>
-      <c r="E180" s="62"/>
-      <c r="F180" s="62"/>
-    </row>
-    <row r="181" spans="1:6" ht="15.95" customHeight="1">
-      <c r="A181" s="20" t="s">
-        <v>223</v>
-      </c>
-      <c r="B181" s="20" t="s">
-        <v>224</v>
-      </c>
-      <c r="C181" s="20" t="s">
-        <v>225</v>
-      </c>
-      <c r="D181" s="20" t="s">
-        <v>226</v>
-      </c>
-      <c r="E181" s="20" t="s">
-        <v>227</v>
-      </c>
-      <c r="F181" s="20" t="s">
-        <v>228</v>
-      </c>
+      <c r="B181" s="62"/>
+      <c r="C181" s="62"/>
+      <c r="D181" s="62"/>
+      <c r="E181" s="62"/>
+      <c r="F181" s="62"/>
     </row>
     <row r="182" spans="1:6" ht="15.95" customHeight="1">
-      <c r="A182" s="22" t="s">
+      <c r="A182" s="20" t="s">
+        <v>223</v>
+      </c>
+      <c r="B182" s="20" t="s">
+        <v>224</v>
+      </c>
+      <c r="C182" s="20" t="s">
+        <v>225</v>
+      </c>
+      <c r="D182" s="20" t="s">
+        <v>226</v>
+      </c>
+      <c r="E182" s="20" t="s">
+        <v>227</v>
+      </c>
+      <c r="F182" s="20" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="183" spans="1:6" ht="15.95" customHeight="1">
+      <c r="A183" s="22" t="s">
         <v>229</v>
       </c>
-      <c r="B182" s="22" t="s">
+      <c r="B183" s="22" t="s">
         <v>230</v>
       </c>
-      <c r="C182" s="22" t="s">
+      <c r="C183" s="22" t="s">
         <v>231</v>
       </c>
-      <c r="D182" s="22" t="s">
+      <c r="D183" s="22" t="s">
         <v>232</v>
       </c>
-      <c r="E182" s="22" t="s">
+      <c r="E183" s="22" t="s">
         <v>233</v>
       </c>
-      <c r="F182" s="22" t="s">
+      <c r="F183" s="22" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="183" spans="1:6" ht="15.95" customHeight="1"/>
     <row r="184" spans="1:6" ht="15.95" customHeight="1"/>
     <row r="185" spans="1:6" ht="15.95" customHeight="1"/>
     <row r="186" spans="1:6" ht="15.95" customHeight="1"/>
@@ -21924,29 +21936,29 @@
     <row r="297" spans="1:2" ht="15.95" customHeight="1"/>
     <row r="298" spans="1:2" ht="15.95" customHeight="1"/>
     <row r="299" spans="1:2" ht="15.95" customHeight="1"/>
-    <row r="300" spans="1:2" ht="15.95" customHeight="1">
-      <c r="A300" s="62" t="s">
+    <row r="300" spans="1:2" ht="15.95" customHeight="1"/>
+    <row r="301" spans="1:2" ht="15.95" customHeight="1">
+      <c r="A301" s="62" t="s">
         <v>278</v>
       </c>
-      <c r="B300" s="62"/>
-    </row>
-    <row r="301" spans="1:2" ht="15.95" customHeight="1">
-      <c r="A301" s="20" t="s">
-        <v>279</v>
-      </c>
-      <c r="B301" s="21" t="s">
-        <v>280</v>
-      </c>
+      <c r="B301" s="62"/>
     </row>
     <row r="302" spans="1:2" ht="15.95" customHeight="1">
-      <c r="A302" s="22" t="s">
+      <c r="A302" s="20" t="s">
+        <v>279</v>
+      </c>
+      <c r="B302" s="21" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="303" spans="1:2" ht="15.95" customHeight="1">
+      <c r="A303" s="22" t="s">
         <v>281</v>
       </c>
-      <c r="B302" s="22" t="s">
+      <c r="B303" s="22" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="303" spans="1:2" ht="15.95" customHeight="1"/>
     <row r="304" spans="1:2" ht="15.95" customHeight="1"/>
     <row r="305" ht="15.95" customHeight="1"/>
     <row r="306" ht="15.95" customHeight="1"/>
@@ -21970,57 +21982,57 @@
     <row r="324" spans="1:6" ht="15.95" customHeight="1"/>
     <row r="325" spans="1:6" ht="15.95" customHeight="1"/>
     <row r="326" spans="1:6" ht="15.95" customHeight="1"/>
-    <row r="327" spans="1:6" ht="15.95" customHeight="1">
-      <c r="A327" s="58" t="s">
+    <row r="327" spans="1:6" ht="15.95" customHeight="1"/>
+    <row r="328" spans="1:6" ht="15.95" customHeight="1">
+      <c r="A328" s="58" t="s">
         <v>318</v>
       </c>
-      <c r="B327" s="58"/>
-      <c r="C327" s="58"/>
-      <c r="D327" s="58"/>
-      <c r="E327" s="58"/>
-      <c r="F327" s="58"/>
-    </row>
-    <row r="328" spans="1:6" ht="15.95" customHeight="1">
-      <c r="A328" s="23" t="s">
-        <v>307</v>
-      </c>
-      <c r="B328" s="23" t="s">
-        <v>308</v>
-      </c>
-      <c r="C328" s="23" t="s">
-        <v>309</v>
-      </c>
-      <c r="D328" s="23" t="s">
-        <v>310</v>
-      </c>
-      <c r="E328" s="26" t="s">
-        <v>227</v>
-      </c>
-      <c r="F328" s="26" t="s">
-        <v>228</v>
-      </c>
+      <c r="B328" s="58"/>
+      <c r="C328" s="58"/>
+      <c r="D328" s="58"/>
+      <c r="E328" s="58"/>
+      <c r="F328" s="58"/>
     </row>
     <row r="329" spans="1:6" ht="15.95" customHeight="1">
-      <c r="A329" s="24" t="s">
+      <c r="A329" s="23" t="s">
+        <v>307</v>
+      </c>
+      <c r="B329" s="23" t="s">
+        <v>308</v>
+      </c>
+      <c r="C329" s="23" t="s">
+        <v>309</v>
+      </c>
+      <c r="D329" s="23" t="s">
+        <v>310</v>
+      </c>
+      <c r="E329" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="F329" s="26" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="330" spans="1:6" ht="15.95" customHeight="1">
+      <c r="A330" s="24" t="s">
         <v>311</v>
       </c>
-      <c r="B329" s="24" t="s">
+      <c r="B330" s="24" t="s">
         <v>312</v>
       </c>
-      <c r="C329" s="24" t="s">
+      <c r="C330" s="24" t="s">
         <v>313</v>
       </c>
-      <c r="D329" s="24" t="s">
+      <c r="D330" s="24" t="s">
         <v>314</v>
       </c>
-      <c r="E329" s="24" t="s">
+      <c r="E330" s="24" t="s">
         <v>315</v>
       </c>
-      <c r="F329" s="24" t="s">
+      <c r="F330" s="24" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="330" spans="1:6" ht="15.95" customHeight="1"/>
     <row r="331" spans="1:6" ht="15.95" customHeight="1"/>
     <row r="332" spans="1:6" ht="15.95" customHeight="1"/>
     <row r="333" spans="1:6" ht="15.95" customHeight="1"/>
@@ -22741,18 +22753,19 @@
     <row r="1048" ht="15.95" customHeight="1"/>
     <row r="1049" ht="15.95" customHeight="1"/>
     <row r="1050" ht="15.95" customHeight="1"/>
+    <row r="1051" ht="15.95" customHeight="1"/>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A327:F327"/>
+    <mergeCell ref="A328:F328"/>
     <mergeCell ref="A1:A4"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="B3:E3"/>
-    <mergeCell ref="A300:B300"/>
-    <mergeCell ref="A180:F180"/>
-    <mergeCell ref="A107:P107"/>
-    <mergeCell ref="A81:B81"/>
-    <mergeCell ref="A71:B71"/>
-    <mergeCell ref="A64:C64"/>
+    <mergeCell ref="A301:B301"/>
+    <mergeCell ref="A181:F181"/>
+    <mergeCell ref="A108:P108"/>
+    <mergeCell ref="A82:B82"/>
+    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="A65:C65"/>
     <mergeCell ref="A27:C27"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
@@ -23158,32 +23171,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24">
-      <c r="A1" s="70" t="s">
+      <c r="A1" s="73" t="s">
         <v>100</v>
       </c>
-      <c r="B1" s="71"/>
-      <c r="C1" s="71"/>
-      <c r="D1" s="71"/>
-      <c r="E1" s="71"/>
-      <c r="F1" s="71"/>
-      <c r="G1" s="71"/>
-      <c r="H1" s="71"/>
-      <c r="I1" s="71"/>
-      <c r="J1" s="71"/>
-      <c r="K1" s="71"/>
-      <c r="L1" s="71"/>
-      <c r="M1" s="71"/>
-      <c r="N1" s="71"/>
-      <c r="O1" s="71"/>
-      <c r="P1" s="71"/>
-      <c r="Q1" s="71"/>
-      <c r="R1" s="71"/>
-      <c r="S1" s="71"/>
-      <c r="T1" s="71"/>
-      <c r="U1" s="71"/>
-      <c r="V1" s="71"/>
-      <c r="W1" s="71"/>
-      <c r="X1" s="71"/>
+      <c r="B1" s="74"/>
+      <c r="C1" s="74"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
+      <c r="F1" s="74"/>
+      <c r="G1" s="74"/>
+      <c r="H1" s="74"/>
+      <c r="I1" s="74"/>
+      <c r="J1" s="74"/>
+      <c r="K1" s="74"/>
+      <c r="L1" s="74"/>
+      <c r="M1" s="74"/>
+      <c r="N1" s="74"/>
+      <c r="O1" s="74"/>
+      <c r="P1" s="74"/>
+      <c r="Q1" s="74"/>
+      <c r="R1" s="74"/>
+      <c r="S1" s="74"/>
+      <c r="T1" s="74"/>
+      <c r="U1" s="74"/>
+      <c r="V1" s="74"/>
+      <c r="W1" s="74"/>
+      <c r="X1" s="74"/>
     </row>
     <row r="2" spans="1:24">
       <c r="A2" s="26" t="s">
@@ -23339,7 +23352,7 @@
       </c>
       <c r="B11" s="68"/>
       <c r="C11" s="68"/>
-      <c r="D11" s="69"/>
+      <c r="D11" s="72"/>
     </row>
     <row r="12" spans="1:24">
       <c r="A12" s="37" t="s">
@@ -23361,7 +23374,7 @@
       </c>
       <c r="B24" s="68"/>
       <c r="C24" s="68"/>
-      <c r="D24" s="69"/>
+      <c r="D24" s="72"/>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="37" t="s">
@@ -23383,7 +23396,7 @@
       </c>
       <c r="B38" s="68"/>
       <c r="C38" s="68"/>
-      <c r="D38" s="69"/>
+      <c r="D38" s="72"/>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="37" t="s">
@@ -23405,7 +23418,7 @@
       </c>
       <c r="B54" s="68"/>
       <c r="C54" s="68"/>
-      <c r="D54" s="69"/>
+      <c r="D54" s="72"/>
     </row>
     <row r="55" spans="1:8">
       <c r="A55" s="44" t="s">
@@ -23431,7 +23444,7 @@
       </c>
       <c r="B67" s="68"/>
       <c r="C67" s="68"/>
-      <c r="D67" s="69"/>
+      <c r="D67" s="72"/>
     </row>
     <row r="68" spans="1:4">
       <c r="A68" s="37" t="s">
@@ -23453,7 +23466,7 @@
       </c>
       <c r="B89" s="68"/>
       <c r="C89" s="68"/>
-      <c r="D89" s="69"/>
+      <c r="D89" s="72"/>
     </row>
     <row r="90" spans="1:4">
       <c r="A90" s="37" t="s">
@@ -23475,7 +23488,7 @@
       </c>
       <c r="B105" s="68"/>
       <c r="C105" s="68"/>
-      <c r="D105" s="69"/>
+      <c r="D105" s="72"/>
     </row>
     <row r="106" spans="1:8" s="47" customFormat="1">
       <c r="A106" s="44" t="s">
@@ -23496,12 +23509,12 @@
       <c r="H106" s="46"/>
     </row>
     <row r="120" spans="1:4">
-      <c r="A120" s="72" t="s">
+      <c r="A120" s="69" t="s">
         <v>181</v>
       </c>
-      <c r="B120" s="73"/>
-      <c r="C120" s="73"/>
-      <c r="D120" s="74"/>
+      <c r="B120" s="70"/>
+      <c r="C120" s="70"/>
+      <c r="D120" s="71"/>
     </row>
     <row r="121" spans="1:4" ht="60">
       <c r="A121" s="37" t="s">
@@ -23560,7 +23573,7 @@
       </c>
       <c r="B167" s="68"/>
       <c r="C167" s="68"/>
-      <c r="D167" s="69"/>
+      <c r="D167" s="72"/>
     </row>
     <row r="168" spans="1:4">
       <c r="A168" s="37" t="s">
@@ -23582,7 +23595,7 @@
       </c>
       <c r="B190" s="68"/>
       <c r="C190" s="68"/>
-      <c r="D190" s="69"/>
+      <c r="D190" s="72"/>
     </row>
     <row r="191" spans="1:4">
       <c r="A191" s="37" t="s">
@@ -23604,7 +23617,7 @@
       </c>
       <c r="B220" s="68"/>
       <c r="C220" s="68"/>
-      <c r="D220" s="69"/>
+      <c r="D220" s="72"/>
     </row>
     <row r="221" spans="1:4">
       <c r="A221" s="37" t="s">
@@ -23621,12 +23634,12 @@
       </c>
     </row>
     <row r="239" spans="1:4">
-      <c r="A239" s="72" t="s">
+      <c r="A239" s="69" t="s">
         <v>361</v>
       </c>
-      <c r="B239" s="73"/>
-      <c r="C239" s="73"/>
-      <c r="D239" s="74"/>
+      <c r="B239" s="70"/>
+      <c r="C239" s="70"/>
+      <c r="D239" s="71"/>
     </row>
     <row r="240" spans="1:4">
       <c r="A240" s="37" t="s">
@@ -23648,12 +23661,12 @@
       <c r="D241" s="56"/>
     </row>
     <row r="264" spans="1:4">
-      <c r="A264" s="72" t="s">
+      <c r="A264" s="69" t="s">
         <v>331</v>
       </c>
-      <c r="B264" s="73"/>
-      <c r="C264" s="73"/>
-      <c r="D264" s="74"/>
+      <c r="B264" s="70"/>
+      <c r="C264" s="70"/>
+      <c r="D264" s="71"/>
     </row>
     <row r="265" spans="1:4">
       <c r="A265" s="51" t="s">
@@ -23773,12 +23786,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="A300:B300"/>
-    <mergeCell ref="A320:B320"/>
-    <mergeCell ref="A340:B340"/>
-    <mergeCell ref="A355:B355"/>
-    <mergeCell ref="A239:D239"/>
-    <mergeCell ref="A264:D264"/>
     <mergeCell ref="A220:D220"/>
     <mergeCell ref="A167:D167"/>
     <mergeCell ref="A190:D190"/>
@@ -23792,6 +23799,12 @@
     <mergeCell ref="A24:D24"/>
     <mergeCell ref="A54:D54"/>
     <mergeCell ref="A67:D67"/>
+    <mergeCell ref="A300:B300"/>
+    <mergeCell ref="A320:B320"/>
+    <mergeCell ref="A340:B340"/>
+    <mergeCell ref="A355:B355"/>
+    <mergeCell ref="A239:D239"/>
+    <mergeCell ref="A264:D264"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>